<commit_message>
changed the name of file
</commit_message>
<xml_diff>
--- a/mergedIPL.xlsx
+++ b/mergedIPL.xlsx
@@ -631,40 +631,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ROHIT SHARMA</t>
+          <t>SHIKHAR DHAWAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ipl2023_73</t>
+          <t>smat2022_131</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>137</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
         <v>7</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>114.3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>42.9</v>
+        <v>44.4</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -697,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -712,25 +712,25 @@
         <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AD2" t="n">
         <v>20</v>
       </c>
       <c r="AE2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AF2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUTExMVFhUXGBoYGBcYFxcXGhoWFxcYGBYbGhgYHSggGhsmHhcVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGy0lICYtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOMA3gMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQIDBAYHAQj/xAA/EAABAwEEBwYEAwYGAwAAAAABAAIRAwQSITEFBkFRYXGBEyKRobHwBzLB0UJS4RQjM2JyghU0Q7LC8QhEkv/EABoBAQACAwEAAAAAAAAAAAAAAAADBAECBQb/xAA4EQACAQIEAggDBwMFAAAAAAAAAQIDEQQSITFBcQUTUWGBobHwIjLhM3KRssHR8TQ1QhQjQ3OC/9oADAMBAAIRAxEAPwDuKIiAIiIAiIgCtVKrWxJAnASYk7liaW0rSszC+q4NEE47hifAL5o0prhabVaH1X1CWSbgcSA0Sbt0D5TjzQHctedexYALlE1TmTMNaBiZjGYk5LW9H/Gak9jjUpCm7AN7xPzYXjhkMzjlsXJtLazVbRTFNxwGZklziBm5xzOagpJ8IQHWHfFWt2jg+qXMaS0Gm1rbwAwdjx3KNrfFC1NF6lVfBMxUcHR0DdpnI5bFzeJafeXsq3djMrAO2aM+OIFNorWZxqAYlpF0mcTiZGC6HqxrnZraG3CWvdMMdEmNojCMF8oNzwxUxoXTVazPY9hxYbwHqJGMH6lZB9eouSaq/E4OFMVDPyte05gnC+wnME7Jw64dXo1Q8BzSCDkQgLiIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgORfHq3uZTpME4zyIILXY9QI2zwXCpJGPJdZ+P2mw+0U7K3/Sbfcf5nzA5xj1C5lYtG1KzXPY2WtME8ffqsMylfYx2EfRUudOAClaOr1epg2mTxAPrkpijqNacjDd5gnzhYzx7Tbq59hqLBGZ6bVVAPuFuFm1ArSbwOBwwmQrjtR6u1kY48ljrI9plUZ9hpbGnZ+q9qPI9F0OhqWxnzHbI4Yqxb9W6YyGO9adfG9iT/SzsaLRrkFp2g5Ls/wAFNcQR+x1X94uJYXHbiSBzjLfK4/pOy9m8hWrFan0ajKrDdc1wcDtkGQVMiu1bQ+ykUXq3pMWqy0q4ze0E8HDBw8QVKIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiA+YPi9ZyzStozN4tcP7mBbLqzYRRosYBjGPFxxcti+NGrHaOoW1g+VzadX+ku7jvEx1Cj9H4KviHZJFvCRu7k5ZLNhkFI2ehisWyPwUjZqm5VEdB7B9I4zmsG0USQpKrXjNYNpriNqzKxiNyAtgOKhbYcQpm21RiohzZmVojZo07W6gJkeY3rVCcwVt+tRkAe9q1GoAujS+VHJr/OzunwB0q99K0UHGQwtc3f3pDh5NXXFwn/AMfaTjXrvAddFMAuHy3i6QCNpgYcl3ZSEIREQBERAEREAREQBERAEREAREQBERAQ+tlk7WyVmRJLcOYII9Fy2la6TahaXiQcp8J3LrWmrU2nReXHMFo4kg/Y+C4PbrBZqXerZuMwN5471BVSdkyzh3JXaN5sGk6DzdFRs7gVPWezDYVxqjUszHyx7pki67ePmAkDETkt51UtzzLLznAZXjJHCdoVeUFF7Mt05ynxRtNpDWglxAA2krXrdrFZR+PA5EAx6clGa1uJeL7nEA4MnA81rlehTqOu3XOMfKydmOcEmOAWYqMjMpSjxJi26boR/Ead8YxzWJStjXgljg6NyhqelrEO62nOAOM5ESPmHEeKlLBZKZdfojAjGBE8x4YpKCXBmkKkpcU+RresNN3zDLJawWYro1tsQLXDnC1LQGjXWisKbR3oOOwRmSp6Ull1KtaDc9OJ2f4CaPNOw1Kh/wBSqY5MF0+c+C6ctF+G+l6QossbGkdiLof+F7hJceBmd63pTKSauiGcJQdpBERZNQiIgCIiAIiIAiIgCIiAIiIAiIgITWujeoE/lM+ILfquYaU0XNWnVYO83KRMHkdq6prO6LO4b4H1+i02wtDs1Ur6STR0MJ8UWmavT0ETXdaCxoquLnFwEC88EOIYZAJkyY2lSOhbNce4jDZkBMZ4DmthrUMCdgUfo2lIvKGU21Ytxpxi9DX9NhzqgdnB9Cr9lp1WGaTnMnMA7852OGO1UaZJY4kAnaQtlsNAPpNcIMiRyKxCbjsJRUnqaNX1XuhwpsDA8Q4BoAIz9cYCl9BaKbQb5LaKlkAGIUNbnxwWW5S0ZjIo7ELpgCTC03V+uaTqrQYdUcKYcNgccTPKVtdvfIWlWWvD3wAXOIu85J+ilgvhaK03apFnatSbEKdoutEABpA/luEfRdEWkfDsdoH1jiLtOmDvLWm/HCSPNbupqCtAgxc81TkrBERTFUIiIAiIgCIiAIiIAiIgCIiAIiICC1xcG2Vzjk0tPibv/Jaho6tC3vWCxdvZq1L89NwHOMPNcR1c024NIfmJnpmq+IjdXRbwtTK7M6Fbqv7p3LAb9/2Wv2HWnsg4PDWnGAO8Q07wQPLctQt+udSoblIQSY3k47AsOhq9UdFSrWYx18GDedgDIBc3flwUcabT+LQsyq5/kV/QnKOshrVT+7AbOEkh0CcboHAra9ULzaJvYC+4sacwwmRy24clzevq/H7wWll8bIIbugHPhkrTdYLTQ7geDGUY5Zwsunf5TXrZQ1mjstotAhatpa07dihtF629sAHQHZcJ/VRWndJSboOGMcf1/RaKDzWZtOsst0WtMaTzaN3qonRlIOe0MH4pE5w0fW8sO1OImTHX3uXTPgzoChaG1n1mXnUyy6ZIgOvyDGYMBWVD4bIpdZ8abOj6gWXs7FTwi9Lo4E4eULZFRTYAAAIAwA4BVqRKysQyeZthERZMBERAEREAREQBERAEREAREQBERAF88/E3RX7FbnxIp1/3jTxJN8dD6hfQy0z4n6q/4hZCGD9/S79PAEn8zOoHiAsNGU7HENW7Cx3fdiWnI4Ymd22FtVmtFlZ3ajQ3DJzYwHGIPNc6sVpfScRiCCQ4HAy3YeKm7ZUNoDb14Bo6YkA+iilF5r30LVGtkj8O5tVp0lZCQykGuOwMaM4x7xgbFhW5tMg3wADmHRe8d+eShrBQptc5zXGWNhs5SSQ2N2zxWBpS3doTEiIOe2IcPEz0WHFt6EksTJx1KGWgU5u7XGCcZEn7+ax/20DE4kYgc8PRR1SpG3fx8FaL1MolLMzJdWLjmuh/C7Xmz2A1zaS4MeGkXWlxlpIGXArnlls5dgAT7yWwaM0IGd6pDnbG/hHP8x8lbwuDq4qeWmtFu+C+vdv22WpHOapxvLjwPoTVbWuhbw40g8QJh4glpwB5LYVxj4f6TFC2NvGG1O4Tsk/LPXDquzqXpDBrC1VFbNJ/o/Mjo1M8bv37QREVAmCIiAIiIAiIgCIiAIiIAiIgCIiAIiIDlHxL+GZrvdarG0dqcalLIPP5mzgHbxtXHbVUq0C6lVY+m9shzXAtIM4YEcOq+oNZtNssdB1V2JyY38zjl02lfPesFZ1sc6q83ql4gnzEcBkplh5ui6z2Tt77lor95qprOoLc1p+kc4GcdDmsd1pP6LLqaMOyUp6GcTkeKgzRJckiNc6T9ln6N0Y+ocsN5yHvcpuw6BAxdh6qZp0g0QBA4LtdG9GSxKVSppDh2y/Zd+74dpVr1lTeVb+n198saw2JtMQM9p2lZl1eVHtYC5xAAzJwAVNivVheILKf4Rk5w3n8o4DHkvTZoUUqcFyS9e5d7372c5u+sjKs1nLpIwAzd9BvK7ToDTlGuxoa+HholriL2Xn0XIG08ANgyAVxji0ggwdhGa5uMwbxS+OWq2tsv1ffrw0SNqeJyPRaeb/Ty53O7Iud6va6uZDLRL25X/xDnvHmt/s9dtRocxwc05ELzWIw1ShK0149p0aVaNRfCXURFXJQiIgCIiAIiIAiIgCIiAIiIAqHuABJMAYk8FWtG+JmmjSpNoMJmpN4jY0RhhlM+AKmw9B16saa4+RpOahHMzSNftYDa6xuGKbJbT3YZvPP0Wo6Lkmc2uEEbjO7p5LLtJ7pkGDwV3VrRrjTvEYEkjrl5ALs9NSjQw8aUNFt4LXzfEiwEXUquT4fx+9i9RsbNyv13UqDbzrrSTAJ359TwVrTGlWUiWt71QbIwBjaoGxWN1VxqOzMy447cmj2Oa5/RvQ06rVWurR3Set+a7O7j93e9icbGCcae/b2cu/057SrLbTccKjSeePmrekbe2iy+/kAM3HcE/YqYwuzzVP7BTvBxEluW4cgvYSjVyWja/DR6eHorrgjhLLfW5jWSy1Krm1bRkDLKWwbi7e5bNTxE7NijCVcpVi0AbPrt6LEcOoRtHfi3u+fuy4aEdRuRnX1SSrV6VUwkrNiEutcpjQmnatmdLHd05tOIPveoYNVxir1qcakcsldG0ZOLujr+hNPUrSO6Yftac+m8KXXFbJXcxwc0kEYghdG1b1kbXAZUgVPJ36rzGLwTpfFDVeh1KGJz/DLf1NkREXPLYREQBERAEREAREQBUOcAJOACrWha960Bs2ekZcPncMgd3E8FPhsPPEVFCH8LtI6tRU45mXdZdbo7lN11v5h8zv6RmBxWjaQrOtAg92DIJMune47uCx6VKTeMk7ScSepVx79gXrKGFp0I5Yb9vv32WOTOcpu8mQlrspILbxHLb9wsq3abLLNSo0u7ULYeR+G73cOJzncqrYBBJwgZqOsFj7Q9o7InAbYUlXB0q04TqL5Xfyt9eaV7rQmo15U4yS4oxbFYJMk557424qZaAMBgFW4AZABUlXNHsQylcocVSVVB2R13fVUE5+SjdeKnks78nbZve1tEteCuluzKg7X9/hvyPCV6EuqtjFPc1LlA4R16LKY3csenTkgDOfDipI0Yy27FXnJIjluW2MVzs1fp08B5lV3FA5mpi3YWTRqkEOBgjd6rwsVrIyoascyvxNos6vq7pMWii1094YO57+qlly/VjSpoVQfwOgOHDf0XTmukSMivL4qj1c9Nnt+3gdjD1M8O9FSIirE4REQBERAEREBH6ct3Y0H1NoED+o4BcWgvdJxkknqul/Ea03bO1v5nT4D9Vz/AEZZ722MyTuA9+a9J0TBU6DqPi/Q5mLk3Uyl2jZC5lRwvQxpghpILhEgnYAo9bPUqtplgDWgAObh+Rl5xOO0lrSYzlaq3JdLDzc7t+HmvVEE4qNrGPaqRqEM/Dm76BVPBartZsCdpVhzyVbjryNQCjWyCZAAgFzpABOWMZ8F7Sp3jGAzxOQABJJ4ALO0HohtqBrVi5lIS2lTbm5zQA43iIaBhLszPDHndIY9YeL1S0u3ppfRadrd7cNNVsWKFB1Htf8AX+PAw6VJrwTTqBxH4YumJjCfm2HDerQCyn2JlC3OpU3yxuAfmbjqd6Dh/NEwrO0rXo/EVJzkpNtWUk33vbZLT8VfVcZK0IpJpWd7e9bluFUB798l6AqgPfvqurcrmVo6nLp9+81ntEu9/KPucOhVvR7IaSr9kEgv/NiP6Rg379VSqS1bI3uXSELVVTCuFqhvY1MYhWKgWW8Kw8LeLMlqm6Mlv+pOmO0aaLj3miWz+XIjoY6ELn5Cy9EW7sK9OrsDhe5HA9IKoYvDdZBpb8Of1LFCrkknw4nYUVLHSARkcVUvNnZCIiAIiIAiIgNB+Kbzdot/MT5Fv6LW7Gy6ABmalJnSS4+bW+C234k2e8LM7dUI8RP/ABWtaLoVCbwgAm804E3m3my1s7AXYuwXpsFNRwcNVx/HNp6HMrr/AHn74GJpmvD3gCP9McGNMPPVzQOQKh3FTGnHU4JDg6oXDGQ92RkucBA5BQs5bz6bV08NbIre+/68SCp8xXXMx0HgrMK49Uwp1ojQocyWVcJimTiRhBEkcY9VIaI1qbQszaJpFz2FxpkuhkFxcb7MzieoAyWFTqFrg5uYM7D6qttZgMtotDpGOJiDII3HfyXFx2EnUqO8M0XZ7pWaVteW6fHbfe7QqqMVaVmr/v8AQUi8B9Wo4mrWLmuBEHGHEn8pywyhWFXUe5xlxJJO3ivF0MHhnRi3L5nvbbTZLRbLQgq1M7stl7b8SpoVxrcufv6qhoVym7Ec/fvirLIjPe8tpuA+YNAH9TyQ3zhZVUBoDRwAHkB73LHa68/DI1Wn/wCaYePNXqZvVCdjMP7j9h6qj/lfu9+ZEzKpsiAq6mAn374Lxh5K3aTLms34nkM+uQ6qPdmDwtwVhwWZUVg05lbRYMVwVBbIIOUY8jmrhzVIW01pc2R1HVGuX2OiXGSG3Sd9wls9QAVMrWtQ5FmLTk2o4DkYeP8AdHRbKvJVklUkl2s7tN3gn3BERRm4REQBERAQGuVmv2cHax7XD0+q0lul2U2zcAu4BoJkgDN3XpngumW+gKlN7DtB8dnmuMaSwcRx9F3ei4xrU3Tlwfr7f4lDFNwmpLijAOMe+aoBkk7sAvS7Mquy2V5ZeDXETiQPpmvSN21ZSseEoUAJIABJ3AE+SOG9YuYKV4Aql4tjIhUlyqKs1HIgXO0VqpXu47sVYqPVF6cFuomyRsdGqG945NBJ5Mptb53Ssqwghgn5nd53N2PlkoizNvhjTOIa139hAM82geKnCubOOXQhehdYVZsNS8X1NhN1u6636EyVjaRtBa2G/M7uN5nM+CzbLQuta0ZNEff/AKWklaN3xMF0+/e9KLcVSHyTx9Bl/wBrJs9me8wxjnHgMMM5OQUcnlWoSvoiKtLbrhxkfX7qg5qW0xomq1odcOYgiHCd0tOBKiXgg4ggjYcCN+C2p1IzTs7mzjKO6Ol6ltAsrYzl0+OHldU8oLUz/KM4l3+4j6KdXlq/2subO3S+zjyQREURIEREAREQFFXI8iuM6asDmjtMTJOOEY5Edd+9dohaFbLG0NdSfEAwMogmG+MqxR6QlgrVN1mSkuLVpbctOYWFWIbjxs7c7rc1jSthYLMHtaBeIMADAHDFx7xmRmVNaKrUqsMc0OJAMzJkiYnNpziNxWPbqB/ZC3aJA/tHd690KN1X/j+HrHpKuVaf+rwFbPJ3pzqOLTd9NYu/LTz31NFLqcRTyqylGN1z0fmZn+GBtrAgEEGZ2zEmN5BE8bxUZpekDaCwYCQ3oM1ttcA2lm+6T0g5dYULTs1+3E7BieE4egKjwPSEus6+o/lw93zUn4XdkbYjCpQ6uPGr6xKtKaCa2k54Db10kd26Q66SALpAInDEHNakHrfqNQVDXaJnPHY4YtgbBHZ+BXPLZRuvewbCS3kcQPAhdPoCvWkqlHESvKOV+EoqVvBtlbpClTTjOmrJ3X4Oxdc9WahWGLQctqqbXxjbsXokrFDK0VPCqo2UuxBw27x+qqs7pMRJyj349FLss4aABh99q1qVMuhrKWUt2B114G9TTioq4NuwgzuIxHvgs91XuyN3mqdTVpohZZs1PtK0/hp4Di4/Mfp0UzSo33spzF9waXbgTnz3LD0dSuNA25nmVlNx9+Kr1ZXlpstv3/UJkpUt3ZvNKjSYACWhhYHudBjvF2JnhCl7dZ5o1KVN7WBtRpLS6G95oJZeP82zgoRulq5F3tHbpwDo4uieqstquax7ARD4vYbWmRG4qg6T0eit4321d7cL2333LKrJXTu7+Fu5W+nIywBRpVGF7S6o0NutN4CDJcSMJ3AKNo0gKV+u0VHsaQGl5F5naNaxzi0zABMdNy9kAYqFdU7KuXtiH7xIOxwI2ghS9W82a/Phfuunp5mkai2ty7vDjqdL1McOwLRMBxLZzDXgPAJ2xJE8FsK1bUWpep1HQBLgLoyF1oAAnhC2lcDEJqrK/adai04KwREUJKEREAREQBc7bjenHH6leIt/+L/3T/MZp/ar7s/RHlaoexeZye2PBv3UFqd/E8PR32XiKfAf2nFe/wDCJvjP62l4erNm/wDY6H0asCx/xbQdsDHk133RFz19jP8A6aX50WF88fvz/Kyxqu8mrVx/FU/3NWr6zCKzSNzfIub6ADoiL1GD/u9f7kPRnJqf0lPnIhNKN7yx3YslEXoimtkZmjHSWu2wceSnaTkRQzIKvzFY9+SvUvk/uHqiKKWxGSTM1cZl0RFTZgyG++qpPvzRFECw7Mc1g6Vb3RwIXqLeWxtHc334f/5c/wBR9AtoRF5zFfbz5naw/wBnHkERFXJj/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAQEBAQDxAVFhAQEBYVFRIVFRgWEBUYFhcXFhUYFhkaHiggGBolGxUYITEiJSorLi4uGCAzODMsNygtLisBCgoKDg0OGxAQGy0lICUuLS0vLy8tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIALwBDAMBEQACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAAAQIEAwUGBwj/xABDEAABAwEFBAcECAQEBwAAAAABAAIRAwQSITFBBVFhgQYTIjJxkaFCscHwByNSYnKi0eEUgpLxFSSywkNTY3OTo9L/xAAaAQEAAgMBAAAAAAAAAAAAAAAAAwQBAgUG/8QAMhEAAgIBAwMCAwYHAQEAAAAAAAECAxEEEiExQVEFEyIyYQYUM3GBoSNCkbHB0fDhFf/aAAwDAQACEQMRAD8A9WWpuNACAYQyNDA1kAEA0AIBoAQDQAgGgBACGSFWuxnfe1v4nAe9ASp1GuEtcCN4II9EBJANACAEAIAQAgBACASwAQAgBAJACAEBgQwCAaAaAayAQDQAgGgGgBANACAEBrekO3bPYKBr2l91gMNAxe9xyawan3CSYAQyeLdJfpIt9sJZQcbNQJgNpH64j71TMHg2Oa1cjOGzjH2VznXqsucc3Plzj4kyStXLwbKHkuWCrXsrhUs1SpSO+m4tnxAz8Ctd5tswek9EPpWcHNo7TAgwBamiIO+q0YR95sRqIxUilk0cT1mm8OAc0gtcAQQZBBxBB1C2NCSAEMggBANAJACAFgAsgSAFgAgBAJAYEMDQDQAgGsgaAaAEA0AIBoAQAgI1ajWNc95Aa1pJJyAAkk8kB4htzaf+K2h1ofPUMJZZ6eV1mriPtuzPIaKnfc08IvaehSWWXdmbJpNEhjRGp/U5KhO2T7nQhTFdjcM2XSqDtMBjWPcVFvkuhu64vqTq7GpkEGmI8AtlORhwizntodHqJJNyFLG+aI5UQfY2n0a9InWW0/4XXdNGoT/DuPsOi91f4XYxuOGq6dVm5HJur2yaPWVMQghkEAIAQAgBYAkAIAQAgEgBACAroYGgGgGsmRoYGgBANACAaAEA0AIDlPpStJp7KtV3Op1dLlUqNa78pI5rDeEZXU8q6ON7AH3lzL+p1tN8p3uzwwNiFXeMFjnJsWEaBaLBlmdr2QQc1KnHBG4yNHtam2ZBUcuvBJHOOTzrbry2q6oDD6Tg9p1BYQWnzAXS07xFHM1CzJn0ZSfeaHfaAPmJVwpk0AkAIBoBIAQAgBYAIBLIBYAIAQFcIYGgGFkDQAEA0A0AIBoAQDQAgBAcp9KVEv2VaIHddSdyFZklYl0No9TzGyvbZwGXSSM43lc2UHJ5OpGagsG62X0qs4PV1GPaTq4QPVaSpwjeN2WdVZ7TSeAWlQNJE+WV6+06VIm8JMYCYJW8Io0nKXY0Vp231mLaDw06kEAxuOq3dKfcjVzXVHPdJLEKlN1VmbwWkcYMc9FNQ2ntZDqEmtyPfKTLrWt+yAPIQuic0kgBACAEAIAQAgEgBACAEAlgAgK6yYGEA0AwgGgGgBANACAaAEA0AIDzjp5t20OdbLKy71IpimQWy4kta4mdDLgNfBVLL2p7S/Xpk6lPucXaaFUlzqIgl2LsYHExjCrblnksqHHBhtOzXvD3VXh5jsFoiDIiTdmAAcJEzmpPchjCRH7NmctnSdFLOWsIcZ3TiqVjy+C9BcclLbOyi6oDNQtvYtBnDSP7FS1TS6kdsG+jIbP2bbAGjrr0HudU5sAknMnHMDHCGjCZKknZB9ERQrnHq8l622MlrWwA4VmOOozg+9a1WbcsW17uD0fo1tOraBVFa7eY8RdEdlwMSPEOV3T3OxPJR1NCqax3N2rJVEgBACAEAIAQAgBAJACwAQAgKyyYGEAwgGEA0A0AIBoAQDQDQAgBAeY/SHRZStLy041qbahbuIDg7zFIHkVQ1EP4ifk6mmsbpa8EdjUmlvaMDdxVVlhGHbNop3urYcdYybO8rXaSotbCotIIvNkEAmVhwM7sGSuLpkEEZXQe0VhRM5Njs2rSqNvNd8DxB3FbqKI5Nmo2lF4D7T2iR+IH4LKXDNG+Udh0MptNJ9UGTUcB4BokDzcTzV7RxxDPko62bc9vg6FWykCAEAIAQAgEgBACAEAkALABAVlkDCGBoBoBhANANACAaAEA0A0AIDgvpO2b9W61AEjqrjgAZEBzmmdBiRjwGMqvbU5SUkWqblGLg+5yFntJaWumGlt4xwE88FRcOcHQjNYOfq7ZqV3uDLrGk4T3uGABJVlVxiuSv7spvjglY7PWYAW2ijiCYJe2CdeyEk4vsZhGxd0bCj11Fznm00CXQTGEwBmbowzWslF9jMN6fUs9HtsOqVX0nCHulzXNILCW4mYwyUdtWFlG9Vzb2yNhWql9ahTmS58wJLjDSch8wJWK63JNIxZaoyTZ6nsSwdRSu6uN84RiQBEeACv01+3HBz7rfcluNgpSIEAIAQAgBACASAEAIAQAsASArBZMEkA0A0A0AIBoBhACAaAEA0ABAU9tWQ1rNaKIzq0KjB4uaWj3oD53sO0rrRTqiDTvMcDoe6QfCI5KtKvktQt4Nj0fe1jmVqV1tYDF2EmTMTG+FFZuzjsWaPba5R2TNuQ1rTaG5NwijhB1kYrTLJ1XT1bJWvaD3yKddrg4Yuinh3pADR94+axKTQjCrsjj216NltFQ02CG04EDAGIMRrv8FKouUOSrOajPg3X0cNdadqtqR2bOyo8nSXA0wP8A2GPwqxXHBVtnlns6lIgQAgBACAEAIAQAgBAJACAEALAKyyYGgGhkYQwMIBoAQDQAEA0A0AIAQDQHhX0w7Hp0ba6pZpv1qTatel7IJJa1zQN9xxI56rSTSaybxi3F4OT2HtG6RlOUE66csFpZXuJKrdvU6RlOy1my5rAdQ0QHHjhnCrNTiy2pQmiO0NrCjTuUWtDJwLQASRvHFbqpt5ZpK5RWEc0576tYMpi852nGD2juGMyfip+Ix5KqzOXB7T9EOy20LLXLoNd9f6xw3BjS1o4CT5lKp7lkzdXseDvVKRAgBACAEAIAQCQAgBACASAEAICsgGEMDQDCAaAaAEA0ABAMIBoBoAQAhk8e+lOp9aLaBLGRQqD/AKd43HcnuP8A5FzK9T79soeOn+Tpuj2a4z89f16HD2rYjakVKRgnUZFWI3NcMhnpk+UUTse1km7qZMSpPegQrTzNjYuilofdL3EDHDVaS1EV0JY6Vvqdbsfo8yiQ2k2Xuy1dxJOjROfhwVWd+VmXQtwpjDoejdFqYofVDG9iTvdnPzuCr6DVuV7i+j6foR6yr4N3g6Vdw5gIAQAgBACAEAkAIAQAgBACAEBUQEkAwhgaAaAaAaAEA0AIBoBoAQGC31+rpvdMQ0x46eqivsUK3Jk1FbnYonnO3LF19nrUf+ZTLfPL1Xm9FbGu+Mp9O56HU1uymUY9TznYN9jSx3skgtOYIMEei7VyWTm052nV7Lgi9Me5VZMsxNrY5rOIoXTdMPeTLWnOIzcY0w8VDbbGpZkZXJ0FisbaLTjLnd5x7zt3gNwGC51t8p8y6eDKWXwWaFQhwcPZIPktKbHCamuwsipR2nT0K7XtvNOHqOBXrqro2x3RZw51uDwzKpTQEAIAQAgBACAEAkAIAQAgEgKqAaAkhgYQDCAaAaAaAEA0ABAKpUa0FziA0CSSYA8ScllJvoG8HLbW6cUKRu0WGqcZdNykIwzIJOO4RjmrNeknLrwQS1EV0OcsO2qloqVXVnHF0hs9hk4BrQcsI8cdSuV69pHFQcP6f5Or6Ndv3qS/X/BfIkLyvU9B0OL6QWUU7WHAQLQwk8XNwcfIt5yuzprHOrnquCjfWo2cdx06Tmsc0HMLdvk0XQ1ex677DW/iATAMPGjmTiD8OKknFWx2siSceT1gm8eC89NNywW18KMgIy0CzHl7UaPyzV7Ttz6b2dUSCDeDhqfiI85XrfQNEsTnPr0x4OH6tqJLbGPTrk3OzulrDArsun7bcW8xmOUrrWaJr5WUIatP5jobNaqdUXqbw4cDl47lTlCUXhotRmpdGZlqbAgBACAEAIAQCQAgBACAqBAMICQQwNAMFANANANACAp7R2pRs4+sdicmjF55fEqWumVj+FEc7Yw6nNW3pfUJijTDRvd2neWQ9VehoV/MynPWP+VGgttqrWggVKjnknAHuzwaMBloP0VjZVTFyfCRFGVlstq5bMR2O/2oaNSTl8/PGjL1Wt8VRlJ/RHRh6XNc2yUV+ZjfRY0XGid7iM9w3xmrei010pu7UdWsJeEVNfrKYwVGm6J5b8suWau5ojExocSOeZ9VU1foGmve6Pwv6dP6Emm9fvpSjP4l+5Q2k2naHUwbwe15LBESYMgzpGPLgufD0F6ZSnZYtvfydT/7kNRiFcHv7dMGG3WllJpNVt0tN0ycMpGOqh1ehjXGNlT3Rf8Acm0uslOUq7ViS7fQmzZNntFNj6jyG3pdT1c0GCN4mPJdDT+juVSbypM5ep9b9u9xik4o6ena2Nb2ThvIOHkFQj9mHv8Ajnx9ES2faKMl8MOf2K1dxd3ibu44D+kfFd7R+m6fS/hxWfPVnE1fqd9/DfHhGKnWdEOaCycBEOA4H9ltqfTo2T9yEnGX06fqS6X1SVVftWRUo/UnaNnGL9LtN3DvKlV6i65+1qViXnsy/ZoY2x93TPK8d0UaNocw3muLXCcQSCIz4rqNRmvKOb8UH4ZvbB0tqsgVQKjd/dd5jDzCq2aKD5jwWIaqa4lydPsvbVC0YMdD/sOwdy0PJULaJ19S5XfCfQ2KhJgQAgBAJACAEAIAQFNASQwMICQQDQEggBANAarpFtcWWleEGo83abTlOpPAfoNVPRS7ZY7EN1vtxyefVaznuL3uLnOMknMldqEFFYRypScnlljZ9kfXqNp0xLnHkBqTuC1smq45YjHc8G7tbKNkJp0walXI1D3QdY/T1K533WzWPNjxHx5Lv32rSpxqWZeTU1aIfJ1nvDP912IJQSSRxJWzk228kbn2uPa0y13Ld/Q1yWBQBAg9puR9eYWmcMxkgGtJBLe0N3vBSyCnFxlymbV2Srlug8NFTaOy6dqNKk8dkV21XDhTxg8Dg3mq9lEFWopYSZYjq7N8rJPLaNoLBQBLgxuWuSm92bWMlJkKdNvfcAB7IiOZ4rZt9EB1Bf4N1KwuDOcGJonHTQfOZWc44Mk6FZzcWn91BqNLVettiyWtNq7dPLMGXqez222m4sAbaWiRoHj5w4YeC5aqnobMJ5g/2Oz94hrIcrE0c71UGCCCCQQcwRgR5rrxeVlHOk8PBmpmDIJBBEEZhGk+GaJtPJ3PRza/XtuPP1rBj94fa8d/LeuPqaPbeV0Otpr/AHFh9TdKqWQQAgEgBACAEAkBUQwMICQQDCAmEA0ABANAeY9KtpdfanEHsU3dWz+U9o83egC7Wlr2V/VnK1E90ygT2o3tMcoPxKtFc6bYxNnoXxhVrmA7MtaMcPfzG5UpL3rcPoivK9xliJgIJknzOfFXUsFdvLyYzSIyyWyaMcjJ34HesmBMF3KI/L5ackfJnInOAMuIE5zkeactcAjQtLQ97xjhcEDKMXeMmPJabZSeH0RJJRUFh89zOat7C64yd0TwJKylghJCiSbzzJ3DILG7HCMjq49nQ5+G5F5MBUcDgSBhpwVauKqzmWcvv2LtkpW7WodF/Ui/fhMRhilanXB5e7v/AOGbJQssXG1GbZlZ1F7Hj2XjDeD3h71l5ur+JYbX9DTeqLsweUv3H0ys4bWbWZ3K7ZwyvCATzBB81Ho5fC4PsW7JbpZRzdOpifE/p8FcNMGw2fbXUqjajc2mY0I1B8cVFbWpxaZtXNwllHpVnrNqMa9plrgCOa4UouLwztRluWUZFqbCQAgBACASAEBTCAkEMDQEggJBAMIBoCntm19TZ61WYLGG7+I4N/MQpKo7ppGlktsWzx0vkT/fET8F30cc2JN99MDMkEczdd+V/otZy2wbI5PbFs6LOfuEN8o/UqHScV58nNiuCxZrO6o4Mbm70GZPkpbLFCO5k9VbsltQWWyvqmKbC7wGA8TkFidsILMmbQonN4ijLWslOnhUeHv+ww4D8T8uQB5LSNtk/kWF5f8AollVXV87y/C/2U6uJF1oA3CY8zJU8Fjq8lec89FgxVaDDgWifBbqTXJoZ7HZ2U2C6BBkjmSfionJyYn1JCrecQNw8VnbhAHIjBjcIBJnVxjOAJ9wVfV2uMMR7lzQ1Kc8y7Gvsdlr2kVHCqKTG644mJDRA7RiCudbOunmfJ2oQlPiJkqMq2eq2nWIc18FtRuMgmAZ3TgQcQt4WLbvqf6djSypSbjNf7LlV3ZBjEHJdSme9KXk4N1brm4htSoX2VgOVOoI8CMvzeihitt/HcVWP3FH6HL2d0uI8PdeP+pqtMvFxtTHkPj+qM1O26E229TdSObDeb+F2Y5H/UuTrq8S3eTpaOeY7fB0iol0EAIAQAgEgBAUwgGEMDQEggJBASCAaA5P6RrZdoU6Q/4lST4ME+8jyV3QxzPPgq6uWI4PM6FTBzdWGPLCf6TPNdZclBrBtNk1b5p/apuMeR/soNS8VMraritnRbMqFzXzE33HDLHEKStYhH8in2Rtdk7QNB/WBgdLSImM4xBg7lpqKfdjjOCxpb/Zluxky7Q23Wq9kQxh9lpxPidfRaVaSEOXyyW7Wzs4jwjXDBWikA3IAc3CBzReQWmsAAGPZAHpChTZtPDZSAHWujvA+im/lRqZ3sWqZghVEggiQQQfAiCVW1VblDK7FzRWqE8PuUdn2x9kLqb2B9FxvYlzWuLQbpaWgkEiREbvEc6yEL4/F144O3CUq3wJ1Z9rqU33LtOm0NECYAxIJwvOJzRRjVH24mHJze5l+qJn5yC6unh7cEmcHU2KdrkiptCtFjcToQfcPgtZL+OiCv8AHRzNCpF7fJ/UehA5KwdTBNlpEXtMTyy+HqtjXB03Qy0llopA+20sPMSPzNH7qnrI5rf0LGleLD0VcY6okAIBIAQAgBAUggGhgkgGEBIICQQDQHIdMNr0GvNGoHOh1IuYMAQG1DiTAPfBiZ7OmauaemcluiVb7Irhnne1TSZWoOY4HraZbWutLad8ExdBAxNIiYwBbhgr9W5P4itPa48GGy2o0a4vZF2fp6H/AFcFnVr4CnqIOdTwdX0VrXqTyTjePo5wj0VhrEYlOaw8GzouzG4rMkaE2tJyBJ3DFaOSXVm6hJ9ENrCTEYk5LO5YyY2vOMFp1gqNcGvbdJE9ogCN8k8FD78Gty5JXppqW2XH5mdmy3PMMq0nOx7If2j5gKN6hLrFokjpHL5ZJ/qV2WOqXmmGuvjNuoUrur27s8EP3exz2JcmH/Cq7rz2U3X2udA3wYI9IWfvNS4bN1pbX2GHH2mkHVpEEeIKymn0eSGUHF4aG6nKymaEWgjXgoZ6euby0Wa9XbBYTJkE54rEKK4dEZt1VlnDYoGSmKpz/Smpdsr2g4l7A3xvjzUVvzxaJqI5uj+pzJqEUwR3nkBo/EYYPMjyVnodHuZnmXU6bcQ4/kZHvAA/mR8GF5N7su0dXWpPyuVWEnSLwn0+So7Y7oNfQVvE0z1orgHaBYAIBIAQAgEgKQQDCAkhgkEBIIBhASCA8q6aum31xwYByYwfPzHb0i/go5ep/EZze0KN4YCXCHtGZluJA8W3gPHmppdCOD5KlvLXNxxa9uf3gMDzbB81l4awzK4Z0HQe1yKjeN7+qZ/MHKRLMSjqY4kdhs0NBr1HC9ca0tYe72iQXOjEgfEKvqHL4Yp4z3M6eMdsptZx2LFC3WhzgGPdOjKfZHJrcFpKmmK5X9TMb75PEf2N/tF7erotrXTabzDhF5vaEzHDDxVGuL3ScPl5OjdJbYqfzcEekdkL6rC1zZuRdLg1xxOInNbaW1Qi00aa6h2STTRqrPs0h01atOmAQcXtL8DOABVieoTWIxb/AEKlekcZKU5Jfqb+x2qnWtRdTxDKN0u3kuBVKdcq6sS7s6NdkLLm49kc3abJUa97iw9p7nBwEtMmQQRnmuhXZW4pZ7HLuptVjkkzcbOoOq2Z/wDFtIuTcqPweBGcnGJ81TtlGFq9ov1QdlD95GvNjp02U31XOJqtvNawDAcSVZVs5yailx5KTorrgpWN8+CLLNReYZULXHIVALp4XhlzCy7LIcyWV9DWNVNnEZNP6le1Wd9N114II9fDepa7IzWYkFtUq3iSK7jr/dSIiOU6VtvNok+zXPrTcAsyjyi5pXyzSWnF7GjJoLvAnsMw5uP8iy+uC5Hoyxs9sufU07jcsGt7x5u8O4EXLyay4WDYgG7IGvu5fO5ZND1+yVb9Om/7bGu8wCvPTWJNHbi8pMzLQ2EgBACASAEBRBQEggJBDBIIBoBhASCA8m6WH/PVjvc78sD/AGhd3Sr+Ejk3v42a6108JGbTeHv/AH/XNTESNNtJpa17YwzbwgzA3RprgN+OOxKueTL0JtTr9ae7daR4mQfd6LanLZX1iW1Ha2S2Ppua9ji12hG7UHePFSWVxmsSRTrslW8xZuae2azpHWRvuBrJ8S0BVXpa1zglertfcjRrYh2ZBnPPVbShxhEKm1JSZd2ntF1ocHikRDYEEunE8OKgpqjSmnItaiyeoakomtY110kNPeIy3Ky5xTw2Vvam1lI2Wy9qCyh5cwkuaBEwRnvVa+n3mtrLOlu9jO5PkpbLtlRrBce5sg4AmPJTW0wb5RAr7IP4XgjadpVKhaH1HEXogkxjlgtoUQisxQnfZNYky5St7bopVgSxuLXAw9k5gTgRwKhlRLdvr6/3JK74uPt2LK7eUWKNmoPxFpaG/eaQ79PVRystjw4G8aKZPKsM3SK3Untpspm8WZv4REcd610lU03KXGSTXXVyiox5wc7VtgZ3mmN4E/2XQ2Z6HORzvSi1A2cvbpWZA1ky3/csyW1Is6ZfHj6Ghoy4lwzcYby7LeUy7mtF5Lz44NtZ2gCB3WgAeA8vgsxRHJ8lmoIYBpA0/b4+SyanpnRWvfslE/ZaW/0kganSFwtTHbazsaeWa0bZVyYEAkAIBIAQFEFASCAkEBIIBhDBIFANAeT9Kx/nan/cf6rvaX8JHJv+dlZ/daY0xG8a/OvFSkKNLtikerdd71LEbnM0xxGIkZ5jVavoTQ6lboU0X6xLhF5gHhDj5Y4c1tQ+WQ6zojrLTai07hv8cByxnwUtilse3qVaFBzW/obPZuEktA7MRB0OeOIwcByXnbNZdPRysfEoto9L/wDPoq18ao8xlFMz165IwOIyJ9xJ046eGIg9K9V+P27n1JvV/RU4e5SunYiy1uLBhBDSDOYN52B3H9Vt6xmGohKL4f8A4Z9DrjPSzjJcrP8AYuXZuD7RJ/qe79lF6q5Tvrri8f8AIz6Qo10WWNZ5f7GWq7sYOwA7v7Ze9a6ijVaRb1NtG2k1Wk10nW4YbMeziA06QYykCcdfnFdHV6yX3SNsXy8HL02gj9/nVJZSK+1aYkOb7QnDeDhhy9Ve9MtnZQpT6lH1KmFV7hBdDO6ydYwODoJEgRgRxxwWt/qFelntmR6X02zUxcomrBfZ6wY4gsqiQRMAjMY5K7VdDU174EGo0s6Hsn1RlfWcyoWk4HEKVRTiVCwa4jFR7eTJyPTK2NbTaxjRNWoOV3tA4feDRzKWNpIuaOGZNvwUNnEBpIGDOyN0xjHLDXMrUtyNocGgakgeeHz71tEifUz1sRznd6wOGqwDvOglaaVSmZ7Lw7GfaEaj7i5WvjiSZ0dHL4Wjp1QLgIBIAQCQAgKAQEggJAoCYQwMIBhASBQHkvSqoDaqpBwbaXt9wPrK72l/CRyb/wARmCjjTzgtdnu/b5xyUz6kJqdriBeGbJBGsHvN3kajLILDJY+DmujtUi1dXPZfLTHCS0+vqtKXieDbUrNefB2NpqEmnSaTF4BXeiObFHUUSBgMnMP5XOd59ledrr93RT+rkek1FntepV/RRX7EpGM7wAZ33sD/AE5ri6DRR1VMkvmR2fUNfLSXwcvlZFzsLsDPnoIPhHzC1d07ZV02L4k8E9dNdULL638Mo5NiwdpgPshvuvH3q9qfi9RivBx9N8Ppkpecg7uO4gD1n4LoesSS07Ryvs/BvVpmKx9x3B49QT+i5mr49OrR2qMP1S1ojbRJAGgHLDE+9eh0zjTp030SPM6jdfrJJdWyxYqkgjSIA9Gj3eRXmaoy1187JdF0/wC/c9Re46CmFa6to1O3qc02kd5jyRyj912/s7PNDj4ZxvX0lqU/KMVvqXqDKzT2mgeS7ceJOJ59LnBhrVHGiKsi7Anzj9PNMc4MrCeDhuklta57CT2mXnXeEAD1hRXtLH0OhpIvDLewJLWAzh2jGJJJkcdx1xK0XQmmbi/NQDRjZw3u7Ld2gcfLBZyRY4LoGPH83wPoUMHSdCLUG2i5h9YwjTMdoegOgVLXQzDPgtaSWJ48nerkHTBAJACASAEBrwgJhASCAYQEwhgYQDCGTxjabif4txzFUvHjLsV6GniK/I40/mZmoO7L/AHzJHLJb9yM1u2xAI+6PmMkRvE5LZWFtpRqPi0KKv8AGX5Mmv8AwmdrSH17PFXJfKzm19V+aN/XdHUD7VVzTxHY/wDorh+kvdpJJ/U9B60ktdFrwidpMt/lnnLB/uK5/oLxqJxX/dS59o1miEu5mpexO74ke5T6mmC9TraXX/BBpL5v0i3L6cG0aIcOXjkFxdfdOGslKL5Op6fXGWijGS4Fa3kgychv+dygV9l84xseVkswprohKVcUngrWPuvGgquHkAAu76zFQ08Ir6HE9Hm56myUuvJYtLRDvEfA++PJbeqWyhpIpd8EHo9UZ66cn2bK1mqXXDCcZgzAjwjdrxXO9N1M4L21jDO36poq7X7ks5RHaAmi+dI9Z/Rdb7Pye+yPbccD7QxX8J98Gu2Z2qFRpyj4L0dnzI803yUrKf8AL12nJrXEchI9yz/Mmby6nnPSI/XN4spzzJVTWfif95OppPwzpNjjCNM4gH3hbiRstnum7997p5EtEcm5ZZrVGsjZFgBc0aCfkZeiyRmy6N1T11Ez/wAdgzORcAc+BKh1CXtv8iSh4sR6auCdoEAkAFAJACA//9k=</t>
         </is>
       </c>
     </row>
@@ -758,77 +758,77 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DEWALD BREVIS</t>
+          <t>JITESH SHARMA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>sat20_2024_08</t>
+          <t>smat2022_135</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>191.7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>19</v>
+      </c>
+      <c r="X3" t="n">
         <v>9</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>88.90000000000001</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>55.6</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>21</v>
-      </c>
-      <c r="X3" t="n">
-        <v>16</v>
-      </c>
       <c r="Y3" t="n">
         <v>0</v>
       </c>
@@ -839,43 +839,43 @@
         <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC3" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="AD3" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AE3" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AF3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK3" t="n">
         <v>0</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>Batter</t>
+          <t>WK Keeper - Batter</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQREhUUEhIWFhUXGBgZGBgXGBYXGhYWFxoXFhcYGxoYHigiGh0lGxcaITEhJSktLi4uGB8zODYtNygtLisBCgoKDg0OGxAQGy0lICUtLS8tLS0tLS8tLS8tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCCAH/xABDEAABAwIDBQUGAwYFAgcAAAABAAIRAyEEEjEFBkFRYRMicYGRBzKhscHwI2LRFEJyguHxM1KSorKDwhUWJDVTY3P/xAAaAQEAAgMBAAAAAAAAAAAAAAAAAwQBAgUG/8QANREAAgECAwUGBQMEAwAAAAAAAAECAxEEITESQVFhgQVxkaGx8BMiMsHhFELRM1Jy8Qay0v/aAAwDAQACEQMRAD8A7iiIgCIiAIiIAiIgCIiAIiIAiwYvFMpML6jg1o1JMAKuu9oGzgSP2oGOIbUI565YQFpRVzB777PqiW4ukBr3nZf+UKeo1WvAc1wc06EEEHwIQGVERAEREAREQBERAEREAREQBERAEREAREQBERAEREAREQGKtUDQXOIDQCSSYAAuSTwC5Zvv7VAwGlgDmdJBqkCIAvkzW4jvG3rK8+23el1Nv7FT/fZmqkG8atZ0mJPkuJMquIHXnI5/KPijyMpE9tDeTFYoRXxD6t5DS4loMHQRAN/vRa7WPY0HsyZ5Sf7+ATZ2BIuGgk8uHofoprZ+7WLqOzgQ0cXT8IhQSqJalmFKT0IzDmkBLg5s62tPUE2W3sPeOtgqgOGqlonSZY78r2Gxtx16rY2tutWIJAmOFzPmVFV90sQ2mXNE2908Og/RYjUi95mdGa3H0NuNvQNoUC5zQysxxZUYDIBGjmzfK4X6XF4k2ZfLW5m8z8JiabxIe2zhwe0ag/yk+ccrfTuCxLa1NlRhlj2tc082uEj4FWCqzYREQwEREAREQBERAEREAREQBERAEREAREQBERAEREB84e2HFdptGt3IyZWg/wCbKxpnS2sKP2Fu07EMYZ0+t7+vxV99tWyWtqsr5YFRmQn87LifFpA/lWpulgX0sO2o+GtcARJ0HMqKs3bIs0EnLMlN3t2aVKM/eKudKmwCABCqVPeHDM9+sweasOB2jSqNljpHMKrHLUuTz0PWKYz/AChRGMYINlg29vXRouylryY/dEqIbvLSqENDajSTAztIEnRJRbzRmLSyZz7eOmBijkaJPeH/AHef9V9B+z1pGzcKDwp+PEx8FyDe7ZHY4ql3S7tG5oAkhxMQPSOs9V3LYWC7DDUaR1ZTY0/xADMfWVdgmopM51X6nYkERFsRBERAEREAREQBERAEREAREQBERAEREAREQBERAUr2s4VlXAEOMOD2uYP8xbJcP9GY+QVZZT7XZ1GnEktuByaT81c9/sGKlBriJ7N+bw7rgD6lVPY1Vpw9Ajg3IY/zNJlRzk0nYt0aaai+NyvYbBVCAwUcOxpcWuztGZrREPAOtp56Dmp/YOCNCoGmMrhcC0HgfMffEz+HA1soXEY+nSrDtXhsugSbkxwCrSd0si3FWbdzQxmyX56j2VMrwe73c0EEQMoHu5QZ434RfHhNl1i4F7y5oAkuGXv8YbpHkP0lsDtGlVrvbSeHRYwdDE35WUjjqwa1a7VlYza7uVreLEOZicLXDA9zGPdlIkOLHE8xxI4j6LreFrZ2NfEZmh0cpAMLl2PZnxFBgB7lLvRzrSYPk1vquq02gAAaAQPAK5Fu9nusUKyjspre34HtERblcIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIDU2lhBWpPpn94W6HUH1AXPMTsaphmubUaAHPLmlpBEwJ8LidP3l05Qe9tKaBdHuEHyNj8x6LFk35EtOo45cyp4Cva60tqbOoVanaVCGu6ujS2hstejigHefyK/KlGm8kiiHuvd4z68Ln9FSUbPM6sWnmzY2XhaNKoXMc1ziL5XTHO0wtrEPzua3mQo5uHDYJotDuYYBHgv3C1iHhx0B1PAAyStowUpqxrNqMWXjZ+wmOqduXGRlGUAAHJYT98FZFH7DrB9Bjhxk+pJUgrrSuzkyk3k9wREWDUIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAoneR7Rhqgc4DM0hskCXagDmbadFKzGq5D7Q95mPxmH7J4qUqEl2U90vfLHGRYw069T1U1CjKq2luTfgr+ZhyUWr8V6kJ+3upu77bc/vipjD7y0suoCxnBiqyw1+qrWJ2J3iCcqoXU9TqWlHJFlxW9NODBn7+7LUp1n4nvQWUxoOL/AB/RRWD3bGYalXWhgxTYB0Wraj9Izk8y17o4+mKTKTqjRUOYtYXAOc0RJA1IE3jRWZcB3pxZ7ShlkPpZy1wMEFzqfp7oPkuvbsbzUcYwBrvxWtGdpBaZ0LhOrZ4jSRMLorDy/TxrLNO9+VnbwucyrJKrKHvPP+CwIiKEBERAEREAREQBERAEREAREQBERAEREAREQBQm3d5sNgh/6iplJ0ADnE+QH9pCi9vb506WZlAdo5ph79KVM/mqaT043Egrnu194qFTI1vaOI7XNWqS+S9ha8sZmDhM90hzQJ0OptUMNOo77La16d9n0Vm3uTI5zSWvv305ll333tpYnAvbh88PdTaXn8PVxdAB7zwezIMWvrqFyM4oSWvIB0J0BBgglSVTEitULy0NgANAmwY0xqT+iito4PORBAd10gSSSToAASZ4BehwtBUKTS43a78rN3s9LXVu4pVJbcvL8nRd28QCwXkaHmDyI4KfqYVrrxK43ht6m0as0BUMd0kRFWOJYRpMwNQDrK6HufvkzGzTc3s6oEhpPvDiRN/JeWxOB+HedF7UPNLnfW3FX48WdujilO0aitLyfv3ctGGwgGgXjEmSQOCz0q8Nk2i/1XMt79/my6jQa5zbio9piebQY9f7hVaFCVd2jkt7ei+75JZu3BNqerUjSzlruW9+/ediK3t2iHVDk7wJkEcm2B8CZ9Fm3F2pVpYqlV7TK1pOYnNGSHZsxg2i9gdFC1K7cSAKRIIs5pEPyXMtv3hfhcRcRdS2yQAYEBuWrlEyT+E+5XsYQpvDOnSd4xi11s9eueerzPPylJ1Nqazbv5ncdjb40qpc176YymM7ajS0i0EiZaDPvHu8JBsrO2s0mA4E8pE+i+cNg7Xfh3Ohz2tLtabg1zSO7IkFrrfuuEHpqpGptpvbAYWiKdSpDW1WuNBwIOZzy1riBJN25jbiuTX7NnTlJ/tWd+Xl18k99iFdSS4n0EioOxN9XUyKePaaXdaW1HgNde34jGudluPf7oPIXi80arXtDmuDmkSCCCCOYI1XPnTlB5+O59SZST0MqIi0MhERAEREAREQBERAEREAREQEbtzbNLB0jVrOgaAC7nO4NaOJXH95d7q+Mc4Fxp0dBTa4gR+YiC4/DorLvhgH4upiKr3k08PSmi1lwXkZyDI1yhpMa52AG0qk7y7Pbh676LCXZMocTF3lrXPiAIAJI8uK9F2bhaKV5ZztfTTTzzWfhpnz8TVnuyXr7sWHaFSgNksY2O0eQ7gCXggO7o4ANI8hxMmiPbEefzBPyWagdRx+MfWOfhposWIb738J+II+a6GHw3wIySd7ycvHd0svxoVqlXbkm1ayS9+Jiw9mzEnvH3osWhhg8DckHmAsVbDuqDKe6wxmDTmc+LjM6BDZAOUDXUmBG3SbECJt5Xv9UNZwOseFlJOnCTvLwvlk75rfq/aQjOaWR+YXABvut+Hosj8OW1G1NHNIId7sHryX5mLtSfMrbDgApU8tMiN665k5vZtI1cPTptdl7UBz8s3GkAgaZgb9FTxhGMblDbcVOYuuxzaeQGQ2HSIl2Z5Jt0IUdVbcePkquCw0MPSUIK2b782/tbokWMTXlWqOUnw7sl/NyNrYJjrlonWRYg9CNFkoBwP+I4j80GeHvEZj6qxYDdXFV25qdBxbrmdDGxzDnkAjwlZqu5WMAllIPA17OpSeR5NdPoFJN4fa2pON13X7r69GaL4lrK9upVQbnxPzKz0GDtKZe0ubmEjSWSC8dJDYnqvQo5SQ8EEF4IMggiAQQdDPArI8HzIgDSJ94yNLQLX101G1r5i/Al97N5BjK00qWSmyWgklxkmTfidLAwOE3UvuPvXUwpLXS6gSMwgAgmJczrbQ6/FVKlRDQPC3QdANAveFxIzgEdw6umBHQ/XSyqYnCKODdGktF8q7s/fNlzAVacsZB1/pbtJ6aq178nZvkup9I0awe0OaZBAIPQrKq7ujtOlWp5aT3u7MMH4gh4GWADFie7cixMqxLyad1c6FWnKlNwkmmuOoREQjCIiAIiIAiIgCIiAKO25WLKDyBJsIsJbIza/llSKqftJxxo4PumHPe1oI4WLj8GkealoQc6sYrezWctmLZVt4dsVcOwVGOBD31WVGkdxzrDOQHd5xDRlc05QLaqrbc227GOa+pSpNcJksYWZ5gy6Scxt81FFxqVDUc8uqON3OOYuP5p1+Y4QtzF0XgAmmQb6ggmNYkDMP14L19DCxpJXtfPP7c7aabtxxaldzdlpwI+q3rBFweR/T5iVu4XZL6tJ1b3WDK11nmXEyWhwaWyCQO8RNom606hDhI++nw+HMKT2fjHNwbhnhmaCM0ZnB1F4ywbuEEyBYTzVftWvUo0Nqm7O6XHW/mdHsbD06+LjCr9Outt63m/T3QLQ7O9gLBmcS4tj/AAzEkQZ7VpsTx4wDkxGxaLDUD6jQGsLpLQMzxUyBrQHOMRLgdSLwBdbG09r4DMf8StE5ZdUyx3svee4OvLSRA0t1idr7Wo1SOypdm1oAgGc0ADMbEzA6zrqST51x7TqrJzt3uP8A5PVUanZUGtpU09/yQbXdnOXFWs9eWc2zYmDYcv7Q11yJa5jWi4AJJJERJtOkWMTWt6TTbk7JxLQwOdLge85gJbZo90mPELSdi/yu4/vD9FqbQrZh7p0Av1c0K5gsLjYV1Uq32VtXvNP9rt+5tlTtHG4CphJ0qM7yezZfDcVlJN2+SKWV8unI9h5sOUD4BXr2a7No1m1Kj2ipVY7usdcD3YMQZJObUGMkwqF+8RyI+R/RWPdzadKhSMvLaj9coeHBhIAh7btAs4kGbxBXYxcZTouMW75ad930auuvA8xRS2s+fD78Nd+V8jplPG9sXGrTe5zSQKeU928tEaZojrYLzs7DMbUfiCWA90ZWQ6RlJcCBMniIE90jQyYJm+lPK1oxJzSQ4/iBpZoA0OZDTHemdRGht+De2ke+RQMuFoE5IydmJDXNsZzm0C8A284uzpQqSnaV3dXd1ZO2S+WOWWWrSvmjpRq7Ssmt2St55v8A2Uze0Pq4l1U0KlJjpDc7XNkNDGam0mOBtpeJUTRdLnDqRJ4NaSPOTJ8/W37145pZTpgCXZTLc4aYu73rOE8rXF+dRwFhJuXEu9TIt4R4cV6fBvapxytuXcrJeRycRFQlsp3/AD+LGas0ReY5cT4/cLRrAk8hyGvr+g81JPoO1H6mfvgpzd3CUWYarXxOHYQyozI+q9wBu3MwMkB5DS52X96CDlsTPWqKnHas3yXMipx2pWJz2OVialUH/wCMf8hH1XV1Vd0sLQk1qLWNNSlTLhTGVsPGcWgAOFweMZZVqXjsVKM6rlGNr5tc9/vrkduMptJTd7K1+S08NOm/UIiKuZCIiAIiIAiIgCIiAKsb+7O/acO2lkLiatOMrg1wE5XOBIIENceB8CrOqH7UMaabKPZvcyoC5wLY90ZbebsvoVawUZSrxUXZ3Iq8lGm29CH2K1mCf2Lc9CtWw7g5tQ0y/O1rjSqtIJFznaRMEtEBRu9u1hWfRYapqmlTa19QAtaapkvLcwEEgNnyVaGEDtQCZnzOvh4rLiQ5sHMb8ZBuLar1dLBbNRVG7u3D75vTK1/E408UpR+Gsl3mhjYL3OHSSBqYAkjn14+kV+s4y7xdH+lp/VWfDtALs2aI0B15+Ph4qt7UIFXu+6WiP9wKkrKyNqL+axu0HZhI6LaNEhpJIWps7M2mwAAl8GIJN/d8eFlIv2VWpjPVoVmgmxfTe0GfzOEeS0TVknqyRt9PfgeG05EhriBqQJj9FhxFBxYXBrsoyjNlMDvDjouqbiVi3ZOJeREHEO15Um+miqdTaeIZsp9B+HeKL6jOzrCco/Ea9zTOslroIOphVliJSlKKjpJR143z71wJNiyTvqrlYZUyzHqeg/qvwO16QPJoj5yrJhNxcVVoMrMaHMeA4Na4Zi0mdDHAAwJUPTwg0LTM6GZmdI5zwVmnUjVvsNO3Mjk9j6kzTc5Yw4zp6q1f+T8XlzjCPiJ/czf6S7NPlKqO06xBLSHNIMEOBBBGoINx4LVVKf7ZJ24O4tJ5Wt3mOtX75Ddey+MuU3g6UNAOvyA4T96qu4QF1YNAnNlaBzMm3xXV9h7GpsAdUh7/APa3wH16Kriu1aWFW1O7b0S9W9y8+WTtNRwFSu7QyS1b9/jiyr9i585WmBrlBPWLfd1u7O2xUw7Wsfh6VdrSXNp1aYJYXQTlcRIMgHQ6cFeS4REC3RRG0aLHasafILjS/wCRxqfLOjeP+Wf/AFX270X49iyjnGpZ/wCP5v6lj9nmPNenUeQ1uZxcWAk5C59R0CWjuwRHmOEm4Lne41E0a2vcqBzRrZwhwB6910eJ5LoiqYicJ1HOno81fVcmZhGcFsz1XDQIiKE2CIiAIiIAiIgCIiALlu9lE4nEue8xSaezYBq7syQ49BnzeK6kud72MyVWtGgzfFxP1R1Z04uUHZ21Wvv/AFo2nLRpwqTSmrrnoa2DwdNoswD1v481unDU3CHMDh+a/wA1pUavBZHYsBc74kr3vn1Op8ONrWNDaewKLriWn8sAegHxXK96sL2eKbTHIz4SDIPKF1PH42Gk8FzavTdiMbnfTc5rgRTaA89rlIBEU2l0AnlyXWwHaNW+xUm3Hg3fRp5XzXpa5zsZg6aW3CNny+/vU6H7JmUG0q1X8Ptw7I3O4CG5QRHIOcSCR/lCzYjb+06Lajcbgm1abwQYALWg2cD2ZdLNPeiOaomJ2S/OKBb+IHNdlLGAhpaC3iDdpEibNeScvdB6Ls018OymBXe8M90VC13lmygkDQX08lYrY+kqrlKKd7a7rcGrW99alLCVJw+V2NfduqKewaxnUVBPV5az6qTrYRlTZ2zqL/drVcNI5gh1dw82tKhzgnnCPwlm03vLzAuDn7SPUC3JbeOfUqU6FMFrRh3NcyxuWU3UhNx+68rFTtGlKTcW18zlpyy6kkMDVSzS0tqQGyN/qlHEVHvc+pQdny0pADAT3MgNmgC0CBBU7uR2WO2hicYKZa1gYWNdBy1KjYc+3GWPP86iNjbCZQc41aTK8iGh8gNvJMXk6fZUxso1MM6saOVgqlpyhpIYG5oAk/mU2I7Qwdpqk3dpK9nZq6+2V7ZrxIqeCxN1tJa8T1tbE7YGML6dJ37O18NYHUXNdSBiSJzS4X5gnoq57X9nA4mk9gl9QZXBomSwgBx65TH8oVnp03XLqtV0k+9UqOHWATAHQL3RwI0iTb+qpLtRRkpQgsk1wv365rUtLs9tPal9zlux9hVm4hlQ0nw103tbJAsY4roNKpUEACPH9ApoUQLwvDWN46qjjMTPEz25JLu77/cu4elCjHZi2+80xUcBcrRx1ay3sUOSh6rS54b1VVRu7FhvK5cN0aZc2nGoqSegDXT8481d1Cbs4QMYSPAfM/fRTa6drZHHqS2pNhERDQIiIAiIgCIiAIiIAqDvwIrN6/f1V+VH9oFPvU3dSPUCPkVpU+hk2H/qIr9N8raGGn0WCjROq2RWIiPC/wB/cKgonVcjSxmzhB6iPXoq/teji6VLJgXmkYa1+UgF7RmDYcRLSJNwRqVby+9zK/HMa7r/AFErKbi7o1laatIoW4m2DhX1W41tQFxDhUfmdM+93zPGDreSr0zbVGpdrgRzn9VpvoDiOh8LwoLFbvAOzUszHHiy15m7dCsurtPNGI0dlZMtwxLXCx+72+C8msJMHj8lVG4jF0ffaKjQZlndd5tcY9CpXAbYo1LaHiCCCD1BuPNZVnoZd1qSxqtWQPB+ajHAG7XdR52QF45E8BKzsmCazheTXvZRn7Q4cFkbV8/v+6zsmpJirp9/eq85QVDt2lDoKzVNoDhE8FjZNkjaxNMNGij9nszVwdY0HMmwHqsNfHEi50Uv7PsL2tU1CLM738xkN+RPkpKUPmvwI689mBf8JQ7NjW8hfqdSfVbCIrRywiIgCIiAIiIAiIgCIiAKpe0Gn+Ex/I/1HwzK2qJ3m2ecRhqlNol0S3+IXjzuPNORvTlsyTKLszEgWK28S5vBVhmINMQZBFiDYgjUEcCg2mqewzqNq5J1fpdeM5mxWg3G51jdUdwK12WZuiW7U6E+PVH4kHX1UIarwvOap/crGyNonjihaY0utHaGEo1ozsuDZzTlc0dHC4UaKFTi7+y2RRaB36h6xxCKI2iMxNLEYc/hv7VnI914E8xY+iz4Xb5PvBzTycProsmN7IQQ42Jm50UPjdtYdlhUk8hLvkrNOMpO1rkUpKOZYBtWfsLy7abhzVPrbxMm1J56w0fMz6rKzeejb8Or8Po5Wf0dX+xkP6mn/cizvx4OoWOo8HvNcRAJN7Aak+Cq2J3kabU6Qnm7vR4D+qicbXqVKb81RxltxJywCHGwsLNNuqnp9mTlFyeVvfu5BU7QgnZZ+h1/Zm6OKr5SQKbHAEPcQe6byGgzpzhdI2LslmFpCnT8S46udzK3qbAAANAAB4DRe1TjFR0MVKsp6hERbEQREQBERAEREAREQBERAEREBpYnZVCq7NUoU3u5uY1x9SFE43czCVL9nkP/ANZLf9t2j0VjWDFuIpvLdQ10eMGEMqTWjPnLG7eazEVabGOLG1XsacwzENeWtJGWJIAWXF7cZTMOz+Qb+qhdgtNSo0uvkAcf5WuLyfPKtParsz3eQ+q70ezqEqabjZ971Krx1aM7Xy5onDvRT1Af6Nv8VrDfMGQ1jvMgfKVB08G43ANuimhsQAglpa46SIzDl4reHY1J2fq9TEu05rL0PL9vYmpAY1g5S79YX63C4uqHF1UsIiGgRPmp3CYBoEOFuUa+KyDCGmSaJ8WG48jwPRXodmYWH7fH3fzKc+0a0t5D0N2g8TVe5083E/ArZqbHY0d1nTS6lMNWkmRldOh4+C2KiuRhGGUUl0RSnUnN/M2ynYjZsE2UbUwEa2V4q0p1iVo1MCCLwsTowluNo1ZR3lQOHhbFItBAeJYSA4AwSwmHgHh3ZupjE4GOCja1ETBaXdLx5qvKhbqSRrXeZ9L7n13vwOFdUMvNGnmJ1ccoGYjgTqRwJU0qt7Ng7/w+hmJNiRJmA4l2UHkCSAOAAHBWlePlHZk48G14HcWeYREWpkIiIAiIgCIiAIiIAiIgCIiALHX913gfkiIYZ8x7r6V//wA6nzpqNxPvn+Ir8Revo/x6I5VX6n19WZTofAqy0f8ACb/J9ERXN6Ks/pJKomD9wfwn5Iiy/pIkYsb7q1x9ERZ3BGVqxVPv1X4iyYNatoVEu1X4i1Zq9TtXsZ/9u/69b/kr2iLxWJ/rT736npKX0R7l6BERQEgREQBERAEREB//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUSExIVFRUVGBUVFxcWGBcWGBUYFxcXFxUWFxcYHSggGBolHhcXITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OGxAQGi0lICUtLS0tLS0tLS0tLS0tLS0tLS0tLy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOwA1gMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAABAAIEBQYDB//EAEAQAAIBAgQCCAQDBgUDBQAAAAECAAMRBBIhMQVBBhMiUWFxkaFSgbHBFDJCByMzYtHwFYKSwuEkcqJDstLi8f/EABoBAAIDAQEAAAAAAAAAAAAAAAABAgMEBQb/xAA2EQACAQIEAwUGBgMAAwAAAAAAAQIDEQQSITEFQVETImFxgRQykbHB8BUzQqHR4SNS8QZDYv/aAAwDAQACEQMRAD8Ay85Z7wUkADAAQBigRAYACADYERQAbGAoAAxiBAQDAGCBETQAbAAGBEEAEZITGwEKADYCYDAQICY0wEKNAXEoOgKSABgAIAKAgGAgQAbATFAQ0xoBQAi4nHomhNz3DWXwoykYK/EKNJ2vd9EQzxpeSH1Es9lfUxvjEf8AR/E60uK023uvnt6yEsPNeJfT4pRnpK68yYjgi4II8JS01ubozjNXi7oJiJDYAAwECAhGNAxsZEUAGwEwNAQICYDAQI0BcSg6ApIBGADYAKAgGAgQAaYCYoCGOwGp2jSbdkRnOME5SehSY7iZbsroPr/xOhSoKOr3PN4ziE63dhpH5ldLzmjbQuOwecLhYkYfEFDcSEoqSsy2jWnRlmgy6wuKDg945TDUpZD0ODxixCatZo7So2gMBAgIUaBgMZEEABATGmAgQEwWvARPw+A0u/pC5W59CRKTqCkgEYANgAoCAYCBABpgJigIp+MVyzdWvz8TyE34eGVZmef4piXKfYrZb+Zzq8ArLlujdoX2O0t7RHM7Njk4DW5qR5yLrRJKhIbT4LVY6KfM6ROqkNUZM7rwB+Yi7ZciSoMs8D0MeoN7X9ou2H2HUpeI4Gpg65puLMtr9xB+st0miFOcqNRSjyLMG+s5zVnY9VGSlFSXMMQxsBCjQMbGRFAAGAmC0BEmhw9m37I8d/SBCVRLYsKOGVNhr384FLbe4VzN+Rc1tzew9eZk1T/20KnPocTMx3BRoBRgNgAoCEYCGwADQEwQEc+hmB6/H0sw7JqEkeCjb1tOk+7Cx5Cc3UquT5s9r6R4VNFygWAtpytM8y6kzGPhheUWNJzbD2iGxowgjEXHC7Wyje4k4lcii/bXwfKaFUblWQnvtYr9WmqnozFUd0YvhtBmpqQL7j0MzV132d7h9VOgk+WhIOGf4T6So2Zl1GdQ3wn0MAuuofwz/A3oYwcl1HLgah/QfpGQc4rmdU4U53sIXIuoiQnCR+pifLSK5F1HyJKYdU2AHj/zCzK3LqN62+igsfDYeZk1TfPQrckhPRAGaqwt8I2/qZO8Y7CUZTZFxHFDtTGUD+9uUqc7myGGS94RlJvBGgFGA2ACgIUBDYABoAwQIknoVX6rEqf1DMR87TpS2PGw3PYuPIXpBzYZRfXTlM89jTCyZkMgOzD1lNn0NF11CMOef1kbMldEbElVF2dQPEgSUYtkZSSHcD41h1rqGqi199x6iWqnLcqlUi1oWv7XaIajSfdNRccri417iJfHRmRrQ844H2aZFmIzHUAkcpXWhdnRwMrU2vEsvxC87jzBH2lPZyNmZBGKT4vrGqcugZkPGMT4vY/0i7OXQMyEcWDsGPkph2bDOgdY52pn5kCPs0t2LN4ANKodyqD19zpGoxRG8mcKj0V/MxqHzv7DSJ1UtEWRoTkR6/FTsgCj3/oJBzbNMMLFe8V9RydSST4yDZoUVHRDIhssTIloI0AowAYACAmKAhsAEYABRc2AuToANz4CNEG7K526GUb8QVGGuYqQfX7TozfcPIQvn1Nd+0PiLsRSNRlRdMo/UfHvlMZlsoc+RgqFEVGIQuWQEnW5Wxsbjca+Etea1yCyt2RqOB13KkEkja57ztrMs9GaqaZU4/BtVrFCCWBItubjewOnzMtg2U1EuZC4coa5WmxCnU5drX5r4AnUbScrrmQg4vkeh8ezPwdiRopTL6gff3kKcrvUdRWTRhuF061CiGsLNZrG+a2wYjkDIVp66HS4bSi4uMt2SBxh/hX3lOdnU9miL/GD8A9TH2jF7IuoDxhvgHqYs7F7Iuox+LVOQUesM7H7LE4vxCof1egAicmTWHguRGdydyT5mK5YoqOyOZiAUAAYACAixMiWgjQCjABgAICYoCGwARgB24d/EX5/Qxrcoru1Nmto4Sn/AIjQZWGZWRGGt2yrZjr/ADX9pphLdHnakHpI1XSbhtJanW5ASQbE6jUWMhJ5XdDprNGzMO3CCWYg2zaE94G1++0O1drE3TW5q04LTw1LD0981RWZvi0APtYSMltcIPR2IvTjgNPr+tQ5S2pXkT3+Bk3Kz0K4RzR1KvhWHFNjYDtAg6DUHf1kHNssUEkarj2FH+FunM5SAO/OCBLoaWM81mkzB8TxAfDAgWyEpr3NZlHyIb/VKJ7HVwatVSM3KkdobGAoAK0CLdjt+Dfu9xGU+0Q6i/Bv3e4gHbwfM50sMzagQsN1Ix3OaoSbc9oEm0ldnSphWBAI1O2ohYgqsXqmNrYV0F2H3+kdhRrQZLMrNII0AowAYACAmKAgQABgDHYZ7MCdufkdD7RornHNFo1WAqlajVilxnUE/AxYMw8jY2MujucCrojacRrdYoB2AJil4kIabGVxzhRz3F7b2vqR42kFuXPY7Y/pMKoFqfVpSuqC9zl+I6+HtLGmymDjG92RMd0lGLKv1eVwxBsbhlsNfO/3hJWeoU2tkyfgwCfOV8yyRK49xBuqFNTrdQvhYg7fKWrYpe6RiuMp1QNO97sSD8QB1e3K5Fh5GUyfI6+BpvM5lNII6YDGAICFATLHG3yjLfflfu8JJmGjbM8wuH5tc1+Vr3+8Ar5brKN4Z+rzjQV+RAX83+b7yPM1P3PQsOJ7p5/cRsyUfdZMrVFGjEa9/wDfjJIojFvYrjKTsAggFJAAwAEAFAiAwABgA2AmX3BeNhVNGqFysMoqEEld8twNxqddxJxlZo5+KwimnKO/Q02F4kpUUye0Ba217c5dOJx6crmS6TYhxVNMPkFhc+YB05//AJJU4KwTk5OyKhMFSuSWe5Outr+FrGWZmNUFzuGpTVNabOp+ZH0i33FOnl1Rq+B48igajfmF1v3+Pnr7SqUNdAjN21GYviJX99fUEEeoFvSN92LHRg6tVRRneI4s1ahe1r2AG9gBYTI2empU+zgokaCLAGMAQEKAixxlQqoI01+0kzBRgpTaZE/GP8XsIjT2EFsiRwo/m+UaZTiVtY5LgHzXsN77+MCTrxy2O/FN08/uIyqhsxnG/wBPz+0Ljw2jYJUdAbBAKSABgAIAKAgGAgQAbATFARa0qzFFbUfpJtzX72Kn5zXTeaJ5zGUuyrPo9UNGOUVSzgE6WJ8AANeUk10KFJXOPEekKq35SxJ7xp7SSi2W+020sdaPFVdblLAm+uuvhIu60uJ1c3I5UsRZGAFhmvb+/GOxQ2Mx2IJCrYgWDa877e2vzEpr6RsdPhUM1RzfJfMhzKd5tCjQAMYAgIUBCJ8YxJajYh+grwItXFnPefWMVkAse+AWGsx74BboWMgXMbBCFJAIwAbABQEAwECADTATFARo+j+HFXDV6bA6MjjwJUjT/TLqcnHY5XEoKTT8DM8SDUiQ4B5BgND5d01xalscSScXqU9XG3J8d76/WTykcxIwvEyNzp7ekTgGdlzwfCviHBa4p3vzu/8Ax4yM5ZVoWQi5bmq43haYqIpAuaYNtNl7Og8JkkrnWwryxaiQfwSfCJHKjT2s+pWcYpKpWwA3kWrGnDzcr3H8KwgILML32vCKuQxFV3sid+DT4R6CSyozurPqVHFCobKoAtqbSDNeHu43ZN4fhlNMEqCfKSirmerOSm0mSThE+EegksquVdpLqUNUfvCLaZtvnKzem+zv4F0uCS35RLMqOe6k+oKmAQggKI8qBVZrmZ+vSKnKZUzownnjdE6QNDGwEKSAUAGwAUBCMBDYAAwEzqlJhTatkzIhynuzMCfUAE/ISyEU3qVyfJbrX0ubLovSTLVsFFxTvlJJHZvZr87k/IiSZl4hCCy5fH6EHi3DwSdLg7iEZtHJlBMymM6Ni+lx5S9Vih0EOwPAArAkX8/6QlVuCopGu4XSsw7pTKVy+MbC6asEFOoMvWWCpff84DAd+hhHXc6eFyOlKP6rr9xYnDtTIVtCVRv9ShvvFchJJNpdX+zsUvF6eZ0Uc7yuS1NNCWVNlhSp5QB3SaVjM3d3BXqhVJPKDYRjmlYzLvcknnrKjqKKirIveF/wxLInNre+yWZIqM3V/in/ALvvKTor8r0NCuw8pec1hMYiFjsGHsecg4ltOs4ECUHYY0wEKSQCgA2ACgIRgINGkzsFRSzHZVBJ9BHuKUlFXbsi+w3Q+uVz1CtNL236xr92VL2PmRbnHlZjljqd8sdWaDoJw9Kq18K18tVcy5viQm1/Ehj8gZbTSehLiObDRp1lunZ+T+mhkcP1nDcZUotfI5tr3g7E9+8sfej5GDFU7SVWLvGWq/gvmxQfUTPYoYwqIXEN6u/IRgH8UqecW4Fbwmg/EeI0lP5KZ+Sjc/O0vSssvU0Ye1NSxD/StPPka/pbVH4piuUjsoL/AJcoAUg2tpe+srmrPQ2YLDKeFWffV/HU4YzoixPW0aiVUAOqknkDoRcHSJowRxatlasynq0GAuRp38vWCaexapJlJxqvsg8zISepsw0L6lTImwv+F/wxLInMre+yUZIqM5U/i/5vvKjox/K9DRLsJac1nHF1MozdxgOKu7D1a4uI0Rd0U0zHdYDAQJJAKADYASsBw2tXuKVJ3tuQOyv/AHMeyvzIklFvYrqVYU/fdvvpuTlp4agGLg4ioo1QNkpKbgfmHaqEX5WHnJRiuZCUK84txeVfv/C+ZMw/Sii6UqYoFMlyyoFRKjH9VQrqwA5W5nUSbjZGCOAqVJ9+f1+BVdIeNVK+a7HKBZQNFA/lXYD377xRWp1o0KdGFqa9eb9S34ZxRqZSqrMp7L2sN9LjfzETeV3L50FXpuMktUT/ANp2DGKWnjaQOUqA19CDewJ8bjL5gd8kp3kcPC0WoywlTdXt89PmZ7hGKzrY6Ouh8fGKSsYpQlCTjLdF4lLSVBYdlgBnONVigsPzNe3gOZlsEEKbqSUUab9nHEcPhqFeoKidcVyqmZS4Ogzd+pPK/wCWTzOLuzdiqLrSp4eC7qd39+XzImMVjdj3G3PRtBK2dyGVd1FRhcc+EqpUpMUP6rGwYdzDZh4GNalOIw9OpHLNXRqMN03Sq5p1cKB2TnqU2BLbdrq3UqfIn5wtbU5H4ZJSapzvbWz+V0RamCwuKFqSpVqtcDq8+GqC2x6uqSlQd+Tb5yLiy2DlSd5twj495eOq29TKcT4TVw7ZailT3MCp9D9RI5Za6bG3NDKmpJp6Jp8+hY8M/hiSic2t77JRkiozjfxf8w+sqOjH8r0NENhLTmsicU/hmKWxZR99EHhmNyjK3yiiy6vRd7xGSk6YDAiCSQCgB3weFzn+Ub/0jSuThDM7F9j+kNXImHOUUgCwVVCDe2oUAG3L3vLU20RjgqNKr2kVr46/AzLIbVPNAL+OYn6CPQnZ6nGlRy68zHe4owtqK+Y25Df+kWxK7bsWWCrlWtffXyP9/QSLRetyRxTjlaspw6uVw+YEgaGoRbc8l02+cnexgeEhOr2jWq+/tnDh9IU7FBsLWPd3XkG+pZXwFOqu7o1z/kvsPiQw09OYkDhVaU6Usk1YGIxYXQanu7vOCROhhp1pWj8ehS1dSWY/3/Twkzv0MNChG0f+kSrRVmvaxHPnHcnKCk7lkMU2QKxBIO/MjkDE3ccYW1uVnE6tyBHErqyuxmDfJTqP+prIPqZJ7kI2UWzuwzNSpDQIM7HutqYvEb/TH4mgr9Inq0DTqBatNWATrBmcG9rI+4057jYeM6dadN3izDV4Xhq0nK1r9HZX6+aObYRaYUI1we8WKsN1Pfy1535bSM7N3irJ8jFOnUpvLUd316rk/Pr4nNtpEgZw/wAX/MPrKTpR/L9DRjaXHMZE4n/DMjLYnR99GdMijqFhKy4BgRBGgCovoOckBe5BSy0+8HXvYb/X2llrGqikkQeIi4VvhNj5H/mCJzWtyK2inzX2B/rGQa3IWrbctCeQkijVux2Qog3F4ty6McvIl4LhteqC9OhVcfElN2HyIFo1CT2RTLE0oO05JPxaLjC9FMXUA/cFL6A1CtO/hZiCToeUapTfIoqcTwsN538tf6AeClKNSsMRQqCmyqwpP1hUsbWJAsPKOdFxV2KhxWnVqqnFPXr/ANK8OdwxB8B95SdGrTjVjlnqJnt/XmYwhTjSjlitCK1QmAmy5HDKWVGK4hiyK5NNVYC9zrcaaKTvsD3SSjocv2qs5SScVaTWt/D+SS/D6K9nJUN7jOzqrLa+oQ2BFxY3PpCyILE1n3sy8km0/N6vysipxXAGLhUrUSSQAGYoxzbDKR9CY4om8X3c8oS06ar5/Qq6q5bId1qOD3XXT7GBrTvGLX3oMoMTe2jVDa/8o/5uf8sAjd+paYMgkG3ZTs0x3nm0hc0xSfkdOCpUrVzTXtM2c6kDRddLnXyE9HWo0/Y1HwVvP+zwU8VP2yU5Pm0/K/0JhnnTsGbP8X/MPrKeZ0o/l+hoxtLuRzGROJ/w2kZbE6PvozsgdQsJAuAYEQRoC36L8OevXCoLlQW8O4XPmfaTgrspr14UY5pvQ0+L6G4mrTDoEN7OnaKnbS4YAi47++EqkYuzKo8ZwzXP4GUe4LI6lSLo6ncEaEHxkvI69OpGpFST0ZFp09GB/SV+eh19owtuje8G4k9CnVAVqnUYDD1VojZnf8RUJIHMgID5To0l3EeKx7TxE7f7MnjCNTN/xFWpVsruEp0TRBYMbdXYFUGX4g1mXtEm8nZGXPJ7kWjgQcVjwc7Gnh6DUw7u5ptUp18+W5Nr2Gg00gJvRHfh+Ip1MJwoM4YkKza3OVcHWWq7HcAFrE9574wejl98yv4nU6rDYjBJUWvQpUMO1KqLFqamsqpQqMvZawF1Ohtvfc0V/cZu4ZrioPz+TMQhMwHskNJvvAd7jLaHwjImx/xM0qaUFp5jVo0r3NhlKVEttfdgb+FucnmtFffU89DDqpKVWTtaT+N0WeF4/WJYgU2AGYgM4C5nqNozLuS4G1uwIu16lE8HTVt18Oi/j9yGOL0KzBOranU6yjlDKrHMKtLN+8tmGiudbb2BtpJxkmyc8LVpwclJOOWWza5Pl5swXFRZ38Krn3aVxO1H8uPp8gU6fb05KQP9IP8AuML6F0VeROwuh8tP/l73iL1uS+h9FDxROsdKdJFd8zkKrFxlKXbnZm9J3qVd1MMktWtP7/Y8JxXCujipPlJ3Xrv+5a9JnopVzU2XJUUOLEWBOjgeRB08RORiYOnNqSNuCbq0tOWhjHqDrM3LNe/heYztJPs7eBaHi1Md/pJ5zH7NNkfF8SV1KgHWJyuThQlGSbKqRNZYSJeAwIsEaA3H7OsMctVwzBnPVqECljlQliCxAUWfc6bc7Xup6Js4PGZ96EPN/fwNaeldNKDlVrVTSDseygbKqLUU2B/KQwAKg6qQdQZTWoSlJapXONF2MN0wxS13p1xTVC62ZkfrKdWwQpUR7DMLNlJIButuUnCOVWv9LHqeBTk6Uk9k9PUoQt8w5kD2J/r7yR3Gvkeg9F8BSxFOnWbMjmn1TulVkuaDAUgVBAN0cn5Hvm+jO8EeN4nSdPEySXj8d/3LlV6ladTMlF36sVEaooWnTAynLnvcgAbaSeZLdnPjTnPSMW/JNnFMbhkxFWocVQAdKYLipT6xymbRrC2UA6eZhnj1LvY8Q1pTl8GQcBiuHUQzLUwyVXb941LMA657kEqupKn1ke1h1Lfw/Fv/ANbIHSXjWD/D1aWHqA51QBFRgAwqBmcsQBsLc9h86qtWLi0jdw7h2JhiIznGyV+a6GD75kPTi5wBBA1t3iA2X3Dq5qKjprVpKaZXcsg2dQdyNiPHyBlbMrHFrU1SlKMvck7p9H0fn1HLVFNlqUntnZ1cE2tuBmN97HfSxldr6MeSU4uFRXsk1/R1Z6gYYnEkfuwRTGmaqwvltbdQTfN4DcSxd0hJQnF0KH6ve6RXP1fQyWMBKEnckk+ZvBbnUcUoWR1otZ2P8q282AA+0XItjpJs6HSBLkKhhg9hchr5vbY+3qZqwmKeHnm5czn8QwEcZSy3s1qvPxFxeiQikjYkeo/+s18UqU60IVIO/LxOJwqhWw1WdKorbPwfkyonFO6AxkXoOFFvhPoYEc8eoupb4T6QFnj1JsgaRQExsBHo3RvqMNhEFZmLVUZyqFlZRUsV1WxBIVARmAsNjLnfJZHCxOEr4vENwWi0u9tNyScbgKgDpiGo1lAXMVswUVeuyG65cubl3Ei8zylWt3lf/ljPLhOJi33b+VjG8co06dVkpOHS5clcuTNUOdwiroq6gADuPMy+MnJXktT0HCaDo0LSVm2yvDWdfEMPPYxnTb1RywhzG3g31jZCL1O5X1iJ2GMsCNhjCMBKIgVgke8AsPUfeBJbCddjALAsQ1wSDe4I0IPeCIEJRUlZrQtKfG6mhK02cbVCilx89vnaSzMxPh9LZOSj/qm7ETE4hqhLOxZjzJ9vASJqp0oU45YKyIONHZ+YkluE1oMqfmI/7f8AxVbe7CLkN+8196JHetpp/fh/fdeBbI7YE2Pnv9h584ArIseLqeoZWBBtexGumt4PYzTyvVMyUrKLHVcWw2PsIFUqUWOGPbnYwIdhEeMd3j0MZU8O+THys6IoCYEQkgDUkgDxJ0AgJu2p6JheiWKqAZUCrbL+8OQi2xta9vlNfZyZllxXC0e7e/lqV/EuguMQGoER7fmCPc6cwGAJPhDspInDjWEnLdrzX8NmYq0GU5WUq3cwK+x9jK2jqRlGWsXfy1ORfbwIPr2fvAb5Efh72qMO4kfSSa0RTTfeZrMF0bqPTWqXoUlfVTWqBCw+ICxNpOFCcldGOvxbD0ZuDu2t7L+0LivR1qNJawrUaqM3V3pMXGaxNr2sdjFUpShuSwnEqeJm4RTVlfU1PB+i9KjYVKIrVAFaqWDOtPNqESmoOZrcyP6SyNNLQ5GJ4hUraxlljqopWTdubb5Ge6YdHxSc16RTqKjEKFuOrYDtIV5ahvLawtK6sMrvyOlwzGOrHsql88VrfmuvyM2o/rKjrDKWw8oCWiOwWDJCyRXELJGhWOVTSBBkOvV0IPn7yRCb0FR1dm7yP/FRf3P/AIwYU1eTk/uy/ke7Xud/DvJ2H9+METbuz0HA0sNgFoV7Z+uFlrOWIzlc/YWmhyX1XUhtNOc2UsKqqdm/Gx47iXEsROTpSWVJvT+evyNhxHLUpVKFcdl1VT2rG1XskXJ1s4PPa0ao3i0ttTAq3ZyhUjv08ep4yuEQfpHz1+s5x6J1J9RNSX4R6CMi5S6nJ6Kn9I9IgzyXMjvhF7reRgSVaQ2VnVFATLLowl8XRNgcriproP3fbFzyF1GsnTXeRRiPypLrp8dD07iHEsQytaowZFLdjKoLhXAUWLadYyKdT+WbW2cijh8PFq8VZu2t3pda8v0ptaLcj8Q4niKdNmSuxCUsSO1ZizpXSmjajlmt5CLM+vUnSw9CU0pQWsobck4ttb+Bnv2m4XJikfk9JTvsVJBt3DY+BkK25v4FUUqDj0kzG4tSVNvzfU8j5GVLc69S7i7bkWmbVmPJlVvW4P0k/wBJnX5rfVJnpvR5w2K4ZcX/AOkrDa/5OzOjSf8AgfoeS4jpiKi6yuaHpfQo1HoUahxGY9YyJQya5QCzHONwNrd5lMqedXHgMRUoKcoKOtk3K/06kbi/E1NXBtSVXXE2QuesVyFZRrkZRpnbQg2N5Ky5luHozUKsZO2TW2jWz6p725D6y4XF2otSdeprPR6oMEF7FmqnLuLAkHx8ZW4KW44zxGF/yRknmipZrX8La+JQno5hqVQ0qgq1nYsVp0zYUqd+y1RhqWtbbvEqnSUIuTTduR0PxLEVKalG0Vs5Pm+dl0Hv0MoOyVaVRhhxm61SQXplBfKDbW+g1vbx5V0slRZovTnfkH4tWhF06kVn0yvk78/+WDX6I0qopVcOzJSOfrTUIY0wmt9Oeh0v3S6eH7ySCHFqtJzhXSctMttL3OmE6OYKsRSVsRTcjMrPl/eqPzEC1tr93taTlhVa5XV4ni6Penka2suTGDofhqlLr6eIrLTGbNnVWOhtplA5+clLBNTyLczr/wAjqRi5TgvS/wDZlOlfCRhKioKnWB0FQG2U2YkWIv4TLUp5JWZ2sBjva6XaWtqZmu1w3gD9Iki+T0Z2ptZRpyGnmM1vcCRe5dF9xeX9namntz7ydz9vnFcmolxh+Jq9N8NiA9VKmXqqaZs4rKuWkaRBGXTQ76ct77sDKefu+vkee47h6KpKe0r/ABv8/ovQ2FLB4tWwuGq3stLDjMCWArL1oZWcgkgooubgZyBe2+/NTcZOPj8Hb5HlOaMbiaJRipuCpI1Ftja+s4EouLsz1Kd0n11+JVYu/KqB4Gw94i+mk94lc1ZviPrEaVCHQb1zfEfWAdmuhNkDSKAmaj9ntTq671eqaqyoVWmozXLEXY6GwAX3EuouzuYcdDtKag5KKvq38jfr0sr2NuH1vHR7fP8Ady/ttNjlvhmH54iP36nB+nTrq+BqheZGbT1S0O3RNcGpS9yvFv78TEdMeOLi6qVKaOFVMpVrEg5iSVsTprITnmO5w3BzwtNxk07u+hnwo5HQ6DwPd5SB0VpsQa9SzL39pf8A2n+smtjPOSzL1+jNdhVRanCRVRalOrTxSWbUZmYsgIPO5UTp4Z/4XbwPIcT72Kn6fJGu48lsTw8I3Uj/AKikuQL2AaIsFDAjlbaHIooyShNPXZ/Aj8EvVODTKP8ApMTiMOSL2bq6ZYOL99lJ8byEkjXKq4xqu/vxT/f/AKWGHKrxWoQulWkQG73pZBUt8ioPihkdEyM88sCtfde3g72+/EmcHKrXxStYVTVzG+5p2GS3gPuJno1G5SUns/2I4uMnRoyj7trevMkcSxVOpTCUSrF2KnJzy2Z7d51GvjMmLqJ08tNXzPl4Cw9KdOpmqq1lfXx0RwwtVKfX06v7tHDVMp3CnsuRblqJLAznnlFxaW6T5eBOrCdTs50+81ZXXXkVeEx74fEUcO9RK9OtTqtQcLZ0VELm5+G2nz8LTsZU4OXO5jxM1UqOSjbr5lDheJ4g8NpP+6WjXIRV7RqZnqEAXtbVgflOgnRlWvZ3Xw0RyqtKag4Xun8Sl/aNiQ2LZR/6SU6foM/++efru82e44TBwwqXVt/T6GSsW0+LQ+XP2vK9tToOLn3Vz+RaU8K703qqBlQ668ydAO+2npIpMnUxUIzUOZJwmFZzkQXP96mRs3sWVsRToq0mXnR38XbLhqFNHTrFauUGcZj2lzvcXFraAnSTVdwjlRysZSwc5qrWk5aaK/3v5mg4JwGqzhauJqK24yljrz7THfxtKo1M0jNX4lBR/wAdKNvH+is/ad0Yq00SurNWVbrUa3aUGxUvbcbjN4y2tFrXchgMZTqSccqi3rZbM89GGffIZQdJ1IdRgJU9xiG1GSJC1aZ3UA/33RlDhUXus6SBvFADTdG+kP4Onkp4frqmIbXtZCFUlVUWU8wx+cujG6scLiPeqLXSPzZp63SKqUCvhuqXfKHDEnvJIBMUoaWuYYx1vzHYfpfTRMhpVO64yH/cIsugSptu5lOlWNSrWDUx2QoGxUltSdTvyHyjSsj0HC6kI08rlrfYo3YWPuDvJWOq5KxT1qiisv8AMSfnlsfpLUu6zBOcVWjfm38bF9w7j69WlOth1rJSYtTJdkZCSTdWXY3J1lsKzpqyMmJ4bHEzc81vQtj0rokKPwtR8rZ1NTFVWZWIynK5BYacr98nLE35FFHhEoXtU3/+f7NDwLpdRWi7dVTpNRJalSUntl1Ivci5NyxZu4iR7dNNsrrcIqOrGMZNqW7fK33ocU6a0MysMIc9IuaZNXY1B2y1hrck33kHiF0L4cHq6x7XR2vp02G4npZh64X8XhmeoumakcobzBIt7yqThP31qWLhlejJrD1LRfJq9vv0JFTppQVQaWFKVKaMtO7XRM+7W5nbl84KUFZpbbEfwes5NVKt4tpvTV2++voc8J0yolKZxFCpUq00NMuGFnVhZswJ1uN7g6y2OIstRVOE1byVGaUW72ttba3kR+H9IeH0Khalg6ozKyMxZS6q260wWIseZuPnL541y0Zl/AqzWs1f1t66EXF9JsEtKhQXDVjTw7LUpBnUHOhLKXIJ0BPjfugsY7t82RfA6l1mmvS5j+JYxqtV6rbuxY9wudh4Db5TI3d3O7TpqnBQjslYj4SkzVMic1uTyXUe+8bXMorYnsdFu0aKhhman1dLsoNS1zqfDw8YmzlQrOEnLny/kdg2yP1NJrFvzknsi2tz4+HOSj0KpVG3d6stsX0u/CqKFKmHcDMXJNhmZr3Xmx33EqVFSd2zNVlZlTR45Xq1A1Rza+17Aa/CoAlqhFaIpuzScaRWoiqAFcaXUAXBFiDbcecdRd0dDWqkYaljrsQdBy/5mU786No3R1rrcbX8IFUXZ6OxTsLnQesTN6empNkDQKAMs+jta1emNxdreBynaWQZgxtOLpufNGo4viCZYzjLQomMRYhgMBkDH4cG5Ghkomili6lPS910M9SwpqVNG2vf+U6C3jtL3oiUsSu0zL7vYuaXCWIAB056amVXRc+IO1lE6fgCu0GrkqXE2naUfgADKwB0vINWOlQxVOq+6x9AbxM1w6j2GoiBrULnQwJMZAiMWBFETHcpOJRVIuJewvJpXKqslGLbLXhWBYi3kXPfflByRwak3OV2W64lnPU0hYDRm7vAd5kbW1ZS3yRMw2CCl1psMwW7E62J2HiYavUEjF9oknc3Nz3/ADlraMrTbuWWBpnutbXTviuPLoaPH422HJ30jqe6ww0c1aK8TH16asSyMNdbHS0xnpIyklaSOBqsNMx+RvESyRetjkTAsWhYSJaKAMlcJa1amf5x76feSh7yM+IV6UvI1/FtZeefRR1JGxYjgXtACJicQCDJpCYOCUUFMEWLMSzeZNzJTvcIJZS7wm0rGSPwqneNOwmDivR6rUoK1M01ztlGc2NtgRpYa6d8tpq+rM9XEODtF2Zl8ZwfGYe+awUbsGVgbnKCADci5GttLi9riWtRfInS4jiYvSoztTR7Ag3v8/pMzUTrU+KVVq1cD5/hHrI2XU0riq5xEMx/T7iFkWridN7piWm3wn1ELDXEaNuZExlByL5Ofh9pKKKKnEKVr6nGjgXd1Y2svLvPIyd1FWMVfGdr7uxcrVcJkBtfcjf3ld0Y2dMGDT/KSPSDlcLEnqmNMor5S27HU+P1PrBSE10KU8GdTrlI8LyzMVZOpbcK4cQRbT+/aCYpR6Fj0gojqHNrMF1H9ITvlZZg0u3j5mGmQ9GwNAQIAWBkS4UAH0Xysp7iD6G8a3K5q8WvA22OF1v4TSecRR1JEkiPVWCGVmMwpOo0P1lkZEJJg4fWVKYDHKwJ079eRjkru6FF2Wpa4fFjkR6yDRK5LbH5Re3ifIQSuRbtqesdFqVN6f4gBSzF1UjXIiOUVEPJbKPMmabW0OU3dlb+0TCUepDvYXemrE22JyE+dmIv4+EY47nlXCXz0xcdx9ZlqKzOpSd4k78PIFgTR9ohhFIQABw0LAD8LGIb+G1iAf1IgA1iBzjIjfxdpJMCZgcaL+MkmQaO3SFw2Hc8wIpPussw0b1ovxMFM56ADQECAWLEyJcCAAMBczYCvmoKfATUtUecqRyza6MrPOREOywC5xqUrwGQsRgg1wRJqVhOKZX/AIF6eqajuP2MnnT3K8jWx3w3EUJsxynubT35x5egr9TYdG+lRw9koMrMVLVKbkgE5iFdSSBmtYaW0GoNgZPM0tUY6lPvaFV024+2Mamr1EYA1M1NXFqdtLMF2N+V22NzoBJX0CnT1IWCCooysDzNtpnknzN8bW0LBK2krsTuOFaKwDhWEBi62IAdbaAjm1X6xgc2xEdhXOT1hHYTI7sDHYR1wwykGAFl0jxI6hrc8o9SLxT2LsGr1kY4IbE8h/dpQdtySdgKtzYbmApNLUVVQDYcvrAIu6uTmkS8EAFATLzhuIvSAPI2+4mmm+6cLHQca1+uojUBJjM5zN4ADOe6A0AOe6Kww54wIWM4elQajWSUmhOKe5Q4no+4PZ2lsaxROhcjPwOsNRe/Kx19RJ9vErWHkuYaKYimdUzARuUJIahKPIssLxnLoysvuJW4dCxT6lrQxgcdkg/OVuNixMkK5vtI2HccKh7jFZAO6wRWC4wuI7CuNuIrMLnKse6SSBjMl4xDPxOTxjtcTZ3xLmqqryJzHwA2Hv7Sqp0NeDeVub8iv4iwBCLsv1lTOlRTfe6iw6ZUL87aQI1HmmoEExGhIsWkS4EAFATJWCbsv8j9Zooato5XEoruvz+gKFY3teXSRzEzoahiSuM6CqZGwJskqdIiaCovFyGJtLwQx6iMQ4KJEBCmO7+7QA5VOHU2UXUbRqTBxRR8R4XTptdLg+BlimylxVw4XFOrAXv5yVrocGy7pNcaytliCRvEI41KY7oJgRKhk0RexEaobyaSIXC1Qx5UFzm8Qi2oCyr5CZqj1N9BdxFBUa7EnmfvKzrrRaFhxEWQDlcCN7GSjrUIuCpg3uLyJPEzcUrH/9k=</t>
         </is>
       </c>
     </row>
@@ -885,25 +885,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SURYAKUMAR YADAV</t>
+          <t>JONNY BAIRSTOW</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>smat2021_095</t>
+          <t>t20blast2023_002</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>146.7</v>
+        <v>116.7</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -912,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>26.7</v>
+        <v>50</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -951,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="X4" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
@@ -969,13 +969,13 @@
         <v>20</v>
       </c>
       <c r="AC4" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AD4" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AE4" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AF4" t="n">
         <v>0</v>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUSEhIVFRUWFRUYGBUWFhUVFRUVFRUXFhUVFRcYHSggGBolHRUWITEhJSorLi4uFx81ODMsNygtLisBCgoKDg0OGxAQGi8lICUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPsAyQMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAACAAEDBAUGB//EAEIQAAEDAgMEBwUFBgQHAAAAAAEAAhEDIQQSMQVBUWEGEyJxgZGhMkKxwfBSYnLR4RQjM4Ky8QcVkqIkNENjc5PC/8QAGwEAAgMBAQEAAAAAAAAAAAAAAAUBAgQDBgf/xAA5EQABAwIDBAkDAgYCAwAAAAABAAIRAyEEMUEFElFhEyJxgZGhscHwMtHhBkIUFSNisvFScjOCov/aAAwDAQACEQMRAD8AqOTsKZO0LnCsicE7E0p2ohCdzU4CZxSlQhMQo4U8qNyEJ2o1GE7qgAJNgNSoQk9KVyG39tvLgGSxsHf7Vze3d6rnTjKjb5hqJcMxNt3dZv8ApEaFAur7vFentKCoF5xTxtQHskgSCLmDAFiQdCIsr1Db9drs8l7IhzTBk7yDuP1CmCoiy7ZqNUcFjm1A0g3cJA+MK6FChIoCjKBCFG5RuUjkDghAURKYoiE0IUoUk6FyEIXIYTkpkIWyjQlEFdVSCIBCQiYUISITQiKYIQmSITyhLkIShYPSnHNaGskSQ4kAg8RDhNj38eS32lecdJ3B2JqBjs4kNDtRbgbyLz4qhEmFdthKq4rFtcQAJFvATLQeFo8lA52W9o9b7ja6PBYczALvBS1MA5xgNJj4njzVt4CyN1xVZruyQACDzO7RNTqxaTfd9q/Lu+tFax2zTSs/XhfRU3U5ngLz3KQ8OuFDmObYq9s3aBpPaQZaHi3LT4T5r0jmvIutgeR8ePJel9HMea1BjjqOyY+7aVDhCqDK0EydwQFQpQOQFTQo3hQhBCaFIAhhCmUBCicp3hQOCEJoTIoQoQtlwTMKKUKuqKQpmIQ5PmQpRuQhIlCChCOFGUQchcUIQ1Gy0gbwR6LgOj+y3V3spDWTPIbz4aL0EJujWFo4ani672y8PcxuWHEBzgezHePIrm90BdKQkq/sHopRa2LFxmXHfeYHALTpdHqLDIYJ7vr6KxMD0opNtVbVpHnSqGJ0kxAXU0WF7Q5rrESD3iUtcHZuBThjmZNIWTjOiFCqXPqXJAF9wG4cFxPSnoo2jRmnJIN+cn8l2eO6R0KLsj6pzcA1xF+YEKg3a7Kzwx7HAOsMw7LhyOkwpbvtgwVR+46ZIleNVqDheLcV3XQumW4cEiMznHvGk+hS6c7IZSEU/ZcDlHA8FqYBgZSYwaNY0W0MCJTJrt8SlVRu6YVpxUcpikrQuaIICilCVEISSlCUioUpnFRFGUJCFKElAjKCEIWw1JAxyIq6onSQgoghATpkpSQpTJJEppQhHTgEE6SPith1EZXltyXNPLP1bQSsNxW9gKjHAgH7LjpvGXw0CzYgZHt9lswpzaeXuFT6mu0NPXOygHOyAMxkmW9k5RcCCTpzVrZeKq9VLoBgwBpa1u9T7XDWsmZkcYAHElS7NbTNMkVcwAjlYDSec+SwuJIyTFrQFjtrVqmbK40jnblIAILffzAsNz8lNRbUkio7O0EQcuU2Ak2jfJsN8bpM2CLMxuC2SZE27we5X8c1sC4Mqd4xEKpaJmVzm0Nntq4mg14lozvym4OXK0TyBcD4J9uR1kCLNiBoLmPSFddkfUdJMtpAagdlzpdfh2GysTE1czyedu4WWmgOv2D1WTEOApRxPogKSFyaVtS9OUycoZQhOUwTEpKCpRuaoynLkzlVSgKBIlNKtCiVoU3KYlVgpAVKqilExyBJCFI4ppQykChCdMHJEoJQpRkp6NQg2PfzCizKKqqVG7zYV6bt1wKs4ykTVph7xkqEtNQvIDDEsBEdlpIDZ3TJ4rrMH0XqhrYFrzFRpa7s5+HBcZgcZ2u1cTBBEjuMro8OWAANbbfD4m0CR3WWKAM0yb1hn5EqttbZ5oOHaY5znR1bKoc+JILiIsBEyY4a2QBzhlaTu3ndfzso8aadMksaG2MAegCzRiXONiZJsPyUBsmyhzgLfhNj3g1HHkB8/moA5UqG06bsQ7DkPa4TFT2mPLReQBLRIInteCsymDWkMB0/E+iWPeC8jX4PVT5k2ZRhyUqVCmQ5kEpiUIUhKGUOdCShCPMmJQApy5CkJOKjlOXIZQhaAKKVGxEhVUkp5UcpwUIRpSgzJSpChHKAuTErR2TsLEYjtMZDN9R3ZYPHf4IkDNCzJVnDYCrUa57WHI0S55swAfeOp5C66nC7HwVAy+vh6j+D6rcrT/4qZJf4uHcqfTHbOemyjTcS22YBoptPDKwXDYuMxJuFqw2FfXqtaBAOvLXy8yFwxGIbRpufw9TYfe2gK5Sm0VpNKA6m4NIOjhAcCeBub/Q0mYmsBfDnvDqcd9ysHocY66dX1Hf7SWjyj1XV0Wk+9Yckrxz29O/dECTA74TfBUz0LZN4HfZYWK/aahgUw0HeTMc4aY9UbcA6k0uLpdBvwC3mgDVY+1MYHdhvs+8eP3Ry4qMHRq4uqKNIXPkNSezzyFyrYmpSwtM1qhy8zoB2/k2WFsHZ5zOfEue60/Yt5SRJ7hwXY1ejZqgmg4Gq326TiQ+CAQ8AjQ30kaI+jeBplwZUrNovqtPVuImIgN1sJnfExG9dPtCq5mUbSokFlqeOw0gt5nKJb3EQT7u9eirsa6MPR+lkjm50wSBYOAILYaZmTBDRKGnLAa9b63wTwY3NreRcCHda27ugwTK80r0HMJa9pa4biIKAFenYjBmuztCnjqO6rTLGYln4mk5XEDmDyXI7U6NEBz8OTUa322FpbWpb4fTNx9apa+mQY+exHYQDyWoO1+fOdxzWAhKeUxK4romSSlNKEJygJSJQyhCRKaUxKFClaLHI3FQhGhVUoKUqKU8qYUI5TFyBCTwVqbC9wa3M28VV7w1pcchdXMLXaw5i1r3ATDhmYwbiW+87kbcZ3UcbjKtQZ6tRzy6zQ4kgDTsjQDcAFNk/icyR5QB8VFUZL4GjGjz+oXsMJhKWGb1RJ1MXP2zGXmvLVsa+u4l2XDT5PHyUeAoZq7WEdloOY8ALudymI8VdxdfO8uNp9I3eFlFSrto0nmHGrUO4CcupGu8lNg6b6jgA2G7yT2hv03/qrdIGPfWqmGtEAngILndkwP8A0kZhaHsNSlToURvOcZMZk3a1vaBvHgN7lbK2Ocj64JgtrOcJ4POYea6gVmi5tPNYe2cKG4nONHUxln3nUvaHeQQkxjy3rT7AAABMZnHQDkIv3FfPak4qv/TH1ut3my94GfwlPdefobc9g+f7WpjMbLYB13fmq2ApNJJeYYwEvO4NF9FQZVLiIBvobXHEX0RbXcXEUGQKYh1Q+9UcPZFtAImO5e2w2AOCw/Q4f/yPzfw53/4/tGpudV5Gpi2YvEdLibMZcM1dytxP1k6dUXIU3+YZnPquF3DstPut91tuWvMlaWzel+MwzWhtUPYQT1bxnaG6CN7RyBAWLhqec5YtH6fmm2u7tBo3C/yH1xTH+FoBgobgLQIg3y7fXNLjiaj8SahPWdcn56aLr8H0mwVWpNTDvoVDP77DPLCN5dlED+pdHhsQarRVpVRjGM0qUop42iDugwKg+64DNwK8v2XRs557vmVY2O97avWU3ljme80wZN45jiNFjr7MY8ENcRGjpcOyfqHcY4grvT2gabjvaaixnusfDvXZ7b2NTxLOupFmcugVGjq2VHadVWYf4NbcJs48CQBw1RpaS1wIIJBBsQRYghei0tsU6tJ+MbkbVYAzE0XECniqR7MgH3+B11BkELlukeKo1Xnq8xykBtR1nuZFm1BJzOabB+pbE3ElKNn1XkhjTI8jw4XtBFjyvuszjaYAc4i/yY0jUe8b2BKUpiYshJS0tW0GURchJQkppVVKclNKZBKELVCYFIJwhVTp0ikpQmJTUzcfXBJxUf5hbdnN3sUwc/QSsmOMYd/ZHiQrVB0l53SPOSfkFBhHZi48VNgaDnPc1sS8SBzdHkNVafsavQq9U9kuLM4y3DmiZcI3DK6eEFesL2BxbN4kDWBmvLdG7cc4C1h+Fm1W5qmXgP1TY8uazOww5rpB5i35qRuHqsqHrKb2G85mubuHEfeb5jiq1V+anw7Z+ZVyAY1H38l0bvMe0jSFo4hrK7KNSsCAHB7WN1cRI13N4z3LNxNV1V7Q90MBswbrWC0MM8CmSB7IIvrDRYeSxaNTtBx4ysGz9kYfCuc9resSY/tB/a3OBFuJ7LJzi9uYnGjcJhoAHNxA+px1MyQIgTlN1qkBna4Mgef6DyWe6SSBqST5f2WhVguaCCRmbIGru0JaOa18Js4txBqsw8Uy3sU3uGaCBDo1g3jXRd6uMZhwS7gYktAJEdWSRcza0WMlLMLRLxvDlNie+AMhqs2hTDRA1gellm7THagan9JPw8luvawAkuLagMCllIka5pP1bfNsesyXyeC60Hh7iR6Hy0I5iRzXBgdTdLtRP++B5G6v0WinR7mzHPVVicjck3iCecAvPmVNR7QY3i6T3T+ioYbtkvO+pUju6x8fJdGNlxlc2C5njP291bqAQBw+iVE0qYqMrtCGqPGM0d/KfkVTlaFRuZsDw/EP7FZsryW16PR194CzhPeLH2PevRbLq71HcJu0x3ae47kSSGU4KUwmkpiUMp3BMiEStSU7UMIgEKERSCSYoQmcgeOye+f9P90RQjhyPxCabHbvYoHgCfb3S7ajt2hHEj7+y1uiIa6v+8eGMax4zGIMgjLO45S6PwrtaG06FWq97KjIh1IBzmtc6mModDSQ6XueLggkU4GtvKsK6+XhHlNj9cFYqMs7lUnwTzFYAV6hcXRaMufmllLEmh1Q3WV1XSvpCHmph6RY9sBzqrARmc3O4sEkgszPzDmuUpuOQtGjYcPOD8Uz2QGmPc4/W4p6ohoI4Qb87T6LVh8OygwMZ8PFcKtU1nbx+Qfniho1+y8cifgFTaFYcYaCN+YH68UHVyQOLJ8cv5hdwRcqGwJPyy6DD1uroCq2OtqO7BludjbFxYCIMiWyTruNlrYroaGU3vNRxrMY57rdklvaLQ/2gYB7c+HDG2VV62i2hmAfTPYDnBrXBwyubmPsmNI3mY1I1n47HVmNo1Q1rSxoqPIyXqOLQHEElzLAkgAmDMC58ti3VKdY9cMO9ecy39sd2gtvEjMp/g2M6FoAm2mjtZ+ZRoLZFaHspVHEF2ao0uhwL2tnKc57LjczFxIlUsfZx03fAK3tSq1zaYpkljARmOYl1Rx7TxmuA6AYga3k3VDF1A50jeB9FPtn03NpCQR9VjoC4kCNLHLRJMY5tTEFzTIiO+yn2a7U8P7qns6zG825z3n6KmpnIb6EE25ghUtjvzU28mUwe/qw+P8AeVtaOseazbv1Hs91pIHBOTuRKy5ZIKdlQriHPP3nf1WWrgcK6rUbSpiXPIa0SBJOlyi6V7K/Z6wZ1jXnJ2iJgOaS1zb3kR6hIdt7hptvcGY5ZJvsreFUmLERPPMfOaxSlmTFCV5pP0nOQ5kJKaVEoW5CTUQSUITwhcEQKdyEKJwTPZDhzpH17SIxInTf3LW2vhM7hUYbzMbj3HuTDZeMo4fEf1TG8CATlMg37Vnxmz6+LoE0RvbpBIGcEESOMHTO9liYDBPq1hTpNzPcHFotJAGdzROpGWVo/wCUYg1KjOpqEgDMAxxLC8HLmgWmDEqpgMS/DYinWymab8wGsi4cAebS5s816xs2sanWtovOephnOoVD7RYCTRLp3sdWcy9/3d09xuLfQILQC0ix5zxysIiPO6TUcI2rIeSHCxHmOYMjX3XktWg4MLXgtcw3BEEWm4PIocN2mObbl+nivacDQJxVF9Vreu/Y+3oYe17ASD3veJ4FY2xBXrY2ozH4ai1zcOSGhrXNe11RsPMucJs4LkNqy0ndyE/Vz0BFxPO0qx2act65NrG2Wd7di8mptlr2xuz68NUea9N3Jo/PwuvRcLsbC4upg64oCk2v+0NqUmkhpNMOykREXb9QiPQvAV2sNGu6n1uc0g6DLmEh4AcATEaT4rqdp0gYeCM5tMXLTl/1J7AVQYJ77tIIOWliBx7R4rzymyKoHOR5SO66bEk5iCSRmJAJJEuuSBxXUbP6H16xqlrmA4d5Y4uLgHObmzZSAZiAbxqFRxvR3E9SMV1X7nLJeXNBAmAS0nNc8AtbMXSL43hIgZ6nLxCydDVkEtOR/wDk3VDC0pYeZE9458wqDxBjgtHA+z4+v9oVbHUoObifl/daGGHELOx3XIKDFiaQdwBHrCrbNPZA7/jA9AmxVQ9W5g1uZ4WlUtjV5psANyL95kKWkb272+y1tYeiPb91tMvf64fXepE1MhEV0WNxutroXVDcQTAc/I80hAJzsLXgNnRzgxzB+NXf8TqLXHO05rsqtIBjqa7A2S4W/iUyb/bXKkmZFiLzwI3hdXs/bFTEYTFYWs9kGiXNe8wS9rmuDfvOJ36zczJSPa2Dc7+q0TaCNc89Z7Pum+zsS1sU3W1+892vZwXnyYpwnK8vIXoIUTggyqQoVVStwBOiAThSqoQiIShOAhCiIWlgzDACeY7lRLJgcbK5jey224fBZsVG7BW7Z7nMqb7TFkqtQaE98KTov0sqYd1MPaHNpGqABaW1LkZuGaHd/esCpjMwIWh0ayuzte1pMtdLmtd2feAJFrub5LdsZ9KlQr9I2WgB0DPVpI7iO4Km2RWxtegA4B0loPM7paDnq2BbMrrOivSzD0XsZUDmMacSAYzBlOs+lUpi17FrgYG8c1rdHKlGhXrOGNFYHDsyOqOgghzj1YzOvGUGLe1pdcZjNmMe4f8ATAzA5ZdvAaO0fxcNArNDYDDSLqlSwzAH2bsc5k79cswJTWpWwLmOeHlu9mIk/W4T4td+7STMJM3CY5j2tdTBjWYH0tPLQt/bmbXmO92Pj3Yj9hrVMudzcS4wIFhlsJMWhYvRp0t2PO9uLd5klcNSw+Iovb1Tnh7SSDTcRLDqJEHdEG+lk+A6QYihWpNLo6jOKbXNAyNqDtWgEjTVaRgQQehc0ggkRwIqARE264A7J5LG7EEWqNIcImc7Fk9/V813exn5cTtd32RVPrUPyVfa1Zw2C0Ekl9TLcmwbXcQO6KYELlsP0qqU34suY1xxTXNcZLcpc1zczdd7jZWtodIRV2YzChjs1M5i6RBguJEfz+i6/wAJV6RjiP3UyexrYPP6uSp/EU4kHNr/ABc4EeSxNmOlvd9A/XBSVAHN7ifMWVDZ9QB3Jw9dVN1xDnN4n5fom7mkOMdqTvYd8kdqzsO+S4HTX0hYWw8XlquaPZOct87fErXptBfUn2Rn8dVg1KfVua4bxPwPzXPEEtc140I804oNa4PbxA912eHdIU6t4DBUi1rruDmhwkAWcJHxWhSw7G+ywD68korfqfA053d5x5Nj/LdW+n+kcfUdJLWjmSfJoM+I7VkU6Ln6AnyHxVnD7MeT2nBviHH00WnVqZRcgD60VMbRZMNk+g9Ulr/qrE1LYemG8z1j7NHfMJ1Q/SODoicVVLjwHVHu49xCw9s4Pq6pbuIDgdJBF/UO8lQK6DpUDmp8MhIO+S647rDzKwYWJjnObvPzOa5VW02PLaX0jLs/CiKaEZCaFZcl0AahIRhC4KVVOAkAnYnQhSULGeAJ/L1VPFbREBpvLokXkc+BVmm+Dv8ACJ3/AKLLxlKIh4LocSBpuifNZqpBdBWyhLWyEVHCtyOdO8+XNH0YeOuEH7Y7+yS31A8lhYjFFrSIAmbgRrqAN2iLoriiKjyLlrqThO/UX9Ft2XSJrOZ/za5viPuAs+PxAbTbUP7Hsd4OH3K9B+9qCG23y8Fwd4KxiaXW4bqx7QdUMcQa1S4WXhNoMflaJBDS0l2UNBaGgdonflNzET4q43FBr2kDNBfIGn8R+/TQg+SzYvDVcMHNqCJcD3b1XhOkHv5ptQxuHxjW7jh1QR3inSMGY1ls5WsooLQA/WCAe8t159lZFCl/xj36ZGDldzGhsHcRmLv5Vo7Sxri0yIndPzWVs/GAZg43cW3P3WlrW+pvv+NMNiTQp1CM+jLGxzfPkC7yUPptxVWnTdkarXuJ5MDfPdHO5Uu26hqMDnEksd7xJMEQDe8ewR+IcVm0qkEg6OVnH44OmnEdmJJk2Mt3CBZrRyZcqmajYa7cYn69V639N1g/CGlM7riBnkbjO+pHcvO/qnCmnim1Czd6RoMCLOFjlbQG3FBSdldG9p8wlj3dofiFxwj8kGKic1pFjz7lUqY9h37j57k/e5rRLjC8+xhcQ4KxSBEu4fOyoY+lIbyYPlKYY1xENabyO7h8lKGveANAD3+Z4X9Erxm08Kxpa508hf8ACY0cFXLp3fFFgukFWnFIEZWtbEgSAdAOIAhX6fSJ/vPJ5AR/SqlLZhHaieyDfm6APmtOls60ReBIgxJ4x8vJeGxJpVKhexufYvVUauIbTDHPNuZUmExoOhN9SM0knjr6Kai2KgFvw6DTUggSUTdk8IB5xB4Cd6GtSaHMBIkbgbkcBOl+PPuXJF1pdKqX7qi7gS3zAI/pK5ldRtusH4YR9tp7jldb1XNlq1suFgdYqIhNCJyHKrwFWVutKRKFPKFCJhTlCxEUIUTW5qgadI9bwqONBAMka3jUmYsRuVwO7RjWIiL7tDulUsb2Qbj2gJHIaOPgsr/rK2stTC5zarok5SDfUhwidPkrHQ6jarU3EtaPAgn4hY+0KusBve0zPgux2ZhOqw7GHUQXfiJkpls7q12f9h9ku2hei4cj5LYo1A0HK2XE3tOul9y16eDBbAItYm53TZYeFLgczY7NjmNrHgujouJbNqc23mT8Fn2ywsxj+cHxA9Mo4BadjOFTCM5W8D759qz3gNBDB56n5rGfS7XsTMza3l4FblDDOAlxk5j2rQRxB53Q4kkaa6T+aW8kwHFYlHY9Sq8tbSrVQ2crQ6AHHKXS53sgCL75Cz9r9H6lCAaNRjeyCHkEBxDjAcDDhDbG03XqPQR7RRdSgCvmcXkmesiIc24kAEdm2WfvAmL/ABDqtFFjZmoHjeAWjI8gG+8tsOXJMmPeyjLXZ5xr35pZUq72IFMtsMhwm9hkO4LyZmD5T4fP63KzT2WHRAieI5961XYpg3A3mbc9CkzHsa4gNET5g3+B+CxlxJkrcBAgIaOyAN3P8h5EKzS2aIO424akzfwA81Xrbdi1h+W8/Ed4CqHa73SbieE6cFUBBK3RSY0XjWY4kaeG9C7FMaPdLt8kcbz66rCOJPH0gAedhO/f4qN9a0kiTabCwmwG64+tFBUhX8VtmZbFuMESeMG/lfvVSpWNQ5gBOhJEiJs75Kq/EsmCS6dTbhqjwGNA0BcYiN3juCOasM4V8YmaWWZ7Te1pMNM249oKs5SvcTE7tBw5fXBRFa6YIasNSC6yAoURTK6otYlIFCk0qVVTtKdyBqIoQqTmgvMkiBaN7rR9clQ29Wge1cyTadREu9VtYa5g6E8Jixv6+i5/pU+NCbk3MExp8lkzetwEMlYWyMN12IaDBa05nQIs3d5wF22LdaB4rH6H4OKbqp1eYH4W2+M+QWridZ7vknmy6YfiWzpJ8Mkm2k8iiY1geKEOaTDi4AOzEtidIgLd2biwBkbUzixbmJmDcrnmUt/GUmMAuY01H6JrtXY5xbg9jgCBFxn3i/ke7XBs3aYwjSxwJEzbMcc7c9F0GM2lTZ7TyDOg/TRZ7trU2w8lzzz1A+JWU9s3Ik2uRKLEUwQIEclgp/ph1ukqW1ge5+yYVNvieozvP21QYzHB7y/I6+hzua5pEwWwYBi15VGrWc+oCG5Y3lznFxj2nZie0RwtyCv9XLByKCrTEgjePgmrdiYUNDN3zM/O5L/5rXc4mb+XgqOIpVRFwfEoHYepAJykfi8Fs1gCAUTB2SIU/wAkwhH0+ZXMbXxIAv5BYooOgkjvNte5O3CnXj3R8VthgAIjh8bp3UjFxabcCY4+ItzCp/IMJ/d4/hW/nVfgPD8rKo7LqO0LQDO93iSITs2UfeqGOAEepWuyi4CQbjUfd+6owk208Jh8O8MptM6zkeHyAt+BxdavvOc4RkAMxn6yIVSjs6m33ZPFxn9FYAARKMpdAW6UzkDkRQkqFKApkimQhaicJk4UqqkBRFAoMZiMuWTAJeT+FlJ9R0eDPVCFdw7SG59BB0962/64rj+kkOqdUyT2g0TvLtDYeqmb0re1ga6mDl3hxEnjlII1Q7CeMRiDWggMuRuzOmI9SuLKTgZIWt9Vu7DSunw9AU2NYNGtA8go69MEGd1+fABWSVXxLojg1oce/cF6HYjJrOfwHqfwvPbXqEU2sGp9PyQqxY7S0jXcoqryB7J4GLqzQ90e87tuPJSvAPgvUZJD0kG4Wb+0Nt/bmFK2oJjdPxUhZI8rHnp8kFTDt1yiRYGOPDzVl1lpTtI05pVGRzglQnDgaSCOZi/JStpO3u3cP1UoMcU7QQ6N0n1+SNpAE94QdWSbuPhAujZRaN1+JvKFQxxXQ7D2D1tXDitLaeJbVFN7SCS+mLB32QeGp5I9q7PnCYeoBDqDn4as0EnLUY8uzci4EknjlWj0dxBqYGtSaR1uFc3E0uIyGXgDhY/+xauOY19R5Z/C2jh+sZwbiaLc4HKwvvJJ4JHVxD21+sfpJ7IF+6abp7WFNadFjsP1dR529HCOxy4OmPrmFTxDMriBoVaa63qq+M9ofhHxKrtpg6EE5g+v+vRZtjvcMQRoRf53nxKiUbijKjK8wF6ZMVG5SFRlVVkoSToUIWkk0pimapVVKCgrYXrRkDS4kEWgGHNLXQTpLSR4pwmGo7wquyKvTALgCqWN6IUzSzNFRrrA3a4RqTBv4So+jWANGm5pmS8kyItYC3hPiu2xOHYabpaLAxysuX2f7Pi7+orPh6r32JWzF0WMEtHzwVwKpjtzd7jJ7tArX5qnW/iHkz5L1+wm9R7ufoPyvI7Wd/WaOAJ8/wABPRPtO7mDuR+73z62UDPZ/nU7dB4J9qlDrFNUMR+IKOubjmWfGE+I08W/EJYnd3o0UgZfOact9fknZxSOiakrKJslGo5ooTFEEIK1ui+0xhsQyqfYuH/gdqTxix8F1Ven+zU6tKZbgcVQxFI/9mu+Ms7wJfPErz/ce4rv8dehVJvm2ThSeZFSpBKUbQpgVGu4xPc4R/k4dh5XbbNcS1w4XHf+QD2hcdtDDdVWqUvsPe0dzXEA+QBWfjva/lHxctvpZ/zdbvafEsBWHjfaH4P/AKcuG0SX4Jrjrunx/wBqmBaG44tH9wUMoCU6ErzIXo0iolIVGVBVgmTSkkoQv//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUSExMWFRUVGBcXFxcYGBUVFxcYGBcXGBUWFRUYHSggGB0mGxcVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGi0lHyUrLy0tLS0vLy0vLS0tLS0tLS0tLS4vLS0tLS0tLTAtLS01LS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQIDBAYHAQj/xABDEAABAwIDBQQHBAgFBQEAAAABAAIDBBESITEFQVFhcQYigZEHEzKhscHRQlJy8BQjM2JzgpLhNENTsvEWVJOisxX/xAAbAQEAAwEBAQEAAAAAAAAAAAAAAgMEBQEGB//EADMRAAIBAgUBBAkDBQAAAAAAAAABAgMRBBIhMUGBIjJR8AUTUmFxkaHB0UKx4SMzNDbC/9oADAMBAAIRAxEAPwDuKIiAIiIAiIgCIiAIiIAiKiSRrRdxAA1JIA8ygK0UPP2qoWGzquEH+I36rJh21TOaHtniLToQ9tj715dHtmZ6K3DO1wu1zXDkQfgri9PAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIix9oVjIYnyvNmsaXHoEBCdtu10Wz4cbhjkdf1cY1ceLuDRxXz/2j7V1VbJinebXyYCRG3owG3iblV9p9uvqqh9S+/fOFrfutHstHIZ+N+KhjDe2oNsraG2RWSpUubadPL8TyRrieAPGw9/FXIqc7gOe4q5G54yIBztmNVkxQE3DRZwOg325b96pbL1Eu0dRLEQ5khYRwJaRzDgug7B9JlTG0CYNmaMiT3X9cQy46haNHFisSbW8jfIg8FIwRxkZEXFjxOWViPH3heeslHY9dKMt0dy7P9paerH6skOAuWOGFw523jmFMr56ZUOaPW07nNc0g3BsQBcZcCL+5S/Zj0mVbJA2d3r4yd4AkA5EAXPIrVTrprUx1MO0+yduRWaSpbIxsjDdrwHA8iry0GYIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiALQ/S5W4adkOQbK44jfPuYSABvuSNVvi5Z6Zqd0ktKwfdlt1JZbkNCfBV1XaLLKS7SOSxsFxf7LDlz087rJgY02c518NrWAyzvp+dV5S0Rc7w81s2ytksA431WKTOlCJB4GnE3Dlla27O4I5ZBZbKF73ZA4uI+i3Ok2RD90KZoaWNvstAP51VZdZI5+/slUSC/s/E9SqY+x87DfGL+K6e5wtZYNS0ar1niafBzOZr4CQ4EG400N9SFCzttJiYcJJPIA3N892e7mF0bbNA2RhaeBIPO24rnD2PjNnXsTlzytkdxXtPUrqq2p2v0QdoDPA+B578JBHNjh8jfzXQVyb0MUJZLK4g3MQ14Ei3wPkusrfSd4nNrK0wiIrCoIiIAiIgCIiAIiIAiIgCIiAIiIAiIgC576UacOdHfcx5HUEaea6EudelOUB8GeWGTLjm352VVbuF1Dvo55SkFxIFhYe/+1lMUOmSOpg2NpPC54552XuzqgHIAnwWKcbHSpyuSlK4qVixWUIdosYbOa5vUKaoKxr293NQsXMqaCdF4WlW59o+ryw3PvViOeaTP1dgh4zyobcrWtr0Ic1zCyxaS8HiLZ28gPJbFM5wPeN/DNU7Wb+qDuB872svYrkhJ8G3+jqjayjY8XvJmSdbN7oHuv4raFrXZfacEdPTwl4xuaO6LmxJJztk3xWyro07ZVY5NRPM7hERTKwiIgCIiAIiIAiIgCIiAIiIAiIgCIiAwduF36PMWmzhG+x4HCVwClpA13dHtNa62dhcYwQNN+fivouVgcC06EEHoclwSoa2OpfCdWFwA44RhaPcPJZ662NmFekkZu1PZjF/sg9eSxtnSyC4Y7OxwjS53C/0WdMQ6OF/IX+ayqKnYXA2VE3qa6Ubx0L1C6oey8oGK9sORDhxzvbp71h0kvqanCDkdwzsp95axpda1gtNpJTJPi5/kKDdy2EbaG2VGZc8EYtADp1UZI2pL2lrmGM2x4tQbjFbect2WvKyzqOS0liPBSpY3eB5fNIs8nHghYYySbjLOxV3aMf6jofmFmzgAXWNVvFoWHRziTpoBc3KLkjLgwjDYxBpyBDxbKxxCxy11K61Gch0C532dpBLO1gzYw4v5W6eBNl0ZacMtGzJjmrqIREWkwhERAEREAREQBERAEREAREQBERAEREAXJPShsqKOobLaxlIfcZYSzJ2f71xlyK62ovb+woauPBK29r4XDItPI/JQnHMrFtKeSV3scYiqSYwzeDflY8FLbJNwtXkuyR7TkWuLT1aSD0U3sraAawuuDvWKZ1KTsbBtl+GBx32Wo9n6xrZMg421NlkVlRLML3sOByt0V/ZUbIr95v1PVV3LrErUVZMrCcr6OvpyIsp+RuS1aWFslv1guNM8lfoa2WLuSd5p0IXmbxDRn1jrKOkqhJOxtu61pHLx8fgre164B2DefP82Uj2AoWTVBLhdrGk21BJNhi+PgpQTk7FVSSisz4Ny7HUw9WZbZu7vg3h+dy2JUsYALAWA0AyCqXRjHKrHIqTzycgiIpEAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIDhvpN2SYK1zm3wzj1gtpc2DxlvuAf5lrVBUZWItYfMX+a3T0q7fZUVjaGOxdTxuke798ltowR+7n1IXOXyW3ZjdoRmcj5rJWjqdDD1OyjdJMDmC7Q6w4aLLip6e2cbTfkPotZ2XtE2z0GQB0z5KbgmLgcRsLXsAB0WXVbHQjrqSDKWncLhgHT32AVG0Zow0BuWYte5Vp85jNgRZ3mDv6KA2hVPe4XO+/u06rx3e4ehl1815Q5uYP/HjxXS/RXQhtO+bfK7rk3IZ87nJcup6V0hsCN2Y3C5ufiuj+j/tTD65+zCMEkYaWG+UgLGvcPxC97bx0WnDx7Rgxcux1OgIiLac4IiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIsXaO0YYGGSaRsbBq5xDR70BlKM7R7YjpKeSeQgBjSQD9p1u60cyVy/tR6cY23ZQResNv2st2MHMR5Od42XNNodoKmr/W1MrpHHccmtG4NaMgFJRuRlKxb7LVLpa6SSQ3fIyZ7iTmScz1U3W0+I4h7W/97qtRoZjFO2QG1jn0ORW90jcWfFZsRpI3YW0okK92HXJw1HisqPbXdw4Trqp87ODhZzQV7F2Xhd9n4rM7M1rMtiCG23OFrW6rN2TRSTeyMPGQ+yOnE/RbLSdl6dufqweuimY4wG2aLAaZWsotI9u2R1PQNhbhbrxOp5lc87SSSU+03Txus79XIwjc5jQwjn7JHiumVGa5l2ubaccmfFzldhn/AFLFGMj/AErn0H2N7TR19O2VpAeABIy+bHW+B3FTy+TqDas1O5kkMjo321aSLi97G2o5FdR7M+mpuIRV8eDQCaMEtz3vZq3qLre4eBy4z8TsCKxR1kcrBJG9r2OzDmm4KvqBMIiIAiIgCIiAIiIAiIgCIrc8zWNLnGwGpQFxR+2tt09LH6yolZE3diNiTwaNXHkFzHtx6WXtc6Cgj7zS5rpniwa5psRGw+1mD3jlyK5DtN1VUvMk8jpXne91z4bgOQsFbGjN8P5EHUiuV8zpnav02vOKOgiwjT10ouerY9B4+S5Ptjac9VJ62oldK/i43tyaNAOi8NFIPsn3FeCjefsn4KWS2liF2zFwrIp57DCVkx7OJ1IHvVM1JhNr3vnw5H5KbpTSzWdiGeN7XRZfLmCtp7L7XDbMf7O48OS1F8ZCqhkIKoqU1NWZfSqunK6O4UjWubcHyWVFCVzLYPa10AAkBLNMQ9ocraOW47L7XwTyCKPFiIJBc3CCRmQM73tc+C586E4cHVp4mnPZ6mzNiVbmqijkuM1luj3qi5fsYcsGXxXG+01aHzyvGmLC38Lch8z4ro/bvbohhMTD333bfgLd4+RHmuQz94gLdhKTXbZzcbWT7C6inucyvKtuY6LJibZJqcv0tlf5LelfRHOZRsra9RTOD6eZ8ThmMLjbPW7dD4hda7L+m1oY2OuicX3AM0YbY5+06PK3hdcgNDJb2b34W3KkbOkO73heOm3wSTaPrnY+2aeqZ6ynlZK3i0g25OGoPIrPXyLsz9Lp3F8EronHIljy0nrbVdD7M+lysg7lbH+kMH+Y2zZG8yALO9yhKjNa2fyLFUi9mujTO7orFHVtkaHNNwQD5q+qtiSd1dBERD0IiIAiIUBZq6lsbS9xsB7+QWmbQ2k+d4vk2+TfmeJV3tFtAyPwg91uQHPio+LctVKnyzn4itd5VscrrNkvMshu3OR5373E8FSdkvG9vv8Aop+oHff7PtO4/ePNWXeH58V24yiuWcWVSr7vqQMmypBuHmrY2XJy81Ol5099/wCypJPD4letx8X56Hqq1fZX1/JEx7JP2nDwufjZWdq7JDWYm4iQeWh5AKfipZXaMcejT/dZTdkzn7DvEhvuuFXN05Jp/uSjUrKSf7L8/k0EbPkdox3lZZ9F2eF7yOH4bjyJW6M7NynUNHU3+F1nQ9l3b3tHQE/RZo0qMXd6+ehonia01ZafL8s11mxIZWGPC0A7xk5p3EcfmtLcDA7ukieOT2gSACwkFuE6gnO/Djc26+7s4MiZO8NHBmfjc5haD2r2E8VQjY3G+YAsDR7TvZItu0udwuq8WozSaRbgZyhJxk7+F+DfOy+2GzxMmyaTk5vBwyI6bxyKmKavjme6ON7S5ubgMyM7G+4Z81Bdk+z7qOEjD6yRxu9xdhjB0wx5XNhYF2V7LLkpq12TJmQMJuWxRgEniXEkk88lz6Xo1KWaW3gdOt6YvHLHfxNK9KMYinhZxiv1Je7EfgtOjZvXWto9kDNnJIJDxeDfzuVBVHYMg91v9L/kVteHX6WjnxxntJ/T8mkALN2ZSmRxAtkL534jgFNVPZNzTpKB+G487K/s6gEN8szqSDfprZW0KDjNNvQrr4yLptRTv70zAk2ZI3LD4gj52VLNlyHcB1P0U1JMSdPf/ZXI78B5/wBl0rx8X56HM9fU9mPz/kiBsZ/3m+bvovJNgyWyLf8A2+i2SGE8B71JUUBLmDCM3DeePRQlUiuX56E41Kz4j56m50UzobBp0AB8AAtmoqwSC413hawc1fopi12S4tWnfU7NCs4u3BtKK3BKHC6uLGdIIiIAo3blZgjIGpyUktO7TVd3EbhkpwjdldWWWJCOddyuOdZWISr0gyXQSsceTuemmYc8DTfP2W/RUmmZ9xv9LfortM67B5eRsq7KVyOphupxwHkF4IlkyWAJJsBqdABzK1ul7TNMzYy6mAc7DYVAfJnpZrWlt72yxL3MkRUHLYn2Rq82JabWdtHmb1VIyKfEQ1hvIS4nU2AAte+d9BdebM7VVjqxtLJDFfFheGYyWgC7nYsRFgPpqoOqixYeVrm7NjV1rFVZetYeI6b/ABKlcgkeBqxIaFrq1srgP1dO8NvlYvkZc+TSP5ipANXsLQHlxt7GHP8AFdRepNaCXPvW7ug6DeFQ1ZUve1cOQCxyyylcjlsUkK05quphS540a3X9pKdgfhcHOaxr8yQDd+C17Egg2vlvCzoa6GR7o2uDi02OVxoHWvpo4e/gtKqKeSao7ro7ym/qnGUYQ5zi6KRzAQLuaXWvbeDZSfZage2pBkLH2xd5r2Eesc0DFc2c67WkWaMrjJVKq7l8sPFRunqbSygj/wBOP+hn0WSyhj/02f0N+iyGsV1oVjZTFMxxs6I/5TP6Wj4BVsoIm2IYAQcrZLKa1eyjJRvqW20LIK9JXl8+n5C8J3IyKZN7KqN3FS61aglsVs0L7gFYqsbM6mHnmjYrREVReW6h9mk8AucbWnu48yt923LhhcfBc1qze54HPxWigtTHi5cF+ArLaLgjePgdD5rAgcsuN9iD1y+8PtN67x0W05tymif3R1d/uKywVGvfhYLHSRwHME4h7iFkQzXC8e5JbEL2t2qxrfUB7MR9tjoJagEZFowMy55nhktP2nPUR3a6SYCwNmUsFOwAgEAHEXaFb5HsRxeHvqqmQB2IMxNjjyNwC2NouORKyK3s/TTPMksTXvIAu4uIsNO7eyrlFsuhOMTlDXQ+pdK+ok/SL2YxoIsNCXvtbPPIFb36NNnSRwySSMDfWEYCWgSFoBxEnXCTawPAnethpdh0sZBZBE0jQhjbjoSFIhI07O4qVsyskehVALwBXGtVhQjxgV5o6+a8AXtlG5KwceZ81burllSWpcNFshFUQgapEbHMpZqUSNEzAxrXWlIfLEA7Fa7GNxOYC3D+ryuTlcK7suOg9dZssjXCSNwLn3uA++cYDcAPdGLPWylpaWujlYRFI9sbnYML2EOaXYrOkkudDhuQCNLusseGrkbIfWUAaz1kfeEbYwD63u2d3S52I8xldZuTZuv5N9sq2he4FUGq5szJFTQqap1m3VYKxqyUWFzliF/C5PwXi3JS0iWi4gW+0c+nM8gvRkLfk8SqGu1J8fkF6dLHV2Z5NGZ+isZTFlUMma2TYzyWuv8AeJHQ/wBwVqjHb+J/us7sbtYPc9pcSXSSgDPRhFgOFmkLHiLJo6eCjKUZNbK3n6G3IiLOazWu2dVhjwjhdaTSOvMWHSVpt1tcLYO0tRjeeF7eC1iVhAxD2one7d7luoxtE5eJneTMmIEGx1BsVlDPL/m4zBHMaqqraHYZW6PAPjvH54IW5XGh0+hWlGJkJW1Z9aWH8eWlyLG3DS9t11J0T8lB7XdaQOO755FZtHNY2SaPaTujYYyroWDBNdZsZVZaXQFW1q8YFeYxeXFjxrFdDFU1iuNaotk0i3hXmFXsK8IXlz2xawoWq7ly8whS4ylrAnq1dAVYalzzKWAxXGq7hTClz2xQGoV6VYlkQ9PJpFESvDn2uAG5nruHMrJqJ1gbPN3PdvJsLZuIbllwGuZVtNcmetLgkHPtYW00bz+8/h0VMgIbmbukOf4RwG4bvFXIY93nb67zzXsbgXGQ6AZdB9fopMiizPkQ37uvUqjstQOhqHHL1RkL28Q5zQCLcM3jyV6FhNidT3j9FLU7Gg4hb82OY8dVlrxi7X4OhhKs4KUY7Pf53NkRRX6WeI96LLlfgbfWR8TTarN11a9SA88HixWg7N9Ibmm08eMaYmGx64Ha+YW57L7RUtRkyVuL7pOF/wDS7M+F1uhJHLqwknqjJ2e3Dip3fijPxH54lX2ttf4c1cngxgEGzm5tPAhetdiGYs77Q4H6FXIzM1jbsKjtnVGIWz7vdPXip3bbMitd2W02edxcbeAF1ZLukIPtGwUM6mqdy1aGSxU5s6oBLRfMrOaSdiCvtWG2YaK4ZrLyx7dGaCqsSwWSrIaV40epnlfXMiY6RxyaNOJ3AdSubVNUXvc9xuXG51t0HJbxtugMxYwvLGXOgBu+2QN+WK3PwUf/ANIs/wBZ39LVy8ZSrVpWitEfWehMZgsFSc6su3L3N2S426voaiX9fet/7PbU9dEL3xssHc+DvH43Wl7WozBIWE3GrTxH13KR7H4zMS32Q04+Bv7I63z8CsuElOlWyNb6NHY9NUqOLwHrk1os0X9uu3xsbvjVbZFYcrAmuu9lufnblYkBIhesF8ll62pGhNkynmcvSyLBqJl5JPdYUxdu14KSR42YW1qgsaX/AGSLAjUE5DLfmQpHZkQbG0cs+Z4lRO0zjiIcM2OY4Z/vBrr8ciT4Kbp3ZC27fuHQbyrl3TNLv9DIk+6N+vIcOpSQXszxd03Dz+BXg7o0JJ03klVCzGlzyBvcSbAeJ0CgyyJdY1ePAAutM276RoIrtpx69/3r2jH82rvDLmueba7SVVVcSyktP+W3usHLCNf5rqlzSNUaUmds/wD2If8AuI//ACM+q8XAPVO+6fIooZ/cW+p95jnUqoat/EPivEVZoO7bF/ZQ/wAMLOm9v+X5heotseDkS5+JB7a9krXNnfsz+J3xKIrZd0rp98ymrNh1Z1CIqEaZE/B7Syp0Re8kODyFSMeiIoyJUzH2n7A/iRf/AEarrkRVx7z6fcvn/bj8X9jT+2vtQ9H/ABYpPsJ+yl/GP9oRFzF/nvz+k+pqf69H4/8AbNgk3qObqvUXYifGz4L0+gWHNuRFJbEZblreFkHUIiiycSE2zo/p8wpen9lvX5Iiv/SZX3zPZ7bfwn5LT/Sx/gx/EHyRFnq7Guh3l8TkwWdsP/Ew/wARn+4IiynSR9GIiKkvP//Z</t>
         </is>
       </c>
     </row>
@@ -1012,25 +1012,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ISHAN KISHAN</t>
+          <t>PRABHSIMRAN SINGH</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>smat2021_081</t>
+          <t>smat2023_135</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>142.1</v>
+        <v>128.6</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>36.8</v>
+        <v>42.9</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1078,10 +1078,10 @@
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="X5" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
@@ -1093,16 +1093,16 @@
         <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="AC5" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="AD5" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AE5" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="AF5" t="n">
         <v>0</v>
@@ -1124,12 +1124,12 @@
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>WK Keeper - Batter</t>
+          <t>Batter</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUSExMWFRUWGBsbFxgYFxcbGhsYFxYdGBoYHRggHSggGh8mGx0dITEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGy0mICUtLS0tLS8tLS0tLS0tLS0vLS0tLS0tLy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIANIA0gMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABgcDBAUCCAH/xABEEAABBAAEBAMEBwUGBQUBAAABAAIDEQQSITEFBkFRImFxEzKBkQcUQnKhscEjUmKC0TM0c5Ky4SRDU8LwFYOis/EI/8QAGgEBAQADAQEAAAAAAAAAAAAAAAQCAwUBBv/EADcRAAEDAgQCCAUDAwUAAAAAAAEAAhEDIQQSMUFRYQUTcYGRscHwIjJCodEz4fEUgsIGI1Jysv/aAAwDAQACEQMRAD8AvFEREREREREREREREREREXF5q5gZgcM/EyNe9raFMFm3Gh5AX1K+f+ZPpPxuMLwyV0ERBHs2blpPV1WT5il1Ppn45OJ3Re2kDHggxZvDlBFEt6En4VSriCOxmLavrdg308j5r0BFgjjJJza73rqT106ldjgHGMRhQXQTuj1PunT5LDBwaeXWOCV5I+y0n0sraPKOPIJOHkbe4c2rI8liXtGpWQY47FWPy79MGIjpmMjEoAP7RlNcRpRr3TXVWNyZzzh+ImRsIe10dZmuHQ6Xfra+WcZh5ojlla5taUQdiFYf/wDP/FvZ498J1E0ZA12LPH+QK9lYwvo5F+Ar9REREREREREREREREREREREREREREREREREREREXlzbBHdekRF8m/SQ154niY9DkkLWhoNZR7oryHz36qb8j8nRsYx8rA+R2pBshvYVsT3K0edOElvH5Q37ZbKfIFgLj89Pipdw3juGjOR0rQRv2HlfU+SnrEkhoVeGa0DM5SnDYQNADQAPLRecVAs3CsVDM3NFK148j+iw8YxsMIPtpQyumpOvkPRaMjtIVWdvFQrmXgbJgWyDTprt5hVtylxI8M4k17m5sjyxw2trvDbT0NG1aU/MGFlJZHKHENLj0oDveyrXnjBBuIEg1a+nDsaOo/L5rbQlrspU+JyubmavqXDyhzGuGzgCPQhZVhwptjDVeEafBZlUokRERERERERERERERERERERERERERERERERERERERFTnOMjJuKB7A5pOHfGSQACWS0HNPx/ALjyYENL2fUopnRsBb7QkF+viEYH2gLduLpdjikeUxOvVksjXCtbcXDf8AkHzUu4fEyRoJaCa7Wo85mV0urABaFE+W8AIZGSRxiIuLM7Gvc5lvGrddns61Y1WxzXwtk2JcZGtc0ZQMznBgB957q1obV5rv8VljikYHeFrCCQ1pJJcaFADYbk7BYpcZF9YORxc3Rrracrs+2R1U4jqAbWJJmff5WQaI9/woScS9kYjOBhia55ZkjrMWj/mFvVt7WfguXzLwjTDRUT+2AAFXkILiNewH4K2pcDGwE5QD6BQbGkSYxgvL7MPfdA+6A3/ur4pmvIWJaMsdytbgfEBPE2QNLdS3Kdaymt+3X4rpKO8kx1h3djI6vQU0H8FIlYwy0FQ1WhryBoiIiyWtERERERERERERERERERERERERERERERERERERV1z9wQNDpmgnxtkFAmjYD9tGijdnSr7LHy3xHKy72CsHHYYSRvjOz2lp/mFKm+G48Rvexzhmjc5j/VpIP9VNWZFwrcPUzWcuji+Me1f4pRFR9wWXd9a1AIXnFcWaxwkEu3RwcGdjVihp26rqMw5P7SOga0NXpv6rxHhpXD9s5prUADTvqVpkQrABC2TxB0kNkEEef6rgcD4W6fEOcGk0MoNW0OdbvEd26D3vJZuJcQaxpbmHh39d1Lfo1wJZhjM7ed2cfcApnz1P8yypMzG6lrVMrbaqS4DCiKNkY2aAPXufiVtIitUBMmUREREREREREREREREREREREREREREREREREREREREVAcz8KMs00kRp2d99nDMd1O/pR5tbFhJosNMPbV4iw6sbYB1Gx19d1xOCYdrmtJ6gfkteJa5jWu4z4afdU4SHFw4QoNBxzHYYV7Nzmt2LbNevWvVZZuccbPQZARW+hA173SsNvDQ2Q0PMf+dV+4/CWNRfbtal67kFV1Q4lVpheHzPt077BNuA6nsT1C+huV/7nh/8Jn+kKsuJYFrI66rW5K55dhX+wluSB75KI1dGWvymh1ae3dU4Rj6znAbCY7wPVS4vLTY3t9D+FdSLXweKZKxskbg5jhYI2K2FtUyIiIiIiIiIiIiIiIiIiIiIiIiIiIiIiIiIsc0rWgucQANyVBeaOf4YSY/HmI0aysx7Ek1kb57r0BzjlaCTwCWAk2CmmMxrImlz3AV069hoq9535tkJdhYqZtnIdb6q602v9PNV3xfnfEPf7RrY4w02BlzOHSy4nxHyqvJYuC5nZ3uJJNWTqST4iSfiF0sFgKnWh1WABeLGe3aBrvflrNXrtDCG3ndYMHh7fLGSac01eu5tT/lIh+HZ+8xoa4b7Df0IUNwkdzZgdLG3X+Gut76KQcrveyYwhwY5xORxHX3jGe4Isj4jqFt6awzn0hUbfLM9hOvcdeUlZdG4hrKhYd/MflTNrbog0ksNuzONkChWnmsEWKdHbJGiwda8+oG69nEZ9IxXmV8kXL6DKuVxl4ax8jtmNLvWhoPmq0xMTmsgaNCQcx83nM78yp/zhAWQ+zfLmdIRTRWjdy4j4UP9lEsXhc1ODXOpgGxoG7HSgSvp+gcM4MdVI1sOwa/e3cuH0tWaXNYDpc+ilfJ3NZwbPYuLDFmGXO7LV6EB+w2BojWyrLh4/CWtc45A6qJILTY0pwJBB/RUXLCJGGN2zgR5jz+aiUkD2OLHWHM1AsgA1eZo6XvYVGN6OLqudpidbTffx18SpcPiRkykTHNfWkUrXAOaQ4HYg2Pmsq+eOVOccTFLGHySPjIAPi1b0Lq2d6OVl8N+kaB0wikBaDoJCABZ2sWaB/e09Oq51TB1mPy5ZtMi4j3sddpVIqsImeSniIimWxERERERERERERERERERERFqY/GMhjdI801os/0Hck6V5rbUd5raxzWMkLQzMHPDn5PCNCe5q7oak10teOMAlbKLA+o1p0J217ufsqBcW5mxE0ucuLGN91g1aB3cPtabn1qlDePsDp5JA0tL3WRdinVTgeovT5LtwOsubq1w6Ht0PpotOaIEZXCsun3Qf+3qO3yv6jCUmCmyplAdlAMdxP3XMxhy16lNploe6OwEgfbxUSxuHOo76fMhdyDFRRR+J9HW2gFz7Ggpo3070NN1kxeAJ33Ffhrf4LxJw8nWlQKZzEg+/faORU2aRdcTF8YnNiH/AIdl6kayu8y8bejaHquhhIZnNe04yexVWc3hIBa/L9qiNQNdNNlixmB0OnZbeCjOVjurTlJ8ifCfn+a008O0VDMknckz527lm+oS23kpFwHmeXOyDF051VHLejh+6XdQeh3B+IUq4hxCLDQmcnya3rm7Eb79FCJcC8jVoOo1Bqz3Le/8Qo97TFYHPReXPsBxDtA5xGtkUcupodu65uK6Hp1MQ0tsDMgbxGnCd47dZKvodJPZRIN409+/KOJj+MYiZzpGvyAWXOoF7nkdzYAA6DQDQWuS18z3sLp5i/v7Rw8630+Hdd7HNFiMVZ3rQa9h0FaD0WDhHC5JpbjjfJr9hpdQJ61tp3XTr4enYEW56bbGw5LnsquuQb/daUGKxZH95n028f8AssTMK90jnOLnOcLc5xJJOUWST5qbx8pYlgt+HkA75b/JaDMM1r7PVxHwBqvjVL3qaMg04twhemo+4dK5UODDdTr2b1IGg9AXdf4V++yNWfX1PddqaAWXaa/Ls0elC/n3WnPCT1079/8AZUAA3WkzorV+jHmA4jDmGQ3LBQvq5h90+o2+A7qbqkPooxOXiIaDo+N7fI1TvjsrvXy+NpCnWIGhuurh3lzASiIikW5ERERERERERERERERFWH0myXiY2B1VFY0unFx+d0PkrPUE5qwUH1oTTNdIfZtDWXkY0Am3vfu6yaDR2Oi34amx9QCoJGscYuB2TrMDaV6MRUoAvpGHQRO4mxI5xIB2mVBg26D/AAPHuvHun0Pn1aaWPFvOzxTq8LhsfL0P4FTfjMLHYbM2GNga9urGmi14cKJPva0fkohjIwBW7TsD+h6/dPwK+mpVOsE81xXNy2H45eixYGOzE54LWEua41egA1Het6/iUyx/LcEbZD7R7jCY84ytFtkIGnnSgsHFjGz6sdY3y5w7W2FrfEBemreh7BTHFc34SX2pY2c+2MQfmytGWJ27RdgkfpspIxPWEXjMdI+X4DG2gLgDyVtTqCxpaADlvr8wzCeUw0xoNtbeOM8nwxtxMjxLkiDDGWlgzlw13FGifJYeIcsYXDtBP1qpGxlrqjy294JbYHvhoJ10WzjuaY5DiGuje+OYMAaX1lyt/U66Ln8Z42yZ8UoiLREGgs9oSHNY6wOzTVi99fJeUhiMwzk87j/iLa8Zk6b6LW40gDEcvE+iw8ycOZBO6KMuOXLmzVduGawB01C52EcXbm8oyj0ZpXwXc5g4/DO3wwZJJCx5eSHGg2so6gVXkuBwo+KQ9nu/HKVXRzljesHxAReJ0Em3NaHxJymykPLnBYps7pGB4YCcuxcexO9V0vVb2B4hFOXxukGGw8dhkUZMWZoJtzq8WagPDsNbtcvg0pa9zsxYBpYAIunHxgggtodV38HJAAXuhjfJQDrY63dbaNQ1vWhvtquR0gxz6jgXcIja1/E3zTPG0q/Buaxnykkj7zroZtaPC61eUuHvbNLM1zvq4AI9oXU9jrObfQgAHqCCPJQbmGYmcupwzyyFtgg00uLXUeh01Vku4rEH6h4AqxmIBNnM6/s1eg0ux5KtuZ8U2TERAA6NfduJOrwaN7HZZ9HiKkXuAJkaCDPM7knyTGO6wmoYmToI/A29d1mwmGFBztT0HQevc+X/AOrFjmgrOx2w0vbU0NfPoF0sZDgWtcx7nyuA1eyTKc3URx5TmA2t5Gy7D3hloJ7Pf78JXOa0uXG5Gny8Uw2tW5zf8zHBX8qX5L5faZ8LivaEt9o4FrQP2cjD4RISdnCyCOtDW1dC+f6Se11a21j2gldDCtLad0REXPVKIiIiIiIiIiIiIiIiKDc5vl9uz2QYymC53ltNzOIABeMjfEGkkguIdTeqnKp/nvHmfGSRO1iiIaGdC6hmefPoD0A03KtwFI1KsDhfy71prvDWXUhnlecDio3ue6Rkr3Ne9r8rmtkBFOOlGzQB22UKxEpqiNDuLsHzDu/yI816gZTazuobAuJA7AWsc7B+8PwX0OHw/VSOJnS2g/C5tWrnIK4HFZSKN7Ef+euqx8NxHhBHVeuNstjgN6Neq6vF+G4XDwsfhnyOBIDXvIfHM3L43se0U0teCCw61qs3VA2q1p+rzXjWksJGywYjEkfh+S2cNiMzAO5r8z+i6XNHKcUUM0jJpHy4cQuka7KGZJtLbQvSj16LY4dy7F9QgxTS8zP1qwWC5vY+7V/bHVTtxVNxBEwSGi25uO6Lra6i4COUqPvkuOMjpEPnQas/CcR7wHUuPn9m1I+Icqxsmw+FildUzazvAtuV/QCt6NA+SwDgmGZiYoYny5nSvZMyQDO3xtAkFCsrgLG+4XrcTTe5pEwROmw494hYmi5oM8YXLx7tW/e1/wAhXHwmIJJBJ0Gm+im/E+XWgYpwe7/hS0t0HizN6npv0XPHKbBho8Q2Z3tJBEXRkCmsllEZcDvoSvHYqna/Ad5AI+xXooug29zC5rMToXWdNT8Nf0USwD7mjHURuNesl3+HzKsKfgULJsRFLK5uHhyiSSrfTy1lADQauOtaAHRRLhnDI3cQxEUUuaKPI1ryKJZV+6a1s1sO6VsZSYQ4kxE6cRIHbGy9pYd7vhAv+8eHNdKPEGjRIvciy4Ds3sT3OvxWDE4CQ61JlGw9mQ0Dz8WvxKsLhuEhjAysF9zqfmt4ltVQ+QXHqf6gv8FO3N3oB6ldJnQ9vif4D8x5KocHiHQTxyhxGV7S7QtsNddZeoFX11C+ko3ggEbEWPQqnuYuHRvBOUNPcdfUbH81ZXJ0jnYLDl24jaD/ACjL+imr45mKhwEEajXwNvIcpWX9I7D2JkHu+37rtIiKdERERERERERERERERF5ca1VI8Oh+syvneabI9zx+8cxJvXZvYamldr22CDsdFTmEi+rzPw+tROLBe9N0BPqKKxfiKtFv+2YnUjXx297TO/D0KdV3xiY8FI8Pw2ECsgOnXVZfqMH/AE2/JYmSaLUxmIeBYaT6UonVqjtXE9pK6Io0xo0eAXF5p4PAI5JGhwIaTWY9ATp2KjPC8JLJwx8Aw8gM0kb8xLGRxmMZSY2Xme57bzGhv5Lu8XxrnMc0gjN4SDp7xpTjCcLoN8NBoAGnQaKujjarYkzBkSSY7LyO4qSthaRNrdkfiFwzM/ETYpz4Xxw4jCthpxaSJGXldQO2p81t8vkwMw8coztihe12UHWQztmYQOwy6ruMwlC/tLzPhdSKJrt1vp5rM42rENAAtYTsI3JP3WAw1PeZ99yjWMeyV+FE7ZCxsIbMWXbX24kgjXRxBsLLiuLRNlwIfIZ3wF3tJgxwzMzeBtkW5wFE+hPVdGaAXWU/0WN+BB3aPK/yWxvSdSRmaCBNhI1nt4+UzCxOApwYcb9m3cF44zxPDtixhbOyR2Jc3I1gOYUAPFppWq1sDxCEnBxud+z+qlkx1pj2uZIwO03zNqvNZW8OvoKHp16UskfDjV0EPSJywGfefpDR9I0AHf4I3ANBku+3OeJWrhMc0YmeXO9gdiGSAsYXGSJjnkx/w5rbv0tRnD8Pn+v4vGFoy4h1taHHM0B1tvSrrsptDgPLVbLcGOopTYjFVKxkgCwHgAPRb6WFpUtCSouzHS5svs68yf0C60cprVb/ANRaSsGIw1KIhWZwVH+NzUCrK5UjLcHhwd/ZNP8AmF/qqu4tEXyNjH2nBo/mNK5IYw1oaNgAB6AUqcMNSosadAsiIiqUKIiIiIiIiIiIiIiIiKq+d4PZ8QLq0kY13xHhP5K1FAfpOw+uGl83MJ9QHN/IrTXEsKowroqBczB4m/DRXT+qEhanCogRRPot+Vjx10UgFrrpON7LW/8ASW9QCsLsHIyzG97PuuNfLZbHty1BjxsQvYWMlcvH4nF1QlFjuwH8RRXGdx/GRH9rHmb+9GSf/gdflakznMceqxSYQEJLkhvYufgePibVkoNGyOo8iNwt0cVeDTmWO4101WviOBQyC3NGYbOByuHo4arQm4bioz+wlErf3JdHfB40PxAQXQiF2YuMCyR16bGlss4uzSxShz+YGtOXFQPjO1kWO24W/A7DyC4n5h/C6/wKy+ILH4SpVFxJjtQe4/VbLZwa137qGBsbftuaVndM6tHhwrvRXkr3KFLM+u6wYiUAElRI8cLPfDmjz/rskvHXSNtt0FlFl4CJhb3DY/acRw7Kun5z5BgLvzA+atpQL6NeDOAfjZRTpBljB6MB1d/MfwHmp6qKLcrVBiH5n2RERbVoRERERERERERERERERcTm7hRxOFkjb748TPvt1A+O3xXbRCJsvQSDIVP8J4jQF6dCD5fkutNxkDz+K7/GuSIZ3ue174nPNuy0QSdzR2JVL8y4U4WTFD6zmbDK2NjDeeQluZ1Vo1rervQdVobQcbBW/wBU3dWDLxJpF6C/MLSfxZrN60VZO4+Y2Rvc22yAltOJIyuogjoV6j5zYPs/gtfUuWz+op8VYjuYY61IH4fBYjzNF3v0tV+7nCPfJf8AKEbzdIRccBdZoHpfbTqsm4d7jDRK8OIpgSSp+zmC9GxuN30r81kj4u462B3/ANlXD+PY1+UtDGh9hp6WN230d5FesLgcXNmD5i1zdcl5bb3BrRVUujMRUMAQtFTpCkwKw+IcabX7Z0dC9wN6/JQHinEcGDcb6cPtR202OumhWvPwljNZRICeswcR8HttpHyWB3DIvstDuxzANPpV2PirWdDvBu4SpKnSIP02SbmmVgAbL7UHcPG3xWPEczWNC4H+BzgPkUn5e0JJ100Gw9O61YuX3ONBeO6LqtIEBYjHAgmVIOSsfNi8RHDJK/2bpGNIsatc6nakHWlfvDORcHCbDHv8pHuc3/LsfiFQHJThh8Syf/lslaL7hh8Tx869CQvqYFT1cOaRuLHQ8Yt/HKDus21i7fReWtoUNAF7RFqRERERERERERERERERERERERERF82c/wCGc7G4lxIdnc5wro0EtAPn4bX0kSvnDjeKkccUWuBjnm8e1uyOLmUegqttNlXgSRWEDl479nhJgSJlYVQDTM9vh796KKz8NaYi0PLi2QBvhIGUiyRewvpvqs2H5XFAnqLW40aGu4/VSPDRZo9OgGi7GDwdJrqgcJh28btadgBqSocRiHkNIMSNuRI9FFmcEiaaLb3Xf4PhAIpIi28p1HdvQg9CNwVqOBv0/qujhZg1zZNg62u+eh+Ctpsa0nKFM5xIElcriuDLtW055aCRs2dg2J/dmHca2Fn4FO2QBriczTTX7SMPRkvcdnbHyK2+JAMdro29/wDpyHr9136r07AxvIcbY8jR7d9tj0cPI6FC0h8j3797yEZYK6GKjpvx1rTXv5KKR4bxnJTXHfTwv12c3b47rsO4g9h9jLWb7JB0eB+6T1/gJvsStTwvJ7/Jw+CPAcQeC9bIC8OjIadDtRad2kefULzw390Cy45QLr3tNT0H9FuvBHv9veHUea57xkyG6t4H3uoHzC042RSJbrBjv/mVlhoNQA+4C3MXAxpdC2ixjPeaP2Z0GYt60XOodSr15H4icRgcPIfeyBr/AL7PA78QVQbph4SN6o/DZXB9D0ubhzdKqR/Xe6cHeRIIPxvqub0nSyMY0GQJAtcCw2sRoNBzmbVYR+YuO514b8fz4KdoiLjq1ERERERERERERERERERERERERaPGf7vN/hSf6CvnaD+7E9fb7/8Atr9RdHo/X+5n+anr/Kf+rv8AFajNnerfzK73CPtIi7lD9Sp2t/8AKgrfIz+7zXP4p7wX7L/Zj0RFuatZ0WSXUR3rcOvnRO/dYeW3n2O50JrXbREQ/MvfpK/ebWj2B0WhhTcMbjqe53+aIsKnzDs9UGnf6LvN/s/5VH8V/aQf4zv9BRF5if0j73WVD9QJD7h+6fzVufQl/dJP8Qf/AFhEXO6U+Qe9wqMHqVZCIi4K6CIiIiIiIiIiIi//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTEhMVFhUVFhcYFRgWFRUWFRcVFRgWFhcVFxUYHSggGBolHRcVITEhJSkrLi4uGB8zODMsNygtLisBCgoKDg0OGhAQGi0mICUtLS0tLS0tLS0tLS0tLS4tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgEDBAUHAgj/xABCEAABAwIDBQYEAwYEBQUAAAABAAIDBBEFITEGEkFRYQcTInGBkTKhscFCUmIUI3KC0fAVU5LhM2OiwvEIFhckQ//EABkBAQADAQEAAAAAAAAAAAAAAAABAgMEBf/EACQRAQEBAAICAQQCAwAAAAAAAAABAgMRITESE0FRYQQiMnHR/9oADAMBAAIRAxEAPwDuKIiAiIgIiICIiAiIgIiICKhKt/tLL2323Og3hdBdRUBVUBERAREQEREBERAREQEREBERAREQEREBERAREQERaHafa2lomOM0jd8C7Y94b7r6ZcB1QbPE8Thp2d5PI2Nl7XcbC54Dmei5jtF2zsY8so4O9Ay35HFrSeYaMyPZc52w2uqa115pLRtJLGCwAve2gz1tc5qLulOgyQSbH9tq+rJE87gw/wD5xkxx+VhmR5krRGRxO8MncDc391ht81cBB4/NSJLg+2mIU798VEjjyc8yNPTdcbe1l0vZnthY/wANZFung+IXaermE3HpdcWZ6e6yYyOI9iEH1ZhuIxTxiSF4ew8RzGoI1B6FZS+XcLxOaEju5ZGfibuuIzH18jddW2C7RxJu09abSk2ZN4QyS97B9rBjtByPRB0xERQCIiAiIgIiICIiAiIgIiICIiAiIgIiILNXMWMLgLkA2HXr0Xzz2h7TPqZi13dkMJAdG4PZbhu35aF2R1FlOe2TaEhgpY3HxX7wAgX0IaT+W1/NcTlc7IcBpysOqCzKM9b/AGVoq8YnHiOlhdUFG88076TM2+lpoHVXA3z9CrgopOV1XuSOh5FJqVNxZ9ngNPA/ILLg65jmOHmrURz4dQePkVd3gcwbEfMcipVZOWhOfA8DyI5FX6eps4B2TgRfQgjS9jqLahYcr/DcfzN+45LHMm/obkaX1/3QfQfZxtO+YGCa2834DvXJAFy0+mYPJTpfNGweNmOqic42cHAAnK4OQa7ln4b8Lr6VY64B5i6gekREBERAREQEREBERAREQEREBERARFrNpq3uKSeX8kTyPOxt80HzftJi3f1M897gyHdub+HMADpZaJ7j/f8ARe5Mrj9Xz0Xukj3n2PEqbeoZndZOF0pe4BS6jwhgt91i0UTWNAC2VPITxXDyb7r0+Lj+MXDhkfRWazAYnDILNG8r+47ks+61sjnePYU6GztQTa/EFaR7X7u/Y2BsehXXJcOEjS17QQdf9lbrcIj7ss3RYixyW057J5c2v40t8ORiqK8xu8WXmP6Lf4rs24SWjFwQFjV2z8kTd45Lecub93Lrh3O/C/h7gX2dqRw6j/wvpXYnEv2iihkPxbu4/wDjjJY73tf1Xy3TVJLr6H5LvvYrVb1LK299ybTkHNabjzzWjJ0NERAREQEREBERAREQEREBERAREQFpNtafvKCpZe14n5+Qv9lu1j4hB3kUjPzsc3/UCEHyKZL8NStls9HvSG+gWoiOTedgfkFJ9mYrRmTmT8lnyXqNeGd6b3ufZZdM5jdbAqL1eNvuREOgP1Nua1FSag+Im3m4D5LH6X5rq+v16jqDKhvMK+2oFlyikrZwfjJHIFS3CquSQW+az1j4tccnySgYg1pzIy6hWZccgOW+3rmoRi7ZGlwN88lHdxodnI4eTSVbGJpTk5Ln1HVw+B+bXt6ZrDxui343M6ZKC0tj8M4z6WKkODTTtcGvdvM0525WKm8cnqonJq+4hcMVnOHFp06DVd37CYbUsz+L5R7NYLfUriuNRd3Uy28/f+yuw/8Ap+3/ANmqL/B3rd3z3PF/2rql7jh1OrY6qiIpVEREBERAREQEREBERAREQEREBERB8t7fYB+x1ssQcCL77bcGv8TQeoCv4C3/AOqQOZ+al/anhQ/xF7333ZImuH8rdzL/AEhRrZ9gEZHDfPssd77ln4dWOPqy/mNLV7wG7E31WF/hribvfn1Nx7FdChpGOyIXv/AYycmhZfUsb/QmvaCwUIy3Lm1hoc+v95KWbPU26c1l1FGyMcB9Vk4PDck8P6Kmt3TTHHMrW0WEb+Y4j5qHTYTumzoieuq6tVU28wG2i10Zi3t1+R5FVmrlNxNIBTbM75G6xzR6D5KT0GCGIDxE20vqpdTUzBpZYeJmxP2Vrq2eVZjMvhA8bwjvalrRlvtFz/Cc10vsaojCypZw32e9nXP0UFxWLekZY5gOI9LZLq3Z5T7sL3cXOF/RoWmNW7kYcmczj1fv3/xK0RF1OIREQEREBERAREQEREBERAREQEREHP8Ataw4vjie34ruZ6Eb2v8AKVyzCjbvGjKx+y7/ALS0PfU72gXcBvN/ibp9x6r59qXFs0nM2JHI5i1lhvPmurj1/WfpvqKYNHmvdbiwYMteC0bKvktHjtaQ4C+g+qxmbq9Oq8sxj5N87Eix2/IN820uOPJX6DanM5bvK9vqCoQGSS/i9yvdPhTyfia3qSfstPpZk9sZz7t7mU7qttCLBoLrciAPUlepMSFUA572seBkGm5A6nioY/B3h1zIwjoSbfJUmoizMPufZR9PH5WvJyTz8U/wnGHDwOdcjjrfrdZs1XvarmeCYgRK3PiAR5qYzyloIGt/lqst8dzemmOabzb92c17O/ivewJ010y+i6vshHaEu4PcT9vsuSbF0RqqtkRcW/E4kZmzRmPmAu500DY2NY0Wa0WC6ePHV7cnNydz4/tdREWzmEREBERAREQEREBERAREQEREBERAXO+2LBg6lFQxg3oneMgAEsfYEnnY7q6IsfEKNk0b4pBdj2lrh0KJl6fMTJOSxMUpg4sOtzYrM2iw+SiqX08urD4T+ZhPhd5Efdayapv7iyxmb23u5cs6mwPdcDvG3I5j1C3lLhDDqWHpcj7qzRy7zBztrzstVic8jT04Kkt1enTNYxnvpKosFhsLmMczmT81i1eztK7RznHmLtHsOCiEVbISLb2Zt5qYYfBK1ge63kfumpcpzy4346RrEMKbDLHbQkeeRC2ldVEu/vgsDH6jeeDfxC2hFr8lgT1ZJsLknQdSrTNslrmu5m2R1fsToS+eeo4Rs7oct55D3fJrfddfUa7O8EFJQxM/E8d5Ieb3gE+wsPRSVbSdRz290REUoEREBERAREQEREBERAREQEREBERARW55g0XKiWO7SvbcRjLmNVPQjfbjhLZWwSDJ7d9oPMZHdPTVcPk3mmzhYtP0XUserpJc3kmxyub2UJxih3s26/XosrrrXVbfT7x3FjDsSLNVSprd/VaeUkHPJVbLl5K3xnfanz1102TKkDT+ysoYo8gNufnwUe7wq9Tucp6iPlWVVzEm/NbvZfDN53fPGnw/1WJhGElxu/TgFNqKCw0WPJySeI6OHht/tUowrbiVn7tzWuEYDRwNgMs/JdBwbEm1ETZWiwdwOoIyIXCq2B5nYImkvkLW2B1vlc9Bz6Lt+BUfcwRx/lbmeZOZPuVpi9suTMlbRFQFVV2QiIgIiICIiAiIgIiICIiAiIgIixMSxOGnZvzyMjbzc4C/Qcz5INZtJiYibk0veb7jBxtxPIdVybEu0LduH0oDv4re9wuo0746gtqYzvMewbh/Tnw4Z3XIe1bZt8dU2UNPcyaEaB9yS08idR6pbYnMla+PHpKm7nMaxt/CBe55kkqkgusOjbbJZzQuXd7vbu489Tprqqja7UZrVS4cApK+NWHwAqM8lidcWajzaELZ4fh4HBZsVIFtaaEDgo1y0xwSeV6ip7BbaJtgsWFtlI9n8DM5BeCIgc/1n8oPLmVnmXV6jXepid1sdisEzNS8Zuyj6Myu7zP0tzU5OQVqCINAA4ZBabbPaBtHTPlPxW3Yxf4pHfCPIanoCu/Oep1Hmb18r3UZqe0Z8FZNC5jZI2yFrd02cCALi+hz3h6KSYNt7RVBDRIY3n8Mg3c+W98J91yrYTZ010zu8LgxrS5722v3hPh11ubn0XrajY6ppSXlveREk78YJDbknxN1b9Oq6fhi+GPdd6BvmFVfPuA7X1dLYRyEsH4H+JnpfMei6HgfahBJZtQwxO/MPFH/AFHsqa4tT0tNRP0VijrI5Wh8T2vadC1wcPcK+slhERAREQEREBERARYeKYpDTsMkz2saOZzJ5AcSuN7b9o81ReKm3ooeJ0kf5kHwjoFfOLpFvSdbY9o1PRkxx2lmGoB8DD+pw49B8lxTaHH5qyUyTSFx/C3RrRyaNAFrHglSTY/Yaate1zw5lP8Aik0LwPwx8yeegWskzFO+047JMTkbTsjlt3T3vbTuv+MEl8R5XNyOZDgp/iWHRTxuilaHMdqDwIzBB4EHO619VhURhEIaGMbulgaANxzCHMc3kQQCozjXaFPQv3KujLwfglhdZjx/C/4Xfpv7rKztaVHsb2CqIHExDvY+Frb4HVvHzC0D43NO65paRwIIPsVM39s9ERnTVV/KH694s6HbnB6pje9c1pP4JmgOB88wfQrDXFL6dOOez25811167lTqqw7BpfgnETtQQ+wtzLX5W8rKO19HFHJ3cc7JbgEEZE3Fxa+TsrHI8VheHf2nboz/ACOP73r/AG1McK2dJSkkWsb/AF5FXaOhc9260Z8b5ADmTwCkuHNMAIgbvPOsjwN24/I3X1Kzxx3VacnLMT9rGFbLzSkbzXRs4k2Dj0AOh6lTGtxOmoYm988RttZupNmjkOHVc82l2nlhuJpvFqI4/jPpewHU2XNcaxOWpdd5O7wFycv1E6n5Ls4+OZ9OHl5bu+X0Lh+3GHzse6KpYQwEvBuxzQOO64A2XJdosXmxarZHC1xYDuws0OfxSP5E9dAo7s1s1NVSiOFm87i78LBl4nO4D5ngvoDY7ZOGgjs3xSuH7yQjM9G/lb091tP6sfa/sjs+yip2xCxefFK63xPsAbfpGg6LcubdekVUoLtP2dQzXkp7Qya7tv3Tj5D4D5ey5fjGEz0r9yeMtPA6td1a4ZFfRSxq6hjmYWSsa9h1a4XHmORWmOWxS5fP+FYxLA7eikfGf0kgH+JuhHmui7P9poNm1TR/GwW92/0Wv2n7MSLvonXGvdPOfkx/Hyd7rnVRC+J5ZI1zHNyc1wII8wVt3javmPpXD8QimYHxPD2nlw8xwWUvm3CcamgeHxPLSORyPQjiF1zY7b6OpLYprMlOh0Y88hyPRZb4rPMWm+02REWK4iKhKATbMqB7U9o8UN46cCR4yLyfAD0/N9FH+0bbzfvT0zv3Yye8avP5R+n6rmEs5W+OOe9KXX4bnG9oZqh+/M8uPDkByA4LWwB0jwyNjnvcbNaMyTyAVmjgfLI2KNpc953Wgakld32J2OioWbxs+dw8b+WngZyb9Vprk6isy0eyfZuyMCWsAfJkREP+Gz+I/jPy81PBHbIaDIAZADkshUIXPdW+1+mHIxYNbQslaWSsa9hyIcLg+i25YvPdp2lyLaTsnDiX0bw3/lSXLf5ZNR5EHzXN8a2dqaV1qiJ0fIkXYeVni7T7r6k7lH0zSCHAEHUOALT5gqOzp8mhj8uI4KSHaeV8fdzQseBbxDwuG7a1tQCAOFl2PGezegnuRGYHfmgIaPWMgt+ShWLdkdQy7qeRkw/K792+3r4SfUK2b1ZVbO/FZWz22GHxU4Ehm7wDNpZvOcc/xg7pA0FytHj3aHUSgspmCnZpcEOlI6vtZv8AKPVR6pwWeOUQvhkbIb2YWkuOnw2+IdQpZgXZhWTWMu7Ts/X4pD5MacvUhTZO+6S9TqIIIyTckkk8bkknrqSugbIdmc09pKm8EWu6R+9eOg/AOpz6LpGzOxFJR2cxneS/5sli7+UWsz0UlUXX4T0w8JwqGmjEUEYYwcBqTzcTmT1KzUSyosKqoqoCoqqiBZaDarZWCtZZ43ZAPBKB4m9D+ZvQrfqhSXofOeO4HPRymOdtuLXD4Xj8zT9tQsGCYtcCDmDcW4WX0XjeDw1URhmbdp0P4mu4OaeBC4RjOzM8FYKQDee8gRcntd8LunXlYroxyds7npsP/elb/nv9wqrb/wDxVVf58Ps5FPzx+kfGuzLlfanti9j3UcV2iw7x3F1890dOvFdSe6wUM242XZWx8GzN/wCG+3/Q7m0/LVYYsl8tNenBpXXKtFXquB8b3RyNLXsNnA6g/wB8VMOzHZP9rm76UXghIuDpJJqGeQyJ9BxW+tT2p0l3ZRsp3Mf7XM397K392CLFkZ42OjnfTzXQl6svB1XPb3V3tLIFWygebJZekRLzZVsqogpZFVAgqCvSoAqoCIqONggrvK2ahn5gtdUyEuvu34W5HyWW2iJGbrXGgCLdde19szTo4e4VxYbsPPB3uF5G8zp82n+iI6ZyovEEm8Lr2UQqvJXpeHIAWFV4fG6aOZzQZI2vaw8g+299PmVmheXoKbqol0QXap3BYbzcLImzJWC8kZIOf9qmz3exCqjbeSIhsgAzdG42BPMtJHoTyU62WwdtJSxQNGbW3eecjs3n3J+SvQtBJBFwRmCsyM8FbvwhdVt+quK0/VVSuBVVAiCqoiqgIiIKFGoVQIPaqqKqAioqoMCepDH6X3tTrxsRlpayyo5r8Tl9uKxJQb6WNzb1PBe25aXHmp9+InXUna++Yg5H3CSva5tnW6/ZeY7EXPNY80QIztnwv7EpbIrmW1lU0duOXyIV4qxRCzbcrfPNXyoTVV4K9FeSgLwVVxXlB6VFTeRQKlYVTqiKwU+qyG/H6IiIXyrTtURQLwVCiIkCIiCqIiChXkIiC4iqiDyqqqIMWt4ev2Vyo+yImfZr/F4ptFYOp8/6KqJr3U49ReoOPp91klVRRC+1CraoilDy9CqogsoiKB//2Q==</t>
         </is>
       </c>
     </row>
@@ -1139,25 +1139,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TILAK VARMA</t>
+          <t>LIAM LIVINGSTONE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>smat2023_069</t>
+          <t>t20blast2023_127</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>166.7</v>
+        <v>53.8</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1166,88 +1166,88 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="M6" t="n">
         <v>2</v>
       </c>
-      <c r="K6" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" t="n">
-        <v>29.2</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="W6" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X6" t="n">
         <v>20</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF6" t="n">
         <v>2</v>
       </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>33</v>
-      </c>
-      <c r="AD6" t="n">
+      <c r="AG6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH6" t="n">
         <v>16</v>
       </c>
-      <c r="AE6" t="n">
-        <v>24</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>-0</v>
-      </c>
       <c r="AI6" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxASEhISEBIVFRUVFRYVFxUVFRUVFRUVFRUWFxcVFhUYHSggGBolHRgVITEhJSktLi4uGB8zODMtNygtLisBCgoKDg0OGhAQGy0lICUtLS0vLi0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAACAAMEBQYBB//EAEcQAAIBAgQDBQYDBQUECwEAAAECAAMRBBIhMQVBUQYiYXGBEzKRobHBQtHwFFJicuEHIzOi8VOCkrIWJDQ1Q2ODk6PC0hX/xAAaAQABBQEAAAAAAAAAAAAAAAAAAQMEBQYC/8QANhEAAQMCBAMFBwMEAwAAAAAAAQACAwQRBRIhMUFRgRNhcZGhBiIyQrHB8BTR4SMzQ/E0UpL/2gAMAwEAAhEDEQA/AM+BCAhKsMLOUi4BDUQlWGFiIQhYarCCw1WKhCBCCwws7lghBadyw8sLLBCZCx0LOhIGKrezQtlLW2UbsToAJykR5YmpG17EDe52t5zOV+1/sywem9O6nKL3IPUgAXPm1vCZ3iXaWpVuO9UANw1Y52Xa9we6NhObuvoE6GtA1K3gxtAnKKiZv3cwv8I8Vnklauze8d/h6WGkn4Hj+Iom1Nzl07rHML+t7ek7suSvSSsErK7s9x1MStjZao3S+/8AEvUS3KQSKPlitHss5lghMkQSsfywSsEKOywGWSGWARBCissArJLCAVghRyIJEfKwCsEJm0UO0UEKWojgWJRHVEVIhCxwLEBHVWCEIEcUTuWEoghcCzoWHaICCEIWEBCtO2ghDlmS7b8TZbUkGoI1BYHNYHl4EfEzX3nlPH8Sz1axI2quOp0YgW+ELIVfVck3OtrXBO1z5638JzQk206X1sBy8TNNwPsdiq6CoMqAjug318D0kTH9mcVSqWNJ265VJsPTl4zkSsva6d7J9r2VKEue7qNzaxt4a7mAqc7ggdTuLbWmj4J2QxGIcrkZEXUvYk+Sg2F5ocb/AGYkIClRs1jcPbTyyicOqI2mxK6bBI4XAXnVKo6MGRrMCCCDzB3nrXCMV7WhSqc2UE+dtZ5ZxXhtWg2SoLeNrA7/ANZuf7Pa2bDFb3K1GFugIB09SY5cEXCaII0K0pEG0cInLRAkTRWARHyI2wipLpoiNlY/acIglUUiCVkgrBKwQoxWAwkkiNOIIUe0UdyxQQpKCOqI2kfURVyuBY6gnAIYEEqICdURLCEELtogIU5BC6BERFOEwSoJi8L2Uq18RWyi4as5HkDdptqNEuSByBP6HM6yd2SqjM9hqGY7WOqLfQ+e3W8be8DS+qcjYTrbRT+G4UUlVOg/VpNrUKdQAOoNtj9ZT4jj7UmLVMLVKDmuUtv+6DtLDhHa7AYk5ULI4FyroUI+MqXRu1KtmyN2Vph8KiLZRYGNYkptLA0ksCSAPhKLifGsAhKmvTzDkGBN+mnOcBpOy6zt4rD/ANp3Dc+HDqt8rA3G9tR9ZU/2e4crhmY/jqMfRQF+oM3r8RoVaVVV1uj6MpGgX+IeUzfAsPkw9IW/Dc+bEt9z8JZ0twzKVW1ds1wp8REQnZIURCYBEcMEiCRN2nDDInCIJU0VjZEfIjZEVKmWjTyQwjTCCEzaKFaKCE+gkhBGVEepxVynAIQEQhAQQkohgTghiCLrgnbTsUELkFocFoJU5w1wr3PQn4Wb7S/4FZ/a1rDVVCkW1DFjf5zLhipBG4N5pez9VFzqlsrqlTKDcI2qlbfh90Gw018ZEqIzmzDkp1NKMnZne6gcY7OVKpYhmGYWBBIykEG/dIJuBbe1ieesjDhQopRDL30WzOWZjUN737xJHTf+u5pupGspuLHvoB15C8hdq7LlU0MBN7JniuILUcpG9r/eZHCdmR7ZKqLlUA57ZMzMb6oxp7bbn6a7XG0WyhiNOf1knhSgb7RI5CwLqSNpVWuAY4aojkE5GAsORUjnrsZDx+Eo0aCJRFgxBO+ZrDdid+Qmj4tiLI2T3m7i6E6sQAbDpe/pMXiq+YgXJCiwJ58y3qZIp2lzgeAUSd7WsI4lNgTtohOyxVahInCIRE4YIQEQTHIJghNkTjCG0AwQmyI26x4iA8LJUzaKFFCyE4sNZxIYEFzdPpCMapmHBIuiEpgidEEicM4IN4rwQjgtO3gsYJQbJp5L4NXWm1QnQlVt42JvIjSJi6TGzpclMzEDmlu96i1/ScyC7SE7E6zwVszxBVT2hay2uWJ2AlLj+1+FVS61H13KCxNtRa4jKYui9JaRdTmYW05Ag7Ha+lpY4bAEuVSoq22BAsfDUSs7MA6q2Y8u4hBX7dYZ1poKrKzEfgG9iLNmBAHiJa4TGK3ukEdR/SQOLcNqlQXNJx0KA+HOVOHophBVdTlJQEqDpmJsCATpFdHfRKSWclYdosbrTRG1z3uOQVT97SoUSDgHaoxqtt7qeIv3m9SPl4ywBlhEzK2yqpX53EoxFecBijiaRQTOwTBCU4Z2CTBC4YBhEwSYIQGA0ImAYJUEU7aKCE6scWAonRBcJ4QhAEIQQjivBnbwQu3ivBJgloITmaNs0bLwC8VKE4WkrhDf3o1F8rEC4uRsTbprIdFGc2UE6XPgBuT0EXARnxuJc6CnSpUkHRWuxPqQIr4z2Ln8BYdSkjk/rsiG5ueg/lZftRhmwtX2i3NJiSltkbNcobbDU25cpoeG8fw9fDj24GfYWcqdba6bTTYnA06iFaihlbcEaTLVv7MKLljRxD0gdcpGddOnOVvaRvFn6EK0ySMN2agp6tx3CUKOcF8x2XOX1I5X2me4JUrY6s4Zm9ncNUNyLIBcINNz9PSWNP8As1UNarimcA7KoT5kn5TW4ThtLD0xToqFUfEk7knmYofGz4TcpCyR594WCplddlK6WFlI0Gw05bToaZ3gdFlxuLGYlbc+RJOnprNLjsHVom1VCtwCDyIOxVtjLaWMBjZG7Ova/cqaOUmR8T/iba9u8JBp3NI4eGGjCkJ7NFeNgzt4IRwTFOwQmyYBjhEAwQgM4YRgtBKhinIoIT8QMENBvBcKUs7eNo06TBCImcLRtmgNUioRs8AvGGckgAXJ0AG5PgJoeG9mSQKmLqCih2X3qrj+FBc/IxQCdAg2AuVS0w7sFRSzHZVBJPkBLXC8Joq3/W69m/2FAe1rnwOW4Q+es1eDCU1KYThtaoDu1QiiH8y/eI8CPSPtXx6ISKWFwNPm7sGyjwC2BPnJMcHF/wBQP3Pp1UeSf/p55SR56D16Kl4pRenhmK4cYek5UKhN6766vVPIcsvjMZSrmjikbZayimTyzrcqD0uC3qJpeJ4/DOaqU6tTEVsi1HxD6KVRh3KSfhW5voPUzNYiktRSrc7G/Qg3BHiDYy0hpO3pZYBob6cOAtv+dyq6ipNPVw1O4y2PhmcDt3G/jxWvw77qY/SS/OZfh/HwHSjVPfHPw5XmvSjcXEwsrXMcWOFiN1u4nNkYHtNwdQodRbGVvEa9lJJsACSfCTcfWANgMx6CYzthVr1VFFAF9owB6hecWJpe8NG5SyODGF7thqUPBLFKlb/bPmF/3AMqfEC/rPRcDjkyIhxS02YAmniaefD1Lj8DG1j1Ab01mBVFRVQaBbIPICXw7S1sMKdPKlWk1IMaVRQQSSRe/K4A67Te1VJljhgYL2uOGthfjpw/lYGhnL31E7tL2Pm6w79ir/HdmFfvfs7J/HhXFamfE0nsw8lmfxPZuuv+Gy1P4dadX/2qlmv5Xk7B8a4eVFRaWIwpY74er3b6/hNgRp+7LTDceRhZeJow/cxWHGvm6lZXS0DwL5SOh+2YKwirmHiD1H3y/RYioHRirqVYbqwKkeYM6HnopyVlyvTw1cchQrKTp+7SqABfRpRY7sqlTMcGxDqLtQqAq48g2oHQ3IPWQXxubupjJWu2P5+clm1M6TGrkEgixBsQdCCORnc0b3TiMmCZ28EmIkQmC0RMEmKulyKcvFBCStCEAQ1gm0QM6Xg3jbtFQuvUknheBNZu9UWmnN2uduSqNWMrWuTYbnQSwqPkVQNLWBI/5r9b6yfQUX6km+gH14Kvr6402UNFyfoFuKdLCYCmHyZLj/EqgNianhTo7ID/ABWtzEo8b2yxNs1DLSDHoHqHxZ25+Q0mf4i71FNRizOPeZjckDY3MCgmZGHT+pl3TYZDELv1PHl/PVU9RickmrTlAKn8Q7QYxkBOJra7kOU3HRbWlVxBnf2ZqOzFhuzFiBpzPWO4mmMijlofiCfp9YeQMA1trD8/n9JPaxjPhAHRQ+2cbFxJ1O5v4J7hFILWyfv0yg/4CfsZGU233EPEsUelUG6kHztuPgbR9qIqMX90Nfujl6xhjHMnc/5XNb/6aSPUFPyzxvoowT7zS7qCBr5g+aYo0qb1aYOXMdBrrbcadL/WXVPGuvdBMymL4YEq+0XRg2ZH5g9CenKaDE1DkzW72UHkLtzB5A30vtMl7T0+SRk/B3u9Rt6adFsvZWQSwugYSS33uh3A8D9VbrjKdNGZtzKHirhclWpZS2a1+Vsth8zC4Oril7fG2TmqHWw5Ejmx5D9Bupiv2i1lyohOUHVjfm3j+cj4FSSOqRMG+6078NjtzIOumnenvaCphio3xvd7zraDfcb8rjT7KJnBFwQRO8bNmojmKK39WaOUuHqqEEW72405yPi6jPUBY3a1tgPdvbQes27mOfLG7g3NfqLBYmmnjZFKwXu7KB0Nz9FJwNPu5T125+vhICqdR0Nv9JcrvtuL+vj8ZAxlOxuBodfn/WPxO95QY33ce9OI1qV+YIt4eXxmp4Bxs1LU8TUPdI9jiP8AxKTfxN+JDoCD66bZWj/hVPP6yRibKAg/ELfP+kZnhbKC089DyXcM7oX3bz15W3/1y3Vj2rql67FkVXWyVCvus66Fx4HTfXlylQrSSwupH6vISNM1iNKIHNy7Eeo3WkwqsNQxwduD6HZSQZxpxTEZWq0QmNNDMBhBLdciiigi66IcAToMVcJMYw7QqjSLUqQQpvD01Lnl3R5nc/rrH6vyOkWHFkUeGvmdYj0PObOhgEMIbx3KxlbMZqhz+F7DwC5hntodvdPlyMHBtlJT97Lb5CDmF9eYI+H6MbViCp6C9/Q2kwtvdM5b3HNP45gEJ8T9bD6RYB+7lPK3zg47ZegAP5feJMBXUGp7JggsS2RsoBAPvWtsfnG7gN1KVkeeOw8VziZ2knBvmp+I09eXrGMXh6lQXppmsVBygmxc2UacydJL4dwnEhmptRcGzaGwsUUM3+VlN/ETh0rALEgEd6XsXuiFgdO5F+ytXXKiljbNbptf6xnCMcypUuGpkghtLnTRh4fPSWHZ+v7Fzc+9oddl3BtzHX0kbtHXvXZl5FRfrYDX6Sme+GvqXUj25mN1v3jQjw1WhpWT4VRirhfZ77t8Gu1BHeLb8Ezxdc1i5uw67W6D1tImDqZW8Nfz+0f4iQyZgf0RKpXl5E0BgaNtvBZ5pdK0ueSSd773V3iBdbX3NtdhfS5jNfBLRrqKlRXW6sz0u9a+9vKSOFUDiClIbtZb725XtLcOyE0cFRBewBdkDVHqUiC4GU2yEhb3Nt7eECoqDE7I06kG40HW+pFtdgb8VLw+ldI12g0PH6W430uoeIwntHy4c73yE924Avz52Er8R3lNul/vv8Je4jFMxNHHUshO1UUytRCR3LUwSCgawuPLS8pFwppVatJ90010v6XPhpeJSTOcbO4AW43A43Gh8h6hc1tH2AzDmdtOlu7xKhYd9QOXP0BjxfMy/wAOnxAP5yG7WJA5ExzDvpbnqT5y0Iu66jObxCnUTv5yFVFmYfxH6yRTbQ+JEj4rSofECU2NMvEDyP2VhgrstQRzB9CCnkMMximY8WmYWpQMYJM6TBMELkUG05BC6DExitBeKuU1UaPcDwH7RiaNHk7jMRyQasfgDItUzT9katPDUqmKfWo96VFOdhbM56Lewv4ER2KN0jw1u5TcsjY2FztlX4gWd16FgPQ2/KNNrCI/1hFem83Q0Cw5IvdRK9yP4h9evqLiMU3BRGU6Z7EdNdvtJ1WnmFxv069RKmm4JYA2tUGYbam2v653iqTH7zfD8/0r7ggz1ETLmJIGW1+6TYac8t83yno2ArsyMWYlc9RFL6DL7R0TNbkcpF/EaG+nmHD8c1EtVQkMFKAj8OYqSfhceslY7jtfEUvZswAABIUZQ2UsbkDbVibDS8qq2kfO/wB3RvM+uim0lSynaTrcn9uK1PAlHsMtJf8AGZq4BVwcquTRUOhChv7tRlH72YcxLDH4hqIVqXss7PUuuTQ02dwSLNoTkpknn8Z5mMZWyIBVqD2ZOUB2AUNvlF9PSa7gd1pKH1sl7nU662+cpcWa6lZ2lwST+fZXeE5al+QiwaP4/PJRKwWiCzAEjl1Y7D6TO8QxqlQ7HvXKn6zQ8XwtSupCDXMCCdFFvreZqv2Ir1WJq1bL+4gI/wAx5ekYwqvpqSF0jz/Ucetht5m5UnFcPqKydjGizG/Xj/Ch/wD9mmbpe5I0A12Ow+ck4SlUfUUjbxsJY8P7NUqFwEy9WOubzJ1MKrjFBZaXS1ztf7yXHjNVUvy0zB1/LKNLhNJSszVDj4D+NVL7O3pYikKoGSpmp6m6szCwU2BtqV5TRdj8TTw9aqlVgpPczX7qsrsd+QYHTl3TMJRd3Gp1Vsw89ATb0Ev6eOoYkBMYGDgKntUsoCo2bvKouxt/yLJdTTTSR3m1JFnZfEkEDrr0UCCqp4pHNjuBe4zffl3LQ9vcXSqLTWmwd1zXKZWAVxlVSb82sbb90m2kzfaViMSgJN1SmjAtmIYDvDMSb738L25SRVxeDoO9RQ9aoXd7VFUUwWQAEodA1z+EW7g8JQVqr1AXY3Yte/oAB5DSw8I5htIYsoAIa0Ea7m9uth379E3iNUyVuVpBueG3co9a12PIX+s5hGvrte1h0HL7mF+Byeo/P8osD3szdTp5DT63l2N1V3swqYvL+b7QeJLqp8MvwhU919TD4hTJS4/C1/TY/USDibc1O4d111QPyVcZ77eeijUjJBkOiZJBmNK2SRgNDMAwQhiiyzkEqIxqoY4xjVSKuE3TotUZUXdja/IDmT4CXGIpqrBUN0UBVNrXC87eJufWO9nuHgo1Q6EnKtwG0G518dPSO1uGvyOb/KfnpLTC62jheQ+QB22ug89lXYph2ITNDo4iWDXSxPluoMMCddCp7wI84DPNSHBwuNVkntLTlIseRTVY21EyfHMcKVdX/C4AYfrnvL7iWLCg3/XpM5xLCGrhyx3Lqw8Evb6EmRa6fsYxbckWVxhdPmdmdtY3WgpVbWv4X8j/AKxwVlRs34baQlCuijYgWvLPgXZr9rQk1qNNUazZ37w6WW3PU7x2aZsbC5+ijxxGV2UA35KswdImtSFtG1PS1rkTX0m0PnaR8HwPIzezcVANA+UqLc7Ann1k98Na1uUwuN1zKmUCM3a0evFbbBKJ9PEXSCznfQbJylXA0EdFTrtIyIFFzvyA5zjVLb6eA1Mpldpvi9IuLC3rMZiRkqnTTX9fGbGsSQbGx/XOS6XYSnUp0icVkqOoZVZFuTa+guCZf4DURwveXnh91nsfgklYwMF9TfUeC8/qtkcEbH77yVWNnDDY2mzxP9mzMpVcUhqqL5clh5E5rgekquzXZiri/bIWFM0SEYsM3eubgWPK3zE1UddCWl2bQePFZR9HOC0FupuOCpceOfhED/d28BNJhey71sGcSaiqArNlIJ0S/O/Ox+My1VmNM5dxpJLJmSXDTfKbFQzC9jW5ha+o8FRYvixZ/wBnpDvFtT0/0FzLvDBVSw2UW+ExtPEZK9Un33cpr+FfzOk1eFfNlQeBPkOvrO4nF1yVOq4QxrQ0ab+PM/YKww67X6W/OW3DERi6u4RWpVQSdr5DlF/5rH0lZTkzC0Wc2UA9fDzM5qspicHmwtqf96KtiMhmb2bbuuLDn5KnoyRHeJ4X2VZ03GhB6hhf63jYmGu06tNxwW8yubo8WPHxQmcMMiAYJFy0UUUEIXjNSSCI7w3C+0q006tr5DU/IGKkC0IqmlTpKVFwi6bAXFz+ut4IrqdSQPMyD2gxoDm+vgL6+FhK9OLkKR7AW/mAI+AMqZ6VjzeyvqetewALQs2nUfESvxuGp2N7ofDb4GUeKxGKrWCEUjcHMoOYgcjYi8IjEMhSrUzE6ZlQI3yNolOKuldeCXL3X08tin5XUdW21TGD0++4Wfx16tcUgQy7sy7WHI+ZsPWW4oXGUDcWsPEWj3Cuz+Qn2YZi2/XTYX2A1l7heFVF1bKF28WPO35y7mxGSXKXkEjloFQmhjaS2IEM8yqjA4Cpmy9eQ1PkPGaDgtFVqVVsLU8otyzW77fQeQlpwvD0ru9iClN8o5hwAwv/AMImP4LjPZ16gPutY7geH5xisrKiqZ77tOQ0CWko6elf7jdeZ1K3ZrgDSwjbOG90XkKlRzEWUkee8l43F0sOmZ3VAOVxfylQ1pcbDdXBcAL8FExjMvL1kF8UeQ16nS35ykxvbKmz2RHYbZtFGvmbwsZxBPZOuRxUNsrZgFQaHVdST7w3lpDg1XIQMlhzP5dVs+LU0W7rnkFboAcoNTVmVbDa7G01PaX/AL24Yo2Ct9/ymU/6RU6mEwuHFOzUHo1HYZf7z2QNzpzPjJ2M7W0a2Mw+LFJwKAYFe7mN1Yaa25/KXFJhctPckE3Dh6G3ndUlbisU4tewBb9dfJaLgaX4zj2/8tB/koj7Sp7BvbH8Qc7D2p/+Yn7SHwftdRp47E4hkcrXChQMuZbW97vW5cryDwTj9PC1MU7o7e3RguULoWZj3rkdeV5O/SShkgynVjQPEWv5WUEVMQey5+Z5872Wg7P93g1Zv38+vmypPPnrZQ9xfTbxvNFw7tAv7AMFkbNe5e4ykGoW23mYxg97wljSROYZS4buNvBV1Q9jzGwfK0Dqsvx6mRWouNC62J8Qfyaa3g3DLLfPvv3bn6yFjcKHpMLDNlupI2YDQxzsdxdqyD2ltNDYW2mTqcQroLiBwAud7H6grb0NLh9RGG1TCTYW1PLuIWooYWmNwW8zp8BJ4rhFu1go1Nhy8AJH00tOvTzKynmCPlKKWeqq3D9RKSOV9PLQeiuI2UlGw/pYg3p991UcTx/tnBAsqjKL7kXvcxgRikJIAlqxgY0NGwVBI9z3FztyuGAYbRszpchciiigi6IzQdkMNrUqdBkXzOp+QHxlDLlcQaeHphPeck+JJP5AQcdErBqpuL4RTDFj3jqSd7dZDw/CQwzEeS8vC/raTqeIsh1/euTz8/iI1g8dluDzJXyNzp95AzF11Z2DbArnCeCguSde7c+BvpYS5weApWIYAnbX84PDMQEVuZLHXw5feU+M4mc7lCbDVh4XtmHrac6PcUasaFY4uolMkUwALBdPqJ3iqqVUoy6cjtp4TO18cN1BJ6n62lZiMVVZrKegvpb1O0dEW1k0ZN76q2Ti60r5muWa7ctenlbSZ7imCenVz03Pszf2bX95bk6+IvYiMcQqU1NnbM4BbIDsNgT5mQuFY2v7NyzsoYmyA90Dlp18Za0OHPn02HNV1XWtiF+PJaSrj8UiAGoVBqUqdlOpL1qauL9MpYXvudNpCx3C/aKz65hqbs7XUe8BnJsRvvyMueJ4fNqde/Sb09vTYekmDDkO1hoN+m4Av4ayrZXSUpZKzYPcCOYbb7XK0D8OgqGPiduWMLTroXZtvQKiq8AohFYFs2VG1IK3OXlYHc9ZZrwmicwJc252UbeFj9Y9ispFk2Hs1AO/dZFI+sLFVzTptUUKSGW+YXuDuPDYajWWTcSrpzHHDJYvkeASBsAMqq5MMoIGySVEZIZHGSAT8Tr349yqsXgDRs6nMl7G4sQSNL2vpodR05XEm4jgqU/aFajEqHOqqAcoY2vmuL5enOWGOoArWQD8LW/3CWHzUTvFNKdc/wANT5gj7x2HGqqVsDSQHGQsdpuBb91HnwGlifUOsS0Rh7ddj72nos7w/h61WY5iqrlsVAJu19NSNrGPcXwQRFYMWBJHeAGoynkT+98pYcGwv92qlsuYs5b90HS/kFXN6md4tTvRb+GzeQ90/Nl+EmDF5nYsIP8AFcs2+YC+++6huwWEYR+oP90AP3+Unl4LN0HIIIir97Nbb8toI5W8Y+psvmtvPX+k055LKHe6VKVfY2hlxGIp9Kh06A6j5GWtEaSBwgGnj6xH4ght17gvMBVNLQ9p4ErcUTrlpHJbmnTswvJr0OYkTOGZGG1vnLN9rymOiu91j+J4bJUbo3eHrv8AO8YEuu0VHu036Er8dftKUCW0TszAVSytyvIXTG2hmNtO02higxRbIUgiX/DMOKgpM2yKQPMH+plDaTeF8Qakdrjp5/6CNzAlhsnKctEgzK7rYUZdNmv8dvsJU4ujlYkjuuLn/TzlmOMUrEa2vfbVT4GVuJ4pSfS5PjYA/CRI1Ol70KY00bgaqw0vyPT9eEiUyxLgWNx3idABcEgX8hHv2ulkKqjEjY21LHnfoPvGajErlsANPPbwj7WXvoozpLDdBUoqqioXzG2x2v0A3JjK0WfV+6P3Ruf5jHUQDz6mE7yQ1oGqYe++yosVgg1epYbhR6AX+8J6NhlttLMU9c/6sIzikubzZ0EeWFtxqQsfUz55nAHS60OIs1HOpBHs6RNmUkEGncEXuDcc5Kx1c0mLMCFL5W0/C2a59LAjymapKAumsiViUWxJtvlubX62laMAiztOY2DnOsRvm3H7K3HtFM9r2ZRcsawEEi2Ukg/llp66EN/voP8AOsd9krKUdSwJGzZf3hY6G4Nz02mfOMrhEJZTYoRdVv3Tpc2uQNNDJb8Trhb3QHp7Kn/+ZWt9namJsQhkALC8g6/Nt5bFWr/aelldJ28RIeGAgEfLe/LQlXOLq2UknV2Cj+YsM1h0C5viOs7xFCyVlG7ZQP8AerUxfy1lDVxVSpldmBZCLXAsLG+ijQC9pLPG6uQkLTvax7t9L/zfq0dZgUsIgyOBLHFzidLk28dLhRne0cM3biRpAe0MbaxsBffbnw0ViikXZSFVdASwUAWIAuSL6A/Azoo51ZN86sAb3uSLqbje5Cm8o6vEqlUZWCgA3sotrtc6m/P4wjxitSCgFbKBY5FJ7u2pHlGI/ZqdhZL2n9QOzHU256d54kqRL7UQyGSDs/6ZZlbtm2trwsFWUVyjN0NvjDrDujz+U4tM+8Nr/SFXAJ06X+33vNfdYrchKnzlcaoXGgnnSUjzVnEsAfpaVPFf+04c9VcfAg/eYzFY8s8g6+a2GEPzRM7tPJbvAtmAMufwyl4Iugl8RpM8/daZuypuOr/c+TKfqJnlMvOMNdGHl9RKEGWFMfcVXVi0iTGA0ImNuZIUVDFOZooIUwRCKKC5TlT/AA/VvtAw/L0iijEHFS5+CliNvORR9yhcU1AeKKKdl07ZDT930+5ncRsIopvWbrCfN1KDDfeBjfeHpORTl+5XQ+PoncZt6fnDr+6fIfaKKdD4lw35UOF2P65Qxt/xfeKKdu3Q/cqPhfe/XhAxvvDznYpy/wCJO/5OikH3D/L95Df3l/kEUUbSM3PVOU/ufrKri/8Aj4b/ANT/AOkUUymNf8h3gPotZg39pvifqt7wTb1+0uasUUy7t1rG7Ki4r7jfrnKCKKTqb4FW1n9wIY28UUlKGgiiighf/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTExMTFRUXFxcXGBcXFhYXGhgXFxgXFxUVFxUYHSggGBolGxUVITEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGhAQGi0lHyUtLS0tLSstLS0tLS0tLS0tLS0tLS0tLi0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgECAwQFBwj/xABBEAABAwEFBAYIBAMIAwAAAAABAAIDEQQFEiExBkFRkRMiYXGBoQcyQlKxwdHwFHKSomKC4RUjM1Njc9LxJEOy/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAECBAMFBv/EADERAQEAAgECAwYEBQUAAAAAAAABAhEDITEEEkEFE1FhcZEioeHwMzRCsfEUMoHB0f/aAAwDAQACEQMRAD8A9xREQEREBERAREQEREBERARFRzgNSB3oKorWSA6EHuNVcgIiICIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgLibR7VWWxNrPJRx0Y3N5/l3DtK5XpC21ZYI8LC11oeOo0n1RmOkcOFdBvPivny126SZ5fI4ve41LnGpJ413dyrctLY47eh7Q+lu0SEtszREzMGoq89odWg5KEWu+7ROS6WaVxPF7j5E6LBDd73ZgO81ux3Q8+ya9y43J3mDBZLbNEaxySN/iY4tr+YfXmpfcHpHtsBo94nZ7snrD8r9R41XBjuOSnqnetaW7ZBkWO5FRM/mm8fye/7M7Y2W2ikbsMm+N2Tu2nveCkK+WYXujcHNJDmkOBGRBG8HsXtvo525bbG9DMQ20MG8gdKM+s0caDMLtjltwyx0nKIiuoIiICIiAiIgIiICIiAiIgIiICIiAiIgLHaJgxjnu0aC49wFSsi4+2ArYbSB/lP+CD5xv68JbXaJZnk4pHk0PstBoxg4ANW3dl2toKip4lW3VY6txHLXzXdsMQrQaLLyZNfFjHRsNmAAoujDCqWWOgW/GxZ2lqmJWSWeq6eAcVbIAmkbRe8rpY8HLC7c4CnNRfHJZJ2zMqHsNfEdx0Oa9BtTFxNpLEHQE0C6cWVlc+XGWPbbstYmhjlGj2NdzFVsrh7ED/wLMDuiaOS7i3MAiIgIiICIiAiIgIiICIiAiIgIiICIiAtG+7P0lnmZ70bxzaVvLSve84bPH0k7wxhIbiINKuyAyCDw67bNWGlMwaGn1+9FWz9V1M+xdewBnRzYCDR5AcMwRiIrXeuNfdp6OcsY0ucA3TcSASO3VZuTHbVxZad+ytK6UbFDG2+2DPAwDtdnyXZua+nPdheACRlRcfLp3823cEZJSWLgVz73tUjGf3YGLt0oo0L9tWOh6L9Qaf3UqkkpbpKLQa5Kl52YmE6DQcyuXZLykLmtlbTMZ7wpBeszRCQdK18NxVsMdVz5L0TrZiMtskIOuAeea6i4Nw35C8ss8eIlsQOKlG5AAgVzrnwXeWyWXsx2WdxERSgREQEREBERAREQEREBERAREQEREBRz0gWATWKQH2Sx/g1wxftxKRrWvODpIZGe8xzeYIUWbicbq7eN7ORYbPIRpjFP0grlW2zOkxlpIc41JGpruruyXQ2bkcGdE/1g84qaHLI8qLI2jXuA0ByWbPeo2YSeauXYboa13SYG8cJFQTSgrXdv8VgiJFoaG7j/Wg7lJpDkQFFtJw0bnBc/Ncu7rMZOyV2txcRXgubJcOPUbiKigJBqCCaVORI8Vv2h1DnwC7NkphFQq42y9E5ya6uHZrlEeIg0Dj6gyaPyjd4LpSQmSF4ro0Z/lI+SzWh4zVSQI9ciKK+Pdzz7OhsBFW0PfTSPDzcD8vJT5RPYGylrJXne6nlip+4KWLTxTWLLz3edERF0chERAREQEREBERAREQEREBERAREQEREHjltu2az2xwla4MfIQx1Oq4Gpb1tK0AyXMtNRKe9es7a2XHZXEDOMiQfy6/tLl5AZgX+Kz8k1Griy3du4xhETnb6ZKJ2KfDM3E0uzJNN5UgnteJlK4Wjf8FyLvmhx1Jee0NJFeK4YtPV3Z5i9zOqA0ihJOY4ZLvwAYctyixnip6zq1JqGGnwqtq77wb7L603ZqKmy6dKXMlZ2WZ8mBkYxOoXUyGQy3+C0ZpwpRsFAS6SQ+y0MHeSSachzV+KbunHly1NpBs7YnQwNY/1qknfSp0r3UXTRFsk1NMVu7sREUoEREBERAREQEREBERAREQEREBERAREQedelb0isu9v4eNjZbRIypa71GMdUYngak50avNbJbekY14FMQCj/palLr3tdTWjw0dzWNyVt1SODG04DL73rnyR14u6X2a2MdVppwHfvK34WAAkYKqCi0dY0Oeppke1Sm5Z2EZmtO49wWbLHTVx8m3bsji4UODkFfaMAGQBIzB4cfBaNotrA2oGdPv/ALUYtt7agEgVBp9Kab1WY3JfLORMZLSMjlTy8Vi2X9Ihst4/hpqfhpcADtOjeagO/KcgRuyPFcW6+kmbifk0aN0rTeVDds4//K72j5rrw9MtM/L1x2+u0XK2UtvTWKzS+/DGT34RXzquqtTKIiICIiAiIgIiICIiAiIgIiICIiAiK2R4aCXEADMkmgA7SguRQfaD0rXZZqtEpnePZhGLm/1RzXnN++nK1Pq2ywRwtOQe8mR/eAKNB5oIj6TWh14Wtw/zn+XVPwWC6HVjFNwotV8pkq9xLnO6zidSTmSfGq2LlGElu6qrzTpt04L+LTNaLKC/gTv7Vlhs07fUNV032StCKrp2GzkUI1+8lm8zR5HAdYLZJkagdpAC6F3bOYXAv6x4bu/tUwa2o0osMUNSq3OpmEWthDG00Xm+1Qraq+634r0yY0HnVeWXnLjlkdxd5DRW8PN5I8RdYPoL0M2zpLriH+W6SP8AS6o8nBThfLmyG2Vqu8l0JDmEnFE+uB1QOtQHquy1HmvVdnPTNZJcLbUx1mcfazkjr+YCrfEUW2ysW3pyLDZLVHKwPje17HZhzSCD4hZlVIiIgIiICIiAiIgIiICIsFstbImF8jg1oFSSgzrUvK84bOwyTyxxMHtPcGjz1K8d2t9NDyXR2FgY3QTSCrj2sjIoB+bkvLLyvGe0v6SeWSV3F5J5bgOwK3lRv4PaNqfTRCwFlhYZnadI8FsY7QPWf5BeQ7RbT2y2mtpnfIK1DMmsHcwZc81zC08CqFitJFbtrOCt3rM4K10J1AKaI2rHLQUP32LpWZ1CuLEwkZBbcFoLcng96izc0mbxu3ot0xB7O3Ki6djjpu7FGdl7zaaMLhi3fxdleKlkL9xyXn543G6r0McplNxtHMaEpHDrVXRSNOWS2S3JUWR/aScRwuO+lB4ry1xU228tmjB9/YUNhgLj2DUrZ4fHU2y+Iy3ZIsb6pP3p/wBrCwVJPJbD4XyGjWmg++ateKZLXpku29cG0NqsT8dmldGTq3Itd+ZhyPfqvY9lfTJZpQGWxpgfveOtEe2urPHLtXhJCtUWSkun2HZLXHK0Pjex7DmHNcHA9xCzL5JuW/bVZH47NM+M6kA1a78zDkeS9b2T9NEb6MtzOiOnSsq5h7XMpVvhUdy53GxeZPW0WGx2uOVgkje17HZhzSCD4hZlVYREQEREBEVHOABJ0GaDUvS8WQMxO7g0akqCXlO+1F3S5tc1zQz2Q1wIIA4kHVVvq3maYk6aNHBqpHuWnjw11ZOXk30jxT8KGmlBUZbtyyhoU+tUbA94xMFHOFKjiVg6RnvN5hepj5J2kYsssr8fuhYaj41NhKz3m8wq9Mz32/qCv5p8ldX5/f8AR5/JZt4FfBUZFXKhPcCVPi5h9sc/orRZW1qC49zXfRV/BLvp9lrllZq7+/6IOLlmHXYxxbvGnIHNXR2cv6uHP3SD8FO44CNA6ncsU1lNcTGva7+XPzTHyzpsyyt62fn1Q87Ny0J6J7cjQ1IAO4kHNYhftsAwGR/UGdWtxADI1JFcslO4rwPqvacXAjXuOiiu29lAkD2AgSNo4EU6zd4qK5hw5BYvFcOOt6jV4fny3rqldzWwSQxzCnWHWpucMnDmF17VbWtjJ37gMyfBecbIzS1fGwHCQHOJyawj2nHdUc6KafiJA4RQ1xAAvmIHVHAVBA7AB4leZh4PLPO66T4vSz8ZjhjN9ah963dPNaJGkU6P1yTQNJAJFTqRpTiCrBdcpbgjZRvEkAu788h2KZS2Zzjm3KpdTFmXHVzjTMlXsip7B8CD8aL2eDj4+KdL1ePzcufLd2fmhxu+SEU6N1d5Ar5haLoQ41cAvQTIBrUdpGXMZBa1qgjk1a13bkTzC0+aZTVkrhN4Xctn0/f/AGggsbD7KxSXeztHipsLnh9w/qd9VabiiPvc1W8PF64fb9xec/J6Z/ef5QU3eNzjyVDdvB2fcpw7ZuM+0/8Ab9FjOzTdz3fpB+a53w/F8L9/1XniOT4z7X/xr+jK12yC1sZDLSJxrLGalpYKkkN3O3AjjvX0PZbQ2Roc3f5HgvJNjLlETpJK1JAaMqU3nf3Ka3VbDG/+E6j5rD4jixl/C1cPNb/u/JLEVAaqqxtYiIgLkbT2vBCQNXZeG/77V11CttLZWTDuaPM5n5K2E3VOS6xR1jutVb1aLlO9V3GhPLNdW05xhw92vlVbJGGufa7rc57nBzQCa6Hesf8AZTvfHIrsNzaDxA+AVQ1X81V04f8AYx98fp/qqi5D74/Sf+S7JaqE01I50U+ao04wuQ/5n7T/AMllZc3+of0/1XTklY313NbwxODfiVaLws++aGvDpWfVLnSYtVl2ge27k1Z2WGP+M+I+QXQbThRXdM0bqqtyqZI0nXbE8UMde8lR/anZVr/w8cXUL5wHGpOGPBIZHZ8A0U7aKYCR7tGgDifotFrq2n3sMLiNwxF7W5eFeajrei0urths+z1mjYGNbhYNBUguPvu4ntKyxXXGBRrTmaucSQXHjkt2WyVqTqc/oFgjiacquB4Eq2+nRXrvqoLuiG79zvqrX3bGdxHifmtj8ORolSNVXfzT9XLtF0D2XuHfQ/Ci50twupWrD3ih+BTae+ZYJGAFgYXRvqQ6uAOImblkaDC7ia9i49gv+VuCMhpJMhIGIYnyygxtBcNTiJoPe7KJ73XRPurZuN911yDRv6ZKfMK38FMPZf8AqB+ZUyhsTd+Z3rMIGj2Vf3ynkqECyzDUSDwB+RWRrXDV3MD+imojbuVeiT31T7uOXczCI86GpJ0p2fJbjjmqxjhpVWu3nw+/NUt3drTollzzYox2ZfRbyj+zk/WLeI8xT6qQLFnNVu47vEREVV1k0ga0uOgBJ7hmvL74tWOQk7zXzU82ok/uC2tMWXgMz8KeK8ytbyS7x+OXyXbhnVw570jbfHq3vW5YHYrO3sqw+FR8KLBM4VifueG18RQ/JLE7A6SI/nHhkfkVqjJW7YHf3I4tOE97cllj0WrYH9WRv+pXmB81kbJnUGqipi612hkbXPe5rWje7TPIaZ600UEvS0xvJd0ljc52/wDs+eQn+Z5oeSk1+zSEiOMWsFubjAyI1qAQMcuQp2cVpXtcc7oYwyS2yPqS5ptLI6BwBo8huE4aUo0bzqqZOmEkRPaC8ZLQ8AEvyAaz8MAdBjcHOq7MgnL5LHDd8Frniggb+H6pa50rsTpHAVc4NGQdQHqg8eC7d27NXlA8yR9E1zhhxPkbI4A60JbrlrRdrZfY8wSdPO8PlzoBUhpdUOcSc3OoTw1Kpq3u6XKSdElgga1rWipDQGivAAAfBZyWtFTRY5JOCsZZS41cuv1Z/otdO+Q4WjJZYrMGuqM3YSK03Eg6d7VttaGjJVibl3qPMnyrQTofgVruir3hbMjljfkQfBNmmNjyNeayF3EclcWrGKjIabvonc7IZtMHdK8iIu6zS1zmF3VDKYGlhGReRkSHChoDULQdLEyUUssrQwY6l7mkFrQ4uf1yIqVxZnSi39o4n45HB7GN6ZoIxGL+96IAYnGlTgOLGCQaDqnCsspvDpdYj1DRrH1BowEdHG5+J9RlV1M6neud7us7JLZ6ujZIAQHta+h1GIA0PbmsrWncSsljD+jYX0x4W4wMgH0GKgOgrVZMG8Lp5nLysYc72hXtGq2Guyr2VWNwqsXSdVwOunPKqdzspHk3wqrPZV0x6tPBUk0HaVKGe75sMgPBTIFQdnrHsUsuefHE07wKHwWflnq08F9G6iIuLQiO19ZHmPpBG1kZLnYcRxOOTQK0zA8wojND13DiAfLNdy/7QXyPpUguqaaADIVXOlZ1mnsotPDNMvPlvUYLG3HZ3M9qNxp3aj58lllaXsbK3125EdoyIPYR8VZAejnz9V+Xju++1bTW9E8+47J3ZwctEZq1myhoc7Oj2gjw1B7cyPBUsMpzrvd8grr4s5ax4bo7rN/OM6dzhktKzS8lOXZGPd3o3VWwxaFnet6Mrk6MoQhGq+ihKyNldB4rZaKK0eSqoqYEVKuCBVKgYJjmFVwqCrJtQqg5qyGRhVaK1gVyhLhXpsyJnl/SuaXU1aHUyocJqMqbjUa5Gq0rRsnMXPc21yGrSMLxXEaANL3Z7xnQaUUtCteoTurLNEWsYKlxa1rSTq6gAxHtWQq5Y3ORDHIVgmcAansPJXTSLWld1mjx5LphFMqveTVo8T9958llcOs0cASsdnFTi5dw056q4Oyc7wHhl8VNVgPVceJXd2bmzczsBHwPyXDc2ga1b12S4ZmduR8clz5JuO3HdZJYiIsja8stFpeaDdXlvzpqtgCoUEu7bqM0E0bm9reuOWRHmpddV82efKOVjj7taO/Sc/JbcdejDnMvVtW2zY2037j2rLZJsbRi9YdVw7f6hZw2oosMkJBxt10cOI+oV45VjtrCIy3Uat7Kez9FG7G4YRQ1oTyrUDzopXMQ5h7v+iodZYyHyt3YsQ7A4Z/uDlf0VndILFMurG9RuySUK7FmnBIFVyrq6zFe0LBE9ZgVVLKrwrAVkVUlVp2i9IGEtfKxrhqCdN6redtEMTpDuGQ4uPqjmvNJ5C4lzjUkkk8SdVm8R4j3WpO71fZ3s7/VS5ZXUn90+kvizkgCaOtaDPit5xzXlE4XoOzd5dPC0k9dnUf3jR3iPmo8P4n3l1V/aPsueGwmeFtnrv8AJ3GlVYscTtQr2HJa3jsoVJFb0gVZDkoFuLILBK9C/XsJWvM9WkRtgtUnwKpG7GdM/VJ/hFC6niaeC1rZLQDvpzpTzot6xx0Ffun9cz4rrJqbcrd3TO80GWpyHjoqlubW7hmfDRUZmSToPjv5aK+PQk78/Dcq1aKau7grsVHNP3qqQjU8Va45qtWiR/2gezmi4PSIuPkdveV85NWSL12fmCIodnuth/w4v9sLdaiLSwtH2f1fEKMQ+vJ+Y/Fyqi6+jnO7Kxbln1HeqouTq7sC2kRUqzIxZiiKKlHNtv8ABZ/uD/5coU5EXk+M/iPr/Y38rPrWvMpNsD603cz4uRFXwv8AFn79Hb2t/KZ/8f3iYRalZdyIvZfEsZWY6KqJSNJ2rvvcteTVEVkObb//AF/nXYh05fJEXT+mOP8AVVW/4fP4rNJp4IipXSKs0WI6lEVVlyIihZ//2Q==</t>
         </is>
       </c>
     </row>
@@ -1266,25 +1266,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TIM DAVID</t>
+          <t>HARPREET BHATIA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>t20blast2022_133</t>
+          <t>t20blast2023_127</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>72.7</v>
+        <v>53.8</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1293,13 +1293,13 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>45.5</v>
+        <v>69.2</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1332,31 +1332,31 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="X7" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AC7" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="AD7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AE7" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="AF7" t="n">
         <v>0</v>
@@ -1365,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ7" t="n">
         <v>0</v>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBANDAkJDQkJCQkKDQwNDQwMDR8JGAgZJSEnJyUhJCQpLi4zKSw4LSQkNDg0KzUxNUM1KDE+QDtAPy40QzEBDAwMDw8QGBISGDEdGB0xND8xPzQ/NjQ0MT87MTE0PzE/MTE0MTQ0MTE/NDE/MT8xMTE0MTE0MTExMTExPzExMf/AABEIAMgAoAMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAQIEBQYDBwj/xAA7EAACAQMCAwYDBwQCAQUBAAABAgMABBESIQUxQQYTIlFhcTKBsRRCkaHB0fAHI1Ji4fFyQ3OCkrI0/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAECAwQFBv/EACQRAAICAgIDAAMAAwAAAAAAAAABAhEDMSFBBBJRIjJxFIGx/9oADAMBAAIRAxEAPwD0Wlooq5AUUUUAUYopaAKKKR2CgsxCqBksTpCjzoBc0fI1k7jt3ZrN3cUv2lQGyyIzBjnoQCMVA4p/UWFE0W8EpuG2PfLpEIxzwDk+2R7io9l9CTZuwfwoIrzDhX9R3M/c3saC2kfStxChjaMdCykkEexyPWvQRxOJAneXESiQZQlgmvzG+Mnny32O21E0w00TsUUxLhGAKyKwYZH3dQ86cGz5H1HKpAtJS0UAlFLSUAUUUUAUCg0UAUtAooAoz70Zqk7S8Vays5LhVBmIZUDHZSASSfQAE+pwOtQ2BvabtNDw2FmLJLdsv9uBW3cnkT5D1NeRce7Y3t6skEl0/cud4owIUx5bDJHuar76/eVpriV3klkKrqY6jk7/AKfWqkDmTlj13rO2y9Udo5sg6iwB2JU0xyAcY0kHZl8OqnRx5BdfhOkHfzrve2uGIU6tCrq98D96i1YptHBHyCM5xuf9hXdrlyghMkjxo2pFLlgpxjIHLliuVkmZI06MWX5YNOePw/5AK2fkdvqKm+SatEu24tLHpCyuUQ50s5YL/N60lr20VFUMt7FIAo1W7pGGOeZAUEj0BGcc96xhXSx1ZKqcFR505kIycAZ3wD8NFwVPcOzvaRbnEJvrS7bQrI+DaGYciCDkggkbDOQc1p0fVnbSRzFfNSSOjKySSROOTqxT8xW/7J9tJIHis72QmNmVQ7HbSeoxyPXAODvjfnZMho9YxRTV2IAOQeg5fKn1cgaaKWkoApaKKABQaUUuKAaxwCfKvM/6odoEAXhUTB51YPOynUIQQQE9yCCfLb5eg8XvktLS6vHZQtvGz4P3iBsPcnAr51uZXmnLuS0kj63Y82JOST6nOapJ9EpdjrlNSEA7tpYe4GMfmarkfBzsem9Wk5CtJyZYy2QD8WcfrmuVtZmRhgHJZVC43YnkKz9klbNPVt0htuxCkAEow6/PH5n8qHd9Tnc94F1H5j9q9L7Pdn4Xg0vD4ozpYsN89asW7IWpOoRsNuWdQrF5lejb/HdbPJ1OHMiggorafcknP4UwS4V05kjSPz/c/lXo992IRmJik0huatVa3YV1VyZAW+6MVKzRZDwSWjDSsWY6dgWyWPn/ADNODhRpyM4wM1Y8X4LNbyCMnUDupA01W90xQnxBkO/3q1jJSVpmUoOL5QzUW2LEgbDfTtUy3mKxsjMWjbUNO+OuDv67/wDNQlkKkfDt00jH0rvIxde82BBxpANXKnvPYy++1cK4dckln7vu2ydRypK5PqcA/Or81h/6V3Ub8LNsrZlgnkDqTuoIBB9t8e4Nbg1daKPYlIaWkNSAAoFApaAUCigUtAef/wBV74xwWNp4hHcvK7Y8OsKBgfiwPyryRGUlpAzaiWyp5V7Z/Uu1jk4VJNJ3atbOjozDxZO2FOeZ2yNxgegI8Q64DAA75ArOS5svF8UdIjlskEjOTt8Rr0Psd2c7+KO7mYxJrV0VRpZyCCDnoMgeuBzFROxnZ+ORBeTKZVzmNWG2c7k+dejW5SNABpGBpA+EL6VyZJpukdmOFK32do7VEQRoqxgDbSPzrnjGa6pJq1bimOmN+eeVYs0V9nPTypSg3oGcgYNP08t96irLWZrtNwwOiyYGYznI54rzu9iCSyIRpLMoP+3IV7FdprUqcZxXnvbDg50NcorBk+JV8WoeY/KrwlTopOPtG+0Yl4sOBjAJwf8AWmE6XkTcgbZ9K6pL0fxDkPOozDVJzyCM5rtRws3v9LJ1TiUkTSGMy28mhOkxBBwfYAn5V7BXkP8ASmzWa9ubpyhe0RdChhncnfHkMfIkV68a0jopJ2xKDSmkqxAgpaKKAUUtIKWgKrtFwZOJWcljJI8QdldHUBihHI46j02rwzi/B3spZInXUA7qrqQyvg8wfUY519BXMndxSyEZEaM2PYV5r2o4Wk1jb3JfRc64lVcFu8yRsfXc4PpWGWXq0vp0YsfsnL5osuFyJacMtGwMiKPAyF7wkZxmos73U7CTBVFGQFcqF22xvg1cC1TuIUddYiVQvh1adsVUT/amkKpbmODkjuSqoMcyAQTn3AHrXGmmzraaj/CtPH+IW7CP7JI2GyWZdRcCrzhHar7QywTQPDM7KAuNs1iLq4vWaUyqYhHurLGY9W2+45748613ZKR5VV7iFCU0sj4Clj6jpVpJJFY233/s1Zl078lG5P8AiKpuIdqLa3JBk7xsZ0qCxq6uEUqwO4I04+Veb9obpLecxRWaKSy+Nk1as+Xn+NUirdFpWkXT9s0kYLFA7E9W559hTzxAypItxCyRSDAfTtg+efqM1TWHH40kFp9kue8UqupYw4Y5xgAYJxvyPQ860FlexXeVUhjj7pOPUEbEH0NWkq6Ii77s8649wZrdnkVg8Yff/UHkfYiqgpgE4yeWetem9p7FfsFycDWFypI3UAggVi+GdnprqJZxJFBGpZV7xtAc/wA2+Vb45r15ejDJjftwtlt/TDhc83EI72MFLa0LGSQnbJBAGM5JOTvyGM+h9rrM9jOzKcMid1ma4kutLM+NIwBkADpzPU52rSmumOjllugpKWkNWIClFJS0AUCiloDlcJrjkjIyJEZfxFefcYk/vcHsCdQSWOR8feIUkfz0r0asXx7g+mc3iK/exNGQARhlzz5Z2A6etcudaaOzxZKnFss7cZGOmFGKLldK89yORGoNXO1kGhWyCGCkGn8RkTug4bBxg5PxVyI66tmdueHLcOA0kca530pvV7bWqW6pFGuEXbJ8RY+pql4fdI9yI0OuQBmbA2QetaCFGZwpKpjUwJOkYApyS0kDybgZ2PIVQ8f4IlxpnSTu5F2weTVdSIcCQEsqnSc/jUHiN0saL3g0LIcahyQ9M0Td8BpMrOHcO8QZ4YzJjSXVgpYYxzxnlV5Dw2NcMII43A+JBpPzPWoPDHDNpDat9iPvVeSNoAGoMcZqbdckOKWip4tbiSCaLo8bLn4ulUdraxScEgMYBdF1MQTlHA8jy3B5c81fcRfEcgGMlWUfd57D61RdnrRxLPZKHezYqiMy6Q4JGD6/90i+l2TSu30j0LhaFLW1Uklu6jJJO+SAf1qXSKoUKoGFUKoHoKDXpRVJI8iTuTf0DRRQasQGKKKKAKWiigCo19b94jBSocKwGpdQYeRqTRVZJNUTGTi7Rk4ThcZHh2OKz3aLiDDurePLSTDK76dvP2rQ8RQxzzpyLNqQbYwd8/WqTjPDWkiWeJv70cbRjA3xkEY+QrzmvWTTPThJyimvg7gQisoZCx7y7kPjceLV5AegrkePFZHdzcumVBAAYRn02Bx7k1DsLK8jEMzTJLbPq73MfjtifmARyq3jte+YAXNmV1sgMsBjLADIO/P9Kl7vZKTr4Q5u0OtWSIOHJ2YDZR0O43qWlyl1A9rcKXEqKurbK+R22Bp72TLEZGvLCNFdl0pGHOADuN85OBgetU17cXYdI4LWO9RwuplT7J3ew5k/P8KJfA/7Zy4fJJZTi1kLOjH+3J0kH71rEl+EnO9ZqzikuEWGWLRNHKrhidXd45kHyI2+daJlAMa7+EYwPaqSdlk3XI0oryBGKmMfGrYw48vnitFwuzVdMoQIgXCJjTpHLOKidnI9TXNx4CoZY1Yc1I3I9NzV7XXhxJJSZxZs75igpDS0hrqOUKKKKAKWiigEFLiilFAJRSilqAZ3tYNC204BJDsjAfeBGR+f1rL3N82nSrPojOplxq14Hn5CtZ2qb+xGAuo6mfHxasEfvWLviI2YZbuXOlXUGTkOR8hz5DpXFmpyaO7DagmXHDp9SggjU64wc4b38q5Xd4kRAeIxgDcoukN/PaovCL5QzqyqSDpDAhtXIbn51cvHG+GYR+xUNvWOmbxk3plbbXsbtpUGTBxpbl/1Uu4lCKQQqKPiVcLsaEijRhhEQscDSNO3tVbxm6COkatryWBUeEcv0wacvRMpNLlku0u1ZXkUINR0kDxeX/Fc57oLrOUKqGOAdJb1+lV8LtFGkYWMySKuwJQp5H335VIgt/CC5LmRlX/IbkcvLPKlJFLbRueBxaLKzB1EsisdXPJ3/WrA1wsf/wCe1/8AZi+grtXpQ/VHmy/ZhRRRViBDQaWigCjFFFAFKKMUtQAorlcTpEkk0jhEjGpmP09/SsfwjtvLeXNzbpwZ0ggkZDctcaQuDgAjTueuAdvOkmor2ei0YOTpIte0DapI48agqfmSdvyFZ24tlmSSByU7zTpYnqPLGORq5mZn7yVzrkY6j+P7VWCPxSEgsCN1bxdOY6da8ycvaTaPRjH1iosytzbz2bNJHrnijbfBMhXH6bVPsu0SEASAo3i+I6dv4KvI4w2VwrNp5fCGHQefKq2+7NxygsoWKRjuVOj/AINWUk/2RHo4u4s4XPHo1BKuC3MYy2+euOlVMd091JpwUXMhbLFS+CMZPQAEZ9DVhH2aCMveSF1B3OrSMev51aw2iKGRQI0xkBRtnzxj6mp9opfiHFyf5EWztsASO+4bSxPiGOuD5e/rVwihir+ErhcYxjYbHHnuPbFcEj2DEk77qp0jf12/CpFsNRLZL/DpJPwjyxism+y6XSNZw1tVtbHyjVfw2/SpJrJJ2haxntra4hQcLkPdi6XObRycgOOWCTjPQ/LOtB5HIIO4Ir0cclKKaPOyxcZOxKKdTa1MwoIopcUAtFVnFeO2tiMXF0iSYyIk/uO3lsOXucD1rF8U7fTyM0dlbx2sfISSgTP745D2Oqrxxyl0WUXLo3t/xGC0Tvri4jtoycAud3PkBzJ9AKx/Ge36KrJYRGaTl30ylFT2HM/PHzrDXk81y7T3E8lxIRgM7FtIzyA5Aeg2pscOxP8AstdMMCXL5No4V2Xc3EpZ5+9mmklEgQrqOoID0A5D5edWnZ6UR3U9mVAW4DXCNn4zgAj1O2fxqnhiDKq4yV3UenUfjv8A9VKCMyxyI+i5gfXG/wAWk8x8iNsdQanyPHWTG4rfR0x40bGZPCB0qFJEG6c+eD5104fxFbuASABJkbRLETvCw5j26g9QaV257AeY/wAa+blFxbT4aNU7Ii5QkbspKkZb4T7n50AN4gxP3iNXl+tdpBzIAIHMY2xXN3Gd/Dg4OTQmiMc6hktnwrsSw+nOleLP9zAY6GTG/M8zvzrqXB2DEkdTzpwJK8uvI+EVOg0c0i1YOlVYBVLEaun5/vUy3TbGxICgf60yNfu4IBGx/n851LjGx5DHXpUbIfBU9oFAtZIzgtOyxqD4tWTkn5AE/KoNh2guLV2RZTLBHEx7l/ENsYAPMbZ5behxTeKXn2icMhzbxKyxkf8AqebexwAPQE9aobl9Kv1eZv8A6gfz8D6V7vieP64vyXLMZ1LaPSuCdrLS+0xrJ9luTsYJiFLHyB5H6+lX9eAtHzIyDnNaDhHa+8sgsbSC8t12CT5YoPIHmPnkelWnge4nLLE+j13FAqg4D2stb8KmsWl2djBKwUsf9TyP19K0Fc8k06aMWmnTPCiGZjI5Z5HLMzMdRY9SSeddEQKPMnnXQJjO29KRXqqKR3JUMI5+3610Iwo96COft+opXHhFWoskTIXwFPXnU1Dkg5wJBj/xP8/nKqyI7CpMT9DkqdmFCwryyQzC9tz/AH4hpmj6XSZ+orS2XEUukEsbZOMOhOkoaz8kRbTIpxIu4YcpB+/89orI6t3sB+z3KnJQ+FZvMV5nmeH7/nDfa+hOma9zufu+vrUdzk76WHX7tQeF8XW4zBKpt7tAupGGkMfMeYqe8G5+Lccx4q8WUZQdNUzZcoFQfFtj/wDNdEHMjIx6aqSOE4zzPiFMvLhIEaR5NCgqB5t5AAbk+lV5bpB8HcNjJJGFGSxqqv8AiP2gGCIsLQbO4O916D08z19ucCaeS7YlwYbQHaIkZk9WPX25Drno93CrhcKoGCx+7XseJ4VNTmv4jFuzlMQA2dgBhzjZR5Cqq48RaQj0A/xFS531YGCFB2H6n1qNMPCa9airIoTbNNePpjO1dwPDSEb5qKK0Qmi5D51e8I7WXtjpjMn2u2XbupyZNI9DzH5j0qtI3X/5Cho89KrKEZLlFXBPZN7v511W1DqdJIcb4pxjAZkEhUg4KuNOn58qk2ylSH2A55HiDCrmyKnBAYEbgMDSg7Y51a31sJD3kYJLDDjGkZqtWJgSCpG+KkihEGOldVbfypNHoR70LzxQEuGbSCMalO+nO/y/n713d9a6lCSAcwRup9fI1DFu7DKqxxvQutWGVZWHUc6A6OQ7I2gBkPhYc1q1TioVAXwpXmTy9/8AioCjVu0bKf8AICot0wCtG5yH1Ky6Q2seQ/f+Dl8jxIZl8f0lScS/XjMbRM8DLI3LbzqrmbWwlkYuw+EHxBfaolugVQqosUa/Ci/U1JTfLA5AONQGr5Cs8HhQxcvl/wDA5Ng74Go7Doo51EkkLnoAOQHJafIrN8KyOM8wummCNuqMvuK7iBhHKmSjw4rsUP8AifwpjRMeSOR5gGgZHA2ximsK7FGzpKsp9RppzW505wcUIoiEfCfWuqJnJp6W7HTlGALc8VJROexAB22oEjvfjTOkgGNS5Irq45MAAxGCR4aKKIsh8ZBRjpQnGCcajULLIx0swB6D7o9AciiigZ2DnbZG/wDJd/yoLcyFjJ8yur9aKKAf3rYAGjHiJUqWH1/maWFyxxk6Oo2X88UUUB1ki8OVLK3qxb9abDYXEsdxcRBXitgplbJXbOcAEZJAyTvsAfmUVlkk4q19KT0Olt5ora3u3hcW8xwkioWD/LoD0ydxyqBPeMgCrGyO58CkBT7kb7UUVOOTd39ZCb5JFtE4UySSSFjvpDFAvyFKwwc6nHuxb60UVcuhpc7HUc/nTCSc+J8kdGK0UVIODSuCRqIx5gN0x1pyzkqQCQxODsP2oooQtj3JVVOps+LJzu23nUe3l8UhBx5DAz70UUfRL2j/2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTExMVFRUXFhcYFxgYGBcYFxgXFxcWFxcXFxgYHSggGholHRUXITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGi0lHSUvKy0tLS0tLS0rLS0wLS0wLS0tLS0tLS0tLS0tLS01LS0tLS0tLS0tLS0uLS0tLS0tLf/AABEIATAApgMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAABAgADBAUGBwj/xABBEAABAwEFBAgEBAUDAwUAAAABAAIRAwQSITFRBUFhcQYTIoGRobHwMlLB0QdC4fEUI2JykjSCohWTwiRDU1Rj/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAECAwQFBv/EAC4RAAICAQQABAMIAwAAAAAAAAABAhEDBBIhMQVBUXETYfAiIzIzkaGx4RTB0f/aAAwDAQACEQMRAD8A2xqIh4VRpnVC6dF5JoXisNFBW4LGhGeEoLLzV4IipwVIUAQWXX0byoCYHggLLwUBSSNERGpQDhMSdVWQEUBYL2qJvcFTjqU08UFlgDtAlPJIXEo3jqgDjooCgSUS8oCKEcUS46JS7ggC5o1UQw0UQGKGlQAoAlEOQggvKCUwegHIAygjf4KdZwQBvDREHggKnBG+gAGJrvFMHBNfCAQNCLWjVcxt/paGE07PD3zBdm1vAany5rW7Etr3mo6pW/mXQad52AzvFrXSCfhwjIkjJdmPRzlHc+Cm9XR3RapdWk2Pa3dY1r3fGx3ZPzU3AS3cZa6SBh2ZiSVvn0yIBEE5AwCeQOJ7lzZIbHTL1yVk8UL3FEtSkqoCXHVG8UsoSUFj3zopeKUlTFBY98qJASooFmPJ0QLlOrOql0qStgL0RU4KAFHHRBZA/VB1RRxUbUjcEFkpu1T4IB/BOHDRQLC2FqulloNOyVS2QSGtkbg5wacd2BI71tgQtd0hph9nqU97m73Na1oBHbc50BrWmDJ4DMgLTFW9X6hnnWy7O6o+42BDSXOJhjGN+J73flaNeQEkgLKftwNdcsVJrrpH8+swOe4gzeZTdLKbZykOdqdwwdoWpoaLPRxpSDUcJBrPGRJOPVt/K3m44nCmtaOqjq2jIZycd+RC9LJnlJ0uvrv/AJ9JDEbLaG29pOaS60vAGYp3aW6P/aa3cIXMteb184umZOJJGOea3lO2Wh9O8abDTL7l66fiibuenBU2PZhq2kU6bcA7GMR2Tjy0WalGN2WlF1Z7FUIk6cUgASMZAAzwTQvMimkkQ2RQhDBQFSA3lCZSyiHcEICohfCiE2JPFFreKNxEtOqgkUlED3KFxFreCEBuoFyBEfuilk8BDgp1gKgbwTdUNClgIatT0j2Q2v1RJ7DA/rWbn3Q80jhmQ6ofAarb9XzWm2/tB9IFlJo6xzZDnYtGJGW84csRnktcGOeSajDsiUlFWzy4u+HCIcu4sFts4odtrCzAdpjXEcYO9cnW2TVukuaW5kZY6jBYdkr3XtvgloMxMSu2UOa8zWM9vJ09o6SQOquU/wCHns4AOAbMHOCccYhd5Z7CxohjWtH9IA9F5oK5tVZtFrnOa57YDrswCCZIGOAK9SuEYDyXLqOGiMktwvUkKFh4KXTxRdTPFc9me0R1M8Et1ycUzqVApsbRQHImRuTFxQFQ80sUAPOiia8VEsUYgqHVHrXarG6xEVEplbRlNrmEevPBY19QPUE2jKbXPBMKs/lCxBURFUJyLRm9cPlTCo3QrD6ziiH8UJtG2sLGvvF3ZYwFz3aACfovNLbbKlSqasGSZA+UbmjgBguv6SbSNOi2zNgdYL9Q74nst4Ax5aHHQWYNhfQ+D6fbB5ZefXt/ZyanJztRk19nVm0addzYp1RmDLZBIun5X4ZeZgrjLZY7rnYYZicoXp3Q7b7aLnWesA6hVOTsWtccMQcA12HAEA6lbDa/4aCpeNGuGtcZa1zCRB3OfM4Y4xpKrrMsFNwzqn5SS4a+fzRpg3bbhyvNehzHRC3Wd4udTTpWhoh4a1rbwGbmkbtRu5QV08rkuj+zKllq1qVdjQ9rg0OGMzJgOgG6cCJjNb8uXj6qKjkaXXBtF2jPvnRLeWEHcT4phUOpXOWsyy7goHgbliis75kTaHajwQWZJIQw4KgWk8Ef4g6BBZe1rUFQKw+VRBZgXUQxUmdUcdVejIvuJSwKu8dVY2oNVBIQxEMQvaqDgUsmg3Ewbjj7CUAqPyxUWNqOY2taw+vUMzLjGl0YN8gFV10LF2jSLaoduJ+8/fxWSGXhhn68O9fXaLLHJijs9EcGaLjJ2VVbR+vP37zXsfQnaNR9ko3je/ltOuDspOeS8UqUpyPedNHaEZT7PqHRW1TTYKZLWNpsAGrg0Xr0YGCSOczK8rx2UtsPf/R1aJK2dla7LScbxYC4tAxAOAJLceF5/iuD2nZTSquYeY5HEe+C7GjbJIact53jFc/0rd22E4G7HMDL1K8GGXdSOvJClZpbyglAKArUxHBRvJQVC73KgWEuRvJA9NvyPghNhB0UQunQqKOSeDClQFbMWJvNT+GYtCuyRrEFthZmaBM2izdCWPhs1ICLQeK3IDOHgjDVFk/DZqA08VZ1R0K2ZAGqGHFLHwziNoWe+wz4jcf3WrsVUkQc2mPBdBtBjqV9jT2T2myBIM9oe9QuVc5zat45OwPPcvQ8KzvHk2vpl9ZpXt3GfUfm7/MDdpUb6ELrOiVOpXaKbTcY0m85uZB7XdnuzXKtph8QbrxloeC3HRW0Povex0sBaSBli3GBwgnBer4rg+Lp26uqf6d/tZx6J/fKN1fB2X/WqdO+G4i64M3E3QMpzOfise21DWbTqOJxbgCBImMMFo9pUXdW14zYW561LwI8SFt9llxoNDolriMMoOIzXz0NLFaVZk7e6mernkoZpYKVbbT87tf2VNso1Pn9la2xBZF08VA07vqsrOXYihtlGiY0QNyvLeCLAN8+SWTtRQANEwcArrgOSU02+5QUV3xwUVhoA4mFEJowo4SnA4e/qp1R4phS4+iggBf3dyLX+8EDTOvmECzUpQLA/grByWMWDenHNKFl4ATAawqA711RvHTzQmzGtmyRWjG6ZK4/pDsc0YYSHTJkTuy+hXo1lpk03EQCwg5xgefJazaWxXVKTiWzUOLTOZ0A0jBZrKoS5Z66cMmJc80edbPtDSQL7A7K64xPDRbX+OZENxIOUy0EZ47/AEG8haK0U3MJbdhv5nNHbPAEnJWWW3tiGMa0ZYyXYboEAL7HS6uOSCVr5ny+bC4T/g7s2ptWx1C0gVC5kj5TfbHMYZrM2HRc2k8OcXGWnlhEBcNTtO8HFeibLNF9C/RBF4C9Li5wcMwSVwanTQwaecIXUna+XXH7Hfhy5NVnU5V9mLT9X2M1h1Ux9lIHhAv0avCJsa8dUQeP1SCpwCjnmNyEWR3An0UHMyq5Ocouqu18kobi9p4/RRY94lRTQ3ALRqEBGvkVYTwRvHQKAUlEEcfFWFx0CSeCkgBfwRaUw5oJwRyMHFG8fYShJWqBjXOOTWlxx+UT9FNCzdbJsYeLwN8fmukS0tJ7JGYOa3lOygG8RBybmbvGNV88Udo1WPNRlR7HkyXMc5pJOsHHvXR2DpxtC4+bTfuAGKjGuJBcG/EIOBIznNM3hc9zlFpm0NQqpm56X7D6u0VAMj2hxDsfWR3Lhdo7OLDeaOY+32XXUfxFquYWWqzU7Q38paTSqN/tJDh6Ln9o9JqRd/p6rBuBcxx7yI9FOHFqdPK1ETljyKmzVULVxXRbB2y6iSR8LviG4xkRxE592MrjrZbg915rLs8cTz3LIsls18+C+iw51kjtyLvyOBwcJboM9bstpbUaHMMjzHAq50rj9iHsiox2M93IhdFYtptfIPZcM5yzjArxM+KMZtY+UdSxz2psyjKBlX3eSBC5ypRihBV92ULqkiiotKitDFEFFbSmL44JZRhRRaxmv3/dM13AeaqKAHPxShZkXuPkURCpATXUoWN73LF2zjZ6wGfVP0+UrJuFMKM4EKVw7FnjgWw2ZiKo1omON19N/owqradi6mtUon8joH9pxaf8SE2zn3XuJOBp1vOk/Hxhe03cbRiIAq7VQvN8wrE4WpBoLq7H8ObTdrvpHFtRnMXm4jxaXeAXP2+mJBAx3nd7zWf0fqllWjcOJqNJPC8AR5x4rDLjuLRZM63bNkNnqtfQa1lN4IeAMAcO1dOAMHADQrLsdpY5lxjexM3zF9xiBB3NkuJP5jGmPTFy0G1dnBjXvZLWwS9gygYks0IzgYfXzIZfI68c64YtLababwwmW5T8p09Vubq4qx2Z1c3A113EGo4RLBkZ+YYbl2lAQ1rTJIaBOsCCVXJV8DNtvghCitQwWZiVhRWFRBRiIXj7+yaUS1BQl9NfGqgA5KXBqgCE6RrQmwQD+PvmnaUgTh3soDhvxFsV2pTrbnNuO5txae8E/wCK5Zhj3rgfKV6V00snWWSpleZFQYfL8X/EuXmbDu1yXq6WW7HXoZy7N5sixWV7Ca9rNB0kBoovqYRIdLd04ZT6rH2vSoMe0Weq6qwtBLnNuEEz2Y1G/nwWvhGPP1XXZQWs/sOnEfVW9EnB1qpNO+o0z/biB5LXW95m7xnxGCyui5i12c//AKsHiQPqscjdMskezFI46HyUe7gkM+9fsvFNCTOvmgCgAUceKAmKaSEg9ypAn90JCXKIHgigKY9yoAka46HxTSeKAcgYQgWe8FBMfooAR+yAZie7yKqA4/ROAgCE7eaWU4dzQALQ4FpxBBB5HBeQVKFxzqZza4jvaYK9la/3K8v6WWe7a6wylweP9wBn/K8F26KX2mik0a1EJWuw94FEFekZmJWE1hwA9FsdjWf/ANXZyP8A5qc/5ArCDf5jjwA8lvei1O9a6I/qJ/xY4/RZ5OISfuWXZ6Y4JETzSOe2f2XhmwQUo7/JB1QcPT0QbXjd78FJHA86KF/AeaQ1ycYAQ606+Q9UJLC4+4UVQP8AUogsqAjefX1yUNQbimBkYD0+yYMOnvuUEld48UGuKt8B3KY7/fhmgoQyNx8ZVrApdHHvTtpjP90FIgbr6ImPYKZtLn4pms8EFCYZ5+XNcV+Idkh9KuAfhLH8gbw78XeC7K126nSbNRzWjdJEmNzRm48AuH6WdJmV2dVTpmGua4VCYMiR8ETBBI711aWM96klwUnVHLl2P13FOqW2gb2loORzHinYvVsyDOPvRdB0L/1Lf7X+i50GVvOhxP8AF04n808rjv0Web8uXsyV2eiu7kAwqy/KGa8Q2opxG5KSTnuHj9U5bKY0xr9FNkUVXVLqc0xOY8U5YEsUVgDdEd6iZFBRSG8vFMQN8jw+6Z1MagxxPnggWhQXFaOaIMfsU7I17iiT3oANfOAPknHMJg7hmrL2H6oBGtdG7xK1HSHbrbK0ZOqOHZbw+Z2g9fS/a+3KVnBvPBfEhgOJ0mPhHEryzaNufVqOqVDLnHuGgGgC69Pp973S6/kzlKui/au0H13l9TtndjEDRo3BYBqEbn88z47+9A1FWakmAAScAO0STuAA3r0uEuDMcPjG8/HVohL/ABUCAt2/oxUp2apaLR/LDWi4wDtlziGtv/KJOWfJcwqKal+EmjY2b4Qux/D6yzUqVflYGjm8yfAM81yND4RyXo/QWndsocBi97ye51wH/istVLbi9yYdnQGeHikcSiXZ4efPRJHBeUag4T4pQU7ByKe8NAPHRAVgDMogiVbfHDxKETvHl9UJoQ8I70FbA1HkogMNzsv2UkaBAHn5otHuEAzJ5cFcxUgcfJbqz7EvMpiS6pVPZEhrWgNvFz3XSYiMAM3AcVeEHN0iUrNbjr4fTFct0t6UGzu6qnDnkSXGOxOWG90Y48M1h9LukVWzWqtZmuEU3XLwZiSAL3xExjI7lxVau1xLiCSSSZ1OZK7MWkp3P9DKU/JD2io95vE3icZPxY5yVQJ3qNq6YBbnoz0dqWt04tpA9upvP9LJzdxyHkeyU4xVsok2YGzNmVbQ+5RbeO8nBrRq5271O4L1Ho10Vo2UXvjqkY1CBhwYPyjz1W32bYKNKmKdKncaMIxx1JnEuOpWYYEYThjhv4YYrzcudz4XCNowo478TqwFjAH56rG+F5+n9C8oC9Z/FQtNjZAgisw/8Kg+q8ppNkwurTfllJ9mc511mUwMfBew7GsnV2elTIxFNsxOZAJ8yvK9m2UVa1Onue4NP9pPaPhK9pdWa0CNPeniqax9IY12YpjeDjz3pi4HIZTlHonbaR/V3b/eCrNoz7IIOGM+OGC4DXgJZPA8SoGtHxHLHdnzBStM5sxjUx3d6LGuibgaO4fTFANeZhBA78fJO6k0jC7OpMeqWk12JcR4tOv6J6o3ZjgJ9FJIhssjd/kPSFEops3nfpHkEEBgtJ0PhCtFXgd3vAql9U7s9UL7t3s+/VVIGqVZ3eC7fYmJs5jDqquH/ZErgi/HHBdx0fNynSeWvLbjgCwXrt514kjMjstyBXTpvxA8g/GLZZo7RqPjs12ioMN8BrxzDhPJwXBOI9yvob8S9kut1Om2k1tSSTTqB+FPATLcodDhOoGgXmGxOhxFZ5tQa4MdAa3Frz8xJAlvDXPj6E8qjHczHY7NP0Y6MPtJFSpLKGuRqcG6DV3hw9SsrAxrWUw1rWiGtAAAAVN0CABgMBhlGnBWGpy/xBheXlyvI+TVKjIF7eBwzTy/MSFQ10xMny4Zogg/N4ydFkSc5+Ioc6yRpUZ/5BecsoAC83MeY3rv/wARKhFCk0YXqus4NY76kLgqdTcM9F6ukX3Zhk7Oj6B2cG1XzMU2OcI1d2R5Od4L0hlfHcvPugFX+ZVYWw4sDgQcIa6COcvHmu3dTdvIjjuK49W28hpj6L6lp3S3kJSmvxVQaZ07kahI3N81zFy51cbpnnPmkNXhOEKouO4Yb4SXiBv8PtkgsyG1TOQQdVO6O79Vjsqn95+qaQd7ff7oRZcLS7UeSCDrurVEBW8nSPFI0cPeirx3evuUlyct2fuUBff4N9fou32dY21qdOHlpbTF3ey8QJv0zg6C3A4EYwRK4K8d0Loei+1S0hhIEGW465t+q308qlyNzXKMvpEytRDan8t8MLZaAHC8ZqCTENgGBM3nDTHnar2k9kmBlODjvJIGUnHgu/2s4Pokg/lOOmB8l54GajHmFrqXwkRbY4qe8vRMajtZ79ypZR8PfFY21rHepkAXjoHBp/XkuRK2C6vtZlPNzQdJk8t61zulIyFMxzAXM1qBaYcCDoZHqkwW6xLzK7mN0t2qa/V4XbknOcy3h/SueqUz8Tcwu92R0IqW6jUqUqg6xvw03iGvESIfMtJxzEZLk62yLVTqGi6zVm1B+S44nugG8OIXo4dqgkikoy7ZmdD7YGVyXtMuYWgROMtP/iu4a4HGCN8RA/Vc90b/AA+t1V7Xvb1WRuucBULCYvNpkzE7zHCcl19XY1elg5t5sG68C6SB81N2II1xHFcuqxNvci8U0uTDbOp75PPNWiY+I7t0wkaJi6W9xChqxjiOS4CxcXO+a974hLGpB/3R7xVTnqB7icPRBZeb0ZnxJUuk/lJ4wqhVneffqrW1TqhIQCMY8QVFW8E8VEBSGn2FDx9PeivDscvopf8A6Z8eeqEGOForZt17HEdWBBw+LccwcF0wM4YiNSFWaWGPmJ+qtFpdohnOs6XVjDTJG8BxF6dyzG7TrkSbM4/7o8iJK2Ys7dG+Cs6sK0pp+QNO3aVf/wCufH9FP+p1o/0zj/u/Rbq4PviSna0Ku5ehNGgrWmo8Q6ygji9uHLetRU2TXJN2lA0LmmOZwXbmNJRa8aKVkrpCja9H9kWiwueKdP8AiaL7pDmvYx7YBza4ic9xjAHgsu1dIajCC+hUbuJfUoeEioTv81o2WgtADXXQMg0wB3JK1cuzMzgTJn14nx4roWpSVUXnLfy0rMyz7dDqjCavxdYKpADqlUPNMhjAwnqwBTDMTg0nf2l11DbdmqMuvDT/AE4QIy5HlkuBaxoM3RPKfVZtPadRuTokaM8sE/ySrba5Z1Fr2Vs6p8VAVSJxl7j/AJTK4XaWw7M2s7q6YLAcBLsDpnjBlZdptbqoIe95Bwi+4A46NgLHbSAhrWgDfj371nkzblwQkhaNjY3JoHKSsgERuHd9YVMx7+oT3wd32hYEhJbHdr+iQa/Y+qk+/wBkB9kIA1pjf4KKxrZxn0UQFTif3hKHxnHgUGtRucJQgjqxiJw5qX8PvCIaYyjXMFAU9TGOAQDB44omoN4BhQURxQNMfL5/ZAO140HqmNXgPBJAyj1RaO5CQFs7o5Sj1bo++KhJQD3D3KAAonh5otYRn7+qBru3jyw8kDWI3DX9EAxfzSE+80OuBzgHvUO+CB3e9EA0+4Uv6KttPH4ifr7hOGEd3vDH6IB23jPv6KAHKPQKYZwpeGk8v0UAaeX1RbGInilDhnHmELwQDujeVFWG8YUUg//Z</t>
         </is>
       </c>
     </row>
@@ -1393,97 +1393,97 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>VISHNU VINOD</t>
+          <t>RILEE ROSSOUW</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>smat2023_132</t>
+          <t>t20blast2022_132</t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>23</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>115</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" t="n">
+        <v>50</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>29</v>
+      </c>
+      <c r="X8" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD8" t="n">
         <v>17</v>
       </c>
-      <c r="E8" t="n">
-        <v>12</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>141.7</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>25</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>1</v>
-      </c>
       <c r="AE8" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="AF8" t="n">
         <v>0</v>
@@ -1492,13 +1492,13 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI8" t="n">
         <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" t="n">
         <v>0</v>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUQEhIVFRUXFxYVFhUXFhcXFRUYFhYXFhcYFRUYHSkgGBomGxUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGi0lICUtLS0tLS0tLSstLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAABAAIEBQYDBwj/xABEEAABAwIDBQUECAQEBQUAAAABAAIRAyEEEjEFBkFRYRMicYGRBzKhsSMzQlJywdHwFGKy4RY0U3MVgoOSoiVDk7Px/8QAGwEAAgMBAQEAAAAAAAAAAAAAAgQBAwUABgf/xAA4EQACAQIEAwUFBwQDAQAAAAAAAQIDEQQhMUEFElETYXGx8DKBkaHBFCIzNEJy4QYjgrJS0fFF/9oADAMBAAIRAxEAPwD1VNlIpqBsIKSEpIThySaUlBIUghKKi5I+UpTJWZ9oG3hhcK8B0VHgsZBhwLrFwPQSfRccO3y3xo4FoaXA1HECDcMESXOHEQIHUrx3ez2iYnGNbTByMbchli46SSP3dZnbW0atd+etUc91hLjJgWChtHJWqNgG+h1diajrue534nEmOQJT2VuPEfsKPT5LtRpkyJCKxFzY7rb8YnBNyMd2lMmezfcDnDhBHkvX9199sNjSKbCW1cuYscOWoa7R0L5zAsb8P/1S9l7RqUJfSJa4y0uBggGxg8DE3QuJKkfUrXg6FJebeyzeVnYGi8OkPgODX1C6QPeIBjgvSQUAQUkkVBAkCigUSOYESgiiBAVzK6FcypOAU0pxTHIkQxqSUJKSCQUEUxUFoUpSSUHBlIoJLiRIygkhOESvA9/dufxGJeS4ZGuLGaGWg+9I5wvdsRoRovEt7Nl0amOZh6DSwkzUBFmWknLwteNLjmpTS1JtfQ8/xjCXkAeSd/DPH2Ty08l6cdgUKXutvzNyfFFuGbyCpeMtkkMxwd9WeaUNnVXe60+i6/8AC6zZOR3oeC9Io4UA2Cm0KQ0Xfa30O+x9WeRNpuEh0jxXWqIDbW1nmvXK+xqNQd9gJ58VQbT3JbE03WOrXcDwIPzCthiovXIqlhJLTM5eyvb76GKbR+xXLWkWs4WBHlPoF7uvlio6rhy1wEPY7MDGjmkEEeBEr6a2LjxiMPSxAECpTa+OWYA/NWS6ooXQnIoIoThJJJFEjmBJJJECNKaU4oFScNKYU4oFEgRiSMJKTjoSkgkly4KCSS44SKSS44CSJTUJxzevK8Ns57No4yrUBnO4NJ+64hw/8S30XqpWI3lxDadSrUdpI8ScjRA9FVV0L6K+8U+KddcGMKrqm8tMnKBc8P7q12bi21LxHJKOnJaofjOLyTHgWXWkV1dRumYjFCl9kn8vFdFNuyJlJJZkunUlS4ssz/iigTDTJ6AlX+HxA7rXES4Axynh4q7ka1KeeMtCi3l2GKlJwiTeOY4rf+zwf+m4QcqTQfESPyVI8rSbp0cmFYwaA1APDtHEfAq+k9hSvG2ZbooJK4XHJJqKlHARKCSMECBRQKk4amlOTSpQI2UkJRRHDkkUEsXBSSRXHCCMIJwXHDSmkLoUwqGccisJvIxpe9z/AHQ5/W+Yiw4m0LdV6jWAucQ1ouSdAvPttuFTMfskl3iHEny1S9Z5DeHV5Mxu0sZTa7I2k0EzHcLtJkS0RIg6E6J+w9sHN2bg0XtAIB42B0MXR2/R7RtOlD3Mp2YwwGtERaIJtzlO2PsZzqgqVLRHEkwOF0MnT7PvLoqp2ncbLZQD3EEqm3u2oKIygAm/L4q/2NTbJJCgb0bv9pcfISfVBStbMsqp3yMjsbbh7TJUEGM0Cm7QxeGiSLjQLdYSoypEAGbhwILTHI8+YWP2dszsqge4AuboTIcIsI5eq1Oz6YDiWMyycxjiTqTzPVXSlHYpjCe5OriFo91a2aiR915HqA781m64MGeRXTdvbXYCKjDkqPaA8HQu7s5fu+7fqohJReYNWDkrI3KSCSaEAoymSjKlEhQSSRgAQRQUnDUiimlEgRsJJJIyLHRBOKEJQvAiEkVxwgjCSS4hiKaU5NcoZyMxv/VjCinxqVaTB/3Bx+DVStGZgMTIB+AV9vtge0oB4MOpvD2nq4Gn83j0WS2RjSaLAfebLHce8wlh/pSdfU08O12aXe/p9CPiqNydFIwVMNDC57G5/dBIzO5QCVG2vi2tME3KotrbWZYMYKjgLZhLW+FlVCDkMTmoq56Fg306VN9SpUbTA1c4gNE8yU7MatLtKdSnWb96m4EfCy88w++dZoDezaZMGQTwjRabYe1G955pdlmgEtBDTE3I4JnsrLMX7aMpPoTcNTDjoruhh4HBZ7DY1gxHZ5gc92nrxCvXVyLIUkgpy6EXaNQMY5x4An4FU76pq06rQMvZhob1OQOkcv7KFvntPMBh2Xc8hpPR1rFTMLsupnDjUDu0dkDWtIuRlHHQCfJqipGyTIoSvJ9x6PsvFdrRp1fvsa4+JF1JTKNIMaGNENaAAOgEBPTiVkZkmm20BFBORAgRQRRAgSSSKIhjUCnJpRIhgSSSVgNzqQmolBKDAoSCKQXHCTgkEVxAyE1y6EJpQs5EPHUM7HM5x8CD+S8drsq4TEVqVQEd91Rsj3mOc4giDp+hXtJCwvtU2UXUW4tg71Kz+ZpuIuecOjycVW4qWRfCbiYPeui572PbdpaDA1MfJStgVmVAW1T/AA4aYjs3OMWglw43PoomDx4c1s3ynQ9bQtPkbkIABtbr5qiUuVKLQ5TXNJyTJGA2ZhMzXHGkCJPd0NrQfNd61VjW/Q13VQAD9QXCSXSAZEaD1WQo7Xb2gZ2TiZiJEL0DAPhgEAGNPHqr9FZoGXK3lJv14Hn2y6NarjmuqUuxi+UGRIv5eC1e2ce4PytOgv8AL5rrjalMVmgRmBJJGvuzc+Sym08fmOYHXWLWBmFKTk7lEnyom4XZ5xGNZREOOSob2EtpOyEn8RaV6Xu9sxzKbHVfrbl1gIJ0EAm4EiZOpWG9mVMvxbq3Km4epavVIROCbXcVdpJKy3AgnppRFTAkkkiRAQkkkjBEgigpRDAUwromo0CCEkUkVwToUE5NS1hgCcEkgFJIUQEAE9oXEHMppXRwXMoGchhXHEUGva5jhLXAtcDoQRBC6lVW8u3qWBw7sTWNhZrR7z3HRrevyAJQWbyQaPEN59lOwOIdhySWg5mO0zMOhPDMND1Rwe8jmgNN/ObeimP2lV2l2jsUAHEh1MC3ZsIhrW9LHXWSs9jNj1qXejMObeXhwXfck+SWqDTqQSnHRluMe0VRXMT6j0V03fAi8Tw/WywD6hNr24eCl4em99m03O5QDGnFWqityt4iWxqG7aNSoXniHk9BHzuAqyoXEBrGkzxM3mxv66KTs3Y9TWoI/lEQP10VpVxLaLTpK5zjHQKNOU85F1uLixh8VQwoN6wqF0/yszeV2j0K9WXzNs3bFRu0KeKF3sJcAdLA909CJHmvoTdrbtLG0G4ikbGzmn3qbuLXfu4go+ykqaqbO/x9MqlNObitrFqmpyBVRICkkkiRAEUUUQIk0JIIiGJMKdKBRgsEJJJIgTsU1OKalxkQTgmhOXEBCcCmohSCwuXIroUwoZBI5uXk29tGpj9qOoVJGHwrWuLTo6WhxIHEuJA8GnmvVcRVa0FziGtGpJAA8SdF4n7Sdo4bEYoVcNVznJkqFoIbLT3S132pBiRawV2FpOrJxi7NppO17eldFdafLG5RYXagONqx7jrNjSGGBHS5K0zIjoV5/jWNpOY5jpkSbEROovy6LWbExhc0JPHYXsZWWyQ/gqynCxLOHZOgUrDvDf0C6Ne08B6IVq4iyVhPIZlA5YrFHwWd2piJsrDE1VR7RfAKvgm5FNR8sSLgaXv1jpJpjxyy75t9Vd7o7w1cDW7SldrrPpknK8cJjQjgf1UXG0eyoYahHfLHVniLzXdLR45GM9VfUdx6v8Oyo2o013mOwtLQebpgOAuQbcJXosNVpU8NF1n91t+Gvyv1yMOsm6r5dT1DY2/WBxAANZtKpaadQ5YJ5OPdcOoK0oM3BBB0I4+BXzHT+uykEEZgQdRFoI8QtBsLePE4JwNGoTTnvUXSabvAfYPUfFRU4XdOVJ76P/siOMs0pnvqSy262++Hxh7M/Q1v9NxkP/236O8Nei1KypU5U5cslZjiakroCSCcuOEUxFBSiGBApFBGAwSkgkjsCd5TUCUJStxk6hBNlOBRAsITkyVktte0XB0HOptLqz2yCGe4CDEGobc9J0Rwpym7RVwZTUVdmurVWtaXOIa0CSSQABzJOiwW8PtKo05Zhm9s775tSHgdX+UDqsHvDvPitoPFN05Se5QpyRM2kavd1PoFL/wJVLQHV6TH6uZ72X8TgdU52FDD2liJZvbN+Svb5d4s606mVJZdXb6me29vDicY76aq5zZnLoxv4WC3nqpLd3Zp0y2qO1c0vNO0BsSwHjmNj0laPZu7uEwsmqRiakH7P0bBzgnvE80zAAFz67h4QNJ/sE9GLqx/t3gk007Jc3gnnb4X2EK2LjSdrqTzvvb3rfyPN9o05bPIq23XryMqnb2bNDMSQCMr/pMo4ZtQRymSOipcA0U3S0yJHCNdR5c0lxSg5R7RaP1f6Gpw+uk0jZipCi16sovqy0EcVzptXnNDf1OFbRUdWi6tUFJgLiTAA1JP9lcYt5nKLudYDxWg2RgG0WltEjNH0uI4zqW054eHmt3heClUaqPTYweLY6NBcizY6hgRTqnEVnNqV4FhOSnAgR4AAD4Lrs/FvNR2IDoLbA8JPCOUcOqhYitbKPduZ4uPGTxKkOBZTy6Wk+J18OXkvR9nFR5LZW0PIVas5Pnk828n08OnuJGF2Hh8fVq1AeyrZBH3XP1MjjaNLrKbSwNTD1DSqtLXD0I5tP2h1Wt3caG0XVD7xJvNxFhfgrKptCjiGdji2ZhPdfHeHWRcHqPNZsY1sEv7ac6e8f1R/b1S6P3a2NWOLp158tW0ZbPZ/u6PvPNZWy3Z3/xGHinWmvSHM/StH8rz7w6O9VWbw7qPw7TXpPFWiLk/baOoFnDqI8Fmu0tJMJmFXD42GWa+DXjumMclSjLp5M+i9i7aoYtmeg8Oj3m6PZ0c3UfJWC+aMNXe052Oc08HNcWn1F1vd1PaJVpkU8WTUpm3af8AuM6mPfHx8dElW4VNLmpu66b/AM/IbhilpM9YQTKNZr2h7HBzXAOa4GQQdCDyTll7jTAUCiUCiQDGpIpI7ghSC5pwSY1YeE6VzlZzfvbrsLhiWGKlR3ZsP3SQSXeIAMdYVlOMpyUFqwJyUYuT2KHf7fUtzYTDOvdtWqOHNjDz5u8gsnu5ue+uO2qu7HD8HWzP4Qwetz6FZ+o5b/dzFxRpte+wZ3BNmjMZEc16GWGlClyUZW6u13bu2v5bIw6uLSfPNX2S2Xj6zLPBChhw5uGpBgDe883qvtxcbhUWGFy+Cb8rRN7q0eWv7Vx0DQ244m4MfJQa1XK3LlIMSdP10VmHw8aMXyavVt3b8Xq/VjJxWInWac3e2nReCGbRqgtAH2iZnjH5fopLcK3IIsIvcjTWfiomVoqNBcC1oEHh185UlwBcJa4ZiSZsDxgCf3CuatkVp3M3tjZYdmqtMVBq0/bbFiP5o4dFl2DI4Ei03XpGMpw5uUAG/C0cZHospvNs0UyXjSxPmYBA+aGSjODjLQ0sHimpKL12G4Z404cFJqVsoDWjM51mtGpKo9m1XOcKbRLiQ1o5zotOcKKX0Y71Z0tc4GwHEN5D5rz2F4TKpXan7MXn3+tz0WL4rGjSXL7UtO7q34EXZmAGfM5+Z7bvd9mn+D7zuR05c1cvGjbtpt4ax0PUrhhcOG8TAFja7gfePOOHiuj7QCe6ZsY8ZPNepUYwVkeNr13Vlm7+vM5NcHVG2s0zHyHhMJuOqGJn3j6LtVkU3PB1MeOW5uodZri5odpbTqeKGTyApq7Xrv8AMsaLQKbWax+dzdcu0iSNI1/TxJTcSZLoBI4EaaKq23j4HZix9430/f5oJHUaUpyt1I22NrvcHUw85JEgaOI/IfFVtKkB33+Tf1TKI+2dBoE4uLjzJ4IoKKzt/PezbUeWKgtjpmkz8E9rUAIUmnS+9YcuJ/QJyBVJ2N37Ltulrjgnnuul1Lo4Xc0dCJPiDzXphXgeExBpVGVW2LHNeI/lMx8F7yx4IDhoQCPA3Xn+L4dU6qmv1a+O5o4Gs5wcXt5BKRRKaVlIbYEk1JHcEEohMRSdxsc5y8i9p+0TVxIpB0tpNAjhndd3nGUeRXrDyvn/AGlWLqtRxMzUqSfF5MrR4XDmquT2XmJY2TUEurI0yt3u5XDsIxs95ri0c5zSD6OWD6rUbmVWk1aTrd3O13EZdSD5j0XoTExMb03Y09PCZsznOJg+ERebeKg0Q01wDJFje/hmPCSB6pOquDA/MR2hh0RqJgwRyBWa21jiZpNcYk5nC2c8J6ARZDeyFMLhJYmqoQNTjiBWDjFiJ8OPjchdcRVa8hjTN5JHCOR5+C8+wrXGC6T4krUbJxD3gUy64kskEkGAAJPCEs8TBVFGXgejr/0niaeCliIy5rK7jaztvbrbWxY4imGwWiSe6RJvYnU8oVFvHL6DiQO6WjmT5+atacvklzu6COV/tC3kFFp4btPoCJY6oCTPAd4jnw+KZa2Z5elJRmmVW62Fp0CHvI7SoD2d/caefJx+SsK8mqMtzGXyP9/zXDaex2tqGrMiZDL6DXyUsURTpOqC7rAXi5OnhEo4rlXKHVqRqTVS928rBc05gARAJGhuYnXyUnDYWpVzODM0HL0HLXiYJ8lFotzDvDTh1iZJCv8AE4V1FgwmHvUxDmua/wB8NaGiXFsdyIde/HolMbiuySUfael9LLV+5Zh4TDKvJ8zyis7a56L3+mdnVqX0OHfTDm0gLU3scMxMuc5oIJJJmIPulU+1sEM4dTD8j753AFsTAc17eB4TBUsbonDilXDy+qKze2dnN2v7sAGxDSWnmYPCyc+oX0a9IVchY92UTLHMs8tPCZfAJ0yiIWHhsWo1VKEm43s9beNtut+huYnCqdNqSs7XTsr+H8FIMU0jUSQOfgfJZHG1M9Rx4T5QLD4CVpWVS1tYkyafaAdAJI/fRY5z7R6r0c8nmZWAgryce715HZzpMD99SutI8G8ePE/oFwY2fD59T+il4cEkNbqSAOZJMAI4PcellkjvSYG31d8lKpCUyngqgLh2b+44tf3ScrhMgkaGx9FKoM4HVPUrPQRrO2o0ssvcdmfU0p/02f0heLOpzYamw87L2+kzK0N5AD0ELH448qa8foO8Ld3J+A8pqRQKwEarEkmoogRiSSSSGyPj6uVj3/da53oCV8+VBeeeq903qrBuFruOnZPHm4ZR8SF4a8La4RHKb715Gbj5feiu5+Zzb8/QqZsysadRjpgTlcdO6635qJprp+9VzxTSG205cltaK4lZSye5tq2JLQ1kgTIYeVzmJ6wtF7NzQxIrUn4eg7IWw91MOe5tQvkOcejYCw+zKpqU6RcLCmQ42tMsJHlKmbA2nWwLqgZlDnuZJIn6t2YRzB08Cs/Hz/tXNH+nOHqvKpCL/uLRXtlfN+R6HsylhKjcUK2HoUqVOt2bS2m1pgfedzJb8VU7+YgnFYcssOzY5ogCM73cPIeipNqb01KzHU8lFgqPa92RmQuc3Qkzc/ouR2hWrvbXqHN2TA0CABlYZAtxufRYd3VmoR1bR7n7D9hhLF12lGMZXV7pXikvFt5fDqKvTfTAIywYBNzB+8dNVwwr2h3efcOc6Rbg0DnCkYmvLC2HBrolxEQP3bzUTByHaQIdltA94T8V69rM+MQvyO6s/W5LezMA4l0Gzb6N6+Oqr8VXaOzpl5nNLgdBlsnnEu7zWkZQ60gm/GI4Soz716beDad+pN7+JUNlsItN83e/kWeAqTUaW96XCaYgy0ag9YVnvY3vg0XuB7PM0FxzuALw4t4kgu8wTGiqnvLXhzRcNOhAIuIM+IK0po0cdRpuqZu2pwHVSAA1gJdDho4AiOEysvGRcakK2yvff4rpfLrnvs/gKidOVPRytbTz107tOhQVsdiatXDBvaU6NGm0F1RuTtHAd90G7tABE6E6EqVtAZMPUa9vdxE1mZSc+ZjgAHNPCABrqFIOxsJDsS+q5znVMrCD9G9ghpIDYOWLGTrrKqtr7TFSW90NY5+QNaGjK4zoONvNJ4TCqpOPIrRWbytmm/i7/IfxWJdOLV05PK2uT/jT3FHjagNPEvBIsemtMa+pWXZe/DgrfaGIhlURZ2SPB0j8lV0wteb5pFGGhyQfu8kdWldqa5U+lzyF12YDyPpf0V0NcwpGowO8tcVe1dlqGIykQ0SQXEBsCXZbnUyVd0d46dVrW4qkHuFi/SST7xOtmn3RYm9liaJNrET0181Potjqep0/NMxwtKSvy+9ZeQpUlJbmjFCgcRR7Fzi19UDK4XDRUABmdCJsbr1QleMbOr9nVpVXfZew9IDgTC9mKx+MxcZU03fJ5vxH+F25ZW6ryEU0pxTFjo0WBJGUkRA1JIpFIjRUbybN/iaJoZ8gcWy6JMNOeAPFo8pWUZ7PMNEnEvPUdmB+fzUz2hbQw7RTo16Lqsy8AVDTDYOWSRcmC4crlY/+N2YSAcDVaObcQS4+TrfJMUaGMlG9Kc4xf/GMGvjKSYtWqUOa0oxbXVv6Kxqm+zfDEf5mof8A4/0XDE+y9sHs8S7wewEerSIVAKuydOwxbeoqMMeqk0n7N1ZicdRPOGmP+y6ajSx6d3Vqe+mn5SZQ54faMfdJ/VIrauzamCcKLiHy7N3QdOEz1mylOw7AyRrY5p16eajbQexrwW444iS3LnDhUZfk83Ce5hBDMxgmbQLiTy6Ba9BdrQUaub3ya+TzRmVK1TCYpVsPJwks01nlbNdHltuFmDJJHdtGrp18AbqWC7KWwwBpEtE5j4OPNc2VMh4kO8zI/KF0pBry5zm3sAHC4Gsx1kq7D4SjRd4Rz67gcT47j+IJLEzvBZpJJK/WytffXTY6Y3FM7NxkGW2E6z0UBrA2lTdGawmSTmzcusp20SGcstnG2jrgCeAOqbWDhTpuJkCDERFtesSmXqZdOCjFW3f00OWctMdnAJlotIOpj0UbC0x2lV0usLGSCI18OPqpNas0lgkGXt46QZ/fiomGce1qH7M35m9yCqpDULuL2y+pZ0sQwEjPyMk300v+7p1R5c1rBUs4kkQO6L8fNcMU67etj+G35wPNPxLg0NcAJmIAAJnh+fkiiL8qbTWrHPzscDnkEBt22ECwiVCz96ox8Gb9LaQOHEJ+IxGaGkFo1MxeLxb92VdtCi2C5oHgLTNosok7LIvpQvZS1e/vyHbPwdOtiaVGqSGGQ65bIYHEQ7yErZu2nsfCiGNpFw+5T7Rx/wCoRE+ay+xtgDEUpc5xMkU2ju90ES5x14EeSsNu49uAqtp4fCUGktkVHTUfy46HzK8pjVHFYnkTk9uVSUVda3bvfpkmeqoUqlCgptK2t7Xefd3mh2XvS2q4jDYCu+BctbTbA6uzQPBdv+PYym4ufsyoWTqCSY65QZ+S82r7bxNVxe+vUE8GuLW+TWkAKVh9qYi0V6ojQmq/9U7Q4HDmvyxfc3N/NNeQrUxsrav3WPUv8X4R7RTxOGq05tlq0ZZHMcSPAI4ndLBV2Z8G9jX3IyuLmHoWTLPLRYqnvbjC0U3vFZv3X02PB6EkT8ZVpgtpYWpWY91J2CcBBfh3iJ5lhZYeHxTMeGV8N9+g5Refsvni+icJcr+F33Ck8TTqfdqWa71yv4ogYrdnEsxNOhUYYdUY3tGgmkGkyYfF3EA2XrhVDsmu7u4bEEVQT22GxIMtq5TMTweBNuUq7KWxmKrVnFVbXjutH3q+a71lZ5WHMLTjCL5NO/VdwigUiUEoi9iSSSRkDnNXN67uCr9qOIpvIdlOV0O1gxYweqzXLId5TyXfjanb4p0e7Tmm3/lJk+bp+Czq0tfd5kz2j55nKZ+C5f4eb/qf+IW/Q4vgqcVBN2XczNqcKxc5OTSz7yhCJKvxu7yq+rf7ptXduqBIc13qPyWjT4rg5aVPimvoLT4Zio6w+aMhjquVzXjgVomVXPLbtFs2hMaRx1UndjYLn7Qw9OrTlmZ7naOENpuIJ6Zsqp3VRRLmWmm5zD1yktv4woWIhKrLlaasmU4ihJQjdZ5rQtRiiDLyLSIFomL63Fk520WZh3osZLbk3EBZ47Tl02uAPSefitRu/sSliWioKrgYLSzKO6detlXiMfSw8Oeo7K9tG/Ipp8PlUlZLO3ciDtSDSzS4l97k+Ujmu2JxBc1rQ06cxoIBC6UNmdsxz3OLaYnLEd4gd4yfsynbLwL8TWc2nEcXcGCYk+N4A5K94yjzVLytyW5ntnmVLDzcYZXbu0vXrIhPAMktAIgQYiNfiolKqWvcA0gOBAEaEr0R+5lHuy95dETYDn7sXHSVi9vYUYav2ZdmggzpZ3SfFJYXiuGxc3ClJ3WeaayGamBrUI3qLJ99/ccKTA4kS8WAEk/nw09FyqYvK5pc6SLEGLE24fu6ttk7JfiM7qTmhzIs6Ydmm0jTTkVXbY2dUw7g2qBLhNjIPO6ZWKo9q6KkudbblUaFRw7SUXyv/wAIuMxgIEOEyIMi3VQW0HVqgpMe4k6wdOZtwATTWDZJ5d3w4rW7DwjMPS7VwzVakWGt9GNSfEcZ2VPLV5I0uHYLtJ22XgS8M8U8tGm0l5GVrRy5HpxJWb3twGIpVWurlp7Qd0tMgBv2b+K0gxLcO11V/wBadTOg+6OipcdiHYhwqVrwIY0/ZB59VgYPEdjU7R5+tj0WLo9rT5E7GdpqbRAVnQYJsAr3AUmnVoPiAtqnxxJ/h/P+DJnwhte38v5KChoACpLAR+q11LYOHqC9PKebe78NPgoWN3Uq0xmou7QcWkQ/y4O+C28PxjD1MpXj46fFGNieF1oez97w1Jm4ePIrCge8x2ZzRrkqNae83lLcwPivQSV57uC2cQTGjHyOR7o04HUL0IrI4xy/afu7pPxGuGp9hn1YCmlFArNQ8xJIJKwElPVRt76l/l8wkksieho09UYGomNSSSRqo6MUt3upJK+GxVWHbn/58f7VT5tXk+2Pr63+/W/+xyKS2+H7mNjdUcMPx8fzW/8AZjpX8G/JyKSPi35Of+H+8RXD/jfHyZYYb/JUv9t39RUzcL6l/wCJv9KSSzsR+Xxf71/swqP41H9sjWVPeb5Lyzf3/O/9MfNySSU/pv8AN/4v6DPEvwl4lx7Nvq6v42/0lQ/ahpS/Gf6Uklf/APdl6/SCvyC9bnnmK0HgvQmfXUP+b+gopJ/i/tR95fwv2Ze76lfvd7zfxM/qCjvSSWYvZRoz9r4DqGqv9nIJI4gvQ1OzlbcAkknoaCM9Sp3V/wA9jfFn9DVrCkkmMTrH9sfIz6X6v3S8xpTSkkqUGxJJJIwD/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUSExIVFRUVFhYVFRUVFRUVFRUXFRUWFhUVFRUYHSggGBolHRUVITEhJSkrLi4uFx81ODMsOCgtLisBCgoKDg0OGxAQGy0lHyUtLS0tLS0tLy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tNy0tLS0tLS0tLf/AABEIARMAtwMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAGAAIDBAUBBwj/xAA/EAABBAAEBAMECQIFAwUAAAABAAIDEQQFEiEGMUFREyJhMnGBkQcUI0KhscHR8BVSFmJyguEzQ5IkorLS8f/EABoBAAIDAQEAAAAAAAAAAAAAAAEDAAIEBQb/xAArEQACAgEEAgIBAgcBAAAAAAAAAQIDEQQSITETUSJBBTJxFCNCYYGRoST/2gAMAwEAAhEDEQA/APFrTgExSAqxU6GLpYlqXdaABhC61cJSDlAodSlAUNrpegEfpCaQmaktShB5TSVy1xxVygnSKIlcJXLVBg4LqaCu2oA6kuLqhBwXU20tSsQVJ7Uy10FAhYaUlEHJKZIRgqRrVFSla5TJDpYmEKTUk1lqEIik1TGFdbGoyDExxU7goHhAhwFXMqy2XEzMghYXySO0taPmSewAsk9AFHluBknkbDEwvkeQ1jGiy4n8h1JOwAJK+ieB+EIsnh1u0yY2VtPeNwwc/DZ2YCNzzcR2AADkorLCotvB5Nxh9GmIy+DxnzRS1RkazUDHZABt3tCzXQ+iBSUd/Sjxd9blMEbyYo3W5w5SyDmf9LeQ7mz2QIApGTayySST4G0lpViOK08w0iQq6V0MVyOC1O3CqAM7Quhi0hhUnYVQhnaFzw1acyk5rESFPw04Rq4Y10RqEKfhpK6IV1HBCiGrtJupdaUCEjWqzGxV2vUzZVCHJ1GxKV5Wzwtwri8e/Th4XEfeldbYmVV6pCKvceUWfRQhjuCfl+Wy4iVkMLC+R5prW8z6+gHMk7Be35h9HGDwmBxEQaJ8VIyo5p9DNDiKHhn7jQbceZ7kjlpcOZJh8lgGkeNiptLZJgNm6tw1t+zGO3M1Z7Krko8ssot9DuB+DYcoi1O0y4yRtPf0YDv4cfZg6nm49hQAT9J/Gx82Fgfb3bTSA+yD/wBtp6E9ew9+y49+kKtUGFfqedpJuddwzufXovLS69zzO/vvulRi5vdLr0MbUVhFctSaFOSFwJwkfE5SSPCh0LvglHANyLUMoU/jhZTgQpACpgm5Gj9ZCa/FBUhESonMIUwDcTyyWmNkpNDE9uHJ5IFk8s0sJpI3UOIIB2UULS3moZjuqLse/wBOCbx11VC1JMM+SX6sopI6WzFhy5UcbHpRaFqXJn2pWFIFPtVGZI3uX0Xw5i3YbAYWMfZ1h4nnby25gc+q2Jt1k3zJsrxHhLhqXMJxDH5WgapZD7MbLonsXHkBe59LK9jzLP4cNA3DQtfOIWMYXvLCQWnSwEG97aSdq2HPkqyeC8FllnODFG4T4iSJ3hv8SJzNRMbXRgAPJcfEJIsBo38u3Mrzvjzi+SZjYoi+IPcS5tjW6Ov+7W4LiQQAeTTd9JcbjzJFJi3HXoIDGlrtIdJVc+ZIcCXbk1z22CZA5zi925JslUjDc9zDOzCwik3ClcfhyFp4eOypMTha6J+BG8wWxm1cjwpVkYUjcirU0MRJ5KBbZUbDRV0RjSliYKTGtNIlHyVZMPZXPApXY4jfJSz4Xa6UwDOOCCFopV5YLKmEZTo4jfJQmMFTwKShnDTutSbCeW6WDi4yChJcDKZc5LGLxI6KkX7qJKMWVRRwPc8l+NthJWMLhiko5pcEjppzW5I18PiWjsqGYU4qSfLpQTsqjMHI40AmPJkjjsUeHaiHhbhCTHyaWeWNteLMR5WA9P8AM70+dDdXeD/o9mxJ8bEO8DCt3c/78lfdiB2/3HYeq3uMOLvAh+p5dGI4m23WPxLT95x6uP4quGN3F7Ps7wmVYc4LBtBfVvN25ziP+pK4cz6dBQFBebZTmErn4h5du8Rl1gUS0nSa+fzTMBlUs1ude9kk7knrZWhgMB4bZQRz0fhq/dLt4jkdUsyJsTjpHQaHEaC8OLWtABdTtzW5O5WaK7fgiHAwtkZo9xHwUzsjpHTvdEVq0oTBkzBqf4cuI8kLbNWfQWBzUma4IA1a0+GI5WNkdC3U/RTb5XbefuBJpXsbUSmnjGc1kt4D6Py5o8R5Lz/byG2+6ocT8Ovy9w85fG8AtcRu08i0/wA6rZw0GIlhfHicWIpXOBiGsMJbe42rdbGK4fc7A+DNOZXAgscRbhY9kOJNgmvdayxsafZ07KIyjhI8xOJ1KRhPZcyXBGQ3WxRVHkWy2x+RyLf5bwwXkmrdOjxWoLUznJtItV8ny3VudkcPJTfFrJTN9k2aekVx5O08lh5/lWnkjtZWM4tmdFiyRSo5gwnot7JsosAlW8yykAWhtbLqyKkAv1YpeFpIK1XMo0uvwtkIuCHKY/CSHSkrpwwaxcWeUHk3U6vbDCR6LisJEQR1VTAZO0OugsfFY94mroUW4AWwLVGSkcK2qVaTz2WJpJJQRK+29GMGlgAFAV7unLZZeOyljui1g1VjKbpHaorCKqbnPMmZ+Fw7IwRSxc7YBqcOtIqmwmrdU8dlAewi69fySLKnKLR0a9VCMgc4bgL3gAi7FfNE+eNdCKewtvkTyPuPVAcT5cPPpcNJadux7EeiM8JxF4rPDkAcDza7cH19/qsddjqbTN11Mb4rDBFzfEeTWy1cE7wWFw5jegObfvb+lBVMdjIIpHM0uHLcUeY7UPVQw5kyxplAvangt5+osVun7vJHP0zkKc6Lf7rgb/UI5ZfFklA3pv3S1vcGjZtbeTcQvc4wwvLyy3B7gD5QeZHu2QPjsoa+Rxje0N1bgXpBPOvRFPCkceCBkd5iRR/zX90e9IlFJ4+ztwtlJKT67NDDQth3ofKvwWrlmK8U7BSYOBkwOvUG0NJ2Lt+YdfOiaVjB5UYCdJDm3V2Guvb7pPr0taam4vDOXq9fTqFhLA3M8s1DkhnHweACQPgjDM8yDNiKI6INzjE+L1pOlPgzUwW9L6JuHsU5+5FLZzHLg/mFhZHMIzR5rSzXN9DdQ6I1zzHkmpqxbiJZw+XiNvJNkwoeKUGS5wJgtpulu6YnnozSTi+QGzvIAzzBCzXu1aRvujbiTM7BaEJZbJUlnvaROXywdCht1tsI4csc9gFLqIMsxbXMoUkrOMX9io2WpYSBvGODpQ5b0WbBjALQIzNKdup8Rji4c1qqrimy963RS9B7g82aVp4ctduEGZG3W0bokwswj5lKbwzNKtJcdmpibrZQQvrmp8NiA8KPFM7IiMYKmaZPFimaXbOHsvHtNP6j0QFmkEmDdom2/sePZeB2/bmvTcLFQTsZg45WlkjGvaebXCx7/Q+qRbRGfP2a9Pq5VPHaPD8fjvEk1eg5+ndWsNhtRA578hudjvsrnFfDX1WbVGS6J52s25h3Olx6jsfn6uyWKUvPhC3Bhd05UAdjzNnks7XjjjrAy2Xknuj9ljDZeYcQNRDmNJBaPvC/vG9zWnlta1swhjlfr3YxnsNaav1NdT+Cz8cJ2u1SRuGnyOIadLXN23I27df0TziNW45Hl6eipGKlJTbyzPfffhwy0gtjlH1cv10W7UGDY7UPasjZu9dffQ9Pmbi7dx+fu/ZPlzc+Ho07kVr2vnz3He9+eyGcxxXmaQeZ3CNSlzuYmyuuTSgvrn9w4GK+sRaL+0aCWdz3b8fzQ87FNCZlUpFEHTZq9Wkk9dJ5fO7V3E5I57y8fe3NVVnmdvW/jabhvolE/G8FLxLIN0rGZ4ppjPuVbMctdG3e0PTTONglGKccpnUeLcSX0bfDWNDNr6omxmYWNj0Xm7DS2ctx5OxKuniOCttW6W5It3qcS5Z2PDWkAdVrzwk+zzKH8fhZQ7dvIrNjMuzXTP8AlYccBRkz9Ld0lhRzvDa3SVXFlna/6ejXn4R0jUn5Tw7q2KI86zUAELnDeLBXRjck8I5cq7XXvZ3BZN4QJWHneMo127Io4gzERsO/ReWZjmJe4utJtwuBukbnLLD3hLMNXVFnh2V5Hwni3iT0tet5ZNrA3V4TW0zX1PyfuNxU2gLBxPEzW8zutvPY6YT6LynN265AB33Sv4mEv0sfXopJ5mEOcYkYhjvdY943CysgzKKEu8TWDIGta5oBDQDqJIJ5g6SK7LWyzBBrPePzQe88vRxHzsD8aSp1b01Lpmmy2MXGVa5WQ+izqKR2kyUxwaHxkllkskDgSexdHv8A5CnZXmcccYZra0PbK8jW1rQ5/hgBwPe+/K0Dw2Tffb4hRyijXp+qxv8AHwawmVX5GeeUmGnEGPjfDN/6iN5e2HwmAjU0McdTbHW3ONeq86x83J3Y7qxf7KpiYz1/nYrTRQqo4yLnZ5ZqTWA24Sy1ssYkc/2tgBe1bUUaZZlMkbQRIJIxs5pa1pbY2c2vWgR62vPuCsTojDf7i7b1Br9F61krKhOrm5p/JL3yjYdD+DpnTlR5MXM8vEjapDn+EW7mkbgUF1zdl1WkzgKcocHluI4c+0oDZbGD4WA3pE4wtvuloloVdifDGx1M4tNA/gsoDXWR0WDxTPHH5epKPJG000vMuMMve5+pZ5U4llHQjrN8GpdlUyg7jkks7LnXseiSo2siI0W44N/GRPe6+/REOS5WWNtZWGxrS+kWMxrWx8wFzLr51STO7GELYOIO8Q4Zz2lAzcA5zi0DkvUGYlj2m0ISytjn5cymx1crG/YiOkjUi3w5kxY23DqinKsTpk0qszMmBnwQpLnThiARytTTSnZOSl0DUwhFRaPUs7wrnxEgdF47ibbKQeYK9Yh4ni8DzHel5dmmPY+Zzm0tkdLCtfETO1y7H/1J4AAOyxGiw9vWzXvG4/FXxTrpZ8mz3+8flarXJ7mvQrVRXjiTufsK5e0P1TsQ7b4ClUjP4E/juuzk7e4V6hPRztvJJHIwHfrt+yjdgpJ5I4mU50r2sZ0bqc4NF9tzumYPDiR+l0jYxRJe4OIFC+TQST2ABtGHCboMHJ4wbPinijGRE2KON29vHivaXHtbdufPlV95Hwh9nqGTfRlgYGRtLXmVjW63iR9OkIpzg07AEg0K7KHjuB2FiYIjtI7RvzbQJ5/D8FRwX0geHDrxLJ7MoLjpjdojaQQLYaJ27D2kuJ89ZmWHY/Cutkb3F9inB1UAQeWxv4oOtS7Rsjc4r4szm4qmtF3Q591cw+NbW5Q/FDJVJmJY9oK2dI42NzCdmJZfNRYmXe153/VJWSUeSIocxLwN0FNMvOiUMNhO3FtrdYfE8rPDNc6UQa472sjPyQ3cot8FVWBgkLSSO6Sc6QJLBJc9HodO141yXH22Q78ippM1kNMtQPkt5Pe1HLMGkHsnSphLtHMqunFvazdw07mt5qtinDUCTdqm3HFwofFUsZKfkk+OMZ/E6EZylV8wrazUzY7K3lmVsPNCWAzbSKtbWX5k4Os7BPeNy4Nf4+uqVclPv6LmcZYeTSaQfJl72vpehx4gPoqDFYVpN0F0bKIySwef80ozafsF8BEeuy0ncGYh7Xy6o2AU8+I4sIBA9rYhn+4gntW63uD8n8bE6yPs4vN6F59gfmf9vqtL6S8c1sceEaBUjtbx3ayiSe9uLV56+brvVVfb7Ok4p1OdnSPJcT9m8sdsR/AQeo9U10gdTbN8tq23v9VrYjBB/drugFFpA9Dy+CqR4Hw3B/VpDq0net6C2ptI5m+DZZixTYxTQPU7WfUpDN3Drss3N8ax0jnR+y6jVaaNbgD+fHmqH1hXUsoc6+QqwueuB52OoPIj1CKOA5WxzThu0c0bXtb/AGuY4hzf/ePgR2XlzZ16p9DGWvnfJM5pMMbCxriPK573NLg09aEYuuVop8kVYViNvZNkynxAVq5lhGtdTVaw4oLSuUZaqWp8nnOJ4fuYCtkQf4WAaCBRRDLA29StiS2KsYJG6z5xwwK/pxGyx+IcsJYe6K5Z/OQocbGHDki0c3c1LB5tg+ES/c2kjTF48RNpJZZXQi8HVq0l047kC8/C557oTzqAxu0r1GHNBIywRuFm4vJGS+ZwBITZOP0Y6Y2J8o8/wLCQq+OeQd0RY3DiN1AdUnYBsg96xTvUWej0346V8XjgH8ni8SQDojyTLWiO1Y4e4WY3zALXxOFDdiupptj5Zwb3bCbhD9SBvAOo0VpYuVuk0rc+WNNEfNcjyoHYuJW/4dpmBq3PyRucI5hCzBhwcC+3F7QLdrs6RXbSBXxXn2fYh2JxLpdQNeVvuHMjuL29wvqiLGZO2KNzxsXDTsa2PPl/N1guhbypedemUdRKzOcnQt1DnUq4/wCShG7of56FSOnLR6fko9NybNJJ7WSa9PmmYratiARYu9xysdxsfknGTwNmXmOAY86qLL6t3b79P7Usz+kyHlVXsSQPnV0tyS29CLANEcweR3/NQOJ3o1ahohvisG5wRwdG+QPxPnAcCImm2uAAJ1nY17tvyXpnEXGrcNHpY0gDYBooAdAANgF5TlONlY5p1EFpFEgH3cx0/Qdlq42WSc+Yl1bnyjkOuwVo5wMqU9/yfAW5Jnzpqe4c+6JPrmoUF51gcQWNq9vcFpf1SRo8rqPuH6hNjJLgZqaJVrdH7DCV5pPGL0MNrzrEcRYgHaU/+LP/AKp7c8nc3eUn/az9lbeY0rPYURSankqy4IKizSUH2ifg39lcZmkhHM/IJcr0ngfV+Onct2TUzHAh3NcWRPjJD3SSnZD0bI6G5LCmLI8qMbQCLV3NCWM7LebEOiz86wuptJltS2vBg0eskrY7ugM8ASWV1sRj36IjyrK9I5Kxj8G3SeSwvTPts9NH85VykuSjgs+DWgLBz3PnA2LpQTQ/abLO4iYdPIrRVLjacecpQu8sfstwcVn+5XYeKnHsgOGBzjsDSI8JggW9iEZTcfs3x1fkTTig6xeP14dp52f0V3gyFj/E1RNe7VEGh0etpvXbHOLHCMGm+bY7bFBL8WfKynFrTsSBVk0TXPotXJcG2RkryXucNIbFHIyEuYdet5c4HU0aWiq+9ujnJw1F7mwjyyfBxHDO+wbIK1vL2B7ZTHM2UPaG/wDTLnDdztIGnT1VfAywYh2GZMzDujjw0ol8FjPsXQTumN6fYjcxmkHkfFdXNU/8IspxGLYdLnNIDBZLWa/KNdEm6aCRZ6hLMuEoRq8Cd5IJtoMb/IDiKLyC2gfCYOR59bFQYmZj8xhphDIW6mymRvhMIafqzPDYLbsBLew6hNjngLHHVFrfEQ5umNhEv1VgZQDLJMt+yWtBBJ5qzHwwyUtYx+hvhNk+sPlicyQljC5rYvK5lOcW83EaTYXGcExucGjHR7kA2wDmJvZ+08xuE7bbOB9FAmjjIoonO2j2dKI3OYyENcHxnwrfFRDWB9PIN6nCwSLqTY6MxHQY2HUQ1se+ppe8kG2Ne2gW8zRAbsKoLB8JiQ6TjWWGxtJcPK3xY2v2JfekB4ANbuBFCrVrIOGYnmRni2QITG/ysYRNGH+ZvmJcNQGmwCQRYURaMscmNZJ5KWeSgEUy8LMa0n6wza7Gm3Co9ZBGrZ3Sr+PRQT8KtLXXiWeVr3A0NJ0uIoHVd7WdtrHNMSSLXaiVqSYEYmUWnvxIApNzTBiPEPha/wAQMcRrADQ7TzoWdr5G91VxMTgL5KGfBqZfiWXuVvYPQ7kgSJ6Kchl2QWGxkt0I8M2MRCEkpH7LqvhCfLP2a+BBs2p8S9o5rNxWYeELKxZc7Mns7q8pYRlppc5Z+jZxOMA2CglJc1Zn1hx5tKuQvO1jZcuyu2by+jtUwohLGSm7AtB1FJ+VtmFLudB1eTmmZI6RvtBVpi1LJXUqK4ixN4djY09AsbMMOGHbrst7P8W9rSaQbh55XytNEkGw1pAJI32JBH4LTGDnlsc3GutYfJqYphBbsdiSf9oP6lVXOAF0dgCocVjJCSPCIPYyC+dnqOu/LdVfrDgbdGavq7n0PLpurnNyzRdiARRF/EKfKMSA51Cjt8gqkzgHOax2rzODRXIBxDS4jmaUrMulB2amQWWJhJtvJlZljWNkc2jzPQe/v6quzMY/Xl2H87J/EGAewte9vtWL9Rv+RPyWS1qozSnwGOVVLdGxVH01ChY6XytFOT5QRXmA69bC80yuV0T2ua4g2W032t+Xl7Fep5ZC4P8ALIJGOa17JANOprgDemzpINgi9iCm1JMz3SlFPBpHKierfx/ZU8dk50Hdn4/stZ0+nmq+YOLmGk7ajIrJZAAZf9rQe0H1J/Za+J4eeWai+M/F37LCmwZ8e7N2iDH4wsiolZJ24i2jt6XRu26MJPsH3YKiQSPcFcy4kOq9rWRjp68wUmXZkCQEuE5NJjtVRGE3VnoMca7Qyy4dO6SEc2xEklNFj/hJMlfFPAin8ZqbI7kuAy4lczRVrAyAs10UO5vnj3mgdupVKHM3tcCCjY8zTFaeGypxfbPZo2RUFh8Ry6Bbb+CocI412IdV8lv8R4TSzumWWfHKM1FDVyUugZ4dxjpJKf3RifDFBef5XitOI01zKN58G6g4nZSmScSutras46IM+wYfGaHRedMjexzjpBoHY8l6disU0Mq7KB8fG63nSQDsDXPr+ilksPBfTNutgvJO427w4zzPs7/GgrbJnEOaYwBdW0ggWB1JWiY7Nf6R8zf6BRRsa6YA0B56sgCw1wFk7Ddo590kaluaQR5FgopZDO1vKtLaDQ0n7xiHsP8AcS3mQeYBTcbRuFm8IZY6HxDK0DVpDC1zHh2m9VFpO1kLTzDDgm7paa1xk590m54awD30g4MPwrXtHsPB5gVbSLPftXqvMBNW1u7UNvgvbMc6J0Do3bhzSCF4tmmH8ORzAbAOx7jpaXbHnJo0s8xw/os4Oaj0aDsT7T3DqP5S9J4JnFaQbr3feJdRrrZK8kaDyR19FWYhmObHIbjnBY4HTQc4EtcL5HU0Db+74KkZbXkbZXvWD0LGYcuOyp5piPCjr0WhJi2hxb2PXn8QsLieS2Gk66TUMxE6CmE71C3oCsTij4mq1I/GGYhqysZIbIVvIrDwSFlgt0efs6uo/wDPdmt9E+YZa8NsqhlE7Y3Enb1Rvmj2vjAFboTx2WhrSfkmyxWkkZa7J6m1zkXGYjxn+UchzSRB9HeUCRpeQksrpU3uO7X+SvpioLB5uWApukKSktK1nFNrhfOPq7r7rczfjESbDkgrSu0g45Cnjk0v6mBK2QdCiXFcagx6RzQRSWlFLBWSUuwhw3ERDgXGwtTM88jnjDGGyCHO29CP1QVpWjlTNnfD9f3QkvsrxGOEXozvfqT8mgLuSvLXun5CJos6Q43I4NAAJFHdxvsDsbTJdmu6eX/5FchlDcM6ucuIH/jDGSfxmCoykXh5L787bA77Myea3PD3BzQ4nnGAAGA7+UbDaksVxa5wrdDU8mpxP8oKNNTeCeJS5l2as2dPdfmO6wsdZ8x/n83U9pk4sFCWWi6go9FEK7lU/hyxyXWh7XX/AKHBw/JUQpIz+hS2Bno3HmNfh8wnaCdLi2VnYtkaDt8dQ+CHMXnr3ilqce45k5wbwbk+pwiT0NuLRffdx9xCF1dcosopPcux4m3UjcWRyUC7amxDHNvstPzR6bLmDnCiq65SjjnsrD4fpCTh/i12Gbp0k+5JDdJIrgLk2cpdCdpPZdDDzpW4F5GgKY4R9atDq70aW/wdlzZHlzhYbyvujduNw+vwDWqrqk6NeVkmTyqHByP3axx9wXRg33p0OvtRte0QYKOJoLW7HoAuxYWNxLtIvptureFeyZPGJ8BIwW6NwHqFrZFl8zonvjY0gHzPcaq/LTR1O/u5L1RjYpT4b4/Qgir27IX4hyPEQtk8B2mEkuMbtLHEMab0aXHUCN6dp+az3JQFzsinhgViZCWm26fMBV2NhexC4cGXRxsYxxkOp3XzRyVpcN6Atj2+pB7BR4p4IaL3Op3us7X8EX8CAadnGQDcaq8l7loP9vX4qtcVKWCJrOGBeJyuaMW+NwHuVNe3YqESgtLKvbekLz8DMOogHnztaXT6GNnnFJUvQo+BmN9sk9RvSjl4JZeoEho5i+ar4ZAyeZGM2fQ0nNZ+y0uKsu+r4l8Y5U1zfc5o/UH5LLH8pZXw8MDZsYiZj44S1pDwzTIejiDTSB301fw9VZw+STPbqDdvU0VRyhw1N1cg7/kfmvRopx4dNq1pprUo5ZNx51Ph3MOlwoqPSjT+imR1yCz+ClbwxHRcRy6XsreF/QdwFjCuIulFSPosnY/ygcgbr8lEeGozQoDvRFo+Fg3ANSSNMXkDGN2aHEGq6pKeFk3BO7Kou7PiuHLIu7OVC629Vm4OBjw7xHltaS06h1cA8aatx02du3qtD+nYUnec0HPrzNPlDhpd7II21CqJsg1S4Krl7HcejsOXsbydGPc6ifkujLmarL49XeyT86TTgsJv9q+x/mZy8tnYEEi+Q5lpo8iY24LDmvO4eaj9ozf7OyQSNgHAjcbgiutHZP3/ANJhei4/DGqEoq/7nED+UoMTipsO1z8OWSPaN49RJcD0aXdeRrrVLMjgsX8+S6MILuvySnZJPllWk1jBoZZxozEAtaQyUe3DIfDProkHkdv90kFZXE3EGKa10XgBoeKO7L787sEX02T/AKi08wN/TokMEz+0cq6K6uWTE9DDduQMcK5L4mIZ9YZKIyQ4EAlri03pcQCNJ3/hXo2ZMYJnGOhqDTs5reQDTW4rcLC+rgbfCrPLouHCNPMX6klCdzbyjRCpqWWzUkkv724508WR8D6FM+tbbvPPenfpaofVm7VS59XaOn4ndU8svbG4NB+JB2c++ntcu9KJmObVazX+r5qqMOOwXThmen/6j5Ze3/smDQweSYY4lmKmayXSzQ1jnRlgdZcHODtnOF7duful4kwOGxLJS4QNPhubG4Nic9pIpp23+RCyDC34fJPOHaO2yZHUYazyZZ6acpbtxn5HwqzDRmWdzXOc4s0eRzWgC2uBsnc2NwOXJasUsQ2aG9tgOv5qIQt63Sa2Ju1dSlyvk3lM0qLS5LJmj6mxv6LvjN5XfxFKs+NqQibvZ/496nmn7YcFhj2AGjXejzXNTed79KpRaGmq2PNcEbevT+Uh5p+2TaSulYen4fqkoTE3+BJTzWeybR1ealxw3SSVCwncwkDY+KSSLAOIofFNfzSSVSD2D80gN6SSRXQTpC7GwFJJAgmNSDdkkkWQ45gTgwduySSgBpaLXSNgkkoEQHJdDdkkkUQbpXdAtJJEgiFxv6LqSBDrBuFxJJEh/9k=</t>
         </is>
       </c>
     </row>
@@ -1520,25 +1520,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MOHAMMAD NABI</t>
+          <t>SHASHANK SINGH</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>t20blast2021_122</t>
+          <t>smat2023_094</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>114.3</v>
+        <v>127.3</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1550,94 +1550,94 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>28.6</v>
+        <v>18.2</v>
       </c>
       <c r="M9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>5.75</v>
+        <v>11</v>
       </c>
       <c r="Q9" t="n">
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>28</v>
+      </c>
+      <c r="X9" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD9" t="n">
         <v>12</v>
       </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>2</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>41.7</v>
-      </c>
-      <c r="W9" t="n">
-        <v>12</v>
-      </c>
-      <c r="X9" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y9" t="n">
+      <c r="AE9" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>-4</v>
+      </c>
+      <c r="AI9" t="n">
         <v>3</v>
       </c>
-      <c r="Z9" t="n">
-        <v>23</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>14</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>11</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>21</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>24</v>
-      </c>
       <c r="AJ9" t="n">
         <v>1</v>
       </c>
       <c r="AK9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>All-Rounder</t>
+          <t>Batter</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYWFRYWFhUZGRgaGBwdHBwaHBweGh4cGSEaHBwcHhocIS4lIR4rIxkYJzgmKy8xNTU1GiU7QDs0Py40NTEBDAwMEA8QHxISHjQnJCs0NDE0NDo1NDQ0NjQ0NTY0NDUxNDQ2NDQ7NDQ0NDQ0NDQ0NDQ0NDQ0NzQ0NDY0NDQ0NP/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgIDAQAAAAAAAAAAAAAABAUDBgECBwj/xABHEAACAQIDBAYFCQcCBAcAAAABAgADEQQSIQUxQVEGImFxgZETMqGxwQcjM0JSYnLR8BRzgpKisvHS4RY0NcIVU3SDo7O0/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAIDBAUBBv/EADMRAAIBAwIEBAMHBQEAAAAAAAABAgMRIQQxEkFRcQUTMoEiM2EUNJGhsdHhNUNygvAj/9oADAMBAAIRAxEAPwD2aIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiVm3NtUcJSNWswVRuHFjyUcTAJ1SoFBZiABqSTYAdpM0XpF8qGFw5KUgcQ4+xYUwe1zv8AZ5Z0x6ZVsc7ZmKUQepSB0Ftxe3rMe3QcJrgTSRbJKJt+1PlL2hWJy1ForwFNdQO1nuSe3SUD7fxbG5xeIJ5+lf85CCD4zuKYINhqPhPLntjYdn9Oto0tVxDuOVQBx5kX9s2zZPyvVdBiMMrfepEr7GJHtnmRLZrC9rAeJmapQe27Tl8Y4rcz3hb5Hvmwen2DxLBFdqdQ6Baoy3PIMCVJ7L3m2T5Ozkm27sm+dDvlErYfLTrsatEaa+ug+63EDkfCepkXE92iQdmbSpYimKlF1dTxU7jxBHAjkZOkiIiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIBTdJ9uJg8M9d9cuiruLOdFUd59l588dJ+kVbGVPSVmufqIt8iDko+O8zcflr25nxFPCqerSAZ/wAbjTyQ/wBc83pUy7BefukZMlFXwiRs3ANVN9yjjzMuv/AiR1TLbZmCyoq20Eu6GG3TDOs28HShQio5NNOwKg1C37Z3o7AqFvVsfZpPQaWG3SalADcBI+cz3yImpYHoxazEDuk8bCUcjwt7/wBdk2B6cy08LeQc5MtUIo0nHdFkdTY2bhYaTSMZRelUKOLH2ab/AD3z218LaaZ052TmVXUajf2jgZbRqtSs9imtRTjdbmv9D+lL4LEI4JNJyFqLfQqSLsB9pd48RPo2k4YAg3BAIPMHUGfKTJpu4z3n5JdpGrgFVmLNSdqdzvyjrKPBWA8JuRzZI3iIiSIiIiAIiIAiIgCIiAIiIAiIgCIiAIiIB8wdLcV6bH4mpzqsB3U+r/2zHsKl87rw+MgVm67njnck97G/slt0ePzp7QPMb/bKavpZfQ9aN1wqS3wtIcZV4KT0BM5x1C0pkcJkJkXD0WMmGgQJ7YHVXF5MoMOUjU6BMmU6BtCTPG0H1lVtmgrUnuPqmW1rSHi0zKRPQeN1UtnFr9aw1/XZPS/kRY5MWOHpEPiVIP8AaJouPwuWuVOgzb+W++nhN6+RdMoxg+9T38rPadGDukcqorNnqUREsKhERAEREAREQBERAEREAREQBERAERODAPlTH0DTq1EYHMtR1I7iRLTozQOcvwC28TaZ/lAVP2/EOjB1dg4K6jVRmF/xAiZ+julIkDiZnrS+HBqoR+LPIvDjUpgZjqdwG+ZE6SUk0bSQgtOmueogZjv033kDaGMpEXOFUqQpuqC/XbKpuSDqdBpKIRT5XNU5NZvY3/ZW3aFQDI6E8ri/lL5QCLzxg0lpuhCEZtQCCpAubaXtw8Jv+wtotazE93wkZpRZKPFJGx1ayJqxAlHjOnmFQ5Vzs1/skDzO+WG00TKXYXsDpNAxSVLPWCKgDDS4S2a9sznW5t7hvM9g10PJRbV2zaKfSWpV1SiwXmVN+/ulkmILAEjKT5HuPPsmt9HMfXq0TUIZQqq2ZXD3VywUlG13o1wGzbtJtWGJqJrbNzG6/jE1bDQg7q6ZofS7D5KqOPraHtIP5E+U275IcMFp4htbl1BPPKp08M01/p0tkRuTgHx3e6XHQSrXw9NbsDTqOpC2F+tYXB36gXl1KolFXM9ak5Sdulz0+JwJzNRiEREAREQBERAEREAREQBERAEREA4lftvDs9CqikhmUgEb/wBcJYRPGro9Ts7nz1tTZgfDlxvppft00bvGkdGj80vaT75tPSPCCk2Ip2tmZrcrOAf+4zU+jT9RByJB85hd+FxfJnUw5qS5ova2Gz3B8pH2ngEqKmcOWQWB4gDUC/G3bLmgnLfMj0ddZXGTRY4p7mtJhajsCTZVUIB90bhpumw7FTKbdk61xYSVsmndi1uQnkm3uSiki7xlLOmnKa+cHVBYOzMrCzAm9wN2h08ZstNraGZ2p8Dvnsb8jx22ZU4DCIlPIlO2t9ee6/fJyHKJlShqZlajprDuyN0jUOl9HNh6vYuYfwm/wmw7Jw1kwi6EFaev4VuT7ZSdMHyUHNt628z+UuuhbOy0VcHqLYXFrhVy38biTgr2X1IVHa7XJG8CcxE6ByhERAEREAREQBERAEREAREQBERAEREA0X5QNnZsj20bqtbeCLlT5Zh5TzTZmGanUdGt69xY30Ovxnt3STBmrQdQLsNVHaP9rzx7aaZKqnUEi5B0PEbvKY6sWpP6m+hO8V1Re4Yyz9B1b8ZS4Otul6K6qhbsmc13KLEIwZmbUDhJOwtpsFKumS7dXUG/iPdKrHYpnJCjS8y4OgwAIIJB7yO20lYjdvZG21MaxcI1FwpAy1BlKX5EA3B8JLqOQRyIHnKnCFzTBN7i/wDmTaOMzDK48Z610G25Z0tZzUMw0Klor1rQtiL3Nf27hFrstJycpYE232HCbXsOgFfS9glhx5cZr2BotVxSgWsAWN9wA0v39ZZu+Ewopiw1PEyyjBuSfJFFeolFx5slxETaYBERAEREAREQBERAEREAREQBERAEREA4mifKjg1NGlVt1kfLfjZxuPiom9zWvlAw+fA1ea5XH8LC/sJkJq8WTpu0keYYerYCXznPSFvGarRqXEvsPivm7TA0dOLwU20KpDooHUJsSD6vaRxlvhcPhjr6WuhUDrZQwY63IUC4G7fID0s2o3yVhsTZQrU92l7c5NPBYkurRbO1JOtSxTs1ho1Nt5NrcOEx4XbTs7K1I2U2z2ADAnQ23jxEkYB0KlQmvMi3tMlNSRVyi2vvhyVjxpdWyxpNpcTDVO/9aRh3stuUj4irYHxkSDJvRQ3xT9lM/wBy/lN1mj9CNa1Ruaf9w/3m8TZR9Jz6/rOYiJaUiIiAIiIAiIgCIiAIiIAiIgCIiAIiIBxKXpcwGCxF/wDyyPPQe+XU8z+VbbDq1DDq1lYhqluPWAQd1wT5TzhbTt0PYu0l3NAQlTbgd35SUlbhODTDDWRHBQ67uBmJZOg8FnRqNw3/AAlhQWq2uYjwlThcWNL7x5y9w+OUISbXtPHFk4zRIw4cDUk+ElLm0mPCYxCL6dnj+hMlTFqLW1PCeKJ65Epqlha8h1XLnIDpx7pHeqzEAC5Pl3ydhqGQHiTvPbPXgisl30SKrWZbi5TQc7EXt5iblPF+k20XwzYauhsUrgHtVla6nsIE9b2VtBMRSWqh6rDyPEHtBmuiv/NMxajFSxOiIlhSIiIAiIgCIiAIiIAiIgCIiAIiIBxEg7R2pRoLmrVVQfeIBPcN58J55t35VlUlMLSLn7b6DvCj4kd0lGEpbIi5JHplaqqi7MFA4kgDzM8K6d7QGIxdZ0YMqlVUjcQgG7sLZpVYvbGIxL5sRUZ+IB9UdyiwHgJjtrN1HTWu5c1YpnU6FlhnDKGG4i4marRBG6VmzKmV3pHceuncd487zYKNKcOtB0puL5HapyVSCfUoamEsdPb+clUKT2tYnxlzWwJI0Ej0UZGGmnd+chxkuBGPDbPc7gQO1tPZLTD7NYeswH4d/mZa4cArff4WmZafZ8Z5xnvCjBh6AUWAEy5uU7BDymdKI0Mg5ElE0/p6g/Z05mslvANf2Xlt8n23vQHJUa1N7ancrbge47j4Sg+ULFBqlCiOBLnyIHvMw4BbIJ2/DaSnSalzOTr58NRNcj3tGBAINwdbid541g+kWIwgDIxZB6yN1lA5jiPCbxsPp1hq9ldhSc8HIyk9j7vA2irpZ0/qimNWMjbonVTfdO0zloiIgCIiAIiIAiJwTAETVdudO8Jh7qH9K4+rSs1j95r5R537JoG2/lAxVe6oRQQ8F+kI7XO7wA75bCjOeyIuaR6ltjpDh8MPnagB4IOs57lGvidJ55t75Rar3WgPRLz9aofHcvhfvmilt5LEk6nXUnmTvvMVSvwUWm2GljHMslEqknsdsfi3qMWdmZjvLMWbxJJlZUfQ2G72yVayM54D/AmLDJ6t+LA+WvwlrjyPFgl0UI3cAB5TNmnQJpcHwnKm5liVit5Ou0kIyVF3qbHuOo93tm07FxgqKDxlI9PMjLzHtG6Y9lVGRxynI8UpWkpdV+h1fD5uzXQ9CoLcWnZ8IDvEw7KrZgJdLSvOGzqkahhwOEkBAJz6MicqsXPDgJ2TpiXCIWPASYqTXelNUimQDJI8bPNsfiDWxbOe23cNPjL3DDSU2EwhzsxNgouTa+lxuHEyWu3qCEq3pgeJyKR5B7z6fw9qFG7OBrE5VGkXOS4sd3Ka9Ww5puU1sdQeY5HmRp7Jd4HatCoQErLfcFfqN/V1T4GddvYeyFzvQg2Oltcp05WY+U3cUZK6ZkipRdmZtgdKcRhrBWLpxRrsPAE3XwPhN+2b8omGewqBqZ4m2ZfMajxE8eZ8u+FxObePz85nqaenLuWxnJH0Vg9o0qovTqK4+6wMlz5upYplOZWKkbiCQQewix9s2PZfT7F0/r+kQb84zD+a4b2mY56Rr0u5cqq5nt0TQdk/KXQewq02Qn6w6y/6h5Gbls/aVKuoek4cHlvHeN43HfM0oSjuixNPYmxESJ6UvSDpFQwaZ6zWJ9VRq7HkB8d08o290vxGMDWPo6GYLlQ7y24M2hc9g0lNtHGPjK74isbA6235E3Iig8TbQcTcmYDWzsgAyqpGReAuR5k8TNNOOcK9t3y9hOPClxbvZfuYKyFSVsVsSDuvobcN0xZDx85abRpgVagA+uxA59ZgR3giRWXiBpN9FqcFLqZ6seCbj0I5pHvmIiSiLW5HcfhAQGWOJVxELHA/NpwN2PuHxkrDUCXGmioSe9tB7L+cy18Nesij7C28S0k4PDs4dkRmBZgLA2sDkX2IT4zzh+LJ63giMgFrGZKCXI/yfASQuEBYK7qGIvlUhnsOJA0UdpPhIdbFvm9HSXIu4vvdv4vqjsE97IjYn1ai09Kjoh+yxJc/wJcjxkzC0UfVWVvwn9HwM1jCbMAdmbWzWOa50YAq3PjLqjgRcMAVbTUaeMzaig9RHhm7W2sX0a/kSvHN9zcMACnDyl1QxQtvmubLxvB+zWWeJQLrfQ8bz57UaWdF2e3JncoaiFaN1v0LVsYtjMRx6jUnwG+VCVtd47pzVtx0maxdgl4jarG9hYTXsbimqNkGvMncJ3xWLLHKm4DrN7wIwVKwBUEsTZABc3GrMRyA117J2NF4dxLzKu3JdTl6vXKPwU9+vQwVaCL1QOqmrnm2/XTW3LmZq1fDhmF19dST4m82zaCZUdRcKo1zEFmc8yNNL37+6V2Jwtsh5KJ3oqKjZLByOJt3bNUTCAMVI8PfL/FO64aoli65DlDHVPvK2psNDl3acJxtPCZSHA7/AIyxogFFO8bu8f4MjwrKR65PDNeqjPTVx3H9ecxYNM11k/C4PJUq4c+qwzJ3bx+X8JnTZmFP7Qi9rA+AJ+Ehm6fsTvhmLD4bNdn0Qf1HlMjXfkqDhwsOMssclzkXRR+ryLhqQcsTpTp6seZH++gHPuk2rYIp3yc4KgHqUwbqgemTzN3UAH26SyfaValiajqxQ52uAdBYmwHL3cwZj2emtMkWL1kJHIZlAXwFp22r9NVPOo/tYzHSaq1HdYyl2R0NVT8iMUt7Jvuy/wD+PsR9r+hP9UTVMh/QES/7HT6GP7TIg4ltQgNwpJJH1n3M3d9Udg7Z2w5CspYdW4J56G8xU07NZPpU7jWIUlGHCjydSUpuT3Mm16RFSoQbkOzqftI9n9x9kgmqFIJ9R9D91vyO+3fLvGYf5vDPwKFDbgabEKfAHxGnKQMRgtGRtA2nYp+qw7AfZeVaaVlwc1f8jTqYuaVVLGE+51/ZwbqfVbjyPAjzB7iOc64fD65Toymx8Jk2IxZSjDro2RvbkPnmXxBltVwvzlJrakMCeeUrY+R9s2JpmCWCtxVIrUd/sYdSPxMWVfbaQ8NgMxwyWv8ANFj3Z2tfxmx7UojOBb1iAfwUENRj/NVQeBnOysNkWpWcfRUUTxRc7/1vl8JXxK5K+CqwWGGfEVLaKMi/rvnWjgLOmnP3SywlSlTwyK7jOzF3FiTcnkB3SK20xmuiXsLXbt7AZVPWUoLLRfHSVpvEWu50x2HCMlS2hIRvwt6p8D7CZIGIS2QXdxopzAKBx375W7RxdR0YEgC19AOGvfMeApmooYHrWvft4zDV8QT+X+Z7LSygviLzDG8v2uoXS6W63Mfe/OVWytns6dSmwcb7kBdN5zNYWlmmMCkg7gB7h/vNNOUNVScZe/8ABVGc6M1JYKnHuqNc2ym4vpv0t+u2V37U76A9T2+B5STtbBq7h1DKl+sv1WPA24fGYaNO7ACU6bw1RnxTzbb+TXX17lG0cX3Mq2VeQtMaY9hrZbEZUUk7hqWIG+x18hJNakhJD1VTLqbqxFrXtdQbHdv5iRnwDu75Sj5UFgjhmsddF9bTjpJ62vOLUY3SXMx06blncxYraaeiAZSpLX01uPzljdKgUob6buI7COE1jafLdb9bpirDrX4yinrpr1ZL3p01jBtlTCZkII3e4yDgKRGelxAzJ221A948Zr9PG1EYMrtpzYkdxBNiJK/4ns6O9KxU70O8ciG995qhrIy3wQlp5LbJebUwoKU8Qu+nZj2obZ/Ia92aS8Hs0CsX+65Hkov/AFyfsLHUcRn9GDlFiUcAEB73GhIK3DecmUcLkS2p9GjoOZVShXxy5Zepp2a2ZQ01hml49StMsPWc5V8TYeNhecPRCqlFfUpkZz9p+A7Qvv7pYV6RZxl1NNsics9tXPMDVv8A2zzmGnTXOQvqUxa/2mO8ntka9Xy6Tnz2Xc3eH0PPrxhy3fZGTCrmxFBOToT4HN7lkPFEM7tfe7HzJ1k/YRJrPUO6nTd/EDKo82Ehmnew/wA90ho6fC88kvxeWS8SreZVcltfHZYImft9k5kz0HaYnQObcqaSAH3ywSiRrv5zFTThp/tJmHIBs28DTtEpR62WDAPhAR9SvbwdPzEjtTDKDa+lj3cZnwb2TEIPsB8vEqjC7gdgOsUlsByOonM1F4JyjupX9mdzwy1SToy2lH81sUiUitdTewcGmx+8ozI/eVG/mpm1sodKbgcrjkxsD4AgDwlLtqnkRao9UsoJ5MGBHtuP4zNm2cBkYcA4cdzWJH82ab+NOKktmcatBwm4PdNr8CDtej1yOa5L9lR6j1P/AIqVvKUe1sa4orSUgZ3UPYC5Yn0huT22l3tzE2qU6ABLtSXNb7VYqPMJTbT78pcFVBq0GBJbNWqsCoIAzFEGu82B4cJy68qlSap0n3Ozo4UaFB1q6TvsnzsQ8TQLPZQWI0AUEnyEkU9jVMt2CJ+8dFPkTf2STjNoVixDOwB4LZV8QgExpsus1ytF91ycra+z2yMPCn/cml2Pa3i/H6IHT9gQaNiE5dQO/tygTBsjFegzLSZWYMeuU1UC2UKH8TunJUW3dluN5CUZKpv9a02w8NpQabbf0exzamsnO+EuxseI2yKlnqO+ZR1Te4vx6u6ZExefrWvb1lGhUaagfWEqP2QtrbXlJtLDkML3Ww38Qd1pvjCMVaKsY5O+WybiHDISCCLXFuzWRsIMil97HRAefM9gmM1QrWbqt2WCN/pM6VXfMAGAci2h6qJzvztc+3lPdjyxGdizsm8U+s5+2511PEC3mZGwDMM77iWvcbwRu1memFGHzjT0jll55RoundadKaWWx323SO5LY5q7SrsD843ZfU+ZF5lbHF8uenTqGwu1RSX00tmUgnxkRlsCATb3TJlGVCO4dsrempPeKLFWmtmzs1HDt61AqedOow/pcNaRcb0dpuH9HWyG1wlRSdf3ii1u0gdvOXuB2QWUu7Ki6XLHgSV0HYRqCQdxmc4FMgIcXDsuYk5WUC6WFtcxBG8cBreZp6Wg/Tddi6NeqvVb3NMweIxGCcMrqCyA3Wzoyk2KkkWJU2JA3eM3nYfSRsSHR0VXGQXW+RsxOtiSQbqARcjUSu2nhfQLTYlXo5yWVrFcjn0bXXcPWvf7vZMOC2d+zAv6ZXGcJaxWoClRH1U3B6qPqDM/BOnJJO6f/ZJycZxbtZkmpWCUyw3lSE5/OMzk95BQeExJQyoqfWOrd5/RmOmmZ1U6qi0796U6Yt/MTLPDUSxZu2w/XlPa782rCnyWWdLRL7NpKmoe7wv0OMPSyYZ2HrVHVB+FBnY+dhK6wKk2so3lvhzMudoANkTMFo0167je7ucxRBxt1RpxNpjyKgFSooWx+apkgAHcCb739wnQoStFy6tv25HDq5aXRFTYfYqfyNEtP22r9hP50/1RJefDqR8uXQ1+j9Xxmb66d8RPVuRZdYH6Zf3WI/8ArMh7P+hp/hiJzdZ6an+p2fCfvNP3O+2f+QxH6+skutnfQt+7T3tES+l8iPsY9d95n3ZAb/rPhT//ADtKXo39Kv8A6Zf7miJl0Xz5mnXfd6X+JZ4b6ZP3ie8Tcav/ACz+H9kRNOp9aMNH0s86f1h3CQ8X6694iJvexnW5ebN3CScRw7viYiekSj2jvf8ABMGC9Sp+6f8AsaIkZbEluSq/0OH7vynGI+rEREMxp6o8ZlwPrU+8++IkpbM9jujYOlX0572/tSR3+hHePfESij6ESq+og7Y/6fX/ABH31Ji6SfQ1P31P+x4iVPZli2O2C9et+Ie5ZdbP+jPc3uiJhh96fY7mo/pcO/7mLFethv3n+uQ+nfqJEToQ+UuxwZfM9zXIiJyzaf/Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTExIVFhUXGBcYGBcXFxcWGBgYFxUXFxgYFxcYHSggGBolHRUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGy0eHyUrLS0tLSstLS8tKy0tLS0tLS0tLS0tLS0uLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAKgBLAMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAADAAECBAUGB//EADwQAAEDAgQDBgMGBAYDAAAAAAEAAhEDIQQSMUEFUWEGEyJxgZEyobEHFEJSweEj0fDxJGJygpKyM0Oi/8QAGgEAAgMBAQAAAAAAAAAAAAAAAgMAAQQFBv/EACsRAAICAgIBAwQCAQUAAAAAAAABAhEDEgQhMQUiQRMyUWFCoYEjM3GRsf/aAAwDAQACEQMRAD8AqEEguOpWlwCtHhP4tjoZVHO0uywSR8gjZh+ExAXmZdo9G0dLw5mXPlmBe+5vMSquHcXGTvdWsFiQWtceQB/RWGYRuodZKoQ3TJUXCMu30UWUmgzM/VSNIACNEzGKqYNkauHpyHEEkeqBiqLnmczh02Wl93MD6JNpgfFZFqyKZWwmgJ+MWB5jqrDcS0O+Ns/llVqvhk8lm4BviLyA0nQEyY3PmhTJqmXuJYcucSKjgCCCBt5KvSw1Jv4WAAGQQJJ5zumdVeTGl9ead2Ga6zruNxqq7bC8I16NcED5I1OqJ2JMKj3eQDJ7IuFF5O2nmjTfgU0izxTCF7IABKxauFDWw6xGoW0axIN15r9qvaUn/BUnbA1nSQb3FP1Fz0IG60Y8P1Z1EGOWWJFniH2hYXDyym41nSRLQcrfMnX0lc9R+1jFDWhSccsC7g3NmJzAa6QInaVw7gyZA0jeUB1S67EOLjiqqzLkzzk7bOzofafis01adJ7JuGgsIHJpkj3BXT8J7X4fFvDASx5FmPtcawdCV5FM6qRsQQYIuCLEEaEckOXhYprxT/RMfKyQ+bR7tVYI1VGqIsuf7GdoX16Zp1X5qjNyILmHQyNSDb2W+4x6rhZMMsU3Fnbw5FkipIcPt1QapO4UaruSHPJDqaLDNqWUDWOklLnKh3c6okhb7CNxBCiHzdAbGisMIARUVYxcdEZpkSJkbDlzVV9RSY8i491VEDGDfbf+aE2qRfNHKEZwBGdpn8zeXUHkqdQgG0wrigG7L33guEwI3A+qYVJCoMrEQVf71pBgEH5K3EETihmpBBHomLo39lVe/dEolHTcL4oR4mRm/FT/ADAXlvLey6zDY1j2hzXCDzt5i68tpVi0ggx1FiPVdFhsfRc2Xsl25aSAfMbFEm4mfJhUirVoMbmyuBcbO6Domw7mg+NuYxYDflPRCpYc1KhtzVs0203Ad4AY+LklUObD8OrS7uzvNuvJWcDjGCQQQRz/AEWLi67miz/ETNvqo5y05pzCNf0Vala2dXg8Wxwg2G02Ktd5TbvM6brjmB3xG7ep+gW1wqoXWtlUuhc8Vdmq+tJkFNTqF0yh/dr2sVbZRgdUSTYptIBiMPmF5jeLe6pYqiGss2Y9x5LYq0xlVV+l1UoUVGRSfiGiAY84m8K/wtoJkXEXJHyWNiWQZ0vZaXAsW3xMsAPFPyQwS27DmnraNDEUd2x1Co4irlbMK66o0EkHXbdUeIOBb43ZQN0c0vgXj/ZTpcUaA7MHSSvDOP4lz8RUc65L3EnmST8tgvXK9QZrGQvOe2WDDcSXDSo0O5XmD9J9Vs9OmlNpl8rH7U0c/wAN4a+s8MYLn5DmV0NTsNWaLw49NF1HYfhrWUg+Ic7nrC6lzSdgfK63zyyT6BxcaLjcjyl/Ytwp5i/xcot7rnMZgnU3Q4L13jLms+J7GzsSAvPe0ZDrtIIGsGUWLJJ+RefDCK9ofsA8CvUt/wCv6OC7R1TWdFyX2ftjvnf6B/3P8l1hErmc3vMzfwVWJDZxfmrGFIiTKp5FPTyWWjXYd9UDRDdi5F9FSfU1QnvtGqNYxTkWatYbIbcV1VJ1Tn8imphN+mqF79mtSIO/uka0E/l0I6KsyrBUar5Qadjb6LwqhjrXaY9Qr1GmwD8wcDPkYu3qOSwhUmx9OiJQxJaImB8weYUcPwA2HxFLKbabFCZVjdXKeJa8FlS4uQW8+YVDE0CyDeDodiOiJL4Bci134yQR+yrBu6hRqRukT+/RWog2TrUiL+6tUsPYGdVSad5vOnl05KyzGnmR6BW4sikFpcaq3IblIJExqFo4VjHEOqEkuaDvbzWRwuiJJPw9dvNa/wB8BLQ1pyss0RqRuefklyS+CM0X8LYS0snxe0DzTY3AnKGwCGmesAXUqWIqNDR3Z8zf25K5jKxFJ1QCCRBB5abpVA27ObOIM2gDYLo+EEn+IYk7fUrjy42XRdm6gGYGTy1M84ROIeT7TpKLgTIunx9UsZmBA87qWHqiwDCB1T46ozIcwnkOqOujD/Iz6fF3aOYPMGPkUPGcQkQz+yrOqBxNrbKbaWsaJDkzSoRRW/8AJDSCXdOXVHw3d0qjRE2JcTsNv66qwxmRvUkT5KtisO5+dwi8R1AURbd9G04gjNNtVy3GOIue8taQGNv/AKiP0WhjhUNHLYwRaLwuarG8z6I/JMcEizRLS2ZE7jQHyXP9r8NmY18fC4AeTrH55fZaBqHfQIjqXeU6jSNGl3/EZhHqAm4E45ExuRJwaFxnhADJJquIZ4adM5QGMEaxdxM+ESSl2OoxcNqMhpMF2bW8O6rsGYUPbM2IHsbqFKhTptILmtBMSSBJ5DmfJdByvozxik7POOMUO9qVCWZi2SGkkTGwjc36WWaMC2DNJrDAnKSQZF2meS6bE1aX3k5ajXCQDzBOluSNxem3JoPRGptdAygnbOS7HOytqA7VdJ2DWroDX3WHwuMsj/NP+55cPktCZWTkRvI2aeM6xpF3vQRKcVenqs50xqisqc0nQc5E6hiyrV3kWT1aqA586o4xFSkRJjZKm5QJ9kybQqyz3vsn7yFWZUICRqqtQty0Xz/dMXDmq4q2QzVU0Aci82t8uSv08YHMyOu03I3afzBZlNwayZ1QqVaCq0svajUrUcu8jYi4KHmQaNW/Q3IRK9ovIO4+h6qqI2F78xE25fup94NnADkdfoqHejmpCr0V6g7G7wPENZZ8TItqFd7R1GuptNNu/wAQtHRc82qB8dpRcZxg91kpu8zz6JX03taGSA4Hitam7KKjoBmJkLTxPE6lY+Nw8tB7Lm6T55XM9VoUavumTgViNnDYbN4rASGwdyVawOONOrLRMeECbarFbiXWGsXjlK1sLhGgtEy43jlus7VDHXydrWxbWNzvIDel/SywsTju8eZJH5Bt6qHGshpDJUa3Lc0yYtB05lYOH4gAdJMHW6jTaE44LydG6tpYTYHl5pn17QD5/ssEcQi3skcdzKDRjdToa2IzRHkh1OI3ABiFiU8QfJM6red1WpeiNHEcUfs6P66LJrPuNzvfdPVxIvz6qi+rf6pkYgpUErG2pR+EVm95FQwHCJ06/os7E1ZNkLvxunRVdltnf8KxWXCtm5YCCeeWw94C5HHcTqYn4KgYQ8tYGtLnTG8aSpcN4xlpOY7c/sQfmfdO3GGnSLaDmhxJN2h1zr8S3LtWZW+6OWxrKtGoX+KZkgtIB8tlexPF3OpmQAbz5R9ZQsfiK2b+I9zgDyA+gWG/GF74G5j3OqYlfbEylXSNnCw1jW8gBPojh0KqXX6orak+axzVuzbjdKg9Ug222TA5W9EzMORJ5CeiBVfIshSGN0Te7kgGpChdReeiNREuQQPTgodE6p6lT0V0UNUd/QUXm3VRc6VAAo0gGTL1HPuhuKYhXQFlhj9p9EQOCqMRApREy9RqkGxRKj1n50UVuaDULYOHKbawGqqirBBCd727WspqRSCmuSAJmNEOo4DVV9NUJ1ZEoBOZYqVLCDoiUsQ7WVTYZKNlt1lW4oDZ/Bp4Sq57oDoLje8C179FIcSq95mDvFpbTksgPIT96UH00FuzWrYlz3EuMu09t1AYi/LyWeKp5qTairQmxqjFSdUTD4kzfqsgVFMVzzQ6Bbs1aeIJt7KzVxhEA2IlYpqaQVYrVi6JdcW9PPdA8YxTLzqg0JkoVWoAFQqVo9LIQq+ytYyPIi0+ogOKiHi9/wB0zkaj8AOXyavZzCtqvdScCc7DEagtIIIUcbw3F4cHK3O0GztD0sei0uwWFP3mSRZhMRJklsX2EFd/icMCDZOt43qxdKfaPBa9fEPMOBnrZWuEcNynMdV6Bx3hYBJ0joFjNwZAmEf1bQH0ad+TncSIcfNQpvgqlxWoe8c5p/F6GIGnoEqOMDoBEH3CbPiTSurFQ5UG6fRqMxRiJtyUKlTlZCzcrjpdQLpWXSmavqWWswglBdWuoA2USrSI5BC68hM9yhmUKhVpAOXQWlWA1unfVBJtAVQotBs/RE4g7PwFhRQ2vSzqUSw9MTqYCFnT4mq0nwggRoSoU3wpRGyYUgVAVQk2opRVj94kShylPVXQNluo0FCFIKOfkpscZhDVDbTJxAQjUKO92iA8hREY2ZJxUHBRJRUBYQOUg9BCclVRVlgORabvmqgqWhO1yqglItl8BD7y2iAaiH3iiiRyLfepZkJrDAJBEiRbUItKnNiLclqwcKeTvwjPl5cYftkRVva/lp7q1hmHN4jzMDQW+ZRKNIDZW8LQvmXa4/Dhi7Xb/Jys/Knk6fg2OzeNFOsypaD4XGfwuygE+oavRXkjZeUMoBssPwukA9DtPO5811nCeOAMayo8hzQBmOjotJ5H5Lneo8HJu8sFaf4N3A5uPVY5umjQx2G7x2krA4vXytLR8RkDoNyugxfFWU294CHT8IBBk/oFxeKrFxL3G5/oDySvTeDLJLea9q/tjfUeascdIP3P+jB4hgmiw5fJU6eFHJazAS+pPT0kIAZ9SF3pQTdnEUmlRTqYQRKDVp5fhJ8jf+y2qDJsUm4cOHv8jCGeCM1TQUczi7TMNriY2PJTIsjYmlJdGxt6IeJplpAO7Q731+crh8zjLFJOPg7PEzyyRe3wCyp3hO1u6gVjRqIlNTJmxUS+9x+yfKioCxVOiHnkKbnBQlWCxbQnY3Y6dEWmxpmTdDChROUmOnRDLk4qxfdSi7J1RGqgXpYioTCBmV0C5dlkSrLBAVVjlY70IZIZFhXvKAbzKi6odVA1FSRbkMXJF6BUeod4j1FORaD+aZrkFz7JmuUomxZzJ5QA5SBVUFYTMi4Ol3lRrBuR7an5BV5W52Nw+auT+VhPuQEzFDeaj+WLyT1g2blXhzZki0AHzQnYZtoGs/JbFd4AqE6AH5Qsqg6S07ePX0/mvTqKRwHJlF9KXx8vQSrlFkKeGozL93G3Ros0e1/VFZTMhGkLcrEB0QqlIDQkdNRC0aHDqpDn90/KNTldAHnCHx/hdWg0963KXMkCQTBtNjZTePiwdX+DPrVGtaTOgmN0AukeRbPmYVnHUc2RuxcJ8gJH6IGEbmY53OoY8mmB9Fb80WvFg6MCs+RaWyOkXE7JY6mBVqxTNMZpDCSS0EAgEm5WzwIUxinOq02vbkzHNdrYEl7m/iiPh3kLT7bFhDCGDPAJflax2W4AIZYgzvcc7rPKdZFGhyVx2OMa+DPVHwdnVByf/wBgHfqVVrqrVxXhfcjNTHuJZ+o9kxy1KUdiFIzn/wBR+q1+0+BihSrRHicydnCAQfQyFh4f4SN3ECOU+M+wIVx+ODqPduBNvCegM39lyebByipL4OxwMsIqcJdXVf8AK+CvRpAtd4my0D8Q35c0E0ds3tf3QcJRcXQDEj6aK6KTmtJJEzbe0LjvpnQTteCk5vQIEkWVp7kJ1z05IkLYApNCK8DyTMhECRDYSDVZyKDm2Jn0F1RKK5Kg/RFrDlcILnRujQDGcToSmDkOo+UwCIXZdzKRKASpygaGpjkqJSeVEOVpEbBu6KARS5CKJC2SDkjEyFABJSirDNKfMolwj6pNcqoKwwXffZZh3EYlwEiKbTPUucfLQLz4lenfZZgC/DVSDBdVgbNJDRE+5RYo3NW6C3a7Sv8ARe47hwyjUhvi8Rk3tbfSPquMq8RGVgHxNYSettR/xHuu84lw/JRf43+JrgW5gWSAwyBlkf8AkPsvKcSYI/3NPq0j6ge67eLJ7Lu/2czk4/8AU+3W1dHtvBeB4XuMOahaKrw5wDnFoeGzlbOjR8M2mys8MxlFjqrq3dNrgkMDWzTa2Jlhpg31k62XK9nuJUH4eh39N9WoGl13OyhohrRra2bbqro4uG3p0WMgkjUwCwNLbRa0+aB4Zzu7ZneSMfwbOIx7XGmQ2pWYHBzsrK7jDZIAdVeZlw5CwK5Tttj3Vn1Xua5t2tyu1aAQIPXU+quYrtLiHCO9gRENDR05SsDjFZz2VC4kutJOpMhPwcd43bF5Mu3SIVjlYSfwtkfRC4TSjD051In3uo8Yf/h3nmwD3ICvUmQxgGzQPktX8hH8f8jYO1YOMkD4gI8Q0LbnQiR6onGcTno0xDQRkBLcoghrxltq34fKAgNxZZmAiHayOhFuWqpYriL8rhYkw4WHxMJcPqQkzg9thuOXVGRia0LGr4gZyNdLeodHyV3E1cxJ5mfdZNOe/HTTz2/n6LNmm+jVjj0bTQQCSRIlgOxqVDLyDyAhvouxxHZelTwtXSpWpgFz2yWjMyQGwbtyxc/m6Ll6VMSB+CiC47y8jruLepK6Xh+GqOwffOhoLKmYkxnArt7sEmJcCK9rmI5pXLi9PI3jSW90clh25T52lWHtt8QuQPU6JqktAtss6o8k2O++y4FWdtukSqNHX+f8lVeLq1jB4iRoTI8joqpbKYhUgL0ah6euiC5Szo6FJl2jLvDuSoCmQ8BVe9dpNkzHuGhVahbluo0C89NVQxREqV90Nzd0aQEpWBIT+qcBPkRCyzCkRZCzqRfKBoYmNUUWlIOUZV0VZItUE5coZlZVkgEycOUgoQGnBhFLUJzVChzUXpv2b4lzcKcpj+I63oP5Ly5em9hBlwY6uefnC18KCllpr4M3Jm4wtMt8Y45VdmacsA7NAMS20i34G+y4Hi1iYP8AmFuv7LrMaJc6Oq4/tAeQ0t52XUywjCHSox45ynK5OzvOBAdyHcmBgHIBT4viCykPzOMDoNyq3ALtyDQw4euv6JuIO76vA0b4W8upWqP2oxyXuDcMwdR4Ja0kNidgOUk22RK3CappeI02lzpvUYd5/CStQ0w2i6i3Umm4+QLgT/8ASFiG3Y3r9FcU5X2DKaj8FPiXA5pZTWpj4BYPdoR0A+a6bD9j5a0vrZM0ZQ8NYXeQLiVW4YxpxFFrtDUbr0kj5gLY7Zg/eL6ZRl8t49ZXH53Jy4cjUX+Pwd70zh4eVjimqbv+jmOOdnBQFTMKgc1uZpJaWu8bWmIb/m5risYYqN9fovZO2Dv8A3P8ZY3XWwBP0C8b4034XJ/EzSnjbk77M3LxRjkWirr+78mPXZlcRtKzsLTPfzoDcE7wSPrK1MaJh3ogcMo95VY0mIm8T8TifXRJz5Ixab8WFixykqRtVMrWBjTr8R3N5+sm+qpVnkkC8A25DmQF2NLs+wNvUcfIAfqVmY/BMp6D1N0vL6jhaqPY3H6dlXcujlqeNIO8ctlHEYppIgeZ0/uqxp+U9ENw2XN1Rs3ZcHETAaADAiXC8TpqpNrGNG+cCfkqDXat0OxR6Dtio40Upv5J1qYm3T6IRarbHkWPT5KpUNz5qIjGsOqiHJJpRg2Ee6blDyckRsJZVCMrZVKVOqBNkgAoADUgbKJUQoSwguoFqZifMoSyLQpEJBSeoQhKI0oSkCrImTcVC/NSDkz38lRbZEBel/Z9gHVMK+CfC8iJjUA+R1Xma9e+yphbgnuP4qjo9AArWeWD3x8kWGOZ6SKOP4XVBPxezT9AuM46x7KgcSZac141GmnWF6jj8RckrzvtW0uNtXOa0DqT+yYvUsub2tIa/S8eKLmm+je7LuihmbPwhjfXf2C1+C8Ph2YiA0TJsi9nOzzhTp0pgMEuP+ZxkgeVh6LZ4tgCyj3bbueYJ6brq48/tVin6an5KPZHD/ea9Z78wa9uVoaJOVtRkELfZgMCa3dl1fODl8WUNB62Vjsjw403DLAOUgSNpHVX+N8Npuc3vKgY67v4dIy6SBcyZOnuky5FTacml+jHn4erSjFNmHxHglOiKj3uJNN7e7AMHxCWkx/XhK0uz+KrYgzVyOp07lzmNJnkDtzJQuL08O80zVfWf3bRoGszAgkZs3xGA4+6mcRQYx1JrKuUSCC+GyZF8puJEFc7Pkc57N30dXi41DjfTUe7/wCk/wAfs5ztZxI4h74+BrHhg6BpM+sfRcRxPCl1OeV167iOEUfurnik0PdRcZuYJYdJ01XDnh+amfJP403CDT+TRLHj5DWipRVHn7sOS0j1VLBPy1x0gewAP6rrauDDXDquJrS2uRyefqUrNPcTmwfRcWeq4epLR5LO41h/DKtcAaXBvkr/ABqh4FyV1I3S7ieNVCMxE6Ej5wpOfB1ROLUctZ8c/qAUGsJ3M76R6Loo4z8kqT2k7A8yiBt5BBvqFV7sFPh5aVGiJlx7iN7qBE3SaQNfPzUiFQT7BgJ4SdbVV3PlXQL6LbADuk5iAx6stMwqaLTBvw86KTMPZHY0wT81OeZVWHqjIa5OkkmiRs11EpJKiESVMvlJJXRCMpBySShQ5coykkoiEQ5e4dgWxwyhG+Y+pe5JJI5P2Gji/eU+KAl/Rc06j3mNwzdu+Bv0k/okklcfyjq5/wDa/wAr/wBPXuG0gA4+Si6nndPskkuogW/dJl6q404LTDkqmK70jPTaSLA3kXBty0CSSppPyJ0Uo7NdlLEPGezG2Eb3hpbe/IwpsxDhJGUEiCQ1oJHW10kkOqH/AE40ujNx9Z7hlzuyxEAkCOUC0KvSZaEkkD8myEUl0jnON0I0XnvG7VyTAByn5AfokkkX2ZfUV/pJ/s9R7LUv4TT0CNx0w1JJc9/cCvB5FxZ3+IfMZZH/AFCqui5n2SSXRj4OQ/LBOakkkiAJ5ZRZSSQsJAcW68cv1QBdMkmLwBJ9kgVNtUpJKUVbDDEpnVgUkkDQWzP/2Q==</t>
         </is>
       </c>
     </row>
@@ -1647,12 +1647,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ARJUN TENDULKAR</t>
+          <t>CHRIS WOAKES</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>smat2023_068</t>
+          <t>t20blast2023_105</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1686,58 +1686,58 @@
         <v>4</v>
       </c>
       <c r="N10" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>4.25</v>
+        <v>7</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10" t="n">
         <v>1</v>
       </c>
       <c r="V10" t="n">
-        <v>83.3</v>
+        <v>50</v>
       </c>
       <c r="W10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="X10" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y10" t="n">
         <v>3</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>4</v>
       </c>
       <c r="Z10" t="n">
         <v>28</v>
       </c>
       <c r="AA10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC10" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AD10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AF10" t="n">
         <v>3</v>
@@ -1746,17 +1746,17 @@
         <v>4</v>
       </c>
       <c r="AH10" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="AI10" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AJ10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK10" t="n">
         <v>2</v>
       </c>
-      <c r="AK10" t="n">
-        <v>3</v>
-      </c>
       <c r="AL10" t="inlineStr">
         <is>
           <t>All-Rounder</t>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxASEhUTEhAWEBUWFRUXFhYWGBUYGBUWGBcWFhUYFhUYHigiGBolHRUVITEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGhAQGy0mICUrLS0tLi0uLS0tLS0tLS0tLS0tLS0tLS0tLSstLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAAAQIEBQYDB//EAEUQAAIBAgQDBgMFBQYFAwUAAAECAAMRBBIhMQVBUQYTImFxgTKRoVKxwdHwBxRCcoIjM2KSsuEVs8Li8UOi0hYkNFRj/8QAGgEAAQUBAAAAAAAAAAAAAAAAAgABAwQFBv/EADMRAAEDAgQDBwQCAgMBAAAAAAEAAhEDIQQSMUFRcZEFE2GBocHwIjKx0eHxFDNScoIj/9oADAMBAAIRAxEAPwCXwrhxrE3NlW1yNyToqjzM0LdnsKq5XLZyL+HM2W+11AOmnPfW0r+zOMVQ6E2JKsPMDRvkNfnLzEMqVHNRQ17lC2S1zswDsA2llOtxk6G816z354BhcxhaVLu8xAJ3nbX9LI4jhlVarUguYgXuNAQdQxv8I1G+x0kZ6LAspFiurDTQaD8RLfinFlqO4fxKyqGZPtKSQVzbi5tvra4O0Zh+LIgVQjMig+E21JqB7mwtsCPeTh74BI+fNlUdSo5iA63y0esz5Kuw2EqVLlELAbkW36XO58t5HvLg8Tpk+MPUsxZSwpsTmChgVYH7AsdxrHjjfRTTAXw5beE52cgA8iCoP8oj53/8UPdUo+/5+B1KpLwJl7U4+CTZWCkjw6bZXDD3LIf6ZQQ2knUQo3saPtdPkiBiExISZEIhiExJIJjTKDHdqKSXCAuQ9jy0tuOuukrl7V1NTkFjtfYSs7F0mmJ6K+zs3EPE5Y52WujZnqHalTlzJvvY3t7S3wXEKdUeE6i9xzFvLpDZXp1LNKCrhK1K7224/wBKVGmBjCZIoQgmNMDGkxIkGMJgTGmJEEExpMDEMSIJCY0mKTGkxIwEhjTC8aTEiSwjYkSeFqQZJPEaxXIarZfs5ja3T0kaEcgHVZYcRoUQhCOmRCEQmJJNJgYRIkSIhgTEiThExvazi9TM1KmcqgWYjcnnr0tNPxKvkpOw5IZ56pes2UAszn3J6/rpKGOrFoDBvryWz2Thg9xqG8WHP+P5UBQTv+MdTYgXt9/Tp+t5veEdgs4BqVCp6AA/jL/C/s9oKNWZvW0xDXYF04wzzqvI1YDmR6zvh8S6EOhylTf8wfKeqY3sLhyPhOm3/mYLtB2behcr4lNx5iOys1xtqmfh3AXuFpuG8QWsmZdOo6SQZjux+OtUKMfiGnr+hNgTOhw9TvGSdVyOLoCjVLRpqEhjSYpMYTJlXQY0wMaTEiAQTGkwJjSYkYCQmNJimNJiRBBMYTAmNJiRQlvFnO8IkS1sIQhLIRCEQmJJITEhEJiRJTGwnWpRyjU+I/w8x69I0ogCVxiEx1SmQNdL8ufraMKHTzikFPBVR2oP/wBs/t94kPsPgwczkeIWHovK0suMLnpsg2IufOxv7DSWSYNcHTao/hWw/IAdTMTtS7hG49yuq7DblpkHY+wWr4OottLfTpPO8B28prpTwz1dbX2H4z0Hg/GKVamH7sqbaq249Zkd2Rqt41AdFzxWxsJjuM4fNmBF/KTO1/ajFU2y4enSNjrm6crajz+kzB43j3cGph1fXUJvr53MfJuCl3gAggrLUeGmjiqbAXHeLceR0myDg8h6ED6EWiY/h+azBbMGBA22INjOFUm5uLHmPObfZ/10zPyy5ftlgbVaRw/n3S1E5jb7pyJklTcX6hr+o1/KRDNKmSQQdQsgIjSYExpMNEAgmMMUmNMSNIY0mBMQmJFCaY0mKY0mJEEt4Rt4RIoWvhCEJYyQxpgYRJwEGJCSMFTub9PvO0Co8U2lx2UtKmajwxupTv7sX/jN7eRkfNbXc/j+t4+o93J5C9vQA2+6cTa2ptYD5nXX5yFrTMO1Ik/rkpajgXZWaDT9nxP6Gy5s+5Ov60hhznsL3P8AF5C+3vEq7f1C/wBZ0wNPI19wfpGxNXK1wGsWVzBYYuy1CLZr+3qp2FwQIqEi+YEegtaXmNSm1Hx0xUNjlBtoVtqfmZFwtJmU5GysLEcweoI5jX9byeaCtRQqCMpIK9DZbgnn/vOefVc4u8vSy6bC0A1odsSZ5/ysInCcZUqKq2Snm8aDL8GZDoQrDMVzi2liRqbXOo4DgP3eqVDltNRrYdN9z56b7S+wVFQlzKV+ICnXNsO9U57EgCwGmUi5Ga++krkl1lpNaG7qHjuAU6j1Rcq7B7G/NgQGB3BW9xbTrK7B9j6lJ1fvCMrOzEb1MxvYgaADymiTHlqqs2HKeKym9zlN82cWsvUam8usXkK3G8WZwESmytJDlkuIUWZlC7l1GvmdSfa5ldxqgtg6XK3K3P8AFbmOo0OvpLysniW5y5mtcbgHcj5yJ2xcDJSWx1vp02+8S92e54rNA8Z5Qs3tRlM4Z7jqIjnKz9M2X/MfmAo+sikyRiDYBfn+vMkn5SKTN+nu7iVyYCCYwmKTGGSIgEExpMUmMJiRIJjDAmIYkYSExpMDGkxIwlvCNixJ1so0mKTGwlihECYhMSJEiTuHjT+v8rfeZAknBVN19x68/wBeUq4xpNEx4HpdXMA5ra7Z8R1Ciq1vx/GLWp3XyItf02/D6zriaNjexKk6+XUTle3w5iDyFj8xJGuFSKjfn9KI0nU3FjtQoT5vhJbTkdpNwbvzt9JGq1dLZD5E7j00nNL/AGiPYyHEUy8QSOkn0WvhKjWiWtI4/UAPVabBYsIQSfYeek0fDan96DY+IMfMEWvbkdCLeXnPP6WNC6IuY9TNN2X4iWq93WYMzowAAA1Hi1IGpsDqZkuwrmGY8t+cCYHNaVDFtgs1uLjSeE2nyBU3F94qnIL2Zh6aEjSU3COJmo10QsftPoTr0bl6S5xVRhmA12+mxkPDVVa1rhmPLTXT8xM/7StpjgblM4viKgGY0hfoCAbeRB++duEu7UszXAK3s3xDW1jb9aTpiKYQXdi3q19ems40axa4GgA1/CMbmE7ntiQoWJcK6szBQG3bYHW15R8Rr3qNUY3J+EHcDkT09Jf9o6ZyIqFQ182vkPTzEx9ZWDEHf53/ADm7gMOGjOdT+J991zPauJc493H0gg+cfITGa8YTJn/D3tckJfqT+AnOpgmsSGDeQNz8iJpB44rMFJ42+ctVFMaZ3oUC3MADc8o84BrkXGgBJubC+3K/KOXAWKJtNxEgKETGkx9emVJU7j/zOZjgyllgwUhjSYpMYTEiCCY0xDEMSIJbQiQiTrZRCYsSEsVEQxDAxJwkJjbxY0C5sIkQEqVTxxG4v57H35GNq1qZGlOx63tb2G8cuAY6A69JFDMhNjY7GVmspTmZr4SPTRXKjq7QG1dPENJ63hIXI3bL6kj6RnfufgzfzG/05CODsdtT5AX+kV6NQ7qT63kxICjYDq0E+S4qtudv5fzj6TlLOpCkG668xqCeZgcM/wBj6RhoP9n6fjGblmApKhqm7gbeBAC2GNxxptntmUi46ajY/OZvH8VIcPTQfW0ua1IvTp2bemhuDe/hHMbiVL8DLNZibetpy76gkhdpTpGA7wUB+PVW0ygdd5ZYLitXRQAt/wBXj6nZmkBcX+cXDcNyeLb8oIqgaKQ0pUbjdbxsRqFRUU9WZiCfpOJR1Bvsu1ToLbfOSMeuZrBC+Wx8NrXF7Zukp0rC7hx8V723Fzc7+3ym/h5fRbyC5zEZadZ3M8REDlyUigGJQAZyEzG55vt9J0AtVUOpS1yOd+t5xRldiUDgkC9io0Gg3Mcylbg0mObTNmUtbppsJK4yb8Pm8eiGmBlte/Axb/zPquNUoUazWCfAObNzJnWrY5bG5qlb+igf7n3nSnRqE+JVVNsttQLW0NtT7zpUwKgDJ8SqQtx15kjnBNQaT8/tSNom5j29+EgaKixFTMzN1JPtynEmSMXhWp2vrfbeRSZZaQRZUnNIMO1QYwmBMQmOkEExpMQmITEiASXhC8Ik62phCNhLECI0mKTGNEnSkzrg1u48rzhOivlpu3lp6/owKn2+nVWMOP8A6A8L9L+yMDXN61baymx82NhFSoKq3GjjcdfORGOXDDrUqE+yi33ztWwZRVencMoGYcjpqR+UF5E630HkrVNroIiRF+uvMbfyn0Wyq79Bp5H9EQfFuuHUlhmdzY6bDT75yxGJ75AtJSzsbsii9raX03BMszwimz4enVxVOiLBcty1QvbMRlUWXkNTzgZmtu/c89OqkFNxGWmZAGuguZ8lFXC1iL94dtfAdOe8jYp6ncVlD52NNgD0uVH4maPtCvcnJRqHIBmzXXXNfmNfoPeY3A4l2dwbkZdyeYOknw7C9mY76W01UWIcG1Cxsw2M19dLba6LQdkEIpopJOUAC/QaTXjDA2mf4AFIuNDsR5iabDncXnGvaWPLXag3XbNe17Q5hsRbkubYcWlfxGkAlgJdESsxQDOQTpBJRALzHH99SxK1kYix8QGzL9kg7jS3vLTiGHDklAbixt1Ui495M4rhVLtbxZAxNuWmgPvb5Soo44fvbj+BVSmQOqqPqDf2nT9m0nuw4zWM25fo+uvBcv2lWZ/kuDLiPq57eY8+B4JKLlKTMNCbW/XzkqtXKUKZJu75iCeQ2l5xrg1HEZFwr5KhK5kYtlOZL3ViLDxXG/Me8XinAauQZlYBQMrBTa1rb7EGx2hd6y2exJmD6Ju6cQTSMgCARvx5G+6rP3C/xVGJ52/3nOthaSfFVYaX3G0U4XEjQVdOWpkfOalNw/xpz9Pi99Ied+ue3gm7qn9ppwfEm8Dmo/EMSGIC/CosPp+UgsYpMaZMBAhQOOYygxpgYwmOklJnMxTGkxI0XhEhEnW4MaTFJjYSw0kbCIYkUJI/iFNzSVVUtc62+l/pOZknC967rTSxZiABp9b/AH+UjeCYPBWcO5rSQZvYRHEcVxx2Ht3YIOWmi6C12a+ZwL87SxxNegqiuBUqKcreEi+UkZrC2hF9QTp9ZDx18zK26OykdCMu1vvEl9k8StGsEcgUqjC9yQEYm7C4IsDa9jpqb6WjAZ8MKrRJLSY5q5Ub3ONdh3usHASPD50krSYfiWFwlFMTh6XfUHJFV0JR6ZvtUQ6kXtzEhdrONUcZSNO2Qqc1MjUhvU8ielpkuLiklXEJh3JoMdBfQnXNa2hFzYHmADrvIuHrXFidrfcIsLhBAqvmdROo4IsZiniadOIFjvPHx9VbU6pqI7kakC56EoGI+bTK1sQcM7VrZrXAX7bNsPoT7S3p8VWkrLkZybEcgPCBqfaUdU944d9bXyr/AAoDvodz1J6cpddMZW9eHzZU8NSIc4uH0nbj84+6TC9smGrUGV+qaAn0IuB5XMveHdt8QjKamFYIbeINmB6nQD1tv6yqXDFTmABv6fjJKZrfCLdDt/tIH4FtWO9+o8hPUX9Vep4zuP8AQMoOv1GOhJHUFeg0uNZ6YdWGQi9/KYbjHarEVamXDIPOo+a1uq2I08xJWHJ/d6lMDKMy66m1wSR76H25c4HdZRYG9+f65Slg+yGU3vLrwYHgIB5TeJiREiFaxfa7qjGhtpF9pNxsZi0xOvIKibiPEs1hUUb7KljbUnaT+EWYllFrvdl5o53U+XMHmDEUWzP10UDpy+ZjKdI5wV0f/Dv723HkZpNplpkEnmfx/UHdUXua5pbAbyEX8ePsVtcMDTak2tmItrsQ9M+2zGbOj2lsGNUZlynW9joCdCPK882WpjCFDU8ypme4RgwCq12JHLW5MMdjyy5R+gTb8TAq4dtX7lWpVKtCA069PVbxcFRxFJsW9NMJh1UsGL3epre7BLBNjp4jMR3mHdT3NIolasQCWJful0d9SQCTm9Nd5Fx2LepSKXOW66DnY7W62vb1ktcSAc2RfCoREGbKLCyjUk5efM26mQ0sKabzN2x72HirGIxRqU2loh0xr4a+A0+BU/E+HPRsT8LXKk6Ej03t57SCTNnwrhFfGLWOe7DIXU/FUDEgksNlTKCEGm1rnfJ8VwTUKr0mIYqbXU3VhuCD0IIMckBxbvw8gfdKmCWztx2KikxpMUmMJiUgQTGmBiGJEAiJEvCNKKFuDGkwJjTDWEAgmESJGRIMl8KxIps1Q0xUyKQASSAxtYm24tfTnIRkjCUqj3WkhqM3hy8iBa9zyGo10toZFVpmowtBid+A31sreCqNpV21HNzZbgXuQDlFrxmiY2UStiyzBv4iLG3wsR08/L8L2etmHT8DLHj3ZathaaPVAyu2UgG+Q7qC+lzodRbUekp0JBsTrybk/k/Q/rymhQcxzB3ZkadFHiWvzl1SzjfreeXhty06Jh2eqKaoXZ72VQSSQMxsB6EydjMHTVC1ShVoVGRO6XKwXMqqWLFyC2axAt62GkiUa6rURnAy5gHVr5crXXxW1tYnbrLleIU6KMj4z96FV6ZsBWIVUdWZyKg0ey5QBfRjc7SKs5wcI9JnW97jrE6Kxh2tLJPtGnMG82gniYUOtgsM5YJQxGbvO7VQjahclww1PekCqcv+HlaxhLgaBTNTw9Soc6jZ7Es5ITMri96drKAGzA623tuK9pu/Rsoy1RjDWSoLDwIaq0iw5VFBUeYUcwYYztAj1aTpfDJTY1CFCkGs+rvZjYgkBQDso87SFrapaLHffhtxvtwvKsF9EOiRttx/W/lBVdjcE6rUQ4J6bZi6mzkrQXMGvdyDY5LnW3i1kBMBUyBhTYq1ypymxANiQbagHSWWN4ymakcOe67liUVUCquYguRZmLFrAEHSwttpOXFeLd5XeomZFJK0lBC93TGiUwFNlAHIabyekakQR1nl687XUNbu5sekc5200UCiTqPT9fWcMQdcinU3zeQ5+/5zsgtcki3K0jUn1Lczrr0Gg/OWSqjBcn5K1HY7s/Sroa1YZ1p7Us2UMRkvmNx4QHBtcXymajhPGqDM6BlwFNSwWnTCU3dB/wCozDc6H4TYX3JtbLdn64oIzrUylyQxVrFbDSyBrm5LcjbQ6i80OF7RqiMc9PvCykf/AI2V1ADHvH0bvNwCbC4B5zne0aFWs9wDjE29xpEcTrxXRYGpTZTEtuRx8db3v04KfgKVWpXZu/rHD5EdUqux7wlrHwv4goUE3BBuR/VgOP0f7ZqiUWSjmABKMq3CHMdha7a8txte01r8bolmYrRfLYk3UZmzZ6jsVN2vdrWuBcc7yk7S4qn3ZVaeUEDKpLkgs91u5JDkLTGxO525vgGuoPAuZgX8j5290WOAxDSSRYHQDltb+/FZ+lmOvPl7WIv5aid1TLub/rf1P3WnCg4zG3JV9r3vr7D6TpVrDl7fnOhELmXExlC64fidaiSablMwW+U8gyuLt6qPa4sdZ07XZatKhWVk8KIjIgA7vNnIU2GwIYAakC3WV9ydAL30Frm58upnCvfJUW5UgC6EEHQg6qRpaVa9JpIfv+VaoVHNGWLedlVGNJimNMglWwEhMQmKYwmCjhLeESESULbxpgYGGVhhBjTAmMJjIoQTNj2ZwVE4QmodXqG6g+IhALd3YaXJYE9DpraYwma/g6h8PRSqjLSz1WLAqAyeCnUZw/hKKarE5tNOo1gxBIZIMX/ZV3BtDqhnh+gtD2oxVOvw2sQVujIHAOYK6umYXNrix0PMEGeU92AN7joeXSxmoXi+BpDFUKbsaNYLTVFpktZaIpA94zgC5VWuQT4dpjBUZNB4h0G3seX8p9uksYBpptcCDEyLRqPHhClx31uaQbxe/A6z1Uqu1111/H/eVwxIIFt9vQfoSSHFswOnPylXXuGy2Frk6bm+/r195dc6FXoMBBB+cVYrVUi40OY6305H85MwpuDsf/Ei8E4XWxDilQU1Ha5y6aAWGZjsF1Gp8utptU/Z1jkpk/2bnfKjnMfLxKB9ZGcRSYQHuARPw1R7SWNJWVwGBqV3WnRpl3YEhRYEgC51Ok6YvhmIpv3TYep3gFyoUswG5NhfTzmk/ZXTP7+yspVqdOrdSCCrBqaEEHb4pL49Wxf/ABl6mFpNWegEJQbFDTUMD65iNL62NjaQPxThVcxsQGzfjbfSLqZmFaabXGZLo/O2srA1lIIWxzMbEEWI56+wjKJBLW6gD0A1+s0PGFr4/iFY06FRajFR3ZsCuSmqNmJ0ABB1Ntxzkofs54giXFNWOpyiot9eWth9ZKMQwRnIBImJQdw4yGAmDE/PJZ9mBUWsLkfnrGZwNbBvOdaeEqs4oojNUz93kt4sy/ELcrEG/wBZsMN+zHFMt6lZEa3w3ZvS7Bfuv6wqmJp0ozuidPgUNPDPqTlaTx+FYQVr3PxeWxkXDN4yzAgX6a+Q+stu0nA6+DYpWAQnVCmquL6lW/RGl95RDFMFy5rXvcdRzufaEKgcA4GylFIiRF9FPoVx42+05A8gAF/CNNfcge5/KRsM6lRrlGgv5nkPMmXlLhNdwMmHqEeShP8AmFT98B9emwS9wHMj+0TaD3OIY0nkNFO7E8VSjiCangL0nppUJCik5F1ckg5b2y3vpmkztRRZqAFVagxFKgzsazrVLUw6rdK1M5XW9RtG8QyrsDc0eK7NYjdsK58g1I/9QkGggov8DIxDAo2ZcwYZWsNmFiQbX3lEupVqmenUBNt+FtOXwK2WVaNKKjCByt1v6qnMDAxhMkQwkJiGKY2MiRCJeESS25gTAxhMJYYCUmcyYpMaTEiCQzrxjGE0adMs4Wmu2c5DmZnuV2v4jr0nImWtPgoUrVreJmCsqH4aa2GXQ7vaxJ5G4HnXxGKbh25nCTtz4+XnyWhgMI/E1C1pgbn28Z6cVm6FK4JS9S4sciM49yoM74bhtc6jD1/anWH+pZvMIwsNZPpXma7tyrMhjR1Put8dh0gLvd6D2XnFbAVaZLPSqoObOjhfdiAvzMzfEyQ6kHQ3tPeA08v/AGncOpo1J6a5GdjmCjQmxOaw52B9biWKHazqpDHtjgR+j+1BU7KFGXsdMag/wrv9jvFaCGvTeoKVaqE7smwzAB7hb7kXBtz9jLvDdmuN0Cz0MeKpYa95Uc388lRWUN53nmfBuz7VaqjE0a1PDtoWUIrL0NnBJF+imb/gHCcThMWhoY16mDU60yXLMPsZDameXjFvSFVrsa9zmuaZ4gEW+eCFuHe5rQWm3Cym/s0pYj/iGLbE/wB8FIqE5b3LJb4dNkG2lrS87JIDjuJVydO8RAfJM2b7hOPAKhpY3GYiqLJX7ru7XLAKuVs42GoGxMgcDrtRwOPaoO7rVXr1AhILHNTAUix18RbaRPrsqZi0i4aPxPkIRNoPp5Q4GxcfzHWV27PY0UeH4niAUd5WNarr6kIp8s5PzmU4P+0DGUWapVqHErlIKVGCjOSLFbLpbXQaa+k0PYRqWO4ZVwfeBKil1I5qGfvKb5dytzb2Mj0+F4DhIZsZUp4qsVutIoup6IjX3NrubAD11tB1IOqNc2STAEbCwg8FVLapFMgwAJJ8d5HzVWP7N2GKr4nHNTCOxVVANwtxd7X5nKuvrI3H+xXEcRiWxCYykGzE09agNNQfAFsDl0te251kH9mXaeitarSqlKPfEOlrKge5vTHTQiw/w26TrU/Zj/bvUOJVMPnaobAhsp8RU38It9q/nblBee6ruJdlsALZrRoPnEImDPSEDNck3i86rp+27EKmFw4axqd7/wC3I3eW8r5PpPGcVTrin3xo1FpkeGoUYIb7ENa1vObKhwrCYrG5qRqVcLSt/etmFR7kgLoP7O1tOdhuGnpFMI6MHuQFsqg2HvKdTGHDjum33vbXZX6WEFX63W9dFiv2cYKl3K1rBqjX8XNRtZenn1m5Bmc4NQNKpUVaLKhN1CoQoJ0a1hbcE/1S5OJA3uvqCPvmTWqF7y4rVZTDGhoXeq2kzfFaFOpdHAYdOY6EHcHzEvUr5tgbdbG3zlNxNAGDDfaRAmZUsC4K844zgjQrPTJzWsQftKwzKfWx18wZBM0nbulauh+1RU+4Zx+AmaM66i4vptcdSFydVoa9wHFIY0xTGkyRCAliRIRJ4W5JnMmKTGmEsMBIYhgYwmJEElTUH0m57WJ4UqDYojfMA/jMKZvccwq8NoPvamFPqng/6Zm9ptmmDz/C2+xH5axHGPz/ACoPDa4IEtRVIGgvM/wczRUl0nOLrnJi44NtoRuDvK2uFqVhe3gUkbaEmwtfbYy2qYAPyiJwlF1AIOl9T59YQQGFzwfDl3I1l7QojQbflKY500U38iPynCpxasm9LOP8LC/ya33wswQFjitFUwfnI9TC+Ug8N47Tq6BsrDQq2jA+YMtUcnzhEBRiQqytwxG3QH1AO/rKjEdksKST+7oCdyoyk/5bTVlyOU5NXHPSJrnN+0keacw7UArE1OxGE1GRxffxt+MenZHDZcjCo6/ZNR7fJSJsTkMQUFkv+VX/AOZ6lAKNAXyDoFR8O4PQojLSohBe9rk3PU3Ouw+UtqFEjovoLSSKAGsCDICSTJKkkAQAmZOrTnUp3/iMSrTMj3a8ZOueJW25lFV8dVV85aYysddJUUMwroTzYCJouEZkNKzf7TGAxaqP4aCD5s7fcRMkZfdvq+bH19bhWVR/SiqfqDM/OspCKbR4Llahl5PikJiQJjSZImCW8I2ESeFtyY0xTGkwliJCYwxTGmJOgmbTstVFXAYikdTSbOP5XH/yVvnMSZf9hsWExPdsfDWRqR9SLofmLf1SDFMz0iPP55K7gqnd12ny6/yu3Bb9Jp6O0o+GUslRkbkTNHQozk4uu5cUoq2itiZ1FFbTi4UQlFZc3qg8pDrITJjlesjsyi9zeCWowYUGvwgOQblWGzrow/MeRuIpxOKw+rDv0H8SfEP5qfP1W/oJI/exHjGRNEJ3GdVI4dx6nUFwwP57a9D5SazI0ynEuHKx7xPA/MrpfXZhsZFo8Rq0jZgTr85JqooWxZNdDGXIlNR4yDuCPWSk4ipiiEgrIViJ0XFC0qWxIPOc3xoEZPCt+9jdDKP9+tOlPigI3vGhOBCmYylzlLRrL3pqNolFTUY+Sgk/QSXiMZmEzParGClhWUGzV3yefdpZnPu2Ue5k2Ho95Va1BiKnd0iViMZiWq1HqN8Tuzn1Ylj98jkxSY0zqVzKQxIRDEnAhEIkWJOtqTGkwJjSYSxAkJiEwJjTEiCCYU6pVgymzKQwPQg3EaTGkxI4W+xjrUdKyaCqgf0b+Iex0kxMZYC5mH4bxlqQCEZkBJA5qTvbyPSSa/aAE+FDbUk3sbDU235Tn63Z9XvCGCRzHqurw/alE0hnMO3EFbF8b/ikSpiwTo085p9tGd1X93GrAX7wm3U/BrbU+04f/Wx//XIB/wD6f9sgGEqnZW/8mnxXpjVAf4pyYId2PznnA7bMdqHzqf8AZOOI7YYi1xSRb9SzWP0j/wCFVImEv8unxXoyikGvq3ry/Ws6Pj6SakgW8xPJq/aXGP8A+plHMIoH1NzI5w1arq5d+d2N/vOknpdmvduoanaDGhek43tphKYP9pn5WTxfUaCZzH9uXfSlQyj7T7j+kfnKClgxba0dQwjlrCynU6zQZ2WxpEyVRqdpOdMWUTimPr1G/tKpbYgagA+SjnH4bj2MpWy13tyD+K/+a5tO/EcK1yStthf0HIysNxbnb6SSrh2t+mLckFKuXDMDdaSh26xC/HTVv8y/iZNpduri74cjW2jg9ddQOkxG5kvAMPFdc4tmym4DZGVytxqAVVhp1lV2Fpax0VgV6g3W9rdpctNKr4SqqVc2RiUAbIcr21uLG29t5Erdp7MQtHQEgHNvr6Sv7b47CVCj4S4plb9zdiKJsL9VUki5AY66mReK0QlaogJIV2AJ3IubE252tGwuGpvEvbyF0GIxNVv2n8K/w/a8AeKkfYg/fKDivEXrvmbQAZVXkq7/ADuSSZCJiS7Sw1KkS5guqtTE1KgyvNkkbAxDJ1EEGEIhMSIIvCJCJPlW0Ma0WEJYYTDGmEIkSa0YYQiRjVIYq7P/ACH8IQiKkZ9yyXD/AO8/pq/8qpOdTYfyj8YQlNn2+QW2dVxo84H4f6/wMIRm6DkU26nYLn6S1wX9wf6YQmlQ25FUa/uE6j8K+0bU3/pqf6TCElGg8vZQt+7r+CuFX4F9DKxfj/qEWEp1tlcp6Fc+Z9J0wfL+Sr/y3hCVuPn+QrA+dF3X4T/K3+kyz45/fv8A0/6VhCSH/aP+vuoD/rPP2Ve0IQkqiCZGmEIkaWNhCJOEQhCJOv/Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTEhIVExUXExgVFxYTFxYXEhYYFhcXFhgYFxUYHSggGBolHRcVIjEhJSkrLi4uGCAzODMsNygvLysBCgoKDg0OGxAQGislHyAuLS0tKy0tLS0tLS0tLS0tLSstLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCAQj/xABBEAACAQIEAwQHBQcEAQUBAAABAgADEQQSITEFQVEGImFxBxMygZGhsUKCwdHwIzNSYnKS4RRzorI0JVODwvEk/8QAGQEBAAMBAQAAAAAAAAAAAAAAAAECBAMF/8QAIxEBAAICAgICAwEBAAAAAAAAAAECAxEhMQQSMkEiQlGBE//aAAwDAQACEQMRAD8A7jERAREQEREBERAREQEREBEo3bb0nYXAM1FQcRiBa9JDZVv/AO5UsQptysTqNNZQsT6Y+IMb06GFpKOT+sqE+bBlt8JG4Tp3aJxzh/pscEDEYIEfxYeoTfrZHUa+GaX/ALLduMFjgBRqgVDf9lUstUW12vZtNe6TGzSyRESUEREBERAREQEREBERAREQEREBERAREQEREBERATjfpa9I9Sm74LBsUy92tWW+cG1zTpn7JAIuw1ubC1iZ1jjPEFw+Hq129mlSeofHIpa3yn5UTh9TEMWJub53bfvOSSSb6km5lbTpatdyiKdY+IN7nqed/GS2ExAGjAa8/wACBty1/Rn+GdmaJ9rMT56Sw4Ds9h1P7u/9RnCctWqPHs5/UVHF10bmpNtuh6zTVmpk5WJ1BDXsUYEEE2IswI+OvSdTxfZvDMPYseola4p2Vy3ZDfryuLc/1eTXLCL+PbXDqfop7cHFp/psTUU4mmoKkmzVk17wFhcgWvbrfrOhz8iYHiT4aulel3atJgyZtiQRe9twRdT4E6z9X8G4iuIoUq6ezVpJUHUB1DWPiLzQyNyIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgVX0oI7cMxKpuRTH3TVQN/xvOP8DwuSi9/tMD/AGgmdj7d8Qo/6erhnfLVqYd6lNTcB/V94hXPdzaeze9r6TlnEKyUaKAnUgN5lh/kfCcsnTth4lk4da20mcP+tpTsF2jpq2XI2vO2nnLhTdSuYdBp5zF6zD0ovEtjS0j8VT38vlNar2loIxRswPW2nxvJHCVUfY7iJrO0e8acv4tw27M17HXQc7nlP0N6MD/6Vg/CiF/tJX8Jy7iPDgHKkDQn3g2/x8J17sXg/VYHDoeVIH++7/8A2m7HLzcscpuIidHIiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgct9NdNFOGqEZizNTtzsAWBHjmI+JlR4/hM5TW37MDUEgab2BF+Wx5TqXpO4GmJwmZrhqDeuUjcWBB91jf7s5rVxIdaZG5QG+4IIv75wycTLZh1aI/1A08Blpk1DmGtrgAjUc8o2Fx5nmNJPdkUYYc573ZrrffLbu+4jX3zS4qS+SklyXIFhbbna/QAn3ScwdMqikC41ACkHawFjzsAJwtaZhqrSInSCxvDajVSEax1sSFC2tpe46yY4PhKiNrYa8tiOVx+vfJukQVDL7xsfIz5lBYSPbjSPSOZaXEaYasC3sBRzsCWJAF/dLz2JLt653dnuyqCxJFwCTa+24lSqK1S6oASWyrcXHd0FhzOa/SdG4HgPUUKdK9yq949WOp+c744mbbZssxGPX3LfiImhjIiICIiAiIgIiICIiAiIgIiICIiAiIgIiICcS7XVlTH4hDpZtPDMof8AEfGdtnEfTZhjQxaV7dytTsSB9ulowvtqhTT+Uyl43Dpjt62U7jWNz6Iu2lxues3MFjq3qgnq2qb3LKSNLb8r/lInBV0qgIeTHzJlj4dw+ncDvba978LzLPHD0aflztLcM40wZUq0ylxbNsPC4+E38dxFad9dbyscfxVCgoQDvMwB1NwL67/rWQ68TNQjclm7qddbAeUitd8q3yRHDtvo7waNSasyguKrgMeVmbb4y5yt9gMN6vBopOoOp8bC/wA7yxqwOxv5TZTp5+SfyfYiJZQiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgJD9q+ztHH4Z8PWGjaqw9qm4vldfEX94JB0JkxED8h8c4VWwWIqUaujJUZc63yPl5qT4a28Z6pcXYJYHUjqZ1j0l4NHxVZCoKuqMefeCgXHjp9ZWuGdicIVDsrMde7nYLp1sb/OcLzH2044t+qiUKdWs4sDUY7AXJ986B2T7Nmj+1q2NS1gu4TrrzNpN4TA0qXdp01Qfyj8efOSWFoEsqjVmNh+fkACfITna8zxDtTFFfyswcMwFbEYm6uyU0Kmp0OmigHTMdDfkPcD0jhNkApqAq2soGgFpo4PCrTQIo23PMnmT4zMSRzmzHT1rqWPLk97bhORNHB8RDaN3SDbwP5TekKEREBERAREQEREBERAREQEREBERAREQETzUqBQSxsBuTK/xbtCwFqNNiT9s5Mq+JDMDr79pMRsWFmAFybAbk7SpcT7WAq3qQSM/q1I9uoxtYL/CDf2jsAWNgDIjGU8TWS1TEOOYRMhX7xZO8fIKANNT3jqcEwDIWZ2LsGIUWsq3AuQo+0drm9hcC1ze0VVmUZ2tBXE0ydVqU2UH+en3reZVmP3DI/hlbLpfS/uli7Y8MfEUUWkR62nXSqi3ALAK9NhckW0qX+7KlxENS8ybW8QbEXHjM2ev5NvjTuqap4gasdAOcs3Y7CllOJcWzjLSU7inzY+LG3uAlW7NcNOKqquUigneqH7LHcU/G+58PMTpZPSTgxftKvkZf1h8qP0mhjMYabjMhNMWu6XZlJBHfQC+X+Zb2vqABebZfc9NB58zNZ3mpkhi4XilqBmR1dSxIZGDKfIjSSuExjKQNx06eUganCKZY1FvSqnT1tKy1DvbNoVqDUnK4YeE3cBTqgn1jo/8ACyqUY/1Lci+2otfXQSNJWilUDC4nuQFNSDe59xP0kzh8QG8D0lJhLNERICIiAiIgIiICIiAiIgIiICImnxPGikt+ZNl897wIrjWKzNlHsr8zz/KRxFxodf1oZ9O8+kTrEKMK+GnUdPKY6hsbi00MdxkJiUosujIt310Z2yqtgOo52tpvfTW7UcX/ANPTuoD1WOWmhNrk6XPO17DTmRtvJ0jaa4fh8yB3N3sVJtbTOzAAcrBrSm8T4LVrYp7hloAglxuzMAWWmD7TZifAc+htvBS9QPSJF1VWZl2zEENboLgW98nKahFFxrsPdOc1rd2ra2OUdgMmFy0lpkUwo1Fy4NtS38X1m81YMLowI69PdNbF4hVDO7BVALMxIAAAuTc6AAX1nPOG9ualeoiUwrFn7qLcb01BDWYlh+9bvaXK3ICkjpEfxymXRqtTkNhtPlMTHSQ2Ga17C9tiedh0mdUlUvSDWbCCY1Gky05IyAT0jWNxuJ8E+mQJSjUDC4nuaGBext1+s35SY0mCIiQkiIgIiICIiAiIgIiICV7tNWGZF6A3+9t81HxlhlS7RuDWZf5FH1Nx46j5S1e0T01aNbMviCV+B/K0yhpC4WuQ+U7kgHx5A+8W+Bkk72BnRVWe1WBGIIqUa1nCZNyVGvrEcLyYHXlcEHXS+GjwEmoK9aoalbctYAA9QPs22A2HnrPfEMSS/dsoBIBtZRlG9hvsf7QJIYFFZQS7EHqct/hMWXNaZ1E8N+HBT19pjlkwdalTbuvd/A8/xlmasDqNSfgByAleoCindVNuSKbfHab+Frg3uMg/m0kYLanR5FdxtGdq8eVVaKV1oVarAK7AmwBuSLbZbAm4tyJFwZ67K0qrHPUqUq6KtqTqHLCwCg5qhJDWzXO5zi7NyieKUMRUxDN/pKdWmLU0YtS9aAW7zggMbBdBcggMwsxNpb+D4UJRRRT9VcZymvdLnOV12AJItsAABYACbvpg+24J6An0LPdNbm0hL5Uaw8eUybDyE1wc1TwWZazbDqwH4n5AwNkT1MbHWe4Q+EyVoPdQeokS0ksEe4Pf9ZWyYZ4iJRYiIgIiICIiAiIgIiIGPEVlRWdiFVVLMTsABck+6c6HEBX/AGysHDkkMuq5ul+Yt3fuiX7i1INRqKwBVkIIbVSDoQR0O3vlCxaoiBFUUwNlUBVUeAGm/TrLV32ca19o/E1e8HGliCR5H9fGSeOrZVJ8f19ZB4tjudPHkfA/nNTi2MdkAKm2UDXbYXZhzJttIyZIrC2PFNpRuKxGY73UCw5XNxr5X1+EnezTG5VhsBp9oefTyla/1Bp3I1e+nRPG/NvkLfDf4E9RWzgEi3K19fPynny9GvC3VsSy+zRNTyZRb+4ibGGUVR+0pCwOiuA1jbfmNiRfzmialYhWVAytfvMbajl57yTwN7a7/TwmjDSd7mGfNevrqO3inwVC3eylLkrTFNVC3FtGGvJfh8JTA4OnSGWmuUXva5PILzJ5AT7TmdZsYnsCfENnAPMe4z0J8rU82xFwbjz8YGhw9v2zj+BAD5sSx/CbNNs1YD+FSfedB8ryP4YbV699LsDr0Cj85t8Ia/rKnViB5DSBvA96eqlS3T3mw2vvIrinEfUYerXtmKLcDkSSAL+FyLzBhOH4wqWqYzMXotamlNFVKjC6FKg1svz0lor9yeszHek6XFhyvsDofK3WSPD3unkSPxnPOD4eli6+fEA1GOFpNSJZgyZCadUqQQQ3rFvfcS49madRPWU3c1FRlFOo3tsMgDZyPaYMG1589ZGSuuFvX14TcRE4hERAREQEREBERARE8u4AJJsALk9AIFP7Z9rKeHqCjVV1p5QzVlGamrEnuuF7y6WOa1u8NRKzxDiNOquam6VEP2kYMvxErvavjhqVGbW7sSBzsdh8LSD4VwTvmq16Ytc5SVzeDAaHyM5x5Edad58ae9rGaxte5y8hf4an42mllux7lr666mamL4qCcqCwHPy3+Mz8Kxb94Wvm+IvM97Tady046xU4hRUWbkNNNv8AE80OO6rRoJ62q+YIoPdui5jmY6AATRrVKIrHPVA9WQipnuXqVCO8V3yi48N5K+jzBLbEYk70/XUx/VUfM3vsq/3TtjwxPMuWTNMdN3h/bummCw4rKxaoKgZkt3WR7ZspsdRYkDqZ6wva1aWOrCtWPqPU02pBUzDMyUmuCq31Bc6m2vlJnsfwZG4PSSsocVkaqwPP1rFlI5ghcmo1BFxILh/CqFTi9ZalNWSnRpZUt3B+zoqO6NLAbDbXwno19NdM+6zMrrwPj2HxN/U1A5GpUhlcDa+VgDbx2k7lnOO1PDKeCxuDrYZfV537yrfKQGRWsDtmVyCNtAd50umZS9YjUx1KlqxGpj7eRPZ8RYz1lny0oqrmOr+rxDX2enp5j/EkcB3aCjmRf46yF7VsQ6Hod5KYauCAN7ACCem96hXQ03AZXQhlPMHQyNwnZSmrU81avVp0iGpUqj3pIRqpsBc5eUlabbeG0yV8VTpLnqulNBu1RgijzZiBLRMx0RaY6MNw6khulNVPesbd4ZzmaxOoBOtpI8MAGcAAd7Mbcyefy+UqeJ7f8MTfFo3+0tSr86akSd7I9oMPjKb1MO+dVqZGupVgbA7NrbXfz6GVtvXJG07EROSxERAREQEREBERASpekTjDUqHqaWtWsMv9KbMT57fHpLbOJ+kXjjDGVlBtlIQdbBdvK5J+9KZJ1DpiruyJpcOSld6rAt46n5zSxnFM2g0XoJE1sYzE3N/OMOLzK2w3MJR1zGS3Dq4UVHOlusjcMfgbfC0x8RrXy0l+01j/AE7n8vfFa7lNp1DNw7hFN3XEuCXuX1PduTdSR1At8BLlhMEtDBerQW9a7OepLn8rTQ4Ng87KnIat5Df8BLFihmq005Bh8tZ6FY4ede25YuO8C4gaaUMLVFLDrRp0/aCkBUCnULn5HQHWanCuEV6eOxFaot0elSVal077IlJWOQG66q24E6HUHc90icWmk7f9J1pHtOtIDtfw+rWrYNkps6qwzFQSFu6Xv00UmXBBYmecCe4PKe7ays23ER/ETbcRH8ZFNp7YTwJ9BlUK92vpH1d7bSuUu0tDD019a5zm6rTQF6rZdsqDXa2psPGXfjFPNTI8Jyd0AdjYZhpe2tgTpfprK2t6xt0pT34Tr8cx1f8Ad2wdPrZamJI990p/Bj4iaq8Aps2eqWr1P467Go/uLk5fIWmzgq11m0jTBfPe329HHgpXqGnWwFO1so+EvHo97O0MNSatSDB69s92JX9mWChV2UasepLGU+oZ0Tsg18LT+9/2MvgnmXPy4/GEzERNLAREQEREBERAREQE4P6WOH5eIVG5OiVP+OQ/NCffO8TivptBGLp6aHDrY+T1L/UfGc8scOuH5Odlhe02EqbATUReczYfrM+myEklTKPLUef/AOSX4HgScDiMUw9vE0qCE9EvUcjwLFB9yRHBOD18dWFDDrqdWY+xTXbM5+NhueU7J2h7NrR4UuFoC4pmnYndmNQZ3a3MlmY+ZnfFVnzX+le7NYfLTLndjp5DT63+Amxg+9iR4A/l+M2qKBUyjZQAPIC01ODa12Ph9WH5TWyLtV9mRmMGklLd2RuKkIZcCe6JsPNXA7Wm2whIpnozGs9wMOJW6nynLeK0MtVx4n5zqtUbyhdqMJapm6yl43DpjnUoHAYqxt4SWp1pXavcqnpb6yUwj3E8zJXUvWxWi0N7NOidiHvhR4Ow/H8Zzuhv9ZfPR84OHe2oFZrf2pOvj9s/l/FZ4iJseeREQEREBERAREQEq3b/ALIrxCgApCVqdzSc+zrujfymw15EA67G0xImNpiZidw/MeJ4RWo1DQq0mp1L2CMDdv6LXzjxW950Lsn6KcyrVx7EXFxQQ2P/AMjjW/8AKtrdeU61ErFIh1tmmY00uFcJoYZMmHpJSXchBa56sd2PiZqdqcXkoEc3IX3bn6W98mJSe2OKz4hKQ2W1/M6n5WnWscuEtBzZDNbs/wC058VH/Y/lMuOeyH3zxwEWS/Wp9AP8zpKPpdU2kdjhN+idJgxVO4MhDXwpm9Iqg9jYyVXaEsfOegYYT4IH15Ve06d0yzsbSrdpKndIkStXtzzH/vT0Iv8ASSXC1vaaGN387D3D9CSvB02/W883P3p6uD47b2J0Xxl99HdILhmANz65ifPKn4WlC4hpYeEvfo6P/wDM/wDvEf8AFJbx/k5eV8FqiImx55ERAREQEREBERAREQEREBOd8X/85/6j9J8iXp2iWvxL2Jk4R+7Tzb/sYiXR9Ldh9p8rREhCNq+3JSltPkQl6ExGfYgeKu0p/aDn5GIkT0tXtS8d7Q/XKTHC4iebm+cvVw/Bnx+8vvo6/wDFP+8/0WIlsHycvJ+C0RETY88iIgIiIH//2Q==</t>
         </is>
       </c>
     </row>
@@ -1774,25 +1774,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ROMARIO SHEPHERD</t>
+          <t>VISHWANATH PRATAP SINGH</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sat20_2024_07</t>
+          <t>t20blast2023_098</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>142.9</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1801,88 +1801,88 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>100</v>
+        <v>42.9</v>
       </c>
       <c r="M11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>45.8</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X11" t="n">
         <v>7</v>
       </c>
       <c r="Y11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
         <v>3</v>
       </c>
       <c r="AC11" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE11" t="n">
         <v>9</v>
       </c>
-      <c r="AD11" t="n">
-        <v>6</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>8</v>
-      </c>
       <c r="AF11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="AJ11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL11" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFRgVFhYYGBgZHBweHBwaGBgcIxwYHRwaHhwcHBocIS4lHB4rIR0aJzgmKy8xNTU1GiQ9QDszPy40NTEBDAwMEA8QHxISHzYsJSs1ND00NTY2NDQ0NTQ0NTQ0NTQxNDQ0NDQ2NDc0MTQ3MTQ0NDQ0NDc0MTQ0NDQ0NjQ2Mf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQEDBAYHAgj/xABCEAACAQIEAgcGAwUGBgMAAAABAgADEQQSITEFQQYiUWFxgZEHEzKhscFS0fAUQnKCsiMzYnOiwiQ0krPh8RU1Q//EABoBAQADAQEBAAAAAAAAAAAAAAACAwQBBQb/xAAsEQADAAIBAwIDCAMAAAAAAAAAAQIDETEEEiFBUWFxkQUTIjIzgbHwQsHR/9oADAMBAAIRAxEAPwDs0REAREQBERAEREATB4jxOjh1z1qiooubseQ3sNzNZ6d9OqfD1yKPeYhlBVOQBNrsRqNjp3TgnHuN1sXWatVYlmOgubKvIDsA+8A6tx32wUwMuFpMzXNzUAAABOyg6k6EeOvZNYr+1nHkgr7tQNxlvmN+fdyt3cpz4d09E20+8A6dw72x4hVtVoJU1PWDFTbsy2sfWTfAPa7SKWxalXuetTTq21sLFidNNe/acWJgQD6o4R0iwuKJWhWV2ChiBe4U7E3HfJefKXBOOV8I4ei7LY6gHRh2EbGfQPQLpWuPokkAVUNnABtrfKw8QNe+AbZERAEREAREQBERAEREAREQBERAEREAREQBERAEwuK8QTD0Xr1GypTUsx7hyHaTsB2mZs5t7bMeVwSURvXqgHtyoMxt55R5wDjPSDi74zEVMQ+7toOSpsqjuAtI3KZNYfhagdfU9kzqOATksg7SLJxUzWFXunpVN9RNs/YU1ORbeExnwCNsNZz7xEvuWa5UQA2/Xh3+M89k2T/4hWG50H6+swa/BnXUWNtf1eSVpkHjpEQOyTvQ/pBUweIR0LlMy50X99b6i3M2J9ZC5Lfrxnm9vXkfSSIH15RqBlVhswBHgRcS5IPobizWwOGqM2ZmpLc9rAWJ9RJyAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAUnKvbKl3wnYPenuv8A2dp1Wc09sLqFw1971NhfSySNPwSlbpHMxrJrh9EFZF4GvTJsxynsOk2TCUKZFlOvjMrembJSa8FqtTGXQAet5EVur2fObE+DFrF7W75DY+nST4nX1juJKfiY1KqsyTSBBJ5yOTE0ydCQO3KZMF1sLWII3EslldfA0/GYOx3/ACkY6Wm18RQa945+X5TX69O1tNpdLM1zo717IAw4ZSzbZqmX+HO33zTeJqHsuoZeGYfS2YO2vPNUcg+YsZt8kQEREAREQBERAEREAREQBERAEREAREQBERAKTk/tfxRFakoF8lNm/wCtiP8AZOsTkHtDbPjmX8KIvyLf7pXlepLcK3RpXE81JKfvBTf3ihsp3UEgAA821uQNhL2A/szqjIewkkeRmWuGOQKXOUfCCSbH/DfbylKVC7qvJddSSfM/aZ6qXOkaZmlW2Z2NYOjG5sNyDIXAYNXc5KRcjXloO0liAPM+F5Pe7BQoDb7zGwiVKRsr5TqLbgg6mwOms5LSJ0myPTHXvcZMpIsRpmAU5b6gaMvMbzPSvnAGW1+z8p6weDVc4KKiubsFVVzWN+WpG+m2u0ycNTAYZRbXSdbW/wAJyZevJE8RSw7prmMpMw6oLEmwAm18fawImLQxCUwquMqsNCysQToDqOYuJYq0iuoVM7R0FphcBhk94KhVACwPPW6/y/D5TYZz32QBhQxCm+VcQcvZ8FO+Xu/OdCl6e0ZKWnorEROnBERAEREAREQBERAEREAREQBERAEREApOP+0FsmOe/wC8iH/Tl/2zsE5L7XFC4mg/NqZB/lYkf1SvKtyW4XqiDRRkZ/wjn2xwzFJYh0cEnqlhlv6jWRjcSyrlGvMzGw2Ie+YW8BbT1mVQ2jY7SZOUcZTrFguZCL6lTlPgxFjL+HYupuAbG1/oZDUsSxNnUESYw2IVhZdDbbSKlo7Np8l1afaSZl51ABA+ci3radkxauLNt4mTtUjC43iMzG3aB6ynE0asipkKojXZ+baWAVeXj4SNxFXM6i+hb7/nNp6JOWxdFHVGDVVvcX0XMVGvl6S7XCM/dyzrPRDh37PhKaEWYjMw55m1se8Cw8pORE0LwZW9vZWIiDgiIgCIiAIiIAiIgCIiAIiIAiIgCIiAUnKPbYhX9mqW6vXQnxynbynV5pntU4R+0YByBd6X9ou24BBtfuM41s6npnEqfXuAbDS5kxguFoy/3tu3rKLTV+FVtcsmTQpE6i/nKal70aYpa2ZtfAgfBVJYbWI/VpbwzOjAOR4jT1mZTwiADIbXkbxuoVUKd+0c7SK8vRK9JbJPHVlUXveQmLxtxpzkQ2Mc7kmeDWv+UtUaKqy7M7DHNUXxv6foTb+iLf8AHYb/ADB9DNX4VR1zkanl2CbD0aqhcbhiTYe9T5tb7zj5QXiWfQMREtKBERAEREAREQBERAEREAREQBERAEREAREQBLdWmGUqdiCD4HeXIgHzR096NPgcU1lPunOZG5WO66bWJmuftJ7Z9V8U4ZRxKGnWprUU8mHzB3B7xODe0johTwVdVolsjpmAY3swYhhfstl9TOPR1b9DWKXFnUWDWmPicUXNyTPIwZl5MFzIkdyieqZhi5+cy8NT10l5MGZI4bC2nKtE5xsy8LTyrrzl3AYCtWqBaCFnFmJGgTXQsx0XUfKT/R7o8+JsxulIbvza26p2nv2HftN6SnRw1PKgWnTXc7X7SWO57zPP6jrVjfbHllqjfg2zCuSilrBiBcA3ANtbHnrL15zSt7QfcsEp0feLuSXK6cwosdfG3zm78E47Qxa5qLhrAXXYrfkynUTfhurhVS0/VFOXBePy14JaJSVlpSIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAeZzD2y0L/ALM/+Yp8/dkfQzplSoACSQANSSbfOcm9pXSOliVWlSsVpuCX/ExDDKvatsxLf4RaRt6Rbiiqe0vC5Of06AmQEHdLCP3y9QDOwRVLMxsFUEknwmRs1pIvqizb+jnRTPariBlTdU2Ld7/hXu3PO3PK6OdGVpWqV7NU3C7qnj+J+/Ycu2TPFeMJQTO7W/Cv7znuH6E87P1bt/d4vL9wpbekZeP4glBLmwAFlUWF+xQPtOacc449d7sdAeqo2Xv7275TifF3rMXc6m+VRsi/meZkWlO2pmnpelWP8V+X/B6mDp1C2+f4LytPdCu9OotWixSouxXc+XO/MbGYz1bCX8M5VS5HWOi903J6L7mbXazqPRb2gUq9qde1KrsDfqOe4n4T3HyJm9T5xxtDLZrcut49s23oX05egVo4hi1E6KxuWp9l+bL3bjlppLZo8XqeicNufodiiW6VQMAVIIIBBBuCDsQecuSR5wiIgCIiAIiIAiIgCIiAIiIAiJ5JtAF5DdIOkNHCLeo12IOVB8TeXId50ms9JvaCqXp4UB2294fhH8P4j8vGc2xeKeoxZ2LO27Mbk/kJGq1weh03Q1b7r8L29SX6QdKa+LbKzZafJFOn8x3Y+OnYBI5eGvXw9coLshR1A/eI95dR2nKW87TDUWm3dDCDTqr+8HUnwtYfMGY+qyVGN2vgejmiYwuZWkaHw3DvXZEpjMzmw7u0nsAFyfCdU4FwKnhlsvWcjrORqe4fhXu9bz1heGUVqtXVArsLOV2a5BJy7BiQLkb98iukXSMLelRPW2dx+72he09/Lx28vJlvqqUYvC9TDjx1T0jM430iShdEs79nJT/jt/SNfCaLjsU9V89Rix7/AKAbAd08leZ3+8tOL+A+s9HB0sYV459WeniwzC8cnlWuf1tKak90p3czv3S6FmotLTU7nuEvHFKGXObKvLt8AJjYzEZOqvxfT/zI4XPeZ1IqrL2vSJvFcTpm5uT2DKR56yPo4jNrYAb+XfMY07z2VsuUc9/CdSKauq5OkezfpZ7thhazf2bn+zYn4XJ+G/4WO3YT36dcnyxRXW97Tsfs+6c/tBXC17+9AOR+TgC9m7HAB8bdsmmeb1OH/OV8/wDp0WJSVkjCIiIAiIgCIiAIiIAiIgFJzP2j9KCWODott/fMD27Ux9W8hzM3HpbxkYPC1K+mYCyA83bRR6m/gDOE0ybXYku3WZjqSzakk9tzI09G/ocCuu6uEemsouf0Z4QEXJ3Py7p7ZefZt48zKASo9vg9Lp4zL4VxBqFQOuvJl/Ep3H0PlMRBzgjnI1KpOa4Ycpzpmyca6Sl1yUcyKR1mOjG+4Ftuy/6OuJYaSh7J6ooSdPLy3J7Bv6SGLDOJalEZmca8FHudBudB4mXsRgXpoWZQArZCbg9e1yotuRz7JJ0sHRGX42cHUZwqt32AzrbsBBIsSVvaeON8PUICgqIQS+V3Dj3bMA2TQEBWK76kMCdRNDxVK20Y5+0MV5FEshMMnM7/AJxi62Rb89h4/rWMGbjN2kn7D5TGxQzOByH/ALP2EgjZdanaMLLc/XvMv0qc9BOsfGZCLJmdIt+6nhkmTaeWWCWjEdJkcLxbUKq1k0ZGDL4jke47HuMoyzzlghUJn0XwPiqYqilZNmGo5q3NT3gySnD+gXF6tDE00VrU6rBXU7G+gYdjDTXyM7fJp7PGz4vu716HqIidKRERAEREAREQBERAOUe2fiBvh8ODoc1Rh3/An1eaOvyEnPalVzcSt+BKa/1N/ukC50AlV8nu9DPbj2SfBsCKhLOQEuBrfuBt36j1vyji6oCEQADMzWAIFjlUbknUJffmDzl/BYj3dC+R7i+/VGpaxzb7NIpqhdizbk/oDsH5TNKqsjbfhcFsd122+EeKgtpKqdJR955va/hLzSVQbmZvDqVyWPwqGGu2qkG/dYn1ExMNTLOiDdmUDxYhR8zL9ajXzmmrhE1yglblUa1zYEklrkj+LS0twqe7dNJL39TzftPPUYXMcvx8kSOB4L1zWNydzmy8wdhbQ/BtqMtpXpTi2Kb6tmXwVclgOy7u1/8ALHZPT1MStJFRw7lusTlGu+mYDQaa8gt+2Q/Fa+d1F8ygqoOwYjMztbldyx8LS7LeOo/Dp+fD9dHkfZmHJefvp7SX7bLQGXKo5D6afeYKPcs3j89T8plYlrE/wn5yNovfQban1P8A4Myo+jzV5SMmmJ7Q3Y9ii3mZbzWErhxoT6fc+v0E6VJ+TIErPIE9QSRTJHupeQTJNOdJ6MWkSpBBsQQQewjUGfQHBcd7+hSq/jRSe5rdYeRuJwF1nW/Zlic2Dyn/APN2XyNmH9RkpPO66PwqvY3OIiSPLEREAREQBERAEpKykA+cek2JL46uzb+/YeSMUHyUT3w1lL9fLlAN81vLfS9/HnPXT3CGhxDELyZveDwezfUsPKYOHN/OU2t+D3Onfdj0ifxPEVyMqEFiRZgW0FwSbZAO0eUi3e3iZbU2lX1kJlTwaseNQnoqp0N5bc3Nv1pKu1gPGeEOskTbPeY3uDYg3v38pMVcbSdvfPnFVly1FRVCuwPVqZieoTe7DKwLayIAlxNYflaZXkwRlWqRfxGOJGVRkQ6WuWJ59Zzq2uthYa7TBO6nsb6q0vkAbzDr1NCvPcHwNx84JTEY57ZWkeMZU1HgR56H7GYVEgEjst+f3lcTUzC/6/W8sUn6zd9j9pJGfLW6TMus+mm528eXzl+mQAANhoJhFtR3a/YfeXfeev3nSKfkzVaehMWm/wCvrMhXgsTMpNJlKdJhI0y6baQTTLFW+83n2UcWUVKlA/vjOvcy6Mp77EHyM0evv4yR9ndbJxSkpPVcPb+LI2k6uTP1aTxtM73EpKyZ4YiIgCIiAIiIAiIgHD/bJhSMaj8norY96Mwb0uvrIjgfAq1VRlCjqg3Y2BG2lgTuD+rTontg4P73CLXUXbDtc/5bWDehCHwBmu4LAu+HFFGyP7unrqLAe7zba7qfWY+qyvGlp62+fY9PpsmpWvkR+D6MVHd0zoMhC5tSGcqGyjY6A6mXOHdGKlVM+dF6zLlIJsUYqdR3gy/wvCs9ACm499hqrtY6hjc2uN9QLA+ImBwqqxpYxz8Rp68rF2a9uznMjy5WnquGvT+8m3urT0+Nehh4jhbLWaiWXMmpIvYmy2Av3uBJM8ARSoV2cFDc9XSqXRAunIFjcf4TLPR1A7Pm1IVRvzdhbX+WS/CXzBGOuZ0a/jVxD3/0rO5stzw+Nb+O0RyXSet8aMTH8MwzFKeHctVZ8libhQM2cnqja3bLXGeDU6VNatGoXUNke5U2bXmo010t3ie6FXDUcXSem+dDmLsWDBWYMoOgFt7m/Iy30owD4dCKblsPUbPl6ps4sR1rXK2XQ35c+fIqlUrb0/f1+BJVSpeX+5r7Pe/dr5TCqveXKhJs6+n1BllrEZl8weR7J6BfTMGuSCe/f8/P6+Msre4O9vpMqpZpMdAcGKmKaiy5lek41F9CBr/6kbtRLp+iMOXx8iDzWud9bDx2HzvKqbeXPtY7zK4rgDh69Sm26MQO++qn0K+sxFXrBRrbU+Jk5aaVLhnJfqZCNaSnBsBUxFTIiO+UXYKVBA/ifqryFz289pEht+wfMzZ+jGIpihiMPUqCia4QrUIJF1YsVbLqFb03kkTqmp2ibwGHxNNmVMFh6ZRVZnqtnAVvhLVTUy6kbL6SWo4lMQz4fE01Wqqkg02zqwC5jkYk5HC6ixsbWI5SDwmKwtKk+GfEBwXp1RUFFnTOgA92yHV0sF1Gmp2tLfEuJ02qhsOMiimELKi0wzHPmZVHw3DW7ZLZTMO6417PyiKx9HKzrfNkZluOeViLjxmNwut7vHYSoOVdB5MwU/KXag1MsYSkWr4ZRv7+kP8AUJE05lvG0z6QlZQSssPBEREAREQBERAEREAxcfhVq03pN8LqynwYEH6zkOLo1K1JTT+J6LBgGsM6VaNxfu687MTPnetxStSd0SoyhalSwFubG+tr8gbTJ1ON3pzra9+Dd0ct716aJ7gfDCPc1U6r03dK/XOoDHTsOgGnfeYeDf8A4PFOP3mpj1e9v9UgqeNqLnKu495fPYnrXOt+3c+s9ftDBSgYhGIJW+hI2JG1xKFhptunvbX0TPTUN72/YnujJvcDQs6D/pZW/XjJXhKqoamHB93UooG0FyqMGNr/AIi00tcLUf4Ed17kYj1AtL78Hr2H9g+n+AzmXDFN7rW/9EaiXTbo2jh/RgJ7ygzo7vTzU2KWylGs2hJ/EuonnjmGOGwSUKhVqj1C1lJIVQDe17abct2M1n9kr0mVxTqIV5qjgjwIGm8ri6rOczszN2uSTbxOs7GNtput+v0JTDdb7trkjkfKxXkdRMaspU3XzmTiBzG4nhhcXmssr2MRiDqJtfszwLPjMynL7tGJOnOyqp8Sb/yzU2W2o9J1T2R4W1CtV5u4W+nwqoP1c+kzdZfbhfx8fUyZ32yyA9qlILiadQizNT6wtuVZgGvzuCB/KJpNO6i/Nvqdp072wUQUwzc8zr/LZWPzUes5je5v5L48zO9FXdhkqxPclzDoC6qTZQRc+J1P1m4J0cRXC1mqIvvMSmbKBdKKF1dQR1g1tbeRmr4elYfUzIqVC1gzs2UWGZi1h+EX2HdNZc4p8PRPcQ4dRoK7ArVKLhmFnOV/eBzUtlIOU2W3MAyWw2GwzVsQirTCItP3fXYhmYBnN2qrc9a2jaZdib30oAchMqm1hpf0jZ1Ym1yyb4ngUXD0qq9VitK/XDZyysX6m6lWCjs63aJ56EU1PEcOGFxmYj+MI5UnzH0kYWBGt7+FpM+z+kG4jRv+7nYeIRx9/lOrk7lTnHW36M7hKxEmeEIiIAiIgCIiAIiIB5M4nwP/AJnE/wCbU/rMRMvV/pm3o+K/Y2yh8PmJSpvETxpNJ7pfD6y42xiJRXLIsq8rX+HyiJZi5JI0XjvwN5zU6fwmInsYfymrFwY9Wde9ln/KN/G39KREo+0P0v3Rn6j8hH+2D+7w38b/ANInLqHLwlIlnQ/or++pDp/ymcsupETYairbGeV2iIROSSp/DJvoB/8AYUP5/wDtvETq5K8/6b+TO2xESw8EREQBERAP/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIQEBUSEhIWFRUVFxUVFRgVGBcXFhcVFxUXGBUVFxcYHSggGBolGxYWITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGy0lICUvLS0tLy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPsAyQMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAAAQMEBQYCB//EAE4QAAIBAgQDBgIHAgoIAwkAAAECEQADBBIhMQVBUQYTImFxgTKRBxQjQlKhsdHwFzNTYnKCksHT8RUWJJPC0uHioqSzJTVDVFVjc4OU/8QAGwEAAgMBAQEAAAAAAAAAAAAAAAECAwQFBgf/xAA9EQACAQIEAgcIAAUDAwUAAAAAAQIDEQQSITFBUQUTYXGBkdEUIjKhscHh8BUjQlLxM2KSBhY0JFNyorL/2gAMAwEAAhEDEQA/AMBXHPpdgNA2rBQISgQjsBuQPXSpqEpbJlc6sIfFJLxH0wtxgzBGKoMzsFYqiwTmcgQogE61JUpt2M8+kMNBXcl4ajY/flVco5XY10pqcFJX156BSLAoEFAwApAkFMAoDQKAEoELSGFMCRw/CNfupaXd2A9Op9hJ9qjKWVXKq1RU6bnLgev4XDLZRLaaIgUeRgbz+frXIlJyd2eNnNzk5S3Y8igSTAABG2x2JnrObT0oSIlbfQZDr8QIE82PKeunpt0ihWvcmYjiOGbvjll4yhPDnkZgpVQIk+KY/OulSfuo7GHkuqSem99bcLr6FOnCcQzQLF0mdfA2/nppWnK9rHT9qoRV3NeaHcRwLEIJFsuv4rf2ig81JWYI2g9KHFoIYujJ2bs+T0ffrwId/DPbjOjLO2YETG8TSsy6FWE37rT7hmaRZcl8M4e+IuC2kSZkmcqgbsxA0Hn50FNWqqUc8jZYLsjYtr/tBzOCQQHgM+UvkBAhQFBJOu2sfDUrHKqY+rOX8vbu2V7X8+7x3IXFuyecZ8O1lYkNbV2fMREqpaWDgmD4ekCtGHnTjpJGPF4jEtWhJ7cVb6aa8L37yyfgeCsLd7wW0PcqirefMVviy1y44Ln4pe0I0Ay6DWnnk2svPhy8DBKrUe8n5nHCeKWcObKC9hnyWmLHCoXZsSwyokYe2TkUMwBMsxJJ2FOcJTu7Px5eJnU4rijrjvHAMPiow2JZL6Oge6vdhZt2bFkFXKuyFrhadxnB1nwunSaaba01+7FmU/cjq3ou9955+KxyabbR72mmoRT4JBSJhSAWgYlAgoCwNoJOnrpUlGT2RXOvSgvfkl3tAuu2vpTcJLdEIYqhP4Zp+KColyYTQO4UCN39G/CD4sSV6pbn/wAZH6fOsWKqf0I4XS+I2pLvf2NcGEZp6jXUbwfT/KsOxxew4vXhGWJ1mCeemWCdzoPSTU1oNIg4i9lTTcAnmdBMRAn7o8/eDRFLYmldmSdQuIw5yqGOJtTl5faDc+YjTyFdOhq0b1VtTmr/ANL37uBrcF2aDLbZrzst5QzB/EiZrlkZYJ3i6SP6Fburb3e4VMdlbUYJOOzWjektduzXvFXs9aKZrT6MqsXsoytBW02gBJn7Q6bgA6HWkoLdPyB46pmtUWzekmmuK125b8+Ji+22FNlktlmbKbglzLEHKdT7/wCVQqJpJd50cBUVSU5pJXUdFtxM1VR0y07McQ+r4lXLsiwyuVmcpBgHLrGYLsQfMUzLi6XW0mkrs9NsOqqmZBl0aXjMjM1lUGgAkvckwFjKSZJJL7jgSTldp69m3FvyS038FZGX7VOtjD4lbeZBfFrLbXKuS4QWQkwMvw5vCRovMMKuoNRqJy2RLERq4milFZpK9nft31f75lBc47a7nurWBsWycpLkl2YrEs3hXVvFOv3vIVe8VFPS7+X75FNPoCtJXnJLzfoOX+2eOdMhuqomZS2gMh84+IMBBiI/CPOaniVwj8/8GyH/AE/T/qm/Cy9SvxnGsTfBW9ee4DEhj4dCCPCIG6qduQqPtMuSNlLofD05KUb3XaQprO3c6sVbQKRIKAFAoHY5dsomrqNHO9djmdI9IrCxstZPZfdke6Sdc4C6gjYjTcgkHc/Kt8Ixjsjx+Ixles7ym/OyKJjDRmBk/Hr8gIkGa0KbsYrK51g7kk65Qok6AkyVBUQPM71JSk9AsOYbGuJInTUgxET1qidJVVsbcLj6uHeaMtOXAucLiVuCR7g7g9K5dSlKDsz22ExtPFQzQ8VyJ3D8I1+6lpd3Meg5n0Ak+1VSkoq7Lq1ZUoOb4HsuCtLh7SoghUXKBz0+95ndveuVJuTuzxtScqk3KW7I9y9sI8jGuka6jkRUbCSIN8mfI6xM6SfLofy84qWiJoi44yg3J6DbWNQBtoOo1jWpQWpZHcxfEMbkxlhnMC3eQtrK5UdcxPpB+VdXDxUVoaer/lytyNJhMK32zuvetbdrSo5zFQusoGkCAdCRAqbWrudKpWj/AC4ReVSipNrS9+dte/id4uzhrmHS6Lgt31zTCw2cRKsQQeYymOR1NR0tcjSniKVVwcc0H23VuDX3RmO0F5mSyXYs5FxiWJLEF4UknU/CflUpP3Vc2UYxVeplSS91abbXf1KaKga7ADFAi/4X2ouWgxeXIXLbXQKWLAs1yNXOh1MnxHUTNBgrYKM2sumur4+HIquJ8QuYi4XdiZLECSQuYyQJ/M7nc60GqlRjTjaKIlBdYWgAoAKQwoAWgYUbsJNRi29iNnBcsSsCRqR4RyOp68/M11YQUIpI+e4vESxFaVR+HdwIfEcWB8KBw67tMyDod/Lapoz2b0RXPhmcLktudJbSfF5AbDam5x2uNYervlBuEXwuY2mjrHKo9YgVCb4ERHImCdd9Yn1qaZS0WPCrzG6pJJzZpkyesn5CqMTZ0zrdCTlHFpLZ3v5HrfYDg5VDiWGrApbB6SMx9/0Brz+Knf3UdjpbFKUlRjw1Zr7jSPkNjHQjTXn+/LJY4yIRfc7z4Rz0HI/5cqZMjyJjbKdDzPU/OmyaIWOdspKDYQBMDQgDXruInnrziyCV9S2CV9Tzbjmt1tZgkTprqSdRvqTrXWpPQ60YXppl92c7UZYFx8l0AKLjAtbuqICrdjVWEAZxMga7TVrSevEyWyrJJXh2bx7ua7OexPxePsAXGuNbcu/eKll87k81Lr4UQ9TLAEwOleVL4jbTqTeWNC+is21Zd9nq2vLmzM43Ftecu0awABoqqNFVRyAGlQbvqdCjSVOOVflvi33jFIuAUCSCgBKACgBaAsFIYtAwoABQA1iwe7aN8pI+VWUdai7zH0ldYSo1yZp+wXZPD4yw1y6JacsAwV0k+/KtdSo1I8hQopwubW32KwWHt6Wwfw5iW15DU+tUSk5bmilFJ2RExuCtIQEUAHyA61Gxoy6FDjSneQp0/f51rpbGarozDdsuDC0Rdt/C8hgPxdauT4HOrx/qI/YnAfWMZbtTAYMCegEsY84Ee9Z8dLLRzF/RmIVCs52vo7d574tlVUBRCpIWDoAFiPQDQT5V5l63uWuTbu92RXeWOunwjeZ1n1Gg/OkSSOb77wIiPXQQJ6jb119aY0iFi30ktESPzAPXWP30qdr7FsUUnHy4DHOFCqYEnUtC5dDHvyA8xGmilyNuFUW1G1232fvqYe8CxJOpO9bU7HdlTVrDHc1PMZ+o1HkWKg2aoQUUd0iYuU0CzHNA7BQAtABSJAKBIWgYRQOwUgFFA0KqkmBuanTXvKxnxMkqMr8mb3sDbXDYC0xV2uXu8uZEUkwGKj0iP1rVVUZSvzPHYabjSSttoWmJ7XYJgLTuVuDUKwZWUxHMbxImoZdC2NSOYqsNx3DZHLPmynwSQNxuTUY7lznHmZniPG7AcsWEnYL4jHLatkI2MFWtFsj8VCYzBXGRiDaU3MrAq3h1mDuInUVNLW5mqVE4tD30O8Mm9dxLbIuRNNy3xMBzgCP61c7pSpaChzf0I4eDvc9OxjxsJkKPlqAOlcA3xRFSGGaddtZ5xJ9N6mSsN3G06xB01JjaPQx8qaJpEe/dUJmJjmSYy9dZqxK70Jxi27GQ7QcQzLlX7xzNoOkIs+Qk9JattOFjtYKhaWZ8NvuZ81cdRiRQKwtAxRQJjs+lIpGYpl1goHYKACkAUDCgDqkSCgAoDQsezkfW7ZK5sk3Av4mtqXVR5kqBVlLc5/SLfVNI9Kw3CRfwVoOpnu1ZgpZNW8brI1AzE6Va1dpnnoSy6czL3ewa3MULjZbdstohZnJ5lVzacvPrUnUm1ZEupjF5tzvtx2Uw9uwi2rKo2plRqeep59KnSz2uymq078jHcP7LtoyKxO8q4X2gj++rZTezM8cKviTLvA8KZRcR2Jz2rqeIyYdSNTAmrILiU1FplH/o2uEOREZbao4kEZrZEMPUXDPpXO6TV6d3zLFa6S5GnuF7l4QBGkSdg3xNB+E5dAOebluOOrJfvgao2UdSVdcCBrAjcc5Gh89tup94iSIuJzbDTbUiYMHU9Y09YqcbXuyyKXErOMXoU5WIAEmBI3GgM89tOvrV1OKvqaaEbvUxGKxDXHLMZJ+XsOQrWlbRHoqNOMI2QyaZawpiFpDFWmQe4UBqc0DCKQ7CxQOwUAFAwpBcWgBaRKwkUxWHcDjO4v27o+4wPtz/ACqcHqY8XDPBo9KwvaQ2bBI1AU67/CCf7qcpSjPKedjGE4XktUU3ZDtE19r2KupcuH4LaKpZVX8MDmSNfQVfKNnqU9fmjZIhdre2TObZGHuEAFXXI6gEnUBmUch0q6mtSmtNRjszM4Hta1i7AkI8yjL8EnSJqThLe5CGIhsy4xHaDMJ0LANtE7ECfelTbe5Gtl3RZdjML3duDoWCg7gwI/Mkmee1czpCqpNRXAVFNu5qMPbdMzErrlyCNlAJAPWSNhyrm6O1jW8tkl4jd54OomYga7A7+h0nlUlqSSIl29lUmZgDWdeXPmOvPf3aV2WxjdmP47jsxKyTmhjuIEeEdDoZNbYRSR2sHRt71v3iU9WHQQtBISmI6FIYtBFnNMMoUhhQMKB7i0h6hFAWA0AKKQ0JTEKRSGxi/U4mavsaDs/xVQqo50212jQNP6+9Wzg2lJHm67VOq09nqazsdhsDYzvbALgtmOXN4SZEqdCPzp9ZaykUunmTy8e0icc7ScNcMStk3AYA+0gnWfDngcuVaIWevAqlQs7OR51xlsOLguzmckEKNFAH83kKtadvdMlSME7tkXgbG5cjXcufRdf1IqNVZIZvApUs2h6v2bsDICYHMeZgadCP2eVefru7NlNWLW48kyf2xBMnr0qhal6ViFc+IknQGNAI209DA3HU71IuSKji+OtlGGfflmgkmAI11EfpWinCSdzXh6U8ydvkYy6xZiSSfM7npWs78I2ilscRQSsEUDsFMR0tIL8AoGFAxKA0FoADSGwFA0dUhiGmJgKQI6RJNDdhS0FuN02FJD4Ee5U0UVLMmcAwIv3GtFssqWVvwuCMrenX/KtFOdmcPpOgpU78bknCcSu8Nc27oyuxEyZDgSQ6vGg20HP3jQ4xmro4CnKj8TIHEu0qYkMSihwTDECDIOm3p86lCk7aocsTB6mQxV83X2BOwyirYrKrGKc3N3N92T4L3NtS5Ae6yrrvJ+FB+zrWLEydS0Ym2jhpWzW7X2G+tW+7lSIK6Eeg/Mc/SuLVi02mX0zq9cLSBrrr+/Od4OnpFQSdi9IjY3EBFYkncR6k6R1MipQV3oX04OTsjEcaxouP4fhAiIjadT1n9K2wjlR3MJR6uN2tSsqw13FFBJAaAYlMiLQIKRJC0EgigdhYpD0FoHwEoEFABFIdhVEmBQK9h7E+DwDf7x8+lRjrqRvd3I2ap2FmN59FXZ1MR9YxF1MyojJbB2LkeNhPNVIj+l5Vsw9NO8meb6YxkouNODtrd/YXgfBVsW7ru4a5mZF0gqitvrqCxG3KKrew8ZiXUahlst+9+i+ZLxXD7WLtZLqBwNQDyPUHl7UlNx2MMoJ7oy+M+jrC7q9xfIEH21FWrEzRQ8HTY7gOz1jDaqni6tqfzqEqspblkKMIbIsOGt3uKs2VAL98t2TJyqqOCYHPxSPNfYzpaak3pGUnslr47I13bPIxOIskFTlQkag6QpHX4YPoKqxtG/8AMXj6mLD3j7sjPjEwDOnWeu8D9/2Vy8mpuiUHHOKOpyqSD94jqRtBMz5+XOavp01a7OvgqEZ6yM7vPXerjsN2G6YjqkSQhpiYCmRYGgBKB3OpoJXOoqJJIIoJWOlpEkhKZE6iollgoEyxwuG7u2bp3+FPXmfYfrQ1d5fMwTqXeVFYVa44VQWYnQASSfICrFHgiU6qjG7djWcI+j66QLmMcYdN8p1usPJBqPetMaD/AKji1+lo/DRWZ8+BtxxLA4C0qFrlq3ZaF0cknKCZKDKxOfWZ19JrT7qVjiypV60nJ2bl2r793AzmP4zg7t8Jg2uOGksWDACY8HiEnXn7cqy1LcDqQoVpUM1VWcfmvoW1m1A1EVSZwbCE89KLAVfFsMVQuBMA00tSSi5aLcd+jXD2O7v37lxDduEW1IYHKpgsTBlZ2k6eCtdKKvqV9Iyy5KNLVLVvm/x9zQ2XW2zW1S2yEAMhEqVnQRuDu39arnyMbTkszbvzKXGcOwd293Nq+9i6SCq3AShJEgd4B+tZJYeEpW2ZpjGuqfWuKceaf2Mjx3sXxG0xZrTXV/FblhH7PnUXQa2OpheksPaydu8zjBrbQ6lSNwwIPyNUuPBnWjVjNXTuF1YMe49DUVsWRlcKRcIaZBsKZEQmgk2FAgoAdmomi7CKAsdKKTJxQZaVwyATFCCTsTeD4Nr1wACdQB6mpxSWrMOKr5Im1xnCbNkTiFL5QRatSVUwJL3Svi1OuURpueVX0aVlmnuzhrEVKrtSdub9PUh4XtDctCLC27MmCLVtE9NQMx0ncnarlJrYtngKUn/MvLvbY1/pK8TnLkkkToJ3ozMl7NRtlUSNjAb6hbjM3Myfn+c0NssjCEdkh7D4dFEBYHluD+IGoNX0JOrNO6LrCcRMZLhnow5/0h/fVLVjPVw8Z+/S07PQmPfCiSdP19KVjJCnKcsqKPH3GvQGJFsGQo0zHkWNWxidCDhRVoay5+hU4zh1t2kDI3JkOVuXMb1O48ql8eo5hsOyMWZy5JGp3gAAD2AHyFBZJxcMqVkctdc3FvEksCpBPJk5H5U7u9wUIZHTSsnf5juH4viLLk2b1xfEY8bQYJ+IbHbn1ou+ZB4ajOKVSC25EzFcRHEAtvGEux0FyArJAmRGnqOfygclLRmVYN4e86Oi5c/3gZXj3CnwzBWIaNAw2dTqrD8wRyINZ6lKVObjJdpsweLhiIZoP/JXA1WdNMKZBiUAJTAKAOopErMeqBpOlpMsidRSJWCKAsN3KaKqmx6h2E4MLGHOJcageD+kRv7CrYPjy+p5HpHEOrV6qPiU3FcWbt05jrOnrEj5gT7HpV9+Jto01ThZFbiLYU+sEf2kH/EamXQeZfvad5Nf350gtoXGC4DiLkEWioJABuRbBJ6FyM3tNSUJS2RkrY3D095Lw1+hbp2Vy21uXb6BWXOvdg3MyyoEMcqiS66zGs7TV0cNJuz0ME+loXtCDffp6kftLwYYVrYBbxpmIcLIYEgjwkjpsT71VVgouxfgcVKvGUmrWfApVbWNf86rsa3diO1MlFI0nD+Ch7FphZDk/G3eFG8d1ltwNj8McuVWRjdbHKrYyUas1ntbZWTWiu+47xHAJENZyDTKyMWckgmCCWDyBsI2PnRk7CqHSE4u+a74ppW+zXzKDinDe5QOcxzMVIZCjgqFOYrJnRhsdag1Y6mHxLqzcUlor6O61v6FHiUAJ5g9OYgEj329xUXsboa2RFeTAPKWJ/rbf1nn2UUQlaafJoulHNCUVxVl4r7L53NG3DHxPB3uupDWmDofDDIDFwDXMCBmOo5CPPsdN04dZePD7ng/+nK8qU8ktnp6fPQwDCNK880fQlL3RKBigUEkgikOwUDFmgLjxFRNNjpaTJx3O6iWHJNMi2iVwXCG/iLdsDdhPpT2RgxtZQpOR77i+B5sMtlWyQvJZ1+Yrc6FoxXI8BDF5arqNXPIMZbJljoRo0a6Tv5kESPSOZqKPWQlpp+/5JPD8OL9y2jCZZQwB6OuYT/VNTpq7SKK9R0qc5x5XXkejYDA2VKFbS2ybVlzklWdrkhouasiLAMA7kTynfkjBuyPK1cRWqK05Nk5cJkxVlyAT3d9HYeIme5K5iZY/AQJJMc6lm91opTWVru+4xw2xeS3atm2h7lWtKS3humMoB8PhGVTMgwREGiTu7kpyi22uJl+2WF7pbIgD+PGUTlQZ5FtZ+6oaBt5ACBWXEu7TOz0PK6n4fczBOk+9Zzsdg6y/pQQianDm4Vs5LhCdwrAKxXPcRmBWV1BDEz03qxtpKxxargpTvHXO9XwWltO0U4o90ct/urqkhkuyw2OVCHkeJSfF6g0sztuRjTSn70c0Xs1p46cnwZTdpcQ12xYZwFZluMQNPAQltWiSdkn50Sd0joYGnGFWoo7Ky+rf1M7cXNAOkIrE7kaknTrKiKrZ04tR1I9qz98jSfCvVgMqr/RUDfmcxqKLFPgvF/vF/ItezGHIu3LYOl5LitHV0IPtt8q6zxsa2GdKp8SWj5/k8xjOinh8UsVR+BvVcu3tV/LuMbxG1luRXEkesoPNEjxUDUkhaBhQMQ0CYUCJTCqzdJaiUwsLSA6t2mYwqlj0AJPyFF0tyFScYK8nZdp6H9GXZe4uI768AsbLufU8hU6LU6iijyXTHSdOpDq6Wvaa/tdxK3bIJvrnVpFsguDqNDl/i20kNpBJBkE10M6zO5wKGBr17ZI6cX2HmijKY5HX0bn7Hf19aqPXSaeq/V+B/gWKWzjLLsYTOoedlghWJ6eEz7edTg7SRRioOph5wW9tO3ib9e0GDwyqik3SogqhNxTGifaOdcoHKa1TrRvc85S6NxFTVq3f6blbd7ZNCi3aUZCSpcl2EggnSBME1U674I2w6Jgvjk33aepAv8AajFNP2uWTPgVV19hNQdWXM1Q6Pw6/pv33KniGPuXYNx2cjbMxMAnWJ25VW5N7mylRhT0grEVfhIoJvSQ7aeVH786CEo2ehY4PiBtjIwz2yZyzDK0fEjfdP5HnUlLgzLWw6qPMtJc+fY0S7/ErBzOyveZiCe9CKsgAAkrJOgEgQDReJRDC1tFdRSvtdvXv/yig4tj2uFrjmSRHQADZVHICot3d2dLD0Y00oQKrCXCxJOwgH2JYAdfiG34aRpnHgi0wGBe/cCLAZgYzEBVUAkyfQax0ojFydkUVa0KNNzlsuRs+zHZy2jSL2e8hKvl/i0ZfiTUSSBz03GlXTw0orXicHEdMdfeMF7vzPNO3GC7nEFfWuendHouj6meFzPig6iCgAFAxDQJhQBYLYZvhVj6An9KqukbKtWnD45Jd7SLPCdmcTcE5Mo3liB+X7Yqt1oLic2t0xhaezzPsL7h3YtAZuuW/mrpymD8xsaoliW/hOVX6dqyVqcUvm/Q1GG4fasLFq2EBAkgQfdt6pcpS3Zx6tepWd6kmy24FKo7KCTBCgdSeXzrfg01LTcyVEm0nsVr9j8zZ8TiUtltSmhMEgfESBuwGgOpFdaNDKtWbv4tZZaML24/j8md7UcJXC3jZBLKApBMTqJ5edQqRyysjoYLEyr0+sejuZjHAqRJ5gT11BB9Yn50kzoRSbuSsLfzag6D9x+WvvTZCUTRYTs5i7gBFooDsbhFuZ20bX8qkqcnwOfVx+Gp7yu+zX8E/s3wIXSzXpIW4bKoDGe4qlmBYahQAdtT7ayhTvuZ8bjXTSVLir35J7EPthwpbFwNajurk5B4pVkyh1YNruZ96VWGVl/RuKdaGWXxL532KZTAqs2tXY1aaAKCTVx43qCHVsbuXRE0DUXexU47ESGHT9tJvQ1UoapnXD9Jb+cfbl8zEfsoIVL3t+/4J9rCPiLluzbUs1w/iCwg1JzEELoCZg7bGhRcnZEHVhQhKpN6Lsvr3cfM9J7JYpe+xSoC1oXS9u4JKFrpTvgGgA+PXzkxXaxVNxhBy+K1muOm3yPntCpmclHa5gvpgsBMSp6zXnpxy1JI9t0LK9IwIqB30LQAUDEoEFMR7hbwCrG/QkQPXf1rjHiL3HO7STmMkeZOka6e0/OiwK4G6BMASNdeXL51IkokXF4qBOuu37+vrtQTUCdwa9cKMLWtyDERsIEmdviFdbAJ59ORlqqKfvbE65wu1aDd9fS3Jc6t4jm7rUljJP2S9a6riluyuNWpUsoRb24cr8u8yPbjF272KLW2DAouo6idP0+dZ6zTlodvo2nOnRtNW19DE8Wb7JpGq6+41H6VA6sFu1yIeBx5tPbMSLRS4y/icEEKfQCKktH3DydbTafFfVHtPZ7EJ9axKHxNnW8jlSxW1ethxLx4RIYAE+ldaprTjJbW+h4BqzyvdEDD3VOBc2LaqHbDsBmN6HvXQjB+9kZ4yk/0hVUYRg9uZ1dZ111r2UuzSKurWsW7Ya3inv2b1pB3GdA+U+G2yq1oprAMFpjmg2kVVKKe5Qqk6CjOnJ+9Z78U2nf94jGD4BZayCMIpRoy+I98VP3y0wDzgVRVjKMl1aUo8ddfDg/PUsqYysqmtR3+V+VhP9W8MoOFyDXTvio7wOxLIM39ERHP3ozUs3Vvf1u7X56DePxDn11/Dhy2HE4fh/Hb+r4ci1n8JUG4pUeBmnVw3OtXVQstCipia8ffzyu+N/3YreKcMwXds/c21Jw9y9cNskFCiKVAAMDUnQjlSnQioydgw3SeKnXp04yunz14r1PIeMvkUkmMwAnp4lE/Ij5VzmtT2055Kbf7q7E/hyFlUHRYLEdJ1+e3uTT7ytyVrr94k23duK/eKxQj4SpgjlofSle2xFxhKOSSuu3Y2vZDtJiLlxbN1w6EiJADCNRBWJ2G81NV5Jq+pxsf0fh4089NWa8ig+mlv9pT0qit/qy8DV0H/ps86FVnoULSJBQAUyIlAHtRvj9dOZE6DlpXF7jxiiNtd289Plrt71JImokc4kFYYz0jY/vpTXaWKD4DF+8xB1gRy6f5TUkiWUj3eKXbNsC05TOsEro0SdAfu7DbWupg21ma7ESw+GhUn76vYqQxJJJJJ1JOpPqedaXqdPRKy0ENAkUvaB4tsegpotzZacnyRE4JYJtg6NcuHSdAJOkk6Dfep24BRm8meb7T2bgONW3Iu3cKW8CNcF9QbgtoqqzCNdcxidM1b3OGVLNw+fmeLqYetOpKcabSbbWj28iVwm1bIE3bR7q1hlYW3ziLNzvDcYjYSDA/bQ6kXt2/MtrZ1/S9W91bfSw6MfZS699sRaNt0YXAHBMqfs8qjU+AkGOdQlOLVr6CVGrKCgoO6emnn8xcLxApbRFxGH7sZVW6zjNk5Ap+KNKzRzxSirW59nd+QnSzSbcZX4q335eAziOIWe8ZTfti62e4hzjulyEC2rnbMRPyNUvCU51M85O909Hppa2m2xONCpkzKLyqyemuu9v3kNcQxNu44Z8VhgoNyGDrnYNbZRaaOQLb+VdNVaaW5QsPWb0pvTsfmUXHcXh7WBK279hnXCvh7i22UtcuOLIDLAlx4W18z5xGtWjKE0nx0+fqasDga/tlOo4NK93pbjf7Hl3GU73DjzZB7Fgp/WfaufBptM9VjabdJqPG3k2aCzAXcAty8uQqLFP4hWmOvpt+2gii17J3AMUkcz/dUJmfGK9Fld9LOJz40j8OlQk7zk+0Oh45aKMUKidxC0iQUCCgApiPW3fWM2nQexke8bVyEjyaiRXcesGPPUa6U0XKI010KACesec/v+tOzZYoES/i4EDlOp267dKnFE+rI+JuyqyZ/wAln8/1rpYfSHiToRs2cg1fcs4nJakSKLtKZsvU47odT/Rl3DPDbwWwkiSwgKNyOnv+lOTLaWsItci1wzGNd/yHkPKkEnyJtrEsoIViMwytBIzLzBjcaDSnexTKMZNOSvYRrlIkNNiKBrY6e5+dAkyJcuflQTTI5Mik3oXwepW2XLEW+lwN/VBzf3VFbik/daL7D4kMYgz6cv7qlYonFrU7e6SYUe52/wCvt86BJaak3gD5MTb1klln3NRlsVYnWkzP9tsX3uOut/OIqEtGXYCGWkkUoqs6SFoGFMAoAKAPU7rkD22Ou/Ka5djzUYkRnOvOPz8tPSmkXqBFd6di+MCNeJ/fappE8g0Tt7/r/wBK30fgRGKtcauXwvPb8vXl+lXDy3Qw/EEbQMpnowPtEz8qBxgV3FtbdwHmsj2qSepKcc1NojcHaBnfTks/hHSnbUVJ543LNcem2YUEsjHO/wCYpEbHLYn5UwsIb4IB9j68qAtwOTiaAy3G87GdDrSuWKMVuzoWnPQep/ZSJOrFbDeF4bkYuWkkREec9aLlGb3rjzFhpngdIWCB7SOvv5TQNbnJuZdwYJj4mgHownT129N6NBpyen2RY8FufboeksfLKDp+RoexVXX8tmWxd7vLrv8AiYn5mqpO7NtGGWKRyKgakFMBKBC0DEoEep3Lg5fv5TXORw4wIWIxKjdgPWKlY0wpldcx6RoQfSpKJpjSZXYniJ2A+f5VNQLOqOEvllBJ/Ft61rp6RRU4JNnBshj4tegOw9uvnVhFzstBbhSIgEemk+Q50XIe8xh7I05eXKOkcqdyV7po0lriKXBAj0O49qlc488PKnuD31B2FFyKpsd+uiKdyDpspMbh3tBS8eLoZ6b/ADFRZ06VSNR2iQ+86fKkX2EDR/d1H/SgTOxdoI2Ou+oFlEN6geURjP7/ADoHsRlJXTeNNeY5fqPz6Cgs04DlrF5O8bpbIHqYQfqflSbFKF0l2lMoqs2xR3SLAoEJQAtACUAT2vMd2J9STVVjdGEVskKt5hzpWRF0YPgdC/RYXUrZM5NynYg6THcNd09DVkdjLVp6jjvPp+tWXKMljgHWT7ftouJrgBuUXFlOS1FwsKMSw5k+tO5VKhF9g63FoHwnzjancolhmiacSMRhxB8S6fIbe4im3dFVNdXPsKJHkxMEfvNROhY7zGncjYMxouFhO8ouFjoXaAyjgvUXFlEZ5oGoka9c8B/nMPkoP95FQbLIxuyMKiaUdUEhKBBQAUAFAEqarNyYs0DuE0BcQmgTNJg+zQfAHFpdJZQ5a3l08B8Xin8Ou1R6y0rM41bHuOLVCUdNNb8/yPcN7MNew3fd4QSrMq5QZgsFEzzy7xzpSxGWeUzV+kFTrdXbTS7v5+RG4XwLvsK+JdyirnjwzmCrJ5jnI9qKlfLNQSuW18V1dZUoq7dvmTeFdkhftW7nfFTcUEDIIkk6Tm8poddqTikZcR0i6VRwy3s+f4J47AIY/wBqP9gf81L2h8ij+Ky/s+ZV8L7KLfxN+x35AslQGCA5s07jNpt51OVayTtuaKuOdOlCpl+K/Ey99MrMu+VmX5Ej2q5M6EdUnzJ3Zyx3mJSzmyi4cpIExAJBA5nT86U55YtlGKtGm522NjiPo4tu2b60QfK2Nf8Ax1n9qfI5Uek5RWkfmV3HOwww+Gu3hiWfu1zZcgE6wNc1ShiHKSVi2n0jKc1HLuccJ7DJfs27pxLKbiK0ZAYJWcsl/wAzFRliss8tiU+kJRk0obdpYp9G6HbFH/dj8/FT9pfIq/ij/s+ZUcD7JDE4jE2e+Zfq7BQcgJaWcSRm0+HzqcqzUU7bmitjurpwnl+LtKi9wG6uO+p/fzABo0KHXvPTLqfQipqqsmc0RxUHR639vyLjj/ZQYW5h7YvF/rFzJJQDKJQT8Wvx/lUIVnJPQpw+MdWM5ZbZVfctW+jZNjijOv8A8MD9W2qn2h8v3yKF0tLhD5kfF/R6lu09w4kyis0ZF1ygncP5fnRHENtJosh0rKUlHJu+b9DBVqO4JQIKACgAoAkTUDWmLNA7hNAXCaAubP6PcVmW9hzEEZwD0IyP/wAFZMQmmpI8/wBNU7OFVd33X3NTZu28O9nDcyhif/tBYE+fiP8AVNZ5XacjkOEqynWfPXxuVPbMpheH9wgjvHyjyUsbjfs06mr6Lz1LvdGzo5Sr4nrJcF9rImcBtBuH2iUzgICV8PKTPi00Aqud3V0dijFPLiJ621/dh3DYSBD4BSdxC2NRPOTry5eVW5tbX+pQ5S363/8ARX9khlx2NGQIJt+HwiPi0GXSpVHeKNWN/wDHpa33M5iuxWMe45VEgszDxrsSSP1q5VopG+HSNBRSbe3Ic4JwLEYPH4VryqMzkLDA7KenrUZ1k4O3AjXxNOvh5qHL7lv207MYjE4o3bSKVyIviZQZEzofWlRqxjGzMuCxdKlSyybvdldiOzmLscPud5iciKGJsASp8X4gee+1NVoSmtCccRRqV1aF78SyxHB3xPCrCWlBaLLQTlEBNTr1kbVVGajVbfaUQqwpYqTltqddiOy+JwmJNy6iqptsoKsrEkshG39E1ZWqKSsh47F0q1PLB639ST2PP/tDiG4+0Hp8dzelV+GJDGL/ANPR7vQvPrGHa3/pALOWy4JA8QRTmZPUMCPn1NVyT+AyqFRS6h8WvMoO3RP1jh8x/H/8drenRekjbgF/Lq93qaXiVoMwnCi8QPiItGBO32jD8utUxb528zFTbX9VvP7FVxbDoMPeP1BV+zueIDD6HIddGnSPXSrYt3XvfUuoybqR/mcV/d6Hj9bj1YlAgoAKACgB6aiabizSHcJoC4TQFyTw/iN3DvntOUaCsiDodxr6UpRUlZlNajTrRy1FdD1zjWIe6t03CbiCFMLoDOgER948udR6uNsvAqWFowpuCjo9yTjPr+MVGe3euqJyEWjl1gGCqwdh8qnToqK91FMHhMPJpSinx19WSrF/itu2ttbeICKAFHcnQAyPuUnhk94/UonHATk5SlG//wAvyOniXGPw4jr/ABH/AGULDL+36lbpdH84/wDL8kay/FEuXLi2r4e7Gc9wTmjbQpFTdG6tYlJYGUVByjZbe9+SR/pHjH4cRpt9ht6eCo+zr+0r6ro/nH/l+Rm/iOKu6O1vEFrZLIe4PhJEE/B0prD24fUnGOBimlKNnv735H/9KcZH3cR/uP8AspLDL+36lbo9H84/8vyM4rF8Xuo1t0xBRxDDuIkdNEkU1QS1URwhgYSUouN1/u/J1hsfxi2ioiYhVQBVHcbKBAE5J2p9RxsKVPATk5Scbv8A3fkdPFeMn7uI/wD5x/h0vZ1/aLqej+cf+X5ImDucUs3Lly3bxCvdM3CLB8R111SBudqbo6WsWTWCnFRlKNlt735DBvxS0jW0t4gI5YsvckglhDboYnpQ6N3doc/YpyUpSjdf7vyJjrnE7pR7tu+TaOdCbJGUiDm0T+aN+lCo2vZDprBQvGEo66P3vyNntjjv/mD/AGbf/LVXUw5Fn8Ow/wDb836nFztZjWUqb5KsCpGVNVIgj4elS6qPIF0fh4tNR+b9Skqw2iUCCgAoAKBDtRL7hNA7hNAXFmgY5hrD3XVEUszGFA3JoK6lSNOLlJ2SNJxbB2+HWlRWzYtpDuNUtKQMyIf5SCNdwGO0im9Dk4etPHVHKStSWy4y7X2fLTjqehdlOI37PDsEtu2HF1GRDDHJe74wXg/xeQux2+DfWu3gaNOpSvJ2tq+1a7dt7Lx7DyHTU5Rxs7Ld/PT5Eq72oxKz9mp8DMqqjE5hPxnOCg008JBJHiBMV0FgaL4vfmvlpr5ruOS601w/fP8AeY7iu0eMBYLhhJe4ltWBkNb7tvGysRBRrkEc0A51GGDoO158E343Wl9d7eDHKtU4R/dPtc6t9qLxa2e5ItsSXOS5KJcdlw0kaBvCrMDsHHSk8DTSks2q21WrSvL0XcNV5XWmn7b8kax2rxjWyPqsXTbw7IuS4VZrguvcbQzkyIojdWaDNWSwFBS+P3byvquFkvG7fetUQjiKjXw62X3/AHvJbcexObMiK9snD5VFtluFb7HwlmuZQygQZAEnWIiqvZaNrN2fvXd017vcr2f7cn1s91tpw118Tq/xvFmzZa3ZBuXGvgoVJju2YIvxgLMAFpI1kA0o4ah1klKWiy6352vwe3IHVnlTS11+RHHaXFA3VNkSDcW0Aj/EL5tJsxN1coZ2KhYC/wA4VY8FRtFqXJvVbZbvu10V7/Ij11TXTu87ePNjn+sOJjPkWO5DC33VzvO/Ld13JbNyu6zl+HlzqPslG+W/He6tl3vty7d/IfWzte3Daz32t59mx1g+PYu7dtotkQBb74FGXKxuul0hmYZQFQOBDE5gNN6VTC0IQcnLnbVck1stdXZ6qw41ZyaSXf56+oYntDiEv3LeRSFcBYRiAuaCWcPo3PKVHkWAojhKUqcZXe3Pj2K23bd+AOrJSa/f3wI1rtRimAD2ls6Wszulx0Ba27yArCQ2VQNRBJBkxVjwNFP3ZZt9E0no0uXDW+991oR6+bW1tuA5e47fuq6NZKowvrnKxouHzgZcxKtJ1kRy3rPWwtOFOUlLVLbxty2NGHqydaKtxPAq84fUApgFAgoAKAEoAKAO6RaLSC4TTC4TSHc7s3mRgysVYGQQYIPUEbUEJRUk4yV0xbuIdhDOzCWbUk+JvibXmYEnnFMUYRj8KS/G3kazgv0j4vCYdLFtLBS2CAWVy2pJ1IcDn0q6NaUVZHJxHQtCvUdSTld9q9Cb/C3jv5PD/wBi5/iU/aJdhR/29hv7pea9BP4W8f8AyeH/ALFz/Eo9ol2B/wBv4b+6XmvQVfpax5MC1hyToAEuST/vKPaJCfQGFWrlLzXoWf8Arvxz/wCn/wDlsR/zVPrKv9vyZm/hnRv/ALv/ANo+hW2/pY4gxgWsOSdgEuE/LvKh7RLkaX0BhUruUvNegn8LWPmO6w87RkuTPT+Mo9okD6AwqV80vNegN9LXEAYNrDgjcFLk/wDqU/aJCXQOGeqlLzXod3fpU4koVmsWFDaqTbugMOqk3NdxtR18+RGPQeEk2lN6b6r0Gv4XMf8AyeH/ALFz/Eo9okT/AIBhucvNegv8LmP/AJPD/wBi5/iUe0S7A/gGG5y816B/C5j/AOTw/wDYuf4lHtEuwP4BhucvNeg3ifpWx1xGQ28PDKVMJcmCIMfaedHXyHHoHDxaactO1ehhKoO2FAwoAKBBQAlAC0AdUiYUAJQAtAwoASgQUAJQIKBDmGMOp0EMvxEgb8yuoHprTRCorxf79T0ztD2hfA4ZsNdSxcu3clxFtLfOHW2QT3ge483C2wy6aGSdq1zqOCyu1/kebwuCjiaqqwclFXTvlzX5WS0t2+BlOxfF8bac4fAqne3yvjyKzqF38TSAnMyDHlVFKU17sOJ1ekMPh5pVcQ3aPC+j/J6JxbF2rLY/HWBbbEWLViyzqoIF5mYXXHUwyD/9ZHWtUmlmmt0efoU5zVHD1LqEm3bs4L6+dzJdsLxxnCcJjrwX6wbj2XcAKXQZ4JA6ZB7k7TVNR5qam9zqYGPUY2ph4fDa9uT09Rrt5/7u4T/+G5+lmir8ECXRv/lYjvX3MPWc7YUAFABQAtABSGFMAoEFABQAUALSJBQAUAFAxaAEoEFACUAFMQlAi4PHi+D+q3rYuZDmw9wmHsz8aDQ5kOnh0/SJ57xyvwMfsmWv11N2v8S4P0faWXY3tevDkuAYVbrXNC5cowSPgEAwJ10j8hU6VXJwKMf0c8XKLz2S4Wvrz3H8P23S1eZrOCtJYu2xav2JlLkFiHmNGAYjY6T5QKtZ6LTkQn0XKdNKdVuSd1LittN+wre0/ac4xbVpLSWLFkHu7SGQC27E6SfbmepqNSpmsrWSL8HgVh3KcpOUpbtltY7c2Th7Fi/w+3f7hMis7nykgZdJgfKpqssqTjexkl0XU62dSnVcczvovyZTieJW7ee4lsWlYyttTIUdAYqmTu7o6tGEqdNRlK7XHmRaRaFABQAUALSGFMGFAgoAKACgYUBcJoC4lArizSHcWgYlAgpgFAXCgBKBBQAUAFABQIKACgYUAFABQAUALSGFMGFAgoAKACgBKBBQMKBBQMWkMQ0xBQAtACUAJQIWgAoAKAA0AJQAtABQMKBBQAUAKKBhQAlAhaBiUALQI//Z</t>
         </is>
       </c>
     </row>
@@ -1901,25 +1901,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SHAMS MULANI</t>
+          <t>ASHUTOSH SHARMA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>smat2023_058</t>
+          <t>smat2023_096</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>212.5</v>
+        <v>166.7</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1931,85 +1931,85 @@
         <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
+        <v>50</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>31</v>
+      </c>
+      <c r="X12" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>46</v>
+      </c>
+      <c r="AD12" t="n">
         <v>25</v>
       </c>
-      <c r="M12" t="n">
-        <v>4</v>
-      </c>
-      <c r="N12" t="n">
-        <v>18</v>
-      </c>
-      <c r="O12" t="n">
-        <v>3</v>
-      </c>
-      <c r="P12" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>6</v>
-      </c>
-      <c r="R12" t="n">
-        <v>8</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" t="n">
-        <v>45.8</v>
-      </c>
-      <c r="W12" t="n">
-        <v>13</v>
-      </c>
-      <c r="X12" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>23</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>17</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>5</v>
-      </c>
       <c r="AE12" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="AF12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AI12" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AJ12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL12" t="inlineStr">
         <is>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFRgVFhUVGBgYGhkVGBgWFBgYGBkYGBocGRgaGBgcIS4lHB4rHxgYJjgmKy8xNTU1GiQ7QDs0Py40NTEBDAwMEA8QHhISHjQrJSw0NDc2NDQxNDU0NDQ0NDQ0NDQ0NDQxNjQxNDQ0NDQ0NDQ0NDQ0NDQ0NDQ9NDQ0NDQ0NP/AABEIAMgAyAMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAwQFBgcCAQj/xAA7EAACAQIEBAQDBwIEBwAAAAABAgADEQQFITEGEkFRImFxgQcTkTJCUqGxwdEU8BYjYnI0U2OCsuHx/8QAGgEAAgMBAQAAAAAAAAAAAAAAAAIBAwQFBv/EACURAAMAAgIBBQEBAAMAAAAAAAABAgMREiExBBMiQVEFcTIzYf/aAAwDAQACEQMRAD8A2WEIQAIQhAAhCEACcu4AuYMwG8rnFmdJQTxOASD4T1gAjmfFiI/y1tc31PlvMp4s4sqVm5OfwgkabHtIziDPGZzyk6Xt77ysO5J7xkRT0OXxJPXX9ZyMW23QxsoJNo9o0e4uD9ZDFTbODY+RnVAuNPaOBS5R0I6dx5EdROkqqwtYXH19pAyBkcr37RGi7g8pv/faK08dyNr7xxVxCG19DuCJHY3TJHKcxq4chqblDvcbH1mo8J8fpXIpViEqbA9GmMf1g1U//fMRF32ZCbg331HpJRDaPqsGEonw14rGKpfKqN/m0xbU/aXoZe4AEIQgAQhCABCEIAEIQgAQhCABCEaZhjUoozuQFUX3/KAFS4x4s/pjyqLt2MyDiPiKpiX53OoFgBsBHXGWcmvUd/usTyjqADYSos57xvBFM9qOTr1iMWDHvOxTvuYCaPUs++49jHiuy6EXHcTyjhARcA3+gj2hklWpYKpMWrleR5in4QyrYq33ZHs+txpLjR4NxFtfoZzX4LqDW0r92f0seG39FSqVObfQ9+88RjsfaWJ+E6w+7EH4eqLoVh7s/pHs3+EE08VyJIYnLHTUqYxNM3tLJpV4K6mp8krlGPek6ujFWU3uu8+geDeIlxdIEkc6gc38z52wjoAObrLhwZm5w2IQ83hbfXTXoYzkmXs36ETo1AyhgbggEH1ikUkIQhAAhCEACEIQAIQhAAmSfE/OHNb5CkhVFyO5Peajj8YlJC7sFUbmYRxjma1qz1VNwT4T5QJRTsfW5m9NLRneOMSBzGJoknYjXYKTH+EwxJjzJMmeu1gLL1M0nJ+FaSAEjmPcyjJlS6RoxYW+2V3h7IWcglSFHcS/4DLVQWAEeYbDqosBYeUdoombTp7Zp2pWkIrh5zUwoPSPQJ6wj8ULyZFPgl7SOxODHYSwOIxxCyupQ80VTGZep3UWlTznIlPiTQiaJiUkRjcLcGNFOXtBcqlpmRYjDlSR2MkcrqXqKN9ovm6ctY26/tGCsQ2g8xN8VtHOqeLZ9HcE4gvhUB3QcvsNpYJnnwtzNnplCNtb7W8rTQ4PySEIQkAEIQgAQhCABCEIAUv4k4Vmw9wwAG9z/d5htatYFG6HSfRvE2XfPole1zbz6TAs6yw03Ktfc7i2kZdoNkC1Mkyy5Bw41WzN9nrI/A4YMwFtzYd5qWSYUJTCj1mfJX0i/DCfbPcry5KYAVbCTlERpRjtXmQ1MdobRUNG1MmOllkiM7F5yxnq+cTcjpGIB2jKvrFnMbM8SmNKGmIWRmJbeSuJYSIxAuZCGKFn+G8YPvIRtNzte/n2EtPEvg8UrzIG1672mzE+kYs0/Jln+G+ZNRxC8xsrnlIPfpN6nzlwqrPi6Q1tzj8jPo2WvyVLwEIQikhCEIAEIQgAQhCAHhF5hfxGUHGuo6W0/WbqZgPGj3xdVj/zGAP52/KSgGOS4e9ZV7C/11mn4anyoB5SlcDYXnZ6jfd095bM1xvy0JXfYesoqd0aoepF2rKhsSIHHoN2H1mfvVqO1yzFjEny/EnWzN6XlPtr9LOb/DVMJjEbZgfeP1rDoRMew1WsjAEMsuuVY8soF/X6wa4gvkXHnFogMQvWMFqG3lIXNMUy7SORKkm8VmNNd3EjVzJGNg6/WZ9mDVnc2DGJJg8QPuuPaNwT72Lya60aG+JVtARftGbgyn0sQ6ENdgRLZluK+alyLEaH+YKBuRWuMKZNLm7HWVnDNp7b9rTQeJsvL0H5RsL/AE1md4JdCNyb38hNGFaWjPmXy2XT4YYMPi1fogLW/L95uEyb4R0f82o1hblt7k3/AGmsyyn2UBCEJABCEIAEIQgAQhCAHJ2mCccogxLlGDAvz6DTrcTbc7cjD1Cu/KbTDc3R2axX7O56kGRz09DqOUtlk4ApWwzN1Lm8f5xqLdY24J/4dx2ePcXRLXlN1xL8a2istVVDYAX2va59h1nP+IlRmQqwKi5JcoPoL6yQOXgNz/eB0vE8bkdKs5dzq1uYKQLkbGJLn7HpVroaYeu1QB7MFbbnFwf+6SeEplGBANjJnAYMBFphTyKLWYC3/uL1cOoIVRYDp5+8S2tdDxsf0KJKXlcx6jnPNe0uOGHg9pA5hhVdjfY6G38xPwlPyV2tjuQFkTRRcm1zYdT0tGH+MG8A5Ffn0AGjD1Etq4NUR0VfC4IbY3B79ZWqPDKU6q1F5mK7X5eXTbQS9cddldKm+jwYylUJRk5H2sR1kjk4CMUOxnlTKfmPzv8AaPYWklSwAW3lE5JP4j8X9jypTBR7/hb9JjaoRUewtqbTaHX/AC3/ANjfoZlWEwwdzfudJpl6W2UUttJGmfCqki0n6Ox5rG32elpoMy/4eUWXEE3OqEH8pqEma5LZVlnjWghCEYrCEIQAIQhAAhCEAI/PFvQf0vMwx+E5gTcDSaziaXMjKeoImZY3RXX7ynbyEz5l2masD6aDg4WR1/1ayX+XcyF4UcczgddZYbWhk7nY09PQmuCU7iOKWAQdBFaUd0ReZkuyxsbPTsJGk3a0l8XVAFpDo6q++8KQ0+CYpAhJFVjrJhai/L8zIbEamFLSRE9tkhhqYIg+EXtEMDV5TYyUYgi8aVtC1tMjzhh2iTU46rNGwNzIS7J+jvEqBSf/AGN+hmaZSnjItuZomdVuSg/paU/BUwDzsLCwt5nymnI9TorxrdbLTwfTtW0Gw1l9lW4OwpCtVItzGw9OstMfEtSU5q3YQhCWFIQhCABCEIAEIQgASgcTZfy1ywGjeLTrfeX+Q3EWEZk5kXmZenUg7xLnaLMVcaM6yl1TEkDYg+0sVauJTcXSrUq/OyFVOguCN9I9XMLgfpEa+Jen8i04fEXEeU6+kqlLH6DzNved188VBa4v67SiZey1taJrH1LIzX1lFzPitVsvKSwM9zbibnUop36yn4l+di39kyycX6V1l0tSaFg+LUZBrr+kb0+MkD2cMB0bpKYcJUQXCNr5dI1cnr0je1Iry0jVMuzharXU+HvJ6ljPOZJluasiWkxguIm5gL3v3MreNrwP7ktdmgvWvOKNYXkNRzAMoI7T1MYAT9YsrsemtDziqv4AO5ETy7LmqhEAGh36Ad4xxTfPqJTuRdgLgX95oOTZOKA+0WPci001PLRn58U/0kMNQCKqLsotFoQlhnCEIQAIQhAAhCEACEIQAIQhACofEWn/AJCv+Fhf0vMzr1PECPWbBxZl5r4Wog3tzD1Gtphxr8h5GJup5SDIpbRZFaJb+oso166ntfeQOZ4pizKOpFvTykgtRTbtuR+0jsa6moO17e0qlaZZb2houW12HOq6ess/DvDyOAanOpuNxpeOMK4AC20sI/o5giacw9O0WrZZGOftkonDoJKrWBA7mV7OeFkALh+ZgbWHXW20tmGzPDsouQG6kHf1jLOM4o6KltNz3kePsfin0/Bl1fCVrlFQgX0JFo0YOhswIt3lwxua0+awNyZC5vVDW/vSWTTflGe5ldpkvluLPyRr3t7xTD1zzAMTfbf85GYDEKFA/KKJVu35QU/Inl0i+8K4cVMSh3CAsf0F5pso3w3wJVHqH73hX0EvMtKae2EIQgKEIQgAQhCABCEIAEIQgAQhCAAZhfxGyf8Ap8SzqCEezDtc72m6TMfinmdJzTwqqHqsd76L2HrJlNsNma0cUoXfWRwr8z37TnEAoxQrYjQjz2iaKQL995PEHeyw4bFtyE312WcVMBUPjuTfUyJpVrSRTNG0FyABKXLT6LppNdiCV6l7C5AgDVcdbHrJKjjFFgbC92G2rGI1cUqjT7N7Eeo1h3+E9fozrYflW537RlVrEgX16e3SKVsQTp7CJ/LOva8sif0qqvw6o1Sp1uB+smsqpNUdVUatpoCfewkKiXNjuBcfrLThRVwlD+qU8jh1VLgdfI+kZLsVN6NvyPBfJoInUKL+vWSEq3B/FaYxArWWqo8S9/8AUvlLTIqXL0yE0+0EIQkEhCEIAEIQgAQhCABCEIAE8nsa47GJRQu7BVGpJ/bzglsN6GvEGaLhsO9U/dFlHdjoo+s+ecyxrtWSsxJY1AxPqZceNuKmxTBEBWkuoHVj3P8AEo+Yr4L9iG+hnQjC5xPflmVZlWRa8Fx4xyAMxdBrubdfWUfE0yPDYg9RNIo5iKtJCd+UX9bSr5vgVYlgNeljOdNrwzbWNtbRUw1p0lQ2hiaLL0jfllhV2hwaxvvttOziTqOh1jQie8sNINsVR49U3PKdfCLevnGiJfa/aTmVYSxBOvkZG0iZlse5Hk9352sdNAZP8dEJg0QdaifkD/M8wdxt02kTxXUZwgOwYWEXHXLIkX1HGGxllmMei61ENmU3H8Hym58M56mLpB1sGGjr1DfxMHRZKcP5vUw1UOh8mXoy9QZ1s/p1knrycfH6jjb34N/hI7Js1p4mmKiG4OhHVT1BkhOU009M6Kaa2j2EISCQhCEACEIQA8hIbOeJMPhh46gLfgXVvoNveUDOfiFUcMEvTQdVAZyP2PpGcUpda6EVy6477NOxmPpUhd3VR5n9pk3H3EP9RVCIx+Wg0G126kyvVM8q1SWsVU9XPM7eZJ1EaVSSSd5p9DiyN87Wl9L7M3rMs/8ACXv9OX11ibJzAjvFUhadRrZgm3L0SuQm9ML+Hw/TSP62EuJFZK/K5Xo2vvLclMETzHqU8eRo9LgpZMaaKdisqv0kbVyduw9pf3wg7Rs2F8pWsrHeJMoByg/hiyZQb/Z+svIwPlPRgvKT7zI9iSr4XKtdpPYDKRcEyToYO3SSlGlYRatssmEhgcIFG0p+fNzOo7ay64+pZTKPj1u95q9CnWZIy+urjhbGoWc82nmdPaKVDEE1M9GzzmNdOn9Fq4Izz+lreIn5b+FgNdehA/vebHRxCsAVO4uJ8/UFuyjuwH1IlvoYvF0QaTpW5Oa6ul2ZBfTQaFfKcz10fJNa3+fpt9Fl+LT3o1gGEo+D4gxKjmIXEU+pQBKijzTTWTOW8WYWtp8wI2xV/CQe1zpMfFtbXZt9xb0+iwQidOoGF1II7ggz2QORWbcQ4fD3+ZUHN+Eat9Jn3FXxBqGm3yR8sbXJ8ZH7QhNHBTHJeTPzdZOL8GYV83eo9ySAdSTcsfeOMPVBN0RjfdidPpCEqjLV5NNmnJhiMW0iQZQyFTcE9QdhOkFxPITtYcKiOW3tnEzZHb466RxaxikISwov6O6TWYHsZdcuq8ygwhOF/Vlc0/8Aw7/8im8bT/R8UnnyYQnJR1GdfKnS0Z7CDJQslO08qN2hCAEbi05pT8cfG3lCE6n8r/tf+HJ/rN+yv9I+u0KIhCd5eTjPrF0O8KPGv+5f1E0RadekGqVcXamD9nkGxOgvCE4f9XI1lxR9V5Oh6CF7VV9iicT09DRw1Sp/qAC39dNY7o0qVVGqvhloP/1l8Prpa8ISvNinE+MlmLLV18hAYbE/aophnA/C7qP/ACtCEJhr1NJ+DX7K/T//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTERUTExIWFRUXGBUXFhgWFRUVGhYaFxgYFhUVFRgYHSggGBolGxcVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGi4fHyIrLS0tNSsrLyswLS4wLS4tLy0rLy8vLy0rLS0uLS8vLS0tKy0tKy0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAYDBQcBAgj/xABDEAACAQIDBQUGAgYJBAMAAAABAgADEQQSIQUxQVFhBhMicYEHMkKRobHB0RQjUmJysjNDc4KiwuHw8TSDktIVJCX/xAAbAQEAAwEBAQEAAAAAAAAAAAAAAgMEBQEGB//EADIRAAICAQMDAQUFCQAAAAAAAAABAgMRBBIhBTFBUSIyYXGRE3KBocEUIzM0UrHR4fD/2gAMAwEAAhEDEQA/AO4xEQBERAEREAREQBERAEREARPLz4WspJAIuN4vrAMkREAREQBERAEREAREQBERAEREAREQBERAEREAREQBERAEREATDi8QqKWYgAAm53TI7AC53Ti3tF7ditVbDID3aGwOvjJGrG29eAG48eUBGj7QdpcVUaoRXq5TfXMy3HQD3F6CVUbWxCNmV6gPNXYWvrz+sz47aL92ycDfh5WA+U0wqMGvY8Pzv9J7wSZedhe0nGUboHuugAqZnykaE3Zr39bS17N9rjggVaIcW1INm9ANPT6zjQqXf1MxnEm/rB4fqXs/2xw+K0F6b3ICPa5tx0J6fMSxAz8nYDHOjKRVZRxAYrrbmNRrO6+zTtW2JprTqNmdRZm57wunPQmeMYL7ECIPBERAEREAREQBERAEREAREQBERAEREAREQBERAKj7TNvnCYJimtR/CvQWuzegnKOyPZM4pTjK+iEnKB8ZBsT0AnRva3sjvqNMroxY0762ysMx/lmR0WlRoYdB4URftx9bn1kLJYiXUx3SSNMnZei6gGmNN2g+8i7Q7DoUNk11tuEuWFGkzu0xqT7m1pehxjG9g2VSQfFKdtHZD0z4gZ+h8XSBEqm29nKVN1+nOSjdJMjKiLXBxRq9hLL2D7RHD11e5FiN3EbmHI6Xmh2xRC1StgNbcpM7P7LLVkXNYMd4BY24kAbxNvdZMLWHg/V+zsYtVA6nQgH0IuPpJUr/AGMoVEwyrVADa9CF+AEcPDbSWCCAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIMA1m3aaFM1Tcl2+nDra85ovbfDtWy1KbUheyl+PUndLV2+r1GoslPQ5wo1tcZQSTyFzb0nKcXhq9QKisjasHzBj8XhyG2oI52lNjT4NVMWlk7BgcVTdQVYEdCJmqOv7Q+co3s92dURXFXwgEZQD+WkhdrFLNa1Qi9hlYj52mbKzg1bc8lwx+LpjfUUX3ajWa/FUcykb9JTdmHDIWpurGops6uWIHDTNddbjXS9xLFgBlb9USaR+E65D0vuHSRlHDJwy0ce7S0T3rXFiD/AMSV2NxAViGO8qFIHiQg3BUjXXdYc5au3mCBa+W1wdbcZrPZZ2ZfF4xG17qk4aoeGmqjzJE21T3RMF0Nkj9Edn2Y0EZwQzKCQ28aaX62myniieywziIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAVXtFWUuE8yfPdNZVpKqk2EiV8eGYNxJYnXjfWaztB2ioim1POS5G5PEQZjnzNnSq4giz4UJ3V1YNm489OHrMdPCLUBDCc2wuMyUERmZFuSLOymnrYWK69Z0vYpOTOzBi1tV1FgABrzlbjyTTWOGRMT2bpspB1B3g6+UUMClJbAAWm4qvNLtjF2QkSEmThkrG1ytaslE7rlz6AKAOt2+ktPYGkuEqfotJLU3DP7xYhhqSSeekomAqCriqt/hRLeZbnw3DfOo9jsDq1Y8gqnnYamW1uW9JFd2z7NtlqE9ngns3HLEREAREQBERAEREAREQBERAEREAREQBERAEREA4biKhTF4mgTbLUq24WDMWW3oRMWB2FUpuMrqL81JJPHMw3eks/tO2N3VYY1V8LLlq24OoORz0I09BzmhSmMRQBp1xTbhrYiZZpxl8zo0TTivgbWrSqlMtRKbjd7wIPowBkPDGtScGmKiLmUMhN0sTqyH1mbs1gsUPfxAqKNPhbd137pusbXCC7EaSmcjTxIy7QxwRdd0pW39ulhZdBz+5kva20g3G43n0lSx1bvDlUC5t8t5P2kYLL5Ek0iz+zTY713ZzcK7an91ADfXfcm3nO1YagqKFUWUCwEoPsmyilUW+qkD0NrfMqZ0Oba0sZRzL5S3bX4PYiJaUCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAYsTh1qIyOoZWBDKRcEHgQZyDtl7PKuFFSvgWzUQCzUSbMgA1NM/ENNx1+07JMOMpZkdf2lYfMWnjJRbTPzNhtvYil7qut+V+M+MTtnE1hYh/rrpbWb+hZSyMPdJHymCtjkvZdev8AvfMUp/A7FNDlwuTU4X9JIsxCru1Nzr5cZtsHskILsfEeFvFbfrwpjodeYkjC1SfdGX974z5Hcnpr1MmUqNpmstfZHYo6c1zY/wAD6woyKQoyA2JsTdre6WYm5try38J1XsdtM1qADG7p4Wvv6EzlDV9co05k8BNWHxOGqGvhHZOdybv0sb5vIzRpH7XtMq6po1Kn91Dleh+ibz2cz7Ie1EViKWJpMtTdnpqSvmy71nRsLiUqLmRgy8wbzoOLR8k1h4ZmiIngEREAREQBERAEREAREQBERAEREAREQBERAPDKH299pdDAE0qYFfE/sA2WncaGo31yjXy3y57TqstJ2QXYKxUcyBeflba+Cc4s0ibuzLdicxJqWOdiOJzXlc544Nem06szJ+DdnGNWPe6DOudgB8R3gE8L6eU+6FIA9ZIr4Mbl3A2UWFrCwHraTsDggvvanl+cwTluPstFp1RD1bMmFpm2g/CSFptvuR5afKZbz6Yk9BK9poc2z4Z8tO4QtlOW+p965AJ8wZpNoYhmPiOvLlLAKhFKrTHxgHqCpuCORsTNdhtmganU+p+8ntwkVU2JSkn4f9yJhLWytcXOpGh168fKWPYGOqYdr0sxHG1yGHUf6T5o4RQN0w4zDEqchKsNVI0sfymzTahwe2XKZyuo6KGoTnBYkvzOs7F2otdM1rNxBvp85spxHsv24NGoBiAbbiygm1tPEv5Ts2CxiVUWpTYMjC4Km4M2WQ2v4HyrJETwT2VngiIgCIiAIiIAiIgCIiAIiIAiIgCIkHbG0VoUXqtuRWaw3mwvYQepNvCJGIrKilmICqCSTuAGpnBFpU3r1KutxYobDKytcLrwZbEW6AyxbS2qcQ5L12GYWNN83dG/IAi01G0FWmEREAJ3hSSLniL/ALoHzmPUTyuD6Tp3T9jW/u8GMnWy7+fLrMqclFz/AL4z6p0beszB0QZqhyru6m99B1sDb0maMTu3WbItnyzJTsarX1Ay0vG2vPLoo8/SS6TUGLhKpJQFiMjAjgASdxuRIXf4eghy4Y5QRZrAMLk6WY3GmXXeDryklcQrUg6Xs1gLgKbU+g0HiPrlvxlmFg5qttnJd1n5YPKB8QHP7T4z2/D855h28RbkPvp+cMdQeX34SLfsmqMf38vkv1JqHQCLyPn93zEy8JFk3HBp8fsRHYtdgSbm1jr5GT+ye0a2AZiDnpEgsvA295gPhe3ztPMS/ATytgqtNQ702WmWKXPBuVt4/GfQ1aC+WnUnNZfZM+L1PWNBHWOl1NpPEpLw/PH6nZsBikq01qIwZWAII5GSJzr2WbRZTWwjG4Sz0/4WJuB0BnRAZhi21yR1NP2NjinlePin2PYiJIoEREAREQBERAEREAREQBETwmAR9oYxaNNqjsFVQSSemsodTHVMaRUbw0TY00IsWA1zVByOhC9LnkMvtHx3eVKODDABj3lbicg90dLkH5GZtl4diilAOFzcgDpfcRawsOInsYb888GqMo0VqbWW+xCx9Ch/WKpO8gb9d27dKvUYM7WFhc26DcPpN7tvBrTap4ycqgkn9q2gHpaVWk54TDqUt+F2PqOl7pVb5Plr6E4ifNdFtTLe7nfyzZPBf6n0mJGMyriQAVdQ6Na6nTduIPAyk1XxcoYiR8OcQQcOoUrmqoztYgLYZmJ32HPrblJlXKAqL7iKFXmQOJ6k3PrMC1rLlpqETeQNSx5sx1Y+c+S08b8IUUNPdLj/ALufFarYX/fQfO8PW8SjzPy0ExY0fqHP7Nn/APAhj+Mi064aqLcUBHqSZHOUaa4e3KRtke7Dz+0mia3CPdr+dpslMEJo+cPs+pWcpTF2ykgXA3b7X4y7bZ2bSqtTp1bhyFqVFVjrlXIwtuuSVF9+hlHqMQbqSCNxBIPzEivXfNnztmFrNc3uNxv5z6rRWftcIpTScFj4n5j1rRvQXznscoWPOfC+Hz7/ADLJ2Fw2XHgqGCGk5UsLEpmAW/UEEek6aJzTsdtitV2gvfPmJpui6BdNGtYC19J0uYL4uNsk/XwbIzc6q28+6sZ9OT2IiVAREQBERAEREAREQBERAE8ns8gHKM4faj1KpHv1Cc2oC0wUQW47gbcz1m2xvai9xTUW4F7k+lNfd9TKttdiuLqjUHPUHoSfuD9Z6r2Gg6DTnw85VXfsTWMvJ9Bd0uN7g3LEVFf5PdpYxnLFySWvm4XJmuXSWfC9l3Lr37CkuR3NtWCplvfl7wk9OzND9JoBCXpVEZyGO8KBbcBoSRKHXKTydCOvoqWxPOF4+BS7T6NBs2TKcxIAFiCSdwsZ0ZtpYalh2xFLDjwP3a+FVJN7Eg66b5E7W1cuNwjBQW0GvVgBfyuYdKS7lUOpznLChjv3flLJU6Ow8Qagpd0Q5XMFJUeHnvtMG0sG9KpkqCzWBIuDod26dCpVj/8AKsotbuFvz0JIty1aUntRWz42qeTFR/d8P4SNtcYxyvUt0WttutUZJY25NblBUqdzAg+t/wA5XcA1qiryTKfNdJY23StYnwYkHg9/Q2N/wmaJ1+zyb/DP4gPST1bWafBVLsOht9Js8/iE9ZGSJDCfVLZ9RhmWmzLzCkyXshKbVVFUHKdBvtc7s1iDbylvwW0Qaww91UZGZCuUArZe7Ka31u2n7pmjT0ynlp4wcTqPUVp2oOGc+vYpuyKbUsVRZlZMtRd6kaHQ/f6zrcrO1WYVUqCqFbIpyuzKpIIPkQQWBvu0lkpG4Bm2NX2a75yfO6nXftU/d27eDJERPTOIiIAiIgCIiAIiIAiIgCeT2eGAcv7QbNQ7UdXOVXAe4/g/9lm+wxB7ujkUCnXoLpxPdCqSetzIHbil/wDdpEcaTf4c02desj1BkBVqWIVW3AOxpEX66ED0lUVhs61tkpV1/d/0RMFs6u9XFLVqeNqYCkksEWozWGnRRoJOByVa7fDh8OqL5lS5+gWaRKb0aTjEVLu9egHJYt4QFdhc8ADPjHbfpGhiVXMXrOxvbTLoq6/wr9YcklySVM7JeysrhcLjxyfWKS2z8InGpVDHrck/iJK7SDNtPDJy7s/42P8Almm2jt6m64VVRrUMt72GYrl3fI75Hx3aTPjFxQp+4AApPLNqSPOVOcfX0N1eluznb4n9X2Lfg2//AFq5/Zop/lM55iamaqzc2Y+pJMnN2nq/pNSsqorVVCsDcgAADw679Jrae+VXTTXHxNmg0s6pOUv6Yr6Lk+6u6Vnar3PUHT01lkrnwysbUJvM8O51+MEzZFa7et/mPzm7V/EJTNhYy1XJw0+vCWyg92EnOOGVQsjZHKNst995s8G+fD1Qbg0VNWnU0/VsCLKvHxEnja9tJqqbTY7L2oKQZWpLUVirWa41XUHTeOknp7VXYpPsc3qWmd9EoRWX4Njj8dimo4eo/hLpVUXVDdlGek9ipy5gLW9ZauyuMd6RDra1mTQDNTa+R7DcTYypY7tWaoUNh6RCkMubMbEbiLESf2V7Qq9dKRp92Qndrla6kL4lBDaiwvbWdOWrqsW1cHyz6Rqqk7JLjzyXuIiRMwiIgCIiAIiIAiIgCIiAIiIBS+2qqMTh3c2QJWzG9tLf6ymYnb9Q95l8HeVe+vvZSPdA4aS1+1QeCif7QfRZz07rzNbJp4R9P02iE6FKXPj88krv2c5mJZjvJ1Pzn2+6RMO3CbB6YKiZ5HWrwuEQmMjqfFM7LMKprIF+Txx4h6yVRHPTrIrHxCT8KbjSRfYZI9SoN2srm2qguVGtgfn/AMS3YhyF3ayobc8CkjeQ1z1YgAeljPaVulgrut21uRB2TQHdNU+LPceS2P4yy4WrrIuy8JbB7rllJ8r3Mj7NxFxqbZSR56y63mTKtF7NUU/TJacO0zEGaqhtakmjMR+6il2P2A9TJuG2oKjWp4aof46qg+oRCB85mafcjbrK4SxnPyMzLM2z63d1adS1yjBtDY2vra+/S8kPhqgF+7pL5l3/ABA+k02PNW4sUW37KLY+Z976z2DakZ7NbCcXHB3VWuLz6EgbFzfo9LPbNkXNY3F7C9jxk4Tro+Pawz2IiDwREQBERAEREAREQBERAKN7Uh+ro6fE/wDKJztD4Z0b2oW7ugP32/lnP8LS0PQmY7vePqulPGnX4kWm9mm4pr4fT5zQFvGfOWvZ9K6DrxlM+Dfv2mkrrYmfG4fhNxi8CPe/2Jp8YPx1lecl0ZqXYhl/EJssJVtaapfemyw28RLsT8EnEnQcpUO2KZWVb6tY210su75n6y5rSLGy7wCTfkNTv0lM2oe+xyg6+JQepJzN5f6S7SLM8+nJyuo2YhsXnC+pYEw5FMLbcoHyFvzlRrhlFQrvu3TjvHWdDamADw03c5R8Ylu86FvSRhLLZfY/ZwvQ82OuZVHxGwO43vxvOlbJwa01su/iec5/2Jw+bK1tFsfpYTp+Bo+G8T74ORJYwKw0lY2h72m7jLPiW0mhrUb3Mo8konTOx+NFXCUzxUZG6FdPym7Eonsxdv16/CCp9Tm/C0vc61bzFM4l0ds2hERJlYiIgCIiAIiIAiIgCIiAUf2n+7Q/if7LKNR9x/M/YRExX+8fUdL/AJdfiaap/SfKXPY3uJ6z2JTYbbezJGN931lTxcRKo9yWn7EBvfmzwvCIk5djV4Nrhfdq/wBjV/klCwP/AF//AHH+xiJfpO0/kcPX/wASP3ol8f3v7p+8omN/rv70RKa+5tsNn2D/AKIen2nSML7giIn7zOVLsiLieM1jcZ7Ep8nsexafZl/R1v7Qfyy6xE61PuI49/8AEYiIlhSIiIB//9k=</t>
         </is>
       </c>
     </row>
@@ -2028,40 +2028,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NEHAL WADHERA</t>
+          <t>TANAY THYAGARAJANN</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>smat2023_135</t>
+          <t>smat2023_096</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>225.9</v>
+        <v>166.7</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>18.5</v>
+        <v>50</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -2094,10 +2094,10 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="X13" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -2109,16 +2109,16 @@
         <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="AC13" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AD13" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="AE13" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="AF13" t="n">
         <v>0</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="AM13" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQTEhUSEhMVFRMWFxUbGBcYFxUbFxoZFxUXGR0XGhcYHisgGx0oGxkaIjElJSkrLi4uGCE1ODMsNygtLisBCgoKDg0OGxAQGy0mICYvLS0vMC0tLS0tLS0tLS0tLS0tLS0tLS8tLS0tLS0tLS0tLS0tLS0tLS8tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCAQj/xABEEAABAwIEAwYCCAMGBAcAAAABAAIRAyEEBRIxBkFREyJhcYGRMqEHI0JSscHR8BRi8TNykqKy4QiDwtIVFiQ0NXOC/8QAGgEBAAIDAQAAAAAAAAAAAAAAAAMEAQIFBv/EADQRAAIBAgMGBAUEAgMBAAAAAAABAgMRBCExBRJBUWGBE3GR8CKhscHRMkLh8RSyUnLSBv/aAAwDAQACEQMRAD8A7iiIgCIiAIiIAiIgCIiAIiIAiic54iw2FE4isymSJDd3keDGy4+yrVL6VsAXEE1WtH2zTMezSXfJAXtFSKf0pZeXhnaVBP2jSeG+fX5Kz5Xm9DEtL8PVZVaNyxwMHoRy9UBIIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiA18Zi6dJhqVXtpsaJLnENaPMmy5Lxr9K+rVQy+QNnYggzHPsmkf5j6DYr7/xB0nmnhjqHZ6n92bh8CHRztInlt9q3GKeI0sd94zHX091mwRIYnFuc65c55vLiXOcY3JO/qtarXLXEOcQI3Hvb81HtqPMEbiduhH9V6LHPAbEEE/0PzWbmbG4HgPPek3PO0AECfKfkpLIc3xGFqNq0KppvtMbERJY5psRvYhRAy6q4fCZaCPMTMfOyx1aNVp7zT69Y/osXQsz9IfR1x8MwLqNVgp4im0O7p7lRpgFzQbtIO7TO4ubxfF+aPobxmnNKAmx7RnvScR+i/S6wYYREQBERAEREAREQBERAEREAREQBERAEREAREQBERAck/wCIJp7LCOAn6yqPdg/QrlXDWTfxNUl8QPmT/su4fTPgTUwdJwE9niGE+TmVGf6nNVKyLJOyaH2gi3XzWtVtU3YmoxTnmbmB4Lw+xatx30c0CQQYH75qRoYtgIBe0G1iRKnaNcRvKpRk+JelFcDRZktCmzSGCBzi581C5tllJ7HN0AAhT+Px9NjSajw0DqQPxVWrcSYV7tDaoJnxAPgDssSi3mjKcVkznWT4V1DM8KWWjFUBPg6s1t/Qwv1MuJY3INONwb2iQ7E4c+RZWY4/K/ou2Aro52VzmTSUnY+oiLBqEREAREQBERAEREAREQBERAEREAREQBERAEREBz7j/NKhdUwmmKT6Yh0TD51B/LY6efLZQ9IudhGAgh2gstvIcRI9ArZxnhZLXESHtLDEdZ+Yn2Vay6u11FzW70XkR/K7vNN/B0eYKhUpXlHuXoxg4wa8jn2YZK4vcG0ajtMfaIcZ5tnc+Ft994sfCOCr0nNY8kNsI1lwuNgTzBsVdKNJjrloJ8QFjxDPrWBoiCCoJ1G42Jo00pXKpxZlj6lVzQ1r2iTDnQCQ0QJg3JMbKMy3LSXNacKGTJjunSAYEuAEGLwC7zV9rCK5B2cPwWxiS1o2ASM8rGXDNP3+fmV/OydOGcHaSxzouR3i0ACR4T6Aq6cBU6jcLpqOLiKj4J6GDA8JJVTxuJb9Qy0vdUJ8AGxPufcLoeTUdFFgO8SfN3eP4qdXc7vkitWajTcVz+hvIiKYphERAEREAREQBERAEREAREQBERAEREAREQBERAauOwjarCx+x5jcEbEeK5LxZgzl+NEPLqWJpkmwEOY6DYebTPiV2Rc5+mrLg/CU64EupVIJG+h4Id8w0+iKKb+RtGbWXAwZRiwQDMqG4tznsn030qo1THZgTN+fv8lV8lzKpoqUmHvFh0m9nHn4bqWwmT06LQ59Wpa+pukGeoOmZ9VScbStI6cZOayMmWcRl2MccS809LRAI7p3EzH79FY85x7ezLg7uxYj9VXaf8PiJLKtapaHOeQZ8CIiFBZqDQpmiCdGtxb/AHS0W903U5WQk3FXvdcy2/R/Sbjcc81WzTo0u62SBJqACY3EBy7Guc/Qxk7qeGqYh4g13DT17OnqAPq5z/SF0ZXbWyOZKTbCIiGoREQBERAEREAREQBERAEREAREQBERAEREAREQBc9484loPL8A2XVtBe4iNDdBHdnm7vctvkp7jXiL+DoywB1Z+oMB2EC7z4CRbmSFw7FP1YinXky4GTP37met1ajhpf4867Wiy9Um+1/djEZp1YwISq9+HqB7BYGYiys1XjljqJZoEmQT6f7rFm2X6myFT8VlN7HT6T+a58XCok5alyUZ03aOhZcr4sZQ1BjWwZMepWGhi3YqqNfwkgBo+cqvYfKoI70nyj81ZsDhtABFiOi2vCDutTEVOeUtDuPBfEdLEdphmNLH4XTTItBDRAc0jla45K1L84cMZk7CVDXZ/aOqTBJ7xL2gg9QRK79keasxNFlans4Xad2uG7T5FX8RhnThCqtJJdm0n/JSU7yceTZIoiKobhERAEREAREQBERAEREAREQBERAEREAWvi8Wyk0vqPaxo3c5waPcqrcX8Ztws0qIa+tzn4GHlqjc+EjxI50t2PdWc92JxNUvDHQKRLRJBMFxABERYAAeJJJtRwslDxamUfJ31S5ZK71fa5H4ib3VqdFfxVhz/ZvFUggHREN1CxceTfG+x3IhVvHZq+sXVH4xuHY131VNpcxtTSAdZqHS+oyZsA0ERsCCa5j86wzaLWUGVH1dIOp4YACW3kMADzFvhkiJcRLTBUs7xDC4itUl4bqJMkwJF3SREnaFepbNqfFbLgt61/8AWVvPdvw0bailWjl9v7+/obnGmJxQNOpWc2pDXRBJJbMyRZrSZkaQPh8FWcLXDvIGQPA7/OFvOqmCSSSXtLiTcjvAySbmXBaGXYQuqOY25u0DyIJ8rc11aWHUKPgzs0rp5WVmrvjlr8iFze9vLX8Pty9Mix0RI0u6W6LSxeVybXWxleMbalVIifq6oILYOw1CxaDYEGIjpKn62VrxOKw1TC1NyfZ8Gua+64ejfoaNSFeG9H+io0crIM2W2/D2Lj8LQST4AKysy4QZ5Kq51xBQM0WVabWgw4yZcbGJiAPz6Qs4XDTxVRR0XFvJJfnkvwzFarChG714L37+RGvZqfS5WJI8jP5qz8LZsWVjTFeozSWns2Ew8uDpkAX+ECNzNoKrtHG0Xu+pqse5rXAMu1xNoADwNW32Z3WPL6Hcqlx75c10HfTqLXDznRbzXtKrpYmk4U5J6LKztpb3lk3Z6M8/Heg7y/vidrp8Supk9o2oWASHPploAIEapvTEm5cHQIJgGVLYHPmPkPa6k4EDvQWydpcD3CZsHhpPIFcM/jKjXCoKjtY0w6SSLxEnlHLZT1HiRjw1uIpfAO5UonRUZ4CTAEidIhvVpXKq7JnBXXxeWt78E9e7v0us5o4hPodvRc0yjiGvQpsqa2V8M4WDop1m7y0AnRqAB7oMHTYBX/LscytTbVpmWOEjr4gjkQbQubUoyhnqr2v15c08uK+jJ1JM3ERFEbBERAEREAREQBERAEREAUBxVmjqNF3Ziapa4iYhjRAc8za0gAcy4WN1Pqo8S5pQZU0VXNDhGk6NejuOcHFu5h4YY/KVrP8ASy1g4b9aPw71s7Wve3Q5diXT3nC5Jk3dM7z1JPut/hXOWUHmjXANKoLGNUwLRzmJtzFxtC2eK8zp16jdHeApsY55aAapAJNQgdZ+SrdVoPcPofHeD48wfCdwvRYGi8TgfDrXabdnxtfJ35p3s+nFawbalCnjt6lHddotpaKVs1ay4WbyTu88wBbnz895APiAQvlZg84j5Be6T5md5E+YgE+oLfWVlczddpO5xDV7NoZUDjaHRY/E0Fzbzze1o8pVTxrqtUGmyRTJ7x21mZv1aDsOt+kXFoEEE2t1O1th5Ly5zOp9B+pUFXDxq5SeWWXVe16LkSwquKyRTaGWYmkNVJ7mgxIBPvHNW7hjPcVScBWPaUbdJaORH7919o1mgwATfwG4na/OVsMpAGQI8JkX9FH/AINCUXBq8Xw4duXbTgbLEVIveWT5k3xpiCaQpUzZ41Ei0j7I9SqJW4apx49eZVwzSoHFo1BwFOl17p7NpLd+Rkeii4tZaYHCU6WHjBq/HPi3nf6dkjavXnOq5afx7v3KzU4ZZyJW9gcI9gh1Wo8S2A5xIEdB6KTdTWJ7eXl8p/VWHhqKanuq60I1Una1zyT+I/An8llLSBPsOp5en5SsgpaehMj5ByVDF3crmeps0fMqS1jRsm8XmjBhqFBnxX19dUnn03dbw6Kd+jzPDSrCi4/V1jA6B/Ijz+H26Kg0xfUbudy8OngOv52CsmVZJinOcGUnmpTNPVOlpYXw5ghxEHYxym8KpLDUY0ZU3kpNu7fGTve/RtdrI335uaktVb0O3osOHeS1pcNJIBI6GLj3WZeSOmEREAREQBERAEREAREQBcZ49qgY2qd7tt/y2Lsy5nnvCjnV31a1WRUqvFNjLFwJLgHOc3uwLd1rtgeqt4OlQqVLVtOXP04LV6dXbXeOMr4W86Ds2rXtey6XyvdLVP7nP6jCO8PX+nMdR6i+54Dx4/vpuLfK0EW6JS4Kwz8Oa9KrWPcc4B2jcA2I0gxI9Vz2pTI7zfUfmPH8fmvU0KtOpeMP25NWtboceaknvS453ve982/Nt3bPGEqEmDv/AEPzt7Gw2W0/WbMaT1Ph4nl5r7w9VaMZQe4gNcXNcS4NbDmOiXOB09+LxIv1V2zLNGuc+gwtcBRquLmYitVbPZuYWd+G/aBsIuFzNo7SnhZ+HGKeV7tvm1pbpxZ1dm7Nhi1eTlrbLdy01vfnpb10KHQpuJMjlB26n9V5qYN/INjzV3ovcKTA3CF7nUmaSWtc3vPgPAZdpcQd3AyBa5XjMca+k5tY0NOptRoDnAhveIhga1pa1hFhezhe65b29iLZRj6S/wDR24//ADuGk7b078Pjp55X/wCD1+WeuTdGGHeDJHIG3g4D/qWatVggKx1+Jw1kNosHdAcb97S0kkiIuQDcHbnaKvmuIDqr3ABoLmkAAAAGIADQBZdDZu1KuJquE0tG8r8Glxb53OftbY9PCUVOKl+pRzlGV7qTvlFcsuerM7nA3J/H8FPcO8MPxff1CnSEy9wN430t5xzMgfgqu4ro/C+asdg2UqjXNjuAsImDYu3kNkXgHYk2mOhja1SnBOmuNm+S524nCpQUnn/fv5mzheGMK0TTpmtse0qPc1hkTIbTFxyv4784zM8soOoYhwwzKVSls9hqFp0OY5wAPdB0zI8VZKYHZwMQSLho0OGog6QwPiHHVAJjbkvOMpdpRq4dophr3VWuLXwSdLZAJmXaZnwAv189Rr4xVHKtPRrK74PXNLhla1tXlexd8Om42gu+X2b89b6a6nJDVvPILw4azYSAfSYj9+ZHMxn4hwjaAa0OLgdL5IA5mQCDBAg3stTAanNDfsgX6HqX/wDaPGYmB6qE1NJrz+xz5RcSUyHCiriKLN2Oq0w4n7TdQ1AeGmb7dOo6BiK2Hr1ammrTLCx4rNeCHg0ZDK1PTsQ15bqPxBoHlzgXHduOb+Xp19LeJuFu5TmBwzqjmiXvpljZn4jVpulwaQ4iGHaxMA2JUGIoOp8aeaWXv59Gk8zMKiWT95HZ8gxYqUQQZIJ1eBPej2cFJqucEZh2+G18w94O+4jmSZsR0HQAKxrylaO7UkmrZnSg7xTCIijNgiIgCIiAIiIAiIgCoeYZ3oBIGt5qVXAd0AB1RjGOl4OhxFemNuTh1VwzOs5lGo9gBc1jiATAsCbrkVfH1ajmatLYILW02xcGQ4kXc6RMk2N+a6ezsM6129Fr6MrYmqoKzOhcP47ttdF/aamsYTqYxgDajS3QNJuO6eQubWiOT1aLmyHDa0/KVYsLisQyr2oquDzpa55GrugmA7VMtEm1tzEL5iMnpucdGJaXE2IDYJPKAdvVXaeIoYKct+atJLJJvTJ6Lr+bESo1cSvgjpzstSj42oWHWwkFrmvBESHsIcHCRE2B/wDz4qRHE8lxp0KbC8PDnkue9we6bku0i4nutCz8UZHUpMLyAWjeNvPwVKwWJEETtPyt+qsVY4XFuNR2ks0vun+H6E2Hr4nCpxi3Fu1+ttOeV+RdKHE+J0gCpEBogNaIDTI5dee55ytfE5xWeAH1HOA2BJIG+w9T7lQ9CpqbIsFs1CwNi8+v9FLDBYdRuqce8V+DWWOxO9lUkn0k19Gsz5i8Q8gieTuX8jlhFXVLuZLVI5NldbEuDaTA4gOc6SAA0NIm5vuBbqtGng3sZTL6b2hwa5pcCA5sWc0nceS2hTpRn8CinbgknnZ8F0v2MVMRWqRtUnJq/GTeavzb5td2ZiSQY/f7C36edvZTp02hsCeTiS0nUQe9EF3QA2EELQ1Et6Dw9P0WtiHnukD73L+6ppxjJZq5BFtFmbxbVsNDSBsCa1rzb6yReNjyWL/zFUI0lrN77iQQ0RY92zWwRBGnzmvMY4nototDTJPp6KKOGprPdsbutLS/0NfOcc6rXM2Lniw5NANh0tPhJUlSw4hurvWs3ZoAJEkHe43PpCrtMl+MNrabxyBLfmTb3VxYwANi5gfrz8TZTUt2zS0vb0IKrd1fXX1JXhbBMqYhoqxpa1z3C/wsE77gTHpK3c9yhtdmv/0bKzSSz+HcNFZkSWwL62gTcXE+kDh8Q+k4VabtNQbGbybXMHy5zKyYbOK7KlKo+qajqbiWNd8AD5DgGtvdshQ1adRz34NeV3rn2z456CnOKjZ+/wCtTpHAuWVMOysx4hmtppkEEOHZtBcI6kK1KA4NxQqYYEMYwhxkMbpbcAghvKxHsp9eXxTk60t7W50qVtxW0CIirkgREQBERAEREAREQETxKHGg9jTBfDZ6A/EY592VQsBhmtkRPi65PmukZm2aTvJc4ZUhxHiq+KbdNR4X+2vmXMGlvN8TdOlzG6dAeJBEQJHMkfu60sww2FMdtSax5+F/wknoKjYv4TPgvroDw8sa6JEECb/v81hzDGP+BjO2pu5GJb/K4O3Hj79TWTVi9bM0zqE03uc+g6zdW46Anp+/PmGf5Q6hiTTAPZk6mG9wTtPgTHsupUcHUDdJHd6SLeA8Oij+I8odWpFuk62yWO8fSY6FW8FivBqZ/pev57fS5XxVHxYZarQquRZVUxVQUsO0uIElxs0D7xPIT/tKt9f6OMW1moOoPd90PePYuYAT5kKP+jbiBmDNWniqVSjr0Q99NwbLNUguiAO9IO299lY8q4UrEnEYHMQ/VPeMkunk9zS4O89O/IL00sY3NqMopZWbV0+6vb3xOC6dlmn78zD9F+Ee2tiQ+QWUy1zSIIJJsbfylVDPsVUdTw5c3utpGmwgzrDKjj8I2cNceNl0XgnD4ijWxtLFSazuyqarEPaWvbLSNwCPSVUeHh2mEwlaJ7LHAEAT9W5lB5MfdlhE7XW8ay8Wc3b9v+stG+b5/JmNy6SXX6o2sHwJTo021MwxYw+uO6SxrWkidBe8wXRyAix33W5mXAbiaQw9Vr6L3xrI+AaC7VYw4QLREkgc5W39KGGdi+wFCKgaKuqHCAXdnBuYMwdp2UPwtQzDDmkwvaMPTeCaeq2gmXNsN7mLwDCqRx8lFT8WKbv8Lt17+turJv8AFlL9j+ZL1Miyui/+Gq4mp2xgEz8JO0kMLG+TvBVTjrht2CqN75qU3h2lxEEaYlrotNxfn6K5ZrlWBqGo/sKrqry5x1VXtaXOJJk6nQL8gojjSlicaGUx2dMMlzwS4yLNDmWu2ZBm4JbO4nENpw3k/EbVs729Vbr9Opn/ABJpP4fIouR0nOxBLZOpjRA5wXX9j810bL8iJEvIHgN/dVfIsnq4bE66jmFjmlo06pBBkCCNonmr9h6ypY7bNW+5h5Wjztm29dVl2XUtUNnwa3qqz5cvT8/zp1chYBZz7eX6KKxeVxzmPDfz6fPdWd1SROyjMY5c+O1sbF38R97P6otPZ+GlrBfP8k39HDyGVKZsWltjIPMbG+2n5HmFdlXOHqB1U6g27J4cfN1MtB/zqxq1VqOpNzlq7fRFBU1T+FcAiIozIREQBERAEREAREQGOszU0t6gj3C5NmpLKpC66uYcW0A3EuHiT6G4/JRV1emyzhXaZjwtSd1tis0LXoUBCyNw7Rv81z7HQubLcUDsF70g8lgkDaF5GIhZMGc4Zq8NwTQdTRDuosfdeRjF8OYBEktBmZXYeb3J23MwvTKAC0X5otapmV91nUWZNFo6r7TAlQJzcALUrcSgHSPiOzQCXHyAuVskYZaqrL32WFrAL3Omf8LhDh/h73mxqg6FTEVPid2beli75WHzUpRpiLuJ8yimkzEqd1mRGYN1NBYJMtcI+fyJWXAmq6JaWDx3P6KaBaFjq1WqMkTPhfAUXja1/VbVeqoquZcPMLCWZm+R1Lh5kUW+Q/BSi0spp6aTB4D8Furrs4r1CIiwYCIiAIiIAiIgCIiAKh/STgCNFdu3wu89wfx9lfFqZjgm1qT6Tx3XiD4dCPEG/osSV1Y3hLdkmcuweZANE7rPUxIK0swyPEUXOa6k9wbPea1zmkDnLRa3XZRFWu9rdcFtOQNTrNk7CTzMhVPBfBHR8SPNE4+v4rWOJI2UO3FT9ufJev45rdz7la+G72Nt4kXY13QryalQ7BQ2I4ipN+230Mn2C9UczFUdyqw+AN/Uclu8PNK7Vl1TNfFje1yRdTO73wPBatfHNHcpAvefuiT+gWNlEu3v5lSWDf2Q7rPkFiyRm4w2QVqwmq7sWfcZd583bD091LYHIKNGezbBO7iSXHzcblaLs6cNwfZeW58Co5QcjZSsTDqEc14dIUY7Ox1WL/xSdgtVBoOdySqYgrAa5Ws3Ek72X01gRCWFzbawkfFCxMcO1Y3+YLF/FhoWzwrgzXxlOfhadTvJt7+Zgeq3pwvJGKkrRbOs4ZsMaPAfgsyIr5yQiIgCIiAIiIAiIgCIiAIiICF4wfGCxABAc+m6m0nbVVHZt/zOC4TiMMHUjoxFVzHEEtcAQQHdxxM2PZFjri+r27V9IuEbVy7ENcYADHT07Oox/L+6uO5hfDAshmssOm8lpDpIMci4WnYjeBFnCJupDPLeXDrfXra39kVW268uBT8cwAwFqNaIP3vwCkcVQl0DZeG4Nem3ZNlJJEexoINjb9ysmDywvcJ6qYwuXzyUxQoNbZo9eZ/RbRw1/wBRq6lskR9HLqzPgrVAegOoD/FICVcbjqf2mv8AAi/ysp2nAEbD5L6A07Cfw90qbOw09YLsIYutHSTIlmfYob0A7ydH5L6eJCLPoVB1s0geshTTactAA6WFhvK84jAtPxX8OSqT2LhXomu5Mtp1o62IM8UUjNnW/lQcSUrAB23T/dfcdkgeYAgeG11E1srAc5zfhHdHkFXlsWmufqTLac2v4JmhnzXENGoE9Y/VT2Iw720e3aQ4BzdQMgNaftkibAxaFS8BhvrGg8yAuk8J1adQGjVALDDXg27s9eVwViWzaEIN7t35v7NEb2hXckt75I2uGuF343DMxLKrAHGoNJDjGh7mSHDedM7DdXvhjhxuEDjq11HQC6IAA5Aef5L3wZln8NhGUJkNNQg9Wve57T56XBTq4TjFSdi+6s5KzYREQ0CIiAIiIAiIgCIiAIiIAiIgK7x//wDHYn/6z+IXGsF/7Op/yvxpIi6GC/b/AN4/Yr1/0vyf0K6/4vX81kpIi9LEpy1JRmwWxTRFaIQ7ZZaGyInA1Zv0Vgr/ABN8x/pciKNakcT719f9JUFi/wCzYvqIzMdTUwv9qz+8FYMm+L0f+SIoHqSM7rlP9izyC3UReNlqztIIiLUyEREAREQBERAf/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUSExMVFhUWGBcaFRYYFxoXGBgYFxcWFxcXFxcYHSggGBolHRUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGi0lHSUrLi0tLS8tLS0uKy0rLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLTctLf/AABEIAKgBLAMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAFAAIDBAYBBwj/xABHEAACAQIEAwUFBAYHCAIDAAABAhEAAwQSITEFQVEGEyJhcTKBkaGxQlLB8AcUI7LR4VNicoKS0vEVFiQzQ3OiwoPiF1Rj/8QAGgEAAgMBAQAAAAAAAAAAAAAAAAECAwQFBv/EACgRAAICAQQCAgICAwEAAAAAAAABAhEDBBIhMUFREyIFgTJhcZGhFP/aAAwDAQACEQMRAD8Ayxp1u4y6qxHofwqOaU1WMK4XtBeTnPnsa0/Cv0gugCljAgQ2o086wdI0UI9fHarC4lQL9pH2AOhIkjbmOuh5VzF9mMNft5MNiTa9rwsA4OYyQc/i6868gXQyND1FXsPxi8mzz60DPbcTgbvfhwtsp4JMHNOaxPuhHPqBQnvKzXZbjuNdhlGVGgB3YKm8SM3tDXcDlRy9cOZsxlpMwIEzrA5VKAmWe8rou1S7yui5VhEvd7XRcqj3lPF2gC+l2rVq5QxLlUe0uJdLHeW2hkYH1G0RzOs+6hugNUtyalw+ISM2Zco3MiB6mvHuIdubtyyLUwxnO66EjTL6c5IrKNiHAIDeFtSAd9dAB1/hUNw7Po4docLnFvv0zkxE8/XancK4/h8QWFm4Hy78vruPOvnzg3D7t7Kygqmsudj/AGfvH5eYrb4Dgtiyou93mbULmOaZEE5RAmSPhuKn8c1He1wVrJFy2Ls9Qt8ZsNMXAYJBMGJG+sQY1HuPSrlq6rCVII6jWsLhsErhWe4CeY7wKAsnQj738dt5amK7m8EtOzK3MNmI00GbnqYjz2qrei7aegUqyOE7UMjFLoziYzqADyGqzB3Ox5VpMDj7d1c1tww+Y9RuKvninHlophmhN0nyWqazVxmqC4arLAV2wb/hm/tJ+8Kk7On9iPU1T7WN/wAOf7SfWrXAT+xX1NRfY10G1FJjUAu01rtSEOu2xvUJAFNuX6ga5QBKyg1E9gUu8rne0AcFqKRYUs0002jSAXfV0Xq6mFmplwXnQBD3td7yrK4IU79XHSgZ830qTCm1BEhwNdzVETV+xwm4QWZSijLq4K5s0xEjy+YoAgs2yxyqCx6ASfX086M4HgpKFzqytGUiVjLPvMn00oxgE7rAXShUMLtmSY1zWiCGJ5Tmj3VV4feK2myvbENanXKoBUggHMJ9nTXlQKjdWWi3hXm2s4awMzCSYt3XgeQgnfkarY0Rccf12/eNS4S5/wANg2lB/wAPGYjMTltXdBv0zTP2SOdWOI4b9o56sx+JqUOxMFEV2rJsVzuKtIlcU9amFipFs0AZ/tNxUWrLBXAckDQjMoM6xM/6159jOLO9sI1xmVTKgnbSN9wINEOLYNy168yOqq5kEHMQTpAP2Rzbb5VnrevswTrP4GqJNtgMG8jXy+XL1rXcF7OKALuIUZo0Q7CJEuPtNtpt112z/Z0DvWefCiliOp0Cg+h8XqoovxHjeRSTqx0A5bQSfLf4V0tHght+SZh1OSbeyAd4nxi1aEk+g56HYD3EVlr3ba6AVtAKpj2gHMgROugPu51mcbjWdizEknc1UzU8+p3/AFXRLBpVD7PsPN2nxBbN3gmMvsJ7J1K+zt5URwPbi+gykIVgCVARhBnwkaD4VkM9IPWbcaHDweqcI40l7W22v2kOjCXPLmPEdRRnB4+CGVijaGQY+6fpA99eM4bFMjBlJDDUEcq3/Z/jK30htLixmHIiU8Q/w6jzrqYNRHL9ZI5Wo0ssb3RPYOzXHTd/Z3IzgSD94c/eKN3GryPhmNa1cRx9kj/3B+JFerlJEjasOswLFPjpm7R5nkjUu0Au15/Yf30/GrfBD+xX3/WqPbFYsr/3F+jUR4In7Fff9awvs2+C2HpjvVhVHSulRTEUGBrq2CauZBUikCgCumFjeni35VI9+ojdoA53dOVK4HpyvSAeqVOoqOa6GoGSRXctR95S7ygDwDinAL9r2rNwf3G+sUOscMuu0QEHN7rC2ijqzNp+PQV7N23w+IuYc9xcdWUgwgJLDMvTUEb6dK8yxPYjFMO8N0sxme8DM+51JJO+/vqlTLaJ7Z4ThUi5cu4m8Y8VpSqrGv7MtA6eLU+lBH4vdc3DYS+9tiNLrteyEHMIA0B3/jVbifA8XaUswUqCJIGupAHzIqj3GJCghDHIrHpuNakhGgXtWVtNZu2FyuULQXtmbc5Yz5xpNOw/H8MFZYcZskAqHUZSx1h0J9o8qzj8TvpGZrw8mJI9INPu8UOVWK2zLOPHbQnwi2dwAftVIR6hwvtPhDYsWhfRWt23RmZGA1nKFLKREEE66RGs1pv12zeYm3et3JP2XVvkDXgq4uyx8dtP7rXE/wDYj5UkuWNSBdEcwyv8mVfrTRFnv/cDmKcLArxDCcTvWwGt427bHIMGj4I7D5UawvbTGIAP1mxdPRwFP/kEPzppkaPVGwtUOLhbVm47uUUKZYbgRuvmN6ymC7f4n7eEVh1tXAfkM1c472zw+IsNZuWr1pz7DOhIVxsZTX5U9wUYjiPG7zMA18uqE5JkaagEdCQaF3bwJJAInUbfOAPkKWOsBYbPbYH7pO46hgCN+lVjieUDltA5eVQEEeFuF7wz9iT7iNv8VCOIYosSfz6VKbkBt+nunNHxUUMdpNaVkfxqJUoLfY4CalFuuWxV2zbqmUjTGJUNmmm3RI2aiuWqipknAoEVY4fjGtOrruD8RzB8oplxKhNWwm07RTKN8M9TwGKF1VdTo2vpIMg+hmvbcCZtoT91foK+Y+x+M8XdFoIkrOxEeIeo9oejda9+7G9oreLs+CQ1oKtwRADR9mSZGkT5Vq1mb5IRZk02L45yQzt2f2Kf91f3WohwR4sp7/qaE9vG/ZW/+4P3WpYbjmGtW1W5etqw+yW8WpMab1gdG00L3qA8b7W4XCvkvXCrFcwARmkTEggRvPwrO9qe2vdMBh3tXAVYHTMVbSGkGDz0j31geLccu3ye8aZjMNlMRrl2Gw2pOVCPVbnbnBhO872fahcpzGPLlPKY3qzwjtPh8QhdXyBSARcIQ+L2TvzrwxrnMRPv+hqE3G08jpt670t4H0iwppmvHuxvbFsNcy3i7WX0ILE5SY8QnT12+Ner4HiFq8ua1cVx5EctNqkpWBbVqlFyq2SugVIC13tI3KgD0i9AyRrtRG/UbmmUAeM4TiV1fYuXV1I0cjUadaI4Tit90J/WLoIaCS7/AGSwMxPlyoDwvFI8wdZmOmiz85ongSAt8HYXLmswB4w0nyifjVTiiaky7iOJ4iMrXg4bTUI466hlnkeXKn2uI3YGY2j62wP3YoLZ4gtz2RGVjlPUd28GPWfiKJ8KvrcVSSATow8wR18taKQxcTuKygvZtvlMwpe3yIOx10JoXi+Jo6r/AMKsliIzyBoCT7PMD5VqMPg0fadCf5GhvGcBlMJ7QClTA3PeA/KopoQLtcGwxbNcVxI9kKpHrOYeXKu3OzeEcMLbsrQYzKwExpMT1FLHYy4sEqoAPi5yJ3HSp+CYoXGueHLEMNZ0IC/+s++pWBVtdjLMCcUqsd9THxKjyqTA9iS99VF7vLQK53tlCQDmkHxaeyvI+35VoQFPTQHlG0mrPY8xcxG58S6ASdFB299NMVF3B9isDb/6Ac9bhNz5MY+VY/t/cZbroLPd21RMsAhX8QAIA8OknQa6Ca1naLtOMOFhSXLCUPhOUzrrtt0rP8Z7Y271u5beycpXSHGcEwobVYBBaQfKnuRFpo86Z1OhMfn60bxnBS1nv7LqbVsZfEcrF/aYIm8eIkAmd996a+Ktm3dtT4e7UW2KgtCXVcISpE/b1M78hQZLsjlpseYP560yJpOJcGvJg7l0m2bYgGARcVhIh02tlSIgc7jbyayVjDSuajt7E2xKC0WVhmZnZmbOyAM0THl186iw1mLI9/7xoc+KLlja7A6kA1fw2IQbkVVuWdYC+87VFawpYnllk9AY5A8z5RSfI02maC1ettsRUr2bY1JFAeHqcwFHeOYABFKSZFUy4dGmNyjdFPFWrHJxNMwfDbTtBeOk6A0OtYZswGUmei5tfPUR61o+H4Qhsj2tPvqpj1mIIqbe1dlUVufRQ4/woWChtkjMNCCZnTn6Gtr+i7iBt4lgCoV1AIJIJMyCsCJ33iqnFuHi4bCkSFzkjaQANJ5VJwbieFw1k4hrcFrmUWUeSSgOvjB8EHfSDpzpLJaSFkwNXJdHoPbW6xW0I8OfedSYPLkK837WMO/eCxOk6beEaDXUR5Civ+8oxl9sqsqqQRmcmZ0nJsu3Kay3ay8f1q6JiCP3VqcjOULt48h7pqBnY8opqAEaiY6b+nnTCCDIB8p5DpSSCx91zssn3abdTtUSM5MEfwFPDGdToeXKksxOYkfH59KBWS20Ych7zp/Ki/CONXcMwuq0Eb8wR0aDqKBr4RMkjrt9a9F7B9iC5XFYlCqe0lltC/RnXkvMA6nnpuqsDR8O4vjjgxiXSyM1wHUMAuHI/wCaQDOhgx92T6HsNxay6yt622wJVgRJ9+mxogq+Vea9oeylzC3xfwyF7BaWtgwUY6BY5oSdJ22qxtokl7PQb2MRSAzAE7SaeXrD3+HY1Ezvhz0gupbyEBtqnw/EMaLCutn9m6yjSM2WY2LSPeKSk/JOUY1wzYq1ODL1Gm+orD4HGlQSXe05iRAac6h1JzODmKsD1p+SyQG75tZPspO5BmbnUU25eENQx3zI8ca80wABEgHblzo9w3EEWnkkrJLARmIIUtBPOCYr0jheD4NdLB7eFQQCPGbYJkjSX12O1V+1XCOF2La3rZy2i2Vu6m8pY6jNq0aIR0qDkRoyWM4cti8MnitGSrwJEFkIJBgmNRqNwNwYt8L4GUxAQsVTLd7u7kLBigOhXdSQrGN9B1FWP9rcNxTJaF8q+UorNaKe05eMzKAJJ2nX1q/i+HlGQOB4QYiAGllfQ7gyp0mROhpEgHi+LvYJBz50MN7MbkEjwbaHWnWuMM5ZykxbUglZLECdCHE+2RsKKLh8NeusLhJfUnxAuoJk5hElZb2v62oG9GOFdk8EQRetgr/SqQCF5d4seyBAzDQaSANaEkJmNfEm+Mhs6llAJW4okzuRcmNKdw3DxiHtBEtuocvnd0QqiycrEMG0lh5Ca9Ms/o2wCkOgcQQwhliRqD7NWn7L4cZJe5mTOFckF/2gZTLESdGIHTSihGNtYFniVtlGQtIvBjsY8GUGQQvoaB2bj2lLKbgKYgs2Qh1zKMpXPlWVgRXpg4BZAgXrnssokggZue2+/wAT1rBfo2Qnh122DATEHMNTKhEkADzqvLk2JP8AuiyEVKkBH4c+Mvls1zO7EgMEgCGYIGa5sADFQ8S4EbIJYEM9ssuYCDDAkSjGCDEg7aV6zwy4xs7ZQGhQWIkcjPqT5U5i0TryjxHoJ2+NUwzOV1XDolLBT7PnzEqJiRsYnSf51VRZ0Hn8q+jH2Jy7a7z7j50zGrlFsrbUy6B9FJCkwdxrRPUuFJrsj8H9ngQfTMPu/MQDRzg2HzIoO+s+smouJ2AcZiLQMReuxyAh2BX4VZ4dcyEiIgnTyMER8a0KVqyyDtHMdwv3elDGwJHM/n0o/f4iDQrFY4FgD7I3pbnZc4JIiwGBlxWu/UAUAImsxw7itoNCgnnr/OtXiOK2CihmKzH5EVXkuy/CltAq8KCtK5l9DpRjCWDA395mhGNxhs3ZE92TpP49K0vDuI2nXoahbJpR8A7iV8o9nzYg+YI1+lYTjt4SijkGY/8AyNmH/iFPvr0Hiljv7qpbiYgH+0wBjpIBHvqdv0Tpcuy+LaXJMC2NPISeWgq7EvJj1U6jtMh2CMu5/sD5tVDtjiYxl4dGH7q1t/8AdVOH4prKXWuBktvLKARLXFjTf2fnXnvbBpxuI/t/+q1o7OdRSGKYjwxtr+etSI5I8UE+v51qhbHKpUutIWdDpB89KKFRbspnMWs7N91AWPwAmtFw/sFj75GWw6A/bukWwPMhvF8FNQ8I7b4vDApaZckwAwIiDyyEaes0Q/8AyZjOifG55f1p6/HyooZvux/6NLOFIu3z394ajSLSHqqH2m/rN7gK3BSvCV/SHjDrKiN9X8v6/r8aL8G7Q4i/q19F8UQWIPsmCAzGQDFNcuh9Hr2WmggyND1G/wARXifartDi0AQX1KPIOQ+NYOxIMgEH4D4ieFYq+2Itrbv3LZECRcK6ZRm0OkRyII0OlOSa4BOz3fi2EuPayWnCkbAiRoCANIjlQ9cDiUs2kS4kpZClTaR/EFEqpJnUjn1oJe7Q3bNjN3q321y5EZj7DEZwkR4gNY61NxTjpK5RdvWtPE62pynXNq8qF21g7b1Ha+iVoqX84uuHt94xu6tkIAK2gA0KQAoy5R61Dg7RdSQ6rBggjcwDInlr8jWa4rdKhbi4t7udrgyNezFVOZULhYhtjpzAoBb7TMoy5Q8bMZn60O1wWRyRvk37YRClt8omSJjkVR/qx+NQdrryDh93MRo9mB1MsIA5nWqXH+F8SW/ctYXDO1pHIRiHMgHQjUAiABpNV8Tg7rlbV607ELmuIbanK8ADLmB08TanXaqG2uWaoYIy4Ujz6/bU67zG2o1GxrVdmO2TWgLGKm7YOgbd7fL++o6bjlOgoJxHD3pJe13YBIAFsposjXwj8+Vd4Fw/v7y2zct2xqxe42VQF13O520q7tGSS2ypBbD8YxAu96W1a6EC5l2WGOaAW/5ZHimZHkRXpPCuJG2SQRljMykwp1Oqkf8ALbUQy+E6yBuPG8EvdYg3ky3hZcMNwtwK8SdzlI199bbstxYYl3RQFKpmRRIbSMwUzEiemwk70mvIf5G8a49ihfxdm1iL1pFINoAkd3L2pGVDlA8fuB0mRTOyPH8S/ELNu7ibtxDZUkG4zKzdypLb665j76MY7swt2611Wh7mUPm8WzW2mBz8HOdztTOG9hhhb9nEHFo/dWwmULlzAKVmS2m40ihNCpmxuYrWs3+ii0y28WjKy/tyRII0KgSPLTerOJ4ig+2vxFV/0bcYFwYgOQCjgSTGYEtlMnfTnWD8lbwOi3BW7k3KqAI39daWReg+AqoeKWJjvrc/21/jTW4tYG963/jX+Nebqfpmy17LpQdB8K46Ax5bUOPHcOP+snuM/SmntBh/6QfBj+FChkfhhuj7PF+1uHccRxMHKO/YgxMSZ2G+9VLue1BZpDTBgjaOR9RWw7RWBdv3btuWzOCuuURCzodeR0oLx/hv7I3IOZIJ1+zsfqD7q9XiyJxiv6ObuqToB3r5A33Ncs3p5j3morVwZSDV5MNbKglQauqjQm5FVMMCZ7wfA0XwgiC174DYe+K5hb1hd1WPMA/UGKPYXiVplyLcKj7qgIDrInKATrrUJGjHjXsCcUxSOMgdW8pgjzg61Bw289sNJMA6efQfOjWMsWkRiACW57k0HxjgAAbDl1qFXwE3td2br9Hzqz3b10qFVUCMzAANLZtzuA1vU/e0reYfimHzA9/a0/8A6L/GvMezSp3WRlb2c1ySIIU5my6CPZUb0Y4s2BW3+xILqw0z+Jl56yQPcKs3qNRox5LcuS52qTvccLttrbJ3dtS3eIAMrOx3aT7XSsT2w7KMXfEJcRg7EkAglSTAHhJmY303ov8A7QTT9g3vdtfSFq5g75dXy2SoIIDFmIzLFzLrp7KsdqstxVlLPPG4GylQCpBOsBp9dVAj31Lc4D40bMCAddG5bASvWtx+08vj/Kq2KsXXiCumupnlHlWb/wBMiWPbu+3Rh7HCLoMm20T+NMfgt6dLbR7/AOFb3Nf6j4imFsR1X4in88iBj8HgreaDctCSAc1xVKncyWYADQiTpV/AYJbr91YYPduNCEMqsCGLNkIaNQN55VoLNy8iuvd2mDCCJgeuXYnU/E1Tu2b7XbdyETuzmUW4GUgEKRpuJqSyonHa+wVxLhGQJh7rG1cJUgNlg7DckADbUnTnT8JgrdtpaHEyQUDgwuXedV9KPcUvNdYkoCM0qHgwCIj2Y6Gh16w2UqFUZhGbxEgwZOg01PypvM35JY1iT+9/odbgo1tA2V2LkJCjbLAVdIgkRFSXMCjObrKxZmLHnqQdIjbX5UO4dwy/adW7yQJ8JDQQRBj61oE70/Z+R/hVc8sr7FlUE/o+CnZhTPdhpmQ9osfU9dTNNFlQAO4saD+gOvmdN6Iw/NT8K4Q/3TUfll7Kj1C1xXL9jWOtAcXYZ5JPi1hhIYCQYmddVEjnSbjuG/pJ9Ff/AC1z/bdjlnP/AMbD94CtFl4CbsuTcdzeuZXIL2phGP2sygwc3PTWpV7KWf6K3/hFFbnHLI6/+P8Amqt/vPb+zauHz8AH71NzvtioHX+x1phlFpUBBDFYBYHl7iAaEdlf0fXbGIS7cvKQubRMytJBA8QMga7e6tUe0Ohiy08gWifeFNNXj9wajDfG5/8AWoqaXkJcpBX/AGYvMTO8kn610cKt/cX4D+FCD2jxH/69sdPGzfQCm/7wYn+itfBv81LfD2AbucEssIa2pHoKhTsvhOdi3/hoM/aXE/dtj+6f89M/3lxH3lHog/GoucGBoD2Wwn9CvuJH0NNPZDCf0ZHo7/5qAjtPf5t8AB+FQXO0V8/9Rh6H+VQuAcGiPY3C9HHo5/GaR7G4frc/x/xFZc8avz/zrv8Ajb+Ncbi1473bn+Nv40boehcGjfsbZ5NdHvX/AC1iu3Qw2EjD5rty7dXQSuVAdAX0kzB0HTlVu9xIgS7NA5sxP1NedcWxfe3xd5G4Y9Nl+QFatPijNOVdFUpJNJA5zlMHlt6Vbw9+Kixls1TFwipVZddB7u0ff5VcwiW0AywfM1mFxhrq407VBwssWVGhxF/dp6+6ouFr3jydVU7dTv8AL+FDcPbe6YGg61qOHYYIFVeW9RdRJRTm7L/DeM3biKbVoMgDgB7o0FyC4IW2p1jrXFwl3+gsD+1dvH92Kz/ZvHdyzjdczL8GMH89a12Gx6OBB16HeennVmow5YfaK+pjWXmm+SO5+tMACbHhEAFsS0DTQTe8hVrDNdUQe6B1MqH3Iyk+NzrlJE+dPFSok1heaTJdkQB6mpLfnJ9TH0qZEFSZQKqsltIGidFjykmlp90fP+NWGqMsaVhRHkH3a7k/qintcjSfWuFjEzRbFQ1EjUKAakEnU1GX8zSz0WIsa9fnTcxpgfpTWY0h8Dmb8xXAx6UzPHOu56BEbx9xR/dpqEfdT/CK4VI8q6UAHM1MtYmxRG0fAV39dPX8/Cmq4G4+MVxz8TQIRxp6063jCevxpgB6fKnhG/MUUKhxvP0+dRPcapCpjX5mPlStc/5Gigog78/n/Sud4Tzqymp/jrXXtToZoQqKmY+XwpMp/IqwbY5T8agu31XzPTlWrT6XLndQX7K8mSONfZjchofjcaFUkHQAktuNN8o+0fPb1p2KxJI1On5+VAcexfw/eYD4eJifcIruYvxWLGrny/8AhieplJ8cEGPxzFQGJk6n3jQe7b40F3EfCil7CPcV7iISlv2m5Abe/lpQhtDV7ca2oltkuWXrbZhrvzqC9h6SHWR76u2jIrj5oPHKjpYmskQYtir+FwXUVJ3OtX8INKolJl8MSssYSxG2nU/hVrF3xZtM/QaetctuIrOcdxpuMLY2BqOOLyTSLckljg2RYEkKCdzqffRbCXSJjXYx13Bg8jrvQ2yNhRHB3VVgCfa8M9J2+cV6jHGopHnJO3YewHFIAJOZOvTycD2T5jTyo3axIbYx+PoaxdrMjGPaHtLyYVfw98broOa9KozaDDm7VP2gjnnjfHRrs8fa/GomxA50LsYydD8edWIPqOtcHVfjsuDntezdi1MZ8eS73kiZpoMGaq610Metc8ussXG18q4jDUVGzxTCec0UBIx5V1W5VA5pobzNFES0G6GnAaaH1quH50/voooZ01yDTluA+R+tMLeVAFiFXVt+VQZ1mTA9/wCBqgHnUmlA5D8/CpUS3BB2TfNPvphvr119PppVM2zUgtwNTRQWE7T8/qBrTrhEAzHw/GhMAnQ/wrt1NddfdRQ9xfZl5n5g0jdReY9ADQ1XA6U5TrqPwooW4tjExtTnxQAmPeRVAjWc2lCMVjpJjbYfxrfodKs0/t/FFGbK4x47C2Jx5bQTVG49UlxNNbEb16mDjBbY8I5jjJu2SX7sUV7N8AF+2b1w5bfiGhgnWG1+yIWJ9dt6zt65Pnpp1nyrW8WzWrNrCTARFzgc3Opn3kn31lz78jWPG6b8+kasOzHF5Jq0vHtlXiuPtm22Hw4AtgFSQIEcwo6dWP8AOvPsTag1rVXlQXjGDYNmAJDdBsatWihgx1D9lMtdPUZLn+l6A9t4ovgFVlZpgplzdMrGJ9xKj+8KHnBvOqkeZq1w3Dm3dDPJXVLi9bbaMB5xqD1CnlWPPhc49GnDnUJdhXD4dbgJRpjf89KcmDINMx5XD3VNtMsSHj2XQxlIljJjxTpuNKJXbyxmB9K5GbDKNNJ0zr4ssZWrVr0R8QARIEE9P51l7liLzCZyxryJIBJHlrR5kLGSCZ2A5eZJ0FRcUweWLirMwGA8tj8NPcOtdXR6FwW+XZzNVro5Hsj/ALKCrFEOAX0TEWzcAZJIYESCGUrsd9/lVMqTplINS28GwKsTz2j8a6DipxcTEsmx7l4D3bThHcFL1qTabVTMwY9knmCNR6HpQwOCouLsfrzFbbgOLt3rRwuIg230UnTKx1AnlrqDyNZPjPAbmBvGw8m1dk2bnIkcj0YaAj31lxTlin8WTvw/aLpqGWHy4/2vTOWcRRDCYyDvWeN3LqeR1/Grq3IMfCtu9VTMrh5NI9wEZh7x+IqLP5n4TVLBYiNDsd6nggkfPrXnPyWljjnvguGbtNlcltfaLguSOXrTGY1HZuax+FdYwd591cqjWSK/nUbH8xXFc9PlSI8zSoVCDedSBgeYqJ09/wCPypKJooKJppd5FRFo5V3fkaAKgtmJmKntWhvm+tctt5fKulxAHx51MQ+D6fnnToJ5n5fSkGH5/mad+sDYadTSJI7asGZ19+nyqO+uvPyqZH1iNB1/jUDnU6jr60DZF+rRrr8adbgGINIOT9r4D+dIx0JoIkHFrmW2WG+3x/lNZbvKNdqMQIRB5k/QfjWeDV39BHbiv2ZMvMiwt3f3U03TBPn+frUAb2vd+NTYDDm7ctWl3d/hrufIRPurbvK5JJG47EcHRbb8RxOlmzJtg/bcaSOsGAOrelQlbmKusRlDvqQZhZKqFEDUyyj01qx24xoAw+AtaW7eTMOpjSesLJ9Wor2Y4d7N1WKqyQWOn7TvFYgFlIIhY0k+nIhL44vK+30Z3k+aoLoB4fgbNoHTeNA3LQxmUDTQHXQxRTH9mFsWTeuMxgA5SmUSzZQDDEnlO2+9brC4bvAqoMgyksygMp8XiCmSGJYM3i2mh/HbX6zZdMpQW53UiRmBXWOqmT5jSqVrck5JN8Fj0kFFuuTypkBGtVGs8juPZP4UQvIVJBiQYMGduhGlVLh6126TRy02mTsou2wjQHXRCftD7hPJgTpO4McgDQ4cjGcwgIYE6a9I8qZexkDLuToP9OfKp8WpS1A0Og05a6j61knig5e0uTZHLKMPV8Fi7iQAQsZo0nXXlIH4xTcJaJMsSx6n8BsBUWBsabURRIq9Jy5ZmclHhEIsgmYqY2h8KfbQnQD8xVpMONAbiAkTqy7e8jqDRLLix8N8hGGXIrS4K+EPtL7613B8Zax1luHYv2is2Lv2pHskE/bXkeYkHzyl3DNbYPBK6SfIgGfnUWIOV1IMEGVYcuYNRzYoajHx2umLHlyafJ/ntAfjODe2z27ntoSlyNsw+0PJhBHrUFjESLZ9x91art5ZLNaxXK+gW507xRofeNP7lYnCPsPuufpP4VgjNtcnRhJTjaDGDvT7mP4UctEMoPTzj871mOGvoT1Y/KjXDr8gjoT585GnvqrWQ+TC0Tx/XImXhpzPxFPHi9fKmvd9PKP9fSl32o+deYo6R0OdgPxpyXSTr9K44I5wPX+NI3NRGvTlFAyRLgO/0iuG51E+6nW4E5iBppv+O9PRJ6x1+lAUQKPSOhrmv5mpMupn4dPxprzOn40BRHatzrp/OpFsA7gR8AK7SoEkWDh0EaDTXc7zSuMsEKCPp60qVIkcstqdQfIzHrFRYhROnxHX3UqVMTI2Ro0HxpyppuJ+XpPWlSpiMh2lvzeYclAA+An5k0MR9x5fj/OlSr0eJVCKXoyP+TG59D7qP9jIGJVz9i2SPVoH0JrlKpT/AIlGp4xsffxXfYkuf6zfHb4SPhXpvBRZu2rKNezOqjNNwhSmZRky7JByjTxHLHOaVKteqheFP0ZdM6ml/Rrb57q4hWVTwqFAhdSBEDY6LB2gfEFxuybkXLpUoFxEgSAFggajl4QfU+lKlXIhxJHUydNHlV5tTG0mPTlvVHGvGlKlXpn0cBLkgwVicQq8lEn1/wBYoxxO1KEedKlUYJUyWVvdEq8Hvz4T6GiV3QUqVTh/EryqpjcXiu7trlLBnk5h92BIEGQdQeR0OuuhDhnZAXLSXXvpbLEZEgO0N9q5qMqxr6QYFKlXmdTlkrl5s9Hhxqkiv3VzCXzh70GTGplAHMh0P3YPw319nnFMNp4d129P9Z+FKlXR/Hze+vaOd+Sgtil5svNc7/AOnNRnXrK+KPWQw/vV57mhnPKZ/wDFv40qVRnxlkv7KdB1JFjAGLY9JPv1ohwW+ZJ/rfgKVKm+jUw2F8vifpTkBJ2MdNtPSu0q8tLs6a6LMArPiMddhUGboNfn60qVRJHc86MJP+ldzsDzHX8xSpUAPkkTHv8AnrTxaPUDyM1ylQB//9k=</t>
         </is>
       </c>
     </row>
@@ -2155,115 +2155,115 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HARDIK PANDYA</t>
+          <t>ATHARVA TAIDE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ipl2023_74</t>
+          <t>smat2022_135</t>
         </is>
       </c>
       <c r="D14" t="n">
+        <v>29</v>
+      </c>
+      <c r="E14" t="n">
+        <v>22</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>131.8</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="n">
         <v>21</v>
       </c>
-      <c r="E14" t="n">
-        <v>12</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>175</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="X14" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="n">
         <v>2</v>
       </c>
-      <c r="L14" t="n">
-        <v>25</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" t="n">
-        <v>14</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" t="n">
-        <v>1</v>
-      </c>
-      <c r="U14" t="n">
-        <v>1</v>
-      </c>
-      <c r="V14" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="W14" t="n">
-        <v>18</v>
-      </c>
-      <c r="X14" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>17</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>15</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>22</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>15</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>14</v>
-      </c>
       <c r="AI14" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="AJ14" t="n">
         <v>0</v>
       </c>
       <c r="AK14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL14" t="inlineStr">
         <is>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxATEhUTExMWFRUXFhoVFxgYGBgXGBgXHRcXGBgYFxUYHSggGholHRgXITEiJSkrLi4uGSAzODMtNygtLisBCgoKDg0OGxAQGy0lICYtLS0tLS0tLS0tLS0vLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPIA0AMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQIDBAYHAQj/xABAEAABAwIDBAcGAwYFBQAAAAABAAIRAyEEEjEFQVFhBhMicYGRoQcyUrHB8EJy0RQjosLh8TRic4KSM0NTY7L/xAAbAQEAAwEBAQEAAAAAAAAAAAAAAwQFAgEGB//EADsRAAIBAgMECAQEAwkAAAAAAAABAgMRBCExEkFRsQUTImFxgcHwMnKRoTPC0eEjNPEGFDVDRGJzorL/2gAMAwEAAhEDEQA/AO4oiIAiIgCIsDa2L6um4gjMASJjUCYvbQFAZOJxDWNLnGANVom0fa5suk6MzniYJYJLTeQWnuXJ+l/tBxNbraLKjuqeZgiHNIIMNIMgSPVaJBKA77i/bfggYZRqvEa2F+BBPqojDe3U5jnwstkaOGaN44SuN5eIg/e9eFg4oD6l2R7RNmYgMLKwbnMQ7slrvhdOi2qjVa4S0gjkZXxdECVsnRXp7jsE8GlUzMmXUnXa7QG+oJA1CA+sUUJ0S2+zHYSliWCM47TfhcPebPIqbQBERAEREAREQBERAEREAREQBERAEREAXEvbh0jId+zN7J3kES4HQGDI03jguxbUxXVUalW3YY599LNJv5L5J25tWvjq7q9SC950EwBJgAeKAwKFEkrx78vP9FK4PZVX4fDesXHbKqtN2mJXO3F7zt05LcRtSoYjgf7K3nKn8BsF1QSBbf8AYWWejDgPDX9QuXVitWdRozauka4SSL79FjzCn37CqDWywa+y3ibL1VIs8dKS1Runst9orsAeoq3w76mdx1LJEHKBxIHkvovZO0qWJosrUXZqbxLT9718WvbBXZfYj00qdezA1HS1wOWYABAJhvEnnwXZGd6REQBERAEREAREQBERAEREAREQBERAal7U8YaWy8UREuZ1Yni8hv1XBNl4BtNrXHVwnu5LuftXp58CGfFVZPgS76Lk+Jw3uDgwd2pUNZ9ksYeN5nuHfAsFKYTBl05gIPEfJU7MwbTGZbPhaTIsqKVzTvZEGzBtaIa0DwUfiaZC3BlNoklQ+0204da5Igi0DfbQ3XWycqW41PFQQo6sBClcVTF1D4oEGF7E5ma5j8J2iQr3RbFvw2Mw9YCSyqw94zAH0JUhXpyqcBhgajGne4DzIV2Er5GbUhZ3PrRrpEqpUUhAHcFWpCIIiIAiIgCIiAIiIAiIgCIiAIiIDU/aIyaNP/U/lK5VjmZSAeEd67B02o5sOD8L2nwMj6rjuMwD61ZzqjsgEtYAJgDQ336KGta2ZYw7e12UZuzGWsRO662ejhH5ZHBaBX6N12kOp4l87hb0UzsXa9ak4Ne5zjpeVTtFby+pTeVjaP2Oqdx9VBbX6unOeqwRum/ks3am26uSJIGoiy07E4JmJOZ5hotJMBe9nTMNzWli3jNo0dzwVE18Uxxt/Vbdh9kYGiyWsYTvdEnzIULtTAUKk5QGu1BEBdLYT0ZxLrGr3RE5PJeYQAVGE/G35yr1OiQMp1+aowwz1qbeL2jxJhWYZFOpmfUtPQdwVat0RAA4AD0VxTFcIiIAiIgCIiAIiIAiIgCIiAIiIDUOnG1Xs6ugKQeKsS4mIh7dLXjVcr6T42pnPVAklx8pNzF4A3C5XWem7ezTdaWioR35N3z8FzzCYBr/AHt6qVp2efvJfqXsPBNXWtvV/ojWsds/GOdloVDUpFrHFz2tp5TpUGRze0NIvoFICgGixJbmGQujNM6ENkeRjktpZsmnvl3IkkeSi9sU29YxrYsQYGgUc6t1axYhR2Xv8yx0we5tFngDHCVi0sG1zKZbJa2JaASS7fJBBA/LB5rK6UOOQA6LzotUBaW3BG8X7pCii7Eso3ZB7a6P0n1+ta5rGl4eaTQ6nFmgw73hIbpJ81hYLC1mOJJzNmxiD5b+9dFqMBs5rTzUTtSi0AwIUkqzlqQxoRjmjWMQIdKiu2zEMyOylrxUDrGIIM3t/dStd0ugKL2u1xeMupblPHiR5fJT0m9i5WqxW2kdB9mO1q1TaLnZj1T2uYZuXuAzBxJ+4XaVx32V4M/tdoyCmKwjiQWfJdiUlH4SPE228uHv7BERSlcIiIAiIgCIiAIiIAiIgCIiA1/pnQzYeRq0/MFp+a5rgK8dnQjXuXW9t0M9Co3i07p0vYcbLjGOqZDm3bxvB10VXExurl3BztKzNnbUGW5gALWzi6XWtc8uHauS0hk7m5/dnlKwsVt5rRD3eA17lCYvadV7z1RIBjstuXEXmFXhTcmXKlWMVr5G09KNpYaWCCc5hrB2nGI0H10uo6jjSMRSNNhY4H95cECn+IPLbTpaTdQb8Bi6hcOre1wJHu5IbA3mALzYclZZSxFA5srhYzfNNjcgHkperSWuZF1rbzTt4fsdRrYymWgixWubXryFreG6TuJyVm5eDhuV3E4p1wSo3TldJkiqxcW0eMMOk7rqLxTiYymHPqBo3kEtcCRG+DpzV59YxNxqtg6EdFv25xipkfTGdkiQYc2XTuLTljxVuMbRsjPlK87s3n2KbPc2jVqOBFxRbOsMnN6ldMUdsPZwoUW082YyXOdpme4lzjA0uTZSKkirKxDOW07hERdHIREQBERAEREAREQBERAEREAXG/aJh+pxpJEMqAPndrE/8p812RaR7U9kdbheta2XUrnj1Z18jB81zJXR1B2ZxFmzXuqPcW5srj2ZyzxIMc/FbPsHC5/dq08ML2cC5274bX5u3KM2fje12r5reI+hss12Jp0TLjlB37teAVaTzs1c0aWxa97d+X6G2Yjo7Rgh+0pAbmGVrQSSCDEl0+6LarXdtYfZ7WnqziS6acOLgJEEv7J3zbTuVdfphghFPIC4iM+W2+/fEXha3i9qtqOAZJuL8iYsFJnuR5eG+bf09CzS2MH03Oe4udHGwI1dH0VvGOl2We/y5rLxuODWZW6b+/v81AU6xLi71tMLyKbzZDUcVkjKxLo7IP33roHsTqn9sc3cMOfMvBXM6tQTH33LpnsOE4yq7/1OP8TQFMlYrSd2dvREXRwEREAREQBERAEREAREQBERAEREAVFRgIIIkEQRxCrRAcO9o3RJ2EcalITQee/KfgPfeO7ktcaWVWdXUEzGk2gW8AvojamBZXpPpPEte0juO4jmDdfNOMbUw1cseLtcW74dBi/BRzhfQmpTs89CzjOi1YHsdpsyCDuJ4HlCv0NmGj2n3cARb9d6y6vSM5YdeRcyZERlE/e9Qe0ttl++IEffJc2lLI7vCOZZx+KsYi+ketlHNxRAhWcTiC91vvxUzsLYWbtvEjcFLlFZkKUpvIs4DCOcczhA3SmOxz2ZhTc5pdF2kgyOBF1sOKpZQQsDZmzg5/XPFh7g4n4j3bufcu8HRqYqt1cP6LiyTEbNGldnYPY/tis+l+z13Fz2Ma+XGXCTBBJ1iy6Uvn7Ye1qmFrtrM1FiDo5p1BXcdibTp4mi2syYduOoIsQVp9K4N0Kt0uy7crfe1zPw1XajZ6kgiIsoshERAEREAREQBERAEREAREQBERAFw32lbOaMXWFodFTzF/GV1PpV0jp4SkTINUiGM3k8TwAXGK+LdVzPeS5xJknnf6qw8JN4Z4h5JNLxvlfwWQp1F1mxvsatX2ESJaTBOm5Yg2Cd5kytqbiIblAvPj8lXQoXkrN62S1L6owehEbK6NyZK22jgMjbCLKvCNDRP34L3HY0NEak6fr3JQp1MTUVOCu378kt7JJ7FCG08kQmMpBxjd8+SoXrnSZR7g0FziAAJJPBfoPR+Ap4GjbfrKXH9luPm8TiJYid925cP34lQBtGpsBxPBbNsDbtfBFzGuD2kzkI7PeDrf6KA2W0j944Q4+40/gafxOHxkbtw71kF153yZ8UqQWJfbXZWie/ve/wXfd52tWdRwyjrx9F3d+9rLK9+t7C6XYfEQ0/uqh/C42P5XaFbIuAMeQtr2B0yrUYa/8AeM4OPaH5XfRYmM6Ice1R+nv1LVHG3yn9TqiKO2VtejiG5qbp4tNnDwUisSUXF2azL6aaugiIvD0IiIAiIgCIiAIiIAtD6VdNcpdSw5EizquobxDOJ5p7RNv1KcUKZLczZe4awbZR5GVzHEVdy+g6K6LjUSq1VfgvV+i82UsRiGnsR8zzH4t1Rxc4kk7yZPeSsRjzmt7sdrlJgHzsqnKkMlrje72Ux3jM8+jVq9MWjgprdZL7r+viiPCL+NGxcpgF19fVSFMAKxUw0hr+SuNqBrS42AEkmwA5lfnmxKpJRis3u9++OWZ9PdQi29EZL8RlH0UbUJcZOqtVdo0Sb1Geau03tNwQe4gr73ojAUsJTsmnN/E0/su5ffXgfOY3Fzrzu01FaL1ffy50PLWgucQGi5J0UVQxJxFQOgigwy2bZ3DRxHwhYmJqOxdXI2eopm8fjd+nBTVPDwIiNw5K3Tk8VLa/y1p/ufH5U9OLz0WdZrYVnry/e3MmadOArIdJKt7OxcS19wNDwHA8l5RMlx3SrGy03cqNWdjIXrASqWlXGLlgzcDin0nBzXEHiF0Lo90ua+GViA7c7QHv4LmwVymSFl4vBQqq+8mpVpU3kdzBXq5t0a6TvpEMeS+nwPvN/KTu5LolCs17Q5pkESCvmsRh50ZWl9TWpVo1FdF1ERQEoREQBERAERYe08YKNJ9Q/hG/juXqTbSR42krs597VnUs9MtdLwC144DVvjr5rnZUrt3aXWukmRJMnVxO+FDvrt3XX3mAoujQjTeqMmU9uTla1w87vvv7lnY3CGlSoAiAWPxDrX7UMYO/LPmo5rZDuMH5KX6TYprqYLdHCm1vZy9kNze7x4853Kh0zGVWdDD7pyz8rX/6uT8Ui1g2o7c96V16fexH1duANDcrgAALMk6fFf0UM+q+oczgGge7m7RHc3TNzMq5Spu03LIpYfMY3b1epYChSX8OKiu5JPzer+pFOtOfxyb8+S0X0LFDBh+6G73G7ncp3eCyhsmj8A8LfYWcGgWGgQqx1cdLL6EDmy1hMKxghogfVVvVZ+Ykcxe45WKs1F3FHGpbp6krJpmB36q1Rar4ZJheyYlmZFNkrMp0lZwRk5b8fBSJbAVOpKzsQvIt06SuFiuNavH6qHaueGOWrZei3SU0DkqSae8728xx5rX3hWnWuoMTRjWpuMiSlUcJXR2ym8EAggg3BGhHJXFz7oHtwseMLUPYdPVE7nalncRcdxXQV8rWpOlLZZt06iqR2kERFESBERAFovtLxR6sUptZx5kyB8pW9LmvtMf2/wDgPGH/AKrR6KgpYqPdmVsW2qWXFHOsQwETH9lhug6eZ+ilsFTLnQBJ0AG8mwXvSHYRoZXNcHtLRnj8D7SObZIg8+YX2XWxUlBvN6GdG7IrDvvHkqMQ4nK28NJH8R9IhVU6PFSVCi0CTBJXVSMXKMpLNXt5q3JnSns3S3mFh8MYlZFJmUcysus7snS9v1CxyV6pORHe4le0zBB4EHyvqq8PhnPMCAN5JAAAiXHkLKgVKFpqkE6kMMN7+N40VKvjaNNuDu3vSTbV7620vZ242ss2k5YUZSV9F3tLn78syUfj6VWqx1RoawNa0wJM2mSNQDMA7lD4oguJaCATIBMx4wFfrUYAcCCwiQZGbUi7RobKwRdcYClh0tqg3ZJRtd2Vm9Fxb1bu8tTqtOd7TWet8s7rjyDQrzNVaYrjD2jyCvyICR2W33j3D+nyUi7tNg+B/osHZ9qZPEx6Afqs4aclRq/E2Qy1KKLpBO6THPmlf3mcz9DvVeHFlRUBNVnJr3fIfUqNvMWKnhWXhX3CyoriGk8O14DX0le3sEWKUkgAw8EOpng8XYfOB4rsWxscK9ClWH/cY10cCRceBkLjjhFxuXUuhLgcIyNJdbgS4uI7pJjksPpSlaz7+Zo4KebRPoiLHNEIiIAuS+0Nxzvn/wA3oGj9V1pcu9qNGKk82u8wWn5LW6FdsTbu/QqY1dhPvITo9TDch/HVeWg/C1rZce8kgd08Vc21ULhXG4GkwDlL3n5DyHBU7KpkvogEAU6kuJIAazKwlxJ3dlw8QrWPcM9Voe1+Z73S29rhk+BJ8lv2vW2t9r+Hay+yKV7Q98P1IAsglW85B92R8lk12w5XRQEStHaS1I0YsmAfJVgKqpE/fiqXLy4MnEUHvfTw7WgkkOGt3PaCC4aiGjQTpK2DEdFsL1buqrudVZSLw93Za8gSWNYRIsFA0cYMPjKWIyGG5agBJGYZYcQXGYkmJU/tjb2FbTcMO/rqlSmWyWFvVF3vuvaYMACe9fEVJV5dX1eaecm+Lzd83bN5ry3GvFU1tbW7T04EBsYy17JGUhrg0xJIgWJP+Y8bBYbTY2jlw5LMwrTSokmAagBYZ7QAkcLA8eXcsYt3L6DouOdSe5tLxsrPT1u++1kUcQ8oxe5ep6waK3RN394HoD996uhYtKpDqgO5wP8AA36rWvnYronWe5THxOnwufqpIqN0NDhlB9ApCdyoz3efMgYp6KzRd+9eeDWjzk/VVByowd3v5nvsPoubZNgyq7OzPE+v0KNbLfn9V7jPdjdP3/dXKTbKO/ZPCGwh1adWksPhofEQfFdA9meIJp1aZPuPHqNfEQue4s5MRyeP4hb5R5LbugWJyYstOlWnH+5vaHoT5Knj4beHb3ot4WVqq7zpKIi+bNgIiIAtI9puCDqTanfTPjdvqI/3Ld1FdJcIKuGqsPwkjkRcH0VnBVeqxEJ95FXjtU2jm+D2fT6plR1NpL8zg57uyBmOWGD3jEWPBMdXptD6eYSQBDKeQbspJ3iL85WDRxfVX7TiWtDbwLEnykDTdKxKuJNR5e4AE7hpYAfRfUKhOVRubyWa8b3tZ3tbutojM6xKFo++RhY1l1R1gAidPqsjGnQcvqo84fymTO9aUc0rkSKmum6qKNXsLpgqDab29XUED8DpsyXAulo1BuZ1sIhXaWFoh3WPq9ZLhaCMzRF3SZGseBvdWIXoWZV6NU5uUZtJ3uvG17N5q9lkrK+euZZhiNlJOKdvTTxtfK+7LQuV6+YiwAEwBoJO4bhyVs/fqqXr0q9TpxpxUY6EEpOTuzxRG0HEP/MwebSR/MFLHRR+0afuO4Og9zrfOF29z4e+VzqGTJuniM1Gk7e1rQf+I/RS9N0rWcA8gikfxUzHe249JU3surLO6yr1IWjlu9SvJZmRTPaPL+692QPed9yrZPaf+U/KPqsjANimOZUU/h+h4y/idG+f3+iv4bRWa47Q5ffnzV+jv+/RV38J4RPSSh2A8fhcHeGhV/YGJ/eUKg1a9p8Jh3oSszG0czHDiCOS13Y9UsdB/CZHgV4o7acHvRJF2z4M76is4esHsa4aOAPmFeXyRvhERAFZxRGR0/Cfkryjtv1MuHqH/LHmQF1CO1JLvRzJ2i2cd2g33eNwfBx/VYzDAU7isB1gquv2XEiCAJI4Re45arG2fs4VKLnxftAGXa7oAt5r7D+/UYxe09JRi+5ys1zRkww9SSVlqm14LUh8V70cgrNQrc39Gg6TDJ4xUHyeR6LX9t7KdROhjhIPcQ6BI3aAg94KhwPTeDxclTpS7XBprmT18BXoRvNZESgWfiNlva0ukQBNw4SIk5SRlPnuUdK1KVWFVXg7laUJRdpKxUqlSTGvrb0KpqXGqkOTx6BW2PkQdQq2FevQ9KpWPiWS0hXnqh4siBH1X1AWPaCTTIJjiSG+RstjwByVn0yIzdofUffBWdlUQA7MJDrEbstx9SvK9FzIglzmHMwkklzN4k3MKvLObjueXmcTaeRKfif+UesLPwzYyDlKwMI4Olw0cGnwgKSpi55AD7KrVHu96IiPG3cT9x+ivA3sCTwFz6KSoUmUKNN+Rr6lXMQXiWsDTEBuhf3rM2dimuHXOYxppVKeV7GhmbM7K5rgLHsklU51Xa6WWnne3P1drImjSTey3nrpu15fu0YVLZNdzZyZQdC4tbPcHGVqO2cE+hXIc0tOsHgd4I1HNbztfZdQ1nl76ZGY9ovFhuaW6iBFgofpFUpOg5DVbSpMpZiSCRmhz2jWRNp8VDGtLKSz8N2m++eb0diXqkm08vHfrut3G6dB8b1uEZxYSzyuPQhbCtA9mOIymtQJmIeOY0n1b5rf1j46CjXlbR5rzzNLDyvTV/dsgiIqpMFD9K/8M/w+aIpsP+NDxRFW/Dl4M0rZnu1vzFWejv8A0W/6v85XiLvHfDivnof+Szg/hw/y1OZlYlobVpFoyl1YBxFiROhI1C86X/8ARHj8moigh/iGE+WHJna/Ar+MvQwNs/4EeH1Wm09W96Ivpf7P/gVf+WpzM3pL8aPyR5E7QxNQ1nML3FuY9kuJb7w3aKP200DEVQAAA+oABYDtbgiKXovf4fmOcXqvLkRf4vEqsa/fFEW2Ui5iNfBUFEXC0OSWo6N/K35Ji/wfmCIqyId5k7K0Pf8AzFSlH+b6Iir1dWGbh0OptfQeHgOAqWDhIFhoDoo/p3apSaLNDXEAWAPGERY1H+c83yReqfyvkuZjdKv8S/8A2/8AwFFuHaHeR4RovUVv/TL5Pyld/wAw/m/MS/RlobtN4aAB+ztsLD3Wbgugoix8b8UPlRrUPhfi+Z//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTExMWFhUVFxcYGBUYGRgXGxwaFxoXGRoeHRUbHSggHRslGxcWITEjJSorLi4uGh8zODMtNygtLisBCgoKDg0OGxAQGy8mICYtNS0tLy0vLS8vLS0tLS8tLS0tLS0tLS0tLS0vLS0uLS0tLTAtLS0tLS0tLS0tLS0tLf/AABEIAOEA4AMBEQACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQIDBAYHAQj/xABGEAACAQIDBAcECAQDBgcAAAABAgADEQQSIQUGMUETIlFhcYGRB6HR8BQjMkJSYrHBgrLh8XKSwjNTk6KzwxYkNDVDY3T/xAAbAQEAAwEBAQEAAAAAAAAAAAAAAQIEAwUGB//EADURAAICAQMBBQYGAgEFAAAAAAABAhEDBBIhMQVBUWFxEyIykaHwFIGxwdHhQvEjBhUzUsL/2gAMAwEAAhEDEQA/AO4wBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAsY7GJRptUqMFRRck/Dme6Acf297W61SplwarTp3tnqAMzcr2Bso521Pb2SXwWSNJ2lvrj2JzYusdeKsUHdYJYCEGNke0DG0WJ+lVjpoHOfmPx35S3BVnQdg+10gD6SgqKLZqlPRkvzZOBGnEQ4+BFnU9nY+lXprVoutRG4MpBH9+6UJMmAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAcV9s29fSOMFRDNlYA2+9VYdVR+KwJv3nul1xyDS6O6WJKg1Ble3+z0uB398zS1CTNkNM2rsxcTuhiwLqL93C0hamIlpZdxgYnYtdB16d/WXWeLKPTTRHsrUzmAtbu/adFJPocXFrqdA9me+Bw2KC3tQrFQ6DgGbQMq37bXtyBlmUPoeVAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAQ++G0Hw+BxNdPt06NRl8QpsfLj5QgfNO7tZnxlNmJOW7C5v1u3x1OsrnfunbArnydloWqMWtaYZPcz0IraqJ0YdMui+cvtjRy3SvqRWMwaG4IHnOLR3TNA3n3eplXIFjrLwm0ys4KSOZ06hRiOB7RoQRzvPR7jy6pn2BsfEGph6NQ8Xp02N+1lBP6yCpmQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBALWKoLURkYXV1KkdoYWPuMA+bd2dgmlisTTcjNh3NO/Lqswv5gCcs7bSRq01W2bLht5qtMn/AMs5pjgRxIHPsnBY4+Joc5eBuGwt5qGJByq6kWuHFodIhRbIzeHeqlSbIlN3fsUC3qTKqKkWcnHzNdTH1a7ZatLowb2Jtx7D4w4R7mTGcu9GhbX2MxxhoKOtVcKvi+g95E2YncTDmjU+D6vwlAIiIOCKqj+EAftLHEuwBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBALeIayMRxCk+6QyV1OHbJwxavXZiS1VUzkkm7C4Jue7LMkpNwPS2KM3Rfbd985JNXLmBBQ6kAEFCPwm/HlpIhNLuJyQcujM/ZOzhTr58uXMT1L3sDwHlKSdl0uDGr7FDVajdck5gMrZWW/Ag90mElEicdyPMNu+ytmObLlUAE3NxzPeZWc7ZMY7V1ITGYYjH9MpOdAuQjSxGha/aBb1nV5Go0ikMUZTbkd+wblqaMeJVSfEgTWuh5klTaL0kgQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQDwi+kA4ztwPhsWqNYZVYdxGhU+Yt56TI4Umj0lPdUvEn8JtVMvEcL6mwnBHeSNfq72UUxAVrHX7SkEeBE6bH1Kb49LPMPvhh3xOVCAL6sdB6+Mq8cupO+HSya2rtRVQkcvSU7y9cGv7obMfF4hrXK57s3ILoG1tz5DTWaFC2kZ3l2wcjtwE1nmnsAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBANI9r+CL7Paqou1B1qHTXJqr+QDZv4ZDVovjdSORNj+loBQ1jdRfxNv6zNtqVm9y3Ro27dPYlJVIdgzr95VQX77MfDnHxF6aS20YW9+yKbA9GQpALMzKl7AHQZefDnIXusmcbjzRq2P2qUw9Onck5bsfHlJjG5NnKUqikd73A2WcPs/D02BD5M7g8Q1QlyPItbymlGCTtmwySogCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIBB70byYPCJbFPZal1yhS9wQeIANgQDxlXJLqd8WnyZfgR8y7SalRxDrQZnw+YmkzAglDwBB5jh32vzhVI6ShODqXUy8JtNxqtZl4cO+VcfIiM2u88xW0WtdqjOe0nkeUhRJc33so2BZq9KpUv0VN0dtL3CMGIA56CG1HgsoOSbPprd/eHD4ymKlB8wIvYgq1rstyrAG11YX4aTopJ9DLLHKKtrglZJQQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAKXcAEk2AFye4QErOD724v6a1VrXLElM3K2iDu008zPOlkue4+4ho/Y6eMYq3H6vv+/Q1Wns7MhRgCVJGnDy+M7bq6HhZWssm2qIStsSsGsgJHLX9Z2WaNcmKWnd8Gfg93al71bBewG5MpPOu4vj01fETq4UZcqDQafPfMryU7ZvxaeWV7IL+jYtz9q/Ra9NyPq1tTY9lMgDXuWyn+GWxZGpnqazQwekeOPcrXqv55O3UKyuodGDKwBDKQQQeBBHET0D4srgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgGv7wb3YbDK/W6WonGlT6zC5A61tFGvP3y6h3y4Xiy+PHPI6gm35HGd4toY7H1nFVqqo32KKsURV7bC1z2ltdO+07LLggm9y4NEdBqXJJQav7/IuUM4GV9WXRiOZHPz+M8DI47nt6H3mCMvZx3vmufUuKUv1hY/iHzrKqTXQyars+OX3ocP9SjFBafXNiO0cP6Hx986Re7oeJlxTwupqjG6NzleoBZgGVNfsngWtxJtcDhYgm97Ss5VwjZodEs63z6fqZdNNPn9OQnM9yGOMFtiqRkLgM6NfrKPtJ2qeJtzHxl4ycXaOOVwfuSXD48vQzNhbRrYIgYZwtO92osCya8SNbqT2j3zfDWpqsivzR4ep7CjJ7sLryfP16nSN3N76OJJpsDRrKbGm9rN3o/Bh7+6amk+Yu0fPZdPlxfHFr78TY5U4iAIAgCAIAgCAIAgCAIAgCAIAgEftfbFLDreoTc8EUXY+A5DvNhJ7rfQ6YsU8stsFbOebxbz4nE3po/QU+xdXYfmfkO4epnH8XCHwq35/we1h7Ck1eWVen8kJs2gvXo3VFAuxAtotgb2+0blQO0mZJ5Z5b3M9xYMWmjGWKHL4Xi/z+d2Y5cB1GYgC65nGW4Gn3S2vOZZcPg2pvY24+fHP6pF6tiqQGRQ2XiWYHrH9gOV++Sl3spGE298qvuXh/ZiFNbLrfuJHxENHfdxbKHuFqKylgylStuR420vcaEW52hNp2jhnx489Y5epfq5G6zNbQWGg0AsBa3YAJVLxL4o+zioQXCKFqr91Wa3Pl6nSXSLtPvZV9KemcxIW3ADX385PUo4Rmtpdw9dajXK9HfUX+xf9V87jwkJHOSnjX/t+v9/kXThGU3qIShUkG2ZTzFm4HW3OdYqUXZzlPFmjsTT8U/3TNh3b3sq0AErEvTFgbm7rm4WY8R3HytNMNS/8jyNX2Njm3LDw/Du/o6HgNoUqy5qbBu0cx4jiJpUk+h85mwZMLqaoypJyEAQBAEAQBAEAQBAEAQBALWKxApoztwUEnykxi5OkOO90cn25tCpVdn4k6kdgHADuHZ+88/LllPhn22i0ePTrgjGa5UjtsfP+tvWZ+pvtRi79SvBNcsctgxFmvqeF9LaC4B+Eu0lwZ1KU6k+F3Lv9X/Bi4pOuVIuHAI1tYjQ6+ko0a4P3b8C4rkWBUhvxGx9IIpPmysYhhx1/MBYjxXmO8SLKuC7iWNOl9D6Sy5s9g4Pab281uf4ZSXU81Kb19d237+pBuqkjS7dnLzPZJTPVtr0KqyW6t7nu0A9OHdzliIvvL9HYdWwcUHfMAQxItY97NYCXUJPuM89dgTcXNKuq+0VVdhVn0FSiSONJKilh4k2B/hJltjOa7QxLqpJdzadP78yirsmrQXMyFLnLcEXJ426pvI96JeGowal7U7rkxK7HLrxJF++1/fbSJc8nTFak4vmuno/9EvsnatSiwZTqOfxHMS+PI4sz6rSwzQcZHVtkbQWvSWovMajsI4ib4yUlaPi9RglgyOEjMljiIAgCAIAgCAIAgCAIAgGt791GGHspAFwWvcEgFQAOV7kHwBm3QyjCblLuT/Qz6jHPLtxx75L9Uc9ontnzp+kSLdZcp4GzBh4G17efzylocSsz6q54dq72l+TaT+hI0KKdAxC3qBmyFswWyBRYsOP2nIF7EpryB9nQYoyxrcrV+X33fU+a7Z1WTHqfck00l0def7l7E7NovUallIU1KS03UZiovVu2jPdWAUMTYjMpsLCdcmlxyxrhd/l4eSMeDtbU4su7e368r5WQ2PwlVVpI1KqjspLFhcAh3UADICOqobW+jDsuYhoNPsnfNdOfI1f981U80KaSbV0vPzs9KXW/3l/afOn2d1Ku5lOJw/1WUW6zsT2aBNf+YykupWEl7VvwS/V/wVUFIHVtc8WPw5y0FwTN31PDTOtuHM8yZYlNd5sS1qQXDh6PSVGpJlbTQU2qZut39UeF+dp33RUVa+7Z4U4ZHLK4zqKk7XjaVcF98SGpl0oZgOqTTZmJ6o5MO0k8uPC95G6PgZ1iamoynT68qu/yIraFSi2GvSXKorAlcoWzZGvoCeQHOJtOPB6Oljljqayu3t63fFkF0N8q+BPv/v5TlfFHpJVOU/Gl8v8AZfqpaQWXJtnsy2n9ZVoHmoqL5aH9V9Jt00uqPnu3cKqORej/AGOhTUfOCAIAgCAIAgCAIAgCAIBzj2kvUbEU6YbqBA+VbXDAuLkcbWPPTjO08+KOllCvff6faN3ZejzT1kM91jjd+tUl+d/T0ICjTuNf8w+E8Q+xk66FWJvksdew/pFlVFSfBO7ubcp0cNTuahJuSFamALkn7zDtPjPa0kd2FdPr4nxfbeKT102m+7p6EjT3pQ8qpGoN3pg31ANs3jax5TY8NeH1PIWOdd55/wCKKag3SqQRlBzo3HQGwaVnhcoumvqddPjcckevVGputj3H9f6z5pn6QnaKsQgFCmeZqVR6ClOUymNt55Lyj/8ARYo8JaB2nwZFrzocrokMFiVyhGYoUzGnVGuXOOsrAalD3agyyaqmYdRgk5OcFd/EvGujXmj2tg6mbMmWkrA5nSonR5s2ZSLkEdlrX04HhI2eZnjkjW2ScmnwmnddGun70R+PqoEFJGzDMzvUtbPUYZdByUDT1kNqqR6GmxT3PLNVxSXhFc/Mj0brHvA17jfgJVM2tF+iAXQZcwzKCo+9qNB48JByzScMUpLqk/0N/wBkYlXqUytly6kW5MWphQCAykEWIIBFrTRhW3IfDzk2mbTPQOAgCAIAgCAIAgCAIAgCAavtzZ1MYj6SGZKqqPrByUaspBsmUhTe50uOA498GKLe59/H33/QjNrMvs1gXRc9PtfU1zeoZcU2mUMFYW4HQC/qDPJ1CqZ9d2VLfpVzbVoha1Xj8+6Z2z04xI9LdHYW0YgfCTbO1VIy8PiSwB58JNnOUEi/0gkWU2lD1RwPnIssovqg9TMqobdUsQfxZsoP8olXGyIx2zc130vSr/k8RbaSUq4JbvkvVGIHVUnwBNpfnuOS237zo9TC1cuco2XjmynL68I2yq6DzYt21SV+FqzDeuNSQbDnbT1lTulXFmJ9Kztp9lfeZDOkY0ilWYu1uAsPT+/zzWTXHJm4CsFdXIzKjA2P3rcb93KE6OGoxe0xyx9LVehK1N7kNamoohQGWoxzFj1SSvGw4knynSD5TPDydiOMG1Pn0/s6vPUPmhAEAQBAEAQBAEAQBAEA0jev6MXqis2WqQBT6rMApQrc5Rf79Swva/hed4axYNqb9fn/AEjti7MzapOUI/WiH3k2iMTVUqCAqZb2trcm4Fzpw988nPkU5cdD6ns3Sy0uJqdW3fBDOumvEcR+4+eEzHpp8+ps+6FU0MHi2phcyOai3GmqLxtbmrGbcMqxtruPA7SxrLrccJdGqfzZLbEZWxKVgApxGFV2A4ZgyX/mA8p1hTkpeKMOquOnlibtQnS9Kf8AB79KbE4Ku1ZFuvSBdCPsi6nXnfn3SL343uRb2UdNrMaxN81f5vlHvSPh8JQNCgKjMEzAKSdUuSba8f1jmGNbVZG2Oo1WRZsm1K6586rks7u452XGVaiBWDXKEGwKU+FjrykYpNqTa+6OmvwxhLDjhK1XX1kYm0K9Ovs5sSaaLUW9igtwYC3hYykqni3Vyd8Knp9esCk3F+PoT2K2i9OphkAW1U2a97i2XhY2+9O8puLivE8zDpo5YZZtu48r69SqhtN2xlTDkLkSmGGhvc5eJva3WPKFNvI4kT00Y6SOZXbdfr/BrGyq9sLj6agL0fSFSOPXDqPTKLTPjlUJpdx6+qxXqdPOXO6r/Kv1sr2vUUbLoDKFzdGAo5AXbie0Lc+MnI/+FEaODfac+bq/4/c0PBXKn8zP6Fjr6WmJn0rrqZi0wWWnfKCyqWJsBc248tLk9gE7aaO7LFVfJj1mTZp5zvuZstHDYQLUFLoirZLs2TMXQmlYqwJCsAlipBuxIn0GSEq99fxz/B8DHNJO4yfzOhYCtnpU3/Eit6gGYpKm0WL8gCAIAgCAIAgCAIAgHhNoBxnEVzVqNUJJLkknxN55mSVtn3uDGseNRXci8mEa1+tbxPwnOw8sbrgtVAePMeciy8WuhP7nqalLF0Vt16YC+JDjWa9OrjJHkdqtYsuHK+58/lTJfCUeir4OkzA1Vo1VYKbi31ZHvT3Gd4ra4xfWjzc0va4s2VL3XJNX+f8AJXh8c+LwWJNQAFDUXq3H2FDC+p5+Ujc5wlZMsMdLq8Xs++nz5ujKxX0lsNQOEYZsqXJy8Mn5u+S9+xbDjj/Dx1ORalcW/HrfkYG7fTU0xhqgGqrljwIzZM3Lx5SuK0pX1NHaHssk8Kx/C1S9Lo9qYlsRs16lVVUtpZb20dQOJhy34W2IYI6ftGMIO0vH0L+8dXLiMCO1z+tOTl+OBTQq9PqH5fyW9lVc21MV+WnTHqKZiH/mkNQq7Oxebf7msDFZMLiWGr4is1NV/KrHl/xPUTPe2EvNnrLG8uqxJ9IRTfrX+jN3/qdDRw9LklNmP8CqvxltTxGMTl2M9+TNmfe/1bZquEo5VVexQPT+syPqe62e1ByA4cvn1/vOuny+yyxyeDOOpw+2wzx38Sqy/gdoGhmsobMoWx4aMpvbmdD5m/Kevk7WhkpODSXmfNr/AKbnFWsiv0/v9jpu5u0kr4cdGCopnJY25AHgOA62k5+0U/eTPL1GlyaaeyZOwcBAEAQBAEAQBAEAQCzjB9W/Pqtp5GGWi6aZwHYWPeqA7HiAQBpYctRreebOCTPdlnnl5k/yJ5azHmfWEjnSLNSlWvxuO+VlGJ1xZZ437rMGumJU9RiAR1gjFc1uFxpeSrS4Z60NZgnXtI8ryv5FCvVU3IcH8Qv/ADCKfU1e1wzVWq++4zNn49lBUVGAJNxmOpPG4vrIcpImWLHKm0uOnBL4bGVALJUde5WYD0BhTkujM2TDjbucU/VIvDFVBm+sfrfa6za6W111001k7pLvKexxuvdXHThcehHYrHMFyhiF7Lm3pKOT6GmGGN7muSCxGNFRrZ2qOOAzEgfCHfeaIY4rokhSogH7bF+xDw8W+fOEmcs2ox41Tr0JHYuzCly1izEkmx07h4S1I8rN2hklwuERu+mLqjo0zs6F1uzEkgZr27gTb9OcvFW+Rj1CcVFJK2rpdSSovcX5zgz2mXMhkFbLNZfn5Miy6Nw9lWJsa9L/AAuPerf6Zv0suqPnO38XwZPVfuv3OhzWfNiAIAgCAIAgCAIAgCAcX3hwCUcfWpIuVbhlA4WdQ1h3XJmPOuT1NLK4GThUtYWnA0MkqbDsklaKuhQ8ooWz0YJeMihuLFTZoPEA+IjkvHLKPR0UjZ9tBp4QdfxeTxLVbAE8SfUwT+KyeJgVtjKRqM3iSf1lkyj1GR9ZMrwOykR0BQFan1Y00BcELp/iIlk74I9pNxfPmZ67GyEggadkozlvtF407Dv9BBBr+87AZAxBVrjXlcSPQ645UROycZUYAdGVA0JbS9uzmR3yJQ56npz7R4qEefMm2xQAsEQd9ix/5iZXYjHLU5pO3N/lwYmLrEqeA8AB+gjYiFqMy5U2TnsYWq9fE1XHURVpq9rXZjmI7yAov/iE24IJcow9oa3Jlgsc+adnWZpPJEAQBAEAQBAEAQBAEA5d7UMP0eLo1hwqUyt/zUz8HHpOGaN8m3ST6ojcNjwbXmY2mWMWLwyCpscBKk0BjT/SQTRV9MblIFHhr1D3QOC3UrEX60gkiMfjwurNlHebS6TZDpdSKXelXIVKhYI6MSoJtlYMLWFibidVjaGN7m9vJtSb10iC5ZdSdCw07rHnOVNFdtcFB221T/Z0Wa/MjKv+Yj9LyKZKSMY7NLHPVIJ5KNFHgOZ7z7o6FrK3orILGLVoxYsxMepWme+SiDqPs0oZdnUPzZ2/zOxHutPQx/CjyM7vIzaJc4iAIAgCAIAgCAIAgCAQ+9GwExlHomOVgcyPxKsLi9uYIJBHYZElaovCbi7Rz6puPjhoFQ25hxY+F9fWZ/Ys2/iYkdtLYOOoKXqUWyLqWBVgB2mxNh4yHiaLRzxk+DDw20D4zi4ndSskaOKvqbDxlKLWV1tt0qY1YX+eUbWRZF4jeJ30pIzX7eqPj7pbb4izGGzsdW4uKS91r295/ST7qI5ZlYbcqle9V2qHtJ+Mb33EbUSlLd7CLoKS+NpXc/EsuOhlUcDQSxVFFudhIsFxq47osmjCrVr85BZGIz98ArpZRxMmiLInbmJDDKuv7mWUSG+DuGwsF0OGo0f93TRT4qoB9956CVKjxpO22Z0kqIAgCAIAgCAIAgCAIAgCAQW/OFFTAYkFsoWmalxy6L6z/TIkrR0xS2zTOBV8UuYBFd20u+bT9dZl572ejVcUS+EwTMoZha/K85NnVLgksFspCbm3pIbIolKhoU04eMglIjDtoE9Qi3eR+0UWMili3NtV9ZFAqarU5FTAMepiX7CPf74BaNZ4BYaq3MyaFlv6QQdNTy/tLKFlXOiQwm7+Pqi64epblmsn85E6rEzO9RFd5Obs7h4g10qYlAlOmwfLmVixXVR1SQBexN+y3OXhiads5ZNQnGonUpoMQgCAIAgCAIAgCAIAgCAIAgGse0XbIw2CqG12rXoJ2Z6ita/dYE+kiV7XR1wJPIk/H7+Zww1BQXqKCx4C3b+kwqTk+T6GWGEveRkbJxWKc3JXKOQXnIyOKLw0yfUyPp+ILZVIv3Dh46yvFWXWkgSGB2E1e5ruzWN1Tgp8h2Gx85SWSuh0WOGN9Curu5hzoyC+o7COzWVWSSO7hGS5RXT3PCg5KtQW1sSeB7Pn1j23JnaxdKIqph6qNk6Vwwv1TbMfC4sw7xr2gTpu7y/4bEzHqYmuDbpNewjWFJFXo4F2k9dhcMCfCVc0mc3pIkftLH1ENNQRmdwDpyBAI8y1r9xmrDFSUm+5Hm6r/jnGMe9/7O3ezmghw2fo0DZ2AcKAxWynVuJ1JltK24WzHr4qOWl4G3TSYRAEAQBAEAQBAEAQBAEAQBAEAQDQ/akiV0p4U5mJvUKrYaDqqxZrBQCW1JEpNT4cXXmadO4c7lfkcgp7NrKMldrFSdbhtLnnx4W42mXJKO64nuaLHl2VI2/YGDUpZRoDx58JhySbZum1Hgpp0VR7i3HjOj6HVdDZMItl0IsRfxN+Wun9RM8upiyv3jExGHzPlIsb6dh07YUuDvGdRsyKpPR5XW7Kuo4XA5obakftK3ycI/Fcehpm0qvHMBWok8/tL58vGaodDf3GZs16LplNUroLJWAf0Y/Gc5WnwcpTp9DCxeMw1FrEC/C65sp/adFFyRd0y2cHg6lRcSGql1/+MlVXW+t8nItc68p2jkag8VdTzM2kqayp9Pv+zpPsprVGp1sygL0h82DMLgchlVdPCaMEUm1Hpx86PJ1snJRcuvPyT4N8mkwCAIAgCAIAgCAIAgCAIAgCAIAgGk+0fd8VKZxXSin0KE1AxIVlTMy8PvAs1tDcnwlJ43PhdTXpNRHDK5Lg5Ngd5MK5HSKy35stx7r2nCejyxVrk9vH2pp5cXXqbSu9mASnZayXsedu7z5zH+HzX8L+RX8TilO3NfMhKm82GJ0qA68R4dk7fhstfCzX+N06/wA18yU2bvfhACGq20PEE3+E5T0eZviLM2bVYHypozn3x2f/AL2+oNsrkHzy/NpRaHUP/Fmb8VjX+aI7ae++GZcqqzjXWxUqPy5rfN52h2ZqH1VfmiI67Twd7vozVq22QWJAIP4tLnudeDe4zbHs3J4o7PtrAuif0/k9TbwCleiVgeV9PIW0HGS+yZN25/QzZO2Yv4YP5kLVxb8lXQ3FwzWPmbe6aY9nxXVszy7Xyt+6kvqe1Nv1wmXKul+4Wt+HhfvlPwEFKxLtfNKNOj6a3Y2QMLR6MNmzMXvYL9oDSw8JzhHaqMWXJ7SW4l5Y5iAIAgCAIAgCAIAgCAIAgCAIAgHOvbXj8uFpUbm1aocwHNaYvbwzMh8pq0sU5Ns55HSOLthlPAC3jrN+1HK2W2wwHO3iAffK7UTuZ4tEcujMbUTuK+i/+tfdJ2+Q3eZUUH4IpeAs8OX8P6RwRYz9iAenz8mAehm/KI5BS3e3oL++AUthgeZB79fdI2oWdy9kW8j4mg9Cq2Z8PlCseJpsCBc8yCpF+wrPO1ENs+O87x5jZv8AOJIgCAIAgCAIAgCAIAgCAIAgCAIBx3251718Mn4adRv87KP+3N2k6M45eqOcIeE2HMoqMQZAKGAuAbWPDx+bwSZHRLyAk0QeFBpp+0AssluQPl75BIXLwIHcbRwC4gA4C0kg9qNpeLBabgJVg3T2M40ptHJfSrSqL5rlce5WmTVRtJ+B3xSpNeJ3qYi4gCAIAgCAIAgCAIAgCAIAgCAIBxL22/8Araf/AOdP56s36X4X6nHL1NBXlNZyPMRIZJZxf2V8pEuhKMynLohlNTl88jDIB5yCTFb7UqSZI4SxBQ8hg8rSGEbD7LP/AHbDeNX/AKNWZ8/wM6Q6n0ZPPOwgCAIAgCAIAgH/2Q==</t>
         </is>
       </c>
     </row>
@@ -2282,25 +2282,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GERALD COETZEE</t>
+          <t>RISHI DHAWAN</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>sat20_2023_32</t>
+          <t>smat2022_136</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>70.59999999999999</v>
+        <v>33.3</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -2312,86 +2312,86 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>64.7</v>
+        <v>66.7</v>
       </c>
       <c r="M15" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="N15" t="n">
+        <v>26</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>13</v>
+      </c>
+      <c r="R15" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>3</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1</v>
+      </c>
+      <c r="V15" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG15" t="n">
         <v>4</v>
       </c>
-      <c r="N15" t="n">
-        <v>41</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>10.25</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" t="n">
+      <c r="AH15" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>29</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK15" t="n">
         <v>2</v>
       </c>
-      <c r="U15" t="n">
-        <v>2</v>
-      </c>
-      <c r="V15" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>23</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG15" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>18</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>27</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>1</v>
-      </c>
       <c r="AL15" t="inlineStr">
         <is>
           <t>All-Rounder</t>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="AM15" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUWFRgVFRUYGBgYGBgYGBgYGBkYGBgYGBgZGRgYGBgcIS4lHB4rIRgYJjsmKy8xNTU1GiQ7QDs0Py40NTEBDAwMEA8QHxISHzErJSM0NDQ0NDQ3NDQ0NDU2NTQ0ND81NDQ0NDQ0NjE0MTc0NDQ0MTQ0NDQ0MTQ0NDQ0NDQ0NP/AABEIAQ4AuwMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAADAQIEBQYAB//EADoQAAIBAgQEBAMIAgEDBQAAAAECEQADBBIhMQVBUWETInGBBjKRFBVCUqGxwdHh8HIjYqIWgpLC0v/EABoBAAIDAQEAAAAAAAAAAAAAAAABAgMEBQb/xAAtEQACAQMDAwMBCQEAAAAAAAAAAQIDERIEITETQVEFYXEiFBUyUoGRobHRQv/aAAwDAQACEQMRAD8A86ahNSFqQ07CHA0QLQkFPz0wC5YFDFFmRTVWojERtae2tNy0RaBo5LU1Lt2hFCVqcr0gvcZfNQ21NS761DnWpJEWwq2qSjITGo5T7dfShsutAxMmlR3WKmohqPiBUktiLe5HpRSUVEpCHK1Ixovh12SgakCSpCPQilLNMY57lDz0i60XJURgClJFPZppIoEOApjJTlNPZqQzkalFDUUdFoFcbFNzUZqAxosO4RLlGQ61HsJJqa1qBNOwrj8QkrVYE3J5a9o21PLUj61Z27siDUMYC8+ZltXXUkgMlt2XoYZQZ10obBK4LMBGZhJ8xjUwFkAnr71MVA650IMfMOnLQc/3+hqtu4dl1cOp1EMpUzIHOORP0pLV7KdGI07/AEqJIukURVbi96no8qO4B+oqHilqSdiLVyGoqStCRDRYoCw7xKZnrgK5koI7IMgkUF01pyPFFtAE1JIdwKpFPipps03wKHEFIq0ok0ANTwKiMcxpVpPDrgKAQXSkzUwmmTSQpMOhmntboNtqNmpjXAexbipbaio1l6OrVIiyuuNlNep8JxOJSwsJbNpbSNZbMczEovlKhY9+2pNeZ3sKz/KpP7D1OwrV2uLqmHtC5de1kRLcoEcZ7atKtmkeZSh9zVFZbI0aaUbtNi2bOIefGtIEcNvruQwfqTI1/aoHEfhyy18FVZbZyyq82JAOkHQ/9sQOm9WOHxaumdGzhQIOozLtBB2IIIjtRrNx3ZntmGCMEkwswSZMHXQDbnVOTXBrlGLtfcxvFUFu6yLEKQABMDQSBOsAyNddKdhreag4iw7XHXK3iKS1y2RLwYJYFZzjzCT3mIkg+AetK4MEuWSL+EAFQbduTFWOJv6UuBthjQIjXMLAmq9xWnxWH8tZjFaNUkQkgJXWpFkxUdWoyvT4BInpc0rvFqOLgpuapKVwasQMtEWuZCKcoqBI7NXCnm3QWakFhxpjClDUrUAdbNFz0FRTTNOwExLgqxOFZUDnnEDoDzNQeCYB79+3aQSXbY6CFBYyTsIWrjG35kGQQYIO45EHoai5K+Ke5RXlJWS7gbKXHZzBbUAQCYESNBsNSferHh3DCwa3fQhHKlFaJLIZJCgySQffy1Gwd1yci37r3GC5ZuutmyCBJKz5iqKQSfLJEBqNjeHuk230OWQwbNJzAh1cHX5Fg9qpvKUsbpf2KLVKSmt/PgkFbeH8qIyKdIcEFmMEmGJIG/oKkcDu6M8woMeij8X+9ayONxJDnPcLNBOaMxB6TO1Ja4peyQmeYgQAFGszuST9NhUXSk3Y3vUxtdF9j7iG892T4rrrrogYoltNOZ+Y9MvcVMsBHXJiVhvw4m2JcdBdTTxF7/MNpis9w3DXbn/TULmLZyzEy7RlCiAxY+YmIOxNTb5u2GVX/EuYDOGBEkeo1BEabGndxeKav4IRqUZb1E/lPj5RF45w57LKHysrjNbuIcyXF6o3bmDqOe4l/C2Iqb94I1p1IGVvnRtRmiFdOjidGEE7GQSKgYJwNDuNKui7oKkVGVotNNXTXj/S2uXpFZria61aX8QKpsZcmporYBEJOlSfsxpcCtXClYpsCrtYRjTvsrVd2XVaXOtJOwuSje2CBQ/CqbatSBTXt60hg/DkUBsNU9V0pjLrSBkP7NrRBhdKmLYM0VbelFxoqzYimnD61YPZNDK07iLL4atX0L3bNvOVXJJUPlLMGBVTu3k00Me4qsx9u6pJZHBMzmRwTO8yN603wNcIxOXMcpRpWSATpBIG53rXY3hdmGdlk7yWYn9TWOpUlCo7Jb/uWrSKqlK7PMPh68EY3GGqFfIWyMTmBgSPlIUgnaD1iicWxDO0l5XWACVXUliC58zmSTosdKlcQwbviXWyknKh3UAE5hJzf8e+1QzgbpmQA2ViSzouiqjkLJnQOpjfU8wanGUb5SaTtwZakJRbilsu5XtYB0gADouvsNWPqYpyIBzA9Xg/QGrGzwHEPcFpUUucxgssDK7IZZjAOZCImdutOv8AC7qKGdIUqjA5k+V/kOXNOvSJqzqR8r9yhxl4YTgzopLFiGHyks0ajXY5tp2mZIMVW8WuZrjHOWljBaQSSSfLOvs3OnNYOVnjRIzGNpiN9/mX6iq/F31CkS2o0Gw7aazTgllkueCSyslYaX77VJVGyq35gSPZmX/61AwlsuQNTJA+p3POtj8R4VLZS2hB8NWtmANCHL5WI0L+eWjYmOUCbe5bCNmUOUnem/ZJqSOVFVt6LlxFSxAoizTw8ilFTRCQxiaZrUjLrTKTBMsrOGAETTbuFB51ExmOYMQKamMaKjZkgzYfvS2cLrvUJ8Y00S3jGoGXaWFoTWhO9Vq4tyaKlxzyqIE67ZEb1XthSTvTbmKYcq5MYelNAXfwxh8t9TOwY/pH81quM4uFjrWP+GMWWxKL1DD9J/ir/wCK5VQw2Bg9p51jrr6zfp2un+pgeKcSZMUzLB8mU6kfMGUwRzyuw96k4njGdNC4kXQYCIvnChIKGW+RJnvvNZ2/cJuO2+us79P4o9pwOXf/AHt/VX9GLSb5Rza1R5O3cvn4ohvl3uXCuUAFsxIP2hXOg28mYz1HWKfhOKWkVgCFGZCrBDmKoLMKWiYlXOp/AvasuX6/4pz3CedJ6eLVtyKqSXFjQ4riSG3dRCrG48jRgygeCVBkbeRp7qNetMtnzoTHzgDoSSI5ev0qIXIObmNx1HUVY4HEgkTqBBHqD/Bj9KshBQVkJuTkmW+BwVsGGRCQSJyiddR2Oh51P4xh5RAsBVzKAAFAHlIAUaAVXYdHuFmTfSR1AG4rQYa0WsuhEtlzL/zUSsHvt7ms/FS7OjGOVNpLczn2U6U77K0mhJxEGNKK2PFa7MyAxhGilGHbSnrjhG1d9tFNMTQvgNNC8Bqe3EBQ/vEU2xJDMXb85rlXSpGJIzGoN2/FWJpEGmPdKbaNNS9NFtDWqpFkSZh0FSGcChJoKDduVBlkY3Yy+01GZoqUpEVGvGnDdkqscVsH4Tigl+25MAOJPQHyk+wNeoFPFWXA6NpMxptXkVeifB3Eg9gWmJzpI13dJkMOsSFPoOtZfUIyUM49i3SVFfGXczfxh8LrYBxFmShPnU65J2YH8s6RykcprIAwd/T+q9nxDqyvaZc4KkOsgKFYRDHqRyrB4jguDDNa8R7TjYuZVgRI0bQ+xG1VaPUSlC07/PsR1elSllG2/wDZmSqtodDQHssO46jWtBifh26nyFLy8irKD9GI/mqa7byGGzIfysCPoYrdGSfDOe4yg90AtpOhMdCQf6qzwWCYq7oDkSC7AyhBMKYOxn+R2qEipMSSTy8h1/X9qtMDbYLcGTNKSZKqVAIOdVHzQQJ7E7b1IWTyRK4Jc88e49RWkS4QRFZbhV0JcUkAg6GQDEncTsa2OHZMwlAfaufqqmEt1ydigroweLTJcdNsrsB6Tp+kVy61bfGRBxOYCJRP/EFB+iiqq0BXSoSygn5Rzqqxk17jsulMmpCqKZcQVa4xIpyI9ygTUlkFAyVUTNBicLJNV1zAHpV0Lkk0dVBrO6slsSUTP4fh5qcuCirMIBQb1wCjNyY7EbwdKrcQutWty6IqnvatVg4OzCINKBfSjoNKDfFOHJfW/Adbw/lLj8JGnbST7A/pU5rjIVZGyumqMu4jb2I3H6UXg/DXa290koin5o0zaADTX/R1qDiRuv0HT0PTl2ok1JtHGqSlnz8F9wD4szXGW75Gd5kHy58qgr220+nre8a4GmJWQcrj5SAD7EdK8vxCzLAQeY5MP7rTfDfxWyZbd5vKIVXP4ez9thm5Rr1rNKjjvDsdWhqY1I4Ve4T/ANC4rpaHqxE/pVRxLglywR4tuAflZQGRvRxI21jevUsVxw+ESoV9IEso30Op0IrH8c4/4tk22VB5gwy6ZYM+YwBG9OnUbZCvpqcKbkm1435MollB+AR359Kl4dVAByLpOkaa6EdqiK2Y9uvX07VItitJyW35EdACQCe3WOVabB8QDKpytI0YwupAExJrMYiQ1WnBGJDjoVYe8g/xWbUUYzjd9js6Ws3b3I3xPdz4g7jKiLqZnTNP/lUC0lTOPIfGnqin9x/FREMVqoJKKS8FNe+T+Q6iudaFnNLnNacUynJgXGtCg0S7M0HWqJKzLE9jUZIJoyGmAyaMq1jk9yxCzVbjJqxJoF5RUqfIMrlmKiuDNSrzRUUtNXiTsdnNIlsswH17DnSMal4RYXOdz+1CViuvWaiWWNxQyoiAqiDQEiSTEsQNOQHtVPef3/f2pbt9uQB9T/igMTuVb1XzR7aGopWRzUm3dkZxrpQHt8/r3p7uJ3+uh+h1pyvUi5XQxOJXEXIGlQ0idYgRpSLeL/Mw7DkO8de9JicNzFRPDqKSLnLOKu+C1Rh61JUzr+8ge9U1l2UjXSri1tI0NSM844g76ERPMTp6kfxWq+D8EMj3W5kqB2G/6/tVPxy9bdptJkQQFBADfIAZAJ5r1PM86v8AgPyZFYJkyli5hSc0voIMgHTUA6VVN3gu1zpaOzfwUXxcmTEAAaG2hHoWf+qpQ5q8+Lcfbu3lKGQiZCRMGGO08tf1qkTerKd1FDqtOTFD0ouUrxFckVbkyqyGO9Mmn3DrTM4ovcDUoupowYdao7nECGIpn3iazOFyy5f6dac1mRVAnETNXWGxUrTjCwXAX8LNBTAaVKbFrMUfxgV0qQiqXCjUnlQ8Tc5VKZ96q710EmKDDWeUreBCx6/x+29BdR+X3Jy/tJp2b2oehOpYjnrANSIwg5OyAWMGbhJ2QabsZPQZj+tTGwI2AAqwtagACKZeEcqDaoJKxWOhXQ6g7H+DQLtjmv0qZevAggig2z/j+qDPUji7oBasE6kfxU61cA0kjs38UitNIo5cuh1H0oKZPLkO3nkA6iDEd4k9N6UWDFNsiD5Rptlk8/yn+Nqa+KimjTQf0tIc+HNJbwxrlxIp6XxUi8ZdsGKS3YNFa+KYMQKQA7mHM0L7OakHECa7xhQAG/h2zHyneh/Z2/Ka9CPDV7UjcNXtV3RZ2Puv3PP1w7dDVtYchYrTNw5e1VWKw8GKprRwVw+65eTOXWbNzqywl05CTyHWJ7Cj/Zh2oN0ASeQ2gRVEZ5HP19JaWKV7t9gONvwsDc1ULdMnrR79wsJPNj9ABQuHYR71wW03J1PRRuT/AL0qbaSuzmU4Sk8Vu2coLawYHM6/TkKciHvXp2A+GECBQogD39T3qvx/wxGqisy1sG7HXpaC219zJWL0AU3EXpq4fhpXQrTDgx0qzrxNS9Lm+GZx0Jp9qwSDG41rQfYh0pyYQDUCn10EvSJSVmzNh6UtroYqTxTC5GkDytt2PT/f4qEpGx2qyLTV0efr0JUZuEluiYj6jSD03B9P6qLeXWnpK85U/pWu4dw5LlpHA3EH1Bg689qtpxydjRoKDrTcU7bXMeq0qTW1bg69K77mTpVrps6i9Ln5MU1Maa3I4MnSu+5E6UdJj+66nlGEg0mtbtuCJ0of3InSl05B92VPKL2aQmhWLwYSDTzNaTuqz3QNxVLjV1q9baqjFDza7AEmN4Gpjv07xWPV/hHKagnKXC3IDnKvdtF7D8TfpHuelVuKfykctCfbX+Kk3rhY5jzjQcgBAA9BVLxHFAyi6z8xG3/EGs8I4o8LqdRLVV3N/p7Iiu5PmY9Sfc/1Fb/4M4HkQO487wT2H4R9N+9Zv4Q4OcRf11S3Dv3MnIvuQT6Ka9dw2HyjlWLW6hRWC5OloYKKdR88IJaSBFOZAd6eBSxXEy3ua8tytxfC0blWdx3BSuq1tJpjoDuBV0NRKPJppamUDze5bZd6bW4xvCgw+UVncZwd11UVup14yOlS1UJ87FJiMOHQo2x59DyNZK7bZGKsNjB/sVs3QgwRFVHHsHmXxFGq/N3Xr3j9j2rZRnZ2fcweraRVafVhyv5RSKx9R0/3atT8JYtgxswzI0sOeRv/AMkCPYd6ySKSdND0n9p3qdhmIIYaEfiUlGHoetbIvF3PLU6kqM1NcpnpBpBUfAYkXLauJmIadww+b+/cVIit6aauj21KqqkFNcNDxS00Vxpkxtx4E1U3OIiTUjil3KprIXLxk600rnP1mr6TSRouAOSutXlQuH4TIKmmiTNenjKNNKXIxhptVDxR4OUaZl83pmBA9ZWfp3rRIkkDqQKwuMuNevXArFbauQWGjMRoQD05Vlr9jmetVnGhina73+AeMBKmWAB6GJ7VSXCBoOW5qfetrmIYFgJ+Y5iIMaE1uvgX4aRkXE3F5zaQiBAOlxhz1BIG0QdZEYa1VUo5M85p6bm7RLr4M4N9mwyhhFx/O45qWAyp/wC1QB6zWgAFPINdBrzlWo6k3J9zuxioxUV2EEVxIpTNdrVY7A5pRTsvaly9qBnD1plywrb0UDtXe1CbXAk2ikx3Blas7jOEMkxqOlbw+lQ8W6RqK10a807cmyjqJrbk8T4xgTaeI8p1Wek6j2P8daDbuN69idf/AJc/ea3nxJglvowQedJZO55p7jT1ivPUP05dR2PcV36TcoJs4fqGn6VS6Wz3X+Gt+E8WMzpMZhOUzmDLvpEajnP4RWpivOcO5lWVoZT5XGjDt/it9g8QHRX/ADKCfXmPrNbaEtsTpejahSi6L5W6+AxaN6iX+IKvMVH4kXjyzWZxAefNNakrmzV6uVHaKJ/E+I59BVTXV1TPP1q06srs9B0rqhcNxWcd6mtpWdyXk9VGvCSyTC4RwGBOwk/oa87GJKqY+UydBprrAYTHqa9DaxeVM4Ro0ZfJn0GoLAAwD7SPWvPOJQryihFbkuqkjca694mqq1NyWas0jzPq2ojWqKK7fyRMMfFvAEQrHzcjAElT1mCAe9ekcO43EK2kaDpFY3geGLZny7eVdAO7EfUCrTwz0rk6iKm8X2Ol6VRpqg5Tsm3+tj0PDYxHG9SgR1rA4DGOhjWK1uD4grDWuTW07juuCdaEYvZllp1rtOtAGKWl+1JWXFmfJBwO9L70AYhKZdxiKKai2CaZJPrUe9i1XmKo+IccUaDes9ieIO/OBWulo5S3ZspadS3kzRY/jgGgM1n8TxF356VDroFboadRWyOhTp0ocNE/h5M71mfizh3h3Q6CFuS0cs4+ce8hvdq0eBIG5qVxDApftlGO+qsN1cfKw/3YkV16ML0rGX1CjGvSaTV1ujz3DXRzHuP6O1bH4XxBa2UIjKZH/Fif1B39RWKsO0nRTB3kiY5gVbcO4gyXEI2E5wWiUiSqkjeYMdh1qMHjK55fSV/s+oUnxw/g3RWd6h4jh4blU4Eda6tydj2DwmtzJcS4dk1AqqitdxZZUxWWa2elWKR5/XUown9Pcv8AhQgb1ufh/gWeLtyMn4FOubuRtl9d/oayVvAxsakcR45jw2a0EVEACImuZQBuGJzGBHLtXDhWTdrmCmpQVmz0y3h8oyyDJOYwPMSNSw09NK8x+M+HLfxK27VuM7MHCgwoUIovEDZvnE7HKBBIk6LA/FYuoZLI66OjIylTvEto3YqTVdex7mQqIAeZksT1MQAfr61bGvGm37lkoqXJCs4W1bAtpooLRrJ3OpPM1zWViRQ/s7dactlhVHWgyH1dmMS2Jj9aZi7hQHKaMLTUy7hS1RdSDRGWbXJUjiVz81KeKXPzVN+6677squ8PBT06v5iEOL3fzUO5xG427VYfddJ910J0/AYVV/0UxutO9L4jVbHhVKeFmujS1VKMbNF0XWS/Eym8VqXxG61bfdJrvuurftlDwF635mVVu6071ocDJG9Qxws1KtWmXSoy1lNr6SUZVVzJnnzuC7whUF2leSkkyskiYMjapK2iTvoSAcqgNHqZzHWtQPhR711nQgKxmDmJztMxA+UmNTtNW174buYaSmV8oVmCA50BmWdAC2UERImddNDRSjGp3SM86cr3sPw9wMobUakQwhgVYqwI5EFSKe1wGdamLwfxUd8NlKITl+YPcZYNx4iCWYse8DrVJ4bUTrRg9zWqlS3JJv2wai/ZV6U8hqSH6VH7THyRbm+Q+YxNIXjcgcvc1IN5SZ1HvtvOw0309q44hTuJ7HnpGvX39a5GJPpryClvWuBbqf0/qpK4pGUZ0XfYn+uR6U5sZbgt4I0OwJEzGp1APvRiHTXkiS1I1wjn07b8tef91LfGIN7ZGmsOw9Y6RNcb1rQC3pJPzNEzM6nedZjejEOkvJGk/wCxXAnr+1S2xVo/g09YM7RvtXfabQM5I05TEcvxb0Yh015Imc9f2rgxqU9+2BASR180giREZtvQ/wB05LtnLqDPXKRHr5tQKMQ6S8kTMeoiuDmptp7BiQdOZza7HUZjPShpcsAGFaNhmLaCDMDNI9KMQ6a8kbxDtEn0MfXalDN0qUzWFGonQSTJiNNJOlOW5hzHkIA1BEGNIiJ6GjEOmvJCLsdP7pHukTpsJqUDhySPOoED11PPccvWY5U5Uw0zB5gmND0IH87+Y0YoOmvJEV2Pv1qy4bwxrqFw6nKYygw3vMD9aHlwxJmSDsArSN53O20em+tQ8TgrE+Il7EWmnXwohtTqyMrLGszHIVOEY9xqCTuavhPGcNohZEYnKoEwek5pgzpudadxPDC5dV1xLSDICm3mTujZD5eqtoetY1uGWMx/698tOaYtAEkyYhB/WtWZvIAB490wBIhFJ75suh05Eb/TRTrYE5Ri+C9x/HrFg5BJeC3h21GbUyS2wWS0wdTm21rKYjE53ZsqrmJOUHQT0otzBYfMGzudCYldTymRM+4Gp3p3gYaYLOdidNOembflyNVVJufJBxv3Ihu+n1p3jen1qTbw+GUam4xJ3OUka8wu476muYYXpdHoqx7SapxF0/cri52KiSdwN/WlJnYARTC5pviGjIhkEdm029Kern+6jo53pQ5oyDIKddwDSlzzEULXrSlyd6MgyQRmHQ/WlV2giNOWgNBzk6Vwc0ZBmGkjcD6UhY9vpTfENNZzRkGSDK4G6+0UuYdKBnNNLGjIMyQXH5RTfE/7f6ofiGlD6UZBkh5ZeY/qnkjfKP8Ae1Rzc7U1rmsdaMgyQfTkKUsOQj3/AIoJNdmougyQ8sOnrTny8tI7n9aAzmu8Q0XDJB8wB2n/AHtTC+4A7+9DzUuai4ZoMCOmv09KTP2oC3e1OzdhRcMkf//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUTExMVFRUVFxUYGBcVFRUXGBcYGBgWFxUYGBcYHSggGBolHRcVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGC0mHR0rLS0tLS0uLS0tLS0tLS0tLS0tLS0tLS0rLS0tLS0tLS0tLS0tLS0tLS0tLS0tLTUtLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgIDAQAAAAAAAAAAAAAAAwQFBgECBwj/xABEEAABAwIDBQQGBggFBQEAAAABAAIRAwQSITEFBkFRYRMicYEHMpGhscEjQlJy0fAUMzVigrLh8RVTc5KzJEODwuIX/8QAGQEBAQEBAQEAAAAAAAAAAAAAAAECAwQF/8QAIhEBAQACAgMAAgMBAAAAAAAAAAECEQMhEjFBUWEEIjIT/9oADAMBAAIRAxEAPwD3FERAREQEREBERAREQERVqt/Sb61Rg8XBBZRY7/HrWSO3p5a94ZKzb3tOp6j2uj7JBQWEREBERAREQEREBERAREQEREBERAREQEREBERAREQRXNwym0ve4NaBJJMAALTNuelCyt3BoxVZ4swlo6TOq1D0z7ztqF1mwx2RZj1hziA7COcDD7V5K1uWWWRGZjLmM/FB6Vt/0n3FVzoBpUogNaYcR9rFrJ0jgtKu9r1KrRiquyBIaXZt46ZHM56rHUamM950RDddBplmuLmzGLuEkEZkzlzJjUJtdJv8TuS3D2jnN1gmWiPHhC7u2nXDWEPMZxgcW4TxGXSCqVN9RxDdQNBOnCR1T/DagI6gmNSBwJ5Js03LYnpJvqIwiq1xgZVJI4xx1W8bsel5jnijdU3NP+YBIz0LwPVz+K8TbaEPg6ceo15T5rpWus5bIjLpH90TT642btihXANKqx4MxBB01V9fK+y94nd3INNMHCWOwPDp7rmgDvEHhB0X0VuRtwXtnRrEjGWgVAPq1ABjBHDNBnkREBERAREQEREBERAREQEREBERAREQF0r1A1pcdACT5LusLvjfNo2lVzuLSAOZPBB86b3bRF1cV68hsvnWcQENBHDQNWv07homZJOX3R0lWbiwc/Om04dBOGY5GMlWuLJ7fWaQfzz1U21413bVY0s7sgaknNxMDiP7K1aXeEvhxc3MAmDE8XN+sCMo6qiLN5+q4qxQsHugCm6eHdnxOWeSbhqrFgA55cDBBJAzgcdNfeVY2rTg4gfX7xAOQ4eULmlsO4b3gxwBAz016HMK2zd+u8jECMWmLkOY4LncpLvbrjhlZrTAUar+8Zl2k6khR1CwNGQmDM6jPorl7YPpEg/k8PxWMrNzz934LpLtyymuqlaxsNdmCOIPHh8l6F6GN4X0L5tuSTTucoknvhpLT7oXnNu7LDOvx/ss7urW7G8t6rTJbVaRBH2sB8oc5Vl9XIiICIiAiIgIiICIiAiIgIiICIiAiIgKhtzZbLmi+i8AhwMTwMZHJX1w50CToEHhLd2DRL6GTy10SDqRExPnxXD91cZLiC0Tk0jMLa7aqzE4n1i5x9pJ+azrKbXjhkvHlndvo44Txm2lWWxGUpaW4gRIyyxZic85VptsaZJbSniSIGozK2ulRZExkNZXWvWpRGQWd7b8ZPjVJeQYMjiI/OSrXrC1uKM35ddNQtkqtYTDfMrD7UojE0CIHXT8witN21Yg03Fw7wBiOn5968+wa56L0Teqt3MvV08SfkvPrluc816OL08f8j2jIjP85aqzscE16QBgmpTE8pe0SqLuKs7MeW1qZEyHt011zhdnmfZLRkuV1ZoPALsgIiICIiAiIgIiICIiAiIgIiICIiAsfvDVLLWu4atpPI8mlZBQXtIPpvacw5rgfMEIPArTe2ni+kplvN09Msitq2Jt5tyCKTxi0A5mPgvKtp9rJHZzlqYWd9GOyaz7lxBjCzPDl6xAHwK8uWEs29uHJlvTcr/eqnQPZ1Xw4ZOjODxWKq76WZdHeIyGsLF787quovxDvB2p5O6rSxSqMMhoI5cVMMZWs88o9cpbw2wzDyB+9B+Cr313SqHuvD/umfavPbe7qOIAoE+cfJZ/ZlpcNfPY4OMk/OFbJPhjnb9SbftKlWkWtMAZgc44LQ7ynGRGfAL1GpP1lo+9FEtqio3j8Z/stcd70xzY9baw8LP7n7ErVb20b2VQNfWpnEWPDS1pDj3iIIhpU+xGUqTu1q0m1HZdmx3qh0ziI4xyOSzdxvVeh7KvbGQ4ENAGERwGS3eTvpjD+P5Tdr6RRQ2VbHTY+IxNa6OUgFTLq8wiIgIiICIiAiIgIiICIiAiIgIiICIiDy1+xraq042NDmktkZaZeeiu7oWLKJq4BxHuGXx96q73/wDTV6g0a76QfxesPbKyewq9Psu5lIBz1kiSTPGV4rLLY+ljZlJUV+wODsTZB555LA2u7FrW4wOkSFlto7x2tsIqVG43HISJ8AFgqF+QHXTAeyLyHDlEd7wWe43dVmKG7Frb94N7Q835x5DJR3N4wGHHy/ooLjauNktM5cD8Vql3ePB1y4BT2XUXtrXLeERn4+xaftivjeB+eauV7iSsa+C+eX5K74zU28+eW7pLdWzXOaGNc4lsYWguOLMZAZngtl2Du3UdVoW7h9KXdo4HM0mgdxrxwJzdHJqs7oWIDHtDw11YhoFM/TP/AHRyBK9W3R3ZZaNLsMPdmc8RE64nH1nHKT0AGQTGeV03lnOPHf2s9bUQxjWDMNaBJ1MCFKiL0vniIiAiIgIiICIiAiIgIiICIiAiIgIiIND9K9iHUqdXgwlrvukYv/U+1eMbQ3gue2e6mXYDAaBIyA6ea+hd+rM1bGu0CSGFwH3e8fcCvmioyo7NhH4+C5ZSb9e3fDK61L6dHV6jnYiyTnmcz7Stz2Bt4U7fsajcjMggxDj+C12ztw/1g8OI0AmTwAgZ+Cv3u7l9Sa0loa0gdyo9uOeWETHtWbOtadJMt77Z7ZcDEGnE2cp4Dgqe1S0GB81X2Jd4Q9rhDoEddZVC7u5cc1zxx/s3ll/VBXIGip0jJPVTXNRVaC65Tpxxvba/R1SnaVsOTyfY1x+S+iV8++i/9p0P/J/I5fQS1x+mOX/QiIujkIiICIiAiIgIiICIiAiIgIiICIiAiIg4cJEHQr5p3m2SbS7r0G5BjyWZQMDu8yOkGPEFfS68e9OOzCypRu2t7r2mlUI1DgcVI+feHkFLNtY5arzS12zVpPDgw4hp481k9n39zd1hOIn4DjksdY7SwPa57WujgRIPithdvY1jSKTWMkz3WgSPn5rjnjXpx5b9qPeANaW8C3L4rAVawVbam1O0cTzJPtzVI1FvHGSOWWflVqvWnRS0BkqdJsq8xZyawZrdG/7C9t6vBtVgP3XHC73Er6XXyiF9Ebi7zUry3pjG3t2sAqMnvS3ul0cjr5rWDHLO9tmREXRyEREBERAREQEREBERAREQEREBFjdqbftbYTXr06fRzhPk0ZlaxtH0pWLAey7Ss7gGscwH+J4GXWCrJam28ovFdtela9j6OnSog6RNRw83QPctXvd6b+5H0lzVLeQcGD2UwAVr/nU8o+hdq7WoW1N1WtUaxrRJkiT0A1JPILxXfL0vmuypb07Sm6k8RNcl0jgSxsAHIHXJaXekwXEknSTmfaVgL4Q8jw+AVuOje0txav4ZhQQ7iVmKebQeYChq0F57k7zDcUGUirNOjzUjKZVmnTWLm6TjdaNNWWtXZjVPb0cRAWdukxcUrUkSpK2zXND6ha7Aym52MSMJPdp97g7GWQNclsNhs/E5rWjMkAeJyVffXawhtnSjAwzUcP8AuVAdZ+y3QeZ5LfDvLJjnkxx/avsT0r7Uo4WFzLhoyAqM73+9kE+JnVerbtek+zuGDt3NtasZtquAYfu1DAPgYK8NpWwa0mBPPjn/AGUzrfE3ML2eEeLyfUFtcsqNDqb2vadHMcHA+YUq+X9g7Wr2NTtLd5Y7iNWuGkOboV6BsP0wVAYuqLXD7dI4SP4DIPtCzeO/FmcewIsBsTfGyu8qVduL7D5Y72O18pWfWLNNCIigIiICIiAulaq1jS5zg1ozJcQAB1JUW0L1lCm6rUdhYwEk/hzPReG73b3Vbx5kltIHuU+A6u+074cFrHHaW6bpvX6UWUCW2tMViBm9xIZOegGbo8hnqvNNt787Qupx13MadWUZpt9xxHzJWKq1sWXMfE5eyFFTtyZ8Cu0xkc7arZzMmefHzKkpvIOZn4rlo7s8lyKZ1HNVF97A5sHMFVmVcJDCPA8FIx0ZHiulxTxZHL7J5qhfN7vQFYrbNDJrxxEH5LKUKmIFr9QoH08TTTd5H3grNixjtmXP1D5fgsm5i16pTIMcRkrlrtJzcnCR7/6ry8nHb3Hp4+STqsnh6IHKH9PYRrHiuaVZrjAIXDwy/Dv54/laD1l9jUPrFYN1djeOI8m/iVL+nVqndAwt5DRbnBlUvPjj+2yX+87baRRM1eDhozqOZhazaNLzid71LTs2jN2qmwzAH916+PjmE1Hk5OS53dc5R0/Mlc9qIhS9iQIg8VTrmCuunLadrZzULmiJy/qoGPcclM2jpKCu5pK2LY2/O0LWAyuXsboyqMbfCT3vesI4QVDUaUuqPZNg+ly3qQ25puou+03vsn+Yewr0Cwv6VdofSqNqNPFjgR7tF8qlXdkbZuLWoHW9Q03niNCP3mnJw8VzvHPjUyr6mRaxuZvfSvabWue0XAb32aSRq5oOrfgtnXKzXtuXYiIoryX0v7wlzxaMPdpw6pHF5EtaecAz4kcl5hUqTCs7VvnVajqjzLnuc4+JM+xY9j4dHmF6JNTTle0rG5+BPyI+atNOShcRDuMtkeRUgKogpnNw6rvb1MGIcxy9ijA7xhd3iZPMe/ig7udMFTupAj85KC2b3YVljsuoVRXdRxH94a9VFdMOR4j3q5VE5jULis2WylGC2nb4oqAa6j5rHAStoYJEHNYu62WS7uxBWLGoxZoHqr9ns18SQR45H2KWnYvZmAHeZR9V896nPjiPxlZ0u09Ggxupk8tT7ArP6SBkBny19wVSnVqRlSgdclJTfOUZ8QCtRFqm7Ee97yMvIK3QvWNPq4jyiAsdUqsYJdA+J8FV7erV/VjC3mrtGVuLw5lzg2eHHwVdlyzQZ9VBT2WBm4lx9yt06QboFd06cBx5LuXcBn1XBaTkuQyMggu/ogDJJEngsfUK71avCVC1knog4cBBJ0A9qx7H5kqe+r5EDTT8VTCm1ZrY22KlvVZVpmHscCOXUHoRl5r6O3Y27TvbdldmU5Obxa4es0/nQhfLTXL030K7f7K4dbPPdriW9KjR82/yhZzm4TqvbkRFxdHyZWq/n2qOZ8Rmo3+th48Pmpa7QMwvQ5lV/v8AmprKvMzzVPtMQI+sMx1H4qG3rwT4grOzTMgd4dVNEhw81StK2INPKQrtJ2fiFuJUtBmSsN1XWnopFpl1jNRxBIUzlHV4FBWDS09FyVZe2VG2mAs6WI2sQBSOXR3T+gUVHUOefkFRvLsMygF50aPmfkulxfEksojE46v/AA/FWdn7NwZnvPdAHHM8B1U3+FdNjbDqXNVjSMdR5hrJAHPPoACfJb/s30eVnsa59VlMPLRTwAVRBBOJ8EQ0Rhy4npns+5uzm2tBhHZi474qgAOcMRc5gc4iWOa0gEDLI6rZqGzTUbJMNmZ04zpoue7e96jenmF/6OrlrT2T213sLcbWgMAxSRhc90OgZmY1Wr17V1N5Y8YXNyIkGOOoJByPAr3LaNkabYdmwggjg6eDh1yEDnxWq78bFNxQddMoM7QFnqYseBre8XCQMhEAAkR7LMrjq27lSyV5nEKGo+NEq1soUDmrq5jQXFdtoVsADG5vcu4cGNLisZb1iS6qeEhv4qVXSo0NMHhw66yVHhJXWm6TidxUr6nuUV1dkp7K6dTe17Dhexwc0jg4GQfaqpdMlcNcg9T/AP2G6/yaf+7/AOVyvLsa5U8cTdd6jTUEjJ7TnzkaFcOr4siML+I4O6jr0U1QEkVGZO0c08Y1BUVyG1tO64ag6oKDzBkZEc/z7lE6rnI0P4yR7ZVuo1zThqAHqCPnqqtxbEd5ubePMeIWK1GS2PUlp8Vkab4Kw2xXwfFZWqYcF0xvTNbnuPu8b+s5pMMpNDnxq6ZwNB4TBz4AFZIbhXhLnPbSoMk5vqDC0dIkx4rTtlbduLVxfb1DTcRhdAacQ1AIcCCRnHj1XO0dv3Fyfpq1Sp0eTA8GjujyCXe/adabDdbIs6Wb79tQ/Zt6RqT0Dy4NWGv61IwKbXNA4veHOPkAGjy9qoNqSuKjeK0iw167NzChoZgKStXa0STC0jpUcGgkmAOKwlzcuruwUwQ3j/VQbQvnVnYRkOSy9hTFNkARxJ6rnvbetJLK2FJsDz8VYADiATAJzMTAOpgaxyUHaLnEqj3K4qmo2m7Gwtc2WEFzpZENJLoJJMZxxWwWldrmjMAgZgryTdLe1opuo1hRpwymG1nB04WmHB2ZLyGnutGUyt3s8FR7nUaoewsZhe4y12MEtDM/XAaD/EFwvj4+GfWnX7uM1tiq0swTP1iRnAHFaXv7eto2TwWAPqtLKdTuYpJlzMJ7wBEyQpqu2aFFtFz6zSKga91NzsNRrHBxa/Dq6HCI1zJByXmG8O3XXLwS3C1headMvL+zD8OIYjnEiQ3QTAV6usMPU+p67rFtEZnVTUhOZVdrpOs9V0u7qAu7mrbVuC8im1RXrw1gaOAXW1GZedVUvasrFv1qRIH5Qjauqq4uC5Lsis7XS7RH0ZPUIzRdKYikDzcfgu8ZKxHCLhFUZCqPrtzBAJHMcx+8F0NJtSCDnwcPz7lPVaWHk0mfunj5FR1rU+sw4Tx5HxCo4eTEVG4hzb8xwKo1qQboTh5n1mn5hWTdkd17S08wRB9qq3FzGTmv8CAB7ZWctLENkcLvNZq4bI6rBNqA5gEAczKy7aktCYlTtdInj+dUpN4nJQsWd3T2R+m3dK3M4XGXRwY0S/wyEeYW9ssfSqZ/JdnOJVveewFtdV6TBDWVHBozybMtGeuRCxtN0lJTSUXIYM1hb+9dUMDRTXgc94Y0EkkAACSSeAA1K3vYnorviwPNJjCRpVfDvYAY81nK/GpGlbNtAwY35fFWWVzUMjusHtKv747tXloWivSwscYD2kOYTrGIaGBMGF2ud3LulbtuKlE06JLWtLyAXYhIIZMwYJzSWGlQOCYyoAZgDVKlSMlpExco6lUwG4jDSSBJgE6kDgfBQmoo3PUFircOOZJLjGZMnLIZ+CgxQoS9dHVFBO6tCpVqmIrrUqLikFLVTl0CFja7pKu13QFjnFZyqx2p6yu1Q5AJSyErvZsxVGjr/VRV65ZAps5AT5oXTnw0CjvahdUMcTHkp6rYAHJbZQYUXGJFRnL71XeC6UPVHgiLTKptn9X5hdNn/qguEWMvbU9Om0/q+CkoeqFwiYlSt1XoXoW/aJ/0Kn81NEVy9JPbGekn9pXX32f8dNazT4+CIk9LWT9Gv7Xtv9Q/yuX02iLnl7anp516c/2e3/WZ/JUUHpV/ZFv9+3/4nrhEnweP2nr+R+Cpj1iiLoxHdy6IiCF6jeiKKgcpaWiIpFRXSpFcos32sSfVVjZP6weB+CIrPY7U/wBYFauuPiiLUZquiIg//9k=</t>
         </is>
       </c>
     </row>
@@ -2409,22 +2409,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ANSHUL KAMBOJ</t>
+          <t>KAGISO RABADA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>smat2023_076</t>
+          <t>t20blast2016_116</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -2442,91 +2442,91 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M16" t="n">
+        <v>4</v>
+      </c>
+      <c r="N16" t="n">
+        <v>28</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>3</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="W16" t="n">
+        <v>3</v>
+      </c>
+      <c r="X16" t="n">
         <v>2</v>
       </c>
-      <c r="N16" t="n">
-        <v>8</v>
-      </c>
-      <c r="O16" t="n">
-        <v>1</v>
-      </c>
-      <c r="P16" t="n">
+      <c r="Y16" t="n">
         <v>4</v>
       </c>
-      <c r="Q16" t="n">
-        <v>8</v>
-      </c>
-      <c r="R16" t="n">
-        <v>12</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>1</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>100</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1</v>
-      </c>
-      <c r="X16" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y16" t="n">
+      <c r="Z16" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA16" t="n">
         <v>2</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="AB16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH16" t="n">
         <v>29</v>
       </c>
-      <c r="AA16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
+      <c r="AI16" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK16" t="n">
         <v>2</v>
       </c>
-      <c r="AD16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>22</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>35</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>1</v>
-      </c>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>All-Rounder</t>
+          <t>Bowler</t>
         </is>
       </c>
       <c r="AM16" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFRgWFRYZGRgYHCEaHBwcHBwhIRocIRoaIRwaHBwcIS4lHB4rIRocJjgmKy8xNTU1HCQ7QDs0Py40NTEBDAwMEA8QHxISHzErJSw2NDQ0NDQ0NDQ0NDE0NDQ0NDQ0NDQ0NDQxNDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NP/AABEIAOIA3wMBIgACEQEDEQH/xAAcAAAABwEBAAAAAAAAAAAAAAAAAQIDBAUGBwj/xABFEAACAQIEAwUFBAkBBgcBAAABAhEAAwQSITEFQVEGImFxgRMykaHwQrHB0QcUI1JicoKSsuEzY3OiwvEVJDRDU9LiFv/EABoBAAIDAQEAAAAAAAAAAAAAAAECAAMEBQb/xAApEQACAgICAQQBAwUAAAAAAAAAAQIRAyESMUETIjJRBHGx8BQjM2GB/9oADAMBAAIRAxEAPwC/SyTicGQA4S2stmETlcy0LpMzMDethjXYqoyPo6HukGQGB0IPhzjespj+DJcvK5AIFsIAwMMMhUiASds0aCPGp+C4GLCRZu3bbsMoUOXRDmUgqlwlQxCx07xrPGaUaGkvdZc2sPmuZ7gBI0UAmAREkjZmkDWNCojrVnVJY/XLbKH9jdQvqy5rbIpOkqSy3GkiYK86bt9q7K6YlLuFb/fIQnkLqyh/uq6Mk2VyTL+aE0i1dVwGVgynYqQR8RSqsFFTSqRTd9gAZ+Uz8tahBrG4sW0Z2jKokmQIHUzXFf0k9pVxDIltcqJJmAC7EGG05Qfvq5/SPxh1YWgza6lTG32djJ9f+/NcVDHx50kn4HUfJXs5MdPo0TWj+XlUpLBHI+XhFWFjh7uNqVySGjBsrGO4I00pl3JMD/tV7e4M4WYOnhVW2DbmIqKaY0oNCLSEg67f6U97MgZmJPKBz15+GtPYfh78hNKv2XWQR9b0Oasig6BYvxAC+MHX6NaPs5x9LLjOpgMGGUkZWBXXTXZSDGsH0rJtLaQJ/wBPr4U9Yu5O6Qw8wPjFFMDR6ZwGKNxA+QqGEiSpkHYypOlSprF/o24uL+GyFpe0QrD+EiUbyIEf0+tbMmrVsqap0CaI0KEUSBUKFCoAFFRmiNQgRpBpVJNEhy6z29soxTEWpYQ3tEQhZygaSzFSIiAsaVrOCdp8PiWGQMuSDLKArZ5y5GUkGYMDQ93XXSud2+GWXd0dHCAyTIMnODpoPHTN61b4nhuHSwyIXQEi73YEZA8whzAaNucxrBao2cU3R1JGLNJACjbqSeZjbQ/OpNxZBHURXLgcSQGt3MoS24KaT7XJ+yYysHLpoYGgMVEtdtOLYeP1jDpeCj3spVunvWyU/wCWnhJNNFcsbR0L/wDmLAIa3nstEZrTlZ8WX3X/AKlO/iaUbOOt+69rELpo4Np4595Aysf6FrM8N/SphWhcRbu2G0JJGdBmEiGXvfFRWx4ZxzDYkTYv27ngrAkea7j1FXR60VuP2QV7RW10xCvhm2/bABCZgReUm2Z5DMD4VZ37nczL3pHdgiD0M7R41LZQRBEg8jVFiOytgybJfDM0ybDZFad81uCjT1Kz401itHn/ALR8Ra5ibju0kuYjlrA+AqOi5iqjc6/X3+lFxvClMTdQwSlx1MAAGHIkAbDTarbgSjprVcnqy2EbdEnBcOA3q/wFtQNAKjhRUiwkVnk2zdCCRaqqxyqtxXAkeSoian4epSCkGcEVuE4QqL51HxPBlM6amr2ktUsnE51xXh2QxETVWEy6dNBW94rhVuA6a1hMdYZHZddI+cx91X45Xoy5ocdnX/0XYI+wW/Ihle2I1kC4GGYzrDZ46ZjW9rMfo6wvs+H2dZLg3D/WxIHoIHpWnrSujI3sFChRUwoKFCiJqEBSTRmiNREEmiNHRUQnHsONbjIjKSy+8ZVve27o08ZPL1no5uOikaRLjoqtMHwLZB4iajPwuwEJV1dw2Z0VyACq6gZFlgoaTkYjSZA2kO17J3NCFzLAEaHRcrDUETqddBrXNbN8Ut/oXSkTEiSOXNQVBnrqw+PjUwJ0rJYPiN1Fu3bluSioFEFZzXO8AdfMx+6KubXaS1lDXFdJ6gNPll70eMVF5I3VIlYvhVq6f2ltGPUjX471nsZ2GsMc1tmtt9k75TIMjZp5b8602G4nYuGEuoSeRbK39rQflU/2dMrBSZjsPf4xhP8AZX/boJhbnf0Gwloedxo1XOE/SiEOXG4W5aOxZO8ukScrAMBqNs1WzWqgcQ9koy3cpDbKwmeunMUyyNCPHFnJ+1F+3cxd57JzI7l1aCJDQx0YSDJI16VO4NhzlzRpTnabhyJjECAZLqq4jY6spj+351Mx+KW2oHrHhT3aJCNO2PKxp9MQRWau8fjZRSV7RA6EVXwkzR60UbnDYkEfXwqYt7TfWNKwmH4+u0fU+FXWH4jzmRFVyTXY8Zxl0aVHEb+vWhmrPni+Ud6NDv56ifhTicYRtJE1FYzkkWdxBvWb7VsuVe6M0iDGu/Wrm3ig3MVX4/AtdxOFQfbuKp0+yGDNp4KGPpVmNe4pzNcTrPZ/CC1hrFsT3LaDXecon51YUPKimttHMDopoiaFGiAmhRUCaJAE0kmgaKoBgoGhRGoSzkaYVURHW26MXYklj7wCwUbKPPnvvV5dwMFMrFCyMzKuZZhmHuiBrG0c9OlRltotnDqyFC73GILAkftAoImAQY+HOuiZFuOSwBVNRmGhZgOvRdP6vCuf2zY5UjDXgLKPCq6XGsBc4Byq7XZBIIPdCjnyPWqTiXFMIIY2faSxUtafaBOz5uu0iuo3uEYe6pR0VlDBo1BBgwe6QftNr4mqnEfo/wAG3u+0Xp3s0eXtA1OoWJzXkwNjCYS8WFv2oZN1ZVH70EEMQR3akYYOwy4W/bHOFuDOfMMQw8gBWmxPZdcKGdXLZ9IIAiAxnQwd+grmX6qi6CLjc9dB+dJxp7HvSaNdb4hj7TZbqBlHN0ifIpE/A1QdqsY96/acKUKJAGu4JJOvWYpnBDEpLpce0o3KuVUeYBg+VC/xB8S3ffOyCA+VVkGTHdAzajc660HZbCW9kRZuXrMz3c5I5DSdOkn76a402ZzptpUjg9grdJYzKGP7lmrA4RW1Io3pDcbbMY1lyGKp7onXn5dagWlLTCjQSSJrfnhzAyjAeBpB4YYhggHOFGvnprTrJQjwNvsxNhB61suFcLd0DTypkcHTOCFA8gNfGtnwrDwhA6Uk5ci3Fio5zxdmViuaI51UjEEGMwB8Z++txxDgK3HJM+hjX4Gq6/2eRmBcXBEAgBSGA/iG3pRhJJbEyY5N6KzBPcHeDZh4Ga6B2JxSnEJcvMALauVkEnO2RBAA1GVn1qgbgoZ86Ap4DQHzFWbYV8gS2Yd4TTcyYgHlM1PUp2D0m1TOvo4IBBkESCOYOxo6hYVktpbsqykoqpEkaKMuhiCZEVOVZEitikjC0JoqBpNMKHNCioVCAmhQmkk0QBk0kmgTVBxjtRatQqnOx6SQIMHXmfKg2kArBgEQ2hFu2FUDK0lgSyF8pFwqurHWCQeZq3fGOuYmwXyqjwjjXMveALASFgHWJBnSIqi4d+uooF+610gzmW4ySOmVRHzqb+t32gqqbw2YK0KJ0krmOaAPU9KwWjbwkT140LSl3t4gTcZTFssYULlaE1yQw1jcNUm12twp3vhTzDo6R6sIqGt9iRDFAATCympjcKddqfJdo75IG4IVp88wNRTronpCuKcUt3MotXLVwqcxVbiTpG4Lac9atXw1u6AblhGnmQrfA1i8ZktXkzogUuro+RRlfNOVyAIXcj120qdawyO7utsKJy/s3ZJYE527viY/pqLJTA4NpI0OI4LhbihXsIVGwZBA8gRArHcb7H2LCO9hnBY6A5YXXNK5QIAggA1eKCvu3cSv9SuPg4qHxTEXigi6r9Vu2Y0jWTbYdY2O+xouUWtDRjJSRzxwEdRBnUNp3ZPMHlJA0py3fqHxHGZbhRrbKQwyxdlFOYGQrIHYESBJ50pN6VrRojL3FtZel3NKjWGp2+8CaSzRaaGrbya0fDE7hrPWr1oDutJ5+dXvDcWIjrTN6FiJuaNTsCkYkqTMwenWmy+lJexuNj7ZabwVs5/aLH7IZ/UEZR6sR6A1CuXKquKcba0wRGMFe+VjUyDB8oFWQ3LZRnlxi6OnYzFH9YAZ4RVzGWhR3WJJnT41Gx3ajDIQPbyT+5DwMw1JXQbbb61yviXaS/fHfcmdPdAzdOUE1Ad2SM6NmP8ApuCT+WtaW/o5dWdXu9srC6C8W8kc8h1EUeG7eYaIuLdU66lBB6RB6fdXI3xKidY6zHw21ppMZHUjrpp5CPGopSBR2G12/wAMScyXUHVlSPk+9JxX6QcIjAKHeTqQAI8QHIzb8vGuPLcZ5JSRy5E+RG+tKSwDqV00OWTR5sNHaeH9s8LedUVnV3MAOsCehZSQD61oFYESCCOo/OvO5cqO7p+M9aWbrFYObLvlGinxK7EimU2Kzu3EeJC3AADFh+9EdDMEa/WlYTtBiVtMvtQwuFZgRHKYj7Wusidd+VYd8c+WA5yxtnO3SNuQ+FRLuKls5kk6GWkmBH2pOn4eFTlZDpz8WxCyGsgHwcnmBABtjrzpi/2hKMJtuG8Mp+MkaVZ8cZc6sCDqdv5p/AVU3sPnbMxy/CY/CucmzsxjGk6LLh/GQ3fcBBIBzdTJMQfAfGkca4se8LLM2XLoqGNTqMwBJOUk6bCqN7Z/V7oB5M4gwQfamNQZHdtn0mhw0OmGQuxL5WzFmkySwG/gfup4q0Z82pNIlcQxV57P7REBLwAGViQoMkgnfUctvOk4PF6hXKnKSsFJClQpbS2+YDvSe6d5ik4m+wNvfMoDE8iSHaNP5ln1p7D8MdyAH0Z5LjTU5d1nXbedPuDi7MzbTNph9UU6aqD3TmERpDQJEQfWonFNF+v3lpy1chQqDYmSduR0HPf5UCk6tr5/lUo2xejL9p+Hh7DvkkopYN0jXQ+m1ZO1cBAI2NbzFYi87vZJQ22BUSjZgCmvfDZSJJ3X1rmmDuaZTuNPWnS0I3UrNBh3FLxNxSImqdr5C93eqm5iXDd+ddu6TQUbZY50gsZhlV5BM+Hn1FW3DOIOBBMR86rlu284zlvIiJ8pq3Awy94OxBEbAR5ydaaT1RIp3aLbg2DQubrvnc7T9nwA5VbOKxtvEBB3LyzsJImNdKvuGYl2Q59wfjVcl5LFLwLxWx+Hx0rKYjhN92lUQbbEDYQNAY5SdN60WJclso0jU/MAff8AClWS0HX5VfiVKzn/AJOROXH6Mhf4FiR9gt5Mp/GpFrD3pspcR8igggDbvOBqvQZee1a7K3UfCiZTGxJG8eJAHzIqzkUKSfRg8RhmLHuOqzoCraeppsgLAg6ddNfKt05KnWdD0J3E6R4Uh7pABytr1BHpqND4UVKyNGO/WQbahws52hucAKf+v5Cm0xRXQBR1P3yR5VryM5Ay6kwJjcmKZxnY+8TobXxI/wCmg5Lpi2Zo4gbyJ+Z9OVJUg84Hj4fXSrVuyGLXVVtn+ofiKj3uzOMGptyAOTJp150eUfsBFOHfQhGIOogZhtudKS2Gc/8AtuR/K35VbNwu+oEWmICqNp2UA7eINN+yvLINtwY07rbyNh5TRUl9lTlJbSOu4vC2nSP1kDWQSASD4At0JFR//BkI/wDW29eqr/8AeoH6g/IqfX8xSWwjj7PwIP3VzeTOgs0l0LxHAbLZR+tIcrMfdOpKMjDQ/wATH1NIv8BMKgxFuIgCG5ddJNMtYPND/afypJtL0+Q/KmWRoR5HJ2x/E8Iz5Qty0QJZfe3nSIX9wIPQ0eAuPbKqoVgN2kRpMaGCdhy51G9kv7o+Aowo6fKp6hOSfg0uHAYH9qgiInMNNRqSInQafnS4WJ9vagnqfurMhV8PgPypxEBIA1JMADmTsKX1JPodZH4Lc8Oy5r5u2yhOpGY8tvOuT8TCpiLgU90uxU7SCa6z2wwTLw4+z19kAzRzWe+fmW9K49jJYKw3HLrWxRSVMMZSlsko1P3EDLA0NVlm+I8PH7j41a4dgQDVcotGiMkxpMfkBV0zr0KzUnBcVtLollVPXJr8TUpHQ9JqYiWmEkAH0pWy5Nke2iv3mAJPgKfS4FU9BSGCgb1K4HhhccO8i0h3gw7iDkBHSQT6DnS77Ys5pD2G4Lek+0Q25Bck5W0gZQYaVPKI3n0O5hLiCERnBPvDJ3dOheSeURWlVMOea+oP4inVtWuTJ/copllZheOMnbozouWmtiMRlKoS9s5dX0MAZiZnoBtyk1U4vNmgkhSp92TqJ5gQSdIAJ8a3bYVGESpHmppluDWjrkQ+OUfhvReRsixL6MPadrTA+0DELmYuI8ApljB31kfdK+J4m8+HW4yPBaQcndiIHnr13raLwa2DIWD5tzjx8BTtnh+QEIxUHdRt8NhQjNoLxWcrwWJYkSW3jx9DuD/pVnxLAXbbwmMdZC925cYmSJgQTOnQaVt//AbUyF1/1nrTmL4OlwlnXOWidWAJUAA5QwAMKNQOVM527BDFSaZz9MPj4bLcLkKrgKwMq6kqRn8CGgwYHWoVziWKLQLh5kDLb/fOXXKRsVG+sV0BuzGHkn2Y8szx6DPp6VBvdkLbNmiDED3oG/KYPrUU/v8AYMsUa6Mre4hiVJClSNYlV2H/AGqOON39WhSR/CY6cj/Ea1l/shm1znckQxEE78qYPZa4vusdNNSp5+IHU03qRMzwmiV6cDmq1HI508tzyrI0WKRN9rFA4jrUL2nnSc886HEPIml0O6r/AGimzbtn7I+f4GqvH8TtWBNxws7Lux8lGvrtVBie2Rn9nZkdXaP+Vfzp44ZS6ROSNg2FtnqP6vzmo2IxVvCPauORkZyjFiJt5lYLcjmobQ9A08qqOA8eGJzWyoS7lJTUlGgbeBGhidRPQ1j+IuzsyvJbXNm3OsGfgfKteD8R3yk+iuUl9HfeGXgylGg8iDzrlfbXsocK+ZATYY90/wDxn/4z4dD6bjXRdg+LG5hkLNL2ybbnnK+6T4lCpJ6zW6a3bxFso6hlYQwPOrpx8FmOfF2ebcTaIMj1HI03bxUaGR93x6V0DtX2PbDsWUF7JOjc16K/4HY+BrJXOFzWflWpGrjyVxIv6zzH3+FO2+IFTqZpScIE1aYPhqrrFK5RGjCY3hrb3PelV59TXQ+yz27ln9X2QiVI+y3Jh4ydesmsmyQjeRpzsHizmCz3kOU+nXzEGjF2DJD27LPE3glx7TuodDlZSYPUHXcEEEHoaMPOxB8qs/0icAN+0uKtg50WLgWAWTk2o3Uk+hPSuXJ3W0Yhx0JU+oo/0qe0zC7N9n8aMPWc4dx11bJfUuunve+AdmR+Y8yRy03rTJgM4D2++jaqwP3g6gjYiqsuGUFfaJsJcQ42cj1NLGNufvt/caeThbDcges08vDk5kny2qmxqkRV4jdH2z8jRji1794n+kfgKnrhba7IreYn76cYwNFAHgtS2N7vsh2+I4g7JPmh++RUtL987og82/ImksT1+VJM9R9elTkyJv7Jmd+eWfAn8qBZugqIqk7fI0otlGhJPpA/OhybG5Mp1YUstTGsTtGutV17jKgkKJjmdvQbn5VfjxSyOkjO5KPZosFbVyRmggTEbj1rO8bxd227IxyjkV0lTsZ3B5eYNRcLxllxNt2PdJyabQ0D78vwq67cYXNbS6N0OU/yt+RA/uroY8EYUpJWVubfRzrE2u+xOsmZJMnzO5oshAEoyq20gwfCTUm8OdNS7aDM8ctTHx0FNJcXRZF2grOIa263EWGQgghTEj96PDQ+B8a0HaK2r+zxiDuXVAcfuuJkGPUeanrVBausoMEgHQj5EEHnvWi7LEX7F/CkjUZ08DoD5AMFP9RqQlTJJWis4Lxk4HEloLWbgAdRvl1gj+JZkeZHOa67wviS9y5bcPbcSrDaPw6Ecq4ldBYHMIKtBB5RoR8asuz/ABhsE53bDue+m+T+NR1HMcx6RZOF7QkZHoUBXXUAgiCDqCOhHMVjOO9iRq+H05m2T/iTt5H48quuz2NDqIYEMAysDIIIkEHoRV/WaUFLTNEJyjtHFnwJVirKVYbgiCPMGnEwwFdG7U3cElvNjHVBsrT3yeiASznwAPlXPsPjMPdYiw7EbgOoViOoAJDCNdNuYG1ZZ4JR2to3Y/yIy09MTeTYeNU3ZsGzxJVM5LkjwkSVJ8IkeorTNZBqLh8KP1qwY2ZidJ+ww+8ilg6kPlScTqmFURG4PLw6Vyjt/wBn/wBXdnQfsnIaI907Sp5EGFPgU3Mmul4C73dCCR9R51B7XYnDNZNu66BipYIWGYr9o5d4yyfStsDmM4goJ7ywwAJOonKN46kTMedazsZxMhvZMe6/u+DRofUD5Cs/xPDFLzhgA0wY2bo/qCPhTeEulCHG4gjzGv5U/HlcWK3WzqgvdJ+FLF8dTVfw/Gq+dZ9x9P5XVXT0AfL/AE1NziuXKDjJo0J2rFZx9ChKmmyRQIpQ0KIXx+NGkDX79fkdKb9aGbxqInFAcEx3vlSQvkfiKBJpsk1GicUYXiXEy8qvdT5nzP4VTPfO/Nd/KnHeotxoPmCPy+degjGMFUUcy3J2x/E95SAdxoeh5EetdFxbi/gS4Hv2s48wocesiuZ2326fca6N2VYPg0X+FrfwLLz8KTJ4Y8Tn5WisXXRiUMaa6Db6+uqhtQjrUlFSJGTiRmGsnmZPnz0j69NLLhvEETE2rqqEg5Xg6FW0J9AZ+HnUNrY+vry+VIa39b1U4SRapIuO1GB9niXgd24BcHnPeHxWf6qqpmtHxp/a4bDXTq2Uox8Ygz6ofjWcUSKujtCMv+wnapcI/wCr4gkWCxKOJPsiTJBA1KE66bE9CYuO1n6UH1tYGFA09u41b/hqdAP4mmenOsM9sMPGmXw8iDSShuxlIh4nGvcuZ8RmdzuzsxJ8JkEDoARFPpdRGRrWZCDrDkyeRAIlSD4mot9SvdOo5TRpbzahF+JFRILZ0zhXEReth/tA5WjrAMjoCCDHKapuO8ZezesvbPeRs0cmXZlPgQSPDfcU32TxARHtnKDJuCDMiAG36d341VcVcveLLHcER9eFYlj/AL1Vo3Sy3hvydo4TjbeKtLcRipcjURmUggtbcbEgaeRkHUGsb+krJ+sKEy+1Fv8AaEc8wIUEfvZfkV8Ky/BeOXsKzNh2Cl1ysCARPJwDoGGoB8TININ5nJdyWZiSxJkkk6k9TW2OOpGBytANw3bKsT37MW36lDOQ+hlfVajM9C2wt3YJhLgKN4A7H+lgG/pFN3AQSDoRoR0I3FGqFuzW9ncURdYT72HsN6i2RPzrSJcmsh2VDNdusNktWE9fZgkVp2brpXMzpc3/AMNWN+0mhx1o81QA9Hnqmh7JrHzpsseo+vOontjy++i9pUoNkpnNJ9pUf2h5UPa9RP113oNEs5m7keI+dNM089Dsfw86cdqjSAegY/Butd85iHF116jX685rofYN/wDywB5O/wDlP41z0LHxrcdhbn7Jx0f/AKVqvL0PHsy+KXK7jozD4E00DT3FTF66P94/+bVGVqKeiUOGjpE0c1AlzZbNgSD9i/p6qv4sapkGtWmDf/y10f7xD9fCqwb0Y+SMJtDSnXnRkTRIeVMCyLiLIYGqpgyHwq+dajXbU0ko2MmQ8HiipDKdR8wdGH4+lP8AeJH8Rk1BvWTbaRtVraAOU0sYq78hcnVeB5RUhDTSinFq2hbG8dbzJ4imrr5lV+bDKf5lgH4jKfMmpg1061XKYDoeoYeYMEfBif6RSyIjVdiLhK3jG7r/AIkD5LWkNwjn6Vk+w7HJdiPeT7nrUMa5Gf8AyM1w+KHGcUSODTDN4Gkq461WOPNHIU0X9KRmmk79agB0OaBceNMlooi/jFAJzRrjL/EOY5ilkBhI91vkeVOSDpzphBlYodm1HnXd6OeSUJKwdxWr7D3oF1fEN8Vj8KyydT01q57G3ou3R/AD9/51Xl+IY9lfxR/297/iP/m1MBqLH3JvXf8AiP8A5tSFaouhiQGowaZDHzpWbwo2AtMO0Yd/4rij+1CfxqCDrT5cCyig+8zv8wg/wajwuAu3NUtuw6hTl03lvdHxoxaStkpsaWkv1FX2G7NPlz3XyoPspDN5FvcXzBbyqDxXDKjjKCEdZUEzEd1gTz7wJ8iKKkpdA4tEGZFNOtKTQwaMjlTEG/Zh1g0xgwVlDup08qWjlWJ5cxTt/cEbEfDwof7COqaWG1phGkUbNpTCkhW1qBxRMrqeTflFPMsiQSProdKi4xXIWSCoYRpBEkCkl0MkXPY9yHdZ0KyfMER95+Na9HPpWW7I4SRcunRVK2wertLQPELbk/zCtIbh6iuZ+TXM14uh0uedMsfKhnNAkVnHAxIpLOaWdtqQTUogB9aURaiJpOYbVKIc6W4dnHkRRYpWADDWNQRTxXkdqUixodq7leDnWuwnuShI6flUrsxfi+D+9bj7/wAqrVBCunQGPLcVI4ECMQvQAD7xVcuiyIxcuy7nq7H4sacR6r7dydeuvxqUjUEyE0PQL0wGqRhEDuinYnXl3Rq3/KDTWCjTWrLhLNtCZuhVChtC2dlI6e+D8a3WC7P3Utp7Y2reT7TsXbWdDsANdg243rEcLx8rac727hO2pi6Luh5e+fhXTeKXEN9GuwbRWVOuUk7ExvoR8qz5p1FJItgtti7HBLRtMxuNdJVoMwoMEyFXxM6k61zXtPhgltO6wIc+8VJh1U/Z0HuAxyk10TBuFTEugIRu6g/jMrpPiRXOe192FtoNJLNBy6ABUHugD3hc18KmGTegzWjNtRM1JJpLGthQEXg+e9IUx5UV1tqbZxQYUO2n1Ip2aj5u8aczUUQfVqk4DC27rol1/ZoT3n07oAJ0nmSAB4kVADVN4fdy3EPRh99LP4sK7Nm2TKiWEKWbchFb33LRmuuDqGaBAOoG8E5VZa2ZpQu9fr0oe0HOuLKTk7ZsVJUIE7T9fjRhjThAPOiKUBhpn8xSWf6MU81umWQg6fW9EgHucjRjb6NNnX/Sh9bT0qAMPRqwpuibSu6c4bvXArz1U/KfzqX2fMhmO6quvr/+aqnUlmJ6QKsuF9zDXm8wP7DHzNZptlsUUtnYVKRqiJTympFkZLV6n4Huo7+Hs18zBb/l++qpGq2x/cRLXNRLfzNqabt0AmcDxQV8rkBXjUyAGHuknkNSJ5SDyrp/BeMhE9ndQvaXqFLWhpIYTquaYWAY2zDbkOGwrsJCmBuY0q14fxO4gCOhuJsNSrqP3VfWV/hYEdIozxN+LQYzSOlcc43austq0VKL3jmXuER3iTuuVZ1I5Nziua8SvvibzMisyjurO+UaAt/EfePixqxxxc2ittHVGj2jOAGiZVIUmFkAk8+7oANadsV7NSqMZO8eHU8+lHHiS2ugSk+mRryFCVO43HQ01NFcvM2rGfh+FNM1WMA4+u+1GJHuqFHU7n8TTbPGoMRSVcnU60CBXDDfXSnM9R7796lKdKFkHC9OpcjWohNP4ZMzBepA+Jilb0FKzdWTmQMTr+OlAORvsKLDEZmXYHUfQqWVXY6RXH7NrjTojPc06TSVxJ0pNxddPo8qYmCdI8Y3+hQFsnDE+fyo/agk+G/KKrmaNSfOeX+lOo06j7j8j6VApkvKBpNNsRofvptX6cqN7h5aiimExIpK0KFdw5hFue8PWrAf+jf+Yf5pQoVRlLoGfWnrdHQpUFkzh3+2t/zCpXEP9q/8xoUKePYH0O2rrSgzGI2kx8KtsJ7y/wAw++ioV0Y/F/zwZn8iPxq82aMxjpJj4VVmhQrGX+WJpD0dCgEQNqXb2oUKi7IM3t6Xb2oUKHkIlt6l8N99P5h/kKOhSz+L/QMfkjYW/fX1qcNz60VCuOjfl7NTwZz+sJak+z9mDk+zMb5dqy/aFz7fc8h6SdKFCr5/AoXZBfl9cqL93zH3ChQqgYA931pK7fD8KFCiFn//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMQEBUQEBMWFRUQFRAQEBUQGBcVFQ8VFRUWFxUVFRUYHiggGBolGxYVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGi0lHyUtLSstLS8tLS0tLS0tLS0tLS0tLS0tLS0tLSstLS0tLS0tLSstLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAACAAEDBAYFBwj/xABAEAACAQICBwYEAwYHAAIDAAABAgADEQQhBRIxUWFx8AYTQYGRoSKx0eEyQsEHFDNSYnIjU4KSorLxQ8JUc6P/xAAaAQACAwEBAAAAAAAAAAAAAAABAgADBAUG/8QAKxEAAgIBBAEDAwMFAAAAAAAAAAECEQMEEiExQRNRcSIyYaGx4QUUIzOB/9oADAMBAAIRAxEAPwDye0e0ILHCyqzPYIEK0fVhBYBbBEIRwsIJIBsYdbZqux2KLk4cnMXantzH5ly9fWZgJ1nJsM7U3V0NmQhlOe36RMkd0aHxZfTnuPT0wTb/APtJlwbb/wDtINHYxa1Nai3sw2fF8J2EZDwNxLytz/5/Scx2uDsp2rQK4Rt//aGMI2/5yRWHH/nCNQAXN7DM318oCWRfujb/AJwXw5G1gOdxMh2k7a2vTwvI1Tc3/sB+ZmIxeOqVTrVHZjtJYk2+0149JKSuToplm9j18OhNu9Qn+6THDHf854mCcjvna0P2lr4c2DFlyujkkeR8I8tFx9LAs78o9R/djv8AnG/djv8AnKmiNLJiqevTvcZOud0PH6y75H3mGUXF0y9O1aB/djv+cX7uerwrcD7xW4fOAI3cR+56vH8vnHHL5wEB7rq/3iNPq/3h+XzjHl8/pIQjK9XkbL1eTHl8/pAJ4QkIGEiYdZSwx4SNjwkCiGx6tFCvwikCeUWhAQgBHCidc89YIEcCGFEIKJAWCFhARwohhRIK5AherwgsMKu+GEXfAI5Gg7G6QFOoaLoHFU/Bc21X3DmPcDfNytv/AMcev2nlSAAggkEEEEbQRsM9K0BW/eaIqAi4+GoM8mG3x8cj5zHqIU9yOloc9r0346Ogtv8AIHrMj2/0uEQYanTCs4DVCNur4L5kegmyGDbf/wBvrPOdN4I1sVWcjWCuaf8AtAH6e8GlinO34NmR8UjhYbQpf4qjWB2AWJ953MBoSiPy3OWbZyQDIDdaX9Fp8QM1OUmxoxSJF7O0tW/dLYDcJxsXoegbjuwLbCuVp6AKgNMjgZkMfSNzYQStdDJX2Z/CJUwdUVqR11FtdT+ZfEHePlPSsFikrU1qoo1XAYfQ8ZicP8R1SJoeyVIqlSlfKnUuvBWF7et5XqY7obvKK4/TKjt/6Y4/thd2eMWoeMwFw3+mPb+mOEPGPqf3SEGtw94JHD3kmrz9I2rz9JCETDgfWRsOBkxXn6SNl4H0MhCuw4SJxwlhxwPpIXA3H0hCRRR7DcfQx5CHlMIXiAjgTrnnRxeOL8YgIQHXRkFbHF4YvGA66MMdbPrAK2OL8YYvGXkPb6yRRwHt9YCtsdbzu9k9IdzXC1L93VsjZlQpv8LXG45HgTunFUcB6D6wwvAeg+sWSUlTJHI4SUl4PYhgx/L/AP0Mz1XRwWpVJX8zsPG989vjtknZnSprYchtXXojVa5a7C3wtlcZ7OYMo6GxBZXos+s6qKme22wnhmNmyVaSO2bTO9v9SCnHo4uMpBWLHZfLjwkuEx3djOkWG9RItIB6hYKwBBNri8p4dMSGCmqdTVu3w/Fr2PwgXtq31c77PCW8NsvtpGkwWORswCN6tKulcdRQXa+exRtMWCU3C1BmdtvD0nKxlNi7atgVuBcX8CQTwuAMt/CKuXQ7fFkWHxIaotkKgn83jym30ThhZmA/EVG7YPvMLox6pdWcgtrNroPw00/LZm/GTuAHPwmz0NWY1aq/lC0WUEnInXDW/wBokzqsTKe5I63c8Pf7Ru64HryhWO4RtU7hOYWjd3wPXlF3fOEF5RavKQAPd8+vKMU59eUMryjEdXksJEyc+vKRsnPrykrL1eRMvV5AogdefXlIXXn15Sd16vIXHV4RkR25xRW6vGhIeVgQhELQsp1zzdiEICMLQgRILY4EMCMCIYI4xWI2OqwwvKJWHGGrDjII2OqDcIYQbhEGHH3kgYbz6mKI2X9BY393rB/ysClUAnNG25DaRt8ppcGvdVwCoGuXUn+dbAqVPipsD5zHBxvPqZseyuJp1qLU3/iYYa9Mnaadxfnq7OREW6kmb9BqKvHLp9fJUxNDVrNuOY4y7TpqBfxlTTtwRbwORlAaR1B8Rz2C8M41M7mOVx5LmFxtE1gr1VDMT8Fxr89Xadh9JFjWpGqQrqGX4gCQGYcpXD06pJIT4tuQzO8nbfjOeMNRWrdQuscwzZsDs/Ec4Fj8jufFHVFP4svHwmi0HROvVa1h/hopsc7C7W4fF85ntH5nX8NnnNrgqFqa8gfXPfK8/wBGKvcqbuQfn7GLz9jCKddGNqddGc4YbW6sYtY8fSPq9dGLV6t95CA6x4+n3glzx9IZXl6feCR1b7yEImc8fT7yJnPH0k7Ly9PvImXl6feEJXd+B9JA78DLLpy685A68oUMQa/D2jwrcooQnlYhCMBCAnXPL2OBwhAcIwXq8IL1eBisIcpIo4SML1f7wwvV/vAKyRRwkq8pCq9X+8kVOr/eRiMmXkOvOSLyHXnIVTq/3kip1rD6xStkw5dess4HEmlUV1GYyO3MEWIOfiCZTCcf+Q+s3v7O+zWuGxGIQFHU06SvmHB/E9r7PAHiZIw3OhsMHKaUTP1cWKjGmx+JPA7SPBhvB+s5/wC7gkhgD/LfOdXtz2KfCv31Ms1An4HBJqYUnYrHxXc3kc9uXp6bakwp4rIj+HVH4XH9Q6/WXzjfyemxuvg7mHbDoD3lNbnL8K5+oyMq1FoPcLSUAixOrtO+5k66UpFb5HkQR5SsccjNkNnvETlZdKSo7OgNHFiqr+AfGx4eAE2NuXXnIdFUwlFLMASqs1t5Av4y0W/r9/vObqMu+VeELFEVuXXnGty685IW/q9/vG1v6vf7zOODblFblC1v6vf7x9bj7/eQgNox5w78feCx4yEIm5yJ+cmbnInHGQhA8rv11eWHHGV3HGFDIj66ziitxijBPLAIQHCOBCE61nlrGC8I4XhHF4Yv0JAWMF4QgnDr1ji/QhgHd7CARsSpw69Ya0+HXrEAd3tJFB3ewgYjYlp8OvWWMLhGqMEpoWZjZVXMn3l3QWhK2LfUpgAC2u7D4UHHeeAnqnZ3QlHBLZAC5Hx1HyZvb4RwjwxuXwW4sEsnPgzvZ/8AZ8BapjLHxFNCbf62Bz5D1mrw7nA6qOdbDEhEdvxYQnJVc/mpbAGOa5A3GY6tMi1vDw8YmsVIYBrgqQcwQcjceIt4TTGKjwjowxRgvpLFWmGBVgCGBBBzBB2gjxE8i/aL2D1ENWiCaJzI2thz+qfLx3zeYXEnA/4dUk4Y5UqpzOF3U6x/y/5X8NjeBOgIDDwII5gg/MSSjZfDJtZ8hYvRtSi1iDbwI2Gdrs8pyHiTPUe3fYzub18Ot6R/Gm3uDvH9Hy5TEUKXd3YDMK5HMA295VbTpmriStHquj8SHpIyNcaqgZbLDlJix3+32nK/Z5q19HKy/jQlWG4rtH6zrXHV5ytRheOX4GhPcgLnf7faNfj7faFfl7xX6zmYsBv10Irx9brOLX6z+khBiYDQy/D5/SCanD5/SQhE0hflJ2fh8/pIXfh7GQJXcyu54Sy79WMru/VoUMRX4RoWt1aNGIeaCEBGEIATqnkxxfq8IDrOMLb4Y5yC2IA9XhqOHziA6zhqOMArY6jh85d0Zgmr1koqM6jBb55DxO3wFz5SqvP5zdfsywF6lTEH/wCMCmn9zZsfID/lJFbpUTHDfNRNtovRdPDUlo0hYLtJ2sfFmPiTLopRIZMBN3R2UklSIgCNkJakO2/L5HzkdSnCENk6+s5NXDVcMdfCC6fnwxNkO80T/wDGf6fwncDnOvSa41TtH/IRiIAFDE6YfVKrhKrtYgq2oqHwILaxB2+F5h8d2d7x3Wnh3onVDqWqK1Jjf4qdj8StuzI5XE9GENVU5MAQdt4HFPseM3HoxP7NMMaX7xTOXxo5U5FWIKt/1E6SpWHx11SialUqlEuagK2Bv3igahvrfzLsyF7CLR9PFg1sSMKEqF3w1KkzrasgZO7r1GvkB8d7XJXYL5Tq1ld8SxvZKSrTsNjMRrPfldYqimtr5DOVu0V6mEN8jlxvK1WkV23z2bjyznXtaJ0DLqnY3sfAjjMuXQwauHDLIZ2uzi+Z684x5mHiMOUYq3hsy2jfItXq05DTTpmtc8iI4n3gsOJj6vVoJXq0AQGXifeQOvEyZl66MhdeujIFFeop3nryleoh3nrylh04desrVF66MZDEeod568oo2r10Y8gTzgGODHCiGFnWPIggwgY4WGFkFYwPWcNTw+ccLDURRWxLy+c9a7AYTu8ChO2s1Sr5X1R7L7zylVns2g6LUsPQpttVRTa3gy3uPmJdgXNmnRq5tk2K0gKTCmqtVqsNYU6Vrhdms7Gy01yObEbMrzj4jT7A2bFUKROXd4SlVxlS+7XFlvw1ZLi1qHEYtKVUU6ltH1U1wClbWFSl3Lg7Ucrq82HjMhQ0hpeqKgotXIpsabrTSmopsNqLZQVtuBynTxYtyvjj3Zoy5tjSpu/ZHoOjMXVWu2Hrv3l6VPE0XKCk7KxKujIMrqdXwH4xunXJGw7PlMNoWlVoLgBiCDWWrisLWGtruiV0auq1D/OClM2udom2Btkcxv8AEfUTPJcmlAVFIIO4gg9dbZM4vs8cxIMQbKeA1lPKPQqXW+4n02j2IgCY/EYzu6XeYqtX7xSyVDrVKVGnUU2ami4ZdYn8LLr7VcEE5iFoXtEtwe/R1Js9PvxWdaew1gGppUTVJTWD3+Esfy53+0+HKg1VK6lYLTrhxemHGVKpVH+Wb9252gFGuNS8xH7jhcOpxPcVzVwzVS9Jag1skPe4eqrAg6qNf4ba9I6wvZgLU4uLvv8AQqqSnxVfqev0XANj0ZTp07DPaxZ25sbn0vbylDszizUw6Fjc02eiSdrd2xVWPEpqE8SZ02e/ylJacPtJjamGp9/TGuqlRUTLYSBrk+AF8z4bd8t6Oxq10JU5qdVx4od3LxB8ZcqprAg+IINwCMxbMHbMZo2i+BxJ1hZHCUrDWs/xrqtTvcAAM51b3GzPbKWpRna6ff4Gu0a/StMNT1rXKgW/XrhOHrcPaaKqcl4tnyAub+nvM64zOR95h1+Omp+5o08uGhieB9ILHgfSOeXz+sBuXz+s5xpBY8D6SFzwPpJG8/f6yJ+tv1kCiBzwPvK9QncfeTVOtv1laoOs/rChgbnj7xQLdZ/WKEh5+BCAjhDxhBDxnUPH2MBHAhBOcIJzksWxgOHzhjl844XnDCHjAK2HhTZ1JGQZSduy4vPZcPif8arQO1GSsn9SVL5j/Vf1E8bRSM88p6Xia7JiaDWuNZaatvp1SLo3JtUjlL9O+zdoXe4m7UYdRWDVTqUcbROBq1NncVdfvMNUY/lGsXF/Ald84/e1aYqrjg9O4WjpFqZK6wA1aOkqFRcrgALUtsABNgLHdvRWpTNOoodHBV1cAq4O0EHaJwcT2SfUNPD4yvSpEFe6bUrKinaKTVAXTI2HxEDdNm7ijfXNnE7JaJ7uslAOKq4F6+JxFUbKmJrKUpoD4kUiWO6675uxXByOR8L7D5yronR6YWktCjTUU6YsoU58Sb/iJOZN85fBDZH0aK3YSJ6QYFDsPtxECkgT4R4BRzsLX9pKaZXIZru8V5THdue1H7n/AIdP+JUUHWbJaXhc32nhvgcklbHx4pZJKMezU16VwQRdWBDBhcEEWII8RaZbSWiK9NWXDqtdSqrSDt3eIw+oSaYFVrrVpqTkH+JQWF2BImNFPF1qa16RruXa3fMzAaw3G9lQePQnYq9se5oapxAepTABcgAVDvsRmu5vEZ5ypZ15RryaGUOpJm17O6PbD4YU6jBqjM9WsUyXvHbWIQHPVGSjgol+m23mZhtFduwxUVNVg2008iMr+Jsfaa/R+KWqpdDcHYf0I8DLU0zFKLXZb1pXx9QKhc3+Aa1l4beETVM4te+UNC2TDNQOd+Vl+d5zNJoA97fiAPns/SXcC+st/AlrctYgeyiLHYfWVj42BH+m/wBTM+qx78bX/SzFLbJHGJG6Ax4REc/QwGHVjOCdEZm4SF24fOEy9WkLrwkCRu3D5yvUbhJaiytUWFBB1uHzjyPVihCYQKN3yhADd8ohCFp0zxggBu+UMAdWg5Qhbh7SAYQHD5SRbdWkYtvHt9YYI3j2+sDFZKoHVpv6OLFTB06lxdFX8Vr61I+B8D8O/wAZ58rDePb6zVdmKwahUpXvcsQMtlgD+ktwOpUadFKsle56dRNxJAZT0GdejTJO1Evz1QDLWPx1HDLr16qUhvqMF9L7fKbDrUSimTsEkFHfMZjf2lYZbjDq9b+r+HT8iw1j5LbjOPV7Z4mvsYUxupi3/I3PyiOaRbHFJnpvdDwnif7StFrU0i71KwRFVLjbU2Xsq7AM/wARNoelMXUbNqjt/czH5meeacxrUq517lWF1BvbWG/hK3LdwacCeGW9M9A0XpyjqphfiGGp62RJIJP+Yx2lj4ZLzytW0hpHDUq3eUAusGBVidZgSDrWJvvIO+edYjS9WqmpkE/lQWHpIwtQnWWmABkoBb33yvbZonkNitCg9QvTPdO5v8FtS/BNg8rT0rsC4UVKeuWyRhfzB/SeFYRcSz5ZX5ACet/svprTeoXqg1GVEVSbXzu2qDt/LLYcNIx5Vw2b+oZztJ6Q7mk7jMj8I3t4D1tLOLqWBJNrXvfwtvmN05plWARGOTMznYGzGrY7crfKXSkoq2ZoxcnSNKunaOGpU6ZJdlRQwSxtkNpJteX9F6co4g6qEhv5XFieXgZ5U2KuZYweLswzNwQVI8DKVlbZoeBJHoGKoajFT5cR6yu3XV5Uq9ojVdKdRF2CzgkG5Gdxa2ZEsMvXQnI1OL050ujRilujyC3XV5C566MNlHD1+0gdRw68pQWkbsev/ZWqMev/AGTVFHX/AJK1RR1/5Igg6x6/9jQdURRiGLBjgxDrq0IddWnSPGCBhAxvWEDzgFCB5w1PEwAR0YYI4+sDFZIvMzQ9mFLLV1bl6QWsg/mAurp5hvW0zoYcfWd7sfiAuKUf5ivT9Rce6iNjdTRZp5bcqZc0p2orIq0qdTu6ZXWRqeTOCSc22jbsFpj9Lv34Gs+swYMCxuTvFznmJ1u0uHs70xtRjUp/2t+Nf/t6zONhWIuAcs5uZ6BJdkiuQbGdLBYixnKD66635lyb9DJcPVzmeSpmuErRpMQddLzJacwS1QVYcj4jlNLgqtxbfKOk8L4yDfg8+o6OKVCrZ2Gsu57HZfwM6CYuhfVqIVIy+F29wDOhisBrHaRbdEmh6ZNygJ3tnHbTK1aYkxVBRddUeFyzX9zL2j0LPr5qi31P5nvtY7voBGw+j6aZ6ig+FgJfo1REXHQzV9nXr4+q1MKztqjMBmJJnNJvLdSprLIgoFifD5xmrFi1EgqIQLyu2ICLrk2zy4SfFYg6pN7AAksfygbTMViMRWrVLhPhH4ATsHHiYdgN98G/xGkMqT/zhjytq/WbHRmMFWkreOxuYnmmDZqiotQAagYAKb3vbafITXdm2KNqn8L7L52I2TPqse+HwTG9rNGzSF3huOXpIH5ick1Ebv10ZWqVOXXnJanMStU5iMgjd7y684pH5iKMQyQPWcIHq5jDzhDz950TxYgermGD1cxhbj6GOLcfQwAYSngfUyQE7vcyMEcfeSAjj7wCMMMei0s4LEGnUSp/IyttbwIO6VlI4+8kBG/5xboCbTs0favCnvtdBcrZhuPjblb5zq6H0fRqUAyL+MeO0HYVPEG4nS0DSFbD0qjC+soUnivw/pKbUv3PEEbKVc6y7kqfmHAEZ+U6keVZ6CMt0UzzLT2CODxJFvha/mplasuqQwzBzB3iel9sdBfvVElR8a5rx4TzDBMc6D5EE6t/BvFfP584k4mjHM6WBxGc6tT4lmYQlGsfCaDAVtZbSjo1d8kD0F2mV6lUDZJsQDewlWolpLJRCz74krZ5SOowkXehc5FyCTo6hxGWcB62XAbf/ZzxUufiOW08hvnH0xpTvRqUz8GxiPz8OXzlvRT2LTelziGFGkf8NSLkf/Iw8f7R4esu4Wt3YsPO/jOToyhY606F4rGVI6uCxCMwB+E+02mjRqoDtGV+E87oBSRnN32ZsQF1r7rx4FeQ0LMNw9JC7DcPSE5Mgcmefa5OggHYbh6StUYbh6SSoZVqGMkEK43D0ikF4o9EozYHAxx5wQBHAE3niwvWEPODYdXjgL1eQAYPOGDzkYVerwgq8YBSUHgZKvIyEKvGTYfDB2CKCSxAA4nyisWrdI9G/Z7ii2Gan/lu2rfcwB+ZPrO5pPDCshRth2bwRsI4zgaOp/ulKmyA6lJxTq5Zlam1/wDcLzVHMXm/Ty3Y0zvRxvHFQfaM1gcU9MmhUOz8J3iYX9oPZ8o371SGRzqAeB3z0zSmCDi/iPGc4rrKaVUXBBGewiWtcDp0zx0VhWTW/MMm57/OTYHEFTyhdq9CvgK+sv8ADcnVPhbxUzmJi1bMbd3j5b5RKJqhM71XFA5zlYrFSlXx3gJRevfxvy2RVEdzL9XEAeOcgpM9Q2X82Y+srKA28HftH2mg7LaIqVKgFiY6RTKRy8Th3GW25sZRxOiWUhhkHJB9Cf0nrI7HMzZiwgdquzS06CldqsL+hj7SveeUV9H4iii1Sh7t/wALrmpztmRsPOV10g2w5z2bRVDu6FNBsCjf45/rGxejKNX+LSR/7lufWc56xRk00bFitWmeQ09IDxE0vZjSn+IqLtJsJ29IdhsNUB7sNSbwKEkf7WJy5Wi7OdklwjGoz94+YU6pUIPEgX28ZZ/d49trsX0ZN0zSu3GQORvjsD1f6yFwerzmdmtIByN8r1CN8N1ldxGQRX4xSPVijEOCD1aED1b7wQ3EQg/Ees3nixwTw9PvCHl6D6xtbiPWOG4iAUIch6D6wwOA9B9YIbiIQfiPeAVkijgPQfWanslo3bXZd608v9zbfL1mdwFA1ai01I+I5n+UeJ9J6DQCooVRYKAALjIDzmbPOlR1P6Xpt8/Ul0v3/g7mhaIZXRhcNq3B84GAD0HOHqm6ks1Bz4qTfUJ3icp9KVMOpekgfZrgnO29c5Jhe1mHqDUxA1b55+HEHwM6GimniS9jo6iP1s0jC+2c7F4AnZLWHxtJlulRXXeCD62ibHUhtYDzmyyijLaX0eKtM0cQt1bY38p8DfwnknabsnVwrawBamfwuNnnuM+gji6biy1EP9LMLH7zlth6VRmpU6iEnNqLlTcb14dZQNJhTaPnPUbj5yxh8GWOQ2z2TS/ZTBIVbu2W4u5T8KEnK4h4PsjhgdanmNovE2D+oYns72SNWzOLLPRtGYFMOAqLbj4y7ToCmNUDKAw63R0qEcrOgrXE52nFD09U/wBX/UydHylDHNcMdytb0hFONRFkUX2Ko9o5PESXHLquV3Bdg/pErFufp9553Kv8kvlnYx/avgJm4iRMeIjk8/T7yNvP0iDUCx4iQueIhv5+n3kDnn6RkEjduIleo3ESVzz9JXc846RBtbiIoGtzihIclY8eKbjxg8cRRQMRhiGIooAHR0N+M/2n5id2nFFMmb7jpaT/AFlqlOHpL+L5/rFFLtF97N0RsD+P/Sf0ktbZ5CPFOoTyQ0dh8pptM/wcFyMUUiCzpH+E/wD+tv8ApKfZz8I5L8ooo6K2d2r+Cc87fKKKEBImyUcZ+FoooUQpaV/jVP7jKRiinnMv3v5Z2YfagGkTR4ooxE0gqRRQohXeV3iiliIyOKKKEU//2Q==</t>
         </is>
       </c>
     </row>
@@ -2536,25 +2536,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SANJU SAMSON</t>
+          <t>ROHIT SHARMA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>smat2023_132</t>
+          <t>ipl2024_33</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2563,13 +2563,13 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L17" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="X17" t="n">
         <v>18</v>
@@ -2617,10 +2617,10 @@
         <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AC17" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AD17" t="n">
         <v>16</v>
@@ -2648,12 +2648,12 @@
       </c>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>WK Keeper - Batter</t>
+          <t>Batter</t>
         </is>
       </c>
       <c r="AM17" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIQEBIPEhIQFRUVEBAQEBAVEBAVFg8QFRUWFhUVFRUYHSggGBolGxcVITEhJiktLi4uFx8zODMsNygtLisBCgoKDg0OGhAQGi0lICUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPsAyQMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAACAQMEBQYAB//EAEUQAAIBAgQDBgIGCAIJBQAAAAECEQADBBIhMQUTQQYiUWFxkTKBFCNSgqGxBzNCcqLB0fBikhUkQ1NjstLh4hY0RJPC/8QAGwEAAgIDAQAAAAAAAAAAAAAAAgMBBAAFBgf/xAA6EQABAwIDAwsDAgUFAQAAAAABAAIRAyEEEjEFQVEGE2FxgZGhscHR8CIy4SMzFFJysvFCgpLC0mL/2gAMAwEAAhEDEQA/APOopQKICiArsFopQgUYWuAowKkBBKACjC0oFEBUwhJSBaWKIClAokMoYpYo4pctYhzJuKWKe5ULmYqqzGdmCrPhJ0nyqHe4nhl/2rPv8CE/i0CPOk1K9KnZ7gExlKo/7QSnopctOYLl3/1V22zadxiUYz4B4zddp2or1lkJVgQRuDRsqsqCWEFC9jmGHCOtM5aDLTsV0UaDMmstCVp3LXFaxFmTUUkU4VoSKhFKArQEU6RQEVEIgU2RQkU6RQEUKKU2RSRThFJWI5RAUYFcKcC1ICUSkAogK4CjAokBKQLRAUoFGBUoZQgVwFGBRAViCUEU/h7amWcwiKblxonKg306np86HLUbtExXCIi6G9ebOf8Ah21VsvpmZT90UjFVeZpF+/d1lOw1LnqoZ39Q1We4pjLmJucx4CgQidLduTCgxr5nrUbkBJzb6aDwI3/vyqz4LwW5ipS2oAGjOdJOmwHWtXb/AEbhbea5cad9ANP61x1Suxp+o3XXUsO9wGUQN34XnbFR0HuT/OtF2TxztcXCsxa24ZUViTy3ysUKeHeABGxn0qfi+x1tQYZ5jTasvisLcw1xWBgqwZDvDAyDr5iioYkZg5huFGIwj2sIeLHtWuK0MVLvsLgS8ogXbaXQJ2zCWHyaR8qZK12zXB7Q4aG64t0tJadyaIpIp2KTLUrJTMUhFOlaDLWKZTZFARTxFCVqEYKaK02Vp4ihYUJRgpkikpwikihRynAKMLXClAo4SiVwFOAVwFEBUoCUgWnAtIBTgqUBKSKULSgUoWpQkpMtM8bsczCHxtXkf1R+4Y+8bfufCpIFW/DeF8/DYoyZW3oNMuoY970ygj0qntDIMM8vMD8iPG3arWzy7+JYGXN+6DPhKsOyuCt4O0mdlloJmBv61rbz276wl20xG6q6kj5A1ATDlrSIi28xRQzOuaFjWNN6qeB9l7tu+LtxtASWCrbRXE6ABRI0nr4VwL4Mkld+0EEQNPm8pziyWLC5rjqs7AkanyFec8WCYpyqEb6Vr+0PB2v4u8cxAUHkrAZQ/mDuN9NOnzprnDbltxnA0EqQoGsa6Cn4VjWvAm8JpDnuyuFvnSmsDZK4XDKd+U5+TXrjL+BB+dKRVhjLYyWWAy5kXKmbMBbVVCwYHgwiP2fOokV3eCLTh2FtxAXnGOzNxFQOEGTZMEV0U4wpIqyq0poigIp0ikIqEcpkihNOlaArQogU2RTZFOkUBFYmApsigpw0lQjCcFOCkApxRRJRK4CjFIBTi1MJZKQCiAolWdhRisQEoQKMClAohRJcoMtaHs3Z5r37IBFu6Cq5u8FdRzFDEAScqOPeqvD4J7iO6gEIBm1EwZ6ddqGzdZIKkqQ2YMGIMjaI2jXXzqviaAxFJ9KdRHVPwFPw1d2HqsqjcZHTHyF6Rwi8DbS7G6iR4HrXca4umHVblxrSqxiHZht4Kok/lVbgMegtooOrItwA9TJDfxA/2aqU4LbsI+Jv8zFs7Fgqw3Lk6BB0G3tXAOpZHlj9xI7QYXoNOoKjGvboRPYRKhW+NZsWzjlTJLKHbvKegBEE9dK7i+OD3NBsJjxPhVRxfB2sQWZbd3DxqWcjMSPM1D4Nis19FktkGZm8Rb1JPqYHqwpuGp56oI1ED0F1bFfmgXv0AmegX8le2rHNfkm4ltUtIuZwYzWxBiBpJLH51VOkT1gxI2NO5ZNHeUQApYiAWB0AfUGPl18675lMUwGN0EAdgXlz6zqpL36kknrN/OVFIpCKecDpOw38Y1/GaAimIZTJWgK0+RQEVEIgUywoCKdIpCKhMBTBWgIp8immFCmApphSRRkUMViMFOqKNRSKKNRUpZKVRRrSgUaipSiUqinliI9TMa7belNgVJt32CG3PcLq7Lp3mUMBrvsze9EUuUC2pMKCTBJjXaSSPIKPwNEFBiJmTOojyj8af4g9t7rvaQ20JlELZsnlPXX86BbfmP6a/n/WoFwDoodYwEVh2AYAqsoysY1ZTBIE7bdI3NEuHUqSGAKqCQT8XeiBpvqunr4U5hcO7tCKWI70RIAHUzoB66VJS3btgG4RIbMArC5IH7JgRqY1J2G1A97W77+Pz5dHSp1Kv2ifLv0UqzwlcRhIQulxDmRy25Yd4CAIU5B8xWQ4hc4hhBDC4ABo41HzIrX3u0apd5S2lAKokjQsyLEnxO/4UWK4nntkd2CNzBiuJ2lWLcU/M2xg36gNexd5svDE4VgDriRbrn1C8wxnEcTiDLTJ6kx0q77J4ULzRu7WWiSBorK5AncwpPypLuGCSZDddAKpr2KIuKVJGVs8iRBG0ecxWYOseebkGhnuTMXQHMvFR2oLZ4SIW4fDE5dZldTDEJEiCfIDp08aB7BBI8DqdgNYBJOw2qjTtxdDKHCXFCqASAGUAkjKyjTx1B3q1wfHrF+V71vNllWRWGYAiAwE9fATudQK6mntCmbG3WuQr7HxDbsGcf8Azr3GD3T0Siu2zO0QFJ0MQYg69DI96ZdCNDpVmlsKCz2w4KsqMGMK5UhTIMmN8p8B6VBIEaTPy/ver7XZtNOPwrVuaWGHWO8GxHWCmCtDH5aetWuIt8uyqi6jc0BriC3LWypOXMxXQ7/CfcRVfcmANQPiAnSdifwrA6URblMfPAqPkpt1qdawruM0Qsxm8/AeJ8hrUjjHDhYCKSeYQWdOqWyFySI0Y94x4R46qdiKQqijP1G8cAN54du+ye2jU5s1Y+kWnieA4+guqYrTbCniKA01CCmWoacakihTAUQp0UKijAooSyUqinAtIBT1sCdZiDtG8ab+cVKWSkWpuEwzOSUUtlXPchQQqzBPpqNTtPlUVF339I96lqCIAYnTKSYgA6gKT0j061DidAgsLlFw/BtdbKoJhSxP2VA1YnoKlo1u2PrWz6Ry11E6a59p8xOmlX9sDB2FQKBddQ14z01KqfAQQSB6dKyuIw/xNvrIPkf+1VTVNQmNNyv0aDGiXiT4d29N8R40xGRO4v2AIkeJ6sfM1UjESdT703jjqdKjJbM9fOjbTAurpxBywLLS8I4c2NdLaiTPeJYrkVf28w1Ef0jWtyvZzD2rRDc66QCS4NtCfQZazfYDG28PZxV66csm1bQwf2iSw/BK1eL4natLmu3rVsEaM7qvTzNaPaYZUq5XNBA/yb66/Llb7YtL9F1TMbnSTA4LK9puzuTDresKWtsRzC0Z7M7BgNwTpP8A2nG3sBbRGYgMwBPiNJ38Y8BpXoTds+HWka1dvG7acFbq27V3KEYwTmUAASRrm9Kx3EMMA160s5QHVJAErrGgJG0eNO2Yyi1rmMaJ1nWZ9uGnrS2vznOtJfI4cOKzZ4ShGbxAPvNT+FW1tnTfaa0XCez9+7grTiyud1tvbm6q3LtsoT3LROokSDEnoCNRTumUnQjy6zV1raT5iJ7PRUxWqU9VaWXuzIYiQfmAdZnptvUqzeRyVvIAxGlxQdD+7sfGNKg4XEjKDPwugbf4Xm37ZmSm8Tchp/xXVP71soAB8mNIfTdTMsMLZUsVRxLQzEMDh0i46jqOyFJvWcjlWEiCQQdCCO6wMbag+Y8Kl8J4aHJu3QwtIAzdDcJnLbSerEHXoFY9KlYDBHE2QFBLW2EQDradgCNtIY+kM1S7qoEyT9RYHeYac662pjzeIH2UWgxm1clGKf7htHA8R6eNgtfS5P1BiQ03pz9NxLtCBEyNQDMSZhA2LFpRiWVc0FcJZA7qidXg/sDXzY7zqay2Jus7M7FmZiWYkySTqSafx+ON5yzBTpC9MqgaKoB0AHnUc328vxb8zS8C6nhKehc913Hj0Xmw8dTquixHJDH4t/6lRjGizQMzoHTZok9BjhomPb5g1xsN0A+R/pThuN9qPRiKAsfE+9WXbRP+lveZ9lYo8g6Y/dxBP9LQ3zLkAsN5e6/zil+j/wCMe6f9VLFdFKOPq9HztWyp8i9nNFy89bh6NCaWnFrhZfoB8j/SnLds/wCH3T+ZrbGtTGrh3heZU9m4yr+3Reepjj4wjsWi7KgiWZVE+JMCpuIsGzdNq4MwQkEKwXN6NlPWNxUWNIztAMgaRPj110FIHEySx8Sy6z8iKS7GUZ+7uB9lsafJfaz9KBHSXMHgXT4J62uvTy61p+zmC5l1EzBlQl8sABsgJGp1yEkeHxHrWWW4v2ROvjtp6+f4Vr+ydlimIzAqFtIcpzDMrMpOm8kZYjSG3FV8RjaZYQ2e7xVocksdhv1a+SAQYDiSbi0BsQdDfRMdocUTdkqVMAsDuXY5jruegnyI0qJdtgoCTuSu43Xu1G7UMLN+5bWYVgq95iQMsxO8eVUeG4qzKwmQrk5Z2LbR6UVBo5tkcB5StZiJ519ogm3CDHcPFbrBdirNy3Ze5eZXdWflA2wXtCYCZtmPd1mBJ06hvB8F4fFx76pbdWyLhTiQCBpDuzXEzk791gI8TUZOP4Q27Ye3dvXAgR89xsqxIyrrAGgIAHWmL/GApzWsPZWQ6RlJlXIMGIkDLp5EjrVUjEOkEu8Bv69N1xPTqE0GiIgDz9Neox0KTi8BgrwODtthrRdWvLeDBgl218An6Rc1JbURJUN41ieHdnsOL7WriYiO5cDpldHV1DSCVnLrpJDRvBrVYrtHdtlfpAsLMFbPJ7+UEHqe4NonXbTrVB2xwpvZMTYW5dtZVQ5bh5tm4IUC4ApBJ07xUz4gEVQxuHqBnOGb79fGOqOpbTAuD3EATG7Q9gndvV7ZwuDFk4ZVQESTdyrc5gSbhSWDdBJ0kAgDY1V40gXwuYsAlu0WMnNlQIDLanYanxqP2fZ7Vp710d2OS1oqqkm4AIkKDmAU+4mppwQxJJtXFZ4DG0wyOPIfsmI0AbptVnZVPKw1DfUTw03+uirbUJzBsRafMK44DxFreDFrmG0FtgBWzmAt5bTXHAOqNnETsFIGgk5Dihy3bi5WQB2hG1KpJgE9dI12NWeO4qiM31brOjCLeYQCGmR3phdCOh30jPcXx9p4NvMDMQUtr3YG+TQnNOvn0jW9RHNuJI1+fJVF/wCpodEtrElS4+1bYCftDvJ/Eq0/exYPNM7XcQ48gy2l/N6zeIxcaHwkfPT84q/7G8O+lBmYlbaE38S/+EEKttfFmYqP8vhS6uJZJm0C/RCbToOAstrwF3FlbazzMR9Wi6Tys0Md+pEeitNJjuJmxc5eQFUJy5gwzOC0uOhk/go86m8Gvn6VkyfWZghUCeSgA+qWNZAC5vCAPtTT9rsOVxl+QADeulfh2DsBIG23XffrNaltPNUNV4jNcDgPc+67fYDWVaha+DDYHrHzSeKp7hJJY9ST5fKldRAI1JBzCI1nTXrpr86csXCpBEzrHlIg7+IobyRFWV2M3hMGurq40JRrq6urqFYuLHxPvSRS11YsJlcf70FEKGnLaknQTRNCjRKprU8AvPbwuIdSJzW1nKhGoeRBEHYedVFjBDL1mBuBv1rS4LAMuAY5Sc94zAJ0VFgmPMtRsylwB0lc3ylxIbs6plNyWgf8h7LI8dxT3c7sQXjvMMveGkSq/CQPLUedY7CYqMQF6P3Y8wZH5VqePp3SpGuhEjqPCIrDBj9Jtb6XU33iRP4VdxDy0ADiPNecYdubMTrF1p8BcPOg/wC8efQEn+Vae1mw+EXEEFWvBzbYjUWwYDLOxMHX0jrWSSQ9xtyBcI9W0H/NWr7R3YwxtqxJtWLOEycvd0AW44ueBhjGsSdp0aS7OwZZE317Nx38RFrpdKk12bM6LW0ueFyO8XWUcC42ZiSTqSTqfWtFwLA4lGFzDrdVgJzhTBWB8RbulYZd9O8viKxC4uGK+5FbzA9qMVfKG3YutCi1nnEsjZQmZRlKoF0U5Igb+dWKmJkQwNOoM6J3NEak20hSO0XE7z5bF1VthSHdFAGd2AIZt+hGnr5RDu4QWBavo/6xMzaEZXXRlmdevv0p7inDcXeOc2YdmgKGtqCQI0zNtpHqCN9Koe1CYqzhgly0qKrgB89smWJ0OVjPUT5EdDQCtSpMblc0RqARe14136dUKHMqV3kvkzvPZ6e6d7VTcVMZbk5/qr0T+tAEMf3gfmVY9azOJsuhUXEdCRIDoykjxAIr1zsRwoLZjnI3MS2yqF7ouWzmQ5mgyD0yj1rzzHW3vPhMEXdrilxcusLhGe5d75BOrKqhSfCtcMTTqPIpmWj8mOzTqhOOFdSH1iCs5ewj3SFto7vrCorMxA1MKNdImvXOC4QcL4clk5PpN36y5mgi2wG7dCtsGB0LlzqBWl4Dwa3hcLYTDMNbYe/dS2puYpnXMp1IY2xI7oM7ab1H7UvZ+jD6mxzHZbVtmwmIS6qWyXJHMEmCRoJ+OtS6MViWsI+ibifuI0B4AESRviNJVkg06JO/y/PBVHYHii27zIqEsSGS80lroBLXpkSpYag9YAPSO/SFYUY43FMrdt2rqwYgEZTHrl/iqjwV5reJVkIDAyCy5yG6HKNBG4zGdNqv+2yEph7khmNtkOxMJBCxsB3jHhNbLEMirmG9bzku4isI3gjwzeY1WSYEmZkwBMzoNB+VPBgQFPpQIh0OuuxjQxvB+YqRbwhJ1jyoJXdOIGqhXEgxTZp/E2yrQfl6UwagpoMhJS11JQKUtdXV1SsRJuJqbYj2pnA2UZgHuC2sGWhjHlA1poORRDgluGay0fDypmTGhI8z0Hl61tbdgHBWzdY28wLjlW1IAIABPgTAJjxrzfCYmNDXpnBMXy8NYCfSLjZCxw62wc5YsYLHRUk7+FVcSS0AgwZ+cPm5c1t2hNIBwkE6R0HoIG7VZG92f+k4XE3c780BhhLYZxzrltTcurlJIPcgDzNZ/s92Yw2M4SrqkY5r+Ju4e6CxN0YYqzWd4kozRpuJ6Vo+PdqMRw04ZRgkHK7+a/Z77u5JvCxdBIQEHLIkgbjpVV2D4u94lLVhbS2sVdvYcB8xVsS4bljQSFCgbag0uniKz4zOmIN+Pgua/gGl2VjQA6Yvuv0p7HcLUcdtW7KIi/SuGsqKoVcqJavXYUabKSfWrn9IYW9gbqrZZ2HE7yxZ7p5mQgO+hGogEnTarvG4bF4Pn4y7eslr2jLatQFuhVS2QzywARWG+58686w9y4z4h+ZcyyqMoZgrs0mSP2iAP46KpiHPq02MOg1CzD4VuRzrG4tuKyvZrh9guhukkvnVrZBAzbKM+mUiT6kDarXDcX+jKbVq6Si3bl22/Ll1Z0W0Lg0gCMwMkEyIiTXpvFuwOG/0eeUrLcA+k5ixPfYAuCOi+mwAqk/Rz2eH0mHVTlRrl8FQVJ+FE8xJnbWK2LK9FtEkkk6ZTHEmdN8x0qOYdWbIaGtaCS4C85R9MTvN5sImw35v/wBS5g8NfzMSc3NIC9zJIUHwiR5eVP8AD+GYjiVxiuHvXrItkuXclGuKCERS0DN3j1mddKu/0q8LS3j7F7IotthgCg7oZ7btppsIdZ9BW1xPOt8OsNwzIUWyhVAoZnHcOk7n9ZmHxEnxoa2JoGmBTb9R4nTttOniqrMJWaG1XH6SSB2eX4K80y38CWwrhlI1tlgQT/Ug6GN9xoQaC/ieSTdeHv3I7qqoLuYgGBqZj51I43xS/wATvBbgVSWS1bRQfqrk5Z11kkmZ6adKqO0HZ18LNprhe89pm5kEZVJKgKJMTDSd49a0rsG4OygwDc+y3QqGGh7ZfFvf3W74Dwq9eFpBesgWx9ZZ5du6rZmzuDJlRmJgiP5Vme0q3l4mcPftpbW3YHIS2HFq4hZm5mWYkklSf+GPCs52LRhi8LcUlWDI2YaHTMG+RHSvXf0k4QXLeFxEd9S6+eS4gJHuq0+DRvSsb7t5ue+Tre6psoh1RragkE/But0J7jnYu02FDYZCl1QHAV3+tEd5NTofDz9aY7B2le4MwUlLVyAV1Us9uTqN+6Kt+0HGWwjYJ9SjZlvL4plTvD/EDr7jrU3A8OVcScTaK5Ltpi0HTOzowYeTCT6+tS5znXcSe1ZRPNYdzSIDgYPSNR6j8ry7jpL4u+pOi4nEwsAb3mJ9fn4VDewQ0janu02JC4zEQB/7i/P/ANjzUezjQwPpVwD6R83LuqbXCk0gWgeUpvHJm9qqmEaVdcwEbjrp1FVeJMsYogrNEkWUeupSKGoNlYS1wrqUVgWJVE1NXBys1DRoNW2DugiiJSapcBIUEWyrCR10r2DhPMHDz9Gyc9Vyd6PiUAQfPLtOkmvNCklTGkj86tMPxHFYb/W7QcW8wRyysbbnU5W/HUbeOtIrAuhabalB2KY1rSAQZE6E7h2/OKqe2naTGYq2uDxCLb5bzcGQq1y4Jykg/DAPTQzO0CrX9EPDCbub9lc11vNpyW1P+Ut92tD2pFvHcMTHG3y7gyFZiYL5GXN+0pksPl51I7JLbwHDhfvac5l0AlipEIo+WZvvGkAQOnT52LSSBQdkZDySzKL/AFGxjsnqkdtyzrj7GKsd34nS0fJYKP598T7V51wThh5du06lXu32a4p3VmflgH7qqfnW5t9pMJa5OSyUF11RTy7axnuC3qAZIzQT5CaXGYHLxG0x0VybsnYMgMj3Cn71AyA8u3iQqdE829zYgQSAeIn89ytW4grYpsGRI+jLdO0d53TL46hSflWfwWDOBwmMuGRcZ3tWz4hZS2w+bFvlSjGzj8RcBEK9lARqGVEGYe7v7im+3Qs463bwxLFeYLhZWdIuLokHSTq3sKaaYDgN1p7pQYVtTK1rRLXQTuENJNzukKv/AEjWudg8FiWnaGGUyDdtB9fs62xUPs1iMRw60p5dzLcZWNli2Vh3gz2vslu77DTWa0ItpcwVvCFr2a2VK3M+VgVY5e8NdjGwq4wXFme20qDcRSQCYzMAY9JjegDDqQrRqGnh+ZLJaHGZO6fpjh84rO9uMKlu9h8WihbjMGcRGcoVZSw8RsT6eFO9puz68TSzi8O6B1UoQ2gdCZKkicrKZ9z61muLcWfEvnuESO6qj4UHgP61CTiV21LWrj2ydyrET69D86YGOgK3T2dV5tkGHtnpF9yuuyvYC5hrxv4lrK20zsFDySD9owAqxPU/LepHabi64m6FQ/VqpRD4sTJb0kKB6edYvG8bxN7S5euOBHda4xWQd8u00zbxpUimNo7ythh9kvDucquBNwABAE6njK9A7dYu1et4dbdxHKZswVgcsqo1j0pOy3aYYa2bV0OyDW1lAJWd11I06+9Y25j/ADNRTjXn4W9jWClaCmUtkB2H5hwJGs79Z3aKRxoi5fu3hIFy7ccAxIDMzAHz1qlY1Nv3GbYH+/So1y0Rqze4cfyqyxjjYA9y2RxWHwzQK1VrY/mc0RHWQisX431qStoP3hUNcvU+0j8q4YgJsCfRv/EU0YWqTZp7bLXV+UOyqYn+Ib/tl39oKkXMODtvTX0UeVN/6QP2KH6afL+D/ppgwVbgO9UTyw2a2wc49TD/ANoQUlLSVRXWpaes3YpilAPgfaiB4rIlX2FxA0rXcK7X8m0LVy0LqAQO8AQv2SCCCK88slwdmHyNSnuM2gj5SfyFCaYdbVavG4Oi8RXiNbmPFXvaftHdxoRABbtqcwRTMsNAS0CYGwgCgt8VxGNa1hWZcqa27apAGRSBooknKCB61QpeK7n/AJp9iKt+zOOSzi7N8sID97cwrKVJEDoGn5U0YWrFmG0xZamrtHZWFpFjKtLM0OygOa4hxHWTJIEz+V6jw6wbOES0zSQCDl0y5paPGQDWK4xZuWXz3VIDMWVpkHXofntWy7QO72WFhxnaChBEGR9raIBPtWb7X8TsPhFti4pupeHcBBKHKQwM9NfcVTw4dUeGtGvzsXPUNpNwlQ1q2hueO82Ejjpv0VV9LFq6xAZs5W4ANwGGnkPD5VbpiARHLZgRqsBpHh5/lWWwmLLJJJlDk0E/VuRl0y9LkeP6w9KtuAYh20e4gggMiuxAHdzad0TGYeUzRY7PRrAESTHtwRbPxlOphxzLSQC4DjEkiQCbwQNVcKColGJX7D/HaJ2BkSV8DPvQ4DHsl3MdIINzwdBrm9h+FV3a2wfon0iwW5lp07wJ+stOwVl8xmyHyjSJqFbxjLhbjOVL8sISCdLjRKjSD3M2s1DG56gp8THethiKzKeEqV33gHvgx32/zdZs3JZjnGrTE0cyImfvE/8A5pomkmukGz6I49/tC5Cpy02q8WyN/pZ/6LlwUdVPuKU5ekj/ACn+VCWoSaaMLRabNCoVOUm1qs5sQ7shv9oalzfu+woHM7x8gB+VITQE0wMa3QAdgWvq4rEVv3ajnf1Oc7zJSEevuaBjRE02xoiZSWMa3QQhJoCaImm2oU8ISaGaRjQ1BTAFKa+g/ZY+jf8AjRJiR1T8qhCjBqq3B0R/p81v63KfatQ/vEdTWDxyz4qVzvAD5hT/AColvt4g/IH86jiiFObRpjRo7gtXW2njax/UrPPW90d0wnif7EijU+vvTKmjBpwK1jmAmSLp0GnFNMg0oNSgIWj4T2nv4dOUMjp0R1LBfTUaT0qpu3SzFm1JJYnxJ1JqIDRhqBlJjHFzWgE6nipe972hriSBp0Kw4VfyXV1gEZG30VtCdOomfUCrLBMFvnoWbLr+wTII6yA0j1FV3AVDYmwp2N5AfTMKexJAum9IAe9dmZ0uBgCR4kuhb70VqNrRmbxhdXyWzAVJ+2R3wT5Stxg7Rvpcsk/GhiZMMCDvMwGXadqyHaS4A1uyFCm1mN0AR9YdD66BdfWtFw3HwyPD/FPw5dxB+IjTrVJ29n6TnIgOismkaQQZ1+0GPzpGy4OIk8D87lc5TZ2YbKPtLhPZPsONwFnqEmgL0BauilcGGpwmhJoZoSahGAiNNmuLUJasRALmNNmlY0BNQmALmNNMaM001CUwBITQzXE0OaoTQEgNGDTQNGDWKSE+powaYBpxTUylkJwGjBpoUQqUshPA0QNMg0QapQEJ8Glmmg1dmqZQwrbgFjmYm0gMd6SfAL3ifYGkxHEOYMTAnl4jmKM2WFuhtNDpBt6gdXqZ2LsZ71y5/usPebcCZUp7wxP3aznZ/Ff65ftGSLtq4kxorWirqx8u6y/eFc9tZ4NYN4DzXYcnKYZRdUO9w7h+ZWu4HcuMAVgQSO7aRddGU96TqobpVj28tsbFi62vfdQcqg6qp1K6N8PgIg1V8Bv5WZT0CPH7jZT/AAmtNxyzzuG3k3a0VuL90w38LP7VVwb8ldrunzstvt2iamDdA0HlB9F5rmri1ATSTXVrzeERahJoZoSahEAlLUBNKaE1iMBITQk1xoGNCjASFqEmkNCahMAXE0M0hpKhHCQGjFMBqcDVgKIhPg0QNMhqINUygITwNGDTANEDWICE+DRA1HDUU1MoMqeDUs0zmog1TKHKrrgtxgmJK6fVZWMfsl0n8AfasTzyl4XImDqJjMGBzrPSVYiek1ucC2TAYlzP1joiQTrlBzA+P6y3WOFlSdWABY/nA/AVzG0nA4l0dA8F3GxaUYFoO8u7p/C9CtupvWrqfBeQGfK6vXzB/Gtjwfvq9o/7SyyEebKVP4zWPwuDCYa0AdbVzluQBAMhzA9Wbfchj1q34Hi1TFqOdcY51lYhVDEnvEiPE6HcR10qulpg6rbPe2ph41mRpwsfFeflqHNVh2iwf0fFX7J0y3Gy/uEyh+akH51WFq7AODgHDffvXmGQtsdyKaSaAtSFqyUQaiJNITTZahJrJRAIy1AWpJoSahGAlLUBahJpCaiUYC4tQ5qQmkmhlGAgBogabBogahGQnQ1GGpkGjBqZQFqdBogaaBowaJAQnAaIUKkU/bK1KW4oBRhTUm2UqVaNvr/KiASHVY3KfxRBa4fhBcOTPzboBHxDOYPzCJ8iKruBcHuXQCps94DusCWjX4SCMpMnx6eFHj7AvhQ2LxICwEUG3CgCAAMu0UmDwAtGUxtwddbVs1zuI2diX1HOgGSTr0rp6G3sOzDspXGUDUH0WjbEfRmx1rEKVa5cW7ZlWIYTc1EeIYQfLyqh492zfh+JbC4Vs2QgXHieZcMT6/P06VOa6WUc3Ei+yiFa6gBCySFkHaSfesjxXs+17FNiOYihnUwrQRAA0PTbwosZgKlZjXBv1H7husBHTuv1qrg9sU2E0XH9MElpi5kyZHbb/Kv+0nFXxbpcdFVxZtrcy7FgJI+6SV67CqeKv81mO9E+RJ/E1FvG10reUqQpsDBuC0lTFOqvL3DUqoM0BNT7hSotwijhE187kyTSE0rEUBNQmhcTQE1xNCTUIwFxNCTXE0BNQUYC4mkmuJoZoUcJAaUGmxRioREIgaIGmxRCpQkJ0GiBpoUdTKAhGGow1N0gqZQwns1SuGw960hEhrttSJIzAsARIqDXVhuCFAAWy4jYQWpdSgm2TdCBCoL2gYCoIJDXvq2zMOVPWqlbWFIk4hxoTHKcxvAOm508hrqdJprt5miWYxtLEx70NJZRc1sZj4e3lCa9zSZyq9t2cMf/AJLjvAKOUw0OkknQdD701es2SDy8QWbuEBlyAg/Hq8DTprr4VT11Hkd/MfD2S5b/AChXzWsHAAxNyZOYm2+UidIAWdv7G1VuOyByLTl00hiCCdNdD51DrqxrC0/cT1x7LCQdwCLPSFqGkamKIRE0JagrqGUUIiaAmlNBWFFCUmhJpTQ1CKFxNDXGhrES/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTEhIWFRUXFhYYFxgVFhcYGBgXFxgYFxgXFxUYHSggGBolGxcWIjEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGi0lICU3LS0vNi0wLS4tLS0tLS0tLS0tLS8tLS0tLSstLy0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAUDBgcCAQj/xABKEAABAwIDAwgFCAYJBAMAAAABAAIDBBEFEiExQVEGEyJhcYGRsQcyQnKhFCMzUmLB0eE0c4Ky8PEIFSRDU3SSs8Jjg7TSFpOi/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAIDBAUBBv/EADIRAAIBAgUBBAoCAwEAAAAAAAABAgMRBBIhMUFhEzJRgQUUIjNxobHB0fA0kULC4ST/2gAMAwEAAhEDEQA/AO4oiIAiIgCIiAIiIAiIgCItP5X+kaioegXc7N/hRkEj3nbG+fUgNwRcMqvTxNf5uijA+1M5xPgwW+KyM9PEhbrQszbjz5t4c3f4ry4O3ovznN6YMT5wua6IN+pzYLR37firOi9N9WNJKaGTrDnM/FLntjvKLQOTHpXoqmzZj8mk+rIbsJ6pLAeNlvsbw4Aggg6gg3B7CvTw9IiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAvEsjWgucQ1oFySbAAbydy9rh3p/wCVGZ0dDDL6t3VDWneQ0xsd3XNusIDN6QfTG0iSnw8XJBa6c7BtB5ob+px8FxRfMq+x8FE9PpC9ArwSVkjZfYvD0z0li7W/cvsjQepeaZpzDqKzyvAc4aa8f40Q9MbWEG51t3LcOQ/L2fD54+ce91ITaSPV2UEeswE6EGxsNoutJEzm7D/Lgkz7jqQM/YuG4hFURtlhe2SNwu1zTcH8D1KUvzL6HuVrqKrbHLJlppei8O9VrzbLJ1a6E8Cv0yCpkD6iIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIDX+W/KuHDqYzy3cScsbBte8gkDqGhJK/KOJ4g+eaWeQ3fK9z3drjsHUNncuxf0jqrWji3fOv7xlb95XHsNpc7tdgUJOyJQjmdkY4oyVYQ4Qba7Vb0dA1u7VWEUV1knXfBvhhktzWzhDr3Gq8/IntN8vgtzipupWNPQg7lD1los9UiznUdHK512tN9qnQ8nZ5Dct04rolPRNGwKZzI3BReKlwerCRW5z2TksQNddDu3qqxDBXxbtLLq5p1AxPD2uYQRfzUY4iSepOWGg1Y46dq7f6HPSGXFlBVOubWgkcdT/0nE7TwPcuP4zThshA2blGoJSyRrgbFrgQRtFje4XRjK6ucqUcrsfs5FgoZM0bHbbsafEArOrCsIiIAiIgCIiAIiIAiIgCIiAIiIAiIgOE/0jZBz9I3eI5DfqLmj7iuc4MLBdQ/pGYfrSVH6yI/B7fJy5bhTtyprbF+H7xsEStKSMKphcrGmJJXPZ1EXMEYU+BgVZDeysqYKplqJ0LApMUIJ2qA2QqXBIV4CXJTgKvnj0UszlYZDdenhzTlxh7WkFoGu238fxZadTi7wLbXAeJAXQeXO5o3/mtb5G0HO4hRx2vmnjJ7Guzu+DSulh28hzMUlnP1dRttGwcGtHgAsyItJjCIiAIiIAiIgCIiAIiIAiIgCIiAIi+EoDm3p+py7DA4D1J4nHqBzN/5BcPwWLQu611/0lcsaSsoaqmieQ4AOY5wsyTm3B7mtN9CQNL7VyrCojzLbbSCfElZ60k46GrDwalqjMK9jTbbZSI8fjbx7AFXukjYQC3MeAC9idjnNjNKcxJaNl7gXOg4A3VSgnwXubW7Now3HInEA6X4/itrhy5bgrlkzmNcWFpa4GxBvpbaNdQVtnJuZxbkzG266oqQS1L6cm+S/lq42C7nAKPT8poS61jbjuXjFsEY0Z3km2trrWa2uiF2iMute4ZfQb7kLyEU+CU21ybZJymp3DovueFjdeqXE2PNgdTuIt4LUsJraUgkwFoBIJLXlt22vd+Wwtcbdl1tVHFTygOjGreG7he27r3qU4JcWIU5t7O5rvLqA2D9wH8fes3oHoRJiT5TrzMLiO17g0fDMrPlnSXpZCPZsfDas3oKq6anjqZJH/OvexmUNJIY1pIJsNhLj4K/DSWXUzYqDclZHbUXiKQOaHNNwRcFe1sMIREQBERAEREAREQBERAEREAREQBQMdB+TTZdvNPt/pKnr45oIsdQdqM9Tsz8sQQj5LKTa4a867zqPFSsNiAaBwAHgFm5bUfyaWSnbo0TED3SWuHwK8URXNkmkdi6lK6I9Rh4vduhusNVREvEhAzi2thqRx3FbIyEEKLNHc6rxVGj100yhEL3vLnEkk3JWy4G0hzR2KC8AKxwVhMgUKknIlTgo7G2YnEXs0vwK0yTDJATlJAILSOo7RrtC35j9NdiwzQNJ2KEJuJNxT3Ne5NYIYWPEbnNzAgjqdbNYG9r2F7bbBWeEYO2nIA/j8lPpw7YLqbHQkdIqTnKR5lUdis5QQh0T2/WY4eIIVdyQoWR4WJi0XcyUu4ktc8fCwCusRGioeSNQZKZ1N1vA7HTEeRKJ+y0eJe0n+8HU+RZcaKAu2lgKu1Hw+nEcbGD2WgfBSF1YK0UmcWrJSm2uWwiIpEAiIgCIiAIiIAiIgCIiAIiIAiIgOEemajtVyEb2xS946J/dWrUkmi6d6YcHcXMqACYyzm3n6p1tfqNz4LklFLYDw71iqR1aOlSl7Kf7obNRy6LDWm2oUemk0Xt9UFn5NSasRWvADnvOg17uKveS2IxOFrC99puD4FatiFQ1wsB+fVovcAkYznLW+qSNewKeRNaled30OqT11NnbCXhr3AWBOpNtbKK2ctkLXG9jYHiFrontzXOsc7KMzXO3Ei5sezyV7BVRSNDmkE/FVSj4FsZeJf0bQdVJmcAFAoZuislXOANUR5JlTjlVlYTwB8l59GWFhrYS5pDpPnHX4ZnOA6tLHvUDGiXgsBsXEMHa4gDz+C37kjREPLvYYMrfy7lZSjeSXUrqyywculv7NsREXTOOEREAREQBERAEREAREQBERAEREAREQHiWNrgWuAcDtBFwe0Ffn/0m4OKbEHhjQ2OUCRgAsBoGvAt9oX/AGl+g1pXpV5NGrpOcjbeeC74+Jabc4wHrAv2tChOOZFlOWWRw2OUjRRZZbutuWP5SCLhemEHVZVG2pscr6EimkYDoMzuw2HirhlZM0XDC4Ha02+9VUL3A3aAVZw48xos+Nw7BdebmqnKMVqXFPiczgA6PMOBtZYaidt7Broz1gkA8LjTVe8Pxxp0jiJ63dHb8VZyyhzbEDrFlXJ2JTcZLQlYLVG1ybiw+G5TXz5hbj99/BUFO/J6p0PX4qRLX5ALanz/AJnyUMupXfQ2fknhonqczmgxxC5uLgvOjfNx7guiMYALAADgFU8lcLNPA1rvXd03n7R3dw0VwujShljY5lWpnlcIiKwqCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAoWK4vBTM5yomZEzi9wHhfapq/NHphx81VQ4h3zbXFkY3ZW7T3nXwUoxvd+BGUrWRS8pXRmqnkhsYXyyOYRoLOcSLdRuoMT1no2Zom3+qFDkjLDpqPJZU73RtcXFJos6OpLSralmv62vAff5rWI5r6hWEFcBvUJUycKptTJCLdG1wdewX04rJJV6XGvnpt+CoIMYaBe4vawvrbj4r7/AFuNct3E6jaT/PaodkyztkW8k/RNzc7OHDRTOTzA6Rs0ukbHB1iNtnXc7sCqcKw98hzS6A+zx7bLaKuO0RaNLtsO8WVc5KOiLKcG9WdhwvFIahgkglbIw+0w3H5KYvz56BsWfDUSQuJyOsHDdmBDbr9BrqSjZJ+Jx1K7a8AiIokgiIgCIiAIiIAiIgCIiAIiIAiIgCLXeUXLKlpWPJka+Ro0iY4F1+Bt6vaVxOTlPXYrUBkk7o4nyBjYozlaATtJGrrDjwVkaTavwQdRLQ7D6QeVEdNSSBkjTM8FjA0gkFwsXEDZYa9tl+dsdgzQ5h7O3sV9iL2Oe4xtDWXsxo3NHqjwXygja4ljx0XCx71ro0k6fxM1eplq/DT8lRQWyDsC9z0t9i9sonQOMT9rfVO5zdzgrCmYuDUTpyaZ9BScakE0a7LS9S9RUActkmw6+tkpsNKdtoPV9SvpMEYdS34lX2H4YxuxoHYFKpaE8Faw0oCpnVbLoUUhS01gvmIuGU8ApwbYLUuW+J5I+bZ67+iO9VwTnKyLJSUItsiejNl5Z5R7RdbvddfoDk/iYmiFz02izh18ewri/o9o8kR8Pgt1oal0Tw5ptbb1jeF9S6F6CXKPkVX/APQ/B6HR0WlT8rZ4XFjo2SbC03LC9p1adhAJHxupXJvl9S1cpgs6Gcf3ctgT7jgbOWR0ZqOa2hsVWLk48o2tERVFgREQBERAEREARF4mlawFznBoG0uIAHeUB7RafjXpEpIbiO87/wDp2y97zp4XXNeUnLSsqdHP5uI+xHcAjg521yvhh5yKZ14ROlcpfSJR0pLATNKPZj2A/afsHZqVznGfSVW1HQYWwNO3m75re+dfCy06vi6JcNy+YOQ7Um3E9W9a4YeMTNOvKSJmIx5YSfaebddt58PNeuQkdqunGy8ht25XW+K98o5wGtcNli1oO/ZcgcFG5FML66mF9edbs6rn7irq8UotdGV0Hqn1Mj22+HkkJsQVLxEfOPPFxUQhVYfWlF9F9CzFq1ea6v6mw1NKydgB0cW9F31XDYew3AI4W4Kgprhxa4Wc0kOHAg2IVthtSMlj7Jv3WIPn8FMxrCs9po/Xt0gPbaBtH2gPEBUekML2sM8d19C/0di+yn2c3o/kz1RwZgsooiCvuEMOhVvK3gvmG9T6grGAgqSwqPUvtoFFkq7BeWuDJi2KiJpWhU73VM5kdsBs3tO0+HmpnKOYuNr3us2D0+Qxt7r9Z2/Err+jaClLMzk+k67jHKuTeOS0OWEK3IUDBD83s0Vm0L6JaI+Wk7sjcq2Wp4pPaAkb12DgR4EnxXO+V5LJYpmEteADmboQRqDcbwt05eyvb8le02aI5R1Zg8E3G/QhaXjtS2Zgv0XjduPZ+Cow0X6un+7m7FfyZfvB03kr6RXPjaZ25tgc5ujgeJG+/wCK3zDMWhnF4pA620e0O1u0L838m6nI4scbNdpfhwPcVPwPEZIqtxzFjwS02Njoo1MJCWsdGIYmcXZ6o/RyLneF+kFzDkqWZraZ2WDu9uw91lu2G4vBOLxStd1A9IdrdoWCpRnDdGynWhPZk5ERVFoREQHPOVXpMjiJjowJX7DIfUaer65+C55X4lUVDs1RK9/UTZo7GjQKjZoQthe0Oa143jXtXXpUIx2OVVrSluQ3ts1ZZIQ6IO8V7dHcELzh7ug5h4Eq+xnuVR+ilPBhVVhLSWgcXDwGp+5WdO0up5RvLT+9+C+clYLgvI6EbXE91ifJRiryRbe0WQeUc2aQMGyMZe8esfG6t/R9KxlfTPkcGMDzdzjZo6DgLndqQqCZpc4uO0uJPadSrGCGzNRvUp0s914ko1FTtbgscTrIWuJ55h7Df4DVUFXjzBpGwv6z0R+J+C9Ppgdo2FeH0QG7eqY0JQgoJ7aFs60alSU5LVtv+yBDjFQJGvB0a4HKBZpsdh43XTcDxhkwYWaWbqDtHUtA+TgHZvWI5o3ZmOLTfa0keSQjKG+pGplqbaHVWx5Ndx17CUM+i1PCOVbrBlQM42Zx61vtD2u0aq7Mg0cx2ZjvVcPiD1jguD6QwWR9pDZ79Du+j8a5rsqneW3X/plncqatktdT6iXRa7XT3dYLnU4OTsjp1JqMbsiSDM7Md2xWWFdIhttb3v2Xt5lRmR6KdgEWaUhujWk5yPatqR2C1uvVfV4TD9mlFeZ8li8R2rcmV/KKeqhnEsUjmhjGi1zldtJzN2G5JW4YByyhmYOe+Yk4P9V3W1+zuOvatV5Q1Wd+Ub16ewc3a2xoW1UVmdmZHUzQWZG9cpquGWh0lYXMmBa0OBJa5gDrAHYDr3LnWIC7T1LJh7LZl8mZ0nN4qNGh2cMt73b+ZZVrdpUzWtt8itoJ/EHXfcLYMVhIMNSARfKx/UbXY6/W2w7gtXawsksfrEfctwkm5ymcw74h/qZfKe0Ef/kLyK06oT7y8GT8RZ0mu3PYHd+w+SxCQs6QJBG8Gx8QvkFRzlJTybwXMPf0h96h4hJ6rBvKt0tczq97G7YDy1qYmtMh52O9rO9bud+K6NguNw1Lc0Trkes06Ob2j71xXG5MnNU7NXZRf3nfkrGleaUsEbjzwsXOB2fZPHsWSrhIz7ujNFLFSh3tUdqRc5/+ez/Uj+P4r6sXqVXwNnrtLxOSTRaHiFbYPUZmEd/j+Y+Ki3Bsdx29u8KPQSc1PlOx2njs+Nl01oznvVF4AsAGWQcHaeKltCw1rNAeBupMrRrhmyxuaNdXaDaTmIDfFWMg5im+TjbYZzxe8Xy9zLn9oLDgcTTNI9/qtlv3avd8Lq1wGmjmqGtqT67XSWuReWVwcGkjc2OwHYoKWVZjQo5nlNe+T3v3FT5G9EjqBWzcocBjjczmQQXAjILvLiLXc3eBqNqj0HJieQXdaMaj5zom4AOotcDXbsUo4iDjmvY8lRnmy2NaEVz2i6sDgk7hcQSWLbg5HbrdStaCrhp9YryuItmLcngTctHYLm20KPVYvO8WdIQ0gjK3QeO079pO1M9ST9lWXX8HjjTitXd9Ch5jMD2eSjthDrtPUVZ0TNLdRCiPFiD1eSsa2ZWnqQHUhHcbKfhtW6O9th9Zu428j1qa5gOvEA/cjqHQlum0HgQdVCpRi10JwrNPqe6yuGW4OhGn8cQq6ghLzfidvBYK6nOQtB6Wa47SQCOy3kFbUpbGwA9g4uO3yGp4BcmhgVTrtrbg6uIx7qUcvPJAxKpLGhrfXfp7oOhPaVdUMAp6QHY54PhoPxVJhFK6eqF9bG/8dgVzjtRncWt9Rlmju/NdmnGxxqrvaJSMYXPJPUFYVGxw7B5JTw6HrcPgrBuFl1y42B17tN38lJzUVdizk7Ir4Kfol2YbRpvXmSnLn6cQVdxYZGNuY6jeGjyPVvWb+qYXD1pGO23sHDdtaLG3WPBZFiIuLjGabe37yaXRkmpSg0uTTcapdc3WTp3KxhJ+T34OPgRf/wBvFTsZwstYdhGtnDUHd3dhWGgI5m3FubvFh5OK0JXd/EoctPgZcFH9ikb9SZh8bj71jw4B9U3N6rdT2NBJ+AKy4IP7PUDrhPxsfvUKma4xTlnryFsLP+4ekR+wH+K82ieJXkyxwipzOlrXjVzi2Fp8+wC3ipMAJdba5xufxKjy5WAAepGAxvWRtPe6/wAFbUNPzceZ30kmwcGqxaIqlqxzHWEX3TiiHhpsZynK7QHfwO49m49RXnEmFzM9rPjNnjeBuKtZ6LMLKDASHWcLlrbOb/iQ/e5g8R2LP0NSdy5pJ87WP+sNfe3jxus1Uy7HdhVNhRMZMBNwT827jcZoz2OAcO1pVvz12OP2H37mlSvdFco2ZS08X9nkP+K7J/8AYWR+RK27k1VMD5G5bPc91ndAdEBjQ27iCLWvYXvc8AVq0DrR0jPryZj2Nu7zstkw7C+duY5C2VkrsjbWDyAHENeDo+wJAtuVVVRdNp9C+k5Kat1/BfGRwzSNLc7iBncNDls1rRYkkEgXudS4rXsPJrakNqXEHpMAY3ZkuQ3fbebm62GKOMtaXgSOFn5nkNsbAh+QWGgN723EHeVrlLIXVklhYPlkbZ1xq5r22NrFtzbsJWWhtLxS3NVfePg3sTDyei0y89cueLOYRvfk1LPaDRru+Cp5MHmvYRO9bf1kgam3X4LdZtS9jpGuZck2bZgbYBrL5r9IODht9rcoGISh/OBzxkLYyHgtZqxzwN9iGjKbW9rst7TxNRdRUw9N9DTYactLmuFi1xB1B13i4Ubmb5h9oqe2a5kc7ecxtpq/U/Er5TsGZw4ELpq9lc5beraItKy7AN7bt/DyXyeWze78lJDMsttzlExeOzT3qLfskkvaIFI4vdZY6h4dXNaCSxjDbwNz3lXnJLDQ6J8jtriQwe7bNftuAO9UjJM9W94AAtlFtNFTHZMvvq/gX+Bwc3FJJvIyjtcfwBUSdmlhvcrqraGwxtvtcXH9kWH7yq2PBIcdmUu8LWWhPQy83JtFDqTbRv7x1+At3nqWHEsRIJawi9ruJ3cQOOunbpptVnRM+bjd9a7u03sfJa/FGOfHOCzedbnObdoHDLxuH2PFcnFSz1sr2X78jr4OKjSzLdmWHCKuVokYx5bxeQAeptwd5ttXplRPA/I5r+iOk2Tbv2DeLC99Owrd8RL8xjMmZjbFtg0AC3RBygbAR1bFG5ZNLqZk0jWh7XtDCPWcCCctu0D+CufDERqTdNxN0qbjFTuVbyJIucbrpcjbmDdSPeA1HYNxVGI7AtA0BeARssRmA8PhZXXJTUyAerdpsb7LvuDfXYAP2V4o6cGwGzO9ncwvaPgAuvgKju4Pj8HKx8ErSXJW0/QirBw5sd5e5ZcOp8scZ3taX9skvRaf2WNcf2lAwl5mjkt/fSxke7nfr4K1qHc4/mYza+r3D2GWDR+0WNa0Djm61svcxvS6PWFUwkfzjvoYjYfbeNp6wNnapmI1JDS8+sbNYOs6AKSxgDWxsFmN0AHV5/zUelYJJy8/RwaDg6Xfb3dnaVO5VuQv6kqOPxRbH8peiZmLmsD7lWz/AKXD2nyX1FU9y2JFbsp/+x/5D1aS7J/dm/dciLyOzLKm6K2H1qD3X+TFuWA7/wDMt840RU1vdvyLKPvV5/cn1X0LP8yf/IKop/02X/Nn/cciKmjtL4Murf4/FF7hf0tR7rfOVc8b/efsebV9RXYLvS8irHbR8yadknut+5e49snujyK+otphPdZ9KztWDHfUKIqnsyxbxLHkx+is94+RWo0f0v8Ap819RQ4RbzI27GP7r3X+Uapn+oP1a+or0ZkbLRfosPbL++VQ4l9LJ3fvBEXHxP8AI8v9mdnBe48/sjpOBfobf1Q/dCpOU/qUXvD/AHIkRZI+8Xwf1Rpfd8/sQuSvrv8Ae/5yr5hHsfrJP3pERbsF35+X0Zhx/dh5/Y1jkb9DF7h8nqzwH16j9b/xciLoQ2Riqby/eS7ptij8nP0Znvyf7j0RTKOC0REQH//Z</t>
         </is>
       </c>
     </row>
@@ -2663,25 +2663,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>JOS BUTTLER</t>
+          <t>DEWALD BREVIS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>t20blast2023_127</t>
+          <t>sat20_2024_28</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E18" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>131.2</v>
+        <v>90</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2690,85 +2690,85 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>40</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>14</v>
+      </c>
+      <c r="X18" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AI18" t="n">
         <v>2</v>
       </c>
-      <c r="K18" t="n">
-        <v>3</v>
-      </c>
-      <c r="L18" t="n">
-        <v>40.6</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>0</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="n">
-        <v>32</v>
-      </c>
-      <c r="X18" t="n">
-        <v>20</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>36</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>18</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>22</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>0</v>
-      </c>
       <c r="AJ18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK18" t="n">
         <v>0</v>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="AM18" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUWFRgVFRUZGBgZGhgZGRoYGRgcGhkZGBocHBkaGRocIS4lHB4rHxoYJjgmKy8xNTU1GiQ7QDszPy40NTEBDAwMEA8QHxISHjQrJSw0NDY0MTE0NDo0NDQ0NDY0NjQ0NDQ0NDQ0NDY0NDQ0NDQ0NDQ0MTQ0NDQ0NDQ0NDQ0NP/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAQMEBQYHAgj/xABAEAACAQIDBQUFBgUDAwUAAAABAgADEQQSIQUxQVFhBiJxgZETMqGx0UJSYnLB8BQjsuHxB4KSJDNDFURzosL/xAAaAQADAQEBAQAAAAAAAAAAAAAAAQIEAwUG/8QAKhEAAgIBAwMEAgEFAAAAAAAAAAECEQMSITEEQVEFE3GRI2HBFCIygbH/2gAMAwEAAhEDEQA/AOzQhCABCEIAEIQgAQhCACQlftDbFGj77i/3Rq3oN3nMvju2jG4pIFH3nNz6DQfGK0OjcSLX2jRT36iL4sJzLF7Wr1Gs1VzoTlBsu8fZFh/mZ/G7Ws2WmA2tixvYHjb71rHW9pLkkNQbOu1e0+FX/wAl/wAqOfja0YbthhvxnwT6mcgp7ftoyM1uNxqeW75Dxkdu0TsbKijmPeb6Dx+EWsr22dnHa/DfjH+z6GPU+1OFP/kI8Uf52tOK1NvuoHdDE8fD7qjf6xKe33B7yZhwt3Rf01hrD22d5w+1KL+7VQ9Mwv6SbOH4LHI9gHBci+W2U9bAnUS2w20K1M3So69Axt/xOh9I1IlxOtQmDwXbKqulRVccx3W+h+E02zdv0K1gr5WP2X7reXA+UpNCot4QhGIIQhAAhCEACEIQAIQhAAhCEACEIQAIQme2/wBo1oXRLNU5cF6t16QAtNobQp0VzVGsOA4noBxmL2t2qqVLrTvTXyzkdT9ny9ZQ4vFPUcu7FmPE8uQ5DpG7yGykhWN9Tqecj4p7KfA+pBtJF5l9q7eRn9lTOYEWZxewYahV5m4Gu7WS+C1ySsZii1lR9XUISN4sSz68CdB0zSjr1WtlX7RAzbgqDvMFA/CANOZ11juGLZQF4ZgLb+8fnYj0npcAxvcW0I8L2Jt42nPVud1HYj1KZYhRfXfrYhd+VbaC99SOcdfDZcqIMztmCgaLobFm5IOvDzk6jhyC7Ea2AHLmD841icyq665nJW9tQhBJ63v85Oqx6SGaQVQRd3a+Un7ZH2rcEFtAN51O4SNh6bs3Enix3eCqBraaMUVVWdwAbAHkgIGVNOShQbbyD92VGNdySFY013X+14afvhHq3E4jFRG1bLcKdODKRx01vNDsjbCsgDtruBO88AD+KZpNlvlzo6OBvuoNvEEXt4XjVbFENqEHA5Qcp8r7/wC0tPwRJXydEhaUGxNqa+yc94aKediBbr/aaGWnZyaoudk9pa1GwY50+6x1H5W3+t5t9l7WpV1vTbUb1OjDxHLqJy2e6NVlYMjFWGoI0IlJktHYITLbA7TB7U61lfQK25X8eTfAzUxpkiwhCMAhCEACEIQAIQhABIsSZvtVt32K+zpn+Yw3/cU8fE8PWADHaftJ7O9GibvqGYfY6D8XymFLk6k3J1JO8+MQnidSd8JzbspBeKDACLaAyt27iylM2NmbujnqNSPAfpM7szZqgquUM1rnja+5Rz8ZN22rVK9vs0wB4ltT48B5TQ9k8IpN/wB2ta/nunKcjRijfJO2P2fRFzOMzHhwH1lsNl0yfcH78ZOCCPosz7s26Uir/wDQKROYDLpuG7xtPNLs3TBudbajTlul5ki2hRNIo37OISL6gG9uGbgx5/2Ei4vshRcENx4+G6/hwmlBiPrCw0o51jextam2bD1BbdkYaEcjrr4yl2rshhZnpBGI1AIIJ42M6rUQ63N+XTpIOIoq4yuoYdY9bB40zkOQowI969763HXpNpsvGe1QE6MLBh15joZD7R7EVBnp3C6X4/sSP2ecq1uDC3mN36+s7QlZlywo0NoWnqAnYzBaavs12jtajWbTcrk7uSsT85lIRp0DR1+LMj2U25mtQqHvfYJ4gfZPXlNbKTslqhYQhGIIQhAAhCEAK7bO0loUi7anco+8x3D98py7EV2dmZjdmNyesuO1O1PbViFPcS6ryJ+03rp4CUZkSZSQl4XhaAEQxRFiQgBn6yZ6jAHTMSevCwHp6zYbBTLpbf6E7rDmBoL/AEMx+Ff+cwP3jv334W+c1+xS2YAa6a7ydN9uWt9ehmaRux8F+uscVwJ4Qx6lTvOaNLarc959J6DCONhtNND69dZ69lprL0s56ojNQ8pGZ2k0p/eKuHvJ0sFJLkrPancf8Ruqkn18OJBqrbQaxNFqSfBn9t0wR14fHhMpg1C11YcTbpr/AJm8xeHDrY6NvB4+HhMbjKZTEqpG9h53Oh8dfhKg9zhmW1l8IsSF5rMAQhCAHpWIIINiNQRwInRez21RXp6++lg458m87fOc4vJ+xtomhVVx7u5xzU7/ADG/yjToTR1GEbpuCAQbggEHmDujkskIQhABJS9qMf7Kg1jZn7q8xfefIfpLqc97ZY3PXyA6Uxl/3Gxb9B5RN7DRQWnm09wtIKPBELT3aIBADzaAWe4AQAzGIQJiWHDRiehAJ1nQ8AFSmpHG3x3CYDtMhV0caEqRfqDcTbbPfNh0I4ohF+lrXmbJybsPG5PauNy7/h9IlfFYhdUplhyBW56i/CMe1FJCxUn8I1JPADz4nQcYz/GYqorMmREVkRmZWa2a17KLMwF9SLXuAOiivBcntbHMLtLE37+YHqFsOmm+XmGxZYC+h8P1nPtl4zE1aS16lw5YrkK1A1s2VTZmIKnXgCLHWbbZ4ZACWBuN2ulud/nG7i9xRqStFgCeUq9o45xoht13SXWrsO9f99Jndsl/ZtUQ3N7ZRv4XsTpflfxk6rL0+QTC4p3zCooH42JPSwtJr4R0HecMegt+syz0sQz0gjMKbKxdkVAQwW9PR7s12sGvc790tcVhq1Jgq1c62UnxsMysBo2t+8ttLedSjSsiLuTVEoV2zd4cN8zG3Sf4qj4r6FrfoZqh31vM/j8C1TE0wN4Ukm3BT1kRaUrKlFyjpJsJ5Rri4JIuy3ta5Vip08RPU1p2rME4uMnF9gEDC0IyAhEiwA3XYvH56RpMe9T3fkO70Nx6TSzmXZ3GeyxCMT3W7jfla362PlOmy1wSxYQhGIar1Qqsx3KCT5C85NWqF2ZzvZix8WNz850TtXXy4Z7b2yoP9xF/hec4kSKQsDPMIhiwhCACwS1xfdcel9YkDAaJlLBjE/xNGqq/y6uVGVbMt1BTx3/GP9ngPY0/yKNfDWWuz6KqKlQWzVHza8wiLr00Er9kU7ALyuPQkf3mOWx6lp7lk9BWIv5Dh4z2FVb2+f1nt9dB5xWw4grFt3KOvgC5ABso10+vCWtKnlW3IfvWC1FDZfhPeIY62Hdtv+kKL7jGIbu9LStxeGDrpxHCWlTDNly/hv6i9vG0g4d3FiB3eMTQ3TWxDwNJkIBJsN2l7W3G4N5aEA8bnp9JFwePps7I2jA+A9JZfwo4eMNxOiEwA8eFuOkgUReutrAsjgX6Mh08ZZ1l338pRbUxJplWX3rsOveyi+kQ0rdHilQZEVWHeDVb+PtG187X84sdxNXMcx3nX1Av8YzNeP8AxR5/U37rsWJCF5ZnCF4l4kAPRnUtkYn2lFH4lRfxGh+IM5XN52Gr5qDKfsObeDAH55pURSNNCEJRJlu3VS1JF5vf0B+sw5mw7eN/2h+c/wBP1mPtIlyUuBIGKZ4iGe4RIQAWBiXhAC8wVFnCMGChGVtRcEZQCPUfu88bKY53VgAc73A1A7xNgfAj4CMbN2iEGR1zLwI3jpbiIYXFB61QrcBnBF+HdGp85lnFo9CGVSS8l+hNx6xramNFNCzf5jSVCHXkQR8AR8j6xNoIAy1GGYIBlG+zknvW4kAacrkyUy/kY2LgX/7tYEM3up90cM3WPYikC+f2jiwyhFayDXU5bWYnTfutpaQzt3DFsv8AEKzfdVszC3Aj1j67RoWBAOnMHdp0lUylvuN4nHvmyBe5a2bj4WjVNBmzkuCBaxd8uvNL5T6XkttrUgd3llFz1tvvGK21Kds3s313WRvT3dYUxrYj7WwK1sroQtVBoeDD7rfWWGy6rFMrCzAag/vWUlXbOGBALhWNiFNwW4AAHfrLjC1bpmsRqbX32+htfzkO0Jvseqrg3B4W/fhINMA4kcSKdQgW5sgYn00jzsC733AKDbfzPzEp3xDCu5Q5bUwp595zbX/Z8YRjqdEykoq2SNoHvkdf8fCRrwJhNkY6VRgnJyk5MWJACLGcxLRbQhABLTWdg6nfqLzVW9CR+sygmj7EN/PYc6Z+DL9Y1yJ8G9hCEskxnbwd6j4VP/zMlabLt2ndpN1YeoB/SY2RLkpcAZ5tHLRCsQzxEM95YhEAPE9RbRLQAWLhKmWrb7687aqfoYk8ul9RvUgjqZE1/azridSRplYe9e9tdeB8tN/ylgFDDUi1gR485nMBixYAHnccuYHS0tExAFgDxA6eHXUiZjcyMuwqdCscTh1VKjKVcG5R1ZgzXXg1wNRLCjtCpqzUFIyopy3+yTdtd62IsOm+PYeqHG8evGI6sN26dE/JOmL5RIqbaQsGNNswzDVdRe249bDwvIGI2q9wyUNC2cs2mpQrvH2gbeV+MZqq2u/Xz8PDWe1om2t9N1zf/HGDkmNYoLhFdhtmJUqe1rKrOFCr3RZFHBBw8d8saoA7o0tuA48PPWOMuVb6C/68hxlS2KuwF+O8edtOFyD6Tk9ym/AVTlViDqbtffwsPqJS0LEuwG9ram/uC39WeSNoYq17XOYgKOZ3f38AZ4pUwqhRuAAHlOuGPczZ5bKItotoQmgyBaFosIAJCKYkACaHsSP+oP8A8bf1LM8Jp+w63qu3JLerD6RrkT4NxCEJZJnu2dK+HzfdZT5Hu/MiYGdQ2xh/aUKic1NvEaj4gTl9pEuSoiwiRbxDCeTPRiQAS0LRYWgB5Aj2G98AbzfT9ZHxFQIpY7gN3MnQD1IlF2VxzVsVVZjfIiheQu2tuW6OUPxuTOmGX5VE02JwpQ5xYgm/ha1x1vfhv9J6p4wEDja1wSdLEmw5G1uuss3oggXtl011tcbzqfDd8ZUYvB2FrWBJOua2877cZiPQaLbC7Q7xubakncbHkLaE8LiWahmF76a7tOnz0mENVqTai41GgubHy3bvhLnC7fUqBnG4C3H47v7xiui/FEcz/eD3UXzG37+sojt9L2J5a34cP8eMiYztEhsM269hrvHnu0MKHqssNo7RtYg3+Og36/Z47pTLj+5djvYgEG46Dx436yqqYtqhygnfa3E349BvlpgsCHIL3A0ub7sotoAfj4RMKs80qTErUfRmPcU/ZU3N9ftH5ASXKXtqxXDMRoQ1Nhb82hvPPZna5rIFY94DQ87bweo58R4TVghqg2uxh6p6ZpfovIXiT1KOIRItokAAQixIAE2XYWl3aj82VfQXPzExtp0Xsrh8mGTm12Pnu+AEceRPguoQhLJEnMNs4X2dd04ZiV/K2o+dvKdPmS7bYG4WsBu7jeB1U+tx5iTJbDRj4CEJJQQixIAEURI1jWIp1GXeKbkdDlNjHFW0hN0rKPa20M7qi+4puT95hp6C5+PSQ+wIC18RTb3sqkDmFY3/AKhIdTRh4CI1R6FdMSlyV95R9pTow66Gel1XTfgqPY4dNmrMnLudVS2Ua8hawt4HTjPdSgCNBx1N+m82jGz8SlRFdNVcXvyvw6HUywC/vj6+c8BM99opMTs64Yb78bnXqb8uko8b2dc3yi43gn9/u02bpr+/iIlO17nw3H/EEJnN32DiVOiXvxG7WP4fYVYkF7LbkLm3757p0sgb/wC2srsQ4udNI22JFFgNkhPMd43JJ04eessUpADQW+d+ZPGSEQncLCFZLDiTr/i8hs6JGS7ZL/0lQ8jTJ/5qP1mI2BiSr93gQy+R3eHCbztq9sHV/FkUebqfkDMLsqgRYka6/H/E9H09Ns8z1HY6PhqyuoddxHpzB6g6RyZnZGO9mxVj3G/+p+94c/7TTCXnwvHKu3Yy45qUbCEWFpwOgkIsIwHMNQLuqLvYhR58Z1WkgVQo3KAB4AWExXYzA5qjVSO6osPzN9Bf1E3EpIliwhCUIJGxmGFRGRtzAjw5HxB1kmEAOT4vDtTdkf3lNj+h8xY+camz7YbLzKKyDvLow5rwPl8vCYsGQ0UmKYkgYvbFJDYtmbkmtvE7h4XlDjdt1HDAWRPw+9bq/wBLTtj6ac+1L9kSyxiXe2trph0JNmfggP8AVbcPiZlq2067kF3Nr3yr3UHSw3jxvKpu8yqBZV7xkxzvF+9a/h/f5TfgwRhvz+zPObZKqnWS1F1B5EfE2+ZEjBLqp6D5CSsOO7bnpNvJmbLfs9jjhyRvpE3K8adyBmHNbkeGk3lNwwBU3B1vOa4aqAVYi6mwcc0bRwf9pbzAMvcLVqYR8jHNTJORufQ8mtw47x0+b9QwLFluPD3Pp/T83v4afK2+Ua126RtknililcXnsvYzEmd2M1s9ve06DWeFo8/jHzWF7T0msbZKQImk8VUvH2EYxTBEZzoACZDOsOTGdr39pUw+GH2nRn5atYD0zGUhoAE/nb4sRLfYdFq2IbEtuQkjqxBCjyU38xIm0UyvUX7rvbyckfCev6TJOTj+jzvWsemKa80VtTRvESxwW3fZqFdSyjQFSMw/CQbAjlrIWJXUEcyJGrUro09fLijONSR4MJOLtG2weLSoodGuOI+0v5hwj15zTZldgTZiGU6MDY+omiwfaF10qKHHMd1/PgfQTzZ9JKrjubY5ldSNRPaISQALkkADmToBIGG2tRfQPlPJxlPkTofIza9kNl3Pt3Gi6J1bi3gP3umWUJRdSVHVSTVo0ux8CKNJU472PNjv+nlLCEJRIQhCABCEIAeCL75xr/UDYtWhVzKzmhUPdsSFQ8UYDTqCd/lOzyHtLAU69NqVVcyOLEfIg8CDqDOmLJolbRM46lR81u3fIHuqJ5ructrC3Hrz1/e6Xnavs/VwNY02F0csadQfaF9x+6wBFx5gyixqWS3O09VNSjqRkap0yPRcAgga2AvflfUevwnumNTHVpjQDhEFPU+MpRqgcrLa2gnqi080hdQegiO6rqzBfzECdbSRxqyTbeOfyO/9fWbDZ7rWoIXAa4yODr3kOU38bBh+YTnz7YoggZ7kXHdUkevGWexO19ClnV/aFWswyoDZhZTvYbxb/j1nlepwjmxLS7aZ6vpmR4cr1bJo1pQUQWLWQby1zlB01PK9tTuvH0xYIzKwdeakH5TNv2/wpBApV2FiCCqAG41B726YyjtTEs7NQuoUM1lUHKigscxIu1lUk9FM8vD0zcXrtPt4PR6jqoqS0U13OvU6t+VvHW8tKKc5htibeV0zMLNYBgOYA1XjYjWaTB7VDm+a/IC1vGcZxcZOMuUdIyUkpR4ZclekyHbTaqqBSDd5iFCD3mJNgOgvbUyVt7tCU/l0u9UYXvoQi7rn9LzIYTC5q6O7Zm9oh4n7YuSTvM14OilODyS48eTPk6tQmoR5v6NngsGtJRTXhe5+8x95vP5ATLbeX+dUHPXzamD8zNerTK7fT+e55hP6FHzBi9Il+d/D/wCnX1dfgXyioxB3evwkbBYgM1huF7ngOUkYtGKkKLm1h4nSVdSoqq1JDfL77febiJ9FKVM+bjG0Q8ViVSqWUHKd44E8x0k9aytqNL893rKisMyXE0XZnYNXEstKkLsRcsb5UX7zHl85mhJpu+OTtJKl5LXsnsB8ZWFMXCLrUe3ury/Mdw9eE7xhMKlNFpooVUAVQNwAFhK/s7sOlg6K0aQ6sx9524sfpwAAlvMOfN7ktuEdscNKFhCE4nQIQhAAhCEACEIQAr9q7LpYim1KsuZW9QeDA8COBnEO1/Y/EYZ1VVarTeoFpuouSW91HA91r6cj8B36eHQEWIuJ1xZpQ448ESgpHzxiezuIoqHq0iqAgMwem4VmtlVsjHKTcWvobjWQkQFzbcf2Z3bbWyGdSKbFEIOcUyVqG1rKjDRQRcE2JA3akEc1x2LwKOlPD4EVamdEZK4ddbgBAHJOfPlFyLWBGt9N2LqXJU1b/X8nGeJLuVGA2O1fuLnCA99kKgjiQuY2LHl57hHq1PA0Tlo0EquMw9o7MyC9wLa3qMOLXCm5y6WtK2hTxlVnpHDvSpo2mHprakhYA5bqAr5icwve5fTlKWvTKswJW6m3dZWGm+zKSDrcaHgZ0UI5Xqk18JkNuCqP2MjZ6M5Zhcve/ifl4SLh8Cq1crDQ+758JZsDkza6btOI6+UZ2rTuq1F3ix8jO2iNbI56pXuRKezQGdbaixA5i9v1kvZwCCoEUEuuUhwwKG4IZcpGug33GguOY9UMUqDeRlb4Ruq4bjZhuI0IicItU0ClJO7GlIpg35agjdrvuNDJGzdpMoLscqH3b6Zuo6dd0ZCltHs2l7HRQPvOPkOPzh7Ro5lU3JzHS+l+tuA5CZM3SxlPW1e3Hk1YuqlCGhP/AGOVO0i5murG5JJBXvHn1jidoKWlg4III7o3jUcZUNggNBvlxs3ZSqMzC56y4LK9nVfBzlKC37mlx3begtvZ0ndjzGRbnx1lVjsViazVKhw+QUci1BfVMzFEzBu8bspGmg6b5Aq4VWY33fpO2bJ2e1bBXqMwfEYWmjhlVgrezK5wNLk5rkE8BumT+nh0jU4rk1z6ufUx0yexxLbdCvToU6rEKtdWdMrAtlU2OYb1O479x53EqcBhyKTOb969vAaX6639J9C7R7KUaz4Y1KdNkoqbrkIDaAKuQErkza5TfcBqJUYzsF/E1UaqfZ0wKhdVYs7NUqu+RXIGVAGHDTMwAG+VHOnK5eGcXjqNROX9kOzFbGWFNe7pnqH3UB+bclHw3zvPZ3YVLB0RSpD8zNbMx5kj4DhJezdm0qFNaVFFpou5VFh1J5k8SdTJs5Zczmq7FRgk7FhCE4lhCEIAEIQgAQhCABCEIAEIQgAkptsdnMPibGtTBYEEMpKtoQbZhqRp9LS5hBNp2mJpPkyGL7OsodgXYs2clXq27oRVGQudQFDC24rpbcaJqYpsB/D5DWqYYZ2srqxclQxYsWJamiuAALXsCdT0yMYjDq4syg8OvkRqJanXINHHNv1qjXQNdc38QgzuwNOsigDK4B0ZHOuoLMOppcMQyFeV19d06njewVB39oj1Ebce9nBGgsc920sLd7S0osR/p3XVnanURw3BsykEeRE9HD1GJRUbMmTHNybo5c1TISjbrgjof8T3RTMxO+x3HmfdHhpfwE1O2+wONY3WgW03o9M2PgWBPpxnjC9lcYlMZsM+cgXAXNbnuNibADfbfOyyQbrUvslxlV0UTUc1gfd32vYufvseC33c+EWuhJCoNefACXi9mMa3/tKmvFwLk8z+9JKpdjMfkIXDkFja7PTAUc9XvK9zGuZL7I0y8My2GwozW323nrLKpoJrtl/6c4gAZ3ppzsS568APjL7C/wCndAG9Wo7/AIRZV+He+InOXVYo9/otYZvscqwKF3ULlzM6hc/u3LADMPu8+l517A9mATVdnrIHa1OmlWoi0MoKk0wjBWUkBluu62m+XuzNjUKAtRpKnUDXzY6mWMwZ+o9x7bGnHj08lfsnZvsVymrUqni1Rix8huEsIRZme51CEIQAIQhAAhCEACEIQAIQhAAhCEACEIQAIkIRALCEIwEhFhEAkDCEYghCEYCxIQiGEIsIAEIQgAQhCABCEIAEIQgAQhCAH//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAQEhUTEhAWFRUXFhUVFxUYFhUVFRUVFRUWFxUVFxcYHSggGBolHRcYITEiJSotLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGy0lHyUuLS0vLy0tLS0tLS0vLS0vLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPsAyQMBEQACEQEDEQH/xAAcAAAABwEBAAAAAAAAAAAAAAAAAQIEBQYHAwj/xABMEAACAQIDBQUEBggCBwcFAAABAgMAEQQSIQUGMUFREyJhcZEHMoGhFCNCUrHBFWJygpLR4fCiwiQzQ1OTsvEWNGNzo7PSFzVEVGT/xAAbAQABBQEBAAAAAAAAAAAAAAAAAQIDBAUGB//EADgRAAIBAgQCCAUDBAIDAQAAAAABAgMRBBIhMUFRBRMiYXGRscEygaHR8BRC4QYjUvEzYhWSooL/2gAMAwEAAhEDEQA/AMwNOAQaAE0AFQAKACoAFAAoAMUAHQAKABQAVABGgQKgAUAJNABGgUI0AFSAFQAVAAoAKgAjQAVAEgTSgJNACTQAVAAoAFABUACgBQoAOgQKgBQQnUA8L8OXX50gok0ogCCOVACaACNABUChGgAqACpACoAKgAUACgBJoATQA/vSgEaACoAFAAoAFABUAFQAdAB3oAcQ4RnIA4t7ttQ1+Q8fA2prdhUi8bE2ZAqtDMqq5BRyDe2ZbcATc2IPXSqlScr3iWqdONrSOS+ztgRnlc31usd1tfiGB425W69Ke8TyQ1YfmyRxu6UOISNFlKtGhS4UG4vcEqzA6HiRYVFGu4ttrcklRUkkmUveDdrEYI/WLdNLSLqtyOBHvL+8BVqnWjPbcrTpShuRBhbKGynKbi/K4tp4HUeo61LcjscjQARoATQAKQAqACoAFAAoASaAE0APb0oBXoAFAB0ACgAUACgAqABQA62bg+1Y3bKqgszWvlA8OZPADnTZOwsY3ZcsDiY4EsiZUNlJGjyMRe2YWIsOlh4VWl2nqWY2itBussilgGIzXNrarfx5G2tDSFTYMHttoiV7Ynp1UftMpF9OPjyolC4Kdh2N5oyotKDY3yyZWBJ4FZADbyIvUTpseqiJifbSTqAmVrD6zDsCyuvPs5LAA+ouPjUWVxdyS6krFG3ggjiIiUnsy5kXjdUAtY31vcsOvdHWr1GbkrlOrHK7FeNTkIRoATQAKACpACoAFAAoASaACoAdXpQBQAYoAMUAGBQAMw6j1oC4BY86AARQAk0AT2FgKwxC9gzh38c2o9FUfOoZPtMmiuyh3hnUagMdbrfQhiANNdOJ9KikSISmFfEuRHIZLC7EqQoUcV0+yOfW1Ncsq1FUcz0JnZG65dsrKSoUMb3F+fDTyA5elMdVvYmhRXEeY7dMCcBI19yRwijKbpl58yQbX8aFN2HSoxuDZO7MOJnPYoWUZSZLsADoRdrcdOA/C9DcrWEywvcZb5bF7KFjMmSRJLC5Hfjb3HzC9ybHXmRwvTqDanYhrJONzPnIPAWq8UxJoAKgAqACpACoAFAAoASaADoA7UoB0AGKAFCgCx7ibLjxWMRJQSi2dltfMM6LY+Hfv8KiqycY6D6aTep6QXZ8CrlEKAcLBUtbyqHKh+ZjXE7v4KTSTCROOjRoR+FKlYVtshcd7PNjyixwix35xloiPTT1p2Z33G202MC3r2R9Cxc+GDFhE9gxGpUqHQm3PKwvU6d0RMkZcSYkUKAWACg8fsm1vgRVXdlnYaAZyMzG9wG5A6XC348BQ3YErmk7rYqGJUUKoPAmwF9AeA/aHrVaRailYucEaAXta4tTUyS7GzYASTdtciysluubL3hrpw+ZpULYd7FwQw8SoFAA6eJNPI3yRWPbIlsEH0JzKh/Zc/iGC+p60+l/yJFeq+wzDavlMTQARoAKgAqQAUAFQAKAEmgAXpBTvThAUAGKAFigC1ezabLjkF/ejlX/AA5/8lQV/gJKXxHpBToPIH1pqHCSbamgBu2I/H+lJcdYwH2wRgbTkP344XPnkyf5Knp/CQz3K/H31Q2ue6Ouq90Lbnw+dQyVmyWOqRJ4TCEkdwliQQCDwFyzfkPjULkTKLNL3Zw4WId0ZrC7W15c6qy1ZbglY7bZ24+FHdjLkjie6ijrc86dEJFVxW+2L0yz4cHmvvPr1Gh+VS27mRZu9Fk2LvFiJIXdypyqWJHCwFybVG2+BKknqytbc2tiMVgp1xDxtEBnUg2kR1YFAbC2rWFjr3qkpSaqKxBWinBtmYVpGcEaACoAKkAKgAUAFQAKACNABUgp2pwgKAFCgBa0AWHcD/7jhv2nHrDIPzqOr8DHQ+JHpPAEdkh/VW/naoY7Ej3CxD3BF/6GhsVIiZEyKTe5HDrYGmbD9zGPa+pONjfk2HQX6lZZgR6FfWp6L7JDVWo09nIBnZblWstmBswDSIJMp5HLcXHImosUtEW8BbO78tC/OwxUcsdnOQMySOqq3HlY97prqbfGqKuncu1FfccbqYkCBLtcka/35USfaGQV4k3Ns2Gcd+NW8wCPQ6U6K5A+8g8XugoJN1tpoI0GgIKg6ciB6VJrbViZY30H+xtnRwoQRmLg5wRYFSLEW5CxIpE9RzjpYgt59zUh2biypQ2USKyoEORHWQq1tDcL04ipqebrE27lStl6vKlYxmrxQEmgAqABSAFQAKACoAKgAjQAV6QU704QKgBQpAFrSgTe50uXHYU/+Mg/iOUfjUdX4GOh8SPSWyWvCt+Vx8L1Xp/CSy3HLrpTnYERGOYEFb624cwDexP8J9KYx6Mh9rcRvhm5WmU/+mw/zVJh3uhldbMpexNonCzpMBfKdRwuDoRfloTU1SGeLQylU6uakbPgcbh5kV4u6WGl+6WF+8LcCQb8KyZq2nI2U1JZlsc4orE8rcOXCo2NWh2ba5htrry+FKpNCuzGeO23iMQezjbsxxLG3Hktvx9KmjeW43SOxG4gbVd1QSplJUZlXKBfmTe/pTnZCZpMG2tuyx4HGwztc5WgB+8zjKv438hRRbdVJeJHiMvVtvcyOtQygqACoAFIAVAAoAKgAqAEmgBN6AO96ABQAoUoClNAD7Y8uXEQN92aFv4ZFP5U2XwsVbo9Q7FPcYdHPzAP86q09iae4W0cQyA5RryuND/SlkNbsRceIMguVCnp8R/M1G2Pg7mce1iG+HjYfZmA+DJJ+YWn4d9truFrLspmXGrhWNX3HRZMDDcXyl7eBWRrVk4lWqs1sNrSRIfTQL3431qGxKN8RMHN1Fz1typthQPsGFm7RtTaxUu4U6G2gIsdePOwqenLs2Ecdbj6LBYVkeNImikZWVWWWYgFtFbgAbafn1qR+IqjPmrFB9pUyJIuGRi2QmRySScxASO5PE5QT++KmwcN589Chjal2orxKXV0pAoAKgAUAFSACgAqACNACTQAmgDtQAKADFKAsGgBRYgXHHl58qAPTuwsTme41DxRv4Wa+vzFUIaMsvVExiUB4jrUrGIr+04LN3RqbX8uVQyH25FO9o2HzYGUjUo0bfDtEv6Ak0tFpVELO+RmOtV8qmwbi4Uw4OIMNSC5HMdoxcD0YVkYiWaq2bGHhlpJMa7xYRge0S/HX041HHkPkMNnbbjjNnW3zFK4MRSRa8LtHCypZ3A01t+NEUDY52XgsGjgiU666nu6cyOtSO1hrvwMH2jijNNJKTftJHe/gzEj5WFasVlSRkSd22N6UQFqACoAKgAUgBUAFQARoAS1ACaAO+WlAFqAFAUAGBQAoUAei/ZxOJMNhW4scMsZPMlLKfmpqntNon/amXBoiBxvTrCXGcsF+X98KjaJEVDfPAlsNiFA96J7eeU2PrUcdJp96HvWLRmO6G6BnKSYgEJdWWPS7jjd+imwFuJvy5z4nEOnJwW/p/JJhsC501Wl8L27/wCDSyLXrNL7I7HDNpSjGVnaOxFYEqden8qljLmQyhyBuxusZH+vdgliQoNr+ZpZVOQ2EHxI/frZuKwspWASCAxpexzNds2a/wBoA5T4aHxrQwuGdSn1ijfXhw+RTxVXJPJexRxUxWBagAUCBUChUACgAqACpACNACGoATQA8y0ogVqADtQAdqABQBt3saxQOEjF/wDVTSRn989oP/dqrV0qXJ4axNTYU5jUzlIKYx6ZE7UwoYEW4qR61DLQngzE9xttmGX6LO3BjGrHkQbZSelxp/0rZ6V6NdaH6qktbXkua5+W/mP6Nx6hfC1Xpfsv2+3kaLiFuL865pGnONhiRbjTkQtHKbZokFxS3GD3Y2A7MWLE24X5Dwplxwnee2aEn3WMkBPRsiSxn4EN/Ea6PoCbzTiuSfk7e5kdLQSjF/mt/sih4/CRM7xSopfXIxGrBrMgLcbg92/Q/GuqnhaVWKlKKfr57nPqtKLsnZlax+xbMoib3wCFfTj9kNz101+dZVfoeSf9p6d/D5lynjE1eS8hjjtnSQkhwO62VrG9jyv4HkeFZ+IwVWglKez4rYsU60amiGlVCUKgUFABUAFQARpAENQAigB+aUQKgAUACgAUAaX7HMX/AN5iLWt2Uq+dyrHy/wBXVbELZk9FmgrvUiYmWDEwlVjYWmUZkCsAy5+amzDqOB0vTOqk1mt5b+XH5eQ5yS0T8/z85lJ2n7Qtp4LGMs0aNHcgRZcqsoYgPHJckki2tyPAV0VDovDV6C6uTzc7315NfnzM+WJqQm860NVzGSNJAdCFa2hGo/rXM1IuLsalNpnnTe7AmHH4hbf7Z2/jOcadO9Xc9GNyw1OXcl5aexiYyyqyRdNzd6A4WDEHvaBHP2uiseTdDz8+OH010I4XxGHWm7iuHeu7muHhtr9G9K57Uaz14Pn3Pv8AXx3uEmzs/CuXWpry0Bs7DlGyHnwosNdrXH8OEIahRY3MiA3gwpfAd7iZnf4OJQP8JHpW5/T7tivk/YodNWcGuVvz1KPtN2mgimP+sjbIx65e8CfWu4pRyycOG5yc53Sn8iGxUpcNG+pU3U8xf8iLGp1FPUam4pW2Fvig5USqGYAAnUdrHoGRiPtAahhrp5Wiq0Izi6b2f5oSRqW7a4CNu7rZE7fClnhIuUaxkjHw99R14i3PU1yOMwcsO78PQ2MNU65ab727v44lYqkShUChUAFQARpAENQAmgB6TSiBXoAF6ABQAuGJnYKo1P8Ad6kpUp1ZqEFdsbOcYRcpbF69n2HXDYsB+92iSI1tNAO0Cgc7tGB43rSx3RcaWClJu8k07/Sy8ynhMc6mIstFqXva0+EYNjZO1CPFg5SY2ALpOrxgNcEcYl1Wx1GugrJpwfVq292vK33L85LM7/lxpjtubGxUYikcZPspIkxKWFgVkyd0/HrrrUdHCYzDzz4bVcrkk69GpHLV8xjtzfBMKYY4HMyJCiZ0nCvdSR37IQTaxtw1NatDomeKjKdS8JX2a09fuVZ4uNJpR7S5pla9pa/6WsnHtYYpC1rXOq3NtL5VS/DjwFafQk3+myv9ra9/cr46K6y/NEFhirDX+v8AWt5aq6Mqd4st+7++b4e0eIu8egWQaso6N1Hnr58K5npToCFVupQ7MuX7X9n9PA3MB0xJLJV1X1X39fE0TZ21YZlDKwZTwddbHxHKuPq06lGeSrFp/nmdFFKpHPSd0PsRIDwPEanw8PGmOSGwi1uUzfHbC3XDoQcveYDkbWVfQn1FdR/TuClZ4iW2y939LeZhdNYtJqit937L57+RVYyO+h9yTKfIjn/fWup2alyMFdpOIy3iwuVhIP2W8uX8vgKdTYP/ABIjEjVSORJ+FjUk+DG09mmWbYePIRNeQt5AWqrWpRqRaaumSUq0qNS8XZp6ELvdsJFU4mEaE/WRgaJf/aL+qToRyuDwJtyOJws8NPK9YvZ+z7/U6RVIYmHW01Zr4lyfNL/F/TiVM1XIhNAoKACNIBzagBNADu9KIFQAKADpQLDsjBdkMze8R/COl+tdR0ZgXQTnP4n9F+bmDj8V1ryR2X1JCHGdlLHL9x1fzysCRV3FU+tpShzTRXwsslRS5M1fcfCxSwQwSxrJGqYnDsrqGUjCYlRDcNx7pzCuGi2ou3NfVanUS4B7Y2VsAOUkGHQjRlVipB6Hsz3SOhqWlUxSd4XGSjTa7RVN6dycLMqPshlmIJEkazLIVFtGszXGulvEVuYLpCrBtYvRcG1b0RSq4eDX9r1IvfvBSrhsG0qlZEQRuhtmF0UKSOIv2LeetJ0RVf6uvTS7N80Xwa4/NXV/kS4yK6mEr67PuZU8MoPgeNdLGxjVG0OgbaNw+VL3MgfOJ1wfaQNnglaNuYB7p+B0PkaqV8HRrLLUimu/25fIs0MdVpO8ZWf5vzLHhN9sQR2clsx0DAZT4g9PgKx3/T2EU8yvblfT7/U0pdN4hwasvG2vrb6DDHx3+tBv97qQdb/31rZp2j2VojHnefabuzmtiLX8QelSMSLFxfWoyNckeVyt+h4kH8qRvK7jtyCxEOV8uuh5ixt5XNS3uhU9GHsmeyAX1UsPgDcfjUNPawmJi890T+Dx491tQRYg6gg6EEdKjrUVNWauLQruEr3sU/eHZP0aTugmJj3G425lCeo+Y+NcnjMM6FS3B7fncb1Cr1kb8SJqoThUAEaAEEUgBWoAcXpRAUAFQBMbrbO7efvKWSNXldQcpYIpKoDY2LNlF7aAk8qmof8AJHW2v55bjKnws0Tb26kSRCTDGbMZFiSN1BEpMjxDs3AAOsbNb7pUm163sN0jNyy1bWte64aJ6r528dDLrYKFrwvf1KltrZ8uHkeORdUbIxHeXMVzAZhpqNavwrwqxUovfzKroyptpmn7kM0uDtC2V3BbNrpI8EsBPheWFW+PjXI4iKp4mcXz/n3N+m89KL7ilbo4LBieSHaRkisMoFygWQHvByOGnA8OPhVhSqKN6e5H2f3Fj2vu1s2CJsRg9ogSIMyqJ43LEckK94N01P51ewmLxNSSpVqd4vu/FYgq0aUe3CVn4kdvBjmx+zzPKgM8DxxNJw7WNjdGNha4JcWHUnS9qs0Kf6XFqlB9mSbS5Pj6fliOpLrKDk90UlFBPStxMym2kds9tG9adcZa+qORkZToO78xTW2h6jGS13FFc2t9etJYRPLoT+yMTnWx4jRh/fWoJqxJE5YjDGNso4cUPh93zFPhNNakc4NPQNAwtMqmwNjpp4gmkbT7N9SSKekraCN48MjhZFOosR4r4ePHSkptvRjpWT8SpYafKSOpv+QqOM8raJ6kMyTJCLEcfKp4yuVZUy1bDkwM+Gmw2LuDIA0culo3jV8jX4qe8eANwbeByelMHUrZZQ2XnqW8FiIU7xl/Bn+2dkzYOZoZ0yuuvVXU3yuh4MptoR4jiCK5pqzsbKdxgaQUKgAmpBQZD0oEOlKICgAUAWb2fv8A6QV7Qx51VcwKixEitc5gRYKrcRb1qzh4/FLLe38kVR7K9i//AKQbDX1jxH0ZBYu5j7JJhHCFygnNKYoG4FSGd+7cgG/GCqvLrHNyV7tXfld96slroQybgr72/PQj9+5BLhhLh5EeGTFTSSEMM4ka6wKUPeFok4W5mp8FGUKrjNNSUUl4cdfEhrtShdPS/wDr6Ex7G9onsplADNGJGC9bhHjX+ISH4mszpaFq6lzXp+It4N3pW5Md747cwbzyR4zZbtkbKs6MVZl4qQ2VdLHgSRUdCM18Eh82uKK1hothu1+0xsfgRCw9VBPrW5TnjlHsqD8/4M+UcPmu7r8+Zc+w2dNs3FYfAvmIjMhzB85ZRoxzAfdtppWdN4mGKhVxCtrbhb6FuKpypuNPkY1FL1rq0zElEfLGWHC48qZUxFGn8c0vFpC0sFiautKnKXhFv0QpcG45aeY0qlPpjBQ3qJ+F36I1Kf8ATnSdXVUWvFperOjbMkUFwLqBc2BIA63tpUVLpzC1asacL3bttoT4j+msbRoyq1XFZVe2bXT5e4WFk1DA2bkeRH3W/v8AprSjdHOxeV2ZpG4WEgnEk0iBzFa0bDNlaxOYrrc8h69Lc90riKlKUaUXbNfXu0NXB04yTm1exbMa8lkZZTdmUCPu9mVYgFCMp0seOp+FcnQxk6lfIksut97q3G+m/wCamo4pRu3qZH7R0hinmiisFBVso4Rsyhio8NSfDNblXc9GVJ1MNGc9/UxcTBRr5UZ4gudP7HKnLtO6JnpuP4VNrcz+Aq5BWRWm1e4+ib8L/Op0VZIs+M7PH4WPDSABkcvFN9pAwOeO3NC1mIvxHlbExnR0Zyc762+vB+xpYTFPsw7zO9p7Olw0hjlWzDXTVWW5AZTzU2PoeYrnJwcJOL3RrLa40poCokuwoS1Bkn9GFTZSLMRlQkgKABQBZN093pcUrlXSO7KkbSh1id/tKJApUMO7oeJI8bafR9fqlJ2bvy3VuNuX2KuJpdY1d29+4k9tyY7Bq2GxBkuwCs0nfJVWzZUlNzkzWNlNtB0rYorDStOlZtctN+a5+JRn112qmiK80xBtzI0qxKbWhGoJq5c/YztO2OMRHvpc/tKcoHpIx+Fc70rPPGLtqn6/6NTBxy3XCxfN7d5NpYUpDhsOcoiQmbsnkOYZlIvbKCCvMHiKpUacJayJ5ya2KDJi+2lDbQlxF+QWNL+NgzKF+ANb+GTjH+wo372/a/qZ9azf9xs0Tct9kLIY8M8hmkRkPaZ7stszDQZPs3+FZ/SMca4ZqqWVcrf7LGHdFO0N/wA+RStpxYNXyJEUWDErDLZQrEPnD2ysxYKYjYnXveNYNXEVKnxSk/Fv7nd9H0HSjeMY3lByjZLdWtwVr5teGhIH6MhyJhZC5/8ADkYqGEmXuTXzsvcNtFYg8tKgtFbItReIqLNOqlHxSva19Y7J666tacdQ02ocKcn0cAguQWsrFXIK6rcDg2ovoRY2Gpmy8BzwqxKzdZy21V1e+/y347oabV3hedChVQCGB1PAuj2A4aFABe+hIp0K8oSU1wd/J3HQ6IpZZRbvdW4f4uP1T121KcTY3HxH9869QjJSWZcTxidNwk4T3WhZ9ydqOk91Le6cwFjnUcFYEG9r+fHXWszpSlCdK8uas+T5rYtYFzVSy10enM0FdooI79nlfvd5CQcyre6rYqqMQFFj18TXOTp9rRrW269Xu2t2bNNW3X5+aIyz2rbSizIqNmZiWLEIC1hYsSovqTpc+PndwtWVOLUuOnH3fsJXpxdrL8/O8pUGlvAD8K2KeiRnz1JCFqtQZUmhzh9fT8zU6IpkzgFYWIF2Jsijjc8DVetKNnmdorVvuJsPTnBqaV5PSK7+fghl7TNnzwzw9ovc7BVjcahiGZ5L9GDSHTplPM1w7xKxFSdXm/psvodLOl1MY0+S83xKaaCI7YM96ljuJLYm6tEBAVUJwUACgDYtxsOyYNGVRJDJGolijBIa4ObPGb9o/Ellsw7oAbQVcjF5Y2lZrVX9nw7r6eBA5K70uuP+iv7Z2xIwlggkkXDElVils7KBoVu4LJqDoLEeddFRwcJRjVmln5rT00ZlVMTKE5QT7PJlOxCfZJsw90879KWrHg9+A+D/AHLbid9lbYlwsyYiMLnS4IINxdSGFweBBJH9KzsZT6+m4v01TLNCXVTuvXRmvezz2iDGydi5KOFzZSQQQCAcrc+PS9cxUoSoS7TuuZrxnGqtFqX79LQM3Z2vpxIFvgDrTf1EE7If+mqZblZ3q2ls3Z0iPkhjlILLljUPY90tdRmFxcetWesxdWOSk5Sj9PqQqNGLvUsn9TK9t7zxTyTmOLL2zqxcsdShuGRbd25vxue8au0ehXNXqTyt7q1/ctQ/qB0HFRjmUbpa2356N+g5n33xbX1VL3vlXqWJsWJI9489OVq06fQVD90pPyXt7mbLp2ovgpx053fLk4rhy14kbjttYiY5nlJIAAuBoBwA04Vcj0Ngl+y/i397EK/qDpCKcYTyruS+1/qNBjWJ1OtWaeCwsdFTj5IrVek8fPWVaf8A7P2OUkmt+fPxq09NihrL4go8TY3BpMyYrpsfw7RkCkI5sbhoySFa/Ei2qN4j51DUpqWq3CE5U3Z7ERvFsrFhllxEUqo4BR5NSQ3esx+y1ydDa9Ykq9KtVyaJLa2xrZZwhd6nFI7XJFbKjoUJSvodEBpVoJbM7IkdnISQApZidFGvr+NLKvGMHOTyxW7fsSwwzc1FLNLhFe/54mkbp7DEf10hDSHh0UdB/P06nielemHiv7VLSmvOXe+7u+b7ulwfR6w76yo81R+Ue5fcm94djRbRw7QSaH3kfnHIB3WHrYjmCRWTSqOErosVqSkjz7tTZ8uGleGZcsiGzDl4EHmpFiD0NasZKSujKaadmNoWswpy3Gsl+3qe5DYiKrkwdAHSCPOyre12Av0ubXp9OGeaiuLSElJRi2+BddlzTYdi2FkDXADRhGGdRwVmGmXzGnUV1GI6unTXXJKK2u0reDMyhTlWlajJuXcnr4rX1J3bONlxEBLbK+usoWQMgUWFiW7NrkcSAAeQ4AAZNHpGlSqLqqyy8nf3TXzuaNToqvKLdSk83d+XKDjHkBs8axt92RGBNua3Oo9K2P1TrK8XH18mmZbw0qLtJS9PNWGOKkfiQt7cgfQm5qCrKpe7t9fuOpxjwv8AnyNt3cwMUOGQQgRjIpZgou5I1cnmTXCYitOrNymzrqNONOCSR2wUa5gyiSYjQuSQAeeXUD4C5qNJPZEt+eg83mLdiJo1UtFdisiDP2djmyFhfTQ28PhUqlP4Yt+BFBQUm5pNczD9ubUixGIeRFVFYjuhbAkABmtyuQT8a6/BOUKMYVZXf5p8jm8ZknWcqS0OERb7PoeH9K04OXAoStxO6AnwPQ/kedWYtjHZHTs78altcZmtsJKnn60lnxFuuBwaFr3FMdNp3RIpxtZkjsBgMRGHUEF10OoNmBsR0P4XqDFScKMuGgsIKc425m47y7HjxOCdCLqUNuZCkaHzX8VFcatHZm7ujGcRuLtaCMPlRwR/q1cu3zAB8lJNXqGMxNP4ZfJ6/nmVp4alJ3a8iA+mohIkV844oMq2/eJJ/wANT1ek6yekFf8A7Xf009SalRw+XtOXhGyX/s22/Ium7eNwxQNGLX4ji1+YYnj5cPCsTGVa+Id6sr8lsl4L8ZqYedKnG1GOVPfm/F/iLNgtsAG3I1nSgydSJ7C4nhrTEPZXPafu+uLwxxKL9fAtyRxeEasp65dWHxHOreHqZXZ7MpYmldZkYoavmeO+1qTMMsN6YODoAk92os+LgF/9op049y7n5LUVd2py8CbD362NuZq0+x4pyDKGcDgGd2UHqFJsKxszWxvXvuAYRINYbofu5mKHzU3A8xTW29yanWcVlauu/wBmRmP2nDJdJ4h8Vup8eY9RT454vNB6925PCth5rJU/+tV5/wCii727NgRc8DixIGW9/TmDrw4WvwrZwmPr1X1VTz4/neZPSnReHo0+vpO2uqvdfL7Gq7PZXiUsc2gsoNhwGmnGsmSs3ckjqrokIu0LrmmSNV/2YTNYche4t6GjxYmy0JHaGOhETJNOArLlysFUnMCNDmFj41NTbesdba7XIpQX83MAxmGiV2SI5grMocDusASAwPQ8fjXeQySinGNn4HJSzRk1J3Dw0bjgPhxBNWqcWkRTcZaEgDbuuuU9GBHx1qeLUloVp05R2NL3mwqQYLZuJw+Gj7TNATljF5GaINZrC73K8Dqb1iYWcp161KpJ2s+O2po1Uo0qc4pX04dxXt9TNjMYlsHJDI8caiEr3i3eFxoNPEgcDWhgFChh3eakk3qVsQ5VKiWWz5HTH7gY/DQtM0aMFUsyK5MgAFzplymw6E+F6bT6Yw0p5Ffy09Qn0fVte6KlioskUWLDZH7VJFiOtoVYfWG2tiwI8QOd6odJ4zPLJFaLfx5FzC0Orjq9T0PupMk2GRlN1ZbjmLHivwP961g1PiNCL0KZvYThHxGImXOYWw/0RCT2SiQdkJGXXMQ0kgOnBdLE3pqbb1JcyjDs7u9/DTQG8my8mBiM8Mc8iMM/1MJVkIdpVjUAGPLe4I/3a3Iuat4WEZztLjt48CvVk0rmULkkxbpgsNItu9lBzExrbM3Zk6jW4AObXXNrSV6WWbg1ZhSqaZou6JbA45WuVcNlNmtfh94A2PyrPrUXF5WaFKqpK6LNu/tfO2QnUcPKqkqdtS1Cdy54CUE68Dp4Uyw9q6MQ9oO7n6PxbIo+qkHaReCk6p+6dPIrWjSqZ495k1aeWXcVvNUtyIK9KAYNAFx9nOzWeVpyO6gKr4uw1t5L/wA1VMXO0cpdwVO8s3I0RjPwVFt1Ln8Av51muJqJnOaCUjvKp/ZJJ+YFMaY8qW8ErYfUggHmQR/ZqzQjmdipiJZFcp67BxuKkLrhnu3uhrJpytnI8fnW1RyQ47asxqsZye1r7Gn4WRsNEqsLlVVSVBJzBQOPIacaxKsrzbXNmzSeWKTJf2e4IYmaVpSXC5Qq3IFzmJvY6gC2nDU0+hTjN6ogxE5RjdMkfbBsyMbNLpEg7KWN7AADvnsjw/bHpXRdESVPEWSWqa9/YxsWnOm7sw5ca/2VUfCun62b0SRkOhDi2zXNzoJE2b2+DjSTFNe5awJYPZkJuLWXgtwDoedc9jKjni8mIbUFy8NzTw9OMaN6S1GO9O2cZJhDFj9m637uIsQI2uLEEBgG5e8L3taruDw2HVZSoVf/AM8/T00K9etWyNVIfMkdpy22HgpePYyQNp0jZ46ipRtj6sP8lL66j5tSw8JPg0WPEwp+m4mNr/Q2t5iRhf0ciqcJP9BKP/den8EzjfEp/wDX3Mx2lvLj8Ni8YYmaR3aaNkYPIAoci6oDplAsOgrbeFw88NTzK1knfRcOfeU6dap10l4kDvliYA/ZRI2YHCxsxtkEcaXVFF/1h86wZQm455PRtmjmV7IuXsA25KVmwzG8ceRlPNc+YZR4d2oJxTinxHxuaHvzsf6ZCixsC8c0EpTS7xxyK7pbyF/hbnUKWo8Z4yRpZFhVWZlF7KQAmYHvSHXIoCniLm4sDraRyyvvHxhdXei5/m77vOy1K3hNyIzizisOwkXJIjDKRCpZe6YpmsHs33RYXIvpapamL61RzLVaX5rv7yJYbq22tnwe/lw/LFJ3y3bbASduWWIudYyQQWOpAHFhx4aDrVp/p60P7rt3r3Ib1KTvBX7g9iMXkVolzHKMyp3iuumg1t42rKq4Oavlakuaa9NzQpYmLte6+RoWAlYaMrKdDZgVOvgao1KUofEi9CpGWzIL2y4LtcHFOBrFIFY9ElGU/wCIJTsPLt25lbEx7NzHMtXSkcb0ogd6ANY3SAXCwKul0DnzfvN8zWVXk3UZs4ZJUolswzCoUycdDXnThoghAddfnwouhNRru28ZXtWtmZVb951DMfwA8FAq/ipKlh4QX7rt/LReXqZuGvVxE5v9tkvV+foQu0ccqCQAi+Zl5HmSPlY/GqmIj201tJJ+f83RNSqdmz3Ta8vurP5kr7OtpRxuiFgDKzqP1mCFz8kP9mn4anPM2lolr3ch2IceqXO5e97MJ2+BxMYFy0MmX9oKSvzArVws8laEuTRlVY5otHmGREJ4lTXYTir8jGjKSXMvW5u7eIkg7bA7Tyzfag7yAWJADsGNwRqDltrasrFYmFOeStTvHg9/L/Zco088c0JWfI0HZmJnwmCmO15o2BDBV7pLKVsY9FGck8Br59M+UadavH9JFr78+Niws0IPrXcqwx0R3e7HtozKr6JmXOf9Jzmy3vwYnyrX6qf/AJPPZ5bb8PhtuUesh+lyt27vmdt7t8MPFtHC4mCRZeziKuFJtZi2ZL9bG/gQKhwmAnLDTp1Fa70uSVsRapGUNVxG+8W8my1E+JwyucTPGyEEOAhcDMxv3QdATYm58zTY4XF2jTq/BF34f78xeuoXcofEzNd4tsCZYbQrGyKvaMLEyuFsrsQAdAOBva5qCvQdOLbd9dO6+pLCrnaLv7DogI8TJzZ0S/8A5a5v89UJfDcsxJ/dT2nRFlw+MQKkhzRYhbgXbX6wfZYX1cG3E2AF6jdJptcQz8yxb04YYNMRixJoo+kNEQTFM4Ts1dtbAarcWtcBvKNakqlZErsXBTzYPD9piXDhFLlQgzG3eBIFx0BQrwFGwKVnqrjLeTYezJIxBiAi2vkUnOxYgmyD3w3Pu2PTjT1O24Zc22pF7lblwYS8kMLtmHdlmVDcXJ/1UgV4+PW550jkt4sk0h2ZJfJu/ug9/to4uNeyw+FikmtdJFkVXT71oWN72tzK2OvQtVbI7SCUYuKcL37+Hg/4RS939mba2izJK6iEd2RJTHlPAjLGos9rcSCNeo0bam3dLyEUpW7T+WpYf/p/humF/wCCn/xoyd7+ounIwXszTyAPszQBoe7jyQ4SFh3gQ/7tpGAHpasrEq9Rmph21TRNQ7WY8qrWLKmOjte3FqTUVyQyxW3uAQ3J+VKoviMdRcCBxuLxOHN0N1P2RxUcgBzA5W8q0Y1adekqVXdbMy50qlGs6tL926+xEbR2nmGds+c6AHukgc2HG3wq3g8JKXYbTivzTkRVqyvns1J+H1H26W2iuLw7NYZJUta4GViFfiTbQmujhRpLC1KMUldN+LWxludR1ozbb4HpiE3GtcyjUZ5p2jhlWaaA2Jilkj1GvccqD11Av8a7zDVYYikpcbI5qvCVCo7bEXJB2ZuuZSOBU2onRSJKdVyDTFuTdnzn9a9/WmwdtELUhfV3HeUWvlZfFdRVlbFW7va6ficJe90bxGh+IpsiWPZ7jhiQcumo5ioqusSSm1m1InaZ7oPVvw0rFx7/ALd+bL+GXbt3Glbkz/RdlSS8+znk8z3gn+Ws7LdJFxMo+2IAuCgYcbAg/EfzqGu31jYsdUab7It4Wx0EmBxVpI1i7ubiFYlHjPVCG06ajpZK6SUZrjv4/wAhSbu4vgaJu9OmGRcMNFiCxr1yqAF+VqTLmV0PK2MVh8KmP2m698YqREy6kmM9gliQW7xaxHDXhoKh3dmTO0YK3Fa+b0+lywbmR4nsL4qZnmlJlfhaIEACNBwAGnzpSI6S7FwMU6/VfWy5nZy8hkYRhRfOWzXuy634Aik7iS8nFy5e/wDoVPurg5Tm7wYcGDEOPJuNNdKD4DVUkuJz/wCyCf8A7E3/ABG/nUf6ePN+Y/rpdx5u+g+FT3IQHAnpRcCc2NtJ4YjEwutyV8L6keuvxqliaLk8yLmHr5VlZyl2kSe6bVWUCV1eRzLE+9J6UtuSEvfdnaPGRp7q68LniaMjYdYlsRm09rlTrcuRoDwHS/hV/DYTNq9irVr28SGRmYlybm+t63aCyLMtkZlSV3Zj58OxsyaHiCORrUnSU1miVY1VF2Z6q2Diu1gik+/Gj/xKD+dck4uMnF8NDZburow32vbGaHaMkqDL2oSVT9lu6FcHxzKT8RXSdGrPh06btKOnjxMzFO07TV4srOD2gsoySDK44g/lWxQxManYnpLkZlXDyp9qGqOGNwuQ3BuKSrSy6olpVc+jDws9xan0Z5lYSpCzudHa/HXz4+tPauNS5HBptDe+nx/rVeTtFkihqRO01AVD1JrGx0exDxL2HfakaDvCv0bZCxX1bsI/Mizt/wAhqpDWZaexS9uzkYeCE+9lDEcwD3hf4FaqVdZuw6Og+9n22/oGLjmN8mqSWvfs34kW5ggN+7VjqHUpZVvuRdZlndm2bwoyyQzQurK9he9g6sM0ZU9bBvPSqdJ2bRZlzKzvDKDsG4NjPjHKnge9jXkuPhHf4VDHd+LJ62jilyj9Vf3L7ufjc0AZ2BayroLABQLAD1p6ViE5bdn/ANKwsn2bTxE8gXVHH/tGmvcli/7co96fr9x7DNfg1KQnftn60gGJfo7wptx9g/0b4UXCwP0b4UXCwn9Dpe+UXpuSPIW7D/Q6fdHpSZI8guxabKVeCgUqSWwO7KtvdhAsyaa5Nf4jb861MJBOCfe/YpV5NTt3fcZRQ5VsRoa2I0ssWraMoSnmfgKwblTlPDlS4eTg8kthKqUlmRuWwt9sLh8BA0shLBRCI10JaJVDFidFFrHU8xa9c1jqbpV5KXO68Ga9CanSTRX9+t4cJtFcOQjo15l7+mgKag81J1B861+gJNupy089TP6UTSi13lE2nsYEXAsRwYVvVaEamvHmZlLEyg7PYa4SRW+rluG5HkaKVa/YqbklSLXbp7CMTs4xHMrG3PwpJ0XTlmjsOp4hVFlktTuICQCGFjVhO6uiLrEtGhrjICvTXSoasfqTUppjSDAPM0aqhYZ1VrC+UOwUE9BWPjGkoX7y/RV2zSvaNHEqw9qbRK7SMNLuVAVIwOebM1/AHhpWVGo0nbd6FySXEyjHTPPK0rD3ibDoOQpaVCW7I5VFwOmHjIIrSpU2rFWctDUd1MfI+y8Qly7YRlmiHNVa9lH6oKuT0BPWqHSNLqqiqLin5ot4Juranxul5jr2o4UQYPAYGI37ON52J+7BCVJPixlb51mbRL8XGdZcrry29CubtY7EqpVcTIigciG16d8H0qq6kuZ1U+jMNlTyavxLVscz4yWLDyYl3RmDOhWLWNO82ay3W5suhv3vR9OcnK1zOx2Do0aUpqPct93+N/I0jEbHgIuhaI/qnTT9U3AHlarRzpGfRv8A+wfwD/5U0CidnTSUPs6AD7OgQHZ0Cg7OgAZKBClb9R2miPIrl9GP862Oj9adv+3sUcUtb9wyeK628B+ddC6d42MZSs7jNUvccx8xVZQvpxRYbtrwZObv7wYjCXEbCzWuGVWFxwNiNDTKuDo4i3WrVcRYYipRvkEbXxk2KftJXzNawNgoA6ADQCrFHCU6MctNWIZ4mVR3mwYPaTR91xdasKTXxEMoJ6x8jvisDHMMya/iKfKMZrUjhOVN6DaElRlbvLyPTwNLC8dHqglaXajozmq5Gy/ZOq/mKIrK7cB7edZuPERilUjU/OllsLTck9DtudE5xidm1lDZZB1V9VBB5XXj4Vg49RbS5XNfD5ra8bD32s4gPjVjGvZRKCOjuS5+RSqeFppxzMmry1sVFI9L1oxp6FVy1FxcalpobLY0L2Y4xIDijKQsRw4DMxCqGeVUjBJsBfMfSqXS6Spx8SbBN5myH392rLi8Y8iBjAgGGVwDkYRNdrNzvJc/Belc9VvlOi6LpxlWTl8jns9wqeZ/CqMnqdo4p2ND9ksGZ5pTrYLGOut2b8E9KsYdbs5z+oKlslNd79l7lw3ukMUDMpILd0crXuSb9bA28bU/E1erpuRz1OOaVjJvp8H3l/4a1F/4vFh+qo8yWvVgUO9AB3oAF6BQUCB0AVD2hQ3SJhxBf/Ka1ejbtTS7mVcTZONyBixKuqsdLj5jiK6ahUU4KRjypOMmkN8UpU5lNRV4OLzxJabusrFwyLINGsel6WnKNVdl6jZxcHqtDqmKymzH8aeqii7SGOlm1iOUkRuf41OnGSIXGUeBxZGQ3QkeV6jlBx1iSKSnpITJjSfeGvUUjrc0OVFLYQXZuCnTW/CkdRtaIcoqO7Fube96f1pZ1LbjFrsdt2dpJh9oRFjaN8qseQ79wfUfOufx9RKrfmjSwqbhrzHW8eHZ8ZiJJR3jM+g4AAkKL8xlA151o4PDwdKMu4q4ivLrHEicS3IVZnyQ2muLBgYWkdVRSzMQoUC5JOgAHM0xSUVmlsPab0RP77TLhYYtnRvmlLrPiWQ8HA+rjH7IN+XAHTNXM4zFPE1XLhsvA0aNJUoZePE1fcbYaQwRxkDRQD0JOrH4kk/GmrREhIbwbi4CRLqvYPcWZBcFmNgDHwIJPK3Gqs6UZamphOlcRRdr5lyfs+B03N2H9AiMcls7SMzEXtb3Utfh3VBt1JopwyKxF0hjP1VXOtFZJX/OdyT3nw3aw5F0JWTXpaJ7H+LLTKqUnFPa5Ug2k7FS/QGB/wB0voKv/qavMj6iHIroqkShigA6ADoFFAUAC1IBX98ICyRkC9ma/kQP5Vt9C6zl4IzukGlGNyiCMwuyEd094A3Fx4eI/KteEepqNLZ6/fyKzl1kFJbj5cM2UHip4HmPBhyNX4rMis6iv3/mxxl2Q98yAg/L51WqYPXNB2ZJHFxtaQuJrnJMAp68QfSnxnmWSstRslbt0nc6tsxl1U5hyt/etL+ncdYajFiYy0krHbDYhAcsi2PIsT/0p0atnlloR1Kcms0BOImUHRfQXHrSVJZeAsISa38zkj310t46n0GnzpkddR7VtBtiJMw016/lVes21dE1ONnqRmJTOVuwXW2bkt7am2tYeLWaz5F+g8rsaJs3ZX0qAR4huwxaLkWRrmHEogtHmcaB8tluDew1B5Jg+kXQ7EtY/VeH2HV8KqmuzK/itgY1HCHCSknhlQyKfJ0uhHxrY/WUWsykrFVUJli2JgxgLvdHxpVrKGBTDKR37nUNKRppcC9tb64eNxrr9iHw+v8ABcpUlDV7mafSH7UuWJfMWLE3Ja9ySTxN6pkx6A3C3wgnCoWCy2F0OhJ5lQfeXxF6fnvoLbiXHZjvipzKT9RCWSMf7ybVZJD+qoug8c56VHq2WJZIUlFfE9X3Lgvnu/l3k7JGGFmFOKwzxceVQDqLlb8DZh8zpUVXa46HIyT9DYr77/wn+dLdcyx1z5HXs6bciD7Oi4WDyUXAPJQAYSgBQSgLEZvBKERLi92tpx90j8xW10HFutJ93ujN6Ut1cb8/ZlRx8STLa9nQ3UkWuDy0vXTOnm0Zj0Zun4MYRQzRmynLfQgkkN534fClVGcXeL9yaVSnNXeo7Er8AcrfdbvA+R5/jUyd9HoyDLDd6rmvz+BnjJyRaVAv6y3YfHmKhqXStUXzWpPSppO9N37mcMPKRos1x05elRU3b4ZXJZxT+KNjq7odHX48R/SpJShJWqIjiprWDOkfCwOYcj08DToWtZO6Gy3u1ZjbFM/Dl0AqtXVReHcS01DfiM1kINrfyFZ3WOLs0WHFNXEY0ANYcLVTxCWbQdSu1dmrbrMHwkJOvcCnncp3D+FYlXSTRrU9Ypj0bLh1spAPEB3Cn90G3yqKXa3HZUMJN0cC3/44+DOPwNPjUnHaT87+o104vdDTF7jYJxpGyH7yu1/8VxTnWk9xFSithMeyJ8GiCG0yIWNsiCcXNxZ9C1tSLEHgOFCqMHA0fczeFZYwqtfLcFft34tYWFyNbiwI6cCXqak7bMY4ta7lyw2IVxcG9KIRe8W2IoI3d9VjUyHgRdfdXqCSagrTS0/O4fBcTGP+2ydJ/wD0v50v6aX+aF/UU/8ACRZ7UDgWoAFqQUK1KIGBQAoUCld319yP9pvwFbvQXxz8EZnSfwx8SvP748q6r9xz6+FnCaQjnTm2iSEUznMgNgdac4qS1HwbWqO8KC3Dn50QIpydyO2lhkCswUBhzGn/AFqDE0oKLmlqW8PUm2ot6EA/GsKejNNbCO1YcCRUTqSjsx2VPdD/AGbiXa4Zr1fwWIqTbUmVsRShHVIkcQLJ8L1PifhKkNZkQdTWBU1ZfWiNW3G/7lH5v/zmsrE/8jNHD/8AGieqAnDoEYKBBLUopHY2NUZZFADllQt95eIDcjYgEE8OVMn8IkfiLpu1iXYSFmJIkkW/MhUjIueJN2Op18dBUtFtx17/AFGVElLQqu1cdJKEztfM82bRRmyPKqZrDWwAAv8AnWZOblW17/W3oW6CRztUpbP/2Q==</t>
         </is>
       </c>
     </row>
@@ -2790,25 +2790,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SHIMRON HETMYER</t>
+          <t>SURYAKUMAR YADAV</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>psl2021_16</t>
+          <t>smat2021_095</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>77.8</v>
+        <v>146.7</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2817,13 +2817,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>33.3</v>
+        <v>26.7</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -2859,7 +2859,7 @@
         <v>20</v>
       </c>
       <c r="X19" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Y19" t="n">
         <v>0</v>
@@ -2874,13 +2874,13 @@
         <v>16</v>
       </c>
       <c r="AC19" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD19" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AF19" t="n">
         <v>0</v>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="AM19" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFRgSEhUZGRgYGBgYHBgaGBgYHBwcHBgZGhwcGhocIS4lHB4rHxkZJjgmKy8xNTU1GiQ7QDszPy40NTEBDAwMEA8QHxISHDQsJCs3MTQ0NDY0NDY0NTQ0MTQxNDQ0MTQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ9NDQ0NDE0NDQ0Nf/AABEIARMAtwMBIgACEQEDEQH/xAAcAAABBAMBAAAAAAAAAAAAAAAAAQQFBgIDBwj/xABFEAACAQIEAwUEBggEBAcAAAABAgADEQQSITEFQVEGImFxkRMygaEHQlKxwdEUFSNigqLh8DNykvEkQ7PCNGRzg7LS4v/EABoBAAMBAQEBAAAAAAAAAAAAAAABAgMEBQb/xAAoEQACAgICAQMEAgMAAAAAAAAAAQIRAyESMUEEUXETIjJhgfEFQrH/2gAMAwEAAhEDEQA/AOwQhCWQEIQgAQhCABCEIAEIQgAQhCABEixIAESEIAEIXheABCEIAEURIQAIRYQAWEIQAIQhAAhCEACEIQAwrVAql22AuZXsZ2pRSRTAPiSelybdBcayE7Z9qUSt+ihj3QA1jYZ2sbE+AI9ZS8bx/ZUINgRcIWNzexvpre33zGUndI0jFVbLnU7csDoARdQtlNmJJ0udrgb7fOS2A7Vlv8RLC9rrdtMt76adNjOPVMcxQU8/d7+a6sQTY2Y67k2PLy0jyjxzKPfOgCi1l7oIvYW0Ol9ecm34ZXFHe6FZXUOhup2Imc5/9HnaMVG/RnYklCyjQC6++Pnf1nQDNou0ZSVMSBMDMTKELCJCAhYt5jFgAsIkW8ACEIQAyhCEBhCEyiAIQhAAmuq4VSzbKCx8gLmbIy4upOHrKu5pVAPMo1oAcAZzWrvXfUu7Pr1Yk/jH+GohjoI3p0wqA33AOsk+GAEd1l8iQD6GYyts6oJJbNGJw+m0i61JSbEC0steldbjxkBjlsbkgSY9lSSo0cLrnC4qnWTZHRj/AJb2Yf6S09FmeccQmZDbU2sAOd9Bb1noukllUHcAD0E3icsjVUxSKcrNY+RiDEIdmH3SE4ji0TPVqGyhtTqfrBRt8Ji2PpDQuo72TU271gSNd/eHrIc6Y1CywK4OxB8jeZSEVhcgEXFiRfUA7afAyQwBJBuSdZUZWTKNDuLMYsskWLMYQAzvCIIQAzhMoRDCEIWgAlotoQgASodusXWT2HsXdbsxJU2uVAsD1FiTY6GW+V/tpgzUwxZTZqbBwfCxDfI3+EiV1ovG0mrOTY1rX7gNuWwv5ch4RlikYvcoi2C2Iv372uF5gjnccucmQutzuRr+M1V6V97Dppb18Jjy3s6krSG+MxJWkCCbyKqYa2U5VfOhfMWOlr90jk3h4iS2MpqUVhVQhtiCLX2t0MjqSXFiNiR6fhBOkElbM8BiPZkVERboVcBtVzBgRcDcAgTsPYridSvglrVyWfNVBYgDNkdgDYADYAfCcdencFVGrZVA8SwE7fhMEMNhEoDdEVD4sdXPxJY/GapswmkReMwXtUFNj3cyO3PNlYNlI6G0Y/qAqCqVBZkdHzJmOV2v3ddGA0v4DpJ1RBzJaTFbRGcOwrpUqPUC2cIFKsTYIuUAggHW5N/GWPBr3PO5kZJeitlA8BLgiJOzKEWJNCAhEhADKEIQA3wtCEQwhCEQBCEIAEwq0wwKsAVIIIOoIOhBmcIAcy7acMXD1ENNcqMmgFyMwJvv5j1lXqYoHusRfxNp1Ptxhg+FZiNUKtfmATlPw1v8JyhaYvZgD+MylGnZ1YpWqNGJprYWZbjY8x1mlatrL/UR7iUTL/hAcr6X+6QmIYIe7pEki50ui39hcBRxGJyVxmAUuozFe8rKRex1Fr6TqvFX7qjqb+n+882VsQxDEE7cvhOo/RnTYYQszEhqhygkkABVvYcu9eX1Ewat2XAPra/K/wDT0uf9pkx1M1V01XxNj5b/AJeszkrsTM0FyB4iTEi8KLuvr6ayVmsTNiQixJQhDACLCAgEIQgBvhCEkYQhCABCEIAEWJInj/HaWEp56huT7qAjMx8Og6nYfKBSV9ER9IfF/Y4f2S+/Wuvkg1Y/HRf4j0nIq1VshanuNbdY/wC1HFK+Jf21UBTlsqjSyXv7p73P3jvIrC1bajXqPxHj4SZK1aOqGKo/sYVOLVDy+Rjdmd95ZCiOLgXBjf8ARVXlMua9hfTflkPVpHLl62HrO09jMPkwVAD6yF/9bFh8mE5LiqZtmA2vYdTY2HrO5YDDCnTSmNkREH8KgfhKu0TJcTew0M0ze+01WgjNjnAL3yeg++SE552l7UPhMRTWmRYqWdSLqwJFgbajZrESwcG7Y4auAHPsmJsA5BQn92oNL+BsfCaxaJcH2WOEWJKIEhFiQAWEIQA3QhFkgJCEIyggTAzlfa7teajOlJ/2S90KLj2h5s7D6nRRvziZUYOT0T3antstIGnhmUtqDVIzKvUIP+Y/8o5mcvx/GHdi+YlzqXY5nPTvH3PALa3jGeIrFjmc38fAa2AGgHgI3pC/eO51iq+zrhjUTaKhzZiSSdydSb7kn5zJqWXv58o3N+UxRLxHoAkEjwlGtew74TSarWVKbhc5yktorG19t9gbdY8ek/tTQIzsSVXKL3ZTYgdRtaRC0iug16eXQiS/DsZiMOhq0aaE3Cl3uwTMLhFAINyLEnoQOsxyxdNqr8fJD0TbcCyDChyC9TFKpA2CpmLJfn7pN/3Z0ucv4Tx+vXrpVrXcUM9QUaaKvfKlARfX/mHVmsNTHfFe0+LQe19pSQh1IoAZ0KAMGRqm7ucym62AyDWGHDk478dnLlnxklI6LW2moCVI9uldFK0GzlQSC4Cg9ARqfQSz4bEhhroQLkffaVxaMY5IybSfRyLt1ic+PqAfUCJ6C/3sZF0nZb2JFxY2O46HqJjia/tMTVqH6zufhmNvlabKi/PQ/HSaJaO3HH7bOkfRr2kuP0Os+u9IsfVLn1A8x0E6NPNtOqVIYEgg3BGhBHMHlO49iuO/peHDMf2lOyP4m2jfxD5gxmGaFfciwQiwgYCQiwgBthCERQQhFAgBWO3fFvYYcops9W6DqF+s3pp/EJxvEC4lo7dcUNbFOoPdp/s181PePxa/oJV33HQ/1H4/KB34Y8Y/I0qLcW8h6nX5AwYcpurqFy9SzN/Kfzj7gKKKhqOobIjuqnUFlQkX8t/hGX7s2JwR8thbOE9oyEqrBbBibE30Bvt6xjXpMjFHUqymxBFiD4iWp8YXwz4gsSVXIwuTZnpNQNul9H/jMgeI1S5Qv74pqHJ3JDNlv1OQp6W5QaFGTfYyA1AG7H0mOXNnKsRd2YWOltl0/wAoUREezqf3g3wU3++0f4bH5aAw2RLZg2e3f2tb+vSRK/Csrtm3gjPkqNTUFzkpEm4AViz3sNW1RRbxlm4P2SqVFao9yxGjNYE+CjZR4D1idjqdFEetXIVEZmZjsdERfM3LDTqZaafazDu6Jh61MlsqqjJVDFibACy2A2+c6o5OEUl32eVnjyyu+ujm+MwzYV++hyA3Kc1tvl/d69L322sWB45npVKl8wWlUdXAtsp7rj6rgsNOe/iZniy08SWo1DQFQEg5K6sRYHRlYKwJ20va/Sc/xvDXwVHFg3yutOkoufruS1xzsqmx8fVylFxbS77/AE/cyhj4y1/ZVcB4+Xn/AHrHb1LjyFvQiNcPoJi9TWcx6idRocFpa/o843+j4pFc2St+yboGJBRv9WnkxlNJ+S3P3zMe7fxjJl9yo9OmJILsVxn9KwiVGN3XuP8A51A738Qs38UnoHG1ToSEW0ICNkWJFEllC2jfG4gU6b1G2RWY+Sgn8I4lX+kLE5MGyg2LsqfC+Y/JSPjAcVckjj1aqWZmY6kkn4nWNalbTxBv8D/ZmT3DeYv5jmI0r33Go5dbdP76Sj0W6N1KoGNzyFvu/wD16yR4ejEhlbKR3r3At03PTT/eQKVNMvj8rG0l8PVEAi7LDRRghCvlQ5iQuVVbkSxGW42FrkAHQSGx1Re8iqPePfzZrm+4IAvfxvvMmOYDXQfL+7ww+Eeo4WmhcgFiAL2A3J5CKUklbKpLZHJ7/kVUfDU/P7o+XLfl5x0nZ90oriKjogK51W+ZmzbCw0F83XltHWD4Uj4Za5ZsxrLTKi1spIudr31mX1oVd+a/klSVDrHUG/QKNJBd61YAC4F8oqPudN3X5Rt2e4RXoYhK9ekyJSWpULHKV7qMQLgn61o8+kCmKaYWiL5USoQTz1VBrtfKg9ZS2Rnsi7sVQebMAJvdnmSlbbfuxnXVz36ikZzmuQQDmN7gnfeWXtJWYcNwNNzdmLvfnkQuEHwVwIdp+K16VerhqVVhSQLRCaMtkpqjWVgQNQdRNnbjCm+FoAhVo4VMzMbKpew1PUmnFJqKthDciml7CJQszXOw1MwJ5biFFeXK/wAorOi9odk9253c38gP7Ed4fCvUCU6YuzE2G3iSSdgBreNDqfLQfjJTDYo0WpVB9U3I6g6MPiCRBG1aZ0n6PsA+EYozlxVy5rA5B3WKMpIBJuCp/wA6HSdDnnviPHKtVlbMUVDdFVjcahszH6zXANz0FhO59nuJjE4eniBbvoMwHJx3XHwYEQbXg5ckWtskYRYRmRsixBFklBKl26w5q0xTVAzBWe7PlVBb3so7zNYNYWt7xO0t05J2/wAY36acjFTTRUuCQQSC+hGo0e0EaYk3LRVeKYQ02FO92UA3tYXt3lH2gGDKT1UiRtbTvD3TuOhklxPHVapVqhByjJcKo0uWvoNTckxi6215HcdDKO1XWyPqJZgRt+ck+F0VqPlL5bEEgAlsn1mXkcu5G9rnlI90LMEW13ZUHmzBR8NZuOGejVdD3KlN2QkHZkYqSD0uLyJ3WmZ3UqRd8FhKdFsL7amrF3qU3LHOhOhpOoOliBb+I9IjMwqYiniKiUDXVAj0yRbI1lS1+7mW2lxv8JFcY4wleh7O+WslQWC3ynLdcykaAZfmI2xvGGrYgvTRFyhLuVDNnVMpK8rnfnsJ58cWWVuX7/6UlJjzDEphsSj+/wDpCoPAKpOn+j5yX7PU8+CC/wDm0+AvTJPpKxUqMVYEm1726sdyepkx2Sps1UAE2VXa1za+XKDbrdlnV9Btd+bLnGot/wAkl2t7Q1xVFGm4VERLjIrEs6BjfMDyI0mGG4tUTCtXqJTqVDWRKZakgCkIXLjIqk6Ec+fq3xtSm+Krl6Yf9qyqc7oQEOS1lNj7o3jqvTSpkpZSlNEqVmytnY6W52H1FHxnYkfO5PUVPinsjOH1KNfEocThlJeoMz03dLsx3ZCxDakXAtNHbB3fGYokA0UVENzzVFcAW1vdzaTPBsLTOJpezZm7xY5kCkZAW5MQduU592gxLPicQ9yVes5tfTRiBp5ATPLHkqOr0UpTTbI34S3YDgbV+EviEW7YbE1DoNWpNTol79crWbyVpVF1nd/osww/ViBgCKjViR1Bdk18wsR1y1s4rhqY3JsPnM8S9zcctvD+/jJrtT2e/QsQ1G5yEZ6bHU5Dyv1BuPhIdkB2Bb7vyickbKVxN/BERqqe1BZMwzi5F1vqLjXaeisHQREVKSqqADKqgBQOVgJ5wpFlYG1p3jsXjPa4OmxNyoKH+E6fK0adnPkbbJyEWEZkbIQixFBKn2l7I0K4euMy1MpbMpuGKrpmU6cgNLS2TRjf8N/8jfcYDi3F2jz49ztv6/1gBpYqNv70E3Ws5HjMq9YWtIc2n0dsZWrG3BcIKuOw1GxAashPkhzn5KZM/SDwdqGMqVMtkrMaim+5IXOPA5yT8RNv0ZUg/Ela3uUqj/8AxT/vMnvpfIzYVeZ9tt0/Zyk7MlK8hzFO4pc78vOPsAmVQDvuT4neNioZ0TkDc/CSgQW2jOpSUWa3Hd82lu7DUlzsSQD+zAFwCRnDtYHf3Bt1lYSnmKqASdTYXPym9aLErlVrt7uh18V9N/CBM5xlFxLoOxzq7OtcEFmPeRgdSdDoQdJsq8BqqtbKVd2REQA2OUMrPfNbpN2Dx2IREWo/eCi+in5kazMcVqg6P/Kv5SlJniy9JicnKtkZ2e4VWpu9R0IyI2UaXLHSy230v6zmK8BxbO1NqD+0ALshsGtvcAnvDXlfn0M643Eq1/fPPkvMjw8PnITjb1A6YsNmanpoNcpJve241I8mMbd7NMMfoxpHLChBKkWINiDoQb2IInd/orxQbhyC4/ZvVQ/By2vwYTm3afBI1T26i/tAGJGmpGjWHUfMTVgOIVKeHfCUyVpu5dwD711Vct9wO6L9ZDZ0OXJaLD9InHqOKdKVEBlpFv2n2ibAhP3dN+fLxqR0E2imBy+ZiMg6TNps0i1FDYG5nYfo30w7J0e/xI1+4TlVDDgnQffOidn6lShSCK2UscxFlPluOn3yoqjObtl/hKoeK1vt/wAq/lCWZ0W+LEixDCN8cham6jcowHmVIjiBgB56KXY9bmNcTh23Bli7U4QUcS6gWGc6eBNwfQyOKXF5hJ0zqglKI++jHHrh8TXqVrgLhajX3uEdGYDxsNpG9pO0LYyt7RhbSyqDcKu9vM7k841r02AbKSMysptzDKVI9CZHYMgZkca7jxmkZJovFFRlsdYFO9m66Dyl07I0kf2mamrtmphQyZ1N890LFGCBrDvaHTQyn02II5CTfCsOro7HMzqUARKiUyVObM5ZgbqtlFrfWllZfYtPCKmGR8Of2Qe4DNmUMKhSorhlC3KliBqctsuXnLDRKNkzhLKjZsoHdyuXO2wIFv4jKIvZ1CCRiUOVihGUXJVA/dGexJ2ANr9RLcMKmQsrlrFgNVa4UuAWIt9gevjaByTXky9qpsbKL5iRlB+othqPtXmLVEAJutypBFgO9kFuV75r7EATMYHOe6wVciNmJUgllBI3GxvymC8LUFQ1RQSTuByUeO/e+RjMzZirDNotgSASAgFmQ5e8hvYA62PPUSG7QBTQcqwUrchUI7wBYkG6hrWtzsdPKSFbA5wQtVT9U7aXVTqS2igOLnfTaYVuDIwqU6j5j3QLPkADAm5Nm0BAB3GuukYmVHhlTOnsja6Xtfml+8pv0+7ykTjsP7NyvLceR/u3wlo4bwegHu9diy1At0yAXJw4uASbqPbNc9FOgsbu8V2fo4k5kqMCFsfcOQlabJn1H227v7p101UqCNoomaO8DgnqnKi/Hl6y14XsWiOPa1gRkLWUWN8rG1zcWBA6E8pYqfDadMMtNTZSAAHS7DXv3ttoNPGTRbkQPC+DJSsT3n6nYeQkpCBjJCEIRgXyLEixAEIQgBQPpD4Ez/8AFUxfSzgcrWs3lYWPkJzqlUI0noK15zvth2KNziMIt9y1Ib+af/X06TOUbNcc+OmUZyDIzG4W/eXcR6KtjlIsY4pAN+PPTnM1o6L8kHhsQSwW2t9hqT5ddZcMT2YqI9CgXU1a+uTXuDclj4ANt9gyU7N8AGeliGQXLZqaGwsF3qObEkAkWGlzzGkkuzjLi8fWxZJtSstOx0s2dBccxlUnzadEdrZzZsztJELieweJS2Vqb3NhZip2J2YdAecZVExmDGSrQcJe+cLnUDnZ0Nh8Z1tjdwLe6MxPncAff6TJnFwD/ekdE/Ub01ZUsTgylhmUliFUANqTsNpm/ZuoQWqOlgL5QW5a6m2vw+cseKwaPY7MCCGG4I1B6Tmnb/iHE6GjOvsSbCrSQr5B7klD8bHrylaIinJ0PuN8RoYRcrVEvbREuT6AaSm4ntarm2VgL7WH4GVV3JJZiSTuSbk+ZM1lojZY0uyyVeP391SvK9gT68pZ/o4qe2epRBys1nBbnbcac9b+s5vTJ62nWfoe4ahFTElrupCAX0AYXJtzJ29ZLKcYqLLh+oH+0n835RP1A/2k/m/KWQxIGBXP1A/2k/m/KH6gf7SfzflLHAxibK3+oH+2n835QlkhALFEWJFiGLCEIAEIQiA499IhVsW6KqrlVbkCxZiuYsfHUD4Sr8NJZxTs12ZVtY377BDb/VLV9IVP/jX8VQ/yAfhILhOI9jWSsFuyNfKTYHQj4b3+AicUz0I4eWNOPdHQu2eKTD0sqaVKiZFtpkpKO9YctO7p18I2+jLCKKVSrfv5xTOuyqikAjxLMZSuLcXq4vEO7U29yyogZ8qC17WFzuxJtznVezeHp08LTVGHuZ2YaEs3fYm+o7xOh8p0y4qCS+WeVKElN8lVEkubMxAvay+drn/umS1gTY72mpXdNWXQ66a205j8pqVEd3Y8sqrY7ADNcdCS1v4RMyh045r/AEjbEojq1OooIYEMrC4IO/mJhVrFD3jp9rl/F08/umnGVVKEsSuhII0I03BlJBZwnthwlMNino0mundZb7qGF8pPOx59Lc5CAf79I/40z+3qio+dg7qXJ1bKSAfQDSMSBa15kzsj0bUFx4HnL79GfHFwtc06miV8q5r2CupbKT4HOR6Si4Zwe7y69JJUU1FtQdLb+EDTgpRo9KmJNdBbKo6KB6ATZA4giGLCMkSESEAM4CEIhoWLEhAYsQxZhUcAEk2AFyegG5gBx7t3UzY6p4ZB/Isruax3/OSPGMUK1Z6p0zMzDyJ0B+Fowenfbfwis9rFHjBIbnir0nSpTZkdTcPluRoRtzGtrS7cJ+kOg4y4lfZtaxq0wcp03ZDqPnKTi7EC41vNeGRTcEaWEpPRhlxKcqZ3TB8VR09orq6WJz0zmGm4I3U+EbNQa3tKbWc3JBN0NzfKbdL2uOnOcfwlR6De0w9R6bHfISL+Y2PxlpwXGMSlEsXDG1+8trdbZbCaR2eb6vGsFOT76LBS7U0HzU6jqjpcOjkAgje19GHiJzDtF2lrGtUTDV2FC9lWwI2F7EgkDNe1rRlxbO9Rnqe8xufP+x8pGMnhJm90jTDiUoKXuNihJuTqdZmlMDlNgSbFSQbxihaQkhhwf70jZBaOEbX8dojZLR6H4FifaYajU+1TQnzyi/zvH8qH0ccVWrhVog9+j3WH7rFirDw3Hw8pbzGjzppxk0ITEhCUQJCEIAZxYl4SQFigxIkCjKVX6RMY1PCWT69REP8AlNyR8ctvjLTKv9IVBWwTsxIKFXUjrfLY+BDEQLxfmr9zk5bY9bzMAdPT8o2GZe6wIPQi24vNgeFHuxaaMMSbjQnQ8xf+k0YV+9bum9+n4CbcQ+kZYlDluPMeBgYyiuXJEv7L90en9Zi+IrhSoKZehVl+YY/dI6nURkBsL89Boes1vWXQWHO+gjUmuiM2DFmS5q66NtUc3K3PiPxkdiHXkflNzOCfG0zdAwieyVjjGPGPSI1mI2Eypk8x6flM8uU2baOaSfEcoiYxtiUwOU2rpvFqILajX++YmClh+8Pn/WBpVFo7Ecb/AEbEqzG1N+43SxPdb+E2+F526eZq9XukjpeekeH39lTzG5yJc9TlFzGjg9UlyTHESESUcosIkIAZRRKrR4i5vmqN9W2qj6wB3HS5+E3fpzbe2bnrmQ7MLHQa6X030iHRZYStnGnX9s3O3eTwtcW8xpfaDY88qrWv9pb2y3Olt76DxiEWWQHbQXwbjq1Ma/8AqJv8LyS4TVZ6SsxuTm18mI+6Rnbaoq4OqX27nzdR9xMaq9lK7VdlBXCiqjLWIupOQ68zbTx+R0veVg7HY20uNj5SeFV0pqre6Ablr9NMp2PQDncWlaU6TbK4unFnb/j5Talz99GqvrNIcrowuscseszGTqJgzvashqj5T3D3Ty6TBH1kpXwiNsQJGVcOUO9xEYyTWx3h6iW53O5JHym825SMFG+wPmIozr1gNSdbRJNSDCaRSZDpNdLFHnHqVgd4ylxZqdyRrNQXpHLqTooJPQC/ymbcLrhS7UnVQpclhl7q2ubNa9rjaFEyaT2xeDYUVsRRots9RFbxUsL/ACvPRU4J2f4ewqYfEBr3qoQo3BWsiEnwAN/iJ3sxpNHn+pknJUJCESM5hbwiQgIMo6D0EMo6D0EWEBhlHQegi5R0HoIQiAyWVr6RP/AVfOn/ANRYQiZpi/NfJxWZiEIz2UMsZGDr5+phCSzDINfat1MzznrCEDFjvCub7yWGo11hCM6cP4jOsg6TCnvCEBy7LH2WP/FUv/c/6by3CkrZ1ZQQC67DZqdyCdzfKu/SLCb4/wATj9X+a+Cje3b9LproFp4hcqhVAW7rsAPAek9AmEJj5Mc/+vwJCEIznEhCEBH/2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEhIVFRUVFhUYFhUVFRUVFRUXFRUWFhYVFhUYHSggGBolHRgVITEhJSkrLi4uGB8zODMsNygtLisBCgoKDg0OGhAQGy0lHyUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIARMAtwMBEQACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAACAQMEBQYABwj/xABCEAABAwIEAggCBgkEAQUAAAABAAIRAyEEEjFBBVEGEyJhcYGRoQcyI0KxwdHwFDNSYnKCkqLhQ8LS8WMVJIOjsv/EABsBAQACAwEBAAAAAAAAAAAAAAABBAIDBQYH/8QAMhEAAgIBAwMDAwIFBQEBAAAAAAECAxEEITEFEkETIlEyYXEUkUKBobHRBiMzUuFiFf/aAAwDAQACEQMRAD8A3QCsEBQgChALCAUBAdCAWEB0IQdCA6EJFQHIDkB0IDoQHQgOhAJCAQhACgEhACQgEQBgIBYQBAIBQEAoCAWEAsIDoQg6EB0ISZ3pV0uw+BAFQl1RwltNvzETEk6NGuvJYSlgk89xXxSxbqmamyk2naGGXnvl0i9uSw72CZg/ivW6wdZh2dWZsxxzbbmynvBtOjXTPDY13VszsqRmyPAEgQLEEg66LNSyQaQBZAWEAhCAQhAIQgEIQAkIBCEABCgDgCkCgIAgEAoCAIBAdCAWEB0IQdCArukHFmYShUr1NGNmP2joGjvJIChvYk+ceKcUfiaz61Y9p5J7gNmjkALLS9yRum4RYGOcaqAI9+pzek/YgDwPEalGo2pTeQ5pBDh3bEckyD6B6FdJWcQw/WhuV7TlqM1DXAA2O4ggrdF5IZoVkBEBxCAEhAJCAEhAIQgBIUAOFIFhAEAgCAQCwgOhCBQEAsIBIQHmXxwxkUaFET26hceUMEed3BYWEnk1GiXENDC47QJK0t4Mopt4RocP0WrvsKbxAnQ5QO7v7lq9ZFj9NLyBxHo46iwuqAgnYi4HN0aLFWtsmVGEZquINpC3plZrB6d8C8UesxFLYtY8azIJab+i21kHsELYQJCASEAiAQhAIQgBIQAkIAwgFAQBAIBQEAUIQKgOhALCA4hAeYfHLDA0sM+Liq9s9xZMf2rXYZGL6M4SCHHuA9TB8brn3zzsi/podqzI9R4SSGALQlgtc7oXiTc1MsLbbyFnJvGxCS8nm/SXANLYa0DLoBACyom1LDNOorTWUXvwOwhFXFvIsG0m+ZLz+C6NZzWeuQtpAkIBCEAhCASEAkIASEAJUAIBSAkAQQCgIQEgOhAKgOhAdCA8x+L+LqOyYcsHVyx4ffNm7TXA8hDh7qvbZiXaWIVpw7vuYijgHWMTOnaLQIBsSNCTbzVRyWSwoPBouj7alCo0guAqWLTUL4gnU6TvadVhZI2VQYXSTrKtRx7ZyGA1tXJmuBbYmL+SVMWwZSVMK6JuA2xl0g228FLks4IUXg2XwiqlnW08kh7nOL5+XIGta2O/tK5VZ7u0qTqwu49LhWTQdCARAIQgBIQCEKACQgBIQBBSBQgCCEBAISKgFhALCEHIScgPO/iwxzWZoBa9rRPJ1N5d7h3sql0P9xMs1S/22im6J4mmW3jldUbU1IvUyTjkexPFKAxLc7iGCBMSADoZFgPFYqDM3ZFPcl0+J0XV6mV2Zp1taBuJs7y5J2NEqyL4IfSqtSDZZF+SmCzIwtaUTSfDel9GOxGWn2nc3Pdmjyv6q7pk+9yZT1EvYom1hXSmcgBIQCIBEAhCgAkIAUAQUgUBAKAgCQCgIAkByA5AcgInFcG2tRqUnAEPY4XAMEtIBE73UNbEngHCLtLHOyHQ9xFiCPzoqVkfcWa5LGMmm6M8HpvnrKwDwTA6qo4G3Zu02nS61ZyyyoPHGR3j3B6THAUq7S6YINKqwQO9xvZQ+SZQaXGCgxFA1KjKLTmLnMYI5uIaPtWyuG+StbPKwe9YbCspty02taOTQAPGyvpJcFVyb5HYUkHIBEAJCASEAigCFACQgFCkBIBUAoCAIIDkAhKASUB0oCs4vx/D4YgVqmUkSBlcTHOw7itsKZzTaRqndCDw2fP/AEkx1J2Mr1aE9TUqFzLFusFxg6S7Mqclu0zcn5RfcAxzSJ6xzHc2ug6KrKLTLsLMx5F4zj2tBdnL3Rq50m6mMMsidqS5D+HGNw7cT1+KcR1Y+i7JIc90guMch7nuV6imU37ShddGtZke5Uagc0OaZDgCDzBuFnJNPDJi01lDkKCREAiARAIUAJUARACQgFCkBIBQhAQQk5AISgBlAcmQdlNwASRq0RI8Rt5woyQ9lk8u6WUjialYOMXaW7wGiAPSfVdSKb0Oa+ef6nNsxDX9tnHH9P8A0w9DhQex1OLgmPVebla85PQKrbtKpnCcRmyM15Stvqo0+hLJLwPAKr3htQ6aiVjK5JbGcNO2y+w/DAKwptMQPI3v7KxoLrPVSj5NOvpr9JuX8J610KxhfTNIxLHOyyRLmm8AbkSV0tfHtt2XjJQ0Ms0Jt+cGiVLKLmBCpIEIQCIBEAhUAFAIgOUgVAEAgFQHFAASgEPPYXPcOZ5DvU4IbS3ZBrcYpCB1rBP7IfUJ5zkLR/cQt8NLZLdJ/wBirZrI8ZX9yvxHHsPlIDalaBOR2WjRv/42Xd/NKtV6K3PiP43f7lOerr+7/ov2MpjK2apngDOJgCGiDEAbDRWNHH01Kl+H/R7ka9+o4Xr+JJfzi8Mr3cMg5mbX8uS831LTehe14fB6Lpuo9elN8rn+QdXBNMPLYka8iFzmzo9qEpYbKCWC5sLKM+ScB0MEKZLj81xPjqvS9F02F60vwjzPWtRl+gv5l1wXGvpN7LWODy4lr2hwOQWvqN7hXbKlbdPP8KSz+5UVjq01bX8Tk/2wjR4bpJRIBNSoyQOzUb1zW9weCHx4ytM9Bb4Sf4eP6cGVetj5bX5Wf6lvRxjHWa5hPJjwT5tcA4eABVKUJR5TLsb4y4Y/KwNuTiEJBUAQoBCgBKA5SAgEAqA5AIUBUcQ45TpvdS1e1odlG8zDZ2NpPIHewW+rTyswytdqY17eTMP4hUxIcHmwALWizR5bnvMldiFEKMYW/wAnGsvnbyxkNyupyO78+nut2cp4NPGMj3VQaltrfb+fBR3fSTgrqtP6OY+Uz62P3HyK0WP09Spf9lj+a4L1a9bSSr8wfcvw+f25APEqdIZqj2sH7xAnu71hraKra+yb38GOgvsqsU4pteSXhnscAZBae00g9lzXAEFpXjJQcXh+D2udk1w1kltoF0O0a0ONpuphFSkk+PJlhqLl9tvyUtDFtr9pjg4E6j82XvKnBRSjxg+fW+p3Nz5Ze0KQ7IjSn7uk/eqFEm5Wy+Zf2R0Nau2umHxHP7sg4hkfnbRdSEso5jJOLolwYRuB76LRCWM5MmntgueFcaLHFlR0sBADj9WdnH9n7PCQqOo0qa7oc/Bf02qcH2y4NJg8S2qxtRvyuEjn4Fc2UXF4Z1YS7o5HCFiZCKAIUAJCA4KQKgFQHICNxHFto0n1XaMaXEbmBoO86eayjHueDGcu1OR5VhMa91V1apdzpcfNwt4AWXoa61GHajzc5ucnJlu8dUXnaNuRbP2p9SwZLkk8R2jx9SfwUVZzuRJbEmkQ4SNxHosJe1krcjYSmHZmHQ7X8Pz4rLUQU4rPGxlTZKuWYvH+MYwMu4XRpw9lNoO5IzO83Okn1UVpcCU21uM4DhfVuJpuJpvLnGk6wa7mx31BuddbXMHga3p0p6rEdk1yeo0HU669C/VeZJ4SEZgTWqtfXeTluymxxZTaRcS3Vx8fQaLq1aCuiPt5OHqep3XvfZfCJ/E8DRLZNJhNhJa2RyvCsVpSluUu9pYQ7wnDAMJaAASRYRcdy13WVxn2LnkzUJyipP8AA3jqUsuIIBty2K20Wd2GuGa7INbPkPAHMyD9UkehkeyWLtnt5IjwVOKdZ37xbbYyHTdWI+DBmk+HuNJZUoO+oQ5n8LpzDyIn+ZcjqFaU1JeTr9OtcoOD8GuXPOiCQoAhQAoDgpAqAVAcUBlfiHicuGyb1HCf4Wdon1DfVW9FDusyUtdPFWDB0DsdwR6id/BdxcHDLalXz03NOoptI8i8H7R6rBrEsmcSWHSyZmDl8gP8pxMl8Gm6OllIkAS8ta50k2DmPfAAItPVg+NlytW5We58eP3wdDTKMNlz5IXEqbA81GDLFQscNQSQTLZ2sVaolLtUJb7ZRouUfqj84IX1nMJsdFZ8JorP4AoOykg7wPNTLdZGEMEEb3utnKIyyXV7bWgayJ+9VpS9LMnwlkzUe9qKHsCHHMKNE1Gts5xJ1NrAW1mBeeS5lls5YnZPtzwjqR08IrEVkE02uaXNzATle11ywkmO1F5+2ys03SUvTlzyseSrqKFFd0Ss4ZXirUadL+oDQr9qTSkiktmQ6pkgd4HoAPvW1bGDLHoPVIxY5OZUb4mzx/8Akqh1COas/cvdOli3Hyj0VcY7YhUAQoASgOCkHIBUBxQHn/TmvnxLaWzaTo/ifc+wauv06GIuXycbqM8z7fgy4+VruUT/ACnKfZdDwc8cqYnI4Hk6D3teRI/PJRLgyiWGHqS20kPLiI5hxi3goeOWZYb2RpuEVi1zHPaA6CwZnltgPrti5ER6brnXqMsqL2LtLcd2hcZhnOIaAA0EnX6xtc77BbKLIx/JhbCXjgrozEbGI89lb8FXyJVdmeBpP2gW99kX0hhRmJte/rumcIkVjiyHgcpHeDIWF0FbFwflEwl2SUiZw3iDsOHAUzVpuJcC0nM1wbOU9nlANotM6riarTwvxC3aSO3Tdj3R3yQeIYkhleq5oa+oZDIuAHSTzGo8dVc0sfUth2bqK5/PBU1diVbT5bM4/Gw7PpJabW5kmB4D1XW8JHK+4/RJMTsP8n7lngwyWPRd+SvQcd3wf5mlo9yFU1kc0staOWLonpq8+ehEQAlACUBwUgUIDkBxQHmXSGsH4tzx+25v9Iyfa1eg0kcVI89q5ZtZWBg7beTp8nC/uCrBXIPEpa0O3bE/ymQfzzWM/pyZ184ZK4fUljWncCO4xZQ+Ex5L7DcVqOYWl7pbFhlAiCCLDlI8Fp9GtPOOTb602sNk79Lc9ocXOP7QLiR6eShVxi9kHOTXI3idQQbG/nyWyDzsYsHFNk5xpHf+eaQfhmLD6zR4AnR1vdQ1yiUHYOiBlcFHKJG2sPaZcaQQD5JLEsNhNrgp69T5gTqDMgzPf7/9rZLCjtsYJ7lA+rJa0DWBadje3msm90EtmXLhDY3NvM6wszWx3rMga/djmu82kFY2x7oNGVUsSTPWZXmGenTzgQqCQSgAKAUKQcgFQETimObQpPqv0Y0nxOwHeTA81lGLlJJGM5KMXJnlbXFzGvOpcXHlLiSftXpK12wSR5myXdJsKq2HB3MQfPT3A9VmYkPjL4pu8CFhN4izOtZmha7Oy0tFxE6+v52WqEtsMzkt8ljwjEB1QbyHZh4NMe8eqr6uc66ZSj4RZ0VcLL4Rlw2i/oOAcQAB2W+sv5+S4MuoXfpVYpb92D066Tp1rZVdvt7U0OAdwjawMRqL+I8iFld1ObohODxJvDNdHR61qbK7FmKWUFQAg2Gp5aa6nkp1Os1K1Hp1PLwjHTdP0f6b1blhZYDaQa8QLGQReJgwdZ5z5LdV1GydFnd9cTTf0mqGoq7d4TFr0gQBHpOxPMnYKxpdbJ6Z3T+5T1fT4x1q09fDwJVjLm3G4J00dNzvC1dN1875uEzf1bpdelgpwbabwzHcSxEukEAEERou3N+w8/HlkXDkCrB1A25m5WUXlkTykWx7Xl9p/wAfat3k1j1USIRg9K4HixVw9N/NoB/ib2XD1BXmLods2j0tM+6CZNK1m0EoACgOUg6UAhcgKjpPRNSgWBmcFzcwibC8xvcBaNR39ns5+3Jb0Xp+qvUxj78GSHDmFgDLcryEo61qK9pruX32Za1X+nNLd7qn2v7boh1sG4CCJHNt/bVdvT9X09uzfb+Tzeq6Bq6N4ruX2/wZ7jxOQjwHKZMK9dOLr2Zy6oTjZhrA/h8XmYDuBfvH5uscB7bB8LxAbVziwJDb6a3I/Oyi2HfVNMzol2Wwa+UzWUD2neX2FeMbxo0n/wBj6E0v/wBBv/4Hg4HNlJ7OZus/KYv3+9+9NTppUWKL4eGY6LVR1FUpP6o5THm6HvJ95jRXJXxq1rsnwv8ABzlprNR0yNcOWwiRMbzI95+1aKk3Xdb4/wDSxc0rdPS3uv8AADnXjaPvM/cs7LOzQwrXMmzCmjv6lZbLiKX7iVycrojTY6wLbayB4qNFao6qDSx4MuoUOehmm8tNswWM5HZ3qJ/BexmvYeEg8zI+DcXVnuEm4EAE3MmZCrwurhL3SSLMtNbOCcIt/hM1GGw7osD52v5rCzqelr5mv5b/ANjfR0XW2/TW1+dv7kqngCdTHhdc27/UEF/xxz+djrU/6Wm97Zpfjc1HQumGMqUwSYfmvtmGg5fL7qlDVz1EnKZa1Wgr0ajCGf5mhJW0qCFACUAMqQCSgEzIBmtUgE8gT6IDwLgLXh5qNrVG5nF0NdA7RJu02OvJc26a4wdPTd0VlNm3w/EXAdoh/eYa72t7BU3HPB1IayS+oruPYplem5jJDmtNQyB8tMgm48lc0UZeot9ir1LVVSoaS3/Bn8I8ta0ixNx57L2VP0Hgrf8AkZPbWhmU7SQRqDMrbjtRoTyyz4fxCoB2nTOpc1pjXmO/VaZaKlx7XHbksLXXqWVN/GRylj6jXGDcuky1rpM63FvJbLNLVZhTjxwY16q6tvsljPP3LKnxZ5Agi1jYHw2VazpunnLMolivqWpriownsG3GuMPMEix210+WO/RZPRUut04xFmMddcrVd3e4SrxV0yGtFrGXyDvq6DczeVqj0vTpp4e3BufVdTiUe76udgHcVe3k6b9qT5a6LO3p9N01NrdfGxro6jfRW64vZ/O5lsc+SfCfY/grlkfY8FKv6kxzh2NbhKFGoWF/XmrOUgFrqbwIM6y1zfQryfUKJTnk9j0rXxoraazuTT0rJBLKbWkR8z8xgzfK3vj1XNWnw92dafVW17Y/1/wVHEeOYx4llcMBn9XTaNO8lxC2xrgvBTs118lzj8I9Z+HeKNTh9BzjmeA5r3HVzmOc2SdyYCv1pKOxzrJyk8yeTRkrM1iFACSgGyVIBJQAOcgKHpnjuqwVdwN8ha3+J/YHuVjN4izKKy0eX8Lw0MBXKk8s6kNlg6pjDJChRDkSuCfq8VVdpk6seJBJHnLF0tHXl7HO1dmzK3C05AA2GnMr00NsHmJsdZLnRyufWy3ZyzXwsllRgmOa2M1ocoCSfQeKPglEyk0ZRHfKxb3Mh2oYbPNQnlgYGk81OfAyJWix2P27oiGVGOHsSPXRYyewih/itMHh4IH6mvTcfCqzIf7ms9lxupRSxJfg7HTpZ7ov8mfY6wjllEeu3fC4kkdiLJTGtyh0EzbQASO+J9homGycpHo3wjxk0a9AkTTq5gOTajf+TXKxS9sGq3k3q2msRACUAyXKQASgG3uQGH+KWKjCtb+1WZ7BzvuC1W/SZw5MphcTFPa4MeXdKo+mi6rGhupRZBfN+X4hY9rTMu5NZJDyGYNjT/qOLj5yR/tXc6fDfc4nUJ4jt5IrAA3Pp967We1bnExlknhTdebrne6yxtkN74DqsymB+C3J5RqawyeGQ4O2ssc7NGWB6m6Hxs771HKJOqTlLeVwnkfYHDXaWpLZ5ISGn6Fu+vmsvuQ0VmNF/wCIA+YWuWcGUeSTwX6WhiqB1qUXln8dMioz3lc3WQcq+ODo6KSjP8lBhactEu77am8CTouA+TupbE6jTIEQATrJ0DdIadVjkz7djT/CuvGMrst2qQcP5Hgf71toZruR6mrJoEKAElARXFSAHOQEd7kB538WK/YoN51HH+lsf7lqtexnDkocI9pptkxE6Rv4XVXcsbEXHPIBE/jYKUsmLZLxWIzQ0fKwADvgQvRaWrshl+Tz+rt75dqAoDMBJsNtyefgrn1NFR7E7AmCs721DYwpSc9x2q4xPJc9XzL3owJFBzndkSTyHdeyO6a8hVQYtUmxM8weY5jndSr5/IdUAzUMyZFt9xqCod0/kelH4AoviYUu+WOSFVHJWcVxL2vBBgEDlzP+EV88cmaorfKIrXveQLmLm2g3mNlg7pvyT6EFwi04RDXOix/P4LH1JNNMn04pqS8FbTw4YSyIi3p3rjzjhtM68JtrYkU6QAJjYrFJGXcxvotj6lLEuqU3ZXFjmzANi5pi4PILOCxwYSeTa0ukeJ3rf20/+K2ZZgWGH43WOtT2b+CZYCrcXrD/AFD/AEt/BMkl+5y2EDbnICLUegPM/is/tYf/AOT/AGrVaZRKbhsdUeYIg8zGiq53LKinHcZxNSBuRa1j6zot0GlNNmmafY0PM7Wlmk3vPivSwasx28Hm7F2Z7uSZRaxoMlWGlk0bsdw9UTAWF+8GZU7TRrehFBrutzU2vOakGh1PO0znlhcWODA63asbarjXvGMHWqS8ljwzE4WmcOfoWvEZ352hzahZUbVDmhvyFxFycsZY3WDU3kyi4rAWGq0a5oNqtpFjaFTrOra36I0qrqpnL8rHNbAOhznmmHHOPkZUsZKenjqXZhtIZhULm9W0gHqGZG3Fh1k2G4W3skYdyAr4il1bnZmZnMIIhjfpOoAbHYkk1J0LQCCTqmJGUe3InGqtJhIcKdnVG03uaykA4Ppk05qUiIDA6HEEGXCQSJ19z4M+1IpcbiqZp/Rmmw5yGtpQc7XPeSCSxtRsAt1Ja4ZbAiBKzkh4wRKWYm1u9bVls1bJCYh3bPlKo6le/Yuad+zcGrUhsmw/NloN5S8HqE1iNNvXSfRTEhmkw1S6zILzA1UBbHtBSDTOcthAxUcgIld6A86+KIltB3J7h6tB+5areDKL3KDhlUZY0HjKrJFjuWMEfGO25f5WcVuYTewXDaDqr8jXZSb5oJaO90bK7ROal7SlfCDXuLUEt/WsynTNEt8ZFh5wu9Czb3I4c69/Y8k+i1pu0giNrj2WVuHU8MxrTViRbcJwLXMqO7TnNLQKbKjaRLTmzPLnAyAQ0R+9suTY8SSOnBctk0dGmEOLcUw5XOaQG3JazP2Rn1OgBInmFi7n8GSrXyOcV4FRptcaVZxgkZQWPloNaC4gtgfRt2Ou8gCI2NvdEyrWNmDS4BSLWf8AuGtflHWZntim95YaciPlyl8idW6hYytknwFVH5I+J6OsBph9cOa7EUqT8sNcGv1fdxygXEwRII2k5eq2uAq0nyQcX0UZVAf+kdTla3Oyq9lZ1MuqOaBma5pHZAfGXQwdlrc38G1RXhh4LorSAl2JaSxtUPylpHWNbViLyGB7A2RmzSIy5hBXYDryXFPoowgn9KbkGacobmOUOOUduzuz8puA4b2ET1O2EIafG7Kx/AKAq4hpqBxpvaGU6bsheeqru6sOqNgOLqbIcJEOi5IinPfctx2KfpJgGsote1j5jtONek9tJ+dzTRLGtBc6Gg5pHzaQFiSZnBU3NmpFswE94E/esomLNG/UOGhWYLLBVUBd4aqgNW8raQMVCgIOIcgML8RG5sOD+zUafWW/esLOCVyZfg85XXGmm6qtm9IjY1x/7WcGa5po1vAaIpYUOjtVTJO+W8D2XZ0tfG35ORq7Od/wSuqH1T+fz3LqY+TmESpwsZswlp3LDlB8QLHxha50KS9uxthc4vfc5+A/edt9b/kq36KXyWP1cfKEGGINnOPk11/JP0c/kfqYfAXUuH1tP/G72vfxU/pZ/wDZD9TD4YL8M47/AP1n8e5Q9LY/4kFqoLwyPX4fUIgPiDu0Du9Fg9Hb/wBjJauv4IzuBvd8z5jl/hY/oLHzIz/XQXCJdDgLRcgHvN1l+gx5MHrk/BoeB4cA9UIG41jv/FVtRpnBdxZ0upU32lP0yp9TiGSJz0wQR3OIIv5LnTR0IlNjq9Mtkt9hK1ZNmDW9FeinX4Njw4AVczsr+UkC4FtFvitjUyzo9BqzQAKtMgAa55t5LLtZBMo9Eqw/1Kf93/FR2sElnR2qPrs/u/BT2sFk8rMgYrFAV+JcgMj0wbmw1UchP9JDvuWM+CUzFcOJjVVCwkMY4nMttaNdjZuA4QG7NAb/AEiPtlej00e2J5vUS7phiraGhWTQONMb3KECvrbbqUAusBKZJOgch6JkjB0DkPREDhUExz0Ut7Eikz5KAAaygC0cSWODhs4ei0WR7lh+TbXLskn8DPxKALsLUGhFUeX0ZH3rz1yxsz0dbzhox3FHdkX71XRuZ7f0So9Xg8OzlRpz45RPurUeDQXbSpAUoBCgKhzlJBHqlCSvxZQgzPHhNN7ebHD1BWMuCUYjgjTy29Z2VNliLwA6nNdg/eH2yrOnjmSRW1EsRbNOypNl6WKxseabyyQ18LMgd6yBKkDdN1sx3+xCBKL9zugHm1p080JO6yyAae+08igHjU0KAbrFCAGVFhIzQPSqtnw2G5tqPb/aCPaFw9fHtm/ud3QS7q19jIcTBcA3cwPM2XPiXmfQeEbla1vIAeghWUaSW0rIBSgEJQFM4oQMVCgK7FuQkzfFndl3gfsWMuAYzhdcyIHt3eypyaLldM5cIktZ9OHkaN3ImdJie8q/09p2bnP6nCUKyya6D5L0B54dZUWRiOsuQDogOxFTbmgBLoUkDIxUO7ljncywO060qckDs2hSBKNS0FAJUdsgGOsgrCRKI2PqF5az6rZd5mB9wXE6pNd0UdvpcX2tkChQNXFUKbR81Vlv3Q4Fx8gCudWtzpWHutJytmgkNKAOUAhKAp3lCCNVcgKzFuQkzuPOqxkSucmK4eZdrYE27gqU0i9XdN+S2rUge2BcesWlbtDcqrNytrqXbW8DrXaL1C4PKv4HGlSRgfDoU5IADpMrIgGvUiVDJRXVH7rVJm2KJuHetkWa5LcltcsjEGYKAF70yCPUqQFpus9ODkzdRS7LFEjZwe+/LkvLWSlNuTPU1xjCKjEmdD6g/wDUaU6/SDwPVu/ApTyRaevUirZoJLCpA4CgOlAUjihBGrFAVmLKkkzfF3wx55NcfQFa5Eox3CW30iFTsZarReVXAEN0JC1Z8m9/BHpPOh2XqtPPurTPJ6mvtskiRTcrRVHcyAJhU5MSLi6myxkzOKImINlqnwbYcj2EqWCyhLYxnHcnU3rbk1NBlyZIwM1HITgZqGS0d/2D/pc7qU+2lo6PTId16AEdaWxbfz1+5edTfblno3FZD6OSMdhzNxUIPgWub963Vv3I0T4PY6RVsrklhUgcBQHShBSuKAjVkBWYpSSZzi1POx7ebSFrlwSmZLh1eCwxza7ucD/hUJplyuS2LCrVH6QAYuwx6qMZrZs7v9xIQHtHxK9B0+fdSjznUY9t7+5Iaukc4MFAFmUkEGq6XLW3k2RWENYl4harpJI20xywsOVlBmM0TKbluTNI7mUkDbygAose58tEhgknlK4nVpcJHd6PD6pFjScP0SkXAZs1d07wHuAv32XMmsQijp1y7pSZF6FYY1ca1x0aDVP8vZYPMunyWyqPuNM5HrVIq0aSSwoQOgoDiUBSuKAj1igKvGFSSUOKK1sGP4hTdSdUP1HEPB5OBBI7t/VV7IZN1c8ch4/EginXZB6uM3Mg2I+1a4rGYs32SziSJtevSe4Ookw4AkEEQ7cLs9PjKMGmcTqMozmnEdaV0zlsKUyQDUfZMhIhtdeVgnubnwMYkz5XVXUPOCxp1jIdFy3QeyNU1uTaZW5M0NDoKyyY4Ee5MjBWYitXz9XTe4NfGYDR0c1ytbFdynLg62ilLs7IcsffWqOyYWlNR4kEMvAc4ucZ8TqVyXmyWTrRarj2+T0TonwT9Ga5z46yoRmi+VrRDWA7xczzKs1x7VuaJy7nsaakthiSGFCB4FAcSgKUoBmuUBUY42UklFi9FrYK+o0EQbqAUHEQKD29UA3PmzDVpiLRtrssPTUmZK1wR2BbAXXoWFg5Fzy8lkwq2VMBEqSMDNd6xbMoojtcsEbGM1tCqNs8zwXa4tQyLRcrMHsVpom03KwmV2PArIxwC8owkVfFMQ5oltjz3VDWbrBf0icZZR6f0UwLKWHpZWNa51NheQAC5xaCS47lUUkkdLJetUgk0ygJDChA6CgFlAZnC1MwdmfBGXLLmtF3gOmxJsSbaQsMskce6kZOdwEVCAajM0gnJIjfsiO+dNIywM4ujhhrVce1UsHtJyguyRDbn5J/iPIgO5gj1uH4Ij9cZzAR1jYjftZeXa0iezqoywZHEAAmNNlIKTjlGch5T7x+CzrWZGu14iMUiunA5kybTK3pldhFyyGCNXctUnsbIoZLoWEpdqybFHLwF1ciFyu7M8nUcPbgj0SuhW8HPmidScrKZVkiQ0rNMxBqFGwiuxokFVL9y3S8HrvDGxSpjkxg9GhUDpk4ICSwoB9hQDoKA6UBTOCkEauEJKzFKCClxiwZJAqqAV3FPl81up5NN3BX01eic+RMprejRIJyyMSLVWuXJujwNHUKpqG+wtadZmP0lzzoEZ3zHxXRr4ObZySaStxK0iQ1ZGtiVEYjyQq2iq2lqs9gw+g8AqJ00SmoB9iEj7UIHQgOKA//2Q==</t>
         </is>
       </c>
     </row>
@@ -2917,40 +2917,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>YASHASVI JAISWAL</t>
+          <t>ISHAN KISHAN</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>smat2023_058</t>
+          <t>smat2021_081</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E20" t="n">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>138.9</v>
+        <v>142.1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>44.4</v>
+        <v>36.8</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
@@ -2983,10 +2983,10 @@
         <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="X20" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
@@ -2998,25 +2998,25 @@
         <v>0</v>
       </c>
       <c r="AB20" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="AC20" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE20" t="n">
         <v>22</v>
       </c>
-      <c r="AD20" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>10</v>
-      </c>
       <c r="AF20" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG20" t="n">
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AI20" t="n">
         <v>0</v>
@@ -3029,12 +3029,12 @@
       </c>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>Batter</t>
+          <t>WK Keeper - Batter</t>
         </is>
       </c>
       <c r="AM20" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUTEhIWFRUWGBUXFxcVFxUYGBgdFxUYGBcZFRYYHSggGB0lHRYWITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OGxAQGi8lICUtLS0tKy0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQIDBAYHAQj/xABJEAABAwEGAQkCCwQHCQAAAAABAAIRAwQFEiExQVEGEyIyYXGBkaEHQhQjUmJzgpKxwdHwM3KysyU0NWODosIVQ1Nkk6PS4vH/xAAaAQEAAgMBAAAAAAAAAAAAAAAAAwQBAgUG/8QAMREAAgIBAgQEBAYCAwAAAAAAAAECAxEEIRIxQVEFMmGRInGBsRNCocHR8DPhFFLx/9oADAMBAAIRAxEAPwDuKIiwAiIgCIiAIiIAiIgCItP5ecvbPdjIfNSu4E06TdTwc93uNnfM8AUBtr3gCSYA1J0HetXt/tFuuiS19tpEjUMl/hLARPYvnnlhy2td4vcar3MpHq0GudzbQNJGj3fOIWthqZB9W3Ty/u20nDStlLETAa8mmT3B4E+C2ZpBzGYK+LcOS27kh7Rrbd72gVHVqAgGjUcSAP7txksPdl2JkH1Mih+S/KGjb6Da9B0g9ZpjEx0ZteBoQphAEREAREQBEXiA9REWAERFkBERAEREAREQBERAEREAREQFDzAJXyNfVprW211q1STUqPcYzMCYa0djRAHcvrit1XRrB+5fK9zUsNWT2jzlazeFk3rjxPBYsvJaq6C4ho4E5ny0WXR5FvJ+MeAODRPqVttkGYMSpOvVJyNOOBVF3zfU6a0la6HP7TyWYMg5/jh/JQVqupzSRM8F0W0UXmYHFaveNMgmRC2rtlndmt2nrxlLBs3sAvg0rZUsrj0a7C4DYPpZ+ZaT9lfQS+YvZnZyb3shb8t5PcKT5X06rq3OY1gIiLJgIiIAiIgCIiAIi8QHqLxEB6iIgCIiAIiIAiIgCIiA8lfO15XZzN42ukAejUcW5bVDjbHg4eS6x7RMeChmea5x3OAEiTgdzYdHu4vWFoNva34QHtxGQG4nEmcGgBJ0bihVb7OccF7S0vaeSOw02ftK1YPiQKW0mNMJJzIE9qu3Pej3GedrVGEAgVQIwmYOmhjXsUvUuthBLm9YQSIII4EHXxWAbGKUBocZyAPAaADYKDixHBaUMzyR/KK8JcaIOE74TH3a6rXrXY6NMua9tXnGwHYsYDZyHYFmcpWPpWltRzcJBbHYRmsurQbXJe73oLjlnHHitoyUVuaTi5SeEtiW9kFkDrdTeMxSZXJJ2kMaDP1nLulGs1wlrg4cWkEeYXyxeY5sPDXENJYHBpIDgZ6Lo1HYV1b2C2N7LPaamlJ9UCmNpY2HuA8Wj6it1zzsUba8ZeTqqIilIAiIsAIiIAiIgC8XqIDxF6iAIiIAiIgCIiAIiIAiIgMG+LCK9F9I+8MuwjNp8wFyW+rvqU2dVwNIy4EZMxOOQOpBJGuWkLtCjOUVlFWy12Hem+O8CQfMBRW1Ke5PTe69ujOU2G88hiz4pbnh5ABd24DB7B2fqVDNfEev5rNstgbi5yXGc4nLuwmRvwVBep1X6Gu38x1R/OOeXBwIwmDhE8OPaqKlrDGta3TDl4LO5R2drmnCIM6iB9wC1621cWBo90QSNz2KaK4ivKXBlmTQuy0WpoFGjUqF9XCMLXFshowh7gIaOkTmRlnovo/k1dIsllo2dufNsDSeLtXO8SSVC+y+5jZbBTDhD6pNVw4YgMI+yG+Mrb1chHBz7J8WwREWxGEREAREQBERAEREAREQBERZAREQBERYAREWQEREAVLhIIVSjL2v6zWXD8Ir06WOcIe4AujWBuiBwisHAZZ4SWnwMLJsF9Cn12kRsQY8wqaEOL9wXvjuLjBVVl6OR0XMyuTO1jsRN9X014yOZ2zUD8KwjoDpQekeJ3aPxUhebQ5xgQJgdqxq9mhqsQxFFSxSk9+h9O3A6bLQI3o0v4ApFc25Ee0WxOFlsBNRtYUqVOXMimXCmBAdO5yGWq6SrZQCIiAIiIAiIsAIiIAiIgCIiAIiLICIiAIiIAiIgCIoi+L9pWcZnE/ZjSJ8fkjtK2jFyeIrLNZSUVlkharQ2mx1R5hrAXE9gElcA5e2t1sqC0PmGPBw/JYJAHhIcfFbzft+VbRTc2o4MpnUNyGRkYnHM/jwWmwCMiHAz3Edy7Ok0PwTU+cljbov56nOs1ic4uHJPO/X/RZu5mQWbETiUTSd8GIBk0icjuydj2cPJSlWqDodV5XU6azT2Ouxb/f1R6qi+F9anD/z5kLbKcuyGSwreMipy00yASoK00XPy45D81rDdpCzZNmDd1mlj6uhLg1p0IDMyQRmOkR3YV3f2ecs2Wui2lXqAWlvRIMA1QNHt4niBuDsQuM1rdZ2gUmOyHRGRjLUzwJJzORzWLZ6nxgiQWmBG/cRuF6edFTqjXGWWttu/X9Tzv4k1Nya2fc+qF6uTcneW1pogNq/Hs+dlUHc/wB763mugXXyls9cDDUDXH3HkNd5HXwlULdPZXzW3dEtd8J8nv2JlF4vVATBERYAREQBERAEREAREWQEREAREQBa/e3KenRJawc44awYaDwJ3PcqeV16miwMYYc+c9w0ax2nTzXPrXawwcSdB+fYuhpNGrVxT5dF3OfqtW4PghzJu8eUleqCC4U28GZZdrjn9y1i1XvTb1emezT7X5Soq2F9ScbpIzA0HgFiNC7VWnhBYSx8ii05vM3kv2y2PqnpHLZo0H5ntKsPZVDC2m4NnciSO6cvMFe4DMQZzkQZy1y1V2VM4px4f7+hunw8iNo3e8SXvNXFk4PJzzmMtFUajqJGpp7E6t7HHfvUn2jXhsVZLWnIjL1adx3EadyqanQU6iv8NrGOT7fyWaNZbTPjW/ddzLqk1aeUQMzOmQ3WqW+1PfDG9EHIDc9ruyNtO9SttqmzscA6WPEAb9vhGXisK7LGSecqanQcAuZoPDZUyamvizz7Lv8AX3L+s1ytS4PLj3f+vZmPZroAzMklXvggBkKVcFSaB0jPLKROZgZTOuy6so014TwjnRc577sv2G9C0Q8YhxGTvyPopWjaqVQdYDsdAPr+C15rIlVPybJ0AUnAsZIHBM2+lfNoo/sq7xGgJxD7LpC3jkZywbbPiqgDK7RMDq1ANXMnhuPHu5PYahApt2IE9m8hWKVpfSFO0MOF9KoQD+70hPEajxK5+q0sZLlh9yai2UHhvKPo5Fi3bbBWpU6rdKjGvH1hKylxDqhERYAREQBERAERFkBERAERW6z8LSeAJ8ggOb8qrZzlpfnk04B9XI+uJa7edLR24if15q/WqkuJO+Z8VRWqYgQdYPmP/vqvUVQ/Dikuh5uU3Kbm+rIw9fvafTJZFwWIPeXl2EUi12TXOz6RZIaCQMTcyAYkd4xbGDUqNY0S7pCB2xAU/dV1vpFrjUfSe8mmWtwmROYcZcNp6uS21FijBrOGWqovi5FvlFbWtY11Lo1a4c6s4Ate4YiM5cXNa4guAmSIngNZatxvK4abvecH9EudUdhgZANhwY0Q3PKYwgRstYtNOmDFMuIAzL8Ou+GNtFppZQ4eGP8Af7yXy6G9ylnLMdqq11XrQhGyt5ITA+BB7i9+YaS1rdgGkgnxM+EK9gA0WcylA8XepKxy1aRWDLlkpa0hr3N6wYSDuM8yM9QJM7Qpnk/yes1ooUyaReXYhWqiq5pokkhst6oAydJmQdlEU3FpkfgfvVitY6TjJDmnLq4YOcnrDLLYLl6zT2Sk5QzvjdbvljBd09sEsSx15/cxqOjhiDsDg0OGWJpnCQNfd32cArdtf1WDcifBZVUgANaIaDOsknPpEneDGQCja1QB08JU9MZQrxLbf2RpNqUsrf8Akm6QxVKDdjiJ7mhYV41poujR9Wq9vcBhnxM+SrpYi4AEB5pCmHbMxAvqvP7rGjxcFZqkVHDCIYcLKY4MBwg+MOKzY+KTSIYrDTZ3P2eVg6wURMlgLT2EGQPIhbMub+y62kV7XZz1fi6jO9rQyp6c36rpC4Wojw2yXqdOmXFWmERFCShERAEREAREQBERAFhXu/DQqn5j/wCErNUPyqqYbJVI3AH2nAH71tWszS9UaWPEW/Q5dVb933KOqV4drE/qfWD39ikq33ZrGtNERMAtOoO3aDsV6lHnU8ERRrtD3va6ZaeqcwRrpmCQfRSda+a74HOFpIJhkNABy92O5a9eVHmjzgEsGpjONx3xPepm77OatbDMSANJ22Ej70bhhueNt/oW1nZR6/f+spdJzcSTxOf3qgBT1C5mmvzTnHq4pEDeDxkaeaxeUF0/BzLZLf1n3bdh7woYeIaaVsaYy+KUeJdmvRm8tNbGDm1snh+jIpozXtmILyp+3XXTZQNUDZx1dlhDjPWj3eCvXJdVHmG1XtguaC458JJzMDQngq0/GdNGHH8T+Nw2W/EumP3Jo6C1trZfCpbvozXnVNoVtwWzi56NVrjSOk5iO35JgjI98HMLCuC7W1S9rwJa4iel7uGRkR8pI+L6Z02XPKVfmTi1JfTmP+BarI1rD4uTT2f1Nfcrbism9GhlRzWjLowMzqxpy31KzH3G7m8eIiBJgA6awJEjXOc1av1lFEYytkoqWEs93yI6tPZa2q1nHPBrtoqqIq1JIPasyu/4xzTtPqFFWswGjiVFqJ7Z7ElcSdsFM1ZGmPrngyR0RwL8LfBo4qVsdAOtIbGTBid2SIaPASVbsD+apSM3O04kn9eQUndVm5tknN7+k48Z/X3reMcblWyec+xOcgnf0mxo3pV6ju6abQPMjyXXFyH2a2WqbzdWdTcKZoVGtcdOvSjzgrry4mrkpWto6mmi41pMIiKsThERAERFgBERZAREQBQ3Kt7RZnh0EHKCYzHSEdvR9FMrT/aDUOGizQFznT2tbAHk4qbTw47Yoh1E+CuT9DQ3B0g/ksavbQ05iRvmsi1PDZxEd4mVh0bTSzOGTvp+K9KjgJEVfVZ1ZuA4m0zMiA0YRm4ncwAcslOWHoWnLQPwjyIH4KKtJ5wt6IYwuGM7lrOm6TwhumizMZbDndYFrnd+RKcClxRfVY/vuWIy4eFroza61OLbTcNHNcPLC4eoKv2t7axfQfE5wNMpcIOeYIbrxngCbVrrND6LyeqRJOQ0dMEwMzG+y16+Lzi0ipTcDlnBacsbjBLSROhHAwV47SaCzUqnKcZQqxGWPLOE3j3Xun6nfu1EanPqnPLXeMorP6/qS9/gtsVQEEQ2rrE9SoRMZK7SbF3/AOE/+S4qKvu/aVSg5gf0nMcBk7MljgNBkZI1047rNo33QbQbTdnDGA9cZ4ACMh3jgUp0msdEZTqfErnNxXbfllpc3tubW3UcbjGaw61HJ5yJPQcdsT/KKYHqH+qq5PmKleNqtSe+KM+uJYf+3mNp4abcyOLj4EuggdgnfTVYlyXsylzpqOze9x0du1mfRaRsptXotVfVqrvw2nZwqMdm8R5t4yjSi+muyqtSTUc5fTfoYtOhzlrjYR4ENAb4jCSO1qlG2nHUe0DIMDWnOIe1xAG2jAfrDgsX4TTaypVa9pcXPcOMYjsYI6LWkAwcyqLDfTKoAFJrS0SThDYGh0Pbw3KeKwuvna1W3GFfDHphtZlJJ+botuz5k/h8qqlUnNJynl7N7ZaSb6dXv3yadfYw152d+PSHo4KNtDJqUhE9YxxghTfK6nBBHzSO0dWfNqgra3EaJ+cW+eErr2z4oKXfhfvg5ijwya7ZXtk3W7LJJxPIJG2WXYAr9ptmHE52wMKLsvSbhp0mQJBc4CPqxJPosW12RwGdQuzmDp3cYW1/iNFb4M5fp0IavDrrVx4wvX9jovsWLXOtBc5zqjW0wMTiQGuLpDQe1o9F1ZcW9jVpPw2oyAAaLjr8l7IjLtXaVyrZRlLMXsXoRlFYktwiIozcIiIAiIgCIiAIiIAtR9p5i7qxBgzSgjIj41mh2ynzW3LT/as6Luqdr6Q/7jT+CxJ4WUbQWZI5bYXVXf74kfOaw+ZhLdZ3jPGwn6P8nL261cvJ+Srx8Q1S2Vj/AEf3Lz0Gl5/ho1sWivWrsolzcBIxhrQJbIxA9hGS2u9z8Y7uB9FD8kKWK01HR1WAfad/6lZ9prYiXcf0PReq8Oc51qc3lvueY1airnGKwl+5RRGTnbnJYU5rLqmGKPDl0GyKKKYlw71n2jZYtjZLgsi2HNOhl8ymksetqsijosWuc1q+QXMoeJBHEKOpvkRwKkXKMtQwv7Dmob3jEiatdC/a5fTcCSTG/YoxrA+i4nVha4fba0/5XHyUpSdIhQjcQDmtEnE4R2AGfSVz9d5c+j/ksUc8eputzH4sLGt51Vy43fFjuVu3ryv5j0mfhJ32Nu/pMj/l638yiu6rhHseyvP/AAao9aZ/Bd3V6vynNt8wREW5EEREAREQBERAEREAWj+12sBYmt3qVqbR4Bz/APQt4XKvafeHO2qnZxpRbid+/UiPENA+2o7ZYgyWiPFYjUbM7CArV4VJCqtYhYFpccPFUYxydOUiR5ItDGV63z2s8Q0uA/zq2x0g7AEATqpDkmQLE1pE88+u93EEPFNpHdzSotlidSfgeQ7cEbjbLYr1vhl0owVVi35xfSUf5Wd12aaPL6yuDnK2t9UpLqn0+jXL12eDCtrtuCwAVkWp+ax2HNdVlSPIzrC3NWra5ZFj0JWFbHZrL2RiPMvtPRWLaFkDRY1c5LV8jZHk5LCvJktB3BWW0qio2ZB3Wk1xxaN4vDI+z1FVcbR/tCztIkPqsbH0vxZ/iWIw4TBW8eyW5xaLxbVcJbZ2OqfWMNp+Uud3tC5GplxU/Iu1LEyIuEltPC7VvRPeMj6hLTmVevKxmla7VSEQ2vWiNg55c0eAIV2lZxC83PaTO9W+KKJD2VvDb0pz7zKrR34Z/wBK70vnG57R8Ht1mq7NrMnuccDvRxX0crVLzEpahYmERFKQBERAEREAREQBERAFwe+a5fbbU/8AvqjfsOwD0au8LgD3461oePerV3faquP4qvqfKi3o18TfoYttzCtWhobRnfQBX66jLzrQ3uCgr3wi1Y8ZZs1xU4slnke7VPfNprZrJvuC1jp6UFp7QND6rJZZuaoWOmdRZaTnfvPc+o7+OVG39kQdi3Lvkhw8wvWaWMZRpy8NZx67PKf3+h5SbkrLccnz91h/Rmu2l+aUmqloxOnYK9TGa6hGzOp5NUVaT0lJ1TDVE1T0liZiBmzksetorriIGasVCsPkZiW6RSqFS10Kt7hxUaexv1I62WcueMIku/Wa3j2OWllO383il1SlUZO0twvwjjkxx8Fp9YGDhPiFncgqpZe9jjeoR4OpvB9CuPrq2pNt/D2XV+vy2wkX6LI8OMb9+y9F39WSvKB39JWud6z/AMIXhyCzOX1k5q9q3CrzdUeLA13+Zjj4rDfovO2+Znbo8iIm8DLmx8pv3hfTAXzBeroBI1GY8F9NWWqHsa4aOa1w8RKsUcitqvMi8iIpyqEREAREQBERAEREBRVdAJ4AnyC+dLkrY24j73S+1mu/37Uw2au4atpVT5MJXz9czYa3sAHkqup5Iu6P8xk2krXr6qwxx4A/ctgtZ1Wt24B7msOjnNae5zgDHmtKVuS6h4idUvZ2f0TGAD6Om0R5grUryt/xIY4GWlxx5aOzI75zU/e9rgOHvPnwB1Wm3u7E5rBoMyvaQoXDHP5cY+eGvs2eRqsk5Sl/2zn5ZK7C4uBMENG+k9wVVN06bnL81XVbhptbxVNNsQrRn1L1pfGSxKwzBVVrfmvAZHcsSMrkUucW5yqHVJBKuOzCsOdssPkbIU2zT7dVi1XklsExssui/JWWANdB7woZLZG65sw3PI3Km+Q9KbzsTx/xYPZDHa+CjbU9vBZHJa+jYrXSr4MbWHpN3ggtJbwcA4wqOrhxQwuhPVLDyb57YWRb7O75VGPs1Hf+S115yW0+1tzatSwV2HEx7KuEjQh3NuB8lqdQ9FeXv8x39N5CFvEzkvofkZaDUsFkedXUKJP/AE2r54toXffZ26bssnZRYPs5fgpaSDUmyIiKwVQiIgCIiAIiIAiIgIzlL/U7T9DW/luXA7s6q9RVdT0L2j/MV2vRQI/rFn+nofzWIi30X+VfNfc11v8Ahl8mbnbf2ju/8AtYr/tvFEXt1yR5Wr9iStWre4K0esiLcyjHteoXtPUoi1ZIuR43RWH7r1FquRsU0tFTW93xXiKF+U2XMxXdZV2nqjuRFCvzEnY6Dyn/ALOun6N/8DFAnqoi8hf5j0Ol/wAZC25d79mv9mWX6P8A1ORFJSQ6nobMiIrBVCIiAIiID//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUTExIVFhUXFxgYGBUYFxgYFxgaGBcWGBcVFxcYHSggGBolHxcXITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OGxAQGy0lICUtLS8tLS0tLS0wMC8tLS01LS0tOC0tNS0tLS8tLy01LS0tLSstLTUtLS0uLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABAIDBQYHAQj/xABFEAACAQIEAgYHBQYEBAcAAAABAgADEQQSITEFQQYiUWFxgQcTMpGhsfAUQnLB0SNSYpKy4TM0gsNzorPxFSREY4O0wv/EABoBAQADAQEBAAAAAAAAAAAAAAACAwQFAQb/xAA0EQACAgEDAQQHCAIDAAAAAAAAAQIRAwQhMRIiQXGxBTJRYXKBwRMzNDWCkaGyFNFCQ/H/2gAMAwEAAhEDEQA/AO4xEQBERAEREAREQBERAERIXEuLYfDgGvWp0gdAXYLfwvvAJsTWKvpB4Yv/AKtG39gM507QoNh3z1On/DCbfbKYP8WZR72FoBs0TX36bcNG+NoeTg/KZXh/E6Fdc1GqlQdqMG+UAlxEQBERAEREAREQBERAEREAREQBERAEREAREQBERAERNB9LXS58DQSnRLLWq3s4AORVtc3OlzcAecAiekH0oLgqjYfDotSqB1ma+RCeVh7RHPWcS4zx+viqjVaz5nbc2t5AchIGJxBqMzOxZmJYsTckk3JPnGHpi+s9PD1azHQEy96q3tMB3XvPGZh7IP13GXPstd19hrfh/MATxtd56kwcQANCb9spo8QqIwenUZGGzKzKR5g3EsPgKgF8h9xljUHURYO0+jf0qM7jDY5hdiAlcgDU6BanLXk3v7Z2EGfHC7g+XjO9ehXpI9ak+EqMWNEA0yTc5Dfq+WlvHugHToiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAnIvT6WC4Y9UqRVWx3DZqLBgPBWHnOuzlPp8og0sMxB9pxfs0Uj5GDxnDqdIuwCjU8puPC+iBIBY6+Gki9D8KDV1F7Tp+EpAWmXPkadI1YMaatmH4Z0UppYkAnwHymXbhygWsJlUEpdJmbb5NapcGt4vhSnkJqnF+jqE6ATodcWmGxqXuZ7GTTPJRTRyXiPDnpHXadW9AeAzPXxBYXUBAgIvrrcjcDS3/aax0pwwNM92swHRvjlXBV1rUiQy7jkw+8hHMEXHu7Jvxy6kc/JHpZ9XRI/D8YtaklVPZqKrjwYAj5yRJkBERAEREAREQBERAEREAREQBERAEREAREQBOd+m/DZsCjfuVl/5gw/SdEmlel+ln4bUUAlsyMLfwMGY/y3i6FWcs6BYElXrHa5A8BuZtA4/h0bKXHjykPozhR/4fTX9/MTy0zN+kg4lcGuZTSzlFLNYEkKouzd1hzmSSTk7NcW1DY2zBdIsK5C+sF+VwdfDSZemobVSCDsRtOVYRcK7lqQqoAwFyTYE6gXm/8AAWC0LXvlkJqK4LIOTW55xTiNCkDnqC43A1PuE1jFdJsKdm94tMfxdEr1GYsVXNbTcnmBIaUcAptYsw1Oa+mtr9m8lGEK4ZGUp33GQxqirTYDmNJoFQFWIO4vfyvN/wAJhqQOalp2jl7u2a50nwIGKC7CoEJ02ubMbc+Zl2KkUZbZ9G9EML6rA4amb3WjTBvob5RfSZeWsLUVkVlN1Kgg9oI0Muy4pEREAREQBERAEREAREQBERAEREAREQBERAE1npjctRW1wwqC3kv5XmzTXemVM5KTj7r/ADEqz+oy/TOsq+fkaVwjD5KIp/uNUQDwqNb4ESy/BrMXUWJ3tzB0se6ZHCUSobNuajHyIWZIOoW55TJJ72aoLuNUp9Ghrfq09yi6KT2nlM7gKWWm1r6xiMXoGYafu7aSmhxqnla4UWHI3I8bDeRtyLKSRquH4d+2fK2VwxZD2E72lirwdgzlaeV3uHIv1rm7b7XPZJ9XH+suVXLUv1TdTbxtt4TaqLq630vzkuuS2IuCe5o+B4V6kbeUhcYpj7UR95KIy9xNzf3fObTjfbtNW44D9qqN4X8MvVHnLIt9LZWo3kUTsfo6xBfh1AtuFK+SsQPgJskxPRPBepwdCnzFNb+JFz8TMtNUfVRkytOba9rEREkViIiAIiIAiIgCIiAIiIAiIgCIiAIiIAkfiGF9bTZO0aHsI1BkiJ41ex6nTtHP8ZSKllIa4YDUWv1QdO0byFxJiEOXfQ/Gbr0mo5qV7eyZpjVwNCdJizw6XsbME7RrRxgqMUZyW2yAHN45dyJUcIqg6OCeRQgkHuImTxWBUsGW6sNMymxt2XHKRquLNNSDXe/425bC1+6eRcWXqPga7iKITrC6i+jEEDs3OkynAeKO1tQRci41Pn3SzjMP64WLM4PIk27eZ7ZNwQWkAAALaCJtVR41T2ZKxJuw8Zd4L0fbFYxwwsiOC1+aqFtbvJ08Lxw+katVVGpLD5zq9CgqeyAL2uQLE2Frnt0EvxQuO5ly5GpbF0CIiaDMIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIieMwAudAOcAhcba1CqexTOUcRxIvYHfU+6bBxn0k4Osz4TDl6rMrXqgAUhbezE3byFu+axisL6xbjeZ87SaTNOCLabRK4dxFWAVt9vLlJdehTcDMlyTYe7czTq+CrD2Rmttybw7CJHPE8UlxYga6Mrc5UoRbtMt65R2aNnxmJSnccht3zBtxAvU0vYcu+Yavia9Q6/IgfGSMGrKb8/hJqEVyQlOcjrfo84YDmrNqV6oHYSNSfKb3NB9FvEafq2oFv2pJqAHmuikjtsd/ETfppitjLLkRET08EREAREQBERAEREAREQBERAEREAREQBESitWVFLMwVRqWJsB4kwCuax6SMeaPD61jZnAQdvWIDW/wBN5r/Sj0sYeiTTwq+vqfvarTHnu3l75ovSTpJicVTp/aHBLIXyqMqrmIygDwUantM04sMupdRCT7Lo1TojQK1yx5ArbxI/SdNwQuJzrg1UJX19l+ffOg4NiJytZGUcjjI6WnacNiT6gXntdNNhLubYz3EuuW95lLjW8dhxeRK1IKsmValzmIt3TAccxhItLoRcmoohJpK2X+iXG/V8Ro1SbIrBD+Frh/n8J9GU3DAMDcEXBGxB2M+TaT2OnKbxwzp1jsJToBHVkKt1HXMAA1lsQQRz58hO3PBSjFc8fU5ak25S7uf5o75E53wP0r4apYYlGosdM4u9O/iBmXzHnN+wmKSqoem6up2ZSCD5iZ545Q9ZHqknwXoiJA9EREAREQBERAEREAREQBERAEoq1FUFmIUDUkmwA7STtNY6R9O8LhbqG9bVH3F2B/ifYeGpnJ+knSvEYwn1jdTlTGiDy+8e83mrDpZ5N3siuWRI6H0k9JtCldMMPWv++dKQ8Ob+WnfOTdIukeKxjD1tVm10Gyr+FRoPHeQqzny7/wBJYDjn/f3To48GPHx+5U5N8hKQH1vJOOxHrAlhbLTVPHLpeQqtc8oTGgLZkYm+hDAb8iCp+c8m4pp1wShdNXyedx/7Gbh0c43cCm/tDYzTHxnZSJ72f8lUfOXsH652XJlBJsALDXbUnX4zHqsEdRHhprvNGDI8bq7vuOsUtriUVnFtprfDGx9O2b1Tr+7mKn+YKR8DKeJ9LfU5lFHPUB7eoo7yBdj3aeM4MMEsk+nG1LwOtkvFHqyLp8SXxchELNoB9aTQsbiS7E+4dg/WV8b49iMQwLHKF1VVtYd/efGRBjm+8lNj25cp/wCUgfCdfS6f7DeSt+X7nNz5ll2TpFdKmTJWMx/rKosLBEVABrtvIicQPKlT8y5//UjUwQbzXalJS6Xt7f8A0zvsxcU+fp4mUUzI8H4vXwr56FRqbc7aq34lOhmNp1fA99tfdL5qDs8xN3SmtzNZ1ro16VkayYxMh29cmqHvZd18r+U6PhcSlVA9N1dGFwykEHwIny5m7JmejnSbEYN81F7D7yHWm3ivI94sZiy6NPeGxbHK1yfR8TTuifpAoYwim49VWOyk3Vj/AAtbfuPxm4znThKDqSLk0+BERInoiIgCIiAIiIAnJvSH09LM2GwzWQaPUB1btVSNl7+fhvnPSl0q+zUvs9JrVaguxG6objyLajwvOK3vOho9On25fIpyT7kXc957cyiUVWN9OU6baRTRbxV/EGQl3ktnvLLCZ57vYnFUWzv5SpqJ0I17RFNNdduclpTt4fXOSx4+ojOVFKUAQPq0ugZGVhpqCO5l/XaXBoJbqVLgj4dveJocYpUymMndo3PFcZSm6rZrsAbjbUXH5e+c+xDl7sx6xJJ89TN2w1dTglqlQStIre2oK3X9JpLz5/0ZjhBTUVVOnvdtXv7uT6H0pknk+zcndq17k629/BGYWhacuWuZXl7NxOko2chsoFEjf3y6tHX8v0kjDm4kmhgne5RGYKLmwvYTSsUIrqb2KXNt0RUS20rDcp60ju19CJbKSgtiEYuTLoqg7++XBIZMkUHuPD5SlSt7lrjRdVyDcTt/ox6XHF0jRqtevTG/N02DfiGx8jznDzJvBOKVMLWp16Z6ym/cRsVPcRcSrUYlkjR7CVM+nIkThPEUxFFK1M3Vxcd3Ig94Nx5SXOM1WxqERE8AiIgCWsXiFpo1RjZUUsT3AXMuznnpi44aVBMMp61Ykt3IhGnmSPIGTxw65KJ5J0rOVdIOKvisRUrPuzXA7BsqjwFpCpjf67Z4Bo3db5ys6HzHxv8ArO/CKSMjPC2x7pGQ2lwnRh9cjKSvORyEolQWVthL7b9+39pbQcvrzk2iTsf7yWOKlyQyNrgqwHDKjhjTRiqAFzbRATbMx5D8hJuO6OYiiSDSLWBJKAsAMxXMbC4BI0vN04Q+Jw9CkqtSpUarBXXKtZusrl6gIc3By7Ec7cpUeLYmoqij9o9aL7UGS4JvTLlV67Ku6iw6x33FEtRKL7KVEVC+Tl9VhsbgiRiTM10po5MQyGm9NgAWDlixLXYksxJO4HZ1dJhys9lk6ty2MaMvQxH/AJCqn/ugeTZW+YMw9SkdPr3SXQfqNT/eZD7sw/OVLTsbEacvfuJTgwdLl75X+6RozZupR90a/lmPWnrYy9Tof2P6yW2HhlsJujirkwyyXwW6VPXQXPYJmsPwTHKf2aMhZSWBYIclypLK266Ht5abSV0epLTp+uIQ1GJVFdSwKMpUsNgNSQfauNLCbFgOjtWvTWoXUIOqpqM5zAdXqqBoot8JztTrG7jGlFctq7/lbF2PHVN8+45zjsDVpgF0ZQbZXI6pDDMLHY3GsgkzonFMA9JzRrqr3UIM7NlRWdSroy6hbry/dA8NE4lgzSqsmhAJysCCCtzYggkfGe49Q5vpnz7uGiagkrRFAl3DbyjLJFOlpfYgzVCLbISkkj0Hczxx7PnPaotceZ94Ah/aUfXISTPDqXoa6QWL4NzobvT8fvr57++dYny7gcY1GqKiGzI4ZT3qQRPpXg3EVxNClXT2aiBh3XGoPeDceU5Wrx9Mupd5dje1E2IiZC0REQBPn70lcU+0Y6qwN1RvVr4Jox/mzTt/STiYw2FrV+aISB2tayjzJE+bsWSVBJubkk9pOpM6Ghx31SKsr4QUakdo+vnLOJbqKfI99tLfKXqm6ntW3naWMW11P8w91/mJ03wyhFIPmCNDLtHa0sZjYHlYX8tL/XdJNNLgaWkVHqZ65dJJo0NdfI/ke6SloE2CrdjooHMnQAS3SNhJvC8TTFQM7OgXrBksWDDVRYggg2tfkSOV5odQiZbc2bHRfFUKQpYdzTUtc51p0ywyZ2u+W6MQbAntG1pJ4t0vq1QqFkRM7Uz6oMalNgGyGnUJJJJGW+Ub98xmFxNN0JVPWIt1zV6hy6361mLFjbLYZertreQa/EEUFfWqi5vWD1IZjnzZst26troh2+9btnIlHqlbRtiqVEetwRaikIjmuShZ3chNVJckvY2ulQajcA3tNaaZHG4wsclN3FO5IQ2AuRY2VAFFxytzPbIfqTe527R85fCEu8NpFfD6RLG3ID85kKlPtH6eUjcOTrt3W8Dv7pka9tJuxxqJlnO5EWwls8+6UvUtofI9vu2luq9/Ht5+c8lloRxtmwcIqg4X1YexSpmFHLfMXzMWVgSbBRrdQBzM3PgXGKHqadKq60igIDkGzre422IvY3nMOH8UrYdxUpuVIIJFzlYDkyjQjf3zM4TjeGujE1aJVWVmHXqVC2UBhYADQ1CwsPu2nB1WmT6ouLcW729vy359l8m6EmqadNGc6W8Qp1qier9lVCZybBmLXJ633fdvNQ6RkHEupCgqAjBfYuosclwCB5b3NyJLbjdKkoFEFqhpFWZgppgt+6rC+ltjvnImAJLHOTc31J520v8AC1pp0eFqaklUYqlfL4/0Qm6i7e7KhRsT8O7u8JWouR8fASpDpeWPXZQW7jOx2YmO3Itk3zH95wB4A3P5yqmb1PAD9fzkfBjqqxOgufnf8/hJGAG7Hcm/5zLHejQ9jwm7HxnYPQpxnPSq4VjrTbOn4HPWHk2v+qccw+p95mwdCuMfZMZTrE2TNlqfgfQ38NG/0yjNj68bJRdM+j4ngM9nHNIiIgHNPTRxa1OlhVOrt6xx/Cuig+La/wCmcqrr1Jt3TGj9sxGJxKuQtMlBmBGZaVJndl7F9gDe5qX5zXMZgalOmDUQqCBYnY3UMNe3KwNt9Z29KlHH095lm7dkBzemp5jWWHPwPwOv6y9SPVt4j85Fc2I935j8xND4PEMK4FMgnRdx220/L4yThL5VJ002mKxJIuAd/mNbedvhMlgWvTGt9Tr8fznmCXb6fYiGZdkyAbaWMStjcaa/H9ZQ1T9CO/uMtGsdjrLss01RXjg07Livzly95CapaBWJmRmkkuLajb60k1HGQn68DI+HTq35beB7COyU4lraDbaaMcWtyjI09iTwuwUnTXWVYuoGA1HP67xINOvbS+wHy+U8r1CdRoeYHzE9nJUeQg+qy2KhNwfKVB5bAnhmZs00XM957Uo6fWktU1vJlO5FjuOf5GWQj1Fc5URqdMEfX1/cS6dB38/HtnqSPiKtgRzl9KEbZS25sqep1dJj8VW6hHafjLgeQaurgeZ/WYs+Vtbd+xohjSJ9MnKKfIn4Df4yUWsp8D+gkfDNoTzPwUS5U1sv1Yf3Pwk1xYZVhU+U2bot0Qq4usabE0RkFS7obshOUFV0vc9s1/DjQzrfRXiyrg6OJq3NVKVamGOmZabBshPM5VuPwtKs8pQguk8W7Nq6C8TSvhECsWaj+xcsLHNTAB07CLETYZzvo9xbC0cdWOHqGpSxLqWK2FOlVN9r2L3uNVva5vOiTl5Y1LxNEHaEREqJnzrg+kJPUxKs9L1fq7JlR7BqbXLW61xTVSTrYTaOj/EalX11U1aaZi5ILL+wAAdSFf26TZBTYDWwE52g1mSygid/7CLTox3RjGq3LGwHWzWGgFzqAOQF5YxCXBH14y7VFj7wfOeU9fz8RpLK7j0hV1zre+o0YdhHP3y/wo/s2GxDn4gX8RIeIY02zDwI7uR/KZLCBDQR1brsXzr+4VICDvutj590pxyX2qXfuJq4lDvc67yfw3hvrgSCbg2sAOwG5JYW375jM3bM30Zr2Zhfmp8jdD8XWVavJOOKU4cpWaNNjjLLGEuG0iNV4WFrU0Ytldgp2zKc+Ujst7Jv2NMonAEyZlGpAIuxJBO3IA66HTnHSSidHG6sD/MLfOmv8wmdwb5gBf2iSPA9dT7mE5WfWZVgxZ4+3tfXyOng0WJ6jLp59yfT9PNGJ4XhUKElQTmA1zWHVJ0CsNfGY6pTX7VRUKtsy3HJh6xhqCTrYDSZ/wBXlY2sAzEkD7rWXMLdmoI7mtyMwC/5lTzAVvH9nn+c2rVSyamfTLs9KaXiYpaWMNLFyj23Jp/Lu/c2E0KYUFicx10Ud19FXbWWqnDaVUHLlY+CqR3XVQVPiCO47S30nJWjYEjRf6x+kh9FsSzGxJNmC6knR0qG2vK9MHzM5OOGZ6f/ACFkd7uu7ZnVySwLU/47xxrZWtnujEcQwhpNbWxF1PO2osexgQQfDstNobhNLNf1aW9bly5BsKmW199ucj9J8NmAYaEP78yj3f4fxmX+92ftj/1jNWo1E3hwzi66mrMun02NZc0JK+mMq+XBoVOj95Tp8x9fGbFwvhqsgLLcsLjUiy+yu25JDeQHbMVgMNmKqDYG1zyUWuzeAFz5TaVvYBAAzeyG0AAHVBtsAqgeXfOj6T1E8EIwxevJ0v8AZh9G6eGonKeb1Iq39EanxKkKdXINNLjW/O25mLxx1BmW6V+0jjZh7tNpgqjkjWe6bVSzaeLlz3+K5IarTRw6iUY8d3g91/BSp0kamt3PhaXxtI1M9a1/Hw7J5J7ogZKkwtYbnfs8BLtMbt5DwH1eR1HLyHd2yfUWwAmtFTPaQshk3D8UZadJczk0qudFJvSsbE3XtvfyY6yJU0UCWYkk6PCY+MqMXbORnbMwBsCb3Gg7DO/9CeN/bMJTqk9cDJUH8a6E+eh8588CdI9DOKqrWq08jmlUW+YKciuu122FwSPITNq8aljv2E8bpnXYiJyDSfLVPeT6O09ifSxMTMZjOfjPKW7eJ+QiJF8npjuI7HwPzlXCv8M+J+QiJk/714Fn/Avn85P6P/4p/Af60iJ7qPu5eDJ4fXj4rzNg437Lfh/3KUyOB9mn+FP+gsROJj/LI+M/6yO3l/NJ/o/tAin/ADLf8Nf6mmJf/ND8C/8A1xER6O5n8EfJkvSfEPjn5oyfS7/D8l+cx/RPc/jT/p4iIk8H5a/BlGf8y/VHyRmOPbf60/oqSe3tf/L/ALsRI5Pwem+JHuL8XqfhkaxwPc/8Fv6RMpxj2G/B/uUYibfSX4/D8zN6O/AZ/wBJhemPsr+Nv6nmtcoiNB92/il5shr/AL1fDH+qKV2Mj4f/ABD9dk8iaJcxMXtMlS9oSbU3iJtjwVs9xG4lBiIfJEuD8p9FdEP8pR/CPlETFr/VRbi5MzEROWaD/9k=</t>
         </is>
       </c>
     </row>
@@ -3044,25 +3044,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DHRUV JUREL</t>
+          <t>HARVIK DESAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>smat2023_127</t>
+          <t>smat2023_078</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>144.4</v>
+        <v>360</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -3074,10 +3074,10 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" t="n">
-        <v>55.6</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -3110,10 +3110,10 @@
         <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="X21" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -3125,16 +3125,16 @@
         <v>0</v>
       </c>
       <c r="AB21" t="n">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="AC21" t="n">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="AD21" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="AE21" t="n">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="AF21" t="n">
         <v>0</v>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="AM21" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTExMVFhUWGBoYFxUYFxgeFxgWGB4aFx0dGRcfHyggGBolGxsXITEhJSotLi4uGCAzODMsNygtLysBCgoKDg0OGxAQGy4lICU1LS01Ly0tMC8tLS0tLS0tLy0tLy8tLS0uLi0tLS4tLS0vLS0rLS0vLSsvLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCCAH/xABFEAACAQIEBAMEBQkHAwUBAAABAgADEQQSITEFBkFREyJhMnGBkQdSobHBFCMzQmJyktHwJDRDgqKy4VNz8RUWY4PCCP/EABoBAQADAQEBAAAAAAAAAAAAAAACAwQFAQb/xAA1EQACAQIDBQYEBgIDAAAAAAAAAQIDEQQhMRJBUWFxBRMigaHwkbHB0RUyM1Lh8RSyI0Jy/9oADAMBAAIRAxEAPwDuMREAREQBERAEREAREQBERAESE49zVg8H/eK6IbXCbufcguZUK/008PHs08S/YhEAP8Tg/ZAOlRKDwn6XOHViA7VaBP8A1U8v8aFlHxIl3wuJSooem6up2ZGDKfcRoYBniIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIBgxmKSkjVKjBUUXZjsBOO83/TWPNS4egJ2/KHBsNx5adtTtYk212Mi/8A+guZnaumAQuqU1D1RstR2syfvBR9p9JyqiMo6Fj9n4wDfxOKeo71azs9RzdnbVie56+npawtMKt16ev/ADPNKlvcFj7tvh/xPFSp0sQPdIkiRwLXvYWH4fPWTHL/ADHiMDUL4arlF7sjAmnU9GXbbqCGHQiVzCPr5SRb7fhN6te1gLk9yPt6T0M+neUeZKWPw61qZsdqlO/mp1Oqn8D1FjJ2fLHJXNVXAYqnVDWRmVKy38r0idb/ALS3LK3TXoSD9Tz0iIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgHyz9LdB/wD1fFAjVirAZgfLlUD3EgZrdLyK5T4EuIr5GN1AufXpadI+n3AZMVhsSF0qU2plumamcwB7Gzn32PaVv6PsE2Vq7EBbkL6m+unvlVWWzFl1CG1USsXTA8n0FXYbTBxDkui66IL+6WHBkMozOFPa4vJTD01A3vMVnc6qscaxnIjq35sE+lpXuOU3oMEdcrdVYWP/ACOxn0ctj2kTzJg6dSmVdVdSNdjpL41pRWZmnh4SeWR82VKgPbrp759V/RhxVsVwzC1XJL5CjE7k0mNO5PUnKD8Z84808vHD4kUqYLLUF6fUsTplHc3sPiO8+k/o74A+B4fQw1Qg1FDM+XYM7M9gets1r9bTTGSkro58ouMmmWaIiSIiIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAcr+lTG/lni8Op0gxpItZqp/w6muQLY7lSQTroxlX5fw5p4FLqboDoN81z9ssnPfDmp45nVmRMR4TVHX2gqBqTkdfIMrf/ZfpMvKiKadO1rWB+cwVZNys+J06UIxipR4HN+I4PEO6HVS4YgkPpl6E2tc66MRttqL2nkEVjrUdwNspN9pd8Zw2kxuUX5bzSw1BKbgIo32Fuu88qSurFlOnZ3uVbnqniFJ8J2Ktpp0/r8ZFcu+OgR3NUhzYqyupFrXuWsSNdyADY2JItOo4nCJVbK6gjS1x1AGs2KOBpouigf19k9jo0JRW0mc34jhPDxmHr+H4qYRKtfJ0JBp5f4SQw/cnb8NWDorjZlDD3EXnMuJUSahVP1qdRLdDnCqot+8R9s6bhaORFT6qhfkLS3DSbTXveZcXGKSe93+SM0RE1GIREQBERAEREAREQBERAEREAREQBERAEREAREQCK43whcQq30dDdG7E6H4ETmtKk9CrVosRdKjWsdMrHOP9JE6/OWc+VfDxzdPEpo4P1iLofllX5iZsRTTW0a8NUakovQ3FxjFD3/GQFfjfgVAAaTEak65sxvv+rba00+JV2emKaH2r3AvqenuE/OF8OqooAfDqTuppk/Njcn5W1meKvqb829mJZuE8e8drs1JRbuc2ba2wG17ySx+MIG+n3ytVuFVCls2HNtkFNl27VAB+PqJ4w+JZKWWpe6kjU3PeJqyPbOMrMuHJ3D87NiHtYMFQeqg3Ppq1vhLnIflTDlMJRB3K5z3Bcl7H3Xt8JMTbSgowSORVqOc2xERLCsREQBERAEREAREQBERAEREAREQBERAEREAREQBOZ/SlgvEqKAcrCmpVuxzPofQ6fISf+kXmv8gwxZMprvcUlOwtu7Dqq3GnUkDrccq5O4jVxFF6teq9Wo9ViWc3IGgyjoALaAaC+kqxCap35mjCpSqW5MjqPEHWoFYFXHT8R3Em6uCpVwuatqd7D/mOJYNH0Ye49QfQyq4nBVqbHw6lwe+/2TInGXJm1xlHLVF2wPDUwysUrXsNL/8AkzHyzhWxuMRH/RBz4h6MFBfIO97WPYE9bXhuC8v4itY1qoVb3styxHx2+N/cZNc30RRwZWmSgQoVIYhgVdWFm3zE9b3uZOGztpX1a+ZGcZOD3WTO3xKn9H/Mn5ZhwKhH5RSAFUd9NHHoevqD6S2TfOLhJxeqOYncRESIEREAREQBERAEREAREQBERAEREAREQBESi83/AEi0cKTSoAV640Nj+apn9thuf2V7alZOEJTdoo8bS1L1KjzNzzQwtRaKjxarXJUMAqBfrvrZj0Fj62nIOM82Y7EZvFxD5d/DQ5Et1FltmH7xMhq1KocNUqorMKWQ36ItyLH56Ae+aZYNwi5Sehdhe7lVSqJ25E5zVx98bXao4ygDIqA3CqL9epJuSf5SE5exxw2IKH9FVNx+y/8AzPa4VtwrO1r6ez7ydt5jw/CcVULGqhQL5lXKNQDYkddPLrf9ba0sxNOnUp9zv3cnzeiJ0qFeD75Qez03f0Xd1DajWa9Hh6Frt0kpyiiulr3Ybg7+/wB0sVTBJe+UT5qcJ05OMlZo6kZRmk1oR2FpEDygyoc7Y7PUp4YHQfnan+X2B/Fr/ll+xWJp0kLObD7T6D1nPqHDW4himq3ejSHVLZmtooJOmup10GncTd2fQcpqq14Y5+e5c8yjES2l3cfzP5b2/Ij8JxtsLVWrSY5xp5TqVNrg9De2x0uBOmYT6S0R/DxCkjJTcVEGpD5hcr1sV6d9pRKPKNcVBnqK1O+psue3rYWBkYeCVjjKqIudUoglhoDrfS51O4sNZ2pypVpK+XoUvBVqFOSlBSvo077NumeaPoDhPMWFxP6CvTc/VvZx70NmHyktPlIVCBVB/VdCD6XGo+Ut3Auesbhf8U1aYJulW7Cw7N7S+mtvSQngHrB/H7/0cxVOJ3+JT+VufKGMOQq1Krp5G1UnstQaE30sQCbGwMuEwyi4vZlqWWdriIiRAiIgCIiAIiIAiIgCIiAIiVr6QOMnC4Ko6m1R/wA3TPUO99R6qoZv8slGLk0lvDdlc599IfOlSvVfDYdylCmSrupsarjRhmGvhg6WHta7i0oYo5SLWynT0U9PcOnYb956oHLYbA6A+vr/ADktgcH4hygkDqSBYe/Wd+lThShZe+ZTGMpyss3w9++hl4ZwQu9m8v7JIvl0ux+qo216ywcP4VSompRQnJUVmN26jKLe63e+59J+8Cq07VVD56iKLttdVuAe/oe9gb6zffDt4mY3J8w+ak+1fe46TlYmrKTsz63AYejSW1G1888m724r4ZZZb9TW4Rw5VU3GlzlGmYi+gFu506ibajJVQhblgR5elrW1X01II3Ez4MeQXIvruBpc31tsbzzi1IemxNrNuMxJ9NPMBY31vtvMzjkb3Vc6jT5rfwIjjPCXov8AlGFPmGrotviUtoVP1fs6TLS5yU0blT4m2UeyT3zdB/Wsmqhy3INzrbQH8byMThFCpUNRkVWGrLmspP1slvN10BF76g9b591VSjXV7aNa9Onqt1mcWpg6ie3Qyvqt3VLd5fPWLwOCq4wmpVbLT2vrYDqEH4/fa0siUlphKSrZB7Og1ttmF7XJzHzHpPdOuctv1L2XTTTt0/lAABbUkBCdLafPTX5z2pV2kklaK0W40YbCKi3fOT3+9On9mIjvqtjY3Hlv0NhZRfMbi9gJrcNwoSu7MpuRTAIFyb5/rXsbW3kjRw7hMxD5OpVXyHyqS17ZchFhcWHl1uBeawoZnJ1YXC7nooNr6aebppKWtDVTrxmpKL+D5+/vvIfE8AoOayMmXxEYFhcWJNr2ubkEg6CVWpwlgrMdLasrWzLcZipsdT0nScZh1DFvJt+qSV1Oba911H3SG49hELLnQA1AGzZTvbLqw1t5V1v+M14WrKMrP7mLG0KdaF99ss9m3p75MrvLaWzg76HfUkXv9pnceE1s9NDcsMq2ZrZiLDVuma9wbdQZwst4dS65TlPS5U9DYnp0v8vXoPK/NjVq1NPIqaoUVbXJuQx9c3aw8xlfaFBwq98l4ZWvyemfDKxzaT/yMMsPltU9p9Vq7cXe6suT5nQoiJjMAiIgCIiAIiIAiIgCIiAJzL6YaVap4CU0d1QPUqZVJAvlVS1ttPE+3sZ02QfMWJyU6jKQHVBa9tMzZQfnf5SE68qFpxSbulnpm7FlKi601TWryPn+mAQR8xJvhOPsppF8mhtWYkk/s5Oh3seum5tex4zAs7WqorXZlXOdbgXy03Jz302U3012MieZqAWlSy0iAoIarYZewRrC5IAFswvbvcmdeljIYhqDi037/g2VMHUwTdSMlJaO3Pc/29U780YuCVCmLQG6iqHpsrnzHy59ev6unv6dN/A492dadOtR8Si1VGastTRUqGgjeInlzElFItrmY3AFpW6WN/OUmNy61EHiMTmKk5LD9kBib3uNRrm0k+E06lPEO1JMMSatUuamdj5nWolqXsJlJ0OpNpRilaeevv7I0U1XnQvh23m9NyavZ6Le75eb1dlprjRfNRomqS+WmayrUqeGSG8Omb51BB7baaanQ4jxaugql8OL0fDLlavsCt5qYGl7eaxt31m7h/y4AFjhWqqXNKu4fxU8UksVIGUi5JAINie094inimz+JSwP50U8xPi2c0fZ2axYab2GkosytTxye/0PTVMYHCthAzFEqDLWRLBmKgEta75rLYa3tobzNwrFeIjVCFptmZSj+YhgbaaDz/8AjpPf5fxBSWYYdzckMMwsGZHK6AC3kFifNqfNfWaHDVemlUNmXO5ICsX0cAWLHW1wfMdRuTDvbM0YJ4iVTZnp5EuFChLg9xmOnXXL29d7++fj075g1z5DYgC5HTTUAmxNz+MxGoDZLajruT0sAN7duukz5goIuNdQCbW3u19dbX1O0R1yNlWWzBuXP3/G8kTit9GNTxFpZwKmYlj+kWxy5N2C3ylQB1tI/A0QEFrWIGt9Pq6AHW4XQ9hM9Av1KhboQuclDTRGQqTYe1nBOgGs1cTVyXFwbWVbkEgfC2uhvpLGkkcfs1+Nw3v6e78DxxTEp+bUMt2qKuigWUeY+h039Lyp8e40fHZFuCoyEKfLa12UDoc5IPa3qJL8YxYFSkXJKUUq1mAXyjLZQFtv1+M56K5NydXckm3Vicx92pJ+PrrfgoKc3J6I19qVnQpQpwebvf425a5LpdE7wnhzYmqtFCqs17ZicugLHYX2B6Wl04LyRTBSoldjVp1Ua+UBPI92UgEtqEYXuOmhBnPcNWdT5SwY6DLfNqRt13tOs8G4oqM61PKWRa1VXCqVrNZHuoYhCy2e2bTN7wN2K7xp7L3aLrnflnp9z52Nlr74F1iInALxERAEREAREQBERAEREASl808RyV2RaIqVPApsGe3gj85UAzrfMxBBICgne1pdJROc2pU6pq1Hyllppre2VC7XA1LWLahQTZjIygp+F53tkt+Zfh77WtlZ36f3Y53x/BYsOFr5qn6wKq1sz6/VBFTrY62II0IMncRwKquDdjiatQZbmk6AG60xiACSxNtLW01GsznnOgjgpm6ElRmTMAysWRyhbOGIPs2CrvbTwnOOGPkanXtakL5UOY0wUPlz+XNTYra56amdDaxTjFKna2eiz8noy5wwkZSbqN3Vlrk3betUl1vb488xVQ2LL7S+YDbzDUfbLpgscGeoQFI8YNtYHMlN9Gtre/Xt0uJUaqXP2X7iSvKV6jZfEIP5hMpFwQKjUCR6i9H3i97WvL8fTvZrn9zR2NXhTc+80yfT/r9VcvZqLqzaKNe17am3TN6RTrEtfW/QAagai+XZri2on6eBVamIqYfxkTwlpvmFJir5i1iU8QWI1F7m9+lp+8vcBq1aWcVUTUqt0ZrEaZgc4ynNcW6WmN0ms21u4781u3m5do4VwvtO+mj99dzyW/PMjj2RsNyD5RfUDby3IOh2M1OIUrmmB1qAXUkeuo7aaj+c3eH8NqPhPyjMFur1MhU57DMbMwIve3bS8y0eDvUag5ZMrXbYk2CnLcAgN7/dE6LSd7ZZdLEYdpYdPaTfweeTt8edrb8szRfLmIPQ2sAb+n9fOKbm+nldb5rWtawBJJ0A1tYX1m5U4USuIdqhHgM6hQoAayq4J7EhvlNvCcADpTetVKM1vDUZbD9YKQw8xsL2Hb0nsqbi7tr14X4cM/ecJdo4aUGpXa0t9s1ldb7ehFrxFl1LeUnViNAxLkm36wIZ77e1paMRiL5gwVfncZiTtcnU3NvUzbwXAvErVqT1GUoBdltdw+oJzA5QR0HqL6TUo8PZ6GGKN567EBSosqjOxYta/sgfYJPu5W1W71TfTRN3uVxxWAhNOMbPjbpfzWjVuiyd6Tzjimu6XOopUrWtlUA13t/EoP7xleoISdBqe2/uEkMVhmxOKqBCaj53y7BcrN7ROth4a0uvXrLZwLgHgg5qgzNvlGw7An+UlTxdLDU/E823l73FOMpPE1072jZZ8N9rZZ3en9FRSnVpstQBlZWDKxBADKbggkanS/w6y5cL54zvTp4mlSWmXUu9JWDF8wsWAbzKQWDLrcMdOhkcVwOhVAzlzbbzd/cLdpGvwVKSsqeYE3Kvr6aMLW9DaeS7Uw014078fbf1M34e3O0X4eL180ufA6/E0eE4rxaFOoRYsgJHZraj4G4m9MJkEREAREQBERAEREAREQBOG814c4riGJqZ1VEfwrk6jwwFIA7XDH4mdynKkwKU61ZsoztWqMxOpBLsbDsBe2naSjiVQ8W/Qvw1KNSfjV0uduhS24PVzFURnHRlViCPf0k5guWlZAXWsrdRYb+nl2lr8WefGkZ9s1nkkl8fo0bqWDpxk3a99zzsUDjXBXom4VinR8p09CbWBmvys5w/EqKMBZnT3ZXZbH3Xt8SJ1I1hlnGeK1weIYjKQFUZFANj5SKnlP6pDra42taXw7RddKNRWtndb/I8hgrylGlrLJLcs09eGXN665HecLSYcQqtlORqFPzWOUsHfS+17HbtPPLFTJhcN18Rj/rNRx+HwlO4TzLjK+HRiy+GwyM+S1RmsNEOaxci+y6dxcGSeF4lVp06VPPRPgFAiZHRiApQBiXN9Dc2A2B2Mu7yEoNOS3bnuTXDW7MVTA1oT2LJyzy2lfOz420535Wabt1gEqUF2p0VHxYOPuUH4zR4U5/sI74dif4KR/Eyv0uYKiVKpyoz1it1OYBCqhAAdcy21v3JnqnxZ6fg2KhqFHw1BRjmNkBvZx5rJftqd9JNbKi02s+urhJPd+5nr7Mxl1/xv4rS658CwcSqB8HiKq/4lM3A+uB4Z+PlA+E88cptUq4NqYYpnzXUaAZqTi56AqrSvDH1Uw3hjJ4bk3upzXPmIFmsBcE3I6zJhOP1qSBVKFdbZkYso10ADDyA2UX290824xfhaybte+jSWeWqt9OF7Y9mYqzko8tVzu1n/OmTzSsmHqf2rFEbrTojTe/51vuIkB4z0lwOVWsmGc1P2BUFMBj9W3mPwtNTB8Tq0nd1sXN84bUOb3uzCwBGtgu1zpbatc6cw1itdsyjxadKkwGllBYlVJJ1PiancjtCqxjfhl6RcfVN+Z7+EYhysknq73yzs3zy42ztlfQh/o1qD+0G2t6Q+AT+d5cTWnN+QXqo9a9NwrgENlbLdSRa9rX832S31atTopvOFXd5tm+LveXFv1bZP0cXeMW1xIfAYepuT8B/OSOKOVbGU2yJF75Pe+Ep+hcf6mk3K/yN/c6Z7mof9bD8JYJ0KX5F0RxK36krcWIiJYViIiAIiIAiIgCIiAJzLi2mIrD/AOVvtN502cz4+v8Aa6tv+p96qfxmfErwo14P876HhqhAmA1TM7reYsswyR1Isx1uIgIT9Xf4SK4Ph2qguFFjue5knjsClRGUkjMpW43sfvm9wXLQpimbtbr/ADEkiMm+BGJUNA1QKAJSndWV6aKpbNrkZgc1hfMBrfqbyRwKmrRp2sxsGepYLZ21KoOltL+unSwo/wBJHEfz6MAy+TILqbE3JsD13O0kOC88qaSJlAyi2+h6XHofvvNMm9hNGGLtWe0y2ikBvPYA1Hffpf3yBTmumfaW3rN6lx2i2xmdOS0ZsUluNyrhwwtrbtc2+UxHDgCwvY7jv7+49J+rxBDs0yHGLJd7U/cWqtPTafxZrjDCwFtALAH0ntMCo6Ae4WmRsYogYsSLcpas8lVlLV+p5OEF56FEdpjbFzEmJN/fPNmxHaZvUfDHoZHcTN7gdBNkUQ2pIjHUlSmbf11kmshF5l25Sp5cHQHdM38RLfjJia3D6OSlTT6qKvyAE2Z0IqyscOTu2xERJHgiIgCIiAIiIAiIgCc74+tsdU9Sp+aKPvBnRJz/AOkC9LEUqvR0t8UP32YfKUV14bmnCytU6kTisVl2F5HnH663+U2xVDC9xaamLImJs6iR6/LB0DTMuMe1got7lv8APeRIqp1Y/OZUqINmhZHt7khVcsLFLg99RKjxfkw1n8Slmpset9/hLPSxSDr9s204nT7ycZNaEZxjLVHP6nL+NpDdag+R+e00U4sabZatNkPrt8xOotxGmd7GRvEVw1S+ZVja4lcqSemXqVjCcUptsxF+oNxJKmL+xW+DD8ZA8U4NQBJpvlPpI5MSyHRi3r1hxRQ5uGpdRSrDdgf67zZVqoG3yMpmH5jZdL6dj/Wk2P8A3Keht6Hb5yLiySxELalrTioU2e/3TdTiCkb7Tn2N46W9pfj/AMze5d5ax+OJOGSyDepUbKlz0BsS3wBk1FvQg8XBaZlzpcaQepm5wes2KxVKnuua7DoEXzG/vtb4yFp/RZxTMCauEt1/OVb/AC8HWdK5O5WGCU5nD1GFiQLKq9l6nXc+g0EuVGV1ci8WnF21LPERNRhEREAREQBERAEREAREQBK3zzwlsThWCLmqIc6Abm2hA9bE/ECWSJ5JXVj2Ls7o+bScWjELhsRdTqPBq/aMsxVOamUlXUqw3VhYj3g6ifS81Mfw2jXXJWpU6q/VdFYfIiU9wuJZ/kVVoz5ofjgfoP5TX8dulS0tfM3LOGRrLSs2oIUtoVNjcXsuvw+Oko2OwwTbN1sTe2kg6LR0qmBxMVtOzXJv7IkFqVD/AIo+2bCMw3q/ISseI8/RnOhJPoO/aeKlIpjSqt2t6stQxyrvUPznl+N0+9/67SK4fwXxNQbjoTsTpcfAEHv6Sy4Pl4A5gGHcLqbbad5YsNxZ0aXZ1WavJpEJW4yjeyhPwkdiMUzfqWHeWupy8tywUp0YX1U9NOpMzVeCfVCN0VwdCQAdNrtdrX20k44eKNH4TB/mlf5FEAc62A+E3cLhGbe1r/L3+ksg4S4vlpgWvdbg3yg5iL/rAX122G8yU+FsNQygE6a66XHs/A762HrLFSiiyh2ZSg80jLwvhaC7EWGXMpygad7jpYE99Lzr/IdPLSe+hJXS1rC3y+I0nM8LQVchyg21vcsR0u19Ba2g6idP5JokIzEAXyjQW2ubH1F/tt0k7LcedrrZwrjppl5otEREgfJCIiAIiIAiIgCIiAIiIAiIgCIiAIiIBx3nj+8Vf3m++c54h/L/APU/YkUfcx/Rj0XyIun+D/cZsYff4CInqMVPUn+D/om/7i/cJa+Xf0v+YxEnE6K/Rfn9T9xn94/y/iZo4Tr+4P8Aek/YhlkPyry+ps432R/2vxn7U/TL/n/2iInp6tPJ/Q3eH/oan7yfjOh8n/3RPe/+9oiRlojidtfpP/2v9WTcRE8PmBERAEREAREQBERAP//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUSEhMVFRUVFRcVFRUXEhUVFRAVFRcWFxUVFRUYHSggGBolGxUVITEhJSkrLi4uFx8zODMsNygtLi0BCgoKDg0OFxAQGC0fHyUrLi0tLS0tLS0tLS0rLS0tKy0tKy0tLSstLS0tLS0tLS0tLSstLS0tLS0tLSs1LS0tLf/AABEIAPsAyQMBIgACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAADBAIFBgEHAP/EAD0QAAIBAgQDBwEECQMFAQAAAAECAAMRBBIhMQVBUQYTImFxgZGhMrHB0RQjM0JScoLh8AdikhZDorLxFf/EABkBAAMBAQEAAAAAAAAAAAAAAAABAgMEBf/EACsRAAICAQMDAgQHAAAAAAAAAAABAhEDEiExBCJBUWETwdHwBSMycYGh4f/aAAwDAQACEQMRAD8A9G4ULUx6QjGL8LrA0x6RgzlvYdAqhilZCY1VgzENMQZSI1Qq2Er1xud2UAjKSNiSSDbYbRjJbkfc2+gk/ESNFib3Y13gMHUEGF0zDrY2FvS8mDKTsiS0ugZpyNtYdoFjGIapvpOhokWMnRqQEMMt4FqMPTMkxhQCiKQY93mkVqSDMYBQ7mgnS8HTqQ6GAC5pxbFUSR7x9oBoDolw7w3lgTKsEiOUqmkBBCkiyQqSLwGIV6FyJ3uIwyzmUxBRi+z3aQFVW82+Dq5heeD4BilRW1FjPV+BcXXILnlHNaeBrc0dSQtAUsWHOhhxBCZW11K1WtsQG9/sn7gfeMKvOR4gNVbocp9GH5gQtI6TNrc6IPtPgLgjyv8AGsArxynobxStSsSJUTPIEV7zjLA0RaHDSjMGacjkjLQeUwGdptaHpm8XKSVI2gSGdYFqUKKsm2sB2J93Cq9pLJIVBAAqNOEXgkaTSprADpSRhHMitOAwiVrQiveKssnTe0BUNkQeScWtJ54gs8eqqtoqMcyfZaGqIII4O4mi25Kbs1nY7iZYeI6zb0nvPG8Bi2oNbleem9n8cHUayGqYiyxiZlYDe1x6jUfUCRwr3UHqAfmMiLYVbXX+Ekex1X6ESZF434GVWBxqnQ9R9RDyVZLp6H74IqRWBTOlDGgJB1jM+TqNpJoYvlM7SveBIWosCaRjYkyIDsR7sxhX0n1RTAFTGKhhWg6q3kKWkOIAmLCgZ93djGyYGoIDe5zvISm94oVMnRNoCDush3cIGvCWiHYC1oTPPnpwXcGAUjymspvC06lhJNA1WAlvcadCeJa5OkNgO0L0NLG0+QAmdxGFW0LS2YVe56B2c4v3qgnnLkv+t65l+qn8mHxPKMDxo0NOXKaHgXalalekp5tb5BEiUGOMlZ6GohkW4K9QZCms6h8XoZCNWrFlE7UEYrU7MfW/zrMd/qNxc0qa0UNmq3LHmKY0t7n6A9ZrGOp0c72IY7tpRW4pK1Q33PhX1vufiVmG7TYuo7GlTDDTwBCVX3Fjc+ZmOWpNz2Iwv6p3DMpdsvhqEXCjmBrfxH5l5pxxQcq+f0LxY3klX+fUew3al6bKuLoGnm2YA29cpvca8j7TV0aquAykEEXBBuCPKZ/ivBRXoinmbMv7Ms7EKdBtyFtNBKvsNj2WpUwrn7JYr5Mps4H3+xmGLLHNFtcr79ysuGWNq/r8kbd1gXpxgGTtpLM7K3uzJ0xDVIEkwBkwdZ86wIJvGM0BWKvTMhkjjbRdgYDPqbWh6VSKFDO0QQYCLEzlpAPJ5oBZ5ZWpAROvh7x2vhz1MXekYJltCJp2g61UxishidSmZZIpiFvIUWNNlYbqQR7G8ZFA3gsThzKvwTR7dhuJKaaPfRkDX5DQbnlvH6LlgWIyJyLGxI/iI/dHrMR2O4ggwgq1Aahw4sEFtgwGex3sHTU3traWmM4xi8SjU6WGyo4KlnvqrCxsTlHPzjxdM5x1bJLy2kaTy00vL9jVBg9mVgykeFgQQbaGxG+oM8r/ANR6T1MU7geCmtOnmuNyuew66lpq+xlV3w9bDscjU2dP5DUUi4Pkyt9J5xx4VkapSOgpmm+QeFWDAhm13AdlWTGlJomSezFKOHJOgJ9ptOw+NyXoMAtyXViwGtgCvwL78pjMDxSqy3WyW0+zcyT8TxIIBc2P+wfB6f3k5lHJFwZtiUoNSSPWqmOQA/rqdxrbvRqRsN559h8a64v9KWna7lyl/wCL7S3tzudbc5QYuviLjVhfytp1GkR4lia1LJ+scFr3uRcAZbfVj8TPpsMMd07srqMk58qqPdOFcSFeilZRYOL2vfKQSCL+0sqbXlP2ZYHCUTfN4d73NwTcE9QdPaWa1LS2cwbJA1RaSp1rztQi8AsScyBqRuqoEXcCIbJI1xCIIoKwGkLSrawJ4JVBBEmM5wZxiBBjsAGMLnnz2nM0YqMzxLAZdpR5ZuMTSzHX7pS8S4da5kVRpqvky1RRmtE66gMJYVqfii2JpajSWmKSBVlA1nMQgZfa8NXXSQX7I9JZJdf6fYru66jkxyn30H1IPtNbjuNV6tZ6eFQNkOVnbXUXGlzYC9+t7Tz/AIRVyMG2136XFr/WbduGVUdsRh6yU1q+Nw9gFJ8RFyCLAk9CJr06xapKdXXbd1fvRU3LRFx8c1zXKD8N4riaeJTDYoIRVBKOoAsdd7WvqLbX1EyXa+koxFMXPehqtNlyXWrTLFyGNxaxd/axGomhSth6NYYjEV++qAWQIGdV0OzaA7m21ryPa+gnfq+VSayZqTFQ2WoQAGUcmBCn3HlbPPBwnx/VL+EODUo8/Mw/ZyvhxVdEps2psXqaNruFVRb5M1lQUAAuSkGbRb6+I/Z0Y8zp7zGYurRSuarGqGOUOq0lpim4QKb5mJAYi48PleWSDC181cBnYaZXrhB4RpoF/GcmSHdfg7sM+zT5L3A46lWUBEpBkHiBSkTc9ARcWt9ZRdonr2buRc5kp3RFzZnzOEAC/wAKr/zPXQ/EK1FQK70k73MpuKlW7sQDfwsOflr01mww3DjTwufZ3HfHLsXsCh1udAqDe2mwEWNU7RPUTWlJrcJ2bpMmHyuSWDkEkk3YKoYjyzZo7TfQwmGwuWkq72G/WcTC3E2OGwOGrazlXEnNacpYezEQVenZto7JaGcVW2k6a+GKYoGw0jWF1XaAWV9RrP7w5q2kauHu20JVw2m0CgNHEeKGqVbkRIJZtpKqbEQEP1mnLwKm42hrQCyWLuGHpA8SpXQRqq12HpJYmxUQAzA4Le7HrKzGYZQbTasRlMrGwCtqYqKU/UyNRVlfiCLy44vw05hl6kSufhj3Gm0pMGAbQTZ0MRhqmHpVcSblAyhQ2r6i+g1PizenOA7M9n1YmriBemmynao3n1A00539Z92zwLYjLUVglKkGz5RqtPTVRte6gfHIGUpyg1KLp+xt08Mc5aMnD+0Pdk8FQxeauyoio5SnR/dugBDMd2+1zH0sJc06LVilSogR0Z1BZsy02JtfMB+8MoFwPrMF2N4pQw2IWiLCkqM4UtmZ6jFAhN9dc2wFrjSetVEY02UUQAwIIuNc2+/qZeXJLLJSkQ8fwW4HjnHeHClXq0sSGJVmZWXxE06l3Asftrcmw0ItpzBzNTgblr0WTKddahQj+lwD7azZ4jC4nG0jiGOepTY0wAgTvaagGw/iYMX153IlRh8MxOxFt9LW8vWcs8ji7R1xw6u18o+w3BzfvGIIRVyguuhVFXQXvfSeh9lsBUOEqBjcE5lOuigDwgdTqPzlTwLsw9fxP4Kf7trXqHovl5zcpXp0KLorKTTQgKGGYlF0Ft76RYtUnbI6jTFaIiNNGVbMLafPoecjgifvl9haGWmlNtcqKpuL3yqB+EBU4WBrT/4n8DN3E4mihynvJzG09RJ1SVqG4sehnMbUBtJoEDxSjKJ3B1LLOYjVRA4drDWA6Jl/HHnXSUtfGBWEsFxoIjJoBVo+L4kcZR2hKlYEz7EnaIoGEsnvPtZNj4ZDMICoebCkyL4YkRnvJ8XjJEWwZtIjCmWHeQBqwKKqtg9YriFyi9peM1+UUxq3sAOY++AJhcdiFp4N7A3RASAbE2IJ0587fhFlqU8ThXCMDTZGW6nxM1tvJgeu0uSq5LO6oSNA7JoeRBOpG0yPZmutCpVpNqmlSmLaAMdRe9jYZffNKki4tppnn+Gcgq1NQq06iu7Hd8puRc7me20a4airtX8b01cKNgWUG2+u88o4jgQ1SsKjCpZ792DYKrNdTUtY7G9h03npHZ7hg7rO/iJG1hbLppaZxfg9D8Qywy5FKHoiyw+FsiKCRYAa6jYWGvlFcbwNarq9RRcHxBPCKo5Bwb/IN7aW6WSoqGwACsCbAc73v66x3D233uB+MtwTVM4YzcXaFKasbBmyW0CABRboG1+loVqVPNc92Gve+W5v1v1k7n1HQ/eDK2hSNO4IOuwOoG+t+UUnS4sS3LlgRqWNvIQgqWH+axLA1SEs4y6+E3up9+Wt5OsCo1N9R7S09iaB8ToBwG5jn5Stq4USzD3BHlEqryWSxJ0sIP8ARwRHHW4n1NdJI9ijq4IE6ydPCdI3U3hKSRgcp4Uc5KvQFpJwYUbaxCFko3E7+ixukQJPOIDsVqCQRoSrACMljmWRyCcFUT4PGAKoReVXH8f3NIsPtEhU5+I8/YAn2lsVvMl/qFUK0qYHNyb9LD+/0iKgrkkUn/6gS7MS7Hck7+pgaPFqdRlZk/WISUCoWJGbMLdDdj8ygZrztPDd4couL6eEkH6TLa7O93JJM0uIwPe4zvqDqUbwVgPFcryAH72ijynpnAiVQq32k0I3vb8xMf2bwAw9SmpYsxIzMxufJdNLC81fD6uWu6f4baD/AMcvxLhyc0ywrgWBGouSD5EGRo4lRpbY2i1B2UtS0sDpf+EwdTc+s0sii0ov/by8oyDKijWtvHKdaMQxUe3MC/UXQ/lK2viwLpzuLC9yN9jzH1GsNiaumht67H1Bmco1SazX5EAAG4GgJsfp7SZOhpGhRoOtUGa3+ayVPaU/G6/d1qR5MhHldTr9GEXgTReZdJELoYtSxgIGsPn0gmQ0V1Y+KM4UyvqsSxjmEvG2Aeq0g1SHVJGokkBRnk88mySMBUMMgg3pi0+NaRdrxjBZROK1p8EMjlgJhab6zPf6g4NqmGzKL92wc/y2IJ9rg+0u0NjCPVuY/AJ00zxTD0WcgAEk6ADn7TZ8P7ONQ7t6lszH7O+Tbc9ddpsaOApU9adKmhO5VFUn3AgOMf8AbXqxPxb85lp9Tpea9kVLPasp/wB/4zT4ymA6VRobhT53Bt76TJVj4wfOa7EUe8pZcxW4FmFrqd7i8uJLDY3DksHB5WPt/b7oJlg8Dw4U7nPUckal3LX9th8RgpeUiXsRQSQXe2k75CdvaMCNPNfXaUtPKK9UkgWc31Atex1v6zRothc//POeW8dN8ZX/AJ1+lNB+EzyOlZpihrlRs+Kdp6FFbKTUO1qdiB6uTb4vMfxztecSVRaQQU2JBzlma+hGwAHzsIAKCLSvpUFzMdP8MWHJru0V1OFY0qZb8N7QE1AhB5T0TBVQUE8kV1WqDpNdw7tCvhS+80lH0OVM0VVfFHsGNIhSfMAY/hYgY2okaqT7NIVXgKyTUhaD7kQrMbQUVDsTywgAnKjQLOYyRi0Dadp1dJ2i8YxZkN5PJrDu2s+eAEiNBKriTA1VHJV18rn/AOSxcm0qKVUGu2ba1ibbbD4gxx5K7EU5rMC4ekrKeQuOhG4lLXwhBy+fzD4Ci9I5xYKdGBOjegHOJI0uy7S9pB3J0X3M5mzanwryHNowumgGvIdPMyhAsmUdSdhCUcMB4m1PIcoRaWXxMbn7/ISYUn1/9R+cB2crDQ/WeQ8SrZsTXbrUa3pew+gE9gelYWnjGMW1Vx5/eBM836Tbp33DmCF9YlXwwWo3nr8/3vG+Hp1MJigpcbbfjMMDqdHT1S1Yr9Cir4cd57Q2EogVqfqY49MZ+UPRog1E23nZZ5lG5wf2BGaWMs2WAwY8Ilbxat3bZvmZso2A1Ei6ypwPGUKjXlHqWLD7GBLHH2gIR72gtYyQNcgRfPflGXkCNIithYGSwzayJqSCvrGIcYayVQ2iYrG8ZY6CMCL1bC9ttZTcGS7ksPtg+8vKiXUjqCPmU9XF06GUVQQwGhXUEbbcofuUh16TaDe2gP3XhqSeQZuvJfzla/FnfRE8Pzf3hsOazaZWA6AW+TFaLotEGuhzNzbkvoI5SXL53+SZWLU7seJlH+1TmPuYaliXbVVPqdAB6mNNBRYhdbnU8hyEmWC6sbfjFaTORpYD+Kx1/lHOHTC8zfz/AIj78vaOxMj+mISAW16Tybj+FNOr6lh65W/uJ62+DFrL4PQC595ge2WEshPOm2vmDofvB9pGRNovFJKSMstWwkqV3N+kWzR3hmx9Zz413o7c7/KYGqtmEPhW/WJ6yVc+ITtJvGvrOyjzTeYUeETP9s1/Vt6S/wAO3gEqO0oGQk9JHDGYXCYuqq6MZrux3Gi2jnUEzM02GU7QPDsTlc5SJpVojg9kTGKRa8LeedcD40TVyk9Oc2n6XM3sPkcM+ZYBHMmzSiQZpXgimsNmMBUc3klUQZdY2r7RIkz4E3EaZJZjaU3EcOKtQrzAA/H8ZZM9lvK2pg85zZlAJuTexvzlUNC7cIZNVJT+rL+MYw/D8S//AHrj/czEfNp9lpI1kvVflc3UfnLfDKbfrDr/AAgmw9hJo0TIYHh1dedEf0MT63vH/wBGq/vPTP8AQbD2zWn1G/7psPmTNAncn1MdILOiqF3e58lA/OdFYtspA6liPpO0qIGwv67STIP3m9thGI4HB03HOZ3tHw8PmQaZ1PsTz+ZpRTHL2lVxldVMGthHjijrHsE1ri3M/cIzi+DVjVcrSYqzMykWPhJuNj0MsMNwmpTW9RbEk2FwWsANSBtf8DOWKakd2SSePkocTVOcaGO0WGZfWFxFMX2+kig8S+vSdCkcbVG0w/7OU/aM/q2HlLrC/s5TdoDZW9IPlCXBksEgI1iZpAOZY4SppsfgweS7HQ/BlIllXh8WaVcEe80//Ug8/iU1fC+IGx+JLKOh+INJhuj1N2NoOlWMcddIqNDIsVErmRsZ8KpvCQGL1GIkWaNvSvB1KYiAVxNay72trvaV7Jm8bsEHXa/oOcsMVhA9muQV6W18iDvADAWObKaj21dzZF62B/C0pDRzCVxtSQkc2Oht67ARpOLIuiIajc7NoP6uftEa1NT+1ri38C/ZHssj+k0F+yW9k3ibKSLJOMVb/YA8hrb3j9LGYhtSFUdTy+ZQnj4pg5E1/wB1r7Dp6RjC99V8T2J5Z75F/lpi1/Vj7QTGXK1c29RnPRBp87RukoH7lvU3Mrkw9Q/artboqqg+gk8TdaZsSbm1ySTbnr7SroVDxxFteXPyiPFGJC+v5wOHGV1sb3FmHt/nxGMSg0HIXkqWpWDVGJ4j2cbE1BZ3Q0y6+Csad1Zy6X8DXsGlpgezC4VL5mYuQGZ3ZzpfKCxAA3PISxwmCu9Rg7AljtbS0U4PXalXq4OuzOtYmrQLsWtzemCdsp2HS0a35LStbIqcSFVipGo8pDMlxpzlw9AVWZXADJoN72HIn1++VWI4YwbQabyHsLku6L2SU/F8ULG8saJ8NjKTjlG94SfAorkVw+Lp+fxJLjUvz+JW0UAvvOI4zHeaEMcxPEkBA1+JH9OTofiVmKIzjeT7wecdCPXHXSLZBrGnokiLHCmZ0OwItefd5racWgRBPTN4yWPMdJBwJGxtOtTuIDTFcaR3T+akbyppVkCgMtR7C32vxJlziMN4GHkfulBhd7E26GIpB/0kfu4cf1VD9wEUxOJqH7NOmvpc/fLSig63/wA6TmLw4tcfERRneFg1Kxzj9nr5EtsfoZs8I+mkzfDAA1Q+YGnp/eaDCVl2B16Eay4iZY06p5raNBQRaIpTcnmB6gR5aL/xn/wP4ShEKWHVTcDWAxB1jZonmSffT4GkRxRtdugJ+JPCE2JcPrZXq72ux9wSdpnOP8Rz0RiQfHRrLUXTULnVMvw30juAxoNKqWYF2VrC1sxN7EeWv0lU+GIo92w/a1KSKCdWvVQk29FY+0mzfHtJGpq0XFfvQhKOoJYWspK8xe+46c4yQI5XHhy/5pFO7jMJMrMSNTaU3GbkEDpL+um8o+KGxkz2LgZz9He0UWlUDGaChiL7iTYDpGpjcLMtiqT5xJd08tcUDmHhn2U9Jeoz0nrFOppB1qkjygzEjMFSe8FXaS5wFaMTDhoVTtEkP3RlNomUgjsLTJtcMQLaG01TDSUGJNqrW6/gJJoguFc+XwfzkuIP4QL+f+ARzDNpsP8AiPyi/E6p8tug840irKXhyXZx5g9L30/D6zR4S4GmnoLTN8Ocmudf3D/7LNSNBpGiRvDLfUxxBK/BG4Nyd+pEZqUQATr/AMm/OOxpDavKjiVyjhRc6gDr/gjmDcncxHN4j/NE2SzKUKNVGAWoahYeFXfIlPW/7qEnprf2k2rU8NWWti6vf1/s06dJfDRDGxKqTe/mdTsBL/i9BVpl1UBrjUAcyAb9ZVdk+BYempqrSAfOwBJZsup+yCSF9rTPg6MWSK3krXsX64rNrYi/I7j185NXklUSDCUjnbEsSd5U44Dn0lniefpEcStxr0imXAqFrr0hBWWcFFek+7odJJoQd1J2n116Q4pDpCd2OkLEf//Z</t>
         </is>
       </c>
     </row>
@@ -3171,25 +3171,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RIYAN PARAG</t>
+          <t>N. TILAK VARMA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>smat2023_134</t>
+          <t>smat2023_078</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>80</v>
+        <v>360</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -3198,25 +3198,25 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L22" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>10.67</v>
+        <v>0</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
@@ -3228,58 +3228,58 @@
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>44.4</v>
+        <v>0</v>
       </c>
       <c r="W22" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="X22" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="Y22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z22" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AA22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB22" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="AC22" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="AD22" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="AE22" t="n">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="AF22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AI22" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AJ22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL22" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AM22" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBIVFRgSEhUSGBIYGBgYGBoYGBERGBoSGBgaGRgYGBkcIS4lHB4rIRgYJjgmKy8xNTU1GiQ7QDszPy40NTEBDAwMEA8QGhISHDEsISE0NDQ0NDQ2MTExMTQ0NDQ0NDQ0NDQ0NDQ0NDQ0MTQ0MTY0MTE0NDE0NDE0NDE0NDQ0NP/AABEIAPwAyAMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAAAQIDBAUGBwj/xABBEAACAQIEAwUFBQYFAwUAAAABAgADEQQSITEFQVEGImFxgRMykaGxB0JSwfAUI2Jy0eGCk7LC8ZKi0hUzNFNz/8QAGQEBAAMBAQAAAAAAAAAAAAAAAAECAwQF/8QAIREBAQACAgEFAQEAAAAAAAAAAAECEQMhMQQSIjJBURP/2gAMAwEAAhEDEQA/APZYQhIDihCAQMIQFHFHAIjHKcRWRFapUZVRQSzMQqhRuSTsIFkJ51x77VMJTVlwZ9tWBtqrqg31ubFhe23W/nwPEvtK4i+nt8i31WklJdOhcqxU3/Qk6H0IYAz5vP2g8SC5BiagU9DTZt+bMCR6Wm84D9qmLp92uFroPxWp1La+66izAW5i/jzjQ91vIznOzHbHC45f3bZao0amxUOD4fiHiPkdJ0cgKEcUJEIQgEIQgEIQgEIQgThCEIEI4QFCEIBFCECjGYpKSPVqGyIpZj0VRcz567U9psVjWZ6jslE2tTzFURdxpsX/AItTv5D0H7W+PMiLhEIGcB6lt8oYZF16kE+gni/EamuUWAHQAAnrbqYgqr1VvlQ90D3tSdPH/iY9gRubnoCb+OsrVyNifSSZT46efXeSlJ0YG2ov1tfXTUCXDDtkNRrgAruN7g2sbeB/QllGjUeygNmXZjmJHhe2g8/6zZYbs3iamrMANr3zaeI6af2kXKTzVphb4jWpjGplWRjnFjmVrag6EEag/wBtp6R2J+0bEM37PXYOpICFjZ9TYgMWF21BA8/Ccm/Yyoqlma7DkBppNBUwpptZg6sDodB3vDSRMpl4Ljlj5j6i4HxA1RUU6tTqFb6aiwYbaXF8ptzUnnNtOL+y3FpVwKtcmqrstW5JJq3BLG/4gVPqZ2ksqUI4pAIQheAQhCAQhCBOEUcIOEUIBAwhAUDHMTilUpRqON1R2HLUKTA+e+2fEvbYqrVOoLnLr9wd1R4aD5zmXIfS1idTrpNu6F2N7/8AP6My+G4QI4JVSdNwLgaWsOvjIt1Fscd1qcB2Zr1SLAqCdMwI03J8BPROB9kaNJRnUM/VgD6AGbvAIMimwGkz6JsZy58mV6d3HxYzti0+A09wig9QAD6dJkLwpEGg/PXx5zPTEWHL+8Hq3mf40nlqamHvcTlO1fAwU9oOWptrpzna1fWYmIQMLHUEWO2xl+K6qvJjLGH9iY/d4k3Or07L0UB7H11H+Geo2nl/2Y0BRxeJoDRcoZR/CrAD/XPUJ2vOs1UYjGYoQIQhAIQhAIQhAlCEcgEI4QFAxxQFKsRTzI6/iVh8QRLphcQxy0VzNc3NgBa5PrFsk7TJbdR89pRs2lrhj1vpcfSdHwXgTPZ2UBLjvHUm3IDp4zE41giK7uqstNnLLcAWDsTY26flO84bSApJ/KPGY55ddOnjx1flGu4pjkw6BirMfdRFF2Zug/rynL0+J8Vqd5MOzJ/CVUeV2Iv5zs8ciL+8dcxUEKLA2vvaaf8A9WxLpUbDrTRqY7qPo1Q6XyLdbi2Yg3FyLeMzx1402yl1veoxMBxjiIOWrhyq5T7xR+9yBsPL++06fDY/MitUUB+YF+unynH8MxeMcBq7AszsCpQoyILZXNrgbm4vfTnedXg3GSxFzYHXkZXK961FsMet7rWcf4xUSwoqdxfT7vO1/P5Tln4zxQ94YdivIgG3qs6b2DPXyE5E3Jyu9hy7qgnX8po6fFcejVM4TKjKAgQqzg3zFDmJIW1+V7jbaXw8eIz5J3rddp9ntUVazYjKUqGk1OohFitRHQ/MNeehTieyuJ1V1W3tLKwIIIFjr4G4G87adGN3HJnLKiYpIxSyhQhCAQhCAQhCBZFHCQCEISQQhCQFNF2oQlUt+K3xG/ym9mt45QZ6Ry+8pDAdbXBHwJlc5vGtOLL25yuK4jTR1amR7wOU2A7wF7r5GxmZww/uUP8ACB8pjuXsp00NrNowUnW1tz8Npbw1CiBCfdv/AMeU5sfDuy6yZLLc6xNTQcj8pIeHL0l1JVO8r+rRhJg0AJCgbnwEqpEE2Wxl2KckGy3UEaX94A3ImNTxzjvNTXLfUANmHS+4YeNxI1tbwrfDWqZtiRYefSWLh7a2lOI4kzMAlPTc5hkA6AA6+v1m0NsoPxk/xVfwWmfaqOVyfgL/AJTrpzPBdaq+AY/K35zpp14fVwcv2BiIjMheXZHFHCAoQhAIQhAshCEAhCEAhCEAijhA1GL4RTa7C4NibC1r28pzuS36M7ecXixlYr0Yj4GY54yeHRxZZXzfCN5JXt+cqz9f1pEXnPk7Maw6nEQxZFsAN2O1z06zHasttHu3Mgc/IGY1bhCFzUIDX3DXIFr2Kjlv62E2FLDCwYLUVB3bJiaqLbl3Ba1tZOMlie/5tqy6q2YOVffvXIN+om1wWKzrruPUek1fE8AjaENyPfqVK2ut7BjYE3OtuvWZ+GRUXKugtGU8aO55mnS9mBd2bkq29WI/oZ0803ZrD5aWcjVzf/CNF/M+s3M68ZqR5vJd5WgiRyycJZRGKSigKKOEAhCECcIQgEIQgEIQgEIQgKcbxvSo48b+u/1nT4rGogYsRZfmd7CcTicRnYsdyST5k3mPLl06ODHdrHTGqbgnvCH7UNjp8z+v6TCxWEPvL8t5rnxVRNHBI5kbjzH9PhMOsnVd4uoWxExK+BU6q1RetnYfnNLT4rcWUgn1uPT9by9OMNoCDYHp4W3ke2k5GWMLTVrlmv8AxFj66zYcJwhrVfZi+Xdz0Xn8dpzlfFu7dPl8vWel9msJTp0VC3LEAux5vba/QbAfnNuPj/ax5ebrpuEUAAAWAFgPAScITocYhCEBRRwtAUUZMUAhCECcIQgEIQgEIRQHIs1pBnkGaByva/BVf/dUsUAGg1s3ukevdIPUEcwJy9Csbi/OeplQRYgEEWIOoIO4InHdoOzxS9WgCU3ZdSR1I6ic/LjfMdXBySfGtdTeKthkYbCRokEAyZM5Nu7W2nxPCKZ1IHw19DymKOFLtmqHwz1LfWbt6h2mPmMtMqpcZ/FWHwaUxcAX+fxnqWE0RB/Av0E8vLi9ydBv6T07CXKJffKpPnlF51cN3K4/UdaX5jyjWoDvoZTmjNjNnMyoTCDsul5amIHPSSMiIyOaEBxQhAIQhAnCEIBCEiWgMmUu8TvKhAeYc4mJHPSBEFkCSPLVaUBRtJDTnA0nGuCA/vaIs33lGgPiByP1+vOOh2tr43Bnf5+n9pi4nAo5zFULcweY8xqD4/Wc/Jw+67jp4ue4zVef1EMgENtJ2lXgFB75WZWG63BtfqDr63lS9mB/9un8lj8c0z/xybz1GH65DC8Paq60hfvmx8E+8fheensZqeDcKSmWqKS1+6pNvdG5HQE/EATauZvxY3GduXmzmeXX4i4iWMyM1Yput5SVl6GJliURpORMhWvqJjDeSRrGShkQgDAwkQhCBOEIiYEWaVlo2MgYBYGRZI5IGQKgvjAyTqd138ZVkY7uf8IC/PeBMyQlLUOhb1ZvoIKhXbfqczfUwMiVtWAIU3ufDlIX/ET9PpJrYbCA3UHXYjYjQj+o8Jh/tLlhTfKLsVOXMCQFLaX+7sCfE7WmZeaE4Ov7VxnqZC5dXLahXAvTVz7qgg2ABIvKZdLSbdCT0kWmNQW212awue8bnzJJl2W51loqHbTS0gr9bfP6SwKBHJEVfwMssd5XLUMCLCKTIkCYgupNcScooNrbrL5IIQhAnIOZOVOYETIxmKQEYRxEQJXkGXmIwY4EQ0cCsUAYRCSkefnAiU8Zj+xqHdlHkL/WZkVoQqoUAvUk7ky60S7yUJIyJleIZdixXy3tIYd12VWsdydrwDGViillUs1wqrqMzsbAEgGw1uTY2AJkeF13dFqVEyMwuUyupX+E5tTz1sL6aQxlKq2X2dQJZrtdQ+YC3dsdhvsQdteuPW4XnN3q1N2PcZkF2IOxYjTYdB46yetK97bV5U28sMVpCyCDUCZUxE94GZclAhCEJTlDS+UNvAUUIjIDhENYGARyBPWO8B3hIZpK8AlbOu1xfw1PwEsIB0O0FAGw/KBWHJ2U+Zsv11lsih3HSMmBELcjfQ9bfGTdSRYGx6xLJEwMcYRb3NyfEy+ItAXgBiEZgsCciZKK0CsiZIlDCW0zpJQlCBMJIslD7y6VVBrIShCIxlZATLz5xBusYbrGRAVpArbaSy9IZusCm5ub+kmpkKlPNzIPKVhmGjehgZMcrFSGYwHc32gW8fhIMDcSWXxgNG1kjuN46awJ1gMCOBigEQjgIEpJBEJhY/iHsrd3MWvzta1vDxkWyTdTMbldRnkSANpy2N7SVR7gQeYZj9ZhcN7SVmrItRx7NmAIyoN9Bra+9pXHlxt1Gl4M5N12xeEPZwmzFfK6keaQZpASjWMmJTHISGEha0mYCQI7xHxkrQIgUPoQfGJ5OoJAiAlsOlztJ3lFXdP5v9pl14A/LzhIuZYggWCV31k2MrXeBaYoRQHFCIwLRND2mawQ+LD/AEzeqZzvbF8qI38dvipP5TPl+ta8P3jl+I1NJomr67zNxdS48Jo62JCtlALN0H59JyYeXo5a09n4BxIV6KvfvAZXHRxufXf1innXZriteixKhTmFipuV8DfqNYTumfTzcuK7eqXkWMhmiJmmmC8LGFkUNxeWCVq4yx5Zh1uKYZPfrUlPQul/he8xW7SYUaCpmPgrn52tKXKTzVpjlfEbe0VppT2lo/dWofRQPrMSv2rC7UifNgv5GVvJjP1acWd/HROJiJU+6dOnlOdftkeVBf8AMP8A4TeYOp7aktS2UsL2BzW1I3sOktMscvCuWGWP2iyudU/mH0MsMxnVtPBgfSZGHfMoJ35+fOFSaXqJFxpDNpLAdpFJr8fxalQVnxDoihrC97m2tlUXLHyEjwbjdDEo9SiWKIcpYqUF7XIF97C3xEDZ+0F7ScKdINvt+cxON16lGhUq0qYqOi5glyt1HvdbkC5tztAy4jPKT9qNVagV6SFWByqiuxFt7m5J66DrNvgvtHwtXu+0CN5AeehBb5QO/Vpoe2ak4fQEkOpFgSdmH5yijxqm47tZWPwa3lf8hIV+MYenrUqqptqXZbW820+EjKe6WL4/Gy78OBx61gNUqKv4mR1UDzItea0vTpDM2uuwILX3JboNRO/rdveH07n9oS/PITU+AW85rivbrgz6vhhWb8QpCm//AF91vnKY8UjXLmta3CdpkU29kddBZtddgBlhNZhuN8NOKoNRwuIUiqndesDTuWAViGDtoSDbNyhNJx41hly5yvoALFWYKpdtgCfgLzw6tx7GOLtiK/8AmOB8AbSijVcstVmZnDAgsc2vrNdOu+huONvu8Ow4p2xxgzJSKqF0BVAzHlclrj5TnE4vVri9arUe/J3ZgD/L7o9BJ8XqGza85znC3OaoOQbT13mHLPiy4Ptp11NxymXRqzU0HNpl0zrOHJ6Ujd0KsqxVSUYdzI4hjYSppUz6z0HsbUzYZR+BmX55v9082M9A7BH9w/8A+h/0JN+Hy5PUz4uhqU5RkI2/XOZgkGnW4WOWNpRWPdU9GF/LeZhEotdSDtY/SB4bxzidTG4ksoLF3CUkHJWayKOhNxfxJns3AuFrhqNPDob5B3iPvOTdm9Wv6ACeXfZThkfFZ3F2p0GdegfRb/Bm+M9kwKjfnrAy1WwtHHFA8vqdmRheLLVRR+zVKVZk07qVLoXToBYsR4Ej7szmHDsa70mp03qJe+dFuQpysyMdbA6ct+k7LjFINRe/JWI8CFP9x6meU8OwS0jgqyM+esHz3IINwQbC3Rj8BMs73HX6fimeN3e/xoO3fZ1cKvt8IbYWoQAKbuyqxtcNdiGVu8QRaxFuk89InbcR/wDhYgcs+HPr+8nFTTC7krP1HF/ln7dgCTqU7fit4qVmRgtr87zNaWYtdw9gtWm3IOh/7hCX4+goUOBYne23whG6jT//2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTEhIVFhUWFRUWGBYVFxUVFRUVFhUWFhcVFRUYHSggGBolHRUVITEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGi0lHyUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0rLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAPsAyQMBEQACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAACAwEEBQYAB//EAEEQAAIBAgQDBQcCBAQEBwEAAAECEQADBBIhMQVBURMiYXGBBjKRobHR8FLBQmJy4RQjM/EHFlOCY5KUorKzwhX/xAAbAQABBQEBAAAAAAAAAAAAAAAAAQIDBAUGB//EADwRAAIBAgQCCAYCAAQGAwEAAAABAgMRBBIhMQVBEyJRYXGBkaEGMrHB0fAU4TNCYvEVI1KCstI0U6Ik/9oADAMBAAIRAxEAPwDBC00aGFoAMJSAMVaAGBaAGBaAJAoAKKAJy0ASFoAi9dRBLuqjqxA+E70lxUrle9xewiC5766mRcULGmpYAjn7oJP0qJym3ZE6pxSu2czxH2v1ItMPNV02G7OTO/6R6VIlLmNeTkKwftm4/wBVAyzEr3W6zGx+VOyjHY6bhnFLV8Hs21G6nRhPOOY8aSwhcKUACUouBGWgCCtKAMUALZaAFstACytAAFaAAK0ADloAtqtA0MLQAxVoAMLQAxVoAYFoAnLQBIWgAgtABBKAOL9reML2oQBWjTvpMHfMpJjfSTy89BK49aHIMQxJMzqY1jUmYbXn508QnJp4RMgaEazEUgC2U8h15yRHhvGlKA6xfuWnDISrLz8xr5if2pAPpvAOI/4iytwgAyQQNpGhpjVgLxWkAgrSgCVpABK0oC2WlAWy0AAVpAAK0oAMtAC4oAtqKUaNC0gBKKAGhaACVaAGgUAey0AEBQBIFAC8TdyozfpVj8ATQB8mvX2uOsAlmgQDq3QbaU52SuOSbNd/ZTFrbDtZ0jqCV84/BUCxMG7IneHmlcx/8G4yyjyDEBTOvQHfXmKlzx7SPJLsOowf/D/FXFzs4UxIBDT4DPoJiqssZFOyRYjhJNas5zjPBr+GJFxT5zI89NKnp1oz2IalKUNzov8AhriCVvWyRAKsBz1kH00FPkRHakU0AYpbCXBYUAAwosAOWlABlpBQCtKADLQAp1oADLQBaQUowaq0AGq0goxRQAeWgAwKAJigCQKAJIoAr4pMyMvVWHxBFAHOexHslcLW7rjuqoJ/7hKwPKoMRPq2LVCPWufUMMB0msk1kHh+GWs+YL4gbgeU7DwFGZiZUXL+UTNIKcr7XcNW9YuqFlihjqDBiKmou00yGtG8WfOf+HWEKtfYjbKg+ZP/AOa2G7mQ1Y7imiERSiEGlEAIoAgigUAikFAIoAWRSgKcUgARSAWEp4weooAMCgAwKAuGtIKGKAPRQBNAEMaAPWrBYMRJKgd0CSd9pPgaiq1VTtcnoUHVvbka3Bbrrhe4gzAIpDHIJC7ExymNqr1JJos0ouLKY9rHsGLmE7Qa62HVzH9LQTUPQxktyZ1ZLkdRwfidnEKGQMsiYYQRPLzqvKFnYlU20U+N+0WCw/du3O8dlCsx+AFPhRcthJVcu5m4XjCXDNuzdy/qZIHnB1Hwp6pZXuNlUzLY53h+HAfEFOd645AjQSEmOkqfnWhCUbJX1M2cJNt20LgqUiZ6KBCCKABIoAEigACKABIpBwthSgKcUgARRYBy04YWEFADAKACAoAMCgAhQFyaQU8BQALUAMweJKByoJaJAXU7wYHMwSY8Kq4uLcU0aHD5pTcXz+x1WAw4fDoAQwfOcw2PeIn4VUqaJFmNszMz/lVEuLdEZkmJEgzmPfUghtWJ1n6U6OIkkDowluM4UrIXK7baxqd9hVecr6liEOTMzGcKN92UxLfxQJEEHuzpyjUVPTqZUQzpqWjNrhHBuyjTTKqaHQ5VC5jr7xiTyJkxqabOpmY3IkmjPxuS3YdFADG4ZiNSTmzH0P8A7qlw6zVL9hHipZaNu0yFFaJlE0AQaAINAAEUACaAAYUCgGgUW4oACKAGKKUYOtGgBwFABCgAhQAVAHhQBNIKC1ACsxUgjcUNJqzFUmndHU8FxwKEgFVNy4QCZgZyYnnWfiIpOyNTDSzK7Na7jAV8QNutU2WYwszP4ThwxYF1ncgTIDbTP7dKdk0HOeXWwOGUBzDKwDRKkNqN1MbEUjVtw3uXsdxHKjN+lSemwn9qfBXZDO0UcRibgLQplRMEaZidWczzJ1rUp01BGVVquo7sgVIRE0AeNAA0AQaAANAAGgACKBbi2oFF0olxyCgaGKALCmgCaAJFABTQB6gD1AEGkFFvQAeA4mVbsv0nN5h5P7MPSqteHWuXcPO0bF/imLvhwLLIqhQzMQWMEmIA22qr0cXuXOklyKNi5igzOMbbA5K1ogeMTz218KeoxStYe6dR6kcP4tiVyLdyXZIDXLZ92ToSpA08hyps6abuhmeUdJFv2i4qD/kLqW7h8jq3wWaloU9UytXq6NGeBV4zxgoAmgDxoAEmgDxoAA0ACaAANACmoHC4pQHLQMGLQA1aACFABUAeoA9QB6aAIZqAFsaQUi5hibT3bY/zLfuxuykd9PXQ+YFQ1WrpMs0IuzaKPs/7Udo5W6yjPGWfhEdKgrUraosUat3ZnWDiN5W7PscO+m4cBiNtVK61CpaalzPJbfUweOe0FvDsFyrnYgkAiFVTJ+QNSU4OepWrVbFHAIxJvXBDPJVeaqxnXxOh8gPGrkEktDPqNt6l4NTyMINQAU0AeJoAigCDQAJoAAmgAGoAWaBxFADVpRga0AMFABCgApoAiaAILUACXpQFs9AHk1IE/wBhzNSUaTqzUFzIsRXVGlKpLkWvZe612zccmFa/cFsaCLaEIBPMyjH1qpxFxVVxitFoX+Gxl0KlJ6vUx/aH2LdnN7CsFuTJRtFLa94H+EmfKar08QrZZliph3e8TMbhvGVMmwx094PaI1idc3gafmoPmMtWXIs8C9i7xudtjGGhDdmrFszD9Z2gdBOw1oniIpZYCww8m80y17QcQupjLFsD/LuEhuuinTw6+lafDJwqpUHFat689vszK4rTnSUsRGT0S05aP77FxtDB/PGoqlN05OL3Q+lUjUgpx2auSGqMeEGoAKaAJoAmgADQAJoAA0AAaBwNADhSjCVNADaAJmgCM1AEF6UBbPQAtrlAGlheCuQHv3Ew9s65rph2H8lr3m+QqSnSnUdoJvwElKMFeTS8XYv8Twlu1ZHZ2rihzpcvAK91RuQm9tJiJgnfpWrwuio4h3d2ly1tr2/gyeM1L4RZb2cl3Xsm/Hf6GN7MX8na2I9y4zj+m4S4PlJYf9prC4zSdLEyVtHqvM3uCVlWwkXfVaPyOmVpgisZs2bDb2aN9KRMWxSu3IFOTCxyOMi7jATB7G2SfBrndUfDOfhXTfDtFzrOo9kvdnK/E9dQoRpLeT9l+o7jg1tMRZRHWxcYZgtu45s3SobU2rq6ncd0iNtas46lF4mpdNbO6V1qufoyLh82sHSbs73Wrs9JP10tpp4lbiXssF1XtbP8uIXNb/8AUWcygf1RVF0G/lafhv6OzLnSL/NdeP51XuYeJ4bftjM1slP+ohFy3/50JA9ahacXZqw9aq6KyXaQBitQAc0AQTQABoAE0ALagcBQA2aUYeBoAeGoAjNQABelATcu0AaXCeCXbwzki1a53bhyrrtlB940sYyk7RVwbUVeTsjq+GcNw9n/AE8NisQ//UFs21n+R3yx5rr41ahhbaznFed/ZX9yvLELaEJPvtb62LgW4k3BgsNhdZN/FXFdvPTvT5tVnqSWTpJT/wBMVZfvkV0pp5ujjHvk7v8AfM5bj/Ebd0Nkv3L7qym5dYZEOYEKLSfwoNfOdzVrBKVLGRjKKipQlZeDW75vUgx6jW4fKUZZss43fimtO65z6ytxbye+oKnoyHUqevUVNxvh7xVHNBdaO3euz8FLgfEP4lbLP5Jb9z5P8/0dDwDidvEZsh2O1eezTWh6MjWxK5V7x086YKc7xXHsqMypsCQW0FOT1Easc1wS062y9z/UusbjeE6KPgPnXpHB8N0OGXa9fweb8bxP8jFu20dPz76eR0mC4z2FpQ9m1etu7ApcWfdEgof4TJImqtSh0vEJqEmmoR1XjL7GhTqOnwunKUU1nkrPs0+5ucO9pMLkD272LwvLKGGIsg8wFfMYHgBS1MFXvZxjP/8AL9rEMcbQUsqcoP1Xvc08Lxm25zDFYK4T/FcS5g7p8O0k/IVWqYSS0dOa8GpL98y3DFLeNSL8U4v98iMVwjD3gWazB3NzDOl8DxOSHbzKNVGeHV9HbxVv69y3HEXWqv3xd/79jl+McBewouowu2SYFxdYMxDRtrp57gbVWlCUHaSJoyjJXi7oyw9NFJmgCCaAAY0AhZNA4GgCVNKMDFABZqABa5SgKQlmCrueuw8TUlKlKrLLBakNevChBzm7JHZ8G4ThbVsX3ZLn/i3pFlW3y2rI795x4wOhqysFPPkabl2L7vZIhWOpyp9JH5e1/Zbt+niVuIe2lwljhoTLoHZUa4QdZCkFba+AGsSSa2KHCoKyq69y2/LMjEcUqdIlT27Xv+EY2N9pMW9uTibszqVcp1EQkCr0cDh4ysoL6/UqfzcROpZzf0MvGu9w2+0dmLASWYsQNOZ61NCEYJqKS8CPppSzOTvbtLWBtib6Dmqt6If7isnHPosVhqvLNKL/AO5ae6NjhidfAYmnzyxkv+13YoXANTW22c7lb0RY4K9sq9yyymGg5CCJIkzHP+1eefEFCnTxWam9Javx5/k9H4BUqzweWqmnB21XLl6bGzh8WWINzYVhm0I4liBezgL3EVj/AFECY8Y0q3gqcZV6an8rkk/Ur4pyjh6s47qMmvFI55MWjnun0IKmP6TrXqMZxex5W6M4K7X39xnEf9G14u5HpA+tZlB5uJVrcowT8eszfqLLwqjfnKbXgrJjcDb0II5yZ8evL0q/N2loc5Wlqmiiin8/NqtJ3LDZppiWTsnRirfqUlSIGmo9dKruEZtxkrogpSlCcnF2aOx4dxwPad7mXtch7VTCpireikkRAvCRrGu23u4uIwNpqCV4N6f6X/6/u++1huJKUZTeko79kl/7fvhxTCDH5FY+LodDVcOXLwNfBYjp6EanPn4rcNTVYtEmgBbUCoA0Cg0ASKUYGKAPMaAK916UCxgVhS36tB5A/f6V0PCMPaLqvnt4HMcZxOeoqS2jq/H+l9QrJLSp6x5Hkw89PhW01leZGVN2Stt+3FYC2cxQ/wA0+hP3olK6TH1pLKpLuJu2/wDLgcjJ9TE/AfOli7yGxl17hWlzKGjmB6CR9TNMejaEk8snE89w27oZYmI121EEH5Goa+Fp4qlkqX0aemjutS9w3HVcI3OnbZp31umOOBRgQRMg767+G3SpG9dTO6ecXdcmVeGWezuldiVg9GAHdYjYkbR0PlWP8RYdVMDKcVrHX039jrfhrG2x1OLfVndebTsvXbxLL4S5duKwuBLKybhG56Kp8dZ5iOciuBwkZ4h9HCLc+X5Z3+Pp0sIukqSUYc77+HfcLFcTDHJaAFuCpYjccwJ2Hjv5V23DPh9UIqpXeaV7pck+3vfecNxj4hlWi6eHWWNrX/zNfZdx4YQAljr3Yjy/3rdvocZ0zypLtM/EmSqycojL4AgTHSpaVKELzjFJvd9ttrl/+RVnTUJyuo3suw00UjLPQD18KierdjPlZ3sUcZaIM8jHx1qxSlpYnpSurD7Oq2h0Yk/OP2pk9JMjlo5PuCZpduiEgesGnRWg1K0F3kY3kfT7Vg8Zo6RqLw/H3NzgNbWdJ+K+j+wu21YB0gw0AAaAFmgAaACFKIFQAu41KAkLmYL1Py51LQpOrUUFzIMTWVGlKo+S/wBjRcjbYbDwiu2pwUYqK5HD3beZ7vURzB9D+x/OtSEnIFrhDZhvMH1CjXzgfGmqKytCqKy5Xtv9R2PaEMdYHjpl+59KjhuR0VeWv7zE4G5Hd8op1RcyStG/WFcRPeHl+H86UU3oPofKXxelFboR9j+9My9ZorZLScS/e4QXsjEK65lGbKRyWTM+QJrGr8Rg8Q8FOPVl1W+96bex0vD+F1aOGWNUtYvMl3Rd9/K60KuFZezgfwzpyk6zHU9atYTh9LBQVOmvF83++xmcZ4tieJYjpKz05LlFdi/Jk3WEmPStZPQrxT5mlZvZl+XyqrKNmVJwyyHWuGC8qtYtPKhmuvcI7OV7x9OUeXnVKWLlQnOOIqK0mlBRTzJPT15+pt06HSRg6UXp8zezt+/Q1eJcOYy95Oztx3zahxbbKCASviy7dfAxRw+Ky0lSw888+WfRyV/wmvL1KmDbxLqVoZYc8uqTtz8efjuc/ccOhI5R+xPlpW9C8ZamQlknZlezeAkk9PqP2qSqr2JZQvoMVu6Z3MT5x9opyVhkvm0G4k9w+h+YrM4pC+Hl3fktcKllxce+69ivZauTZ2Q8UgAMaAANAAzQBINKISWoArXnpQGcOQyzxosCY0BadJ6wrVr8GpqVZyfJGLxubVKMFzf0/v6FxvnXTo5tCLpJGm/77r9vOlJIpXs/3tEvdBBbWJmesAR8x8qI6kig07cy1bsNdyoo7w035kmPlJqGU1Tbk9htOLdSy5nRp7FgoWt35uAwFKOAXHvJMZpkNy2+NZb4q1K0oaePL6e5tf8AC1KDyz18Cvw/2YS+lq7cuFc7N3QVBFvK2ViTsCynWDprtJBWx8qc5Rir2+v77keD4enBOb35d3aNxHAbVrDse0zP/lEIWSYa2CxhdQM8gf0neagxHFZ04udraNJ2e99F6asnp8HhVqxs9bq6uvl5/hCrd51sup/jBUAmdSNl6bVz3CoSr4yLeqTzPy/s6PjFeOFwM9N1lXnp7K5gYfEZWadifz9676aujz2dPMkVMSDnbz186IvQnhbKi3w3RwpMAkCekmJMcvtTay6rklsRzgqllex2JwBv4n/Da27dvN3SqwICm6QF3JYpEkwPlydKsqeH/lN5nLVvW9tbb9iveyV/r10aaT6NK1tLaHuL8I/wOW5bfNbaUKuqwTkaVZAMrZkL6wDIgyDouDxkOIwejTXjdapqz33s7X9x1Wj0ej/dLbGBxGytq/dtr7rd9RABAZcwUgaAwV/NK38FVlWw0Kkt9nzTa0unvv8AvM5XiNBQrNLZfcwSfD8+1aQ1Fiy8ieu3iOR+U+tKiOccrsWyJDjwj5VUxcM1GUe5jcPPo61OXevqUbDVxJ3RbBpAANAAmgAKAJFKIC5oAq3mpQOsvYIWOH2bbf6l64b7Dmq5CqgjkMpU+ZPSt7g1Nqcpdit57mDxeqskY827rwWhjoJ89q6FmA9AXWRI32I/OfMUCp2dn+/vMzi8ZxurAEfysPDp9yOVNyu5ctmyvmvf9/Bq8Ey9qC5PZjNcfKYPcGYAHkSQFB5TUOLvktHd6Lz0/sKEYuacto6+nLz+51fEvai1bssbR7V3a4ZIIC9o94kMCJGWbUL/ACDlE41PA1JT66slb2S+uuvea88fTjG0Hdu79W/ppoZlr2utogUW7jTZVRLIAtwLlciFzEFgLhJMlumtSvh8pSu2lr37evl4DI4+NrJO6Vt1v6efibGPvdsxvNA0IUb5VkkCTvqT+0DSuIr15VJWvotjtcPQjTV7a8zifaPH9m+/uqGUczO+nWus4H0VHCOfNt38tvL8nK8cjVr4pUv8ttPPd/Y5sPi77EpayK38T6fBdz+9GI45ThpHUfhuBvKsxvYTgxENdLMdJ1yzpvArInxfF1XaDt3Lc04cKwlJXkr+Ow69ctDMqDvKJUydGUr13EZvlWrw6lxDpFKrJ5eak9/Ll7GZxCvw9U7U4rNycVt5/wC502FxbvGKwoXtVSbiQqAMiCWnZlYF5AAJyyB3TSVKKoS/j175G+q7uV1JvTtVtFdt7pX1G4fERqQzR3W62tbn56/qLfE7uJxRIvp2Vq2dWIZAv+UGcsoJMkZk3iG6tUNB4fDxX8e0pS1yqzvrbR6LTd89O5lipKTu56Jc/K+tjleM44XLxuqO7qqjWQqiANTJ35/LYdFgcO6NBU5b8+9vd/v9nM4qr01WT5aW8DLu25UaxJM+KiJHrtVxu+hHCVpDsNqoPUaDz2+RFPRFU0lYv4bc/wBR+WlRyKtTZeBmpoSOhI+Brh6sMk5R7GzvaFTpKcZ9qTLaGoSU8aAAagBdAtw6UaJuGlAnhuFNy57uZUBuP0yryY8pML/3VPh6XS1FDtZXxVboaUp9hqYzFPdY3LhzMTr9gBsPCuzpUo0oqEFZHGVas6s803dilFSMibIfQz8fvSIVa6GDxvEi0yPMK0o/QExr5yB86ZVmoJSb0NTB0nVi4c1Zot2bwI1OjRr9CPznT27q5BKDT8B1sAFlY8vprPnUc3pcjeqUkHwm3nuhGHu974EaeulZ3E6/Q4aU1u1ZeLNThuGdbEwtte78F/eh1yNIA6ydPhXnb3PQuQ9cPb/SPHr8aLsLHsRhbZUnKPprSIdpY5HjtxtNTlDREQDGutdX8PKMpTduS158zlviBtRhG+99PT6FC68EONQR0/OVdRF8mcnFXTgyx2mRkdTHMEabdPSnq04uMhkHK7s7NFji193gu7MIMZiWgmJIk84FJQpQgnlil4KwkKs56Tbdu1iGQdmPT5x9qdF9Yam+kZl4vFqxSyhljOaP4QdSSeoX5kUN3dkXqVGUE6slpy7/ANf3NUEADzHy737VMUNW3+9xZw+w9aZIhnue43hMj22AIF20jieuqH5pPrXG49WxE/E7Thv/AMWHgV1qkXSTQAJoAGgDzU4QReNAG5guGstoERLgMdYMESAdP351f4fxfA0OpUbT5u2ntf6GfxH4f4himqsEnG2ivr53svcRctMPeBGvP711FDE0a6zUpqS7nc5nE4PEYaVq0HF96+nJkLpUpUeonE3QB+fSnIkpxbZyvGF7ZLoAnKpbT9e8R5D51jcXr2gqS3f0/wBzpuG0MvXZpcMsA4a3EZgijw2rQoNxpxT7EZGIm1iJX2uzW4d7OYvFIDatMwDEFtAvdOoLMQN/Goa+LpUnaTJ6OHqTbcI3RrcP4WyM2YDP7pKkMAAf1DQ+nSuU4zxKFe1Om9Fr5/0dNwThs8OnOpu9u5f2ab2iNNegrnjoxijL5+H5pQB5r3x9JFKJYpngN/GMy2wkKAe80bny8K6HguKpUIzzXu7fc5zjuErV5U3Bqyv9hDf8PscUZOzXTY9okNzka/WOdb//ABOhvd+hgLhmIz5rL1M3h/A8RcdsL2R7a2CShKgqNNZJiO8vPWRVyWKpQgqubqspvCVnXcYR15l3/l7EvZdxa0tF1c5kGU2/fA11A11E7ULG0YzUXLV2to+exHDA4jrTUdFe+q5GFirsWwYnYHw6n861ZyvMRU4Xnucl7PXQpJ3e5JP8qToPM/QVBhr5bvc3cfFyVuS93/R11hsx8FEHzME/ID41dRgzWVeP7++BfSmsqsPiVp2tLcYkqhCCSdAZMKOgP1rmeMzoqpGC+fVvw7/sdPwOliXTlVlfo9Er9uu3d295TSsY2yaAANAEUARcpwh7B2s922pEguoI6idflNNlfK7D4WzK51V/FDMRB335f2rArYWS2dzp6GNg1ZqwIIOkiq0VUovMrp9q090XHKlWWV2a7N/YrX8Kh5R5afLatvCfE+NoaTamu/f1X3uYWM+FMBiNYRyP/Tt6beljkfaa4bQgEMToAPek7d3/AHrrMH8RYbFKzvF9+3r+bHO1/hXEYR57qUe1aPzX4uDgcLkUA6ndvFjv9vSsvEYh1arm/LwJVTShlRdwGBdSFA0jnvpzitetxnD04JR6z7tvUyIcIr13efV8dzp+BWchu25YKCuYSRmcrLZo3AkCPPrXLcQ4jVxMry0XYjqeH8OpYaGmr7zfzqAAIC1lmmJua+6CfGgLmbexMEiI69TS2C5WN4sdIUdW+3OnWEubmGYrwvGXVbvFsoddDC5ABI8Wb41u8KotVIZlu7+Rh8VqqUJZXsreZexOJuzwgC44LqpuQx78JZnPr3tzv1NaEYRtXdttu7VmVOck6EbvXf0QtLzf/wB5gpIBtAMOTAWQwnrrB9KlcV/w5N9unqKpf/3NLs1PcPxBOAx7FtDevqusgBo0E7Alz8TSyiv5VFW5R9v9ivGbWFrt9svf/c+Z3boVW01kAeZkV0NXTUw6cHOaRySYYrjGRQBMMD0zCTHrNczQ4vDDQ/5qb70dtDhs8anCm157e1zueG8OIUKWEbyNSSdSTMU2p8X4WC6kJP0X3Yx/BWKnNyqVIrwu/wAGzh8Kg1ifP7f71hYz4pxdbq0koLu1fr/Rr4L4RwOHeapeo+/b0/NyeLcQQW2tnvMwiP066E/DSs/B0qs6nSyv4vdlviFelCn0UbX7FyMJa2TnyaABNAtgZoAhhSjTU9m8PNxrnK2pPkW7o+Wb4U2b0H0076FTFcQGcwhfU84A+P2NVHG5fUrA3eKudFsopjWTK+cQIPjUah2smz87FfDnFgljeDIdchtyBryfNmHxjwqOeHoSVmte1Fqli6sHdSuuxr9YleCdpdF1i5fcDl00AHjzNT0ejpK0SHF4ipiNJbG9Y4NcXvHKoGpLakdBpz+lPdfNoUlQcNTd4RhbWcZhqokbGWI7p15HWkpLrajqrvHQ5Xg2NKX7itqHgzMGdp18RTa1O6uLRqWdmdTh8NmM5Tl8T86pWL1yvxr2gsYcFTcBaPdSC3r09SKv4Xh1fEfJHTteiKdfGUaPzPXs5nNYX2jF4mUZY11ImJ8NtPOteHw7Ub6016GViOPU6SvGDZe4Px+zZxZutYL2uzyqjsrFXlD2hOWJ7p2Gk1qLgcI0VGNs173+xmS41OU87vltsjQb2lt/4W/hTbab925cDSMoFy4Hg8+UVZjgJKrCrdWikvRWKM+IRlQnGK1bf1DxXtba7XBN2bxhVKsO7LSiKCuv8vOiHDp9HVV119vUkePhOVOVn1fwF/zNaTiLY0o5RlgKMuYHs1TrEd2leBnLCKgmrp/dsipcQg8VKrZ2a28kVeH+0SHBXcJ2Zl7hfOSIg3FaI6woFSPBSWIjWvsrW8rEeIxi/jOklu7387nL4ka+vxNXavyt9xWoayVjN9oAbadugGe2QZImVJgg+Gs1wU6UaiyyO6w2KqYeWaDOp9n8X2qAt05aCsWrhIRdjoI8RqzXL0NZfDakhThF6IZUrVJqzZlcbtQ6t1WPgf71rUJXiYWKjaRVWpysSaAFtQANABEUoh1nAcKow8MY7Qlj1yjQD5T61FUZPSXIr4nhygDIAATE6baSTVXNdl3LZWRF/hCAAR3Tr4k6xPXaim2xKqS8DZt8OS2EzAbAHpMVGlmvYlbUErnuI37aDuhQZB26cjToUv8AqI6lZf5Sq+JttZysYbU+ckn7UO8ZXWwK0oWluc7f4yLJYySSRroPd2ygbR0qWMW2muRHKaimjKxPD890XbBORjoFzMbcn3XgEiCTrGojnpVxUJy2WnbyKfTRju9V9yy9y5mtozs0s4KknKALF9gpUGCSyg+EDnNVKNVZKs4pZoK/g7mxPBtToxqN5Zyt2O2n1uBb4LbZ0bIAskMgzROUsrbzqRBg8htNavCuNSr4armazwV14GXxjgkMNi6Uad+jm0n2p9n4LVrhdkMSEI0GisQCZIBlgTHdbSeQpF8Q148P/kuKu55fa4lT4coT4h/FzvKoZ/e1i5d4XZb+EoY3ViY8SrTm9CKgofFleE108Fl97E1f4RoOD6Co8y7dV/QnC8MRlIuhs6uy91gBChYOqmZzb+ArY4txyWDcHSipKavqYnBvh+OM6RVJOLi7aWKj4JWvtb72VGcEyJKrMS0RJMCY/iGlaWJx/wDHwP8AJktcqdu98jMwfD+mx/8AFi9HJq/Ylu/QtY/AItolM0qV95g+hkHZRGuX41m8E47PH1ZQnFRsr6GlxzgEeHQjVhJyu7PRKxiWWgyOX3mumObkr6BOC0kbSD9qrYhN0pJdj+hJh5KFWF+1AY+xns3F/UjD1gx864k7AuewS5sMp8PpyrNxPzs2MO7xR1uBtggiqrRYKvG8JNskfw9705/L6Vbws7OxSxkLq5z61fMwI0AKegAKAGmnCG7icxuKgGltACOXuwP2+FVKsrLxLtCF5eA3HYg5Z166cwCpPyNV6a1LVZ6aHrPEhK5jswKnkYj8inuLV7Eamm1mLHHuJEKAdZ+MeHQ0yhFvUkxDS0MTFY0oSpK6GMxBJMeFWFHMrlVyy6Gdjgx1YxzJMDp+cqfDuGT7zMx+JVCFVGZihfMw2A0GnUmtDC4R1HeW3cUsTio0l1d+8o8Ossq5nMszAk+Z0jpGldVh8OqVLKkYOLxDq1L9h3V7Djtp6XLn/wBOIFedYCF44yP+l/8Akej4+q74J/6l7pFm0mQZhDe8sbR3dJ8zJHivhWfRUsPCNdbPNF+n9+xerShiKjoS3jlmvXR+3uVlXWf6Pre+5q3V04PSXbUl9CnTd+M1O6lH/wAixbuMXugklVNkLJJCzbYMB01UfAVq8bpwXD8M7a/0Y/AqkpcSxSvpd/UaVjN5j0izZrP4nJvDYZP/AKH9TS4Ul/KxTX/2L6GfZtRdvv1uuoPKFbM09NTb18K2fiXEWw1DDJ7pN+CVl7mL8L4fNiq+JfJtLxbu/b6l3GWVIuohBXI0EMGHdUXdGBIPeUfgrM4TUhh+LRUGnF9XTbVL7mjxmE8RwiUqiakutZ76P8HIW1zQB/MPlXpLZ5o3l18BzGAB1AjyGtGjI1u32DLYrhakMk3HsbR2lOeeCl2oH2AY27eXkGKkeRInzFZuI1kbGH+VHZ8N0n1qrMtIfcUEkHYgj4iP3p1F2kR1leJxqitYxCWoAU9AC5pQHmlEOp4YytbLLq0KT1kb/vWdXvnszUw6XR3Q3F4ZZ5ZW26GRBA6H7URQs2YnYGezAmZ9PH0/tUzfMrpa2K7WXJAY6jYkzpyiaVWsJrcWl1AWhCxgQSe9uJ73LmevnUipN8xjqxXISmHE5nOYzIH8K+QO58asKyVkVm29WVMVh810MdsoHwLH9xW5wmGaL7mYXFp5WrdgrEWYMfD89K6Faoyqc8yudFc4qh75R17xLQVbRkuK0e7t2m3hvXNU+AKk62Sf+ImteV3c6KfxLKq6EZw/w5J6PdJWFLxS2XADEIyEEsMuVgzMp5+U9GNVn8PzjwyeGbTlmcov0Lj+IIS4pDFJNRy5ZLfTX/cfh2WWGe3oEP8AqWxOt3YloO67bTWXX4Pi3w6jQUOspSb89jWo8awa4jWryn1XGCXluXTiEjvXVIA2Dq7ctlUnUwNTHKTUMeB8RryjGtsub5LuH1fiDhmFhKdHVvWyW77xWAu9pbLSgJdzlLqCohVVYJnQKBV3j3Da0qtOFCDcYxSuvEpcA4rh4Uqk8RUSlOTer7ht7s1ZjnQqC7d25bLMWLPAAJ1lgux0HhUWK4bicfj10kJKmko3tyS39STDcXwvD+HPo5xlUu5Zb829vJAYPEocr5lWG1V7tsN3TPPLIIjlzIqKv8P4jDYmEsMnJKzv5kuG+IsNjMJJYlqMndW12sc1eUK7KDJD90jYgnU+VegRd1c85aflb6EXtwI2/cxHwIoW42OqbCU1yXEYZcTP19Tq+HzzYeL8vQo+zV4rcup0vOfRmJ/esSuusdBh31UfQMAuk1TkXEPutBmiG4k9Ucde99v6m+prXjsjDmrSYLGlGimoAXSgWopRBti6yGVJFRVaSmiajWdN9w+5xG6dFaOsgfSoYYd8yepiYtdUWty4RBuR5DX5mpuiRA6zPXUJJLMST6DTaAOVPUUthkpuQranDAWalBgWyDIA1612GCw38eik93qzj8fXdWs5ctl4C79vUcz+f3q9ArQkxqpI1/3qN7jHKz0KYtZrkfwiac3dFjNlp35llbHfmNIPpSX0IXU6tiLgyvP50MU5axsEXmjYb2cNMb0y+gzNeNmVskPT94k17xJxxgDrt6U2LsFFXZJtgJmOu39hTVoxM15WQu48sf6V18dZ+ooSHxVl6hqef5Nc5xmFqyl2r6HQcInek4dj9mUOCpGKvjqwYeRRT965zEbnTYX5T6PgBpVKRfQOOmkQPY5LFe+3ma1afyIxa3zsUTTyIU5oAXmpQLqmlEDoAkUANtmkAJ9qAKd5qUALbDc7fuK0uG4WVWqpW6q/bGbxLE9HScI/M9PLtKwxUHSuuaujnOiutRl65TYDYxG9pIAG/wCTTWtRmWzbYLLDfA0+C6oqd0XLRlfz8NRSVmQSVpCMXv51JTJKewVl5GtNkrMbJWegjFPlM89KcvlJaazKxBUDNmMtoR9vLSmLTUW7dsq0FG6SuvL70r3H5UpFe286cydPID+1CRLJW1LVs/n7/CPnWTxinmoKXY/qXuFTy18vav37iMOcuLB/Xb+akz8itcfiVzOwwr3R9BwDd0VQZoojiG09JoQPY47Envt51p0vkRjVv8RiyakIhTmlAXNAF0GlEGA0gEzSgMQ0AGTSAUcSaUCbKLAJ6enjXZYCKjhoJdhx2PnJ15+Ip7Y3iKvbECk+0C4swI8JpqHRdtQ2gQByp0VoNV3qw7/IikgJDmicPc1+NE1oJOOgV3eiI2OwtbkNRJaD3G8StjLmvWki9CalHQbkyks3SPL+9NtoMvmVolQvI8Pz70u7J8tmOwVrflAgHx3NLsR1p7BqOm32/D8ap42GahNdxNhZ5K8HzuvfQq8ROV7NwfwvlPkwP7qtcPWV4HbYaVpndcIvyAKzpGqh/E3gHypovI4660sfM1qU/lRi1XebALU8jEu1AC6UC8ppRBimgAgaADU0AEzUAUsSaUD3DFuXW7NFLEAkRHw1roOGY60OjqbLn3HP8SwP/MU4by5d/aefQHz8iPMHat1NPYx7WlZniNqcgueAzHbeh6IS+VAkaaxv60vMddXIVBvJJ6Ci+tgcmFfvchvH7U3YIQ5srKGIMD70pK3FPUetpUBduo/2HU03YicnNqMRF4M/eOg5D03NCV2SwcafV5hZABr7p3PPTlS2sNu29Nx0SAJ7o2A1J8ztTJTt1mNXzd7IDz4DpXNYzirrRcIKyfqdBhOFqlJTm7tegrG28yEdIPqpB/asWavFm1SdpJnTcGuaCsxo2Uy/xNu7TUhXscczanzP1rVjsjFn8zAY0owUxoAXmpQL6UogYNADAaADBpAPM1KBUvmgDX9mHWxZuYhgCWJtqDsdswPkHU/GtjA0M8VHt1fgrpe9zGx1dwm5W20Xe3Zv2t6GfilNws5JzMSxY7kkySeWs7V0kIqKUVsjA6VuTctWyq7uNxMDcafLlT07D1GL2ZNrEDnInXrp6edEpCSpvkC7LOrDwinJoVKVtENtiVIBEf2+dNb1GPqyuz2HsqDrr8KJBOcmtA7bgSJFDY2UW7FfKD3mYb6Dp6daTmTXa0ighdlYUep2A12Hp86VvXQbls7yJVQD+o/Hr8tqRg22uxBkE+Xh8N+dQ1U5QaXYJCUYyTfaKtmuHO3CakFNngTyAOlZk1Zs2YO6TNPijQvpTFuOexxuatVbGK3dkMaBBTGgAJpQL6NSiBMaACRqAGA0AQ7UAVLz0oG1iGC2rKfptBiP5rjG5/8AEoPSuq4dTtT/AHkrfW5yPE55qqSff6u/0sUQSTJO31rT7ijaysiOWu/3pReYi/YXQ8/n8aCSnUa0Fm03QMNvhHTy6UhJni+5i8/6k+nkd6B2XsZJurHucv0ijQTJO+/uT2i7BPkAY5/QUBllu2eRXOwC7/Ez5Dn8hQgbgt3calmdSdPgOmw8utLYY522X7+9w5ABpH2nypCJtyVw7jc/Q0xjIrkDxSO0zKABcVXgbAkQ48g4ceUVxeJpunVlF9p22GqqpSjNdhWLVAWEaHBbkMPWqFddZmnh5XgjX45c/wAv0qGC6yJZvqnJA1qGOQxpAEsaAAmlA0ENKIETQAKtQA9XoAF2oAqXtadFXdhJOybNG5cJ+Q9FAUfIV2tNKKsjhm3J3YE1ImFiC1OuFhYO7Hnt5CnXH2/yolbkKDzP1JpEwcbyYwGKUZuC5HMD8ikHK5Fx+foaLglfQ9m+tLcLAK8SPH660iY5rmGTP1prYzYInQimyfMLa3KuIuE5fKP3/c1zvF6dpxmuenodDwifUlDs19Qc1Y5so0eC2iSI8ap4jc0MK+qafHAchH5tUFP5iap8rOVD1pGSeLUAKY0ALmgDQWlAZQILFADloAi5QBWJ7w8x9amo/wCJHxX1IcR/hS8H9C7yFdijjOYINPQ5kXDSixBu+7SsWPzAXj7vrSDo8xqHT1pSN7nm39PtRzFW373nn/alYiIX3fSkFe4PP0pFuO5EKaGIw5pj2EEX9vWsfiy/5Kff9mavCX/zmu78Cq586JH1D2KsqcGkqp7zch1NLZMdFtFnifDbJ3tqYjcSPeA503JFapD88mrNny3iCAOANgq/QHU896RbDGVWpRotqQAKUD//2Q==</t>
         </is>
       </c>
     </row>
@@ -3298,25 +3298,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KUNAL RATHORE</t>
+          <t>TIM DAVID</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>smat2023_134</t>
+          <t>t20blast2022_133</t>
         </is>
       </c>
       <c r="D23" t="n">
         <v>8</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>80</v>
+        <v>72.7</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -3331,77 +3331,77 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
         <v>20</v>
       </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" t="n">
-        <v>0</v>
-      </c>
-      <c r="W23" t="n">
-        <v>9</v>
-      </c>
       <c r="X23" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Y23" t="n">
         <v>0</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA23" t="n">
         <v>0</v>
       </c>
       <c r="AB23" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>14</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI23" t="n">
         <v>3</v>
       </c>
-      <c r="AC23" t="n">
-        <v>14</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>11</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI23" t="n">
-        <v>0</v>
-      </c>
       <c r="AJ23" t="n">
         <v>0</v>
       </c>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="AM23" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFBQVFRUXFRcZGhocGhoXGhoXHhkaHRoaHBoZFxoaICwjIB0qHhgdJDgkKS0vMzMzICI4PjgyPSwyNC8BCwsLDw4PHRISHjIqIyk6NS86Mi8yOi84MjM0Oi8yMjQyNzQyMjIyPTIyNDIyMjIyMjIvNDIyMjIyPToyMi8yOv/AABEIAPYAzQMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgEDBAUHAgj/xABEEAACAQIEBAMFBAcHAgcBAAABAhEAAwQSITEFQVFhBiJxBxMygZFCUqGxI2KSosHR8BQkcoLC4fFDwxYzc5Oys9IV/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAEDBAIFBv/EADIRAAICAQMCBAQFAwUAAAAAAAABAhEDEiExBEEFIjJRYXGBkaGxwdHwEzNTFBUjQlL/2gAMAwEAAhEDEQA/AOzUpSgFKUoBSlKAUpSgFKUoBSsfF4lLSNcuMERASzMYCgbk1yjj/thglcFZVlH/AFL+YBv8NtSDHckelAdfpXzvd9qPFGIIuooB2W0kHsc0n8RWdg/a7j1I95bsXVnXyujEdAyvA9cpoDvVKhPhf2j4TGOLRDWLp+FLhWHPRHBgt2ME8pqbUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAcg9uXFnAw+FV4Rw1y4o0zZWUW5P3ZzGOoHQVzXhvAL16CqlVImTpUr9pRe5xh1ZSyoLKIIOqZA/z87v9K3mDcKIBVeswKqyZHHZF+HGpbshqeC7vNwD9fyq5ifBV1Uzq4ftBH0NTxUJiCD3G1LmKRQQbqEjcZhp61Qsk2aXgxpHI7WaxftG4CmS4jEjQgK4JIMdq+q7dwMoZSGVgCCNQQdQQekV86+M8KWdXAGWIkdehrtfs/zf/wAzBZiSfcpv0jyj9mBWmEtSsxZIaZNEkpSldnApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUByTx3hivEy8fHYQqe6s6kfSPrUTxNhSTmts5zfGz5QCeYWZIEevSalPiu6zY66HzMVbyztbtlLYCgcsxBavN57du2W+IgaKOZ5D51lnLzG7FDyKzF4Cjm0wcQRMRIjStXZwlxXM2Lbkz5nBB30ykCDpPMVusJxG1bZ1uFgxgbRqRMD517THBGtllm3d0BMSHHLykiCNvTvVabRc0nsani1n9ARljaFGsGQIH1rsHhhUXCYe2jBxbtpbJUz5kUKw9ZFc04iwdwEIXXQkAxBmSPlU28BKfd3nICl7kkD7wt21J+YC/SrsUt6M/UQTV+xLKUpWgxilKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQEM8UeGXvXjeQqALeoM5iy5tAI5jKN+X1gOKwpuLkV8hMEEdJ1/Cu4GuJ+JrxwuIuqqFlV2yxyWZy/Q1nyw3TRqwZNmmWrXD8Oo/vJOc7lfdiR1AdCY9WNXcTw1WIZXi2rSAuU5oOhkIv0rUYzxVYbJ5A0EfGAY01/Gr7+KbdzIlsEASWgaaaKq/nXFSrgv1wJb4a4Yt+/lacoRm00g6Afi23auh8NwCWLYtpOUEnXUkkySahvs3lmvOwiVSB0Et/Kp9V2KKUbMuebcq7FaUpVpQKUpQClKUApSlAKUpQClKUApSlAKUpQClKUBSqV5e4FBJIAG5JgD1JrRYvxhgrc5sQpgT5Az/AIoCKklRb4Rs+KcRt4e09684S2glmPLkBA1JJgADUkgVyvH8Ss4249+2G927eXMAG8oCEwCdCVJHYjatL498XHiD+6t5lw6fCp0Nx4j3jjkBMKPmdTAveGMv9ntgCIWCO/2vnM1V1EHGCbL+m3kzHxXh61cbaD1ECfWtngOB27cDKNOka+tZjW1mTI/GsxAsaT86ya2bNEbsyuD+J8JgWcYm57r3gXL5HYHLmzTkUx8Q3qe8Ox1u/aS7aYOjqGVhIkHsdQex1FcQ8ZKjKqMAWJBE8gN2HTkPn61uvZr4rTDlsLefLbYlrTGSEb7SnopjNOwIbrW/BjcsWowZ/wC5SOw0q2lwMAVIIOxBkH0Iq5QqFKUoBSlKAUpSgFKUoBSlKAUpSgFKVSgKGuc+JPaHDNawSrcIBBvHVVI392uzQAfMTl2+IVrvaF4re5cbBWCQgJW6wMG432kHRBz+9qNh5o7wLCjMD9hZLFiPM+gUAA6KIJ1q+GNJapfY09P00ss67GRlxeIbPiLrvI0DE6dItoMq+oANYt7gXlyq5H3t4JOnlXv9R1rfqGLbt31MfuiY/qdaojtMZj84IiDz3nX/AGqJTv4H0WLoMWOOmr+ZoML4ZtFSrkuexyhe+USTuN5/A17wA/sdw27utpz5Lm8H9aNuh9JqRnYbducTOsb78tRVq/ZVlKkKyHlvP++g6fKoaUk1LdFeXoYSS/ppJrgz1wisoMyNwRrIPfmK13EOK2sOMs+8uckG/bN0/PoK1ycPuqGS1fa1ZOpUkFlnkp0MHqD6zWXw7h1u0Q1tSzjdnhm9V6f1rVEelinbdr2X6mOPS55umq+N39jWXeC3cSWvXm92xACqkAKvLNmBnfYGdZ7DD/8ADNxHEujAfaHlPfyzr8qlpYr89v8A89Y359t68sYM69iRB9Gnn8zvHKa0ptcbGuPQ4Nk1b5vu/mabCYrF4d2dXZViSySA0AiWViROxggit3wP2mOpCYtA67e8tDKw7skw3yj0NUt2lIJafkR+QO1avjPC0cG4oCsAM0aeX7xB7c+g7V1DTLaSMvW9BauD49zrvDOJ2cQguWbi3F6ruD0YHVT2IBrOr574JxW7gsQLiZpUxcTYXEnVSDz5g8jHKZ77hMSl22lxDmR1DKeqkSD9DVeXHoe3B4e/DMilKVUBSlKAUpSgFKUoBSlKApUb8aeIRg7GYEG6/ltqeZ+00dAPxI61JK417VgzYq04IyPaAXWWhXaTl2AbMCDzg7RVmKGqVBOnZDncfG/nZjOp11OrHfXfepVwm8GVtARoPLBAAErliJGvbUjpUXNv9EB3MCRJ21CgSd920GlbjgGJOU6kmAdcxkiQZJ6AbDbWrsvB7nh7qaj7q/iZ17GuFfKwLgXmRYMZLJghjnDFzuDETE7zW0u8KxKsVN0uFbKVTDM1yTcNvP7s3BNqQT7zNEDatcmGtuHRs0OS5TM8SDP2NQJHpOuule04TamSmctoZZ2MdGkmdP4ddKSyfS9W5tqdL5lzF4DGJn92wvZVslCllsl03nK+Rs0ZRlUl+6zHPKxfDMTbS85v2mS2gdWFkkOAtxjBF3MIa2VzDMdVJAExjLwfDzpaQ8uZk9teUbg8xpVX4Pajy28sTqruAJGvwnoTOnP1qTj/AE3V/wCT8TI4ewa0jO3nZVLRl3InY+YfLSr5UDTSY5kxz9IHevFpcqBBoBAAzcgIGh127xXpNd5MbET6/wBGKk9SKaW7MvhWUXFJWQ0KPLJDEgg6ggAZYLENBKwRM1ZxBVnJUDIVEQMsnUZyNlJI2AggZgPNp5tPDBg4BkNCkEnKZyMQdGkBo1JjcwY9XrTqATLSAC0RmZQFzEqzTKgazB+ek1sePjy6utbvnY8CycpnmfT81HXrXn3Q1SJDCDIjfSNfX+tKrcv5VGu+8En8DoRvt361iX8SYmYiTAG+UHf5fZ569qg9mm074IpxS3HUgfaJMRGgM7GZ6z8q6b7J+JG5hblljJsvprP6N5Zf3g49AK5XexRJaT5IywCYI5lQ+2p2+k1JPZbxH3eNFsny3kZO2dRnUn5K4/zVfNasbXtufKdVpeS49zttKpVaxFApSlAKUpQClKUBSlKj3inxAuFtkLDXmU5F5DkGf9WeXP6kQ2lySk26R641xu0guobgHusjXo1KI0lU2gu+XKF3hp6Tw/jXFHxF25duHc+UckQfCi9gNPqdyat8Su3A7szl/enM5mM7TmOdeoMn+tNbeu6RtW/FGMVaZE4yjLS0ZmExHluSdI0B0BPKQNWPbaq+FsSzYh11gIY7EMDtsP8AYVpL94gZRzO3U8hUh4BwjFYa4j38O9pLpKqbi5JYKWjK2o0G5EaVnyyt0jf0uX/kxpvjb7k04fZa5cFtMpJBPmJUaCTsCT8+3etlw3h5uiwQ4X3ouESCxX3bQREjUkzoeR66WPD+mKssepHYg22jfn2/lW94TgHRLAlQbF2770T8Kujkbf40OvKamCTW5t8R6nLilpg64f7mvtcPJw73wwyqH8oUkxbJVoJP6piQY01q9iuD3LbW1zITcOUasIaMxkwT1M6x862PC7ie5sIIZLr3x2YMbr/kKvNd97/Zbg5Ym8PkgxKD/wCAqxxV8bHlrxDqL5/A0N7CXFS8xylbLFXg66KrErKSdHG5HOrWJ4fd96LOTNcyhwFYMAJIzMWgASsHroBvW+tOoTEB/hu4l7Z/zqqCPmBVcTcJuYzJPvPcWwsb7XSMveW/KmlexZDxLqF3T+hoLuEuLcFtlYORIUEEwATKkHWMp5jbarAYBSxUoJKk5Sq5lMMs5Y0KnSZ07VJLKn3uDDz7xMPcZ51IJNldep+L6GsTAOvusCLgg3bly7DcncXGWR/jur84poVX/O52vFMupJxToj15gdiHAB5lx3329NtK1fGMV7uy+2sJqTqTpAIM9dZ6Eds/GYl3uO75Q85WKgwSgCGJ5HLP/FR3xbiMtu2OZYkRGwDDQdNSOxqprzUe3kytdNrlttf3I++bMcxJPPSI6DfXWdeelTHw5aGFvW76kXTlDjyFcqMss0STmyn8950hVvQfj/XapUtvHW0tm2rWwPKotkMZEEs5EjUp6DVTEnNfli3Ck6v3PnMEoa3KUW0ux3m24YBhrIBHodRXutF4UxbXLCh2LXE0ctlmSAwnIAuzDYRpz3re1iKpKnRWlKUORSlKAUpSgKGuT8Uvm5ce4dczEj0+yPkIFdYNclxSn4BupKn1Bj+FUZ+Eaemq2RjjvDluDMBDjmNyOlRfG2wsQwZSJUg8u45Gp/iMA0iDvy/iK98N8PYVLdwXMOt93fNmuFgqDkqKpBgySfNrp0FdYM+lVLgtzY1JeVb+5s/Zb4Jte5t43EW891295ZDTFtB8D5dix+MEgwCsQanXivCJcwtzMJyD3inmGXUEHlpI9CajGG8R4gMNoGmUKoWOkCCKy+LeKEfD3LbIys6smhDASInqfSK6WWLdlUMM4Ti/iiIM5ldN4/4k7czr/wA1ChpUqCNZkDrO45H+NWzdtAwbi8txMbaxNZOQSQCGE/FGWR17D6fSrITvhn08J4sj9/oY+CQMWVlXU8480HYdeU7GOtXMK/u3YHyx8MQIPI/SdYrHsvFzoD100666a+v0q5jlAZXGx23201Osid/mN67U2lydvFBuml9jKv3SAJZonMR5x5pnMROXNzBGtLeNuBy4dw52uEkmNIzZt10G87aCYNVv25VdVMfrE7/qjb5b1inywJPURpPUDnOo2766VLk/c4XT4WvSvsjPXiFwM10ORciJYSf8JBHw9oAEyBIphuPXTd94SHbKyDMAAoLK0qJENmRTJ6dhGNbY5SB6+s7g9/mTBFYVm3FwEAmdfhDR6AwP651GtrucS6LBLmK/IvJt2BjmYnfQ8+Uc4aoZ4txB97bT7qk7z8ZHPnoo19KmDgBjI0IPaeZ0+h6gGeVQrxFhnYLigP0ZuvZ9HVVuCT3F0gf4D1qY+5k8Vnpw6F3/AEMa0ZgfWprhvFC27FtQHe6oUQ0ZFKKFUkkkmYZiI1zDUFai/CuHG4oKsPQBnM9wBpW94RwC61xFuIqh2VZczlzMFzBVOuhmDHyrRLJia8z4PDxwywdrZPvzsSj2a+IrlzFPauRldNIDHzoBGZmJb4ARqfsiK6tUQ8P+AcLhLi3Q1x7i6hmbKBoR8KQCNdmmpfFZcji5eXgqbb3btlaUpXBApSlAKUpQFK5/4w4a1m7/AGhFJtufPH2HPM9FY8+s9RXQKoROhrmUVJUdQk4u0cYTFn+0PMaW0A7TJJ/Gsx8aOwNSbjfgJLlz3ti57kkEMhUurakjL5gUMnlIjlUP4jwm/hiRdTKNg/xI3SHj8Gg9qzyxtGyGZSLju+p94oX8vSsN7dtluMWuXjbRnuRoqKolmyruB3mtS+NBfQFm2yyqgnsP96mFvgd0cOxV++PdRh7+S0FykTbZczn0J8sdD2pCFs6llSICvEcoUjQEAx00HMdP5Vu+HYrOTyE66QNRtB0G/wDvUGxL7DoB+VSzwu0grPQ9OXer4vc9nps7k9LNnjxBDToT3Hy05/jE71m4s5recQxj+j/QqxjrWYT205QvU9J1OsgA71c4ZcDLlPMaekHXTWTP0jfWre9G0u4HETbWSTEiM3flGo+f5VYuIYM7b9NtOcToSOm9ecIcj5Z0k/c39evr2rLxdoSCNOh316T19ATqKconZbHjCsWUGP5GOhPI9hGvOsN2hmMAga/BInvrpvvVzBPDZdunKCOR+U7nke1Vx9jylgAO8HTrB5eka607A84q5NsvzAEfM/hG/ar1rhS3eBY0gAm3iGuoSNvdraVyPVFcfOtdi3IsPk+zlJnn5hppy7VOfBOCz8FuIR/5y4rQ66M1xR+AFdP0WeH4vPzxj9Tn/A8RCLUiS8QFcbqQw9QZ/hUF4TiSLQ+X41NuHapr0rzpKmUrdHXbbhgCNQQCPQ7V7rS+E7xbC253XMnyViF/dit1WxO1Z5clTaK0pSpIFKUoBSlKAUpSgFW7iBgQwBB0IIkEdxVylAYGG4VYtnNbsWrbdUtop+oFa/xsf7hih960y/teX+Nb6o347cjBuB9pkG06Z1PL0oW4I6skV7tHz7jMCQ2lb/gdsqR0EE8+3ash8KCJ+v8ADtM9evKBV2wQN+XSG0neOQ15aVwlTPqMOFQk2jdXgGTY67Deeo6xEgwZ1HWtUGKF2WcymZGoifN+fMVtrNwMk6bctYXoe579tawrohlfmfKw/VO0z3158oOlWyNKLfESYS4s6neBv0zfw5VsLDh0mT5twN5GvbbfU9Saw7dsG1ctkS1tomJ05ayB8qt8NxGVijfTTWNQRyka+umlQnTF2VvjKytI/wCDymAI7dN6v4nzITudDzkjnrtHb+VX8bh8wJGsnWOROzehPXqTFW8E/wBhjqBpudtYiPznvU1vRKfc11vzBkMeYEb9RGvI/wBbV2Dw1h1t4TDW12W0g13nKJnvM1ybGWMrFh6z6nYb8ueo1EjpPPAfGQ9v3DEZkEr3WeQ/VOnT6aRvweT4th1QU49vyORrgvdXr2Hg/o7rpr0VyFPzABqbcPtworC8YYMJxS8eVxbb/VAh/G2azrDwKxZPVRix7wTJr4JP6Bx0uMP3UP8AGpHUP8A3ZGIXo6t+0CP9FTCtMPSjz8qqbK0pSuysUpSgFKUoBSlKAUpSgPNYXFcAt+01tpAMajcEEEEfMVnUqSYtxaa5RxzimDbDXlsXyAXkowgi4sxK9G2kHXffesd7VvyedeciVO+mw1n17V79rGKR8aqAyUsqrcwGLO0euVlPzFc9vIWIbMZEanUiNBrvVv8ASbimj18Xi7SqS390TrAX8hKmN4HUc53nTf1jrWRi1PLLDzHLXcgxp+HMaVz+/iLjZc/mAGwMek1scFxt7YKgM6EQVckwP1W5b7dvpxomtmjbDxPDJ80SDD3IuR99cpnky+hjY717xWCZSGUa7jcExG0azqO/pWhv8ZDMrrmRh1g65SJ0jr+HeqHxRdgjKrDadthE6eprnQ+6Zc+vwf8ApErwOPR1ytAfUATGYcwo6gRpJJk969W2Ct52ACiQSxUBe5Gv0qA4zizuQ2XIwMgpI3EH006RWS3G79y2qMBOxc7svIECNe9dRjN9ir/c8KtWTi1dR11aViQZ0jkZ5eunKtx4b4LeOItXERrVtDmLt5ZEfCi6E5pAJIiJ51ynM7CHuMVP2RovpA3+dfQvg/GC7gcK4bMfdIrHnnVQrg98wNdShKKTZg6nxXWnGC52t/sQ72k2MuMw1z79tk/Yaf8Au1hYcSKkvtPw84ezcH/TvCf8Lqyn97LUXwp8s9qwZV5jPglcPkSbwC36XEjqts/Qv/OpvUG8BD9NiOyp+Jb+VTmrsXoRlz+tlaUpVhUKUpQClKUApSlAKUpQFKx8diRbtXLjRCIzGdoUEn8qyKjHtExPu+H3oMFyifJnXMP2c1TFW0gcXxl9rjvcc5nclmJ5sf4Vg3LI59vrWQWrwdxXqUqIMZ8JOzEf186tHCuPtflWfNeWNQ4IgwWsXROorytm5HLetiTp8qp/X4VGhAwlw78/4fzq8uGPM1kDmKE10ooFpbcV0P2WccFu62Ec+W6c1voLiqcw/wAyr9V71AZr1hsZ7m5ZuzHu7ttz6I4Y/gDXOSClFok7z4zsZ8DiR91M/wD7ZD/6a55w5/IPSuqcTt57F1d81tx9VIrknDz+jX0FeJm5Rt6V7NEz8Ajz4o/+kP8A7P5ippUO9n40xB/WX8m/nUxqzH6UUZv7jK0pSrCoUpSgFKUoBSlKAUpSgKVz72vX4w+HSfiu5j3Cow/NxXQa5X7ZLn6TBL0W8fqbQH5GrMKuaIfBznNSa8VQtXo2cnvNXpGFWGNY91ytQ5UDMOmnrFXGrXtiwRP4dDWSt8EUUkzouO2oqs1ZY16RqmyD3VjE/CavE1i4x4Qmok9iDv3A+K5+EWsQTJGFlj1ZEIb95TUAwV4BAOgFbAYk2uHYTAL8Xuka8ehf9J7v1lgT2gczGv8AdQK8PNJOVI9DpoNRt9yaez+5m/tGmn6PXv55H5fWpnUW8AoBhmjc3Gn9lR+VSmrYKoozZXc2VpSldlYpSlAKUpQClKUApSlAUrk3tossLmDuDYpdU9iDbI/M/Sus1zX21W/7vhn6XWX9q2zf9uu8T86IZyb3lUz1IsV4TfdCx8mfUe8AXq7WxmWQQYyfMwY17eHb0gDISYgFjbJnaBeCb8q1LqIvv+hY8GVdm/luam4s/airLW7g2YMOkzV8qn2iB61YdLI+0f8ALXcv5uUmFdBG4iruFeD614uLJAQO07CCSfQDWvFtqzp1IG3R6uIawrT1nYO2bjqixLGBOg+daVLawGesS4c7on3iAfTn+FSOx4buuQJnMpZQtu6SyjdlzoqldRrmjUdaw+H8LNu/mIZsomWyiJEyVBMaH7xO+1Z83UR0umXrBNNWq+ZvOHYubjITMAakkn5k1t77aRXriPA1w+Gw1xlHvrru7nmFZVKp/lUL2BLferRrjWOfSYMf19a8qUaZuhNNWdP9nrzYujpdP4on8qllQ72aof7Pcdt2ukfJUSPxJqZVph6UYMnqYpSldnApSlAKUpQClKUApSlAUqCe2K3PDp+7dtn65l/1UpXUOUDT8NxblUUZSYuEKwlBkvW0V+rOM6kToMvpHjH4hfKzhpdrIXJAhrTXAM0jVTnPfTfkFKzs9rQoz2ORqPKp7D8qocSo0yClK9OTo8N8kh8BJn4pgw2oLtpyj3bmI+VRvHYb3V27amfd3GSeuVyJ/ClKol6h2PNs1ueAH+8We9xR9TFKVZ/1ZMPUjqN/HXDYXEKtsq63TDAgkhGua7+Ue6OVSWAkbgCOacZx91Lb2g/xFs5hQWKsUBkCdlpSsMd6+hvzqpbezJ7474hLYVACAthP3xrH7AqM8JDXTZtrAa6RBMwC5O8awKUquXqOIOofQ7dwHhQwti3ZDZsvxMftMdWMchOw5CK2lKVoMrK0pShApSlAf//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBw4LCggICwgICAgJCwoLCwoKCxsIFQcWIB0iIiAdHx8kKCgsJCYxJx8fLTEtJS4rLjouIys2ODM4NygtOisBCgoKDQ0OFRAQFSsZFRkrLTcrNy03Ly0tKzczKystNys3KystKy0tKys3LSs3KzcrKystKystKysrKysrNysrK//AABEIAMgAoAMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAQMEBQYCBwj/xAA9EAACAQMCAwYCCQQBAgcAAAABAgMABBESIQUxQQYTIlFhcTKBBxRCkaGxwdHwI1Ji4fEkchU0Q3OCkrL/xAAaAQACAwEBAAAAAAAAAAAAAAAAAgEDBAUG/8QAJxEAAgIBBAICAQUBAAAAAAAAAAECEQMEITFBElEiMnEFFIGxwRP/2gAMAwEAAhEDEQA/APTKWiinFCilooAKMUUtABRRSOwUFmIVQMlidIUedAC5o+RrHXP0h2Kz91DN9aUBstHGzBjnoQCMVXcX+k+COPRa28xuW2PfrpEAxzwDk+2R7io8l7JSbPQgfuoIryfg30oubjuL+NBayPpS6gQxNEOhZSSCPY5HrXpA4tCgj725hUSjMZLBNfmN8ZPPlvsdtqE0waaLDFFNx3KOAVkVgwyPs6h512Gz5H1HKpIFpKWigBKSuqSgBKKWkoAKUUGigApaBRQAUZ96M1Q9q+MNYWMtyigzkMkYY7KQCST6AAn1OB1qGwOe1nauDhUDMWSa8Zf6VurbuTyJ8h6mvF+0fbi/v1kt5bt+4c7wxAQJjy2GSPc1W8R4jJM09zNI8k0hVdTHUcnf9PzqnA5k5Y9d6rtssqh+KfIOosAdiVNNyEA4xpIOzL4dVdxRZBdfhOkHfzqRf2mGIU6tCpq98D96i1ZNNojxvkEZzjc/5Cn2unMYgMsjxI2pELlgpxjIHLlimrCPMscfRi6/LBrp4vD/AHAK+fkdvzFF7hVomWvGZotIWZyiHOhnLBf5vWos+3ioihlv4ZQFGu2kjiDHPMgKCR6AjOOe9YcrpY6slVOCo866aMjJwBnfAPw1K2FPfOy/albvEB4hZ3jd2rxyYNmZxyIIOSCCRsM5BzWsR9WdtJHMV8sxyvG6tHJJC45SIxT8RXo3Yzt3LbyQ2N/ITGzIokY7aT1GOR64Bwd8b82TIaPYsUVyuxAByD0HL5V3TinJopaSgApaKKAAUGlFLigDljgE+VeVfS72ljAXg8LB7hWD3DqdQgBBAT3IIJ8tvl6TxviCWVld30jKFtonkwftEDYe5OBXzLdzPPcl5CWlkfvJHPNiTkk+pzmkk+hkuzu6TVGQDu2lx7gYx+JqsR8HOx6b1bXBCtJyZYy2QD8WcfrmmbWxMrDAOSyqFxuxPIVV5JK2W+LbpHNsxCkAEow6/PH4n8KHkfU53PeBdR+Y/avU+zHZuCS20yQeKM6XLDfPWrNuxNmTqEbDblnUKoeoV8F/7V1yePKcSGRQQUV9HuSTn7qbE2EdOZI0j8f3P4V6fxDsAjMTDJpDc1aqtvo9dVcmUFvsjFSs8GQ9PNcGAmYsx07AtksfP+ZroSBRpyM4wM1Z8b4DPayiMnUDupA01V9yxjJ8QZDv9qroyUlaZTKDi90cai2xYkDYb6dqm205SJkdi0bahp3x1wd/Xf8A3UBJSpHw7dNIx+VSJWMi95sCDjSAacQ+h+wnEPrnBuGXRJZ+67p8nUcqSuT6nAPzrRGsD9Dt3G/Bzao2Zre4lEiE7qCAQfbfHuDW+NWLgR8iUhpaQ1JAAUCgUtACgUUCloA84+mXiBituH2fiEd1JNI+PDrCgYH3sD8q8aRlJaQM2olsqeVe8fSvZxS8Gknl7tWtZEeN2HiydsKc8ztkbjA9AR4J1wGAB3yBVclvZZF7UOQnLZIJGcnb4jXpfYbsv9YhivJ2MKd4siIo0s5BBBz0GQPXA5ioXYPs1FLGL2dTMucxK42zncnzr062KRIANIwNIHwhfSsOXIm6RvxY6Vvsfis0SMRxqsYA20j8aaxjNPRyatW4rh0xvzzyqllqvsa08qUxjegZyBg05p5b70tWNZlu1nCRJGsmBmM5yOeK8zv4RHNIhGksyA/5chXtt7HrUqcZxXm3bjgZ7trqNWDJ8ar4tQ8x+FWY5U6EyR8o32jBPDiQDGATg/41wTpkkTcgbZ9KeSbo/iHIedRWGqXnkEZzW9HOZ6J9D1wqcWkheUxma1l7uPpOQQcH2AJ+Ve1V4v8AQ3YrPxC6u5ChezjXu0DDO5O+PIY+RIr2g1bDgrk7YlBpTSUwogpaKKAFFLSCloAqO1HAk4rYycPlkeEOyOkigMUI5HHUem1fP/G+CSWE0sUi6gJHRJEIZXweYPqMc6+kbuXuoZpSMiON2x7CvLO1/CEn4dbXRk0XXeQqq4Ld7kjY+u5wfSs+afi0vZqw4vKLl64LThEiWXCLNsDIhiwMhe9JGcZqJcSXdwwlwVRRkBHKhdtsb4NXYtE+rQI66xCihfDq07YqluPrjSlUtjFb8o5JCVVBjmQCCc+4A9awxabNzTUfwVZ7R8StWEf1ORsNksy6i4FX/BO2H1l1t57d4J3ZQFxtmsFeXN+zzGZTCI90ZIjFq233HPfHnWz7FSPMivdQISmlo5MBSx9R0pppJCQtvv8Ak2Bm078lG5P9oqj4n2utbUkGTvGxnSoLGr25RSrA7gjTj5V5f2nvI7a4MMNiiksv9R01as+Xn99JFW6HlaReyduklYLDbuxPVuefYV2eJGaORbqBkhkGBJp2wfPP5jNUnDe0kUcosvqd13qlV1rEHDHOMADBON+R6HnWjsL+G9yqkMcfYJx6gjYg+hppKuiISvuzzPtHwJrZ3lVg8Qff/EHkfYiqUpgE4yeWeterdreHr/4bdHA1hMqSN1AIIFYXhPZme8hW4EkNvGpZV71tAc/zb5VoxZF47vgzZcT8viuS4+iLhFxPxSO/jylrZljLITtkggDGcknJ35DGfQ+71lewnZSPhEMjrO1zLd6GaTGkYAyAB05nqc7VqTWuPBjlzQUlLSGmFClFJS0AFAopaAGrmPvIpYyMiSN1+8V5vxyX+vwThxOoJNFLJj7RCkj+elem1hu0fBNNwb2NX76FoiACMMuefLOwHT1rJqVw0b9HJU4tlrbDIx0woxRdrpXnuRyI1Bqas5R3atkEMFINd8UlTuQ4bBxg5PxVhRuq2Zq74Yt1IA0sca530R71oLS0jtkSGJcIu2T4ix9TVFwy7SS7ESHXIAztgbIPWtJBGzyBSVTGpgSdIwBRuS0kDybgZ2PIVne0nAEudNxHL3cq7YPJqvZYzgSAllU6Tn76gcUu1ijXvRoWQ41jkh6ZoTd7ENJlVwvhfiDPBGZMaTIrBSwxjnjPKr6DhUSYYW8UbgfHGNJ+Z61A4TIGbSG1b7Efaq/lbQANQY4zU263IcUuCn41bCW3nh6PE65+LpVBZ2kMvZ63MQBkRdbsCco4HkeW4PLnmtDxSTEUoGMlGUfZ57D86z/ZiycTXFggd7FisaO66Q4JGD6/80RfS7GSV2+kek8IjKWdopJLdzESSd8kA/rUykVQoVQMKoVQPQUGuvFUkjhydyb9gaKKDUihiiiigApaKKACovELbvY2ClQ4VgNS6gw8jUqlpZJNUNGTi7RjYDhcZHh2OKzfajiTDubaLLSzjK76dvP2rScUjMVzcJyLNrjG2MHfP51Q8d4U0sK3ELf14omiGBvjIIx8hXKa8ZtM68JuUE16OuzohsIJSx7y8lP9SQeLV5Aegpo9oikru5unjyoIADCI+mwOPcmoPDbC+iEE7TxzWj6u+zF/UtSfmARyq6itO/YAXViV7xkBmtzEWAGQd+f6Uz5vklJ16IU/abWrJCJA5OzAbKOh3G9TEukvLd7S6UuJkVde2V8jtsDTj2DLCZHveHRIsjLojiDnAB3G+cnAwPWqO/ub0PHFbWkV+jhdbKn1PuthzJ+f3UJegf5sZ4ZLJYXItJSzox/pS9JR+9bGOb4Sc71lrGGW6jWCaHRPFMjhidXdY5kHyI2+daZlAMa7+EYwPaq5ux4t1uclFklEblTEPjVsYceXzxWl4RYqmmYRhEC4jjxp0jlnFQ+y0eprq58BUMsSsOakbkem5rQ1u0+FJKTOfn1D3ihKQ0tIa1mIKKKKACloooAQUuKKUUAFFApagDNdsxoS1uACSJGjYD7QIyPx/Osld8QbRpVn0RnU6Y1a8Dz8hWx7Yt/08YC6jqZ8fFqwR+9YXiBETsMt3Eh0K6gychyPkOfIdKwZ6c2jo4LWNMu+F3GtAQRqdcYOcN7+VNXt8kJAkhMYA3Ma6Q389qh8E4god1ZVJB0hgQ2rkNz86vHijkwzCP2Kht6z8M0wk3wyrtb+KR9Kgy4ONDcv+KmXMwjQghUUfEq4XY0JDFGwwiIWOBoGnb2qr47dhJEjVteSwKjwjl+mDU7vgmc2luyZZXqsryKEGo6SB4vL/VN3F2F1nKFVDHAOkt6/lVbBI0MSRBYzJIq7AlCnkffflUm3tvADIS5kZV/uG5HLyzyqKSEttHoHZ6Hu+H2QOolo1c6ueTv+tWJqPw7/AMraf+xD+QqRXWh9UcmX2YlFLSUwohoNLRQAUYpaKACgUYpagAopq5uEhjknlcJHGNTMfy9/SsTwTt/NfXd1bR8DdLe3leM3b3OkLg4AI07nrgHbzok1FeT4HjBydJFx2lbVLHFjUFj/ABJO34Cszc2qzxy27kp3mnSxPUeWMcjV5OzP3kznXIx1H7/2qqEXikJBYEbq3i6cx061yJz8puSOrCHjBRZkLq2uLF2li13EMbb4JkK4/TarGw7ToQBKCjeL4jp2/gq/ijDZXCs2nl8IYdB58qq+IdlopgWULDIx3KHR/o06mn9kL4OLuLI932ijUErIC3MYy2+euOlU8V5JeS6cFFzKWyxUvgjGT0ABGfQ1YxdlRGy97KXUHc6tIx6/jVxBZIgZFAjTGQFG2fPGPzNT5QS+IOMpP5ESxtcASu+4bSxPiGOuD5e/rV0ihir+ErhcYxjYbHHnuPbFMJHsGJJ33VDpG/rt91SbUaiWyX+HSSfhHljFUt9liXSNhwptVpanyiRfu2/SpRrGp2mbh9xa2tzAg4TKe6F4mc2chOQHHLBJxnoflnZA8jkEHcEV1cUlKCaOVmg4zdhRS0lWlQlBFLRigBaKquM9obPh4xc3aJLjIhT+rI3lsOXucD1rC8X+ke4lZorC2jtI+QlmAnf3xyHsdVWQxSl0OoOXR6JxLidvZR9/dXMVrETgGQ7ufIDmT6AViuO/SRGqtHw2Ezy8u/nQoqew5n54+dYC+uJ7uRri6uJbmQjAaRi2kZ5AcgPQbVzFBsT/AJLWvHpkt3uXxwLsvZ+KzXFx3088kwkCFdZ1BAegHIfLzq37MzCK8uLIqAtyGuo3z8ZwAR6nbP31SQQhlVcZK7qPTqPv3/4qWEZljkjfRdW764pPi0nmPkRtjqDU6rSrLicFz0a47cG2nj8IHSoMsIbpz54PnTnDOJre24kACTo2iaEneBhzHt1B6g107c9gPMf215SUXFtPZouTshJmMkbspKkZb4T7n50AN4gxP2iNXl+tPyjmQAQOYxtim3kGd/Dg4OTQTRFOdQyWz4V2JYflzpXhz/UwGOhkxvzPM786dLg7BiSOp510CSvLryPhFTwDQ3HDqwdKqwCqWI1dPx/ep1tHtjYkBQP8abiX7OCARsf5/OdTIhseQx16VHJD2KftMoFnJGcFrhkiUHxasnJPyAJ+VV/Du0tzZuyLKZreKFz3EniG2MAHmNs8tvQ4rni999auAyHNtCrLER/6vm3scAD0BPWs9dyaVfq87f8A1A/n3H0r0eh0vhh+S3kUZKlyj1LgHbKy4jpjWX6pdHY285Clj5A8j+fpWir50aLmRkHOa0fBO219YBY2kF9bLsI7jLFB5A8x88j0pp6Z8xMcsL6PZ8UCs72c7ZWnEgqaxZ3h2NvMwUsf8TyP5+laOs0k06aKGmnTPn0hnYyOWklcszOx1Fj1JJ506kYUeZPOnAmM7b0pFdlRSOilRwRz9v1pwjCj3pSOft+opXHhFNQyRNgkwFPXnU5Dkg5wJBj/ALT/AD+cqqoTsKlQydDkqdmFAwrzSwTi/tj/ANRENM8XS8TP5itTYcTjvIxNE2TjEkZOkoazksJbTIhxKu4YcpR+/wDPaIyOr99bn6tdKclD4Vn8xXJ1+g/6fOH27XsE6ZtHO5+z6+tRnOTvpYdfs1A4RxpbnNvMptrxAuqNhpDHzHmKsHt9z8W45jxV5+UZQdNUy9boFQfFtj/807GOZGRj01UkUBxnmfEKbvrlLeNpZJNCgqB5t5AAbk+lLu3SB7EgNjJJGFGSxqo4jxP60DbwlhZjaSQHe89B6eZ6+3OunuJb1iXBgswdoSRmX1Y9fbkOuejjyBVwuFUDBY/Zru6H9PpqeRfhFLdjM5ADZ2AGHONlHkKp7nxFpCPQD+0VNuJNWBghQdh+p9aizjwmu1QjIgTbNcPF0xnapAHhpCN81FC0QWh5D51oOCdsr/h+mMy/XLVdu5uCZNI9DzH4j0qrI3X/AOQoaLPSkljjJboVwT5J3d/OnlsxIp0khxviujEAzIJCpBwVkGnT8+VSrRShD7Ac8jxBhVhcinwQGBG4DA0oO2OdW/ELUSnvIgSWGHGNIzVWsLAkFSN8VJFCIMdKdVt/KjR6Ee9C88UATIJ9IIxqU76c7/L+fvUh31rqUJIBzBG6n18jUEWzsMqrHG9C60YZVlYdRzoAdch2RtADIfCw5rVunGAkYMmFK8yeXv8A6quUa92jZT/eBUS8YBWikOQ+pWXSG1jyH7/wY9VosedepexlNxNEvHYnhZ7dlkblt51Uzt3jiaVi7D4QfEF9qh2yBUCoiwxr8MafmalJvlgcgHGoDV8hVem/T8eHd/KX9A5thJJgajsOijnUOWUuegA5AclruVWb4VkcZ5hdNcCJuqMvuK6Ao2RyriYeHFPlD/afurh4WPJHI8wDQDIwG2MVywp4xtnSVZT6jTXTWx05wcUEUQyPhPrT0aZya7S2Y6cowBbnipUcfPYgA7bUAkSOIjTcJIBjUuSKdccmAAYjBI8NFFCGQ5EQY2OlCcYJxqNQMtG50swB6D7I9AciiigGPiQ7bI3/AHLv+FBbmQsZPmV1frSUUAOd82ABox4iVKlh+f8AM0sEhY4ydHUbL+OKKKAHpYfDlSyt6sW/Wubfht1NFdXMCrJDaKrTNkrtnOACMkgZJ32APzKKpyScVa9/6Jk2R1NbTw2lteyQSC2nOElRCwf5dAemTuOVV1xfMgCrEyO5/pqQFPuRvtRRU4pOV37ZEZN2SbSFwpkllkLHfSGKBfkKVhg51OPdi350UVYOjkudjqOfxrgknPifJHRitLRUgRmmcEjURjzAbpjrXS3BKEAkMTg7D9qKKCFyOSEqqnU2fFk53bbzqNbTeKQg48hgZ96KKH0S+Uf/2Q==</t>
         </is>
       </c>
     </row>
@@ -3425,25 +3425,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DONOVAN FERREIRA</t>
+          <t>VISHNU VINOD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>smat2023_134</t>
+          <t>smat2023_132</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>80</v>
+        <v>141.7</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -3452,13 +3452,13 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
@@ -3491,10 +3491,10 @@
         <v>0</v>
       </c>
       <c r="W24" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -3506,16 +3506,16 @@
         <v>0</v>
       </c>
       <c r="AB24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC24" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AD24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE24" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AF24" t="n">
         <v>0</v>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="AM24" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQSEhUTExIWFhUXFhYXGBgYGBsaHhcYFxoaHSAfGBkYHSggHx0nGxgYITMhKCkrLi4uFx8zODMsOCgtLi0BCgoKDg0OGhAQGy0lICYvLS0tLy0tLS0tLS0tLS0wLS0tLS0tLS0tMC0tLS0tKy0tLS0tLS0tLS0wLS0tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcIAQL/xABHEAABAwIDBQQFCAgEBgMAAAABAAIRAyEEEjEFBkFRYRMicZEHMkKBoRQzUnKxwdHwFSNigpKisuFzs8LxNEODk6PDU2Nk/8QAGgEBAAIDAQAAAAAAAAAAAAAAAAMEAQIFBv/EADYRAAIBAgQDBQcDAwUAAAAAAAABAgMRBCExQRJRgQUiYXHwEzKRobHB0RRC4SMzkhU0U3Ki/9oADAMBAAIRAxEAPwDuKIiAIiIAiIgCIiAIiIAiIgCKF25vTg8GD8pxVKmQJyFwLyOlMS8+4Kg4j05YQPcG4eu9g0f3Bm65S6QD1v0CA6wi5lhPTfs55hzMTT6uptI/8b3H4K9bD25h8ZT7XDVm1GaEt1aeTmm7T0IBQEmiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAuZ+mLfo4Gk3D4d+XE1RJcImlSm5vo5xsLcHGxAnomMxTaVN9V5hjGue48mtBJPkCvKbmV9o4mtiYl9R7nkTpmNmg9Gw0dAtZOyMxi5OyI7IXlz3uLnEy55JJJPFxNzJWKlSzOiPhMfZ5q84Dch5EuseU/apzZfo8Y05qjiegJAHv1UPtYltYWRzGnTbBDmukHgJBHiPtst3d7b1XAVu3wz3NcC3M3QVGg+q8GxBEjmCQRe67RQ3foMbDKLBH7I+JVf3o3Rp12GGhjuYA/BY9srm7wjtk8zqm6m8NHH4duIoOlps5p9am8ASx44ESPEEEWIU0vNHom2y/Z20xQqktpVndjUF4zn5t0fWhs8A8r0urNyg1bUIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgKl6VqzmbIxhbqaWX3Pc1p/lJXL/AEf4INw7XAXdcn3rrHpHZOy8aP8A81U+TSfuXLdzqgp4JjjxJ+02+Cr4jRIs4X3+hcaUDQStiTyhVavt2vRbnbQkHi5zW/AmVI7s7yOxTsppQecgjzCg4ToKa0Jum88BKx4kTNlCbe3sqYV5Z2IPiQJ8FiwW3ataCWMvoA6/xj4SnDkONXKd6QcL2dejWYBnzNcBa7mOBEzbovSC89+kWgXU6bwDmBc0DUz4cTZegwrNB3gc3E/3GfURFMQBERAEREAREQBERAEREAREQBERAEREAREQBERAU/fnEPllEPDaNWlXFYQCXA5GgXBEEOePeFT9ibLy0exafVfUDSfruj4K1+knCP7EV6Mmq0OpgDk+CSOoymI5lVTYGIAL2D2HEX1AMOEzxhw8lUq+9mdGgo+zi14mB+6IFSnUPfcwkk1Mru0nmC0lovo0gaeKldi4JuHPdAEnh1Um6sIkqD/ShDmnsnuJLoAEAAGJJ5ngNei1bbyJ4wjHMltqYFteCQMzXZhI5RY9FHbN3QpMZl5PL80nNJJMST6skmOZnW63cLtN1R5ig9vcDpOUtcPOQ73KTFbuys3ehlxTdyB2xgGOfRDrtbUBg8TDgB5keKuW5zA2nUaP/lJjlLGaDgLaKibbxM1qVKMxe4mOYY1zre8BdB3SpxhwXeu4y/6wAH2ALaiu8QYi3s35onERFaOaEREAREQBERAEREAREQBERAEREAREQBERAEREBp7UwXa0yyYNi08nDRcm3kwVbA4ttSply12kd0kglkC5LReC0e9dlVJ9LOzu1wPaAEuova8RqWnuuHkQ79xRzgmrk1Oo1aO1yqfptopyBJPw8VG4LFZyKoY6s7k0d0cNdJhQ2A2qxroIBuDMTaxt5yrIzaD3tPyctbw0sT4cFVas8zo05pu7M/ea3MKNSlkaA1057N+lcmYA4StrBbfDqWZ1yNSBGnAjn0WDBYvENaXV3sIuQ0Rbyjmq9tvboLnER3hHC5mxP849x5LNm2ZqSisyY3ZacdtRt4FOi90gTGjYvxOddfwmGFNoa3QcTqTzK5z6F8MHMxGJI7zntpj6rWgkjxc6D9Qe/pytQikjm1ajk2tgiItyEIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAoreIThnz+x/U1SFWoGgucQGgEkmwAGpJ5Lj1T0gVcdtHsKRy4Ps3w0tE1Cwgh5JGZsmIaItE3kDWafBJm9L+5HzKFvZs04Oucomk6XMPLTunw+yF+Nn7whl8xBtz+9dJ29sxuIYWPHgeIPRUHF7hPLu48AT1+z+6rxnFq0i7KnKLvEVt7Q+nkdfj1n/ZRLC/E1QykDLiAOlzfwup+l6N3NgveSCPZIHx8vNXDdndmnhrgS7n+BW3HFLIx7Oc3Z6F19H2DbQomk3RmX3kgyfEmSrauZ47fWlso5q1Ko9lQhs08stcA4iziAZE8eCuO6m8tDaNAYjDk5ZLXNcIcxwgw4AkTBBsSLqSlnBMrYhWqP1sTaIikIQiIgCIiAIiIAiIgCIiAIiIAiIgCIiAItPaOPpUKZqVqjabBq5xAF9BfieSoO2fS3QacuFovru4OdNNnuBGc+GUeK3hTlP3UYbSOlKG2tvHhsNHa1Whx0YO88n6ov7zZcZ2tvZtLEuDXVHMa64p0f1YIHMgl8cLuhYzsftO+9uV0OzSIuRDfG97SpnQ4VeTLuFwc6zeTytlpra+bWWTvazbWdue3vn6TauLa7D0KZpUHAteSQX1Wm0EAQ1pEyASTzAkGp7Br9hiqVU6B2V31XiPIGD7lnG7VV3dzta1tjlBc61uIAb+eS2KO5QIbmfD3AuBeT3ehN5kEcbQbc95ukoezW+r+5PT7Jxd3UceG2aTefO388/M6fTaHCQsFbD6qp7A3jqUH9hiuFu06cCYsR1Cu9SiHgOaZBuCDII6Lj1qE6UkpdHsySnUUtOq3XmjXwtAj1nE+K3qYAC16FAg3K2ax4eajN2Un0kta7CPDhLnFoYOObMLjwE+6VA7h7xu2bWaRei4NbVZzbOo/abJI5yRxkY9+NtNfiNT2VMZWxeXHV1vIHxUC6oHiWOkdPvGq7uAoJUmpay23t5a+PwOTi53nlsem9hbfw+MYamGqio0GDYtLTr3muAcJFxIupZeX92sXWp4l/YudmaKZlpc0kQGwY4SOunJXvD+lKvh3htVjcQwxcDs3tOhHEG/CB4qF0JftJamH4Ye0Ty00+m0tGsm7b5ZnZUVR2F6Q8DiYb2vY1DbJWhhnkHTkJ6Az0VuUUouLs0Vk7hERagIiIAiIgCIiAIiIAiIgC18di2Uab6tRwaxjS5zjwAuVsLk3pq22Zp4JhgECrV63ORp6S0ujmGFb04cclEw3YpO9e8dXaNftHZhSaSKNL6A0k8M54nhoLBZcPs/s+60DtIu497IDYkAcff9qjtm4YOMuDsg1ItHQzw68Psn8JVBpWYW0wSSCQI6CLkRYk31XTqWjHhjovXrmdTsuiuLjnvpzstdnbbvXuut1NYLCtpNDYJe5gJMA2HIkQBrdft4mmTJAm8ggSORu0Hwg+KMpZzBI0BBPJzQQCeYOYe5DShhFr8QXC7baHunSbXErnSbbPT0oxUVb5evVjWcJc4+zA0FzI0GlzyET11WyGxe0iIAJgWiQcwvr7R9YgALFSpFhGYm4gX+idTysQtqo2Bxk+zxcOIkd4SJvceCwSyeaW3pGljMAyq2Kje6JLXR3pmDli8WM2IkCZWlgsTX2fB+dw7jPHuzxHI+bT46TZYDaDbiII5eyB52WkyuQ/IQSwy0AgR1abAXnS3xCkU7Lhkrxe345HPxGBhiO8u7Nb/nZ+T6WNutvjQFwSeOUC/wCA81BYraGJxpLabSGG2VsxH7TuPgPIqQfszD0jIpNcdbh7vhUsI5fat1zy+C0BoAAyiYHwj4lYpwoUneCu+crZeSSt9yjDs2tNL20rLdR/Lzt0IfC7FpUWk/O1HggEtBEm2jjMDnE24SsGI3doAlwZBAAJ1HdEAwY1g6xMcbqdFGXAj1vojQudbhAaY8B3dNSsr6BIBgCWWILgcpJvPEHKWaxA53STlOXE9TqQhQoRjCKVs+XXz5N53+Sgt09nBvaVA0d/M0Q2fmwdZNuN7lfjF7AbXfnb3XAjNOji0ExwI11/2WXBktaxoafnX21E53N0FyeQHGFtEZXtABLWl7cwBkuOpmRxBK1hNxzTJ62Gp1U4yStsraWv8/58ij1dn2f2ckteWuaYBaAM0npzPRb27G9mLwJHY1JpA3ovJLHDoD6ni3pM6Ka221j3im00g+Ic4lplxA7o4gxBnm0BVXFUC1xabEcCI8osfNdOlapG0zyHaWFjRmnBZfLwtyy2vnqrI9Hbu7bp4yg2vSNnWLTqxw1a7qPiIIsQpVcs9DdYtz0o7rmdprNw4D4hw/hC6muRJx4pKOibXwIK1CdFxU9WlL/JX+K3CIiwQhERAEREAREQBERAF5x34x3b7QxL9QKrmDlFPuCP4Z969FVXwJ5Lz7tzdtzK1RrKgqw90yQ1xuTJmATwMXmbRBVjCVacanDJ2dsvjzNlRqVE3CLdtbK9iOwGMDRkfLmHlAk8A5xPq/k203cM3sqpH6szbNBIpW9WeYHPhrF5wbS2YcPTouLie1a/MC3LkIDe67iSC4zPLTikjsw0fNss1umao48SLgA6OvlJm4ELoSs1xR0d/wAfX1bIvYarJ2jK3FHOLv8AL4Xzv4LvPiU7tCow0GB+kMaTdpdkqMLf5KbzM+3YrJQwDa+JayH4ecTUpDsu4atJrHkO7wIc7MGd4A2dF5BUNhcY51QU6kueypSLw4DLLszDAHRzefOTqbDiti0zeoxzwzuCahAa08GNBvH3dAudLKTR0cRg54lwqUpJZWzbTTTfnmnlbbxMjN3gA6oH419TsqNVuGD2NrsD3Pa4lrmkOgMEANB711nr7qvbWoMZiMS+m6s+lVcIPYgim5gs0hrsz4JJIkWi4WlT3epB2epTc4kyCXvM9fWB0hZG7u4WCTTc3jIqPmZGkm944ysFf/T8X/yL/KX4Mezd3sZUw1Z76tWnXaXtpUyA3tezaC4OBGYh0wOt9CE3s2Y7DGjlxD6gqVAwh4ZMZWODg9jRF3AZTe+YWKyt2BRseze1wvLaj5afeZaZWKvsdsgCpWyhzXluclpc2wJDgYMWnkLWWWSUcJjadSMuO9mv3PS/jYkGVW1GtcDwE/rJykdXaeA5hfcusAOMmxJOb38Ock8Oq0sI8seWNIzesA0GRzzDrMW1hboGaSTBmTYRPQX+K1Tud6Ss/Az4RzWubVBGRmZ5zNzQ1rXEnKLZwLht+E8xI7eqsIyh7XvOV8kMzMY5zBmD6YaIJe1pbcHtAQe6VHdofXaGucA4tLnZQ5wEFxLrFokAxaAWmxWviMW4n2HZW0CHA0m/rKbIcH95pLO0hwN8ppiBymjA8tja0XjFJPSyfhZ/PzVjHhsPJw4IHrBxmWi7nPPe1Fxr1XzZ7c5vMMNQkE6uLnGbCZideccF8p95zDYw0mS6xLrCeA9ZReHrlmFqPkMJztBJjvPNu9x1FlAlmkeslnByXq7f51IipXNV7q7qjm03FxbUy6XsHgdIHja3DS2hiC93KBHGD56Ty0TGVG2a0ZXDu1APVJFpHD+3VYHXvM9Cu1SgrJ/A8RiqsuJwvvdvPN9dElZW1Tum5WVrx6NNrUqTiauZrgMoINoPBw5GxnhkXZ15lwJewGqGONMGHuDSWibXcBAMkQvSmFqZmNdza0+YXIxNH2dWVtHn13XT7klevCtSpyv30uF+UbcLXmrp+KbMyIigKgREQBERAEREAREQGDEiWOGliuNbXxFCkQ8io/PUe23dBaC6ajMwuJLYEiZ9Y3XVt5QDhqoIBDm5SCJBa4w4EcRlJsqBtQ4fIGYjs25nSWuHZuBZVdGSo48ab3DNYQGtkzC0UIe0Tkm/Bcv46fjp4GpVp05yhNRvbN6X89sr5v62KltzF0a1NpZWdnZDW03NMZeJiC1rufeIIaNCoSlVLXZm8zHv4hW7ebbOGqYc06bmSAJysyAuNYu7stEhrIbMCypoC7uEX9OzTVsrPll4IoYub9s58Sbed48/Wf2MmHd+us2xp9ZJFRjiZ6AO8JK6Hg6jKjCHdnmAyOB/Z0ymbHr4rltetkcx8wA4Ano6x+1dP3LxDXGvSc1pa+iSBlByuZ3THWXjylU69Ne2s9zvYbGSj2dKqldwel7ZZeD58tjLRe0w0kS2bB1yBxAdxsVm7RrpOZsNmAI8JLSeII05Ld2Qw1MFimQC+5EXzDs25RPiwwVO7SqB5wT7EOewg+Ia+38MrMaMXZXz3+F/yuniVsR2tOnWnDhVk3Z3eebXz1622zrLXj2HAusQc0hs6HNwuIynmF9rMEWnu2mbxyy8evNW/aeHz1aB1Dajg8cwabnCR9ZrD7lH43Z1J2LpM7NoY+m4kN7slua/ci/eF+gWqhBq6ezfPS++Wyuaw7Yafeh1v/HTXVsqOOpwab88xEtAve13cWwTHiVuOpiYYBMm1jmzRp4CTmKkBsZjqOKnMTSrVwzvPgBkFoiYNrXW3jNjsdim0mjJT7HO4NJEgOIiZtMt9zT4pLD8Lavp4crXJ49t03w3i1ry6ZaZ6bWvruocgENyudlnMAMriO9mklzYY7NeByHIIGEggvLjAv3fZLCXZwAdWU/+23kp7FYCg9tUUZDqWrZJDi0EQQ430c2RxbxiFoVMEw4fD1w9xL6lFvsxD3R3WltuEfGVmFGUmknvbO6105lWWOwUlxSp5+CT63vG/nr0aInFnuzLAYc4nIXSO8btAiJNgOBCo+9GJLaOGw4dqzO5sQCJPmSct+TT4LquI2IflBY2s5rW0e0c92UkFznt4Bo0EydL9I5LvrhSMaygx3aFlJjWlonPmLiCAJ9mDbmUhR76d7rJ/da+viWqvalN4aVOldPk9ldppeNnlm93sQ+HHH8z/upvd/F0aVdtSvSFWm3VkAh0kC4I4NLndS0DjK/Z3TxDcO+u4Na2mJLS7vECxMCR7plY9g435M8V34cVWEOaM0gZjxY+DDxGo6+K6CqQqRfC77ZP7/fQ85KEoPvKx1TZu0Kb6VdtdzH0g4sESWPpPY97XZrhoLCBlEZezk3Ku9EQ1oGkD7Fxep6QaT6YoOwnY0wSQaLxIJa5p7jmgOkPPtAzF11jd/HU6+Hp1KT87S0DNxltjIgQZBkQFzsZTs+JRtd9NEtvLdmYN6EoiIqRIEREAREQBERAEREBR/SrjarMIynQnPVqhpjUMa1ziZ4XDRPXnC4viMM6m8h/rG8zMk8Z4rt2+uzhWrUM7jkayr3QYzlxZqRwGX+bxnQw2Hp07MY1vgAPipIY5UFwpXe+3zz+hbp4aFSmnd8XS1vLXPnc5tgdjse0OLng8RlNj+eK0dpYJ1J0CHNOhmD4G2q6+191lfWgJDtaV/d+f8FmphqcoKKik+avd+d29frmcJ2ngy+g/wBn6wNuIuAdYPkrfudtR7X0axa4UyQ13ddGVzYzE6ZbtMj6KlN4sM7F4ilSY1hpsh1ZzpEQQWsbGswZabRBsTeXOfR3uAUdfH8bU0iXCxVKE6bWUlZ9L5r4/FeCZt7HxtDDYhw+UUjSrGGw5sU3DM4NJDiMpzPh1gIA4hb7Hsp/I8KHhxp1Zbpak1jw2Y5BzG9YUC5h0jX3+ap+39vMwdXKxoqVC0B1PRobJIzGJnlbit6GNUpWcX6TV9tE+pVq4WLvKpUt42vyto/DxOw4nHBjMW+Z7KXD3UKZEe+fNfttD9dhjyw9X/0D7yuPbE3lp4ipldSDXj1IIc06kzPSTfl52zD4vIJDnMtbKXjXW7Y5DpboFa/UUVle2Vv/ADw8+vU0j2eqi4oVIvzTW9+TLPRrBlPEuNx8tLD4VKlJh+DzK2auIDMZTk2fRyT+0XkjzykeJHNU3E4z9WWAuyvfnf35aSSDm+lMgE+ErFj8S7NBe59h6z3O0vxM2JmJ1W861OUm1fPL4pLntZ6XJ6PYleVk3HfRt6abc/LLzLlgaHyZ+JrVIySXggyS3M99/wCPKB06rSwNBzsHgQGk5atBzovla2XSekgeapG18XWA71So8C4zOc/u9QXZQ4Q08T3gs+729GIjsmODWXJztB7PNJlugAJNm97joFr+pim3vdPNclbRXN6/YleEFOUk9tdrKzu7XeVrfV6W/G7WDMbUZ2faN+T02PHdsXGo4Ag6ggkG2jvAGJZhKLHveyk3tqkSBJgcAXOkhvT4LVp12U5DXl9R5l9RwJJPMmLnQACwAAEAALNSxVKnGXMTqXZT8eJXOxGJ4+6slZLztuzShh1TV9X69fg3a2D7k13hwkEsPqW07vtXjXjFgtHeGjUxOGNKjTDGOLJfUOXIGkGQ2M02y3jVSVTaFAgEuJdwsbHpMAePmobEbXqPqPpkDs2kAZLh4sZLiAdeA5aqCNbg7y208ybg4009yNw257mMMupVCfpNPwN4Vq9GDjRdiMK5mS4rUxMgggNflPIODf41jw2IlsLe3YoOdig8CzGuzHo4ae8gH9xSxxlSo7Tzv62IcRTSoqK0jp+L6789bci8IiKU5gREQBERAEREAREQEBvUPmj1cPMf2VbL7qz71DuUz/8AaB5tcqvXEFUq/vM6WFfcR+2vX5xlWGz+SgEXWtVGbU/FVy5qVjcqo4vxFRxBD8RUgdGw2/8ACrQ2q2bEeYUR+h2Ml1IZC4yQ0xJ1mNJlYWB1N3fZmb9JpuPFv4LfiNZLIsZp2kcVynffZ76eMe8NnM1jiMrrjoQDcZb8rc4F/qb0UWthtRs8uI8RqqPvRt1r6jTmHH4xzVihK0yhiu9Awbl4TO51TIbFrJcJiJkN0IdmDCZHQC5XRKTJF+GvgFTthbdy0xAFi6w8dfzzU7T2+OIUdaTnLMmwyhCCUSSqYTNePAfiVjfgOSxs2qLR+fFbdLGDjz1UWaLSnbQw/o+bETH2n71tU9ngCIWZmJB0W1TeI10RpvVhzbNXDYIAaaLP8mHH8hZmuEpPCVlRRrxNmE4ZnH8lZaWzaZX7fhg+y1zgatN0tdmHxSy5GOJ8zHi6AYbKx7ks7lV/N4b/AAif9Sr+LY7V3C6t26tDJhmTq6Xn94kj+WFNQXfK+Ll/T6kwiIrhzQiIgCIiAIiIAiIgIjecfqCfovYf5gPvVFxNdwMkWHFdG2nQ7Sk9g1LTHjw+MLn1DFtcIOvIqpXXeOhhH3WiPO0yeBX0Y9ZcRTbyWk+qG+yFWZbMzsZPL+6/XaSbgQtQY1vABZf0gFqbJmvtXZXbCC1p8QFXKu4kHM2Wnm0kfZwVr/SjbX+K+HbjdCVvFtaM0kovUomI3PrUznZUcOenxWE1cRS9ZubqPwKuuJ26DZvgozFY4HRuZScTepE4QWmRFYHbzCYdLTyNvKVOUHip6tQDxGigMZRzC7Gj4qK+VGkbOgDrb+yw4pkftOHU6C2hUFw+fD7ltUMS8Km7P3tbpmE9dPipdm8AI19yw4tEimiyjEOWWnjpIBddVU7dhYK+22njBCG3tYrc6FRxYGq2WYxp46Ll7d6C0QYjnP4rdwO8LX+0B71sgqkHuXfE1e1c1jdXODR4uMLoVKmGtDRoAAPAWVL3H2aXkYl3qgEU+pNi4dAJA8TyV4VmjGyuyliqilLhWiCIimKoREQBERAEREAREQBcj39wpwtdz/VY8lzTwk3InmDNuULri+ESo6lNTViSnUcHdHnZu8gJ9aY5LG/ecGwIK9GNaBoIVS9JmT5DUzNBdLQ2RJEGSRxs0OPuUX6ZcyzQq1KtSNNbtI4s/aZdxAWE4mf+YorCUXFz5mGtm55uaBPmtz5A4ua0AyReZE+eiwqDOgsDWkr3XzN2m4H/AJhWwGUm+tUPn9wUWdjVjIDnN/PMLfwm6DnGHuJIu7U5RIuOchwMcFlUHzJI9nVd7Hx+16LPVEnlr8BJWB23KhsymffACsuzd2qTKY7oLmlw7pJmCT/TeeikKmyGCQA115BGv4EKVYeJap9nU/3yfTIpGNZii0F3cB+PhOvkoStsio+5k+dvuAXUsRssQ39WRA4uka+zyH3rXfsxt3QCbGG8Gi7jHQDUm/JS+zitET/ocO1p6+Jy07LcDHHl+PKwK+MpVG2a4jwNvwXQcRsxpBBAyk2iSASOHFzoWg3Y5dmcRDh6w5HiSdBfQI6aNH2dTvZaFXo16v0p9wUrhKOYDNBk8z8Rw8VIOwMunlEwCR7zIv0HVb+Dwc1MxIjXu62Hsh1j4FYVKKJKfZ9GOcop+aR0L0ZYGjkqsNJhcC10uY2YcNJjoD+8OqvJ2ZRNzRpyP2G/guf+j+rkxJafbY5trDNZ0Rw9V4jhBHELpiy0kee7VoqniXZZNJ/Kz+aYREWDmhERAEREAREQBERAEREAREQBUz0m/wDDDwq/5ZRFhl/sz/dQ6/RnENk/cf8AUpDE6/uH+pEWUevp+8iybC197VIYH5pv+I//AC2IizujMt+n0Z+9lfOO+tV/oR+o+sURbrRGj97ovubOP9T3Ba9T1Hf4Y+0oi3epFS9xef4I/EesP+p/mFYGepS+qz/MqL6ijLO3rmajNT7/AOpbzvmnfXZ/Q9EWXoZ3RNbt/wDGM/xD/pXU0RaS1PMduf3Yf9fuwiIsHFCIiAIiIAiIgP/Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUSExMVFhUVGBgVFxUXFxcYFRgYFRcXFxYaHRkYHSgiGBslGxgXITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGi0lICUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBEQACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQECAwQGBwj/xABHEAABAwIDBQYCCAIGCQUAAAABAAIRAyEEEjEFBkFRYRMicYGRoTLwByNCYrHB0eEUUhYkU3KSokNjgpOywtLi8RUlM1Rz/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAECAwQFBv/EADwRAAIBAgQDBQYEBQIHAAAAAAABAgMRBBIhMQVBURMiYXGBMpGhsdHwFBXB4SNSYnKyJEIWMzVzgpKi/9oADAMBAAIRAxEAPwD3FAEAQBAEAQBAEAQBAEAQFC4DVAUdUA1ICAgdo764Ci7LUxLAeMHNHiRYKbArsbfLA4o5aVdhdeGkgOMcQJuFFgTzXA6ICqAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCA18ZjqVKDUqNZmMDMQJPmgII774IktZWYTDoJMDMBpeJ/ZTYHie2968bWLy7EOLQ45QCAL2kDlrYzEK1iSKxu+WLqU20n13ua0yJgG0QbAEjxQELh68u+sJIcZJPHn89EIN/EYtuYmm0AGAARJA4gGPdCT0vdL6UWYaiyjiKb3RYObeB1m55qLA9U2HtyhiqfaUXhw0I4g8lUgkQ4aceSAqgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgOZ3w3yoYJpBOesRLaYv0l3IX8VKQseKbzbzV8Y6azpABhosB5cFYk5pzeL3X5CzYGvlogMVWq3K2Dpr5tbB9ZHkgNFoLyGtbJ5TeUIMuWm3u1W1A4ai3z7FCSpxrWgBsubOjhfoZHyUIM9fHteO8NBHXxCAkNn4/smh1Kq5pAzEhxaTHC3GZ9kJJjD7fxdOqysytUc6ARmc50gXLbnTS3VCT3/dna38ThqdYiHOaMwGgdxjoqFSVQBAEAQBAEAQBAEAQBAEAQBAEAQBAY8TXbTaXvcGtaJLiQAAOJJ0QHznvhi+0xtWo2s2q1zjcRIEgAQOQAjpCsiyOYr1HMcZ1BIPupINHF1gYj05HiDyuhBYw5YLxI0iR+SAtq45znAjhpYDy7qAvrvLiA4kzpOo80Bgw9IklvG/sgLQ06/dlAbOH+Ai8kwPnxhAT1FxNm28OgAKguevfRNtUvYWXgXmbHT0MR/iUMqz0tQQEAQBAEAQBAEAQBAEAQBAEAQBAEBobdwtOrQeyoJYRLhe4F+HggPmnePE0nVX9i1zKYOVrSZ0MG5636K5JF1HGpJHxamY4aygNFuEe6zGuPgqymluWjTlLY3qW7NeJLTGp6LLt4m34aRq1NmuaeNukK6qJmcqTRWnhDYwbI5hUy0PyTYybTynVWUkVcXfYvZ2YbBkzrBlxjSY0HRWKlBiCT3WhvAE8B06oDeoPLZcJj4QfGBKglHq30K4AAmrPeJeCINmiOOhkkdbIyD15VICAIAgCAIAgCAIAgCAIAgCAIAgCA576QKjm7OxJaYPZkT4wPzUoHzh/DF7wAPisBx6+Hipbsrl1G7O1wW5IDRJsbnmenguadSSOqFKJP4PY1OmAGtC45Ns7I2WxK0cC06hQohyFTdqjUMuY0wtYxaMpTTMeJ3Qw0QKQFuH4q7uUi1zIzE7l4Yj4Fm3NbM0WV7o5raO4Db9m6OhVo4ia3Kyw8Hsc7W3UrUyQBPhqumNdM5pYZojsdSq0amR7LZe6CDxGvj+i2TT2MJRa3PVvoRx+V78Pl1aH5p8YHsjKs9gUEBAEAQBAEAQBAEAQBAEAQBAEAQBAc19I7Z2diOWUT1GZtlKCPEtgUgarXEWt5khVqbG9Lc9Qr2aPBc9XY6qe5gprmNyRw4V0ZSN2lUutEzNovquUshGpWKzkXiR1YLNo2TLaDQTBErSnuVnscl9IuzG9xwFxbThrC6Y6SOWprExfRLiOz2gxsWqNczXpmE+ER5rdnKz3hVICAIAgCAIAgCAIAgCAIAgCAIAgCA5r6Rj/7fXFrho9XNUoHlmwtnmWGPtSkzeB2uP1jlquWqdVLYw0QuY3JbCtMaLSJjJ6m1TCuijLqoUshGvVYqNFkyLruhZmyMWGf31enuRU2InemXOAN7jyuPa66Vucz2Ijcqk6ntPDkAQ4kX5OaZIW72OaSPdVUoEAQBAEAQBAEAQBAEAQBAEAQBAEBy/0imcJk/nqMb7l3/KpjuSiJ2LsvKM51N2iNBwUs2IPeLbjaTi0XcNen7rlmrs6YuyI7C72MFzblz/RZuky3aondl70NeRBB/BVvKJOWMjp6WNY4Aq6mmZuDRkq1WKW0VSZFbQ3ho05lVzp7F+za3IDE7fo6lwCpkbNVJIw4LbVJ1QNBudDw8+SvGLRVyTOkq7NbWAdaQPVdUVc5pOzIxuyxTx2EqAGO0DT/AISAVpyMZHpiqZhAEAQBAEAQBAEAQBAEAQBAEAQBAcxvwbYcc6v4Md+6tEtHcYisKbZ4NChuxqlc852liKTXOc+HE98i0AE6uJsBw1XHJNu6OuLUVZkNtHbeEIewtY11MAuDmG0xzLSTcWAJVlTmUlVhexiwtd1MzkDBzbIAnm03bZZyRpFnbbu4x77FY8zV7EptmsaYJnQKZ3TsVhZo8/2njxVJacxJ+y2cx/RXgmtRJp6FmC2Xh4JfY/ymqzNfhGZaZp2uZZIXsSOHpUWAimMrvvTmA6Tw8LKrbe5ZRS2O/wB3ng0WQbix8V2Qd0cs1ZmztOn9dRj+2pn/ADXHvKuZPY6tVMwgCAIAgCAIAgCAIAgCAIAgCAIDBjsSKVN9R2jGl3pwUSllV2WjFyaSPP8Aa22n4p9HutDW1GRYyC45HNJ5gkcNFSlUzHRKj2Zv7cJPdHP8FSvJrQ0oxvqcbi9ktDu0IcS3vCCLOF2kgiDHVYRqWN5QuaGM2RRxFV1aqxznuLXOYyQ1z2iMzmwbxa0aq3bS5lOxhc6PEYE1SKtVkOAiTlBLeDS0C4HXSSolNvVkxilpE3tg4VoIAsAICxhrI1qaRNjeGkHGNeamr7RWjscx/wCiNbD2sc5urmNuHGT8Ud5w0sIFuK0hLmVlHkc9tfYeGrVzVaRTDnh7qTWhoFg0gX6EgEGJK27d22Mfw6bvc3sLg/rSKfdpyHMZfuECO643uNRELOU01saxptPc7LYFRzTlOhVqM9bFasNLkltfFBmJolxgAscTc/aAiOJJK620ldnGot6I7DC4llRuZjg4SRIOhGoPIjkqp3M2mtzMpICAIAgCAIAgCAIAgCAIAgCAICG3pq/VZP5zfwb3j+AWFd923U6cNHvX6HA7NYWV6bTJa+ox2mjmkEGfAR6LDDyd7HXiFeNzoNos+sK2rK7MqLsjFSYw6wuU3dzapUgNPZXRm2aW0xZZzNaZi2Rr1UQLVNi/aBh3iktyIbFmAkXCRbWwmk9zbrYFlT42NJ5wtdzK9tjXOz2M0AHgqMuncYWnD2wtaW5So9DHvcS2pTIEvyQwfelwny/Vb4h2SMcOrtkv9HTCynUpmQcwff7zQ0+7VnhXo0xjErpo65dRxBAEAQBAEAQBAEAQBAEAQBAEBEby4fNSzASWnTo6AVjWjdaG+HnllZnE7SxtNga+/dqMtwAzAmDyge656TWdHbUTysmcWQ6HcCPVddRXOam7EfSqhee9zttoSVCpZaRZlJEVtnalOnJqTDRmIaCSbwIAVXq7F46K5q7vbxUapc5mZscHtLXeMHUdQpUXFkNqaMe2N7MLTrBtVzpdaWsc4A21LRA1U5HLUrmUNCRw1dhILCHBwkLNKzNHqiTqVRC0bM0jSr1FmaIzYKn3gT4rspROapLQhdr5cRixUEltKaTb2zDKSRyMlwn7qzxT1Vi+GWjOt3XouDyeTS13r3fwKminmv4GeJatY6VdRxBAEAQBAEAQBAEAQBAEAQBAEBhxlHPTez+ZpHqFEldWLRdmmeXbfBdSNMOnukyQJMzc9SZXBm7yPTy91o1djbXIphjyZAgE68/zXbN23OWGpnw9QySuOUb6o6lLkSIx4aNYJueg6qEmS7XOb29jqbyCDmcLWnx1CKLDkiBNWs1zXxIJiOF+E/PstUkZtyuXUtpVjmloyybZbxKhxQjJnQbv1GtJcXmSIAPAdPZZNM1R0v8AEy3wQixHPxRLoRIlsv2ntnJTyt+IgiRyPLqu6Bxz3NDdZn1Zc4lphz+J0BPDXSFzVY5qjOilLLTR6Tuuw9gHkEdp3hOuXRv6+a3pLunFXd52JhamIQBAEAQBAEAQBAEAQBAEAQBAEBHVtlNLpAYASC7uDMcpkAOmwnoqZFyNO0dtTzDebCCjiqrLQXZh4P7/AO3kpqK6NaTLMFiO9+PO65lodJob0PdYNDi3LJygm8i0ASbBI2RE7sh9lbSDu6KdxM5+4bD7wUunfmFUtyOvwzMQWkig1wbr8LhYA8uRCdix20eYxFOuGgHDNAvAhgA4nwUOjJk9tFHKbS2/Qs15FNxAIk26aaBQqUkw6sWiU3Xxjnh5D8zdB42056m6SVhB3N+tXaXOJ4d0eQmfxR7krYw4XC9s+mI+NwYP9q1/WV1UlZHNVZ1ux9hGnUY0FppZ3gd6XtDSZDgbkwIPiFh2cs9+Vy7rLJbnY7tjQAABAFgOgXScRVAEAQBAEAQBAEAQBAEAQBAEAQBAEB5z9KuDh1KuDAMsPPMPh8bEhSldWLwdjz/C7QIJnUfpdc84WOqEzotnYxryA4x18VhJG6Zs4umGOzZfPmqXNUzbwOIoFpDiIIOhj1C2UlzKzlfYYmpQgZbxxL5A6AeqOaEElul7jQbhWVHXaHeIssmy0ncwY11Oi4hsNm9rX4K0bsydkRdfFjLzPDrNvz91eMW2UlJJHVbi0M+Ip6xTDnmf7oAPqdPFdiVkcU3c9NFJoJcGjMdTAk+agzuXoAgCAIAgCAIAgCAIAgCAIAgCAIAgCA5zf7Zvb4RzR8TXB7b2kcD4zHmpRMTweuwg8osRxBBUSVzWLsbeysbBAnU/OqxnA2hM7GnV7SmRPLx8lytWZ1J3Rw23cK9lTp9kDz9b/guiEk0c1SLTLt38M6o7l4/PRKkrImlG7O2a802xbSxlc+50PQ47amOkySL/ADx4yumMTmnMw4a8a9NeP4aBbQjZmMpXR7B9GeBc1tSq7UwwcJDbz6n2V5GUjt1UqEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAaG3GzQqeE+hCItHc8J22WmqWnuunXgddf1TPrZmzhzRz2MpOp3gt1vztw+eau0Y6ox4Xb7mCxInW9rrGVNM1hVaJ2ltVroe+/c5ceHWBMrHs+R09otzQobWDbi2WQCNSDr+XopcLlFUSMb9uveYzGIPnH/haRpIzlWZj2bh3V3QLkm1/EmfZbWRim2d3sfY7KAbUqEFxiAdAeJ1udPRSXSPUt2nzSkaWhVZSe5LqCgQBAEAQBAEAQBAEAQBAEAQBAEAQBAEByu8W9tGnXp4Id+rWOV0ERTBBjN1PALeOHk6bqPRL4lFUXaKCPKt58GO1cuCo7SPShG8TnqjiBkeMzPdvgrwqWM507kZisAJzUzbkbG599fZbKSZhKDRH1sU4cDPIplRXMzC2o42bx9vkAqbEXZMYDZziJJygxrOl58DMKHJIsoNnV7Mq0sO0R3ndNSefRVc0jaMOhstr1KtRrn2ANmjQfuueVRyZ0Rp2R3TtunC18C2Yp1i+lUHC+QNPk6L9SvSoUlUpy6pXPMxE8ko+LsehrmLBAEAQBAEAQBAEAQBAEAQBAEAQBAUJQHl++30jGTRwT23kGtqeRycPP05r1MNgV7VT3Hm4jGNaU/eeYYfGupVqdcySyox7pmTDgXX5xK7MVG9GSXQywEv42vM7XbRa+oXtMtdcEcl8pW9q59VR9k57aGEVIyLSiQzqN1smYNF3Yg6gFWU2VcEyooAfCPRHNhQS5F7KTj0Crcsokps/CX5lZzkawiTFLDmWrNPU0a0NTf/Hh9WjRYbUKYkg/6SoQSPINb/iK+m4ZHuN+h83xOVml6kxsj6RMXQYO3e2pA7rS0CoRwlw4+XUq9TBU5Pu6HPTxdRb6nq+w9q08VQZXp/C8THFp4tPUGy8qrTdOTiz0qdRVIqSN9ZlwgCAIAgCAIAgCAIAgCAIAgCA476U9qGjgixrodWcGW1y6v9hHmuzAQUquvLU48dUcKTtzPC30+IXunjwqaWZbUdnEHWMp/IqrSkmmatOjNSW25PbBxGZgBN22PiF8diqTpVHF8j7HDVFUgpLmSNelIXOmbtENisNfRaKRm4mNuBJVs5XIZqezSocyVTNluCAVc5bIiVwdGBoqNl0i/FHKJmIUIlnFVMR3y83kl3/T7L7HCUuyoxi9936nyOKbxFeTj1svQtpkuOZ2pXVE5MQ1F5Inf/RlvBXpPdh6dPtaZPaOYCA8CzXObJv9mQvN4kqaipydnsunWzOnh85axWqPT8DvDRqOcw5mPaYcHcJ0uNJ6wvGjUhK1nv8Afk/S562xLq4CAIAgCAIAgCAIAgCAIDXxuMp0mF9Rwa0c9fIak9AgOVxO91Z7S6hR7NgMGpXa7QcRTbdxPBoM84WbxFJTcU82nJrV+eyS5v3XIanlva3muXl48kcBv1tB1djazm4hsPDR2zQxhBa74GRYW4knRenwuMYzazRba1yu7Wuzf6JJHnY9ucE7Na89PcjkJBXtnjuMovVGrVYQZVWranoYeoqkezl6G5s7E5HB3A2PivI4rhs8O1jut/I9Hhdd0pujLbkddSIc2RcL5s+jMNWgCiYLqWFU3IsZuxUXJsUbQS4sbjGgBVJIHePG2yDjr4cfnqvR4bhXWqpvZav6HncRxaoUtPaei+vocoG5nL6vdngOSoUfEzVasd1uuiluxy0MP2l5z2RP7i4CjUrO/iXBtIMJJc/swHlzcnekRx4ry+K4itRpR7FXk30vpZt6Hfho0Ks22rRS8t2dzUxVLDEfw9B+KZwdSrms4CO80gyQPu3Fgvm1TeIk+2qqnN8pRyp258ldddz0XNU49yLkl0d7HTbP3gpMo53h+HHBmKcGTzDJcTC6406ysovtP7dfjoUzx3fd89CTwW8OGqNDm1WX4ZmyPf3VFiIvdNcno9H0Zo48yRo12vEtcHDmCCPZbKcW7JlbGRWAQBAEAQBAEBo7R2vQof8AyVACYhv2r6W4eJUSairv78uoWrsiJ2ltquWOdSZSZTAl1Z1dgyjnlDHD1KpKrFJJXcnskrt/FfIjXd2t1v8AscViNoUajmgYtzzJfVrBrjkHATVluXwHCwC5K9GvnUsRSzJ2UIye78Ix1fXW1lu3oWhVpuLVOdrbtfV7GLEbyYem8OGNxdcN0phjGNMcC6BbyXqvhc6sLKjCLfN3dvJXepwfjqcJX7ST8PtIiN4d53Y6m6maQYKf1re9mJynK6TAFmuLtPsrbBcN/AVIzz5s3dellrqub5q3qZ1sZ+Lpyio2tr9TjqtCNLHkvctzRw0q6fdqq6+Rj7WRB1UX5M2eHcJKpT1QomLcFC6F8RfSa3RP7F2jkIY64OnzzXznEcA6X8SHs/L9j3OHcQVdZJe18zqKbGvEheQeqBShAVezooJMXGyA18biMrSdIEmeAFyrRi20kQ3ZXONxdYvlx46DpNl9lg8OqFJR58/M+Px1eVevp5I0nVYW7lbYtTwrnrNl+FYZzFTFcyuNqpR7KBN4Zv8AVax51KLfaoT+AXFWd8ZSj0U38l+pjSVsJUfika+zdo1aDxUpOLXDjwPQg2IXRiMNSxEMlVXXy8uhhRr1KMrwdifO/WJJJczDuzWcDRHeGkEzOi4VwehGGWMpLprt8Dq/M6jd2kzb3Zwja1N5dhm1aTnknLL30eQLAQ5zYNi2/QrycRCpTxF87jUSSvspr+ZPVX6xfPZo9SlOM6VkrwetucX08ujJnB4ZtHM7CUK0t+LsMSHx/eoVg13kRPJaYicasV280nybjb3Si387dUVpx7N/w07dE/0ZNbI3/A7uKYWAWNXK4Bv/AOjCJp+Nx1VOwrQaj7V+V1d/2vaXwl/SaKrBq+33z6fLxO1wuKZUaHscHNNwQZB9FEZp6c+nNehczKwCAICL2zt/D4YfWP70SKbe9Ud4NF0Wvl12S83sQ3Y4Hau/2JrHs8Ow0gbWipXPp3afnK6ZKlSjmlr4y7sfrL/xXqjnzzm7LTwWsvovUj6LRRYMRiagBcbAjtHj+7nkVKp1LyCB7Lz3UqYuqo4a7XN7X87ezBcoqzlz1Ne7Qhetp8bfWXjyNPGbzYOq49rSxdRliGPxHcLhoS0WXsQ4fXpxtTlGLtuo6+/78zz5Y6hN96Lfrp7rkJtvb7q7RTZTZRotMtp0xF+bj9orownDoUZ9rOTnPbM/06HNXxkqkckVlj0REgr0ThNvZLh2zATAcchPIVAWE/5lyY5N0JOO61XnHX9DqwMkqyT2envNF0izmkEWI5Eaj1XUpJq62MnDLJxMT6YP6hGrmtKvOk7GFzCFRpo9CGIp1dGbdCpmEaEXHOenzwU2UlZo4qtOVCScX5MnNj7Vg5ahyng7Rp/Qr5zGcLnBuVLVdOa+p9Hg+KUqqSm7S+B1MnivGPWL2U54eyAsxT20ml7yGtHE8zw6laUqU6sssFdmdSrCnHNN2Rxm1Mca1hIZM9XePTovpcBw1UHnm7y+C/c+a4hxbtF2dNWXV6MiMW+0D5henLQ5MHG83J8kYGUuJUKJtXxf+2JuMbELQ8mUnJ3ZKUx/U6h49uxvpTefzXnS/wCoR/7b/wAkd8VbBP8Au/QjAF6J55UBCGZMPiH03ZqbnMcOLSWn1CpOnGayzSa8S8Jyg7xdieob7YsZSTTe5uj302l4nXvCCuD8qwyuoppPo/rc7VxKtpezJWjvsyuMmLZkP2a1KS5h5w4k+IEg8QvPr8HqQeahJSXOMtE/VfB6NcmdlLiUJ6VFZ9Ub+6e0g6sW0cTSDrkNbRfRzxxILuzJ6ZQddFzY2lVp01UlSkrc86lb1te3rbqjpoVKc55YzXuaOwdvg2g5tPFt7Mu+Go0gsN4kiZHXWFXBZ8TFuOtvvy+RpXqRo+1oS/8ASHCf/Ypf42/qujsKn8rK9tT/AJkcFj99a+KLWYeabSO81jc9WTbvPgNpt6yD4KtajOipOolvo21GNv8AKT6LLbzK0q0atsj+F35dF7/caG8NKng8NcB1esdagzfCZc7L8JGl7zmF1ycOpzxmJ6Qj0un4d72tXrvt0LY2rHD0r7yfX6baHHP2tXP28o5NAaPRoC9+PB8FGWZ07vrJuT98mzxpcTxLVs1l4JL5GpWe55zOc5zubiSfUr0YQjCOWKsuiOKVSU3eTuWZdfnirFbmNzULJgIC5zZBHOyBPK7o3Nuk9u50WqhlYR/rGhxPqXaLz+Gyf4dQe8W4/wDq7L4WPSx9KLquSe6TI8tBv7r0DgTcdDbwmzaj2l7stOkNa1U5KY6SfiPQSVyVsZTpd1u8v5Vq/dy83ZHXTwsqqTireexa7bWHote3CNFaqWlhr1W/VwRfs6R8+870XDKGIxNpSlkS1UVv4ZpfotPM9inh4042evn9CBZtXFh15jlDYj0uuuM6zfeRSOFw+W1kdfulvCWRTqkZOEADLxJ5xra/TkuTG4BV4ucV3/n+5pQxLw01CTeT5eN/0PRaLLfgvmrW3Pbued7+bQ7SoKbCYZNxFzNzf50X1HDsK6VG73lqfP4jEqtiP6Y6epxNM16RLw8jp8RPKQRC2dOpFttuxplpVWnZO3zJobwUMSf6y00K39sxpNJ/V9MXaerfReZSliMJpC84cov2l5Pn5P3o0qUY1NVo/g/P9jcOyqjhnp5a1IWz0TnE9QLt8wF6VHieHqPK3lfSXdfx0fozyZ4SrRpuyvfmtTC5sEg2I52XorVXR5bTWjRmo4gdgac/6XPHQMDQfcrk7J/iu05ZLf8A1f8AQ7ak0sNlvrmv8DCus4QhBaELFUICAyYWuab21G/ExwcPFpkLOrSjVg4S2aszSlUdOanHdHuP1GMwrM1JrqdVodGpBI4Hg4GR5L4CVSpgq0lDSUW1f76n1uSGIppy1TPNv6N/df6f9q9v8/8AL79TzfylfdjoNxseaeHY1rB3i4uI1JDiJJ42/BePxzETjj5xu7K1vDupndwunF4WMrdfmznN/cca2LdcxTDWC8wQJd7kjyX1XA6bjg4ye8rv46fA8HitW+IcemhzmVeseZcrCABCbluVBcqyjM3iBKMsncv7NgEmT+4lQSH4ui8sFd76fZtyNLafaZmglzRYiCJi9rDqvMnHEYepJ0YKSm76yy2dknyd9rnt0qdPE0Y55WcVYtO1mMn+HwuY/wBriCHeYpN7o8y5R2GKrf8ANnZdIafHf5GsYYSjbZ+ev7EdjRWruzYio6oeGY90D7rRZo6ABdNHB06StFWKVeJQS7uplw2AaBYDUCNNV0qMUedUxtWfOyNqrQDRAAId6iD7Kxz9pNatmsaN5bwv1UWNY4iVrXPRdh7VnAuqGZpNynU9Gzy/ZfOYrB/6xRW0nf6n0GGxv+jcnvFW+h57UlziQJJMydPIHXzX0dj57Oku8/T6sHCfOpU5Sv4ua2ZZUwTeIlQ4JmkcfWXMxNwQYc1Nzqbv5mEtPq0rKphqdRWkk14m9PidVPXUkmbYxkQ6t2g/1tOnUPq5snzK898FwubNBOL/AKW4/J2Or83urSjf3fQ1y9xMuIJ6NawDoGsAA9F6VKjGkrK/q2/i7nmYnEds1pZILU5ij0JRQISVQgAIC4thCL3Op3Q3rOHaaNQE0iZaR8TCdbcQeS8PivCPxX8Sm7T8dn+562A4iqCyT2+R1v8ATHA/2rv90/8ARfN/8L4vw96PX/N6HV+453Bb3NoYRlClSJqAEl7oygvJdIgku16L363BHicVKtUksrey3aSS9NvE8qHE40KCpQWqXocm55cS4kkkySdSTdfQRiopJbI8WUnJ3e5QqxUBQTcuc+bwLWiPm6WJzGKEBUhAVdGWLz+0KLFsyLWMANxKkjMZI1sLx10Swzh3O3LQJYhzZYWBCLszU2s5n2Uak6PcyllLW5UamiUUTmysv8PiRlqZMrHOPCA8CSD8V3DyC8zFqX4qg11kvh9+rPQw1uwqrwXzIGu6lIyF3mAI9CV6cb8zzaijyNd7lYojDMoX2KoQAEJCAogKFCUAgKwhBkYIQq3csF7oTtoUa66EtaGTKeaFbouw9WWgGxZbyMkfmFETfEq9pJ3uUc5Sc6KAoC4FAVlCC0oSVlAZKNEu09SYHuobSJUW9i91OmPiqA9GifdRd9C/ZrmyoxFEfYcfEx+Cd4m0CjsYzhSb5klLPqLx6GI4zkxg/wBn90sL+BVmLfwgeDW/opyojO0XPxL+Lj+H4JlRGdm5gMc9jKwlxD6ZYRP8zhGvULjxWG7WdJp2yyv5pcvkdeFxChCopK91b1Iziu04i4iyEGIIXYQgqAgACAogLULFWsQhsywAhTcwueULpFTpHNBzuWusUJWqMkdUKlWanw/NCf8AZ6/owUKlSgAQguCED590JLqPxD54FGWhuY6vwnxCjmWhsYmcVIYCBgIAUBno6HxQpIOQgz0Phf4D/iUPdF4+xL0MPHzUlClVSEYgoLFOKE8i4oVKuUhFFBJYhYyM+FCj3K1NEC3MPBC/MvOoQryLKuqFo7F6FT//2Q==</t>
         </is>
       </c>
     </row>
@@ -3552,124 +3552,124 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ROVMAN POWELL</t>
+          <t>HARDIK PANDYA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>psl2023_27</t>
+          <t>ipl2024_33</t>
         </is>
       </c>
       <c r="D25" t="n">
+        <v>10</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>166.7</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="M25" t="n">
+        <v>4</v>
+      </c>
+      <c r="N25" t="n">
+        <v>33</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>33</v>
+      </c>
+      <c r="R25" t="n">
+        <v>24</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
         <v>2</v>
       </c>
-      <c r="E25" t="n">
-        <v>4</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" t="n">
+      <c r="V25" t="n">
         <v>50</v>
       </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>50</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
       <c r="W25" t="n">
+        <v>15</v>
+      </c>
+      <c r="X25" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC25" t="n">
         <v>18</v>
       </c>
-      <c r="X25" t="n">
-        <v>15</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>15</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>22</v>
-      </c>
       <c r="AD25" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE25" t="n">
         <v>13</v>
       </c>
-      <c r="AE25" t="n">
-        <v>17</v>
-      </c>
       <c r="AF25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH25" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="AI25" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="AJ25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL25" t="inlineStr">
         <is>
-          <t>Batter</t>
+          <t>All-Rounder</t>
         </is>
       </c>
       <c r="AM25" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTERMSEhIWFREXGRgWGBYXFxYVFxgYFxUYGBcVFRcYHSggGBsmGxgYITEhJSkrLi4uGB8zODMtNyguLisBCgoKDg0OGxAQGy0lICUtLS0tLS0vLi0vLS0tLS0vLS0vLS8tLS0tLS0tLS4tLS0tLS0tLS0tLS8tLS0tLS0tLf/AABEIAOAA4AMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcIAgH/xABIEAACAQIEAgcFBAcFBQkAAAABAgADEQQSITEFQQYTIlFhcaEHMoGRsSNCUsFicpLC0eHwFDOCorI1U3OTowgVFiQ0Y4Oz8f/EABsBAQACAwEBAAAAAAAAAAAAAAACAwEEBQYH/8QANhEAAgECBAQEBQIEBwAAAAAAAAECESEDBBIxQVFh8AVxkaETIoGxwTLRI1Ky8RQkQmJygtL/2gAMAwEAAhEDEQA/AO4xEQBERAEREAREQBERAEREARMVaqqKWdgqgXLMQAB3knac/wCL+2LhtE5UariCLg9UnZ0/ScqCPEXgHRYlc6J9NMJxBScPU+0HvUn7NRfHLzHiLiWOAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCQnSjpHQwFA18QxA2VF1eo1rhEHM6eQ3NhJueb+m/SA4/HPUveihNOgOWQGxfzcjNfuyjlMN0JRjqdCM6adLMZxJz1t0w4JKUFNkA5F/wAb+J+AErBwb/hltpYCY6uAPdKviSLvgxK1halWhUWtSZkqobq6mxB20+GncZ2z2ce1gYhkwuOslc2VKwsEqNsFcfcc+GhPdoJyXFUrcpF4ygPnJRlzISw6XR7IiUz2T9IGxnDabVGzVqRNGoTuSlsrHvJQqSe+8ucsKhERAEREAREQBERAEREAREQBERAEREAREQBERAI7pBVKYTEsvvLRqEeYpsRPMHDKW1htYT030j4jRw+GqVcQSKNgjEKWP2jCmBYeLATzZh6yqz9ogAXuBoBtdu4X5+IleIW4XUnadFiBaflak0jcJiqhqAG5DC6tyYciPhrPjiOOcVMgJv4SqrNm1DBxKgRuLSFqm8neMVrKFdWzjUk5jYEKRra33h690g6q2F++SW9yt7WOy/8AZ8qfZYxOQem37SsD/pE65OBey7pgmCFOh1BZsRWUVKuYDKrEJTyrY5rFrm5Gm077Lk0zXkmtxERMkRERAEREAREQBERAEREAREQBERAEREAREQCE6Z8NOIwOIojdkuP1kIdfVRPP/DMODZgTc925E9MVEuCO8EfOeYuEVCpK7Nt5cjKsVVobGA7skWS9YLb3QSefIyNoAde1+Z3/AK5TMpr03bqWQi2p2Y3IuCdbia+K61mBqFQSbmyWN78iLD0lOlmxqRI4jDi1m1HmfoZXOJ22G0nGxmVGQm+mkrddrmZUbmJSqixdBsB12NwlK51qI/kE7bfNU+k9NzjHsM4ahq16xN6lNEAW2wqZu0G5aKRadnmxFURp4kqsRESRAREQBERAEREAREQBERAEREAREQBERAEREATzR0s4a2F4hiKR0GdnU96OcykfA28wZ6XlK9pPQ/8At1EVKVhiqYOX9NdzTJ9R4+cjJVJwlpZxvgmELOyviFTS4JFgR3XJ1M2eN4NFQEVy52spW/yA0HiZG0UTMada6spII2II0IPxmarQoqvZe/mdflKTcUlSlCMNLKNWLec0uY85tYmsLWmstIkZuX1mSp7HV/YXWBxONsdMlKw5kKWF/UfOdknnz2e8NOHR+JVndKS3SkiEhqzE2AsD2hm0C8zrsNem8N6f4ZctHGVEoYoAB17TIrNeyGpa2YC2a+gN9dJHCzMZ4jw1w49eK+lq+ZCWDJrUkXaJ+Az9myUCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIkN0j6SYfBU+sxFQL+FBq7nuRefnsOZEGUq2RyH244AUsbTqhQFrU73Gn2lM2a/fdSnrOYdYxOgP0nQ/aLxevjaVGvVp9Wgq1EWn96mrUkenn/SISqT8O6UZUmssWM6tc2vQ2FBqzMdJCTdtfDlLr0S6OjEBq+IPV4Onq7ns5su6KfQkeQ12x9FuigqqcVij1WCTUsdDVIPuU+dr6EjXkNdrfiS9bIOoCUqYBoYRrKiAe5iMdb3QN1pbn5mc3OZ7QnDDdOb5dF/uuukW+dEXQwqsj+PcZI6uoq5GC2wWHsB1SWyjGVF2DECyKdt++c6qKSTe9yTcnXz38efOdWwXCVTNi8Q5quxzBmFi7bq1vu0xbQdwHhKP0qwDUq2ZxbrQawHMZ2NwRyN9bfpCTyEsODeHDyre7W8Und6a3k92/OnUjgqMb9vkvLi+bN7of07xWBypfrcPp9k590f+026eW3hznbujfSTD42n1lB7ke8h0dD3Mv5jQ9881ATZ4bj6uHqrVouUcbMPoe8eBnUTNTMZSM7xsz1PEpfQHpquNTq6uVcUu6jQOPxJ494+O0uksOTKLi6MREQREREAREQBERAEREAREQBERAERNXiGMWjSqVXNkpqzsfBRcwCp9O+mD4UdVhaXW4ojXQstIHYsBuxvcL8TyBoGC4S71evxjmrimtdm7WQ7hUG1wCtraAsLba5OEUMR9tja2brsQ3Wsh/AWGRLcidh4KBJzhh61LsmXXsi41BOZVFh2TcC9ydr8yBxM3nZSqoU0p0fN7eqrwW6vsdfL4cMNde++7aw4StslRFei7AOpLXOQF2qM41utgNN9RsZ+/wDhPBlOtOH7RI6tFZ1B1sBYHUH6WliweEDGzbIopk94XUn0F/1PGbIQf3ltALU1tsD7unefpOT/AImf+lvhs3fio77u2p7qKd6URsvQ7tVdvzRc78X0Zo18IXFMEIaiWy2ByUhsDTUWCncA2voduWKngQSQWJoqczsT/eVBuT4Wm9UAp2S56x7lrbgaBzc6ADRQTpc+IB1sVmYALZKaqTYhXBcDshwjHs+hPPW0swoZmUHKCk4/zJOnVrk+EFZRXzv5riGPGD0KSTfKlfNL+lcNzG9POysVuPdpU9r22qOOSjfT+F6f7TMOoFBvedSyu/e7gG1/AIbCX1AbB7g1Kmx3C07XuOdr6+J8taf7QcMzIiKt6dJs1Q2uczLYM3qNdLnyk8jL/MQSpySTsldW5qtl/PNub2jS7VWy5fn3v6urZzyjRuLzIaE39Np8lZ6UnpRpUqr0mWpTYq6m4IJBBHMETuHs76aLjaZpVSoxSC5AsM6/jA79rjxHfYcdw/D2rOtJLBmNhe4F+4kA2mq2Br4fEoAWo4hXXIw5EtlDAjca2trfUHmJhYkU9Nb0rTpzNDNYMZ24nqKJXuhfHGxWHvVUJiaZ6usg2DgA5l70ZSGHnblLDLU63RxmqOgiImTAiIgCIiAIiIAiIgCIiAJAdMkLYfKNiwZvKmrVF/zqkn5AdLweouDzIt35kYfG17/AzT8Qco5XEcd9L+xZhfrRS8T1jIUUhXvmBYEqdSLtY7ZR5Gb/AAjCZaQB7RF22A1N1VQFAAFtLeVyTrP3CYO+50tbv0Fr+HcOe0lqdPT1PnsB/XdPJZjGjGPw139fZcnTmdKL4sYejamF/EdfLc+gE2At2vyX0e2/wWfKmx8hYfK+npPvJoF79W/P19JpxxG1V739Xd+1F9STfffSxUeOYxKjumZcx+yVbjNluOR2F17vuk63Ez8CwJwyksS4ILAk6gWvf5XPxmnxjo0GqlzTLXGU6VO1YhUfsnfKoUjvBOzCSWD4XU60EtUFM5R1egGmvYF7205gb21vp7vBzuRwctGEbJRfTVbZaZak2296aUqb1S4uNg5jFxnF7NrhZJbXa4RS6uTJLA0CoZn5XAtyGcsVB7rnKD4ctpvU8PZTmAu3aYW3uD2T4AfWfldmuiCmco1Oq7JsLX74bEZmsLgqCWB0IvoL/I6zxWNifFUpS3lVvhZdNlerdOJ2W6qi7St39Dm3THowMOevpaYcmxX8DHuP4CdB3HTmJW9J2etRR0dKgzIVKkeBGvx2+U45xfAPhq7UHN2vmzfiQ+63y9QZ3vBfEHmMP4eI6yj7r8tbPi7dWbWDiN/K9zVqPYgg2II/IyyJx/DYgU/7Ur9fRYOMq5szJ2swyDQHKCVsPS8pbYjMCe8k/C+npMw4pVRAEbKL3JsCb2IBuRpoTt3mdPM5aOMlzVaOtGq2fB/WxjFSki+9BeOVF4vZ1dKWJU0lDrkJNJAyMRvcdoa/7zw07NPLnCeKumLw1epUcrTrU3JJLEKKimpa/wCiDfvnqObOBDRhqPK1jk5uGmSfT7CIiWmqIiIAiIgCIiAIiIAiIgCRfH8EKtAg7qRUGttV15eF5KTXxhApuTtlP0MhiRUoNPZpr1Mp0dUVPBpoP62/nN5Bt4kf18hNPBnSb3NfifT+c+aylWR1OBjvrbx+lv4TYXmec01PaM21aISSDPvJsBy1+UWF/ADbxM+xMLPYS9yUVUgfDVbEnlt+Z8v5SKxeMszP8P8ADsb+FyT8JnxFRraC/hr9R+YMja2HDKVOdL6WZbrrvYjb0lPxK77WX0LEjapY0MxUG+qn4Wv+7K57UcGDhBXAHWoSP0urYWa3eAcp8BeOA8Tprjq2Fa5emisLbNooIU/410/SPcZZMZhBWRldAxdShvsqkWK+OhlmFN5LMQxOVHyqmq+8X7oyneqPPyv2PMgfnN2gLrafHFOHtSrPRa/2TMpNrAm+h8rWPxmOk1vvU/8AmD8p9DTUknF1T7+xtRPjY7XHd325fl8p6vwWIWpTp1E9x1Vl/VYAj0M8pVHVibEEc7G/9CegfZNxQ1+G01PvUSaBPeFAKH9hlHmDJo52djWKku6/2LpERJHPEREAREQBERAEREAREQBMOJo5kZT94EfMWmaJhpOzBzzC4xVqdV1iFg2QgMps2t1Ou/ZbTwPdJ5DdtNsp9SP4SnLhcnE61FkoGkapcAqOsIq5nztfRgHaonlJXAYWlhqePrUqaovbNlAUWpUtgBoO1nPmTPBZrLQhiNJvpte9L7NP6M6MXVEpSW7N5H6ifSMTcc5VqXFa1LrUU5nprXtm7V2X+yrRuTqbmqTvrab2J4rWwxY4pabWo1KqvQzKG6oAvTZKhOVrEEEEg2O1pq4mRmqNNO7XKtKO1ejT8mWJkocUyneynS55Hx8J+YjEuPeHxGomrjeN0s70zSxDZQucpSaqozoGGqXOx7uU+F47Ro5Eq1kVagDU87BHCttmRrED4Sv4GLGicX0pW6pVe1+dB1M6nNqAjf4iDNhA34WH+IMPWZnpIdSo8x9biauPq06VGrVDe4jPv+FSZQ/msjJyL/vbq+LjEgXVq70yT+Co+QNfw7J+E7RTDEaMB5D+vpPO3EP7tgDqBoTvcc52/gvSzCNQpO2JpBmRSRmBIYqCQQNjeek8cyTU8N4abtpsq/p2+7M4lIuhUvaB0drHEipSSrUNRczFabVAGFh9waXFucgqHRDGNqMPX+NJlH/U/jOi8W6QYCoVL4mtpfSg1ZAf1str/OQuJ47wtd8Pia367lh/nrflOnk8fHjgRi4uypeLb+68jEcxS3f3RVMR0NxH30pp/wAStRS3+fSdZ9lGC6nAlCaZbrXJNN1cHRbXZedrek5ziumGAT+74TSPi/V3/wBDTp3s0xyV8AtZKKUA71Ps0tlBVsl9FF7hRym7lsTMTn/EjSNOn/qRrZjG1xoW2Iib5pCIiAIiIAiIgCIiAIiIAiIgFKxtFf7dWYqCyhbNYXGZeR8ifmZmbDK2Hembhame9jr9oxJ377n5zWxdb/zWJv8A7wD4CjTP1Jm62lNB4D6T594lKcMziUe0nTotTf3bZ0cK8UQeI4CzuXRx20ojK1wL0qmcm4v71kG33Jj6VcKxVelWZ1RctCuiU6ZLl3qLlzEkCwC3AHjLEnup4AfSbSPcSOFnZNaGk2tnxukn02VNtiTVLlQwmIHX4oNiKlBzWbJ2LKyKiqGuyEHW/ObHEMKhr1KtHEUDVCLTrUq1iGCjMDobobN4iWKgbXXly8pjxGBpOwZ6VNnGxZUJHkSLyxZvDnRtPaj/AEuqVLfpi2lTZydLUaoZIzgdcdRSKrkpMoyACwQbZbWGndpIn2l1cuAcXsXZEv4e8R8cstroCMthbu7vKUH2qV8uHo0ebVC3+Gmlj6usrycFPP4elW1V50pe76Jbk43ZyyunZI30nzwOp2AO4kesyv3TT4UbM6+N/T+U95LYjmVRp+ZY0bSfFU6T4omZqu0I1WQuKWd89jH+yaP69b/7mnBcWd53f2KtfhVMd1SqP+oT+cnHcqxNi+RESwpEREAREQBERAEREAREQBPhmAFzoBzn3KR7XONnDcNcIbVK5FBTzAYEuf2FYX7yIMpVIHhfE/7SHrj3atWsV/U61kQ/sKstOL9xfMesoPQ02w2GHgT/AJyZesS32RI5W9NT6TwHiarjy6yl/UdDCXymSmeyh8B9J90quVrcjNehUvRBHK49SPyn7iGuPG4t6Gcx1jOvUtpVG5XFiGn3ea+FxAdbHcXB+GkyKeXxk9n0ZjgZCJy/2qVy2JpUhqVp3Hm7NcD4KJ04ORvacl6Z8brHFVwj9WA2S9MBHIQgHNUHbIuDpe2u07HgsJPM6oK6Td3Te3J8+RPCTciuPwhl1ruKI3s9+vI/Ro+8PNso8ZA1q1MYkimHCEDVytyRzsuijwufMzfxJ1J5nf8AiZC8SWzBh4fSeuhCVazlXyVF+X6yaXBIZmL0V5d93J/DVdZvvtaQPCqmYiWEDSZVjTrUhMaLGdy9h3+y/wD5qn7s4pxBdQO8j1M7l7GMPl4TRJ++9V/+oyj0US2JTiF6iIkykREQBERAEREAREQBERAE45/2g8T/AOhpf8Vz8OrUf6jOxzhHt7xF8fh6f4KGb9uo4/cmJbEo7mXodUvh6Z7qZ/ylgZfsLUulvFifJRacx6C4i9Aj8AqL+0C/7x+UvXCMTfrFO4T/AFOfynjfFcL+JN8tXvX9zp4K+WvexucIewqUzvdCPJt/68ZtFSDY6g1ND5L/ACkXVq5WFQbpUfN4oGVSPkLjykicYEIY60iXNxrY2FifDfynLxMPVJf9vVR79S1RdbdfsarVmpEuNQRVuPJ5LpVVlJXUWAB8/wD9E08gNwCCOqJ8O0dLH5SPSo2HexB6o9WT4X0v6CVqNqcdNfWX7UDh39ScrVSoc6WFgfz+s4RjsTcvUb3nYtbxY3/Odj49iwMHiqobS1XXyUgetpwrEOXO1l5ePiZ6fwHC0/Fl/wAV6Kr92Tw1pqfFV76zVxVO4M2qq6WmtivdnoCU9nUy9Hl7N/Ej1lmoqD5Sv8MGVQJNUH0MhxOXwIniVTt6cjf5TuXsYxBbhajklSqo8i2f6sZwfF7kzvPsXp24VTP4qlU/KoV/dlkSrEL3ERJlIiIgCIiAIiIAiIgCIiAJ509tNfNxeoPwUqSehf8AfnoueWunWN6/iWMrDY1WUeVO1MEeBCX+MjLYnBXJ/gGPorhqYp2ACP1h59aQL5vy8LcpZKeNyVUqKQVZFJtsQMn5EzjFM1BfISBztoDb67+sk8DVrKqgVqiWva1iNdwPCcnM+HfFbae9d+q/ehv4U240odfr8UodQHYkFluSAxF2ftaiY16S0KTp9p9kKtyxDAANbW9tv4zn/C+OPSV16+vZvug0ypPMkMmmvcZv4jpnWqUurKJfTtAD7tuVrcpovwyeuum2qXHhJUfDhy53N1TTdXzdfJ/lFzp8Tpl1GDxCP1lw9IOgYe7Y0w9wp1OhFj3ifb8fyu6VF6xGCmxV6bqBoVYEZM1weabTneO4rUrKFcLpY36tLi21tPreardYSGNR7jbtsLDuFjoPATMPBm40m+DW7rvVOtFypRJWSMLk1097PvgWjpF0poDDV6NFy2d3ZUIsQudSQL76Btric/biY/3L+v8ACS9enmN3a7d5JY/M+c1jQHLX+v5zr5TKxy8HGPF1fnRL8EXrrZ0+hoLi7m3Uv+1b6iaeLqvopUAEjnfeTPVnykRxL31F+Y+s2ynGlNQ3+xO4NdJIobKZHYI6SQf3ZWjVZDY0z0b7NsP1fCsGO+kH/wCYS/70824lS7hF95iFXzJsPUz1hgMMKVKnSX3URUHkqgD6SyBRimxERJlQiIgH/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIQEBUQEBIVFRUVFxUVFRUVFRUVFRYXFxUWFxgYGBgYHSggGholGxUVITEhJSkrLi4uFx8zODMsNygtLi0BCgoKDg0OFxAQGislIB8tLS0wLi8tLS0rMC8rLS0uLS0vLy0tLS0rLS0tLS0tLS0tLS0tKy0rLSstLS0rLS0tLf/AABEIAOAA4AMBIgACEQEDEQH/xAAcAAABBAMBAAAAAAAAAAAAAAABAAIDBwQFBgj/xABEEAABAwEFBQUECAUCBQUAAAABAAIRAwQFEiExBkFRYXEHEyKBkTJCobEUI1JiksHR8DNygrLx0uEVJFOjwhY0Y3Oi/8QAGQEBAQEBAQEAAAAAAAAAAAAAAAEDAgQF/8QAJhEBAQACAgEDAwUBAAAAAAAAAAECEQMSIQQxQRMicSMyUWGBFP/aAAwDAQACEQMRAD8AtJJJJAkkUkASRSQBJFJAkkUkASRSQBJFNc8ASSAOJOWaApIhJAEE5CEASRQQJBFJAEkkkASRSQNSKKCCRJJFAEkUkARSSQJJJJAkkUkDKlQNBc4gACSToAFW+0/agyk+pRszcTmnDjMjMEYsiJ3Ob16JvbTtB3NOnZGEte/6wuBI8PiZhy4yfQKmKdb7R145qK6K8NqbXWLyaz8LsXgDjhAO6PRYNG/a4YWCvVa05FuN2EjhGm8+q1hqZxMDoAn4Y/x8Qorobv27t1AtwWh5awg4HHE0xEjPceCtLY/tNs9scKNcdxVcQGycTHkwIDoyJJyBVIVKZjCACOIE/HclZ6E9d26Et0vXb1YguS7NtoHWuzd3WM1qGFridXsM4H9ciDzbO9dcupdubNAgnIIgIJyCAJIpIAkiggCBTkED0kkkCSSSQJJFJAkkkkCSRQIQea+0G0Pr3jaH1GkODmsLdcOFoEA8JBI5Fc/TpDX8xl18+C7LtVsXc3rVjLvWsqjMnUFu/mwrlWHln+uq5dCbPHTlmjZ6IJgHRZd3WCrWeG0wc/Xz49VZ+zewFJmGpVJcYkgaTqs8uSTw2w4rfKurq2er2h0U2zM56AdStm7ZqpZqgbVGsZtM/s6q7RY2U2BtNoaOAAC5u+KGN2n75LDPkyj08fFjWo7Pm9xbGzpUY+ny0DxPmyP6laKrDAaT21G+45rwObTP5Kzm1mE4WuBMAxIkA6EjUBbcGe48/qePrlsUE5BbvMakiggSSSSAJIoIEgiggckkkgSKSSBJJJIEigigSSSSCoe267SLRZ7UBk+m6i48Cxxe0eYqP/CVyVzWZrtQFcfaZZ6b7srmoD9XhqNLW4i1wcADyEOIJ3AkqmLrqlrwOaw5Y9Pp7NrBuixNYJAC6ayVSGjPPgueueuwtBJHqFt6tvZTz16LwzLVfRym434kjRaS3BofqM+a522bU1XOcHF7KLILm0WGpUgkAYnRhZ8ddy3FhrUqxDG2ao0EYsTwHYhMTiDjrlkc+QWuXmMcb1rBvMYJO4raXdQdSrUHtfLsZp1c5JFQZ4uYIbHIJ182BppkRlu5I3XWx9y6M/CHn73eCJ/C71C4wuq1y1Z/ldgUE4oL6b4wIIpIAgnIIAkiggCSKCApJJICkgigSSSIQJJJJAkUEUDajA4FrhIcCCOIIgj0Xmy+7s+hWqrZnkvNJwYCDEtgFhPAlpaT5r0qqR2zrWW1XrUdRqNqNLWCoW5t7xowEA6OGFrMxlrwWfJdTbbhm8tNCLDVDDUY4Nwnww50O00nPLPON/JWL2bOFez1DVGKo10GVpBdzKdKWgaLJ7LrRhtFWn9sSB6rxXKZR9GcfR0VXZam2oajHOaHZwMMeYIW/sNDQCSeJUdqYT4S4MJ9j7RI3xwWsst/uoVe4tIDXH2XAjC/pwPJczZfMZ9+NwscORVdV9t22CKTaWKo7E5rnEd00mMLnDU4SDkI11XXbS3qCIzzyVMbZ+KqCNACPitOGS5eWXNlceNfWxe2NK8mEAd3XZ/EokzG7Ew+8yfMb9QT0q8w3TWPth7mOLZD2ktcCCWkgjPcF2Oz/aPbLK4U7R/zDBqHn60DLNlT3ss4fM8Rqvc+dpdiS1N07TWO1MFSlXZza9wZUaeDmOMjrodxK2tNwcMTSCOIII9QqhJIoIAgnIIAgUUCgKSCKBIoJICiEEQgSSRKqftA7TwJst2v8UkVLSIgR7tGdT9/ThMyAsDaDaix2ATaqzWOiRTEvqnoxsmOZgc1Xt59tIkiy2Qkbn1qkGedNgP96qqpWxEl8lzjJcSXFx4uJzJ5prmZZKLp0m0HaNeFspuo1KjadN+Tm0WYMQ4FxJdHETnvlctYLUaTw4ab0x+YULlLNrLq7iw6m0oNnOe6PVai59pa1mtAqU8JIEZ5Za+q5mhWywnRba7ajWva7IjKQZ48iD8Vh9LHF6/r55686d1Tr3leFcEO7th0AxEkwSSGDxEjPyWbfeydQgjvC4sb9ZUcZlwb4WNb7M6EmTlzmOhuu2ubZcVKiWMcG953TMBdh1dl4pPJae9tpm1KTmUGgU8OFumgGZjlks+38Numv3OZtt7AUqLHOJc2mJznPSJPD8lgXpdeKhQrOkGo4g8mugDPmG4vNYtmofSLQykd58R+6Mz5EBdRttaGsoNbzkD+Vpd6ZBW/blJPlxj9+OVvtHDWFmEU2neajT6kfMFZjWd4yfebI9ND8CoGNM0xvABPV3i/NZop4Hu4Ez8ZXreFFRZDR3hMuE6Dwjmp6F4usr5pOdTfrip+E8RmIWLabX3IM5vPsjWAMpPpotY0OecT3a5lBbmyvakCW0rcMsgK7REf/YwCP6m+m9Wex4cA5pBBAIIMgg5ggjULyzUrNboF3HZ3t0+xvbZrQS6zOOWpNEnOW7yydW85G8Ei70EKVQPaHtILXAFpGYIOYIKcqgIFFAoGooJIHJIIoCkgj1QVZ227SFjGXfRfm/x2gD7GWBhP3jLiODW7jnUWDMHitrtden0y8K9oGj3+DmxoDGHrha1YjIc0HqD1CisaoxRMfGRWa6nwWJXpGdEETm6qJzU4ZDzW6uS5++8TmktEEN+1wk7mrnKzGbrvHG5XUMuDZt9pHeOe2lSBgvdqf5RvXdXZcVKg2aNMg/8AWqjxH+UHT4dFn7P2FoaBRp948ZFxju2Hfh/2W/fYA7/3Lw46ik2T6NGbvjuXi5OXLK6fQ4+LHDz8si4q1PuxTaXuI1ewuIB4cFr762bZVJcDhefeAwudPEaHrqs+67Y55AoU8DD7xESOTVunU6mjmz8fTgs54aZa+VaXPs6+yVaj6hDsoaQNBMmRu3ei5Ha+8e/rBrT4QYHOcirwtNjndpwMEfvyXJbR7L0q5DjTw1BmHNBmRnmQM/P/AHGuGX39smWc/T64q7H8fpl6CFnVm68wRPkpbdcdWiS9oJAOc9fUfvNR0a4cM8iNQV7pZfZ8+yz3c9eg+tJ4gH1UY0Ut4sLqjQMyWM+ScLISYBBI1AOiIxqbcTls7rpzVxOHhbOun7CN3WUAF7zA0HMhZFnZi8DdD7XEzrPARu1+SqLn7M7YKt3tEmWOeCD7oce8aOmF4+K6oquOyq0xWtFD7TGVY4YXYB8CPRWOUQCgUUCgYkgigKKARQFaHb23Gz3ZaqgMHuywEag1SKQPq9b5Vz25V3NsNEB0NdaAHtmMUU6jhI3gET1DeSCk7RU8QI8lk0X6xoRjHXRyiqQdM53aEHiOaYx8aZ8eI8lFbeyvDmYhqsG0OJznRMuy0YXFp0PzT7SILggmuq66toJrNZ9XTLC9xHhkuADYOpJIkcJXa3birHuWaa1X7zyXCWG+a9Gm6z06hbTe4OIiYMRiG+Y4cF2tWoyz0HMsNTGHgTVn2RADiT9omcty83PK93prNeGwtV+mzRY7EAX++4Z4epG/ku37P6vdNd9IcMVSKgc6BEDNs8onzXC3Fd4u/E6pFVzgHNwGS9zmh2Rz4wT/AIWuvG7bTbXh1cgDPBTHssHIfMnNZY2YZfhtlhc8fPysK9tt7DZqrmMfTI18LmxJzyg6TK2lzbXWa0iWVGu4xu6yqzu/Ydj5yLiPILoGdntFrA+z1HsqjWD+/iubcd+CYWSTJYTrPTqQ5jv9036IC2HnMb1w1jbeFnyLO+aN9OA8dWu/IraUNpmlrsbsL2iSx/gcNdQ6Du1XG/6Xpfis68bgY44wTJEEDNpnIz8PQKsdorqNF0DQgweIGTgeYPzVo3PfVOswPacnDPkd4XLbdWTvGPe0DwnE3mRId6gn0WnFyayZcnHvGqyvBwZB94saOgjNKwsAz9SsGtUNSqTEAZAHkn220YGBrdSve8DI701H5DwjJoOQgbzyWbRrmIpiQJlwENnr/krU2Rk+0W57iZ9QPzW1o0TObgeRDx8Ij4IjrOzRrv8AiVPAcRwVX13bgwMLWNH9b2mOUq4yqu7KKDfpVV5MObRIa3k57MRAgRGFv4wrSVKCBRQKIiRCaigcEU0JyAquu3FpNho/VYh34+sk/VnA6BAGYcMQ5EDkrFCoftavirXvGpZw8mlQwNbTnw4zTa57iN7pcRPAQg4gVN2Y8sk+JOgPSB6kQmtaCcx6CZ9E508gP3uUVj16eE4xp1Wwa4PaCTm3fxCwavOTz3LMuqwGoQBmpbqbdY43K6jdbLXUHkuc0EnwgncOI5rtjZWtLmsAAAGQA80y6bI1jGtbuifzUt62unZKf0h7oiRxLjuEbyY+a+fnlc8n1MMZx4prhbTa0tIDeQAC6BtmZglo3aqtP/X9IDEyyHHwNQYPUCfgoB2j2ouhrKTG7mgOM9SXfKFfoZ1nl6nD4q17v+rZBEDPMJtC0vJJaRExHLmuU2Yv51rouq1WtBbULCGzmMDSHZk7yR5KybyuKz4AaTTTcBIc0kno4E+IfHmFfoZJ/wBGG/y0jHkOlgwP5+y7nz368VDtFctG30iKrIqNBgjI9WlOdaGVPqKuTx7LhuO4g+a21mMgtP8AEYAeGIbj5hZ6srW2WbVXs93llqvslQwWuynQg5h/mCF2N5AGhAzwtOZPHeepWv7S7ra+k232fJ9LJ8algMmf5cz0lcJX2keWQHFzoynRvPqtJx3O7jO8swmq1NsLe8eW6BzgOgJ/P5qKu9rWslgxEE4jJMlzoOcjIYR/lNYY/wB/3mnVyXNiR4ZIOZMGJ+XzXv1qPnW7qW7i05vqZnRpe4fIjNTtqZkAOI6OPTP9VHYKRxhoOmZ+c5Kc0WOae88IMxxEb5VR3vY/Y6zrRVrnw0mUzTDScTi6o5rgTmYAFN34layp7sP7z6VaST4DSZI08QfDCB0NRXAiUk0ooFBCEU1EIHBOTE4IHSBmdBmei8t3nbjaK9W0Oma1SpVw74e4uA5AAx5K7u1Pab6HZO5YYq2gOaDnLKej3ZbzIaOpPuqhXu3kQOHHr+iLDi8np6AfqmGoeKY55dyA3J9RuQ6D5frKgEk6rqNmmggO4H8lzLQs6w2t9L2SuOTG5Y6jTizmOW6tCjaqdNhc54AAk+SrLau9Ta6xMnA3JjeA4xxP6I2m3Pqe24nlu9Fqawh0rPi4el3fdrz+o7zU9kVJykJjNRvbvCdK2eZ2+xRqE1qTHNBcGmXGGCA+STuET6BXza7WDTaeLWn4Beddi6NS01xZ6Rh9RmEHFh9mN+7wtV62f+EwZzAJkkmSJOZJJz4ri+HcVj2j26pQr0qtJxa4FxB3GMIgjeFsro7URXNns76ApvLodVxy2SIAaIkBx4nLIZ6jB7XKeVI/ecP/AMyqzDvJTpMo6x5LjXpUXdL8FSMFoBy4QcLvgQfVUHfd1GxWqtZHGTSeWg6y3IsPUtLT5rHtm0ttqup1KlqrE0wWsIqOaWggTGGMzvOpgSsVtYuJc4kkkkkkkknMkk6md6cXH0dc3L30nBT25kDiQPUgFQzvKzrJTLTjMaERvE746SPNbMAfVDIwHA0gyRr0/fFbCzVWOp4RMQZLjmT1WrqtlpHAosY8BvduaCd+Y8nblFWJ2bv7m3MAECqx1JwmRpjaeebAPNW4V53um8K9GqwupPFQOa5hYC5pcCI00zXohVKCBRKCIx0QU0JwQOCITQtdtLe7bFZK1qdn3bCWg+88+FjfNxaPNBRnaZeX0i9K7pltIigzkKUh3/cNT1XJmXHkn1qrnuLnEuc4lznHUlxkk9TJ805oUU0N3LIcJGQ9kZ+c5+X5plIau4CUqLiDO9AWMUrWpUyHEwIHLLP5KUNbzP76KiM6clj1GypbRUg4d+9RkqKgwqMthTvG8KJxQb/Yi3Nst5WapUcGtDhjcTAAew5kncA5s9CrPvjtEslARSc2q7OAxzSDB3ubIHzKpKs6cLvugHqwYf7Q31Kzrhs//NUsYJDXNqEDOQHA+i5sJVn7f0u/sQe7w1Mn4Sc8RGbRxIBI8lUMLrdtqdQVsbnOmmfAXSZxOxtIkwDmMhuaOC5e8GQ7E3JrwHjkDqPIyPJMfZabZwCYWZTpN5jpEfJa2g6HAlbOmc105ZJoNLMTJlpkgkGR6clPVfOY3wfULFpPInnknhyKeRqm0WZkZ8gHEdY3SpIUb25Za6hB3HZFdrKltc+ocXdUzUpgzGLE1ocQTqMXkegVzlUz2YWwU7wYCP41N7OhPikdTSHqFcxVSgU0olAojGBRBTAU4FA8KvO2+0ltgpUwcqlduLmG03mPxYT5KwgVWHbq76myt+/VPo1gH9xQVEBmVLTCZSGqmZkVFCk6GkcY+BlMAxZDzKIbuWVSYijTZAgIV6gYJOu4J1SoGiStZUql7p9AiC05ydSpAVGkCgLpUbiVI9yh35IJKwhrOeI/ED8irC2Nph9lpktBMOGYGgeWjPyCr21PBcANGgNHlr8ST5rfXJfraDBTeHw2SIdliLiTlGUz+9FzlPCx0e3toAs7WuYMTnjxZ5YQTrG/Rcf9GFSlhE4mjE2RGuonhpn05rbXrtb3rXUwzwup4BMEYo9qIyjqtK21nAzxRhkZax06R6KaunW41bgQYORGXAghbGg+QFJbKQqDEMTiNHloGQG8jUfH5LCszodhO/TqupdubNNm1FMYU9UT0zIT1DROqeXIOo7PzivGzN4En8Ac75fJXmVSfZnZC68KDx7gqvPTu3t+bm+quslVKCBSlAlEYHe8il9IHA/D9VOaSa6ggi+mNG53oP1XBdsNLv7HTfTaT3NQuflmGOaQTluBwzwGa7x9lWutt2uIyEjQg7wg86UhCdG5dTtfsjUslTvKdN3cumAAT3Z+z/LwPkeegoWN7j4WPJ4Na4n0AUVFTZGq2V13bVtNRtGiwlztN2Q1JO4Dis2wbLWyp7FmqDm9uD++PzVv7G7KtsNHOHVngd5UGnJjZ90fHXgAFL2/Y22Yy1wpjCSIxnd/SoGbGWr/AOP8Z/0q/LzuYPdjjXXqFjMuRo3KopFuxFrP/S/Gf9KkGwVs40fxu/0q8W3U0bk4XY3ggo07B2zjR/G7/Qmt2FtTZJdSmMvE/U/0cJV6/wDCxwQN0jggoYbE2kaupT/M+P7FMzZSo2MeE8QC4f8Ajn8FeJuYcAmm4mn3VNCh7ds+R7AjkSSFrnXVVaZykdf0XoGvsyw+6tfW2Pafd+CaXamLPZdRUJIGmZy8kLbYWuHgcAciJkQZzGmkZ8iOata1bCyMgtBeHZ9X1YJU6+V7eNOHNBzAMRaZ3tJI6ZgZohba17JW2nkaLyPuiVq69nqUsq1N7ObmlvzVTYAwpGCSB+/3CibnoZHFdtshsBXthFStNGh9ojxvHBgO77xy4AorqOyS6yBUtUQMIpMnf7LnHyw0x1xcFYndnkm2CxMoU20qTQ1jBDWjcOZOpJkknUkrJVcsc0TyQNE8QslJBj4UsKcigjwJr/CJU6htLdEGK8lxkpBqlDUYQRYVLRdHRHCiGoJqrZCxsKnYSE3Agjwo4VJgSwoGYUYT8KOFBGntRwpzQgaUApS1DCgYUFJhQwoGRyTXMB1APkFNgRwoMEXfRBxCjTnjgbPrCy2vITsKWFBI0yjCbTGalhA2EIT4ShB//9k=</t>
         </is>
       </c>
     </row>
@@ -3679,25 +3679,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SHUBHAM DUBEY</t>
+          <t>ARJUN TENDULKAR</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>smat2022_135</t>
+          <t>smat2023_068</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>86.40000000000001</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -3706,25 +3706,25 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>36.4</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -3739,64 +3739,64 @@
         <v>0</v>
       </c>
       <c r="U26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" t="n">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="W26" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="X26" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="Y26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z26" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AA26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH26" t="n">
         <v>17</v>
       </c>
-      <c r="AC26" t="n">
-        <v>35</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>18</v>
-      </c>
-      <c r="AE26" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH26" t="n">
-        <v>0</v>
-      </c>
       <c r="AI26" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AJ26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL26" t="inlineStr">
         <is>
-          <t>Batter</t>
+          <t>All-Rounder</t>
         </is>
       </c>
       <c r="AM26" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBUVFBgVFBQYGRgYGxsaGRkaGBobGhodGxoaGxsbHB0bIS0kGx0qHxoaJTclKi4xNDQ0GiM6PzozPi0zNDEBCwsLEA8QHxISHzUrJCszMzMzMzMzMzMzMzUzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzMzM//AABEIAOEA4QMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAEAAEDBQYCB//EAEcQAAIBAgQDBgMECAIHCQEAAAECEQADBBIhMQVBUQYTImFxgTKRwUKhsfAUIzNScoLR4RXCB2JzkqLS8RY0Q1NUY5OysyX/xAAaAQACAwEBAAAAAAAAAAAAAAAAAwECBAUG/8QAMREAAgIBAwIGAAQFBQAAAAAAAAECEQMSITEEQQUTIjJRYUJxgbGRocHR4RQVIzM0/9oADAMBAAIRAxEAPwAFjUZNMzVzNMo3nU0ia4mmJoA7muWNck1yWoA6JrmuSaRq1APXJNImuGNSA5amJrgmmmpAkBpTXAp5oAdmrkmmJpqAHmlNNSqaAVMaRpjQAxNPXJpTUgKmpUpoARpRSJpTUkoYU5NNTE0ED0qaaVAFsTSrU8H4OVRpth77r4UceCwpHx3SdA3MJvtpzo3DdmcGixdxDO/Pu5MegQMT7/KkWLeWKMTTGtLxTgNkAtZuXdPsvhr8ezi3+I96zDGpTLRkpcDGualsqCygkBSQCTsATqT5Vumfhstl/R51IzMoGiZQBOgklW/3ulDdETnp7Hn9NWvx2IwQt2+7Ww7syo/iAVQULFyVBhVd1Xb7B6VFdGDbFkBrK2hZMagW+8JgAvMOygzmG+WN6FIjzfoybGuSa2uEucPZwzraVS11oLbKHRbYKE7lAxyjXxzBM1h8biFDMVEAklV6CTA9qnUCyKrYjUdy+FoG/d2JMa0NeIGpJ66H6VDmJlmb4D2xjcln239DNOuOnTLB+X3VUpjXzAcidPb1qdMXmj5a8qrrF6n8lpbxIOh3/GpZ86oziZjNoRsw5cvcaUSmJgg6axB3B/PSrKY2GVrkspp5qNLqtqp9R0PT0rY9nOxFy+ouXmNtG1VQPG466/APWT5VfUqH641dmSpq9R/7HcOHhLnNtreAb5bfdVF2i7DG0jXbDl0UZmRgM4UakqRo0DWIB051CmiqypujEGlV12f7OXcYxyeFBo1xh4QegH2m8h7kVt7XYTB2wBduuW6l1QH0EfU1LmkTLJFbM8upq9H4j/o8tsubDXSDyV4ZW/mWI9YNed4mw1t2RxDISrDoRoRUxkmTCalwcUxNcmlVhg80ppqVADzSpqVAG7xIxNiwl1rlso5ByaMfECQ8sCHJgy4k67mr3A426w8F24TlzZF7sPGxItumVwDoYeRsRMCq/t5j0WMMiJpld2CgFf3VHTTX0jrVpg+HZglosUc2LV+24+JLqgI59CO7BXmM071nZiftTYdg8bfcE2rtq/l0ZHRrF1fJtwD6qKx/bBEZhc7trF0/HbdRD/66Osq2u/WZ5GtZh7YxiZzNnFWWKM6fEjjqPt223htCDVF2ox3eWHtYhQmJsMjCPhuIzBC9vyMgleUeRgQY9pGe7NcLOIxCW48A8b/wqRI99F/mrS9uOH2gcKLaIiu7KWRVUQSkEkDUCSafs1cs4LCG9dbxXiBlUgvl1ygCRGksfWi+PJhbqYNLj5LTEqsMAVDWwUDEzl2AM0N7lpybkT8Qt4PChbdzBjuSut7uw/imMrGCwYjXMSPKapeF4KwmCxWI7tXXPcFk3FDEKPAh1Eg5iflWhXJhLF3vsSLlmPAjwzhcsZJmbknbSqu7hA2CwmDDKO9ZDc8QlUAa4533nKvqRQUTG7D9n7fci7fto7XT+rDqGhANCAeZ8R9MteXccxAW+6IBC3HAI2iT91es8c47YVb1uySLuHsvkI+ACElVMwTGXlyMV4liGDGTv+NQ3RDbb3IHvNJXTSdhr6b61A5JkDyiPWrOzw8vqAaOt8DLGByG9JlkSLxxtlMlgqNNSPi9/wCwoa4Dmke/9fWrZ+CXwxyqdd+lW+A7J3Ms3N+nKoeVJErE2ZS1MFSCQfLbzpMXC5SDG/yreL2dCxp6+9Pf4CrJAjaiOSweKjCYHiDW7iOAGysrFW1VoMwwPI7V6x2r7ZG6iW8M5VHtq7sphpcT3cjUQN9vpXmPFeGNaYCI51bYXCFbFu5ByvmEn99DDLPplPvWjHuysF6qZ1VvguL4pk/RUvNkuEJlOvxELAJ1VddgaqKL4VfFu/auNsly2x9A4JPsBNOo0yjaPTu0OOXh2DS1ZADt4EMDQgS9wjmdR7sK8qxOJe4xe4zOx1LMSSfnXov+lHCM1uzdXVULq3kLmTK3pKR/MK80IqsOCmFJq+5ZcK45fw09zcZQd1MMnrlaQD571X4i+zuzuSWYlmJ3JJkmuCKamUNSSYjTTT1yaCw800000jQB1NPUdKgD0VsAcZxN1PwK0sTzRIXTrmIj3Na7E3P/AOhZX/2LpPpnSPwNZLA9phedFvqy3VMW79oAMCdIdD4WU7EbeQ3CxPajJjGusFuNbtG0uQnu2fNLMCdQnz23O9Z2mY5Rk3VdjR4y6LHELTAgDFIbbrP20/ZuR5zlrCdocX+k4x2TUMyoh6geBT6Eyfeq/H4971w3HYlzz2gDZVHIDkKl4DfRMTZdzCK6lj0AOhPkDB9BU6Rkcenf6N/cfBYJreGe2kOhL3GUHbYtoS2ZgfIUDwzB4ZLeOxCIj21Ld2WUNolvNC5h++8ewo/jODwhuPi8TcR07tVRJG4k+HK0sxkx6n2D4Jbt4nhxw6XFtsXbONCVBul4gkaEQAfKoFdrBb/DLacPwts2073EXLaZ8q5/1jG4YaJAyiK0DYbBtiDhP0VCe67xmFtIALZQpI1DHegbuNtXsfh7Vt1KYVHcmRlzZVRQDMGJHz8jVdx7tw6PctWbagqxQXc0nTQsFjfeJJoSYKMm6MLxq0tu5eRDKo7qpnkGIGvtVRw/CqzyemlWF4ZgZ571Nwy0AAY1/IquXZDZR3RoeHcORVBEHyjyG/p9atMPhlHIa7xQGBmKtLU8xXPk7NKRIbajSK5dqkdhUVxhNURILfY0DcuxVhiL6xEj3qqvYq1s1xQafjQubSM9x2XM89q1HZrAC5wW/wB4AoR7ly2x5Mqj8TK+eaqbiFrwkrB6HcULw/ANcw7XO8fIHK5ERrniylpYBhlXw/Frry0rZDfYy16rNlwjsThsTaS9bvXQriSsISp+0maNwZG1Tdo8Nw7C4V7KqjXWEJqHuBuTM32ADrGg30rP3uzVy33im+QEGY5FlWlnWBLqM3g1G4kDWq7/AAYG53a3Cw7rvmPdHNlKhgqoHJdoZeY59Kalb5L8vdmt7JdrLT2/0XGFYjIrvGRliMjk7EDQE6HyO5uK/wBHeHuHPauuinUKIdf5SdY9Sax1rswzRFwSQreK24GV3NtfEf8AxJibe4k6mKlwfAcQLYa3fKShdkzNbZQLYuaiRMZlU9MwO0wOuzI2TtOjY2+zWAwSNcxDB9N7sfJLY3J9Ca8uxrobjm2CELMUB3CycoPtFXVzs/cd3He5mt6NmRxJy3WIUt8Y/VEZhvmGlZ5h1BB6HcVaNfIzGu92NTU9NFXHDU4pqQoAeKVd5D0PypUEWHTTk0jSNLIEaVIUjQA0U009c1IDmmNKmoA4ajuFLLgGIj8/nyoexaVj4iQoEsQJMaCAOZJIHvVvhcELd1CpYowJBYQw8M5WEb86zZ5xrT3JlF0mE4nFuoy24WN2O/oo+tVOKxmMTxK4I/1mH1q54nhnKzbGvrH486zV/Ck/Hdj95dYkGfDzPSWM+dY1KyJR+BWOOYkt4yD6R9K0GLv3O67yDMVWcP4arOWCtljSdpjU66+davEYacMU8jH31V7yLxi1E8wxuIuXG1cgc/L1kxRVi1aTQsWfoTr8pq5s4LLqqAmCpB5giDy3P1oZuHMcyi0AG3J15z1NNjLsKlB8knDVBmNjQGDt3O7LKGy7MRMeYPlWiw3Dwi6T7marruHJt5kfW2x8APnrI6z9xp8Z6VZWEfUV633Ew7Cd4YiZ3mmVyCCCQRsQSCOWh5U91IJHQxUdbFurGUjs33iM7QDmAzGM370Tv570mvuTJdiTMksSTIg79Rp6aVHSq1IKRN+m3JB7x5AAHjbQCYA10iT8zULuWJZiSTqSSST5knc0xpqASoakaemNBYalSpVIB/8AjGI/9Rd/+R/+alQFKooikWZpgKc0hSyRCkaUUzUFRRXNdimqQOSK5NdmuYoAtuz1kO7DplJ9Bmn78tWZxLXLxISEQQGnnqAOgGtUfBcR3d0GYDSpJ21gifcCtQMObdsgLoSWaTqDPKPiGnlXP6mNT1Dou40HWkkVE2ABM5V+QmhUx4UR71X8R4/lWAfQCkNoIrYuoRTkGrRsOXrRDqoSJB61ncClzu2bORcfXrHl51UYm7il8PxHqAQPTnRFktF5cZbRLaFJE66idPlRgNsiQayWDwd0g94WM8jsKkt4hrfhnTl/Sry23KR+GaLFMMulUVjDxcZh8Lzm6A7H/pUT8QJ0micXeRbUhgW+yOhOhMdYnWmwWpJC7qRSXWliepP9q4Ip6VdFbIDmmIrqmqSxzFPT0xoIs5imIruuTUkjRTRXVMakixopUppUBZvOy+BRLb4y8mZE8NpInPcOgAHPUgDzJ6UTxvDLisL+lJbCXrRy30CldNPFlOugIbXWJ6VaLiSl+0LVpnwuGJs5lyz3rwhcAkSwL5Z/13NEYvirrizcNlhhwq2b7vlGrkFCROwNxR6O1ZbMjm7szfZTsr+kDvbsramABozxvB+yvnueVaR+McNwp7tEQkaHJbD6+bn4j7mqTjuLuYO3cwS5sjNmtPO1pySyT1DDL6MetY2pSsYouW7ex6cg4bjpVVQPHJe7ueo/eA9xWOwvZpruKexbcMiMQ12NAvtoW5R1Bqir0vs1GF4Y18KCxR7p/wBYiQi+mgHuaHsRK4LZnT4ThuBAFwIzxMuveXD55YOUegArlOJcLxJCMlsE6DPbyGfJ4EH3Feb4m8zszuxZmJLMdyTUJqaJ8t1u9y77bcEt4W4q23lbilshMskEDfmDyPka5s9qiLeVreZwImd9Nz51Q3jOpoc0SxxkqY6CaRobzzsdD+fwoRsLFxXYFgBIHUkxT4J81teo8Py2+4irPDQ2hG1cvJHTJofF2itscSu3rhtWyLIBAJfQ67b6mfLrVkOy95lDDFBgcuoMDxD76KuWVYSVUkdVn+9A3btsHW2vpLGfOKE0Ci+zKfjPDHw7HLigzg/Ap8R0B1A12n5V3gkuP+0AEDMeo9fOj1feFCzyVY/ua4xF0pbIjVtKu3tSFtU7bKsIc3h1MwB1J2Hzo/tBwRsOwMXchOhuWyhB6SJU89jOm1NwO2rX0L3Cioe8Z8hfJlIhiv7ucpJ2E16ZiziGtlblu1i7Drq1o5HI5MEJKt1lWB0EVrwLSjNLI1I8gitL2SxuFtLd/SYJcoFBQtAWWJmDElgP5fOqLFoguMLbFknwllytHRgdmGx8xXp3YXhCWrCtcVe8v+OGAJCD4RrtoZP8VaJPYtkktJV3ON4Ausm3kIfMBbg5nciYNvTKrEg5vs7VWtxnCsmKOSyvxpZAtguwlyp1TLlbMo5Fco16WXYbAWzcxVwoj3bdx1RGjwiXgidszDLm5RXHGsRbxV3DWLmFeziu8t5wVXLkJ/WAOI7xIEgxyNU2sTsnW5WYDG4FbWGRu7ckp3uZCSoU3HfMY1LMyKNTsOQoLtDj8K+HspZRBczZ7hRQMsqZUnKDq7TGoGQdRWh7UcPXFcStYZFVURAbmUAQpOZpjnlygfxCpv8ASTYtjC2jbRABeCyqgad3dESOUj7qsqtExa1I8zNKkaanGkRpqcmlNSA1KnmlQB6p2U/7ivni7f8A+lqiu0//AHTH/wC1tfhhaGwuOwViylq3ig8X7dwkggwHQtsNgFmpMZxHCX7eJtNikUXbiMranRVsmQDuM1sj51lMjT1XRW2B+n4I298RhoK9XSNPWQI9VHWsXFbjgmGweGvLdXiKMACCmWMwIIgmTzg7bqKg4djsDcxOIW8id2zl7buCsSfGpI1AJ8QB86shqlpulsZKxYd2y20Z23yqpY/IV6N2VK4nAPhmMOoe02mqhsxRoPSfmpprnabAYVSMOgZj9m2mUH+JyNR86xeH7QXUxLYlIDOxLprkYH7J58tDuDrRuyJaprigHHYS5auNbuKVdTBH1HUHrQ2WvTE7R4DFoBiFVSOVxdB/C67D5U6Y/hWG/WW+7LDbIGuPPkTMfMUKTJ8x8NbnmWJw7ocroyNvDKVMHYweVBMtaXtTx39LuKwTKqgqoJliCZJb35VRMKumOi3Vsn4c5ytHIg/MQfw+6rXDXRoarODHxuvUA/f/AHqfE2GQ5k26f0PKsHUJayd+xpkykcqje3a5xPqayb8TZRBkUK/FiTOulI0MFOuTWMbYPKBVHxPFAtpsKp73EmY6GuEljrtToxS5FTm3wafsZxNbGIF1x4CCjH91XK+P0BAJ8pr0DiWFfBZsRhv2Q8V7DzCR9p7fK2w3IGhrzPhOTvEFz4GOV+oVwVY+wM+1abG9pR/hYsNcXvjFp5P2FI8foygL7npWvHFyWyM82k92Vt23h8RxHMLiJh3YXGZ2CAAqGdDJEMXlY85rcYbtXg3xJtyi92rBbzOgQiUzKjTsYHrk8qzXYLhKhruIvICLSgpMETDMzDkdBA9TU3EeO4fiFi3bZMuJe5bVVCscgN1Q0OQBrbLGOsVeUadEtxlxujvheGwV3vHt4ruMSLtw94LgHhN1ypVWYK6lI6irXE8WwtzH2P11uMPbukuWRVLvkVVViYYgZjA613j7C3OJ4e2FGWxae6RlES3gWfkCOlR8Le2LnEMWyKUR+7UZREWEOaBGhLHX0FUIb7g+B4th7JxWNuXEd7lzIiI6M/d22yIAJ+1lzegWge2XELF3h9o2WUeNGFvMpZRluA5lBJHxffS7dW7dzBWcQbQtXXKQsAMA6lmRoAmAJ1rzsmmQje4zHBOpDGuTTzTU40CpTSNNQA80qalQBsUtYLIua42YI2fLmlnYSpSdDkMrGxgetQ3Uw4N/IUaD+rzs6gplaWTLqXzZYDaQap5pTSKK6Ps0161gM/hfwzHxOAYLRMyYJyyw5HSCKisWMH4c7oHLqGCO5ti3nthirHUtBaJ0jNvArPBqU0aSNH2W/EBhwji2qZ+8UKVdm8BQszAZiCQwC78/SiFw2FzkZreXw5T3ziUzeN38PhuARCeZ0MVQTSmiidP2XiYXBgZmuHKRKgN+s8Np80qRAY3MkA7z0rq7hcIGAW4rLnAdy5UgeD4FI8QILEk7a7RrQsa5o0kaH8hXELKK47tlZSqkQ4Yg5FzBo1BzToabh2D724F2AEseYA6eZJA96HCkmACSdABqSegHOtTwjANaQ5xDvqQd1A+EHz3J9R0rRhgpSSZm6zM8WFtc8IpcLrdulVARSqKABvALa7nTKfPNVhUOG0e4h3DlvUMBB+ntRBFcrrX/AMrH9F/1J3ZX4rDA8qoMbgVn4dfStY60DiUB5VjU2mbHBMzlvDRRFmwas0w46UmSmrJYrykiKysVzjuFC6Cylg55CMrHlI3nz+6iLaUUbZykDc7evL74rViySTqPczZscWrfYK4Mzfo4Usy50yPliYZYYa6T08xVriuIYKxisIlu2oW0c125khjNsqmYxLQzByR0HnAdq3lUAchHyo5OD28SsOjlwDDIVzgDXZtHGu2/TnXZ6rGlCMnzwcTw3NqySi+KbLzFcRweHuX8aMQtx7qIqW1dGjINFULqJMEk7RVXw/tAmE4cjo1u5fdy7Jn8Wa47MSwUyIXT5VneJdkbqAtZPfoN8oK3F/itnxfKazbAgkHQjQg6EeRHKsSgjswhGS2dln2i4/dxjK1yAqTkVZyrO51kknTU9KpzXRrmmJVsaUklSOaVPTGpARFIUppGgBUqalQBY10K5BpwaUWHpppqcUFR6VKu7VtmYKqlmJgAAkk9ABqaAOIrQcG7J3rwzsO7t75miWHUA7DzPsDV9wLsslkC5iShfdUYyiRzKj9o3lsOpq3u41GJ0e6QJGcwk8oQfWpjGUuEYs/WwhsmQ8K4dZw6zbUQPivsJ/lTSXb0AXy61uPbxk9amvYl7rDOZjYDRRtsK4x66z7fI1qw43jyK+5yc2fz8M/qmZvi9kqwuqNtH/h6+x19JrsPIDDUGrQrVeMH3ZIUeA6x+75Dy/Cs/ifRuS8yP6jvB+uSawy/R/0ImeoLrijGs6aa1AuGmvPNHpkCsaHW2WNWwwoA1FdJbAqyBg9nC1NbSW8k+9v7D7z5UbbtaSdBtPX0++ucoAgCBXY8L6fXPXLhfucPxjqvLhoXL/Y5mireJNtAykg5oBHmDQ0VJeBKIo5tJ9AD/UV1+r3UY/LRx/DdvMl8Rf8AMvMDxZn/AGttWIiG+Fv94VHjr2EviL1lj0ZgGYejgh/vqHClQojeBJ+dC4waiNo6ab1TyMcpNVRRdVlgk0yvxfY61c1wuJWeSXZB9mgH/hPrWY4nwi/hzF60ydGMFD6OsqfnNa8Vc4e63dgEypWCrQynyKtIqmTpXH2s3dP4u3tNHk0UjW1xfBLF34R3LnYpLWyeht7qPNTp0rK8T4bcsPkuLE6qwMo46qw3H3jnFIlGUXUkdfB1ePMvSwImlNI01QaR5pU1KgC3t4d2VnVGKpGZgCQsmBJ2Emo63+GwVpra2mzLYUz3akC5dYfav3JCJ5IGkQNthe4e2uUJYweGy9HupPuER5+dZ9Yl5q7HkdOK3nH+zDsjXFw1i2w/8u+4B8sj2wpPoV9aF4V2et2xnuQ77gb213jf4z5nToOdMgnLgpk6uEI2/wCBQ8M4O92GZu7T98gkn+BN29dB51rsLZtYVJsJDtANx4Z9ZMDkg8hQ106mTJk6+lH4hZQ+Q0/PtW5dNGNOW5w83iWTLajsiMElGdiSxmSTJ6fSlgdm/PWpXHgIHShsE+p8x+B/vT17XRz2/UrJMGkMZ5afX6VxidQ3UEn5micsEnrAj0/60FibkPmHofP8z9xpGaMpepcrdGvpZxi3GfElT+vsHJoLH8UtWVm64XoN2Poo1ND3xibpItjukk+MwzkdQNkHzNVv/ZEEl2dnYnUsZJPuZNNllclsv4iY4YwnvLj4/uWGG4jZvKHtOJaQUbQgj7gSIMedFJ8jWYucHCPoCACAy7ada0NnDOmmYsvLNrHvvXmeuxeRJXwz2nhmVdXB6dnGv1DFSaKw9hFOa4sj93afU8hSwVoxmI9B/Wnx6oUIdwokGcwXYggT0018qyKW60mzytnqFxG9mZdIkmANgANAB6UNp1FA8SNrEZEFwGG1CPuIIIMGSPI12nZfD/uf1Nej8MlKOLjuzynjkMcuoW/Zcbk7ip0X9Yo1hQAfVv7AVUngVpGIGcQfsuwnpqCKuuGIBI1Ox1JJ5iSTqTtW7JCUmpPhX/M5mHNDHjlCNtul+iDkQL4f+lR4lPCTzAj7wfpUlxiqzvEafd9acvmHrz5aj+9UVp2LdPYqiNYqwsPKAVW8SuZSR1j11AqTAOSQvQDT3Op9orTPeNmeCp0SmDcPOAp2/PSosYEuDurqyjanUZ0OwdDyYffqDTYhznbWYgQOUAHXz1oPEXJZGEag+v50NU0qezGxySxS1R5MlxXh7WLjW2IaPhcfC68mHT05UEa1nHLPe2yw+NNR5iPEPlr/AC1kjWHLj0Oj1HQ9V58LfPcVKlSpZtN9x7ha4a9Y7lbiq5yHOxyuZA3IlZza6COVXGCwy3Mq93azsCyJdQFLgXRglwDvLdxSPEjF4g7jUUHEb74ziC29YF3u1WfhRH8R9YVmJrX4i3bb9KtNI7u9bu2yphkZ0R5U8vGHnyJ61nptpGPK9EbYFiFCiFS5b1AdHvNcVWDZfBLEAR0jSNBU+eNKCxDzPMnX1O/40+IuxlYeTEdQeX3z7V1IY1GKR5vLmc5tsixaQfWSfnP1FFYW7MyNRG/Tz96gxLSs7ZT8zz+6hrLkGRzkepp3uj+Qi6kWtxfCQPX1qsDH8/hR8yszE++tAMd/v8vKjH3CfyWNq4CBJ1jWPlpQ2OAmY1jn06+s/jUNq5lI6fhPP1oq/YLr4QT0gb1VrTLnYtH1KkgfCv8AZ5HX1P5/CnvPlfbcCfp/SlawN0t4bbZpG+kTtv5A11iRKg7EagfjNS5RctmRpko7oix2EDgNHL3ihr+LW2i5lZ22CrGsaSSdAPyBRWHvgDKdRO/XyoS+CGI6fIfkUjP0kc6Sn2Zs6Pr59K28fdV/kDxL37qktcFpSJCW9WPkXYfeAKqU4BbYy+Zyf3mLH3JrUYZ5AWeonr5VE6Qek8udXxdLjg6UULz9dnybuTBcBhEtfAoG0wOn41fBZHtvVVl5aen9asMNdkxIMDfpH9qdOKStGaEnJ0wNt9dOR9hH0qfCqQ2x2PLprrXd+6LZ2l80sGAyxoCZ6TrOnLqARWxt0KxzeEnPonhkEMfFlnl6Vll1TaqK2+zdj6Gt2wzHvA0MzoenUa/P51Hg72pEgwBqdoBj60y4oXAVfwt4cqqpObeYjXXz5D1oHvMrwfNYHXzpmGanFxezQjqMUsUk+xzjnJuHYgD4j76a11w26ATAiSBO8661Bjm2PUbDYVzhX215j0FaauNGVv1WS4i/lZ9SPE0AeQA1+6oLCZ1WBEa6nl+fxofHXf1j+LmfXf58hUmHuQg86IKkTMmtNFxh7/WslxTD93ddBtMr/C2oHtMe1aTEPFwHqB9R9KA7S2ZCXBuPCfQyR94b50rqYao2ux0fC8ujLp7P9ygpUopVzj056p2J4P3GJcYgxiAvgU65lb47itsxnQxqNZ3qbiE/pWJadGa2oH+ztgH/AInYe1Zjhnad4FvEk3EXxIde+Rl+HI4MgnaTtPsbt3Y6uZbdtviOrbAcyeVT0uNudvscbxPJKEafL/YZmkj8KaSQRpKzHvMfWogdRz12FQm8QzHTwkjzg8/bQ+xrqNHn4snwNzUrvO31rl9DBMf8tD3jDGNPzJ9qnzZlnmN/MToKK3sOUF4S+BpEa6eQPP5/jVhhsFbJ/WyCSSF1AMCd9pggnXptrVMiEzzI3A5np6CtOttgLeYgZEuMx6uNAs8yvTyrJ1ctPDN3RQUnclYFxPhqqpdAwyxmU677E+IsPcAVY4LDOqWwWbxZiwWBGmZYjXmJ570JxXEIxW0p8PeAZv3UYQyz0zE/Lyoo5MzZ8i5WVozZjlDHxGftlVUaGYIrJKU3BJ/mbYxxqbaI0wlsOucqArOSpcsIXLbRddSNzqKoLsBntz4czBTy0JAjy2qy4jxJTbVF1MKzHw5VYlmYLzzHNB5ACqXEKBBGobbyrT0mOS3kZOsyRfpicFfn+Fd33UqDr0PnFcWnhgfPWd26iu8aCoJHt5A9K3fi3Of2I7C/aAMg7dPOpbrg6gb7+XpUPD7m4OzaE9TUj2yIB9oofuBcCe3Bjl15nzorCpDoeRPKZHXbUmNa5ZZQa6jn5fWlh8pUrJ6g8/bpS8nqi0Xx+maZxAa/FwnK1xQ2bQ5ZMT7e+grWOxBy6QPDEeGNojpWaxVs3GzJmZ2MMhChSoEgjXbSJJ3++H/EcSiFAzghsoBUHT+M+LMDA08utcfJjc0ldNHoIZFyt0zjiCi3iCLZChHBB0hSwlhB5AiI8vOoeLgBpDAqftKF8e2sIAAJqW1ZZSblzw5CGAcEly2oJI5mN+RG1A3sV3juw1mSpbkJOkbdPlW3plc7XCVWYesklCnyc32m2mvlHM+se3zqEOQNR7D60M96PLnJ39ulJLvgflp7nn7f3ro8I5dWD5yzvESW+goxdSAOUCq3CESTzJP9/wA+ZqxsEzUJ2TNUcY34/wCUfiamxad5YZRuVkeqwR94j3qDG/H7UZhG8I0qWrVBjm4SjJdjFZh1HyNKtX/glr95v90Uqy/6dnc/3RAnA7Ge+gOyy5/lEj/iyj3rVXX0b1qm7KWfjueiD/7N/lqzbVX/ADzqOmjUbMni2XVm0/CGR9Bvv0NDM4W4ynQEwZ10NdWGJEA+1BcTfJdB2kc/wrT9HLiG3TICncHL6hefvRV10tz4hB5/nptVNxPFZFLfaZdD0jf8Aah4S4uJbQ8s3v4jUXRdQ2sv8DxEK6sq6ef41OXdZhjDSDruDqZ9dfvqvyBTH5jlVlhzmQg78+vlVZRV6iYzlVJnWHTMsdTp69a4tkK2p02b+1PYJVtR6+nlT41diPSPrUbJ18hbqzjE2wIIHty9TTg50I58z5/3pWXDKVJ9T19KhQZW9dAP61P0+xXvYOuh10P4UdcYNb2nl6nr9agvprIH8X55U6ucu8Hp0H0qz3VkLYFw2ggrr05CrNmD25jUbnmTzoNU0JH9zXeGuwY5GiW+6BMnwz/Z5bgfjNRlijenPyqRkAOYe59efzpsaBlzRtyFVT3/ADLNbCxQkBgduf4fnzrqxi3IgnQa6xrrM+ev4CocNcDLB1PTkBXLAB9CZOs8hyI9KpLHF7NF45Jx3TorcdfcsQ5J1Ok/fUeHceKRrp5AA0uInxSDoRqevpQ9s6fTYnpPlvTVFKNJUVbbdsbFiWkHkNTt0+lRYbZh1j1O9TYlZ1jYe2/96DDwH9PcxPyFWv0lorchw2kecn7zVphjVVYbxD0qw70qhPM6D8/naoQTW5ziDLe5o6wfCPz6Cq5t1H586sU+AcufzpgqRPn86VRe9PQVJezP7A/xt+C0Vb+3SpVmwexG3xD/ANEgLAc/X6Cg+P8A7VPb8KelTu5khyD9oP2Nv1H+ahuA/En8TUqVLNH4DR3/AIh6D8aKwvxt6UqVWfsER5CrnxD+Nq5vbH0p6VKfKL9mBWPiHv8AgKKxO49RSpUx+4quBN+zNBN/malSoXDKsJt7D886FNKlREksLnwH89KmxHP+H/LTUqqixT4Dc/w/UURiOXr/AJTSpVaXJXsVfFdl9TQ9rdvSlSq/4STu/wDsz+eYqtu/A/8As6VKqr2sZHlAmG+I/nkKscR8KfxCnpVKJn7kdXPj9vpVlc5eppUquuBEiOlSpVJU/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxASEhUQEhAPDw8PEA8PEA8PEA8PDw8PFRIWFhUVFRUYHSggGBolGxUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OFxAQFysdHh0rKy0tKy0rLS0tLSstLS0tLS0tLTcrLS0tLS03LS0uKy0tKysrLS0tLSstLS0tLS0rLf/AABEIAKgBLAMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAADBAIFAAEGBwj/xAA/EAACAgECAwYDBAcHBAMAAAABAgADEQQhBRIxEyJBUWFxBjKBB0KRoRRSYnKxweEjM0OCkqLRU3Oz8BYlNP/EABkBAQEBAQEBAAAAAAAAAAAAAAEAAgMEBf/EACQRAQEAAgEDBAIDAAAAAAAAAAABAhEDEiExBBNBUWFxMrHw/9oADAMBAAIRAxEAPwDzU1wTpiWBrgLq5kEcxjTtF2haDEGswiiBEZqECmBAN1jLRVjOuDjmd0glkkrtJLFTtNViNMIB4doFxOVdsVZrJVuJaayVbwaBaQIhGkAJFrEzEd0vDbH6DC+LnZf6/SWWh4dUCc/2pH3mUhAPqcH6w2Zja54iax4TsartMD0GR1xUuPXfE3drlxhUV/2SMHH1EOpro/LjCJqdRbpa9SpwgrtGSvKQQ3v/AMymbhF4/wANsb7gcw8PL3jMoLjYTq6y30Sys7FlOGBHvLfRCLK20glggiemEeqghkWAvEbA2i1wjLoWKvUJvBARm8bwJE11M9ITRa/pGWi942klPqOsGIa8bwazLTRmpMiQMiG01NtNYknUdnA3Vx7kgbk2glBqBvJUHaS1iyNHSKMpG6otXHaxBNWGJMd43dEHbeblZyiy0rSyUym0ryzR9o2sSC5kLJimasMxXRWayVjiWWtlc8kCwljwzQ/fdcj7q56nzI8h+cBoKwzgHoMk746S5bWAdV5s4PTCgD5R/T/iZtbxnykbzYDy/KuBtt08sxW7iLgcpUc2AB2gwWHgSfOBt4gp25QvlyjB/rEbtUCcMOuMHYTLexXtcnJHKx2JrcdIem+xNiSw8NgWHoR4yl1hPgckee35QtD8xHf7Nune+U/WaZ2u0uDHnU8wGCCmQw88/wDv5Q9mrcDALYbOcYB2wen1zKkahkySO90JXcEef4Qem4kwLHPMue8h+8vmp8CM5mHTZy9w2xycfePUZ8D6f0hdGsrdVqVI7uzKfxBlpoh3QZqVzyi404jtQiVEdpmmDOdopcYdmil7QJO47yE1e28ijRiaYRa8bRpovqOk0wp7+sHC39YKBYYMwkgZEJprEkZGKdvyxbUCOkRTUzJUWugtOIXWmQ04iDdSx2sReoRtIItqJWWdZa3CVlo3mgY0plmhlXpessq5IdZjzEmrYJWauV7x/VRCySb0rkP7gj8v6SaXMVIJIwc77YG2YKl8MD5Z/HwidmoJ29Dn1mK3L2NtqFXujGw3J84G1gdhufQCKvvLDg/Cndum3viZuUk7t443K9iYqPVug8znaZZQD8uAD4nOSfadcOAlfANn9baJPw3c9xgVOCBy4B9+v5THvR09mubcP0zzAbeWD7HeDKsCPQ/ifETquHcGNj7Z26n7qeY9T/P2g+OaGul8Y2x9DH3JvQvFfKn0Gn5mIPygkZ88Toa0AAAB6eO857twD3dhsfDqNjL/AEanAyc4E3PLlfCy08dSK6dY6qzbCDvFL3jF8rtQ8kV1Fs1U8U1L7w2lMZBacBgNR0hhA6jpEKm7rAw13WBgWGQaTkDIhsJGbaaiK7xojq22jrnaVmvs2mWlPqm3k9KICw5Ma0okDtYjEDXDMZIG3pK20byysldZ1mkLpessaojp1lhUJAZJG2TUSFsErNVK95Y6mV7yqa09LO6ooLM7BVUDJJJwIPiHCraH7O1SjjcqcHbwxgkH3ln8Pf8A6U9RaB+8aXA/MiWXxrQCEIcu1QFTDBwvU5yfU4/CcMuTWcj0YcXVx3P6oPw98PdsvaMO4dgPMCdNoeBVVNnmC+SlvzxmWHCNOa9JWANzWDt1GRnM4bjlbB2PZ3d0FjY5K5GeoJBJ6+E4buV09EkwkunoI0qnbIMV1XCK2OWCnbG++04Dh2qtXlcNeockKecujEHB22/hO1p1lhr5yDsM53x0mMp010xy6osqdEoGAAAOgG0U4rwVLASyhttvQ+E4riPxFcG7t7KN+6qZBx6nby2jnBeJ6o28rWuHGC1bqBlevTx9xNTG62zeSb05HX0clhXyZgQfXO2J1OmTAA8gBD6/h/8A9oGCBkVKbnVhle8Cm48d8H6TFE9XHlt4+TCzv+ab00eAielEfUTo5E9QJV6iW2qEqtVIKbUdY1pYrf1jelE1FTYi+p6Q+YvqTtIKq7rBQt3WDgWpBpOQaRDaRBkmmop2tjbSj192dpZ6u3AMorWyZlBgR3TiKAR7TCINVQjSCTGMChZEXG8eaJEbzQM6cR+sRHTiWFQkBBBWw0FZAqzUxFo9qYi8EzTW8jpZ/wBN0f8A0sD/ACnpuv4OtiMpwUv5mHKAWQnoxPodxPLTO84B8V0Cha7ci6tVqUnmIdRspyPTGc+WZw5sbdWPX6bOTeN+XWcPTCKv6oA/ATNZwxLR4g+cilnK30/Oau1+J5ZXskIL8O1IclicdAekuqtAprNeNmBlQL/8VwWUZIUZJ98SCfFCAfKyfssp5segjtahLUfCSOcjl2bOGUEc3n7y30XB1ryzYZz1YjJP16wA4iDi5QyhwOYNkb+eD0lguvDL5y6h0xzPGKill1/TtEqpQ4xkjy88ZY/hKSuW/wAY6oc9dSsGCr2jEfrMSAD7Af7pSVNPZxY6x39vDz5by19LDSx9TK/TmOKZ0cKFqJVamWl8rNSJBTWjvRzTCL2rvGqBNIUxbUnaNNFNTIKu3rISVnWRmS0ZBhJmQaJCaYBMaYIpd6+7ORElEyx8mTQQDapHdMkCix2hNopMLIMIfEgVggcRUrvHysXKbxFS0yx+sRehI4ohRETBWQ5EFZAqvUxNhH9SsW5JEtyTRWNFMekiwHmPxEC9S58jPmAfoRmLXVA+OM9ZsPhEz/00H+0TQYEz52u76svYtqOJuncXTW2dRzBSU/KLNrnG5owdj8r+P1llalnVBk+kAL9aNuUgefNn+U1LCHRxTtQUNNtZx1at1U/UiEezs6nfxRGI/ext+eIcM2CWOTKDjutyOxU53BsPqOi/z/COOPVlJHPkz6caokEapEAojlInvfONaeNgxaiHkKjaZXXx+2IXSCttXeM0iBs6ximaSTRPU9I60T1IklVZ1kIW2QmSgZBoQyDRQbTBMaZiMRtBGKlg1EYrEIzRaxHKRFqxGqoqCyJEkJjQIeILl3hjILFmjVLGVEHSIwBCqBEQVgjRWCsWDUituSWvwp8NW667sa+6qjmttIytSZxnHiT0A8fYEi5+EPgy3XNzEmrSqe/bgczH9WvOxPr0Hr0nsnBeCafR19lQnIpPMxJLO7frMx3J/hBpzWo4XpeGUKtIFZZlVrzg32tue8/0Ow29JOvjo5Qwy58Wb+Xr7Rv43p5qkOMqtqM3luGUZ/Gc3b0+mBPNy5WZPVw8cyxVXEe+WJ6sSc+pOZRPayHxMvbxKrUdZ5rXr12aTjG22xmLxNs5LDEqdVQCYfh+lA36mW2d1c0s1rAKpZmICr052J2Az5mcVdW6sVdWWxWIdWBVlbxBB6Gdour7BDfjmNINmB1PLvt6zqeMcCp4tphqKuUasV81Vo2W5cZCWehHQ/d9sg+n09nd5vUTw8hSO1CL26d63auxWSxGKujDDKw6gxmqep5TVIhTB1ycghb0iVwjtsTukFfYN/rGKoC3rD1TSSaJ6mONEtTJKyzrIZk7OshMpqQMmYNolAyQEiTJCKWCCMIIOsRhJzlOWOkljNZgVhRNMaEzNMZDM1mRSYzSQbNMQxGlhTL3g/w7q9TvTSzJnHaNhK/XvN19hmN/Z58NjV2l7Af0anHONx2th6JnyxufTHnmexqQoCqAqqAFVQAqgdAAOgg1p55oPszsODfqEQeK0qbD/qbGPwMu6vhXQ6UoOz52YMTqdUyulfLj7hwvMc7d3bBPhg9LfqlRTY7KiICzOxwqqOpJlSurv1P92DptOeltiBtRaPNa2GKx6sCf2RCpa6bWacABbqiBsD2inP1zuZG/i+mU8pvqLYzyq4ZseeBvKj/4zpc8xqWyzxtuzbYc/tNkgegwJOjgVSnIUAeQGB+Uxbn8NTTfFuJaeyp1xc6kDJqqdyNwQcY8Dv8AScYuupZjWLUNinHITyP/AKWw35T0XT6UL8u0W4vpdK9bHVJS1SAlzcqFFUeJ5unvMZcdy/l5dMOW4eHnOsXBlbYkZ4lxTRJeE01j2aQjvM5ZhS3nWzd4p583Tw22jF2m8t55s8LjXt4uXHkm4pH0+TD1UYjh05kxQZh10Q4kp7F1AyWUqB4sT0E674a1K6WoU096uoJULWOVewKA4Xzw2R75HhKyn4asvurpJwhRb9QVJ5qqyc1oT4O+CfQAk+APacS4FTZUKOQCpVVFVMrycuOUoRupBAwRuMCd8cMun6eHn5JbqOP+JdFTr35jijW8uFfB7O8DoH9umRuPEEAThLdM9bGt1KOh5WU9VM9K1vB7K0zY5uRCCbCmL6v22K7OvTJABHXeWuj4TXqkFWpqW1Qua788tioRkcjjqOm3T+E68dzl1k8908lSTnZ8Z+zy+rLadv0iv9Q4W4D26N9Me05C6lkJVlZHU4ZXUqyn1B3E7sgWRS2N2xO0yBCzrD1dIGzrD1xiY0T1IjrRTUiSVdg3kcQtg3kSIIFoMw7QTSQRk1kTJLErOsxlVi+nEsa6pyxejkgaLChYdaZMVTbhYSYSMYtSBIkAjN1zDOi+z/hv6RrqVIylROos/drwR9C/IPrIR7D8LcM/RNLVRgCwLz3Y8bm3b3x8vsolij5H1g2sySfSV+t1pqpd1wXAC1q2ytc7BKlPoXZR9YWtANYNRqSjd7T6RuXl+7Zq8BizfrBAQB+0W8VGLxPKVOh0a0hawSeTYsfmdvvO3mScknzMtPWEQyGSCwfrCgzabJxOd+OuB2a3TFKrCtiHtFTOEtIHyt/Inx/LoQ8GTg+kBZt8z3pbUxDrurFWGCrKwOCCPMHqJ1nwnxcOBQ56D+yY/wDjP8vw8BnrPtN+GedTrqFBdQP0lMf3lYH94PVR19N/DfneGcG4e3D21LWdnqQlrFu3CtTerN2dYqzvzYTB6nm2I2xnLCZTTHHnlxZ7i77KF7IgKQnaPY/ZVVk4FtmMkE+CKO8zeAG25Ald8N8SGoUK7BLEwLWOAAgBJt9Byhif3TOu4FTzn9LKFTYnZ6OpgQaNJnmGQejucO3j8o+7PLjx9+/w+lyeonTOn5WPCNEahylud2Jsusxg2WN8zEeHQADwAA8BLfaCqr5R6nqfMwiz1YR4WMgz7ggynt4O1RL6a00ZJY0kdppmJ6nsz8uevcKy6PhNOJrSJaPi3eFN6ii5vk73NTf/ANpyBk/sHDDB6jeE4vwfT6leW6sMQMK47ti+zDf6dJHVaNLayjqHXyYZER0urs07LVcxsosYV06hjl67D8tVp8c/dfx6HfBNsOI+KPgW2hTbSxvpXJYYxdWvmQNmHqPwnBWT6NNk8c+0bgQ09/a1rijUZZQB3a7R86eg8R7keEVY4h+sPVAP1h65MpMIrqBG2i2oilc43gyIV5AiCCYQLw7QDSIJkgZFpgMSudL1ltp5W6RJbaauYkdcqYRZIpDV1Qhpkwrb64s9ctbKYu9MQq2rnpf2S6Dlrv1J6uyadNvBRzv+JZP9M4J6p7RwLh36NpaqMYZU5rP+655n/Akj2AlfCkP0nr7Sp4hdhqVIyp1IdlHiK6bbF/3oh+ktNMespuLDDVMeiXqD69orUj87R+E5Wlc3Wb588ER0HIlTZ8qfuL/CP0Wb48441Uyh8IStvCLq+82x3m9gS0QX6RjY9IVmzvE7TCt4m1AO2xB6g7/lPBvjnhA0mqepkzSf7Sh/vLU2cDPjggr/AJZ7bW0rPi/gFWuoKMALqwzUWE45W8VJ/VbAB+h8JSscmG3mP2ecIOpvYHvaZEHbnfFiFwVqPozIM/sqw+9PbNLT949T0HkJyn2fcJOj0gR6yLnZrbFHLZysdlUsuRsoXp4kzpV1J6kEfTEzbNjGahp+sksHTZkSStOkIhmGcfxD4k1FeoelFWzlc/OMYXqNxvjBG8t9Bx3nIVqmViQuxBXJ95yx58b2PLPa6evtcvE/r9b+PtaKdjK/iunW2p62GVbGcbH3HkfWWBHWJao90/SdKEODatnq/tDm6pnptP6zocc2PDmXlfH7YiHH+HrqtO1DYBYZRj/h2j5W/HY+hIktIeW+8DYONNafVzWUP5VpD82wHoYbDwK+plZlYFWVmVlPVWU4IPsQYVBOl+0Th/Z6rtQO7qUFnhjtF7rj8lb/ADTnEE3BphiuojZEBckRpWPINGnqg2rgijwLRt64tYsiXMwTGmxEug0cuNK01MmWllUYY4mTJAN8Rd5kyRWnwlw/t9XUpGUQ9s/lyJvg+hPKP809T1DTJkzkoDQevvK3j9LMjBdnZTyHyfGVP0bBm5kxfCNG0PXW46NWjj91lBH8YW1sYabmSiHFnMOYfWGByJkybgbDQdsyZCt4+StlvlB3XnZc7n+E1MnO11yk0crIBAwOg8BD2uAOnWbmTpHAKmwDp4xhn8ZkyMDjOOkLqXIGC6VuxOR0HLkf6YtwrUvdegQlK63RiwyOblOfHw2/58JkyeLPGdX++2uDGY+7zXvZljJvvJvHz++2p9O5OrQnAO/iIrqz3T7j+M1Mnrt3GVdcD2ndOMhGc+gGAP8A3zjAO49pkyELlftG0nPpa7cZaq7GfJLFIb/cqTz1UmTJ0w8M1spBWJMmTYAaqDambmQJa2uI3LMmSROwbzQEyZFP/9k=</t>
         </is>
       </c>
     </row>
@@ -3806,25 +3806,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TOM KOHLER-CADMORE</t>
+          <t>MOHAMMAD NABI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>t20blast2023_133</t>
+          <t>t20blast2021_122</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E27" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>100</v>
+        <v>114.3</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -3833,97 +3833,97 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4</v>
+      </c>
+      <c r="N27" t="n">
+        <v>23</v>
+      </c>
+      <c r="O27" t="n">
         <v>2</v>
       </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" t="n">
-        <v>57.9</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U27" t="n">
         <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>41.7</v>
       </c>
       <c r="W27" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="X27" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH27" t="n">
         <v>20</v>
       </c>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>24</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>31</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>18</v>
-      </c>
-      <c r="AE27" t="n">
-        <v>22</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH27" t="n">
-        <v>0</v>
-      </c>
       <c r="AI27" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AJ27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL27" t="inlineStr">
         <is>
-          <t>Batter</t>
+          <t>All-Rounder</t>
         </is>
       </c>
       <c r="AM27" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTEhMVFRUXGBgYGBcXFRcXGBcXFRgXFhYVGBcYHSggGBolHRUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGy0lICUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIARMAtwMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAFBgMEAAEHAgj/xABEEAACAAQEAwYCCAMGBQUBAAABAgADBBEFEiExBkFREyJhcYGRMqEUQlJiscHR8AcVIzNygpKy8SRTg8LhQ2NzotIW/8QAGgEAAgMBAQAAAAAAAAAAAAAAAwQBAgUABv/EADcRAAEDAgQCCAUDBAMBAAAAAAEAAhEDIQQSMUFRYQUTInGBkaHwFDKxwdFCUvEjYqLhY3OSM//aAAwDAQACEQMRAD8AbatzrALhSjtUzG6kQU4nruwyj7Rt7xHhDhO/zbWNB12iFk0xleZTchj05gQuK+EVMR4lSUt2gWQpnOIS/wAaU2aeh6RHTTyNIKOgqCJh9IsS8MUQZnZmUtUdmiNlTnVZK7QrY/IMy1+sNmKqJcst0irw/h4qkExtByiXQGFS0l1QHgrGEpllqPCDkqZ3Ynk4UALRJNpMoJ6RU1GlQ2i5plLeNgtLYRJwPTZJI/fOKTYms13lj6psYMYZPWWoWJqA2XUCACUwJHioOh8oHHFwIoz+JpZbID3jAcplHzBJFTS5aqY/UwUoqog7QV/lmZix5xOmGAcoOwgNgpZ935moTWVROwhfkUZaqVjBviCtEkqtrkkAesGcHwMG0xtzEucA0KWAucSeBVinHKLRWwi4tDFXFpgkyy52EUzgrhSICUuL6QzAo8R+MO2CpllKPCFCTXCos3L9IZabEwoAtFXtJKJRcA1HlMbgOcaUbxkC6s8EbOOKWf4gSizy7cjeK1NPIsDF3F6jt3VgLgR7SnHSGKdhcJeo4ONjor2GlZrqhuLg/IQQxHg2mnABzN81cD8oFU05ZUyWx07wH+Y5fzh4AhPEOc11iQCE/hg17JIBMpJl0nYsZV7hTYHqOR9rQSVhli7i9JdwwG418x/4tFRpOUXMMh4c0HdJGkWPIGiXeJSWlMBBLgiTkpkB6CBldiEtyZYOuxhgwmaiSwt4mrNrKtDdGUiCuPcbyjytcnWKFdjEoAqCLmAgFMkhc7w4FJ009WMM1HUDnFenobszEbm8XFo7QwPlgpUkh8g2VSuqukKmGUzGsLHa0MeJ1UuWQG3O0WMKwwlu0IsDEusB3qGjNm7kZpmi3NtaIqeRfaN1swIt20EVJBNlwaWgyk7iemLzpX98Q/0IsijwhVExJsxSNgbw0yp6ADWKP1RaXyBXVWF3jYE07AdDBo1yAamAmOVqTEKobxQBEJCScELIgBhqoqlcuu8VabDxYaRbWmAEMmC0BLgkOLpVGtqN7RuPMyajMVXVukZE5gFSCUTwwAIvlBMqLXilKo2UC8WXAta8VdB0UMkahLvFzHsSV3AuPMaiOjYfPDykf7Shv8wB/OOfY+yS5LM97aCwBZiWIVVVRuSSABDHwXjEubJWUGXtZaKZiK2bs7khVZgLZtLEdQbXtCmL1EJ/o+crp3R+o1AgfX/2beUEZo0MDaqxU68opRPZRa9nLkVHPEudNZ/tGD+E4tKmnKG184FY3RjM9xuTALB8O/4kFNBzgoxPaFP1VDg+wa3on+qnhdLws4bNP0pmYnKBDFNwWY2ogJWyuxZgwsTDLnNaBdJMpvqFwA2smKmx2UXyXF4Nva145BRzC9Qi6fFeOqZLINeUBo1DUEkRdFxVAUCGi5hKPEsvNVStNMwvDnV16rJyoLm2whWqv6k8Lb1jeO4iachZa5j4naB1Kkk8BumaFHK1o1cbwmPAJ7p/aCwO1+V41xxMvTMV6RWwCv8ApVMWYZSLi3iIqT6gzJTSzra49ooy1gr1BnBJF9whOBzbSxeD8rVb3gLLw5wBYRdlUzAWjQIBAustrocZCixeeezax1iLg0ky7tvc7+cSzcLmEHTSCGD4Y6pa1oqSAYXEOLSY3RmnlgxDXEAEeESyZDKNYr1cveIHzKHfJpdLXBUi9TOJHPS/lGQa4bpwrudrn8o3ASblNsbDQAp+PcTNPILruIWMCxt5yBnhh/iFTdpIKjW8L+G4QZcsAaRek4aFCrM/UNUUq8MarRZKMVLuoLDUoguXYeOUMB4kQ8YXhdPRyexp0SWoAFgLsx2DO27N4mFvhWWUmE/cIHndfyvGPJmTK8y5rlUCB5aLezDTvFuua4y8wL9bqYp0PT+EEsCbM2ZDbmpt6iFGVjQefOp7i8oJnAGi51DLZup7wI+7DlKW1o59RYQlL2neLO8x3diTdmZifkLD/eB0TuiV4iONlQ4jUO1hvA3hzC2Ewk8jDHT4eXfORHuewlNeODe3n3XGr/T6vZMNK+VdYSeL3WY9lGoixxDxQEl2Gmmp6DmY5hiHGM3MwlAD7zXJPkOUc92bsnxVqTAwZwb7Js4ewcdv2jHUQ91knu3vHDqHiWqVs5mA6/CQBfyI1EdOpeIu1lhSCDYHX7wBEXoOIhqriGteC9ex8ekDcfoprtdVYwcwGlzzBzjoEmgQLbKIJWEEtVMO6zX7rkfCkyagdCCoud/GGbCZYN4n4mpQhuoteKVA+Ub6xeg0k9wQcZUABncos62hLxXFnWrlyxszQ0s5MLk/C81WjnkYZf2WrPp9p49+7rotEoyjTlFvsgBFOl2EWi2m8LFOtQTiut7GQzjkIT8IxtpyBmhq4up88hl6gwmYZhTIgAEGpETBS9dtsw1TPRqSLg2jIp0kpwNLxkS4GbFc1zYuExz6YkXbWFri6e0uVdNDDTNdssLHFEgvLtECQCVU3cB3I9wxLvIUtuR+IjK2VOkmQ65ZoV3Vy1lZZbqxXKSbk51lggb9BbS1gMvLKUeEUOOppFOADYlr3BsRYdfWE8R8hO60sL/9A3aVbbH3H1Vt6/rCXPx9TWzVmnKoYEC+neAb84tYM5ain37zqswgk3PwEra/O4PtHGqmtd2LMzMTzPO2g+UZuBrmpUqMP6YBnebiI+60MXTaGgAXXcZnF1MvdDr7wLxPGJcxe6wvHM8AkB5nfBt5R74hJlTAUuBD/WAOypT4clmeUw4tIZpM03+qT5W1/KEmnpwWF9PGC9NjT20BI8rwfw7D5bypbZcpsMoygbHW5A1v46xXEvDAHBEwlPPLT3oxg8qRJVWlyBmtq7AX9zt6RBxFUZwZiMM62ViBoOai/M2PsR4R5rKZJotMZrA/ADYN+sVOJcTVadJS6HMfqkaAKBvva1vaA4Z5zgpvGUx1JEWTt/D+yyw8xtTDuuMyNu0W/mI+Y5uNz8uQO4HQXEFaulZJCzLtmPO5v7w098G+6RYyQY2XbuIirqSpBjm0qbME+xfQHaAfC3Ek3tBLdyykc4M1FKWqMwvaD0nFroG6VxDGvZJGl04SZlwBeJXkFdYU63GBJNmNoJUWL9sl1a8NFt7FINPZkgojWY40rnBSixBnUEmEjH6dnAENeEU5WWoikDMQpLjkBHNGGQuNdRFKtAVDYbQRksbQLxVSUbyiW6qrzaVT4UqGmM+bYGwjI1wDRFO0JJ1YxkAmblOQG2CaMXISUzDkISsHr2mgl+phyxwEyXHgY53gsplU77n8YtTM2QqoHzcE5SatrWWBnEU4tLIPL84ipahl2iCsd2vcXuDE1aJcxzQNlehiGsqMcTvdeuCG701DsUv7G3/dGmwGjlpmcKFXc2JsBuTYaAdeUD+F8QyVSyyLFrr5d0kD3Ag1VV4WY6MOfyYX/Ax5vCYh2GxtQfuaw/8Aklv3hbmKwrMSxpO0xHP+FclYDIAuqrbrcWgJxjwa09CZQQFQTqdWt9VQoNyY9cJ4iPo6KfqZpdvCW7IvyUQz01RoRy09jEYnpuuyo6nlbIJE32Peqs6JpgBwc6CAYt+EtcK4ZTSFSRNQmcTlI7NsubKX1mWy7A84vY7hliWUdxhoQLBei+EHptOr91gCLgi4vZlNwR4gxqfSGYRma6D6gFrt9pup8PG8KV+lnVi0kabceJHDlOnEzZnD4VtGYOvFcoqZ/ZFhMU7EnmCPPaCE3B17Wm7VQFmyyZY1JOuYgi1g1mU28eohrquG5HezyzMzG6yyd+Zzb5UB/Zgo2ELOSUJ6gvKIKOpKkMNmGW2U6C4209AxQ6RZSqA6iDPiLeW/pKtiqPXU8s7j0ShUYZSZb2XXUag38dI3Lopc1cujAcv/ABBmv4VCrVNKbMJitMWUVBKzlOZTLPQ6qRbmNdIo1eMLTinvR6vKExmteWrEXZRK0Oa4GhNrsL841W4uliDma4RtNjMA8uY8JFiEvSw7GUsjWPdU5EEETrESbXj13SNi2GiTWS8i90mOj01Clg1tbQuVCGe6vl7ochWsbMo0Djzhiqa1ZUu7aWEaGHfLXOdFj9gsXF0ndaymwG405yQl3ieklPe42gBg1HNp1aYvwkkgdIlxnFxMBK7xWkYq7SuyI16wjQxDRVL3HuW1iei678OGsbpr3brp/CtAJslXmC5IvDOlGo5QK4Vl5ZCA9B+EHVaHS4m6xGtGirTpICnyhFGLtMnPLPwg2h9qjdT5RytJTLUTT4xemTMIdVgieCbqOoyaKIyAtPVsDoIyCupX0Q21gRqicjiQVJKKNOcT0+HqBa0K/BNK2dr9Y6BJpgut7wIOaAFdzXucQNAh4pV6QtY/ifZTUlhb5jb3hwq3F9oSMWpzMrZWmgJMXmGyh6uDZTdh+DS1Ha5e9lvoLnQX5amBtbgCVymdIZpUy4GaZLfK4AH1Wyn/ABD58m2mWygeETWjOq4VlSsKrtgRG179/ddaNKu6mwtbxmVzFeE6iiQs0xJq5izFbqQWN7hTyHn1hhoJ11Vj+wdD+R9IIcZa0zgdDAjBV/4eTm3ya/MRh9NYRrAKzdzB+v2Wx0fi3Vf6b9hY8lfNJoVDMttbXuCDuLH12Ii5ThhoLFbeN/W/7/OBCbAjUrp5j/a0RV+ISpMvPNJC3AFlZmJY2AAUXPpGWx9arFIS6dBrflxO19Rqmn02M7enE+9puiMgaknUn8OQHh++cBJmL1In6S1aTnC3DW7pNi7XGhBN/TlqTaoMWkzGyy5mZgubKc4bLcDNZwDa5EW53ZnVlUnqQCfeD0njDuIrUzcbjY7iY12KGQHiWnyUtbUZfn+EJn8SKJ51MhlMVdHBuPsN3XF+WuU/4YM4lXXdVHM6+Vj+kTVq3QrpZhlJJsBdTr55so9YXwr3trtczXb1+vBFe0NZJXMuG5FTSzM6/wBVtwWYmy/WJQnKx6eJi3xVXT50kM6BLue6Ps/VJgytB2j5cxU23G4PL/aFytrZqO8mcQWHc208/XQx6DDV6lWlnOhkKpFOliBa4g/ZLoNhDFwnQiYS525QBnLyhk4Ln9wrzEM4MMNTtp7ps1xQy0d9e5dHosSyKFA2iWdxGJYzNoIX6bEQAQRAHiGc03uqDbnaNlzQ0EkaLwbCXOa1puU7UnGUmeSksgmNLQKWLdY53h+EzEnI0lT96OlUE+1swgdBwqMzhWxbHUamQm3FaWhUcoyJ6qqudBGQcApVzgDAUZwjsJbFd4W8Nxab26h2OpIsY6RW0uZCIA0fCyFhMYd5TcRl1SS5sLew5DKbs2681U/XURRSWnaBzyhzahQrYiFPFgqsQsONeHdkrPqUchzhElxmWNzaLCYtLYaGEHFi9u7YwR4flvluwsYnKM0IZc4MzJhxZhNQqOcCkGQCX9nTyuAfz+cFqeX1hSxGs7Kvmy3+F0luh/urlZfTRvC5MZnTGH63Dw3UGY4wDPoSfBanQzz1/a0IPhcR628UZWqygmxOmw3JGq2/CBOIYrJnIEmZ5VmR2OW4Q6lQQRdgdFIsDrp1i5MPP3/WLEmoVxZgCdjcA+e/Ww9vCPMYSqykZc0k6ggwR5gg+9YXosRhnPFj32VHCMPly57TRPRsyFAmXKR/ULsSSxvdrwUmpmHdPkb+36RE0iUb3RdbX0tmtoL23IsNY9K6qLLsL6XvubneJxdUVznJM2FwNPDfwug0aJp2At4/dLeO4gtPMkuVdgSwyoMxXYnS9zqPmYk//q5rD+hSTT4zbSx5gXJPuI98Ryc6lwRaXlcknmxCgDzF/bxiPDrsdemkO4LD0ixr6jJ11JjU/tINu+OMrqxcRAd6CR5+CBYfxPM7TvgTDsANLAkmwPPfnc+MQcb4e6TJU97AzAQQDcgixFx5EiNSZSUtS/aHRO8v906gny28xFHifG1qNTdCPhDAjT16w31tV1TJHZGp79gj4x9AiKIAkXPGPxuswyhE/S9mA9x1ghh+H/R23veF7h2vKzRbXQ+ogjWYyWYd0iHqdMOEDVZ3x1Sm4EyWgaeibzUSgAWNob8BopRlgkA3/OOaJKeYq929yPxjp9KnZykAHKHq9TshixsPTHWOqc0SlU0pPhUaxVn0mpMSUqE6mJKltD5QKi4g2RMWwOZdL9VXSlbKSLxkJeLSphqWIXTXnGQ8KjVkuw7p/wBLtuaIp3dF4DysVTm0WTjEoixYRnwVrAwpvp6kXvCnjLyyxJa0GJtVK1ykQu4nTh76wSl2TKHWGYQF4oqZJpsjE28TDDT4XYWuYHYA8uVuQDDAmIyz9YQTPfMgmnbKo5dKRHOf4kJaokHc3t5ggXHra3rHTvp8v7QhK4yw559RImU6iYVJuLiw0N2N9BbukddRpAqtUNh7jYSf8XD1JF9Bum8BTAeQbSI/ya76A23VHAK7MvZubspZbnduzbIb+Nijf9SLcxCp09PHw8/31hbrMFrZLdoZDEXDvkIa5ACPlCsWGZDm20ZRBSRi4KkOyZ0JDd4C4U6TADyIAMecxdBjv6tMgg6xGvcLxtz2tC9Xhnz2fcIok0sLqdRy6/vmI1n/AH+IPjC5hPESzAzDRwxFjoGUnuHwa1vUGLhxgMSVF7fEB8S+a7+sKVsLUpOLHiCEem0VWh9O4Oihx7CzPeUqsqWJ1PQlQLC+v+0XMMm2XXcaHnqNxpC1xbOzS0Ib6/LYizX1GvLYxa4VrSyFSdR+HL9+EaeGbGHaeBISmJa6YJsNBwReoppU43mGx2F+YH+8GcLpECEHvC3MA/lFCjow7jNoF1/fyhskSpdtxGnREsledxJipCRaiiSX2hRVBN/hVR+AhPVGmuVC2tubR1+cia7GF3FKVFV3AAhhmHFR99Eu7FuosMaofgMgC15l7HbSHeZXJlBLaARynhmvyzyu4YmOi1FDmW1wLxerTDTZWw9TM4Z99StLxKitbOPcQWFYji+bfxhVlcNDNcsDBKThhDCzaCBsblMo2Kqsf2WDRRVOHlnJB/CNwxyJK7XEZBhlG6ziXHZInZiNhBA7+Zp1j1/Mk6wzPNMwiAj0W8YGHE06xpMTTrHLpRMCN+vzgd/Mk+0I3/MU+1HLlfPmfeGfhGisrTT9burc8ge8fcAf4TCV/ME+0I6PhU1BIlWYWKJY7AlgDp53MY3TVY08PkH6jHhv52HdKYw7ZdPBWCRsdP384q1mFy5oKzEVwdwwuInNVLa4DqxFrqCGIuLjQa7EGNyZvI/P8DHkjTcAHOBE6H8LRa8XDTfcICODKNTmSSqHY5LLcdNBrFTFOBqeYAQpR1+B1ZgUPUW0htmOIpVVay6Bbf3vysdYt19RhzB5EbyUQFxbl2O2yQeJ+G54kTGZZThFLl1JRjk3OSxDHLm5iEzhuuyT16N3ffb5/jHaXftL5tiLEeB0Ijg0qR2U8o+vZzCumhYy2IsOlyPnG90PU6+lUpO2v4H+ApxOJeCC73C6nMIK79DEaN4n3MQYNjVXVFRR4WFp8yiZNntdjLNswUsVAYg6WzQXxnh2dTSu1exX6wB1QXsCeR5Xttf1jZwhhmV0T3zqsjEOa58hDnmGxIJ2hCxTiKdd5d9L2hsmVq5W1G0c8rR32PiYfY/LskatMPddFuH8KnTSHRTYHeGidPmKLF2BHjBX+G9QoozmIvrC/jVWM7WPOKUnZnEEIhEBTy62Z/zG94uSqt/tt7wqy6zWL0muHWGnMCG1yaZdY/2z7xkCKesHWNQuWCUcaKscNTpGHDU6QbMiPPYRg5yqwghw1ekZ/LV6QbMiNCn8InOV0IEcMWM/lqw/UnCRdQSbXgbjOBGT4gxY5wJKiEpfy5fGOp4Jh0t6OnV1JCoCO8V+qybqQfhYj1hE7GOicMveml+AI9mIjP6Qe7I0g3B+xTWFEuM8FqXhUmWweXJAYCwK6G1iLbi47x09eQitV1WU3KuB94A+oKk3Hhe/MbQaeA2PSA0tgTbQkHXQgXBFuYjGqEv+Yk8zf6rUpQCqFXi4NlHeueR18SI9S52Ya39f3pCxw4rOA8zU2ufM+Hv8oYbGFajcrsvBNuZlMKedUWG8cR4hlTBVTcwsDMZwTpYOxYEMdOe/hHUMaq8ilmJsPzNoQOJqlWytmOcEhtL3B+rY8gR849B0AMrnO4wPus/HCWiNr/ZdkmTJMkjKwMuYgScg5y7WE5LblM2pGw8hClg+ITcPqzQVLK8hrLnPwzJE3RZpGoYkGxbTUG9wI5xRY1Udml20kNnlG9ipJAy5uakWFufjtDdjuIS6nC0n6ZqecJa9ck4HPII8CAR0A8Y3Gtg5Tv7CyybKLEMG7Ka8sse4zLfrlNgfUa+sUjhCGDM2cZglsSWbs5YZjuxVAuY+JAERhYCXHilnOIMKnIpCgsjEA8hEb4YDuTBG0bKxGd3FR1iE/wApXqY2MKHWCeWN2iesdxUZ0MGG/eMbgjljcd1j+JXdYm6upMrkRWMmD2LS/wCoYomXCjrEpyENMmL+C0GeYOgjZlQy8P0eVbkamLUhmcohE1AUARQx+i7SWY1jExgVyg7wRljMmvSHJBkKFzJpFoYeHa9VyyWNiQ7LpvkZc2v/AFFiHFaPLMPQxiYKzGTM7UyyjM4AXMWVgFKtf4QRGTizTawiq6Be/ODHPWPCUbDtIfYe5CYDlO2vkYC4/cSpmpPcfQ9SptHqswlW10Z72BOZB1uMp39R5iBlVKnIrIXDyipvcNmXUWAZmNwdecYLXtdcHRbLGidfNU8Al5UEGGItAjDKhctj3bddj6xarDZSQYG4XJKNUu5If8SMWKskqW9r3LEHUdB4c4RR9k3NviUggC2gG97wwzZLzq8ojBWBBLEXsRdxZfrHS4HhDfhWGUIN+yNRMLAu005i5J7zBR3SdSdfWPUUKzMJRayJJE257kmw/AWTUovrvJGgt5fVIOAVI7cB1Z0N1ZE0NmBA8Nzz6Q04PTSamneU7AtLaSyhWsVAUrbu9yZrmudT32N+Z6gJMop2eRQhFsqjKLeQ2gJjVFT0tJM7CTLXVNALXu6qSSpBJsx1vFGdIfEPawNgkgAzxI1+kITsPkaTPH6IKKNrXCHKNL2NvAXjDRPbNka3XKba6jW0D573k9u6W1AEtXbs7ZiPgLEa5mJjKph2QnqrSwzL/TSYyrlDNZe7bTUn1jT+GMx/dl21WcabeKu9lHky4s0xLqGKZCb925NtTbViSevrHtpcLulri07IZYh/ZxmSLplx4MuOzKmUqpljIs9nG47MoylP06V2kw25mJ5+DFVveC8jCQpuCYuzZNxaIbSmS7VapHBJtNTZnAhrlSwqgRHS4WEN94szpBYW2i9FuQXUOF7KEsvhHtCDtFJsEP2zHujw1kN8xMXD3HZdk5qvi9DnKnx+XOPWT9+cXKwHI2l7W52vqOcC5lSR/wCm3pc/hHnemiOtaOX3/wBJnDtMFbmr/wBx+VoA4xKBA5DQHpZQdf30gjOrP/bmDyVv/wAwHrP6rqCJoW92vpcL9WxGx0G3PeMWmO3rE/jn5haFIQRKBHDGnHO7tKk/USWAZjgbuxIIUHkAL25i9o1OwCQvwiep7ov28w7gljZmI28IZiAb6i9vmeURTpVydvi69Jcd8U+bWA4e7nif4RDzSFgPCi/SZ01mZlsuRjbMJjWZje1iVsNQLa7QWWuWQ5RwFmb6C2YH6y+B6ctob8LwduxMzSxY/Kwv8vlFbGeCTWyNlDAEy2OhDctehj1HVnFU2GpOggjuG2ngsxr+qquANpulmp4mCC5Nh4wJqeJRUy5qD6olkE/W/qLew6DT3hIxKkeTMaVOUq6khlbdSOX/AJG8SYQSJngQfXY/iBD+B6Oo0qjXZpMiOVwr4gOLCE74if8AgJZ0N2QaG+2489DG8RFqCUeuT8GMWMRoHGD0842ytNsOvxTbf6Y3jVAyYVSTTbK7rbrqs1vyjTZ8zf8AtKzC36ItTJdeW7bbfEdo9GVBThzA5sykkTFAs8tGGutmFxF2Zw/NG4EZFScx7z9UQUi7RLhkx5aTDE2Av+xETYE8UlW+Efw9R+UumVGQwnAJnh841HZlX4Spw+n5XR7iMBEK30v75/zGMFZ98+8d8b/b78kTq+aas4jRmiFf6Z98+8b+mff+cT8aeC7qwmczREZeFr6b9/5xv6d9/wCcd8byU5AiOJPaXMNg3w6E2vr15QtTK43/ALFtwP7QfW/x8ucE1mhud/WI3UaaDf8AAR5zpmvmrtMfp+5TuGgNPegr11//AEJv1tpg+rufj2iWna8s91lN72LAuLcwbnTXaLM2ULbD4enVoHYjTXs17a2IvYgKQx9baesI4ZxOaB+kz6JogEhYJ7XtmRrcmFm9j+seTOf/AJQ5650trpf44DThPAAzBxYtZ1DWH1QLfpEMtp+ZQZFOtyBfswbX3+qNrxfqTsR5kfcK5hdHoCfoN7jXNa2wG1h12384u8PYiHkJcZWUWIPUaE+UAZdWAgTPcAW1tAfinG/o9JMMtrM3cW3VtCfQXMeopVixjWAXAA9IWSKfW1IH6jbxXJOMqkT66pnA3DTHseoBsPkBFXh6Rd3PSWx26Ff1jw6wXwGn/pT5n91B1+F2b8Fh6g8hze8LVx9BtOi7yTvxTVIuDUMgG7CauYdP6c9z8yIzjGqX+TYfKBuw7MkdLSHvf1aBnFM0NRUYGhzZiL3t/SmaX/xR64nnoaKkA5KpI527MfrDlGpJZze70A/CwCBfuC65ws6SqSmlZwSkqWnicqgbctoJz5qkgQiYbiAEqXrY5F5i+w5jSLQxaxvnv5xmOxWtkZrW6ynUlY1mWE7+eH7QjP56eoiPieStlb+5N/d8IyE0474iNxPxPJdlZ+5KxqT1PvGhUnqYFCfruR6RNYnW8LW4JeUQM7xPvGzOPU+8CZtzpcxIoIETbgulEu1PUxvOep94Flj1jfamOtwXSmXhuZecRcmyMfmB+cML/r+EK3Bzlpzf/Gf9Sw2NKPyP6R5vpVpNew2C0sKewqszb/Cu2+8Da5tLDTkOerHXXnoIIVJsL+CwJnGxXwu3toPn+MJ0ZAKcCiO58wPRYiqTp++ZvHuWPw+bQMxqpKsFHn+Q/CHcHTzV2jx8roeJflpk+7r2B4mF/iqZoq3vqT7C35xaM5zqNoD4/OzFVO9rx6S2yB0O3NjGcpPoUvzBeGKkk9nSKebl2PlYgfICAWXaGGrkkS1X6oQga+A2+cN4SDXYDxWh08S2m1vE/QLxXL/w1Kb3umb3lj9YzGTamka69nf/AOqfrG8duCByCzcvSwygWt4ERPiaqXkqfhzZdhbKXljba1vSHsPBFI/3PPovMzqjNBL/AKcvX6i/6RE5QdYFJPawy7WESdo3WMY5VaUQEvxj12XjAvtm5NG+0f7UR2VMokZQ+1GQHzN1jI7srpRMspOxjTuI2ZerBTpc+g5XjZl+UTmUQoxaMWeOt/aPJldCo+calSQddP8AKBHZlC9LUA8tOto32o6fKMyEfVuOukeyh6aecdnXI3wc6tMcW0yajzIhpm0qWPxDTkx/OFzhCSS0wKO8VFh4X18gNPeGqZhzIpYuDYXItbz3jIxeDr16rnsZIAF7cNBOp7vObJ+hUaxgBMIPXg5bAfY9ufyvAuYjHNlAPLex7vSCtQwIurBhpsfun3ihKU27qu3UhSRffcRkU2vIytbPcJ+ifBAuVXYa6qy69LiwHUQtzJmeZMJOgfKB/dAU/MEwzzQSbemvUm36waxDhaTOU5Aobk1v9Vt42OhqWdz3DUADv39IS2NeAzLx+yQO1AFrfKF3HwCy6W0GvvDhi2CNJIVypv8AZN/e8T0OA4fMQNPJL7EMbC19ANI2QMxI0hC6MxTMLX6yoCRBFhOq5tTSC7BUzOdgtrk+0MeOUcyTJQTJZUlSb6HLa255H9Y6bgS0snuU6SgeeW2Y+pNzC5/Fy3YywlgzBxa9r6ywLj1hzDU2hwfP4Rukuk/iwGBkAHx0jwEbJHx2ddZZ1/s5hued+y1ibHaggy2zZStjm5ghgc1rW3F9om44wX6N2Cib2meU1tLZdZQsf3ygdxNLJyINyABc9TaGaJymkD/yH0KyYlMKkAAWEemnqOURJKOuYactY1kA1H4xj9YFynaevhGmcbgD3iFiLcz7R5CBrEA+4jusC5TiYvO143Edj0PpaMjs4XK4oPJY9kN9mLbT2vfMb26iPS1L/a36gQbKESEOMs8lHzj2Jdthr66QQSpcbH1sD+UaasmC3h4DT0jso4roQ+52y/OPe52GnQ/pBBMQdRa418N7HQxj1jkWFhr0HTUxOUcffmuhCKviCdTJaVKZs5XOy3Zso2UW21Prf294N/El7GVPTJmzKGOgU20LXA0JO4t66wTFWb6Knqu/nHlpxNwVXwsLWHnr4+8S0Nac2/vbRdAULlESX2ThgVt3TpcW1/AekNUnFpNFJyzH72Zie9cm5J8z0HkIVxO6Afv9mPQy2+EW6A216mJGVpc5ognePfqpJJsSiFbj9POzNJmKJoAvLK3zjXVQQO9bXnosD0xedayzGHkqj2sIxpi/YufOPWZNwp9TFGMDSSDc6niePv6qXHNAOyFGVmcuWcs2hJJP4nSPRQfaMETOQn4Tb3+UelErXum2u3zt4x2UbKuVCOwF7hiD1tqPXlA/F+0mTZKNNZ1JuQzsNFZGYKSdDZTsRcgW1tDMxlDQ39dfyililBLmqoVmlurXWYgGYCx010tt7QaiQx8k2/0ohLmLUymcmZ2sq53dmdiJaMM1s1zfYAbR4WYtXPkvLN0Bsw0Vls19rm+hvodgeloYMXwlJ5v2rIcmTYEWLBiTffYDyijhvDCyTLtP1DZyRLUXsrLlIJ2szD1MGY9ga2TcA+syugzZXRfnl9z+kbI/u+8Ehk6+/wCsSpTobj9P3+xCYpjiuyITYfd943YeHuIKvTp1131A/AAX9I19FBv+nK50icnNTlKFAeA/zCNwR+hr9oHoQB8+Ubjur7l2UoVMc3GsTkxqMigVCqNTUsHUX0LeEEVb8oyMiVwXsb+kBpc9u1PePvG4yJUImznrGwYyMiVy3m094xWMZGRwUheTp84ztDbeNRkVULwZp6xHMnMLa84yMjlJUhc33/ekYJrXtf8AesZGRKhVnmsCNYkmT2y3v+9YyMjgoXpphNtdx+UYXPWMjIlWWpc09ecWRMNt+cZGRK4Ly8ZGRkQolf/Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhMTExIWFhUXFRgZGBgXGBgaFxoYFh0XGBgYGhcYHSggHRolHhYVIjEhJSkrLi4uFyAzODMtNygtLisBCgoKDg0OGxAQGi0iHyUtLSstLTIuLS0tLy0tLi8tLS4rLS0vLS0zLS0tLS0tLS0tLS0tLS0tMC0tLS8tLS0tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAUDBgcCAQj/xABKEAABAwIDBAYFCQUGBQUBAAABAAIDBBESITEFQVGBBhMiYXGRBzKhscEUIzNCUmJy0fBzgpKisjVTwtLh8RUWNEOjF3SDs7QI/8QAGgEBAAIDAQAAAAAAAAAAAAAAAAIFAQMEBv/EADURAAIBAgMFBAkEAwEAAAAAAAABAgMRBCExBRJBUXETMoGxFCIzNGGRocHwUnLR4SOCwjX/2gAMAwEAAhEDEQA/AO4oiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiKs6Q7egooXTTvDWjQfWcfstG8oCwlla0FziGgZkk2AHeSufdKPS7R0xLIQamQfYsIwe+Q68gVyHpz05n2hI7E4sgB+bhByFtC+3rOPfkNy1gMyUXImom67Y9K+05ycMrYG7hE3MDvc+5J78lrj+kla43NbUk8euk/NQRGPivYiBBsMx8FG5mxsuzPSHtSHNtU944SgPHmRf2rcdi+m2bIVNIx33oiW/wAryR7Vykl2KwvawHMrPLTvtplw+Kb1uJncb4H6L6Oekmhq3CNr3RSHIMlGG54BwJaT3XutwX466wk207l0PoL6T56XDHUOM0Ayz9dg+67eBwPJSUiLifoJFC2RtWGpjbLBI2Rh3tOh3gjcRwKmqRAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiApul3SGOgpZKmTPDk1uhe85NaPE+y6/M/S7pRPXS9bO65+oxt8DBwaPjqVu3p+6QdZVRUbT2YQHv/AGkgy8mH+dcvhiL3BvH3KMmTir5Ik7K2c6Y30aN/Eq9/5eJHZKuNk0GFjW2yCvqel0VbPESbyLWnhoqOZpB6OSjMNv3r3B0clLvVsfZkukQ0uinx04GgCx6RIz6PA03Z/RK1nEDwVgOjzRwO63v/AF3LZHxLLFSXWp1JM3KnFGibQ6IMe02NnbrDJaDXQSQyljxY+zLXz1XeX0llo/pD2Nia2RozGveNxW+hWalZ6GivQUo3WprfQbpfJQVTJA4mF5DZWXyLSRdwH2m6jmF+n4pA4BzTcEAg8QcwV+PXR5ab1+h/QrtV02zWNe4udC90VzrhHaYOTXAclYxKqSN9REUiAREQBERAEREAREQBERAEREAREQBERAfk/prWdftKrl4zOA8I+z/hWLo7D89nu+Kr53fOSHfjeSfFxv7FcdGT88e8DzGvtWit3GdOH9oje6NiuaOEb1U0CsWAlVZcFtERuWUlQ6aBxU405ASwPLXi6m07xwUWKnJU6KmNkSZhtHyTNVG3adroZLj6pVxayhVseJpCkYOITR2xi1+1YZ/ruXVP/wCfnnq61u7rIzzLSD/SFz7aNHhqC05DFrw1vlyXQfQIzCK4fei14WfZWsHdIpqqs2daREWw0hERAEREAREQBERAEREAREQBERAERCUB+QNpU5imljcDibK9pHgSFb9E6c4y/cG25mykekxkf/Eql8bw9j3B4Lcxm0Yhf8QIWfovlCSBvK5a8vUyOzDR9fPgX5r2RAYjmdANVlj6UwsydkoAbFE3HKwOcdctbqu2nXQkXNG0tIabtjF+27C03JBzOQyXPCCfC52VJtZ3sdG2N0hp5QMEjCeFxfyWxNAIuuGGFsT2EMIxZgEFpAubZXtu5Lo3R3abrWcT4fBRqJRZKG9JG0TTsZm4gLX670i0kZwtxudf7JA8zqrLa0ceAvcL2ByXOaxktnziNrAHDK4jtivbE853NvcNSs02uRicW1ds2yLpVLNmyBwbxLTfx8FaR1JcASMJPkfA8e5av0W2jUTQGUhzQ1rHYmyCS7ZC4NJjdnqx1wHYtMlt9KTLHnbFxGl+aVFbJoU3dXTOedNqbBMyQfWyPeQfyJ8luvoPpQ2KqdncyMaTxwtOXLEta9IjbRsdweAeenuV36OpqimibdwMUsjSG2F+1YXB1zAut9GqowVzmr0ZTm93lc6uiBF2FeEREAREQBERAEREAREQBERAEREAVf0gpnSU00bCQ5zCARr+tysEWGroynZ3PzVtjZIfTF41iZfvyyd4jJOih+Zb3k+9bd0qohC+qitbE51uFngH/EVp3RR/zbBwJB81Wu+44vgy5ydRSXFGwT0vWXB8lG2ts6OVrMYeXMFgd4AzAvvt3q8p4+GqyvgzzWuMmjY4p6mrR0kr3Ak2a1oYB90aDLRbJsGPCbdy81AsFL2LHdxdbgFibb1JQSRfV0ONmXBa2aGYFwe5zmuFnAm9wNMjlzW1ROtkVIfHuOqzG/Aw7aMptnUcccXVsitnfPjpfxU+M4QszKfMrM6DLNHdkbpGldN4MVNN3NxD903+C2bYlJZlEzIgtiz/AAtuT7VQdOJMFPIbatt5n8lfdAXPc2Brwew2wuLXDGYb87hTgr2XxIVHa8lwRvyIitClCIiAIiIAiIgCIiAIiIAiIgCIiAIiIDQPSZsvFgktk7sOtqCLlp8sQ8lyrZNK6KWRjrevcWN8jn8V33pXQmame1ou4dpo72/6XXEdrMwTNOYJFyDkd408lw14tTfxLLDzvBc0bBSFWvyfs33qioZ9FsIqGtjLu5cp23NeqY3BznOzA3KX0d2s4NLZGYLu7OYN+Y9yp9oVbpCQ0ZXWahp3AAggkHxI77KdiO83ojcpa9xkDHQPDSBhlGEsvwIBuDyUyWQgjgQPNU1EZDECb3F/91PgrsQwvHNZa5C9tS2gzSUrDTS2XyonssLQg9TXOkVG2oe2F5OEuBNtbDctx6PUwbJlewjsN/Deta2dTumrGAWsAXG+gAyv49pq36hohGLDM7yttCm3JPgjRiKqUXHiyUiIrArAiIgCIiAIiIAiIgCIiAIiIAiIgCIiALn3pgoWmCGa3aZJhvvwvGh5tC6CtW9JdLj2fNxZheP3XC/sJUKivFmyk7TRyammsAtikOOEW5rUIJLhbDTVnzVlWNFtF5FHtOYiRjQOwTYkH1e8jerqjpqQ59dUMLQO1hDg453IaBcDTVV74cWY1UulqrNDXRaZXtxWxSyNqS5tFzI6GPtQ1j3OsMnRO1JtbduWGj289z3NdCbNNussAHAnI21HMKVs17C0tDM+JFvaVLdCxrcItn70lJWMNLm2WULsrhYZjr+skppLNtwUapmsDzUDWyf0LN6yTuiP9TfyW9rQfR9nPK7jH/iH+q35d9DuFZifaBERbjQEREAREQBERAEREAREQBERAEREAREQBUfTdwFBVX/uiPPIe9Xi5X6ZtuPa6npWOs1xD5bb+0AweFwT5JuuSduTMxdpLqjnDCWm246fkpcc+5fDEHDNQ3gsOem4quWZaPItYJXbtfgrGnbM7PERyVPR1oyvqPNbBTbQaGEm17LEosnGaJNMJAMyTyUtuLJY6KuYRfLu5/oLJLWtFrZncsKJlzJbpbC11CmkMhwA5b/BRnzOcQALk+XirCkp8AO8nU96y8iKzL/oSWtne24uY8hxsRe3mFu64X0s2pJSPpKiM2LKgA97XNddp7iAuz7G2myphZNGey4eR3g94K7cPH/EpHBisqtiaiItpzhERAEREAREQBERAEREAREQBERAEUHam14KduKeVkY+8QCfAankuZ9I/TI1pLKOEvP95JkPEMHxI8FOFOUtERckjq80zWDE5waBqXEAeZX569I+0xU1s8kbg5rS1rCNCIwNO4uxKnrdt1NW/FUyuk3gH1R4NFgOQWO2ascPhd27lxVjnqVeRaUjw5ocNCLhZpoARoqrZMuGR8J0PbZ4HUed1skEK85XpujUcHwPQUpqrBS5mvS0Vjl7fzUunhktaxPNXk+zyRkFGgY6Nwyy8PzUO0JdmjFSbNkOgIHe7L2K3ptluHrOA/Dr5lW9MAW315WWdsXd8VjfM7iI9NThosAFlxcF7DDwWeOAZFa3Imomlekhg+Ss4meO3IOv7Lq59GPST5OerldaKS2Z0a7QHwOh5LXPSbWB0tPANxLz5ED3lYNnNswL0OyKKnRkpcSk2nU3aqa4H6MY4EAg3BzBGhX1cOoOlFTRAOjcXRj1o3dpoHEbxyXQOjvpEpaizXuELzueRgJ7n6cjZZrYOpT+KNEK0ZG4ovjTfMaL6uQ3BERAEREAREQBEXwlAfUWo9IfSJRUt2h/XSD6kVnWP3nXwjzv3LnHSD0lVlRdsZFPGdzPpCO9505AeK3U6E56IhKaR13bnSalpB89KA7cxvaefBoz5nJcz6R+lCaS7acdS3j60p56N5X8Vz4u1JcSTmc8yeJOt1hlqNzRZWFPBwhnLM55VZPQ97SrZJXF0jnOcdS5xc7mSSqmV+RsNPaplrMc87h/sFhpY/VvvcD5Z/BbpRvkYWRMgjI03ADyWfEsYZlcHkvrTcralY1PM87VYR1crdWmx8DmPd7Vt2wa4StB3qhfFiY5vEe0aLFseR0bxwVHtmjaalzXkXOy6j3WuR0qnbcWXp9EDqFg2NPiAV62G686y6ItPTAblJDAF96ohfWtS5g+CPuXirkEbC47gprWLWumExERAKkiLZy3aVSZ61zz328Bl8VsNKMlR0VEcbnE2DRcm18rjQbypjekdOwlruvB3nq2EeQkuvX7MahQuzzWPi5VWkXmC4sdOC1qemMTyzOxzB4jgeJGXsV9s/bFPKQGTtvoGv8Am3fzdk8ivPSOmtGXnVhBscrZ4Tlws4+Ssd+MldM4YqUXZkjo10wqqSwY8vj3xvu5vIE3byPJdF2T6TqSSwlDojvNsTfMZjmFxJ0mHVG1WLUfn5rmq4alPXU3xqSR+m6DacMwxRSsePuuB9ilr8uw1jmnE1xaRoQSCD3EWPtWz7H9JFbF9frWDXrBiH8Vw72lcM8C13Xc3xrLid7Rc72L6V6eSwmifGT9Zvab/mHkVvGzNqQ1DA+GRrweGo8RqNDquSdOUO8jamnoTERFAyUvSfpPT0MeOd9ifUYM3vPAD46LjnSPpvVVwdY9VT4g3Aw6l2gc7IvPcMlR7Urn11RJVTmwOdtcDNGMaDvNshvNyVHM+NzABha0jA3cLkeZO8rrowz9VXtq+HRfEVI7sVv6vRfd/wAEedhaS2xbYkHS+Rtu0WLAd/mrbakQE0oA+u4gce04EeIIURzd4GSsqElUpxnzOWvDs6jhyIxhPisRClkWtwOh+CCMFbXE07xA2gD80zcbuPuHxUukpyXjLJrCT4uyHsv5rNUUt52NH9223MuUqhpnSB7mMc4FzgLA2sDgb7Iyeaxu+tn+WMt5fnEhuYBaxWSnZcj/AHPIKS2jBeGvkaHEXwNIdJYbyBk0d5PJQZ6yTH1ULerZoX6yO/e+qO4LPREbFjNKyLKWRkZ+y4kvP7jLkc1Oo4I35tc134T+jyK1Oi2SBI9zs7PscVzk4Atdx3q9g2eLhwBa7LMZc1yYnDPEw3Zu1tLHTh8R6PK8c76m67NBZu8le09YLarWdkV+5/dmrWrYG53yO+68visHUw8rS04M9DhsVTrxvHXkW7q5tisJ2i0Zk8hqqZk+eo8F9mtvyXJY6MiZU7Ycb2Fgtbr6t0rsAz4k6Be6ytLjhj0A7TveAlBDYAtBLibMAFzcZucRwAzz7le7P2Vvrta2nBc/6KfG7RUP8dLXnyI81OxvZA7LM3ni7XPLO3DiVqVRTBzhdvrtJPM3W4bTZhje0XDWjPEQXOeeJGWV7+Pgqyqo7dWeDQvSR3VGyWRRbzbu2ahHRAOLSOXvWxVkkjKSWOxkbgOEOObPvNdmbDI4dMty+bWo8JEgHj8VZwAFjTqNPEf7FR3VmkSc3kzWphjia8eB/XmsVCzFdqsKOhwSzUx9VwxR+Go/L90rxsmkPylje9wPIE/Ba87p+BO+TMVNS4rufkwfzHgsj7ycGxjdusN6tNoR3OBuTR+rqJSQh5cTlFHm48SP9cgOPgtjjbIipXzPtBTh8sQN2sEkRPE3e0AH25K0ftWeGrlkY4sPWOuAchYmwHD3cQVj2ZHnESLF88ZI4DE0BvIWXrbH08x4yv8Aa4rhotVqsrrLNLoml53LPGUvRoQS1sm+ru/Kxsf/AKkVX2//ABs/zItO6s/oBFv9Ao8n8zi9Kn8PkiBVuzEYNw0kkj6z9HO8PqjuHevVMQ1zS4dm4J45G6wxM7s1YwxXGazToqMNxEalWU5ub1Mu24SJZSDciRz2n7TH2f7j7FXmYNIJ+jfkfuu/I628VfV1N81Sv3FhYbbjG4hp5A8xlwVdU0GTmOyDsu5p+q4dwPsutGDlaPZ8Vf6Oz+vmjrxkXNKsllkn1tl819Uzz8mBu0+q7fwO4jzB8COK80tNnhOTmmx5LJ0feXNMbx22O6t3twHzxN5gq5mo/nYXWzIcCeOEtsfI+1d6aZWyyKusiLZZH/YpmEficXtb7bKFSbOxGljtf5kuPhjda/NbPtiAYwLesQD+CnjMrj/FMwcivux6Xq2yzvH0MDI+bG43/wA78PJat5XJXsinoKUdZUy2yaOrb+vFeYNnWkZlx9ytKKWGKlY18gxucXvFiTcngB4KI7awxXjZewtd3f3ArTUx1GnHOS8zohgcRN5Qa65GPaNMI3MltkSI3/hd6p5H2EqSKllurF3vGTTiAaBv11VXtStlkjcCQBa+QG7PxWPZ0ZlaHA9q179+9V9bail7L6kpYKVNeuX9IbrYnXaG5XZbtcR9781UbH2a57Pm4nB41uQG5anE6wsraOuDSQdAB7h/quulOnjKLjLx/lGiM6lCamsim2i9sbrm2E3F8tcrfrvVZ8re/IHse3keClbaoWyPEjQ5rL9pv1XHcbbvisEEd3ABc+E2SoT3qmdtP7O7E7Tc4WhlfUzNs1vAWWKPaLhnZtiMLGknQZlxA1sc/IKVPCwkiSZrMOZu1xFrXtdoNjprxCjSbOkfJJhLJMLBYMeHOsc8m+tlvyWzaOKnFqMbpLicNGi5Z6mGs2szqQHNLSXXyzuPzVndkoaWG+Wm8dxG5antbhpb9aLFOO1feualtGou9mb3hU1lkbjLRYmEEae4qv2dCR1kO8DEzvtmB7xzWuRV8rHBzZHZcXEjwIJsQpf/ADbZ7HvhsWnVh1HAh3vuu2nj4S1yISws1pmX+2KQFkVU3WKzj3xm2PyGfhiUyh2UBOZPuyEeTRf+dWPR3aEFT1nVA4RYljwAQJL3GRILbh3mpsFJ1bLZnq45GDiWtMZbzw4V0KonZrRnO01kzRdpNLYi4es84W8zYc7C6+SQBrWQN9SMjrD9qTcO8N9/grKohLnjDmY3YI+HWWzeeIGbv/jPFYYom4yG+pELX+086k96jia/ZUZVOOi6lhszC+k4mFLhq+i/LdWZKNmKpp2cJGE8ji9zVCrCHSSOvq9x8yc1YdHSTPJKdI4pJOYGFo83BQjHew/38FrwFLcdnwivm22/sT2tiO2rSmtHJ26KyRD6zv8AYinfJ+8orMqbop4YwD71YsgIz14rFEzdl/optKQDZ2oGXeFoRJssnAPogR/26i3J7PzCjPiDmA2vlY+G9SKF9o6lg/uxJh3lsbhd4HcDmkLbAcDmFT4u9NOcdYzv4SS+56LY27Vm6E9Jwt4xeXyRQshLahpvYSAxOP32jFG/xLRrxaVuDmh7IpAOFxwcbA8gQByVFt6LBG2YeqXNBPBwcCPbcfvlbVssDq3DcHiQeDrEj+LErPtE4qa0f3KCtTcJuEtU2vkV+24O2Rxbgv3SvkfL/wCGG3kqDbdfIIGQsIHWSND7AXLietNye+yvukFVaWKnAJkdCzFb7U5aPMMidl99UWz5gZqdwJLsU8zgWAgDEY4xnqbA7typ8ROrVqKlRfX+y/wFOhh8M6+Jinfup8ba2IVVTlz7NBcRkA0EnyCkxbDlw3cGM/aPY0+RN/YpVdtKcuIdI4A7m2a3mGALEzZE7rlsEmlycLs/Z7VCnsVr2tRLp/djNfbvaezp/ngeP+HRjJ1THw7Ae/24QFH2JWfJ8TYXNc4OPbMebQLYQ0P5nRei0W07rb7qA0YJjf61lYU9k0abTbcvg7W8ipqY+pUvkl0NnqduiWz5XvxNHZN7i+/s6LIyt6ztWvb1mjItGWYH1gqb5EXZ2z4KdDTEOF7tsNd4OllZRhGKtFWOCTvm2T6l4dGSCCLXFu7NRaIYGl+rjkwHjxPcFiMwa6zuy7usGO/yleJnvxABwEhFsj2Y2cb8bXPt4LOhixFkcXPczUR9p5+2855neBbzKi7Oc4Y36EuvcagjTNSIg0UuMZda8ubxwjJuXhZY4o7NsdbaLCzJaHqbalQ4H513dfM+ZF1ldtAvw9ZFFIbC7pGkvyytiaQTzUNzbAgE29yyYRhYR4DvWl4SjLWC+RtWIqLSTPboKZ3rU5aeMUrh/K8Osodf0YieH9VPgNrhkrSc/wBq0Wt3kDv4rYdnbFLml73NY3K5cdxJbkO4jMEg6FZzs+PACJBcPc3EScLmgXZYWzxEEajcM7rkng8M+7ddLvzudEcTWXet4mj0NVU0Egc17QXMBu2z43NJsWkkWJabEgac1v8A0f6Uuqg9kjGtkGAXbfA7ETnYkkG7QCLkZhVm16P5O2JxLXwdYS9jrFvVyHqn3boPWvf7vcsFBsz5IDJ17XjGI7WLZAY5WPzabg9lj8wVzbk6Ukk7xf5nyJycKkW7WZKlnEcRcNS0hnH51znk+JBYOSxMp8EbI/rHN3if0VjiZika05tjbFfxZFELfxEq1pYS8ud32H68lnEvtq9OjwWb/PzUttnr0TA1cW+9L1Y+Xnn4Hmmh6ulkcPWlkbGPwsGNx87BVtgWk2s0al3w4lXe0wHdXHiDYIm/OPGr5HnEY2DfbsjLebLHgbGBLK0NsfmYiQADoCb6v9wVnhpeq5/qbfhovojztbVR5K38/Up7D7En8DkVt8vm/u2fxs/zIpel0v1Ix2NT9LNbg+rzWf8A7kfiiKS1IMvdn/Tt/Y1P/wBRUHZn0EX4URVWO7lX/TzZebD97pf7eRk27/Z1T+vrMV7sv6B37JnvcvqLfQ92j0Rx7S98qfuZXH+3eUX/AOZyoeiv0zf/AGrf6nIi5Nn+8VPA6do+70P2fdlrS/Tx/tGe8Ld5v+lk5f0Ii6sZ7SJX0O4zmT/WHgFBrfpG+IRFZy0OWOpsGytApVTu8PiURCJQbU1f+BR6D6OX9jJ/Q5fUUZ90nHUlVH0FN4fkvlT9VfUWYmGYWeqOazbP9aPxPvREloyUdUbH0x/6g+Lv6Y1Gk+gHiPeviLThvZRFbvsg7d/syp/EffKsPSr6CX9vF/Q9EWqXdl+cTbHge6D15/xD3NV7s36I+DvciKspe+y6fwekxf8A41L9y/6MNZ61L+1/zqF6RfUjRFaU/YL9v2PNS9s+rNXREVIWR//Z</t>
         </is>
       </c>
     </row>
@@ -3933,115 +3933,115 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RAVICHANDRAN ASHWIN</t>
+          <t>ROMARIO SHEPHERD</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>tnpl2023_16</t>
+          <t>sat20_2024_17</t>
         </is>
       </c>
       <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>2</v>
+      </c>
+      <c r="N28" t="n">
+        <v>15</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1</v>
+      </c>
+      <c r="V28" t="n">
+        <v>75</v>
+      </c>
+      <c r="W28" t="n">
+        <v>8</v>
+      </c>
+      <c r="X28" t="n">
         <v>5</v>
       </c>
-      <c r="E28" t="n">
+      <c r="Y28" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC28" t="n">
         <v>10</v>
       </c>
-      <c r="F28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" t="n">
-        <v>50</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>50</v>
-      </c>
-      <c r="M28" t="n">
-        <v>4</v>
-      </c>
-      <c r="N28" t="n">
-        <v>31</v>
-      </c>
-      <c r="O28" t="n">
-        <v>1</v>
-      </c>
-      <c r="P28" t="n">
-        <v>7.75</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>31</v>
-      </c>
-      <c r="R28" t="n">
-        <v>24</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>1</v>
-      </c>
-      <c r="U28" t="n">
-        <v>1</v>
-      </c>
-      <c r="V28" t="n">
-        <v>29.2</v>
-      </c>
-      <c r="W28" t="n">
-        <v>7</v>
-      </c>
-      <c r="X28" t="n">
+      <c r="AD28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE28" t="n">
         <v>6</v>
       </c>
-      <c r="Y28" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>29</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>9</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>5</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>7</v>
-      </c>
       <c r="AF28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH28" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="AI28" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AJ28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL28" t="inlineStr">
         <is>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="AM28" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYWFRgVFhUYGBgZHBwaHBoYGBgZGRoaGhgcGRoZGBocIS4lHB4rIRgYJzgmKy8xNTU1HCQ7QDs0Py40NTEBDAwMEA8QHxISHjQrJSs0NDQ2NDQ6NDY0NjQ0NDQ0NjQ0NDQ0NDQ0NDQ0NDQxNDQ0NDQ0NDQ0NDQ0NDQxNDQ0NP/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAQQFBgcDAgj/xABAEAACAQIDBAgDBgQFBAMAAAABAgADEQQhMQUSQVEGIjJhcYGRoVKxwQcTQnLR8CNigvEUkqKy4SRDU8IVFnP/xAAaAQADAQEBAQAAAAAAAAAAAAAAAgMBBAUG/8QAKBEAAgIBBAIBAwUBAAAAAAAAAAECEQMEEiExQVGRImFxBRMUMoEj/9oADAMBAAIRAxEAPwDZoQhAAhCEACEIQAIQhABIsitqbeoUMqlQb3wr1m/yjTzlR2j0+c3FGmFHxOd5v8oyHqZjaRqTZoUZYnadGn26qL4so9rzGttdKahzrYhzfRA1r/0LYedpUsT0hdj1FCjmesT4zLCjf6vTDBr/AN6/5UqH33bRu3TnCj/yH+j9TPnd9q1W1d/I2E5viXIsXcjkWb9YWwpH0WvTrCn/AMn+T9DHNPpjgz/3SPFKnz3bT5rp4l1N1dwRyYySobfqjIlGP8wsfUTLZtI+k8Nteg/YrI3cGF/Q5x9efOeD28j5OpRhrfMesntm7aqr1qVZ1twDHd81OXqJu4Npt8JnGz+nlVbCqiuOa9Rv0PtLdsvpLh69gtQKx/A/Va/IXyPlNTTMaaJqEITTAhCEACEIQAIQhAAhCEACEIQAIQhAAiQlZ6S9KUw90Sz1eX4V72tx7pjdGpWTG09p0sOu9UYKOA1ZjyUcZn+2+mdWrdaV6Sd1vvGHefw+XrK9jsY9Vi9Ri7HieXIDgO4RvEcrHUaFZiTc5k6k5kyB29tYpemjWf8AERnu919AY92ttJaSGxG+R1Rxv8RHISlL4+vzgkY2eixOZ1PExCYGc2mmHS94tuE4Az3ADpuHUek9BPH6zkDPYf8AtnADvTYXANwRcAkcRwPPwj3C4h0Ykan4c1a3IE6+88FSyAb+o0ZToMlO9nb/AInvDBhle97m4zUgZEjvH1gaT+E2srkKQVY3sDexsL5e+RklKXVOpJzFuybHW28lz8pIbH2vZxTdrq3YY6g6BSeI5d8xo1M0TYvSyvQsrH7xPhY5j8ra+RuJoOx9t0sQt6bdYao2TL4jl3jKY6pnShWZGDoxVlNwwNiIKTQOKZuUWU3o10uWpalXIV8gr6K/cfhb2PtLjHTsRqhYQhNMCEIQAIQhAAhCEACJCVXpj0i+4X7qmf4rjX4AfxfmOdvWY3RqVnDpb0p+7vRom75hnB7HcP5vlM6ZiSSSSTmSTck8yeMUm5ucycyeOcSTbsolQTliKyorMxsFBJ/Qd86yv9LMVZFp/Ed4njZdAPPj3QQPhFfx+Naq5dsuAA0AGg/5jdDPIeegYwh5VopvF3Z6IyjGHkLBPG0S86Il8gLxTUhEN57UANmMjyv7TrRwrGOP8E9rWP1mOaQ6xyfg80rjUsRwF8x3rfXwiO5DFhcC+YIsb8TujIX8J7wtNgwVtOF7keFwMp6xNB1bM94INxblp7TdyBwfo44jD9W4e+vhbgRfh/x5NGY6G3PznuvfncHThby5TiTAVlp6P7XLWovmQOo3E2/C3M9/G0sEzmi9nDX0IIPKxGftNFV752mSRsWepduiPSq27QrtlorsdOSuTw5GUmBmJ0a1ZukWUfoT0iLWw9Vrt+BjxAHYJ5jhzl3lE7JtULCEJpgQhCABCEIARm3Nqrh6TVDmdFX4mOg+vgJkGKxDVHZ3N2Y3J7/0k10v2v8Af1yFP8NLqvIn8TeZy8AJAScnZSKoIQixRgEqXS4/xFHJL+rH9JbZTek1YNXIt2FC+JtvH/cB5Roiy6IUQvALcRzhcPvG3dNbpWLGLk6R4ptPSpHqbJN+0f8ALn85JYPZK36zZchb3PCTeSPgtHBK+Rhhtlq+hI58pKYbYIUjrGTuEwKAZADu/Xvj1KVuP1nNPLLwd2PBFeCOpYBR6a+Gk9tg1kolOdKWGuZHc2zopJEMmzAeH0nqrsdSOzYW0lsoYVbaafvKeMRRvabyJaMw23s0oL7lhoWBy1uDbgeEhGp2B5j968ZqeOwoZSpAseBFxKDtbDbjkW4cBYcbTqwzv6WcmpxL+yISXnYNUtRS+oFrniASAfb2lHdZaeidUlGUnINl3XANh7zol0cUeywRYkWIOelcggg2INwRqCNCJqvRXbIxFLM/xEsHHyYdxsfO8ymSOwNqHD1lcdnsuOaE5+Y1HhGi6FkrRscJzp1AwBBuCAQRxB0M6ShMIQhABJAdMdqfcYdrGzv1F5i46zDwF/aWCZd082h95iNwHq0hu/1NYt/6jyiydIaKtlZiwhJlAhEiwAJSOkS2xD/zbreW4v6GXeU/pXTtXB+JV9iRb9840RZdEOuslNlpYX5/KRYk5gU3UBPK8TK+CmFc2SNO0eYY8pAPi+A/tOibSKyP7cmjp/eimWyiDrHKA5SuYbpAuhVvQH3k5gdoI9utbxuPKSljki0M0ZdD9Z1w7201755KZC2c8pjKadpwLc768eEnGLbKymkuSQWo0R35yJq9IqO6dxt63JWPqdIwbaxa9mGRtqRa/iM88pVYpEHliTlRbym9JKA3kyGbH34jw+slsNtfOz5aZ8M+fI3ynDpDS3ghyz3lv3ki31jQTjJWZOSlB0UfFp1gALC2nmb3lg6IJ1ah4byjz3b/AL8JA1kIJ9PplLF0UpAI7cd/d8goI+ZnY+jzl2T0IRYg4kWEIAaP0B2nv0TRY9anpf4G09DcektkyPottD7nEo5NlbqN+ViPqFPlNdlIu0TkqYkWEIwpxxFYKjOdFBY+QvMSxFUu7OdXYsfFiSfnNU6a4ncwdS2rWQf1MA3+nemTiJIeIsQmLEIiDgDFiARYAFpW+lGGYlW1Fsu4i29fnfI+UskY7XS6aaMp8jkfnMbpWbFKTplEEmqoJVEF87XsbZePCMtpYYI/V42O7y4yYwyAnMTJy4TKY4NNpnilSppm3pqxP1jjeokEtTUX4u6J8znG+IoE3KkA+uvKOmwgamBTTcqbrIzEI6ur9reLdZWyFmGgvpEVPtlWmukcn2cgO9YoL9oMrpfgCy3C3744w9LcdQScuPHh+k7VHthlpsifeKFUVbhSqoLKiqq9dc3LbxzLX4ARlhid0E66d3daZPrhmwjzyqLdgKbPdVJ0vp6G/CNcTsQvkx3QWJB1bMWPnpHnR7GELawNxbvynPpDWcqChHWATNiu6LkswIGpvbwEipO6ReUfZFjZuGRgCWdlyst7Kf5rZA+clqSU0Fhh17xurf0OZldx2zmekq0ae65yZmdm0Nw1MgjdOoI3bEW4iWKrg6q0SypUFYkdVSDhlUKo3ArsWuSCxZQLM9sxlLbU1e4jbUq2iYnBUa6Hcya2RFwwPDx8CJE1wzYTr9tOOmaNYnuuJP7NViAzoqNx3WLfQRhtqmBSqBeKt7gkySk7S+47ikm/sZ/VJJHtxzuR+ssnR3ClELH8ZFh3Aa+59J46P7JSoGqtmi9lebALdj3AscpNW8p1uVul4OLZtipPyLCIIsBQhaAEWaAlpsmxMZ97Qp1OLKL/AJhk3uDMcmj/AGe4new7ofwObflYBvnvRo9iS6LZCEI4hTftIq2o01+J7/5VP6zOhL19pb50B+c+m6PrKNJy7KR6CJFhFGCLEiwAScMct0Yc7f7hHE54hbo1tbZeIzHymPo2PDRStqtvOXtkSQO/dy+kl8LnG4wwI3cijK1viVjmvoR7z3gG6oMnJ3GvR0pVJv2TdLCBhOv+DCjMehtPezV3svrHuKp2Eg2zpilRB4hF4ACN6dMXnupigWKpY21P0iUwb9bjym80HBYtgWAPy+Qkg1EE6XU/PlOPR/Atuk24X8o+erZhZbgayb7KnNMDT1tun+Uke2kdpQuLBiYiVFe40tw421B8I9oYfiPSZzYrqhi+HtwkDt9d1H/KfEk5AfvnLdiVtKl0kUsm4tt52VBfS7Oqgt3XOcpFfUiMnwxjsUlcNe+b1Gv4Mim4t+Ui3dOtomEQLSKAndFUbgYWbcSkUJI4XY3856tOqFO39zky2mk/CCAhFjEgEWEIAEuf2cVevVTmqt6Ej6yly1fZ6/8A1DjnTPsy/rGj2LLo0mEIShMoH2ljrUPB/mkpEv32lU+pRbkzD1AP0lBk5dlI9BCEWKMJFhFtAAhCEAIQ0bMwXs7x/YkfgcltyMsVXCgneDMp42tbxsRIL7ncd1+FiOV88svC0k4vkupJ0kTWza1o42zjLIeZyHeTInAnrCddqoSRfl7mT2/UXUqiMMOipa2Z4k8SbXjhMY1+sgA4G4I87RiKROpHnrH+G2fcX3tbcBGaXkyLfgvOw9pWQkAZru6ZDwnVdoDeKGk3Pe6u6L8+tfnwlUwOBfIB1A4jrZ2OttOUnX2c6i4It/LkPAgiTpFW36OG0mam9OqvZJIbkAWuoPcP1lo2Ziwyg90re7vKyNe34TwPd5RdlsVJTvsPIzGvIqlfDLDi6nd+9P0lZ2qu89FbXvWS/fZgfpJasc/3bXQyFx1ZkqU2FgyPvC+lwpOfl9JsVbFk67OeJZ96zm5FwuVgFvcD+84xzjcV94wYixAt53vG06YpqKOObTk2gixBPQjChCEIAJLR9nw/6pv/AM2/3JKxLd9naXrVG5Jb1YfpGj2ZLo0OEIShIq32gUN7Db3wOp8j1fmRMzmybewv3uHq0+JU2/MOsvuBMbiS7Hj0LCEIg4RYQgAQhCABIPaa7ta/B1VvMXRh/pU+cnJG7cpXQONUNz+VrK3kDunyg1aNi6YzoNZsv+ZJ4zMK/wDLIAPp3fvTjHZxd1AvIuJ0KXA3fD2rLU6zUyRvIDY247p4njL3sjYuEqoWWtYmqqqu/wBbdY2CKpz3tSLg5eF5TkIOsl8CtNl7W668fD4SMwdINtlIxXh0aFgeh9IXBeoeWai1+dlzzEZ9IMLh6NAuatVnVRZaThnd72ChCDlzvoL8pBUy7dUVamYzO++fIHOP62y6dNAA12IucshfhcdqYmq6GljlfMvgquBq4vqvWChGNmTRlyJufTMf2k9g03usNL314a2HLTWecVu7m7bLPny4+U4bPq2BANwxFvYacssor5VmSpPglN/O/Lnpnx/fKQmPfeqC2ig8eJt9AY6fF5bw4+uWud9O/wBpGUjcb3xZ/wBP4fb5x8cebI5ZcUe4RRASxzhaLEiwAICeoQA8y+fZzQ6lV+bKo8hvH/cJRZqPQzC/d4VObkuf6jl/pCxo9iy6J+EIShMSY5t/A/c4iolst4sv5W6y+xt5TY5R/tE2ddUxAHZ6jeBzU+RuPMRZLgaL5KHCEWTKCQEIsACEIQAJ4rrdHHNWHqpE9xSuWnAzQKRSbK3HvnX70nLKeKlPIEcpzBvpFXKGdx4JHDPe1zbnJBaSMLhmv3ce85SHwp3srydwCZDP9+MnLgvjdjmjhn4O+nr7yWw5VACzdbjvXuQAfIG5nilUUa6+Gv6idnpB729CM8uJvyk7bKul0NcfWvyzyOenAZ+MbNW5DIi2YNxlnY6W1znrE1Bey8LHxyuR7nPjeMgN0DQk3tbS/AC/zlIxISlydnYudwHtZvrppbxPHxvHC6T1hMNYXIztnqbdwJz5cZEYjbapXGH3GJ3lXe3gAA5B3gLZ2B7tI8PqltRmVbYqTJaLO2LwxpuUbO1iCNGUi4YfvIgjhOMdpp0yCaatBCEUTDRYQhADrhMM1R0Re07BR5nXy1mzUaYVVUaKAB4AWEoHQHZ+/VasR1UFl/M36C/qJoceKJyYsIQjihGuPwi1ab020cEeF9CO8Gx8o6hADEcdhWpO9Nx1kNj9D4EWPnOE0Hp5sbfUYhBdkFnA4pwbxHyPdM/kmqKp2hIohCYaEIQmgI5sJTds1KlPEdV2CuQRZjbPIiW+oYw2hghVWxyIN1Nr2IzHlO3HhvFa7fJwzzJZeelwRbJwjSrRzuNfnH5DAlHG641GoIOjKeKngZ6+7vPNuUHTPXqM1aIcNY8jz4GSeF2i6kXF/DO88vhgeH775zGDHC48CLRt0X2S2ST4JD/5Fy11vbvFzH64mo67tt1eJLcLa2HHTKMcLsdyLipYeHykpS2Oo7bu55E7oHkB3xHKPgpGEvJySwuFBd7DP26x4D5x9hMGxNzYknQCwA7uQ9zqY8w2CFrKAqjut5gc4+WmFWwPicj4XvElP0UjBLsbFMvlwtwlTqYIVto01TPdCljysSR7SY6QbaWihtYm2Q/fCdPs/wBnkBq79t8zfXrZ+wtOjRYXLJufRzfqGZRx7V2WXbeD36QcDrU8/FPxDyybyPOVuXpDylU2xgBTcbg6j9kC/VYXug8hvDuNuE79Vi53I8zR5bTi/wDBhCIIs4D0AnqmhYhQLkkAAcSTYD1M8y49Bdjbzf4hx1VyS/FuLeXz8JqVmN0i2bC2cMPRWnxGbHmxzP6eAEk4QlSQQhCABCEIAeGUEWIuDwMy3pXsI4epvIP4T9k/CfgP07vCarGmOwaVkanUXeVhmPkQeBHOY1ZqdGLQEk9u7GfDVN1ushuVfgwHPkwyuJT9s4x+wpzOWUfHglPnpCzzRi68kxVxSL2nRfFhf0i06ysQqksWZVFgcyzBQBfvIkHhMClJd9zdviOdr/COcebF2ulPEUGK3RKiMxa193fF2t3AlvKX/ipK2S/ktukiRxAszDkSPQ5TlaTG3tmmjVdeF8jwKnNSPLLxBkYKepyAUXZibKo+JmOSiX081LGn/j/KOfVY3DK14fK/081cKlZNx+qw7DjtU2P+5TldePcZEYjD1cOwWqhsey4BKP8Ala2R5qbEcpz2h0gN9zDkjgapFmbupg9hf5u0f5dJ22ShK9d2JY3JvvMeF7sfnMyaaOf7P2UxZ54Fb69DlKauLjX1BnpMML2/tHAamjBatyHUMtWmCDusSo36Z7RDKQQbkc7ETu9Mo5RipIsQym4IIurC+lwRlw0nk6nSzw8vlHrabVQzcLhnrC0bfpn8o/pHd19gB4iN6VRdZ4xOLA4icXLO2kO2xFuQtIfam2ggIXX2EZ43aGWplcxNcsZaEL7JTnXR6oo2JrqpuRe5yJyByAHEk2HnNd2HSUUwFZWI7W66tuniDuk2OuspXRvZjU8O9XsvUG4jHVUIsxXvsSL827o3qomFs4uKhuFCndcny0UZXJ9DPe0uBwhb8nzupy/uzcU+jTzPSU1c7ji6sVBB4daysOTKSGB4ECVDZ/Ssoo/xQvw30Gf9S8bc1z7pbthYmnXZTSqI6ghmKsMlXPMajOwzE3VXHG774oTSR/6r1zfwV/aeFCs11U9ZlYgaOpIY3Gl7X84zo0EdWZSRYkDiDbx4RjjtrscRiHU3R3dt05qy7xCnuJUA3HvHuwScQfuKKsrEbxJzRRfNiw4Z8QLyrww2KU0uhN81KoN9jno7sk4p91TZUNql9V8OBvwmq4egqKqKAFUAADgBGWxNkU8NTFOmOO8zHVmOrN+8pJzypbdz2rg9KO7atz5FhCEwYIQhAAhCEACEIQAZ7QwKVqbU3F1YWyyI7weBHOYr0n6KNgnNRg1SkT1HA48n+FvY8OU3WccRQR1KuoZWFiGAII5EHWVxZpQ/HonPGpfk+b628xLN8OQ4AchGZTTvE1Lpb9n751ML1ltnSPaGd+qx7Xgc+8zOxhWVrOpUrkVYEEHkQcxPShOGRWjilGUOyzf/AGmk2DprWWo2JpL92N2wSogvuMzG+4wAW5sTe9hY5UvauPq1rA2VFN1RLhAeZBJLN/MST4R69K4A7/rPIoAcJkdNGLdeXYz1DlW7xwiLwlPPPhJ+nSOWuVtCMhz0jZ8LYkgaj9Z2oVWW3K1p0Rx7eiE5bx391vtvOSzKN0X0C3JFu65MdIm8Ag7QvuWyvc3KHxOa8muPxRvhql7X71P09483ZLNjU4uL6ZuLK8c1JdojqmOI8PO/d4RhXxpPG069IVKvv/hqDe8GGVQD+rreDjlIam9zPnZ4dknF+D6OGZTipLyOK73yjjo9sk4iutLK1iz3+Bbb3rdR/VESjeWHY9P7hC4yZ1sTody4PkCQD4L3zq0enllmvRya3ULFBpdsltvbUWkG3bFwLZDqg8FW+dhcWlU2XgyzNXq8BcX8z+/Gdat6j3PZuTnx/eUcY4ndCDIE5246C0+i2JHgxdKvLInHVDVYKOyuvjHWGojdUWHOdDSCggDPLhqToJdujHQipU3ale9NNdwizt5HsDxz7uMnkyQx8zZWKlKlFEHsTYNXFOVQWXIM57Ki3udcprmwtjU8LTFOmO8se0x5sfpwjvBYNKSBKahVGgA9zzPfHE8jUaiWV10jvxYVBX5FiwhOcuEIQgAQhCABCEIAEIQgAQhCACSG250coYofxE6w0deq48xqO43EmYTYtp2mZKKkqZkm1fs6xCk/cslRb3BYlGA5MLG/l6CVTHYdkZlYEMo0III8iAeWs+hozx2zqVYbtWmjj+ZQfQ6idmPWSXElZyz0qf8AV0YMudvC8FRTaani/s9w7G9NnpnSwIZfRs/eV/FfZzXUD7uqjWN+tvIbehnZDV4pduvycstPkXj4KYxC68wfcGSuAo76b5NlJsLAk5XBJtoMj6GOq/QzHDe/gbw4FXpm/lvX9oUtg4ymNwYdmUEkBl3rEm+RU5jjY31jyyY5dSXyJsmu0/ggeklI/dMDbepOL2z6rAK1jy61JpV8IpZlUAlmNgBxPKX3GdHcbUSoP8PVLMrZlbEsc+PeB6CcujvQPGqLvQZCwIJL0wVTTdHW7Tew9J5moxxnlVNU+z0tPllDE+Ha6I7A4MKbvYqpsSD2nt2AeQ4kcPGe8ZiCxbu/SXSl0CxL7m81KmqjJVLPb2GffeSuB+zmgudWo9TiRkinxt1uPMTvhn0+GNJ/BxTxZsst0l8ma4dOuABc2yAzJPcOJln2V0LxFbdZlFJb3Je+9bXqrr62mmbP2RQoj+FSVO8DPzJzj+0hk/UJPiCorDRruT+CA2L0Vw+HO+F3qnxtmf6RovlJ+LCcEpSk7k7OyMVFUkLCEIowQhCABCEIAEIQgAQhCABCEIAEIQgAQhCABEiwgAkWEIAESEIAEIQgARYQgAkWEIAESEIALCEIAEIQgAQhCABCEIAf/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIQEhMSExIWFRUTFxUYGBcVFxgXGRgZFxUYFxkaFRgaHSggGBslGxYYIjEiKCkrLi4uFx82ODMtNygtLisBCgoKDg0OGxAQGzclICIuLystKy8tLTUyKy0tLS0vLzUtKzAtLSstLS01NTU2NTAvLS0tLzgtLS0tKzAvLTUrLv/AABEIAL8BBwMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgIDBAUHCAH/xAA+EAACAQIEAwUGAwYFBQEAAAABAgADEQQSITEFQVEGEyJhcQcyQoGRobHB8BQjUmLR4RVygpLCY5OisvEX/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAIDBAEFBv/EAC0RAAIBAgQDBwQDAAAAAAAAAAABAgMRBBIhMUFR8BMiYZGhscEFcYHRFFLh/9oADAMBAAIRAxEAPwDuMREAREQBERAEREAREQBERAEREARLdauqZczBcxyrc2uTyHU6H6TUdoO1WFwOTv6gBqaqo1JFwC1umu/rAN3Ein/6DgO9pUe+F6oUgnRVze6GbbMenmOom8x/GcPQF6lVRqosPE12IC2Vbk3uOXOAZ8T4DPsAREQBERAEREAREQBERAEREAREQBERAEREAREQBERAEREAREQBNDxXtfg8LXXDVatqrWNrEhQ18pZrWFyLW31BtbWb6cC9rdZDxCtcHMvcpvvZM199PfA+QPOAYPb3tliMXUClsq03IApF8jZXbI1j8eU/hzAkZ4lxitX8TuajaDO5LELqBcn9a+sxXrZjkA53vpsAb8tTqJRVcBdPX9X/AK85w6VGtp7waxAOp9dLbGW/2hne+rMR1ufqflMcU99dOfnyFuu0resLWA12On6uYBO8H7ScctTDl6gdaF7rdlz6W/eW0bQ2/QM7FwXt5gsWaa03JeoVWwVrKSDuSBpcWv1I6zy4Wvrf7TZcC4lUw1VHRypB+GwPyvtz1gHrmJo+x/aalxKh31O4scrqd1awPzGu83k6cEREAREQBERAEREAREQBERAEREAREQBERAEREAREQBERAKar5VJPIE/QTy1xWtUxNWrWc52qMXvtqx09NLactJ6E9oGLNPBVFG9a1L5P7/8A4BpxzE0gWCIoAGgAEhKVicI3IacEwOqnbfUfSU0+GMd1JsQOet9gB+d/xnRf8KYJcj8f7TS11sfnIubRZ2SIficOVOUi5F9Abi3r6desw8tiTzO/0k1qYYEXOl/1ea5+HqTYidzkXTIzkOnr+tZWq9Jt8TggL2mN+zn9W/D9c51Mi42O0ewWuvcYhLnN3ga1jltlVbg2te+/ynVJyb2COhTErcd4rCy31yEA3y8hmnWZJEGIiJ0CIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIBBvavWy0KQ6uT9Bb/AJTnXC3OdWAvaTf2vZrULMFVQ5JOpJYqAAPl95BMBxnusivTsTqGGoNudtx6WlM3qaKa0JmuJOU3ZQCNQLXP1G8hvEyoOhvzO35SRjiqFblAT9jI7xPitEfCb9ACfppIOd9ixRtuYysrDY/b8jMSvTAEuUMaX2pgD/MAfpeUY9rW0sfr9xJXRCxq6w1lK0L8t5c3MyKQGYAm3nFzjR032Fqop4zTxCqgJtoR3eljueenLTrr1CQj2Q4NaeAzgWNetVqNrf4si+ngRfx5yby5bFDERE6cEREAREQBERAEREAREQBERAEREAREQBERAEREAREQDm/tTs9bD0zqMpYi5UHxjQkagG0g3FsHQq4g1KauqMBalTphCrAW94NlsDre3IeZk49qAtXpH/pgf+bf1Eij03KgHQNoF6/2meUmpM1QinFGE+LyrY6/zachrtodZhYamKlS7EZV3uCQPMgb+Q2mTxPCVVFsjDIdQQdPIyjhrBzZfDUUfUc/Jh5StW3LbPYyO1XDENdTRrI1JkGZ2qUWyke9+6VVYaaAAnW2osZpcNgqrKL3I5HfTlNvVoa6r9CbfSXR4BmNhblJXzHMuUj1allfL0n1ct7upKg625C9rk2NtdL2O8qr1MzlupinUYowVfeFi5OgDbjL8R6en0cCHE6N7FHcVcYguaVqTg62zE1ALX5lQPoJ1aRf2b8EODwVNWXK9TxsDuLgBQfMKBcciTJRNEVZGabvIRESREREQBERAEREAREQBERAEREAREQBERAEREAREQBERAIJ7UcPdaL9Mw/9SPzkAx+OC5Dmy5bdDfyt09J1jt3hO8wpP8DKfkTlP/tf5Tj+CwdSo5IKC50LDXU9b7f0lE46mmlJ2sjAxuLZmzisQeuhsbbG97y5hqfeP3neAnqBbXe/rebTiXC64sTUTmPd6fPzkdNCqXsMmh1bb8JHKuBZLMtzfY3FeL9fOajiGOJisxI8R20mA/UnScSsdbvqWa1ewJ5mb/spWaniqKKQVrVKCMCAdO9Ta/z+vpaJVW7xwBtJV2RGbH4UdK1L7ODJ2KG9z0bERLygREQBERAEREAREQBERAEREAREQBERAEREAREQBERAEREAtYqgtRHpsLq6spHUMLH7GeesOjUw+Hrnx4d2psdr5Ta/z3+Ynoqc39pvYOpimOLwYHf2AqUyQoqgCwKk6BwNNbAgDUW1jKN0ShKzIRXwlB/dqFtNQajMB8iZhvRCDQgD6SM4l8RhahStSqU3HwupU/Q7jQ6jSYmJ4rUfrK3HUu7TQzcZxSzkDX+0wq+NNT0mCEY7zMwmGkrIhdmRg6ZHi/X1kg7KVxTxeGc8q9G//cW/2mqqCwAmdwfhFeucyKQo+KxsDuMoGrH0kJzUVeTJJX0PTsTF4djVrIrC4JUEqQQVJGxB2mVLYTjNZou6KWrbiIiSOCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgHKvaul8Sl+dJbfJ3/rOeVOHqeQE6d7WFUmi6sCy5kcA3K3AZc3TTNvOepSYkBQWJ0AAuSegA1JmeUrM0wXdNW/CRyn3B8MZmCIhZjsqgkn0AnQ+Cdh6r2bEN3Y/gWxc+p2T7+gm34picPgENKigVjvl9425Ftz5m+mw12wVPqMc/Z0Vml6L8/oshScnZEP4R2Md3HfZRzIJBCKDq1TlboL68+dpLju02Gwqilh07zKLXvZfW+7Hz0B6yLcU41UqApfQm5A5nqx+I9OQtoBNUR1P68usjUwH8mWbE6pbR4fnx9ubPaw/05QV6nkSah25xaOGUUh5ZWNx0PjnUOzPaGnjqWdbK66VKd7lD+ankfzBA4WKcrp42rhXTEUXyuhtcbEHkw5qbbTfQpQorJTVlyRDG4GEoXirNHomJHexvaulxGlcWWqgHeU77fzL1U9fkZIpqPnJRcXZiIiDgiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiYvEuIU8PTarVYKqi56nyA5m5At5zkXaPtpicUSFY0qWtkU2JHWow1Ppt67yLkka8Ng6ld93bmdL432swmEuKlUFx8CeJvnbRfmRIBxXt9icaTRwq9whuC4N6hHPxbUxbe1ztY9YK/7zwjbcn+k370xQpCkosWHj62Btl9L39bX+IiVzm9kevT+n06TWmaT57eRNuwuAQ4epoGR3sQwDByBdmYHe5b7CbbDcKwuCz1VRKV92JNgOi3Jyg9BvIT2Z7RnCZ1Kl1fUAGxD7X9CLA+glXfVsc4q1dUuRTUaICNzbU5BzNiSSBrtPGngKk6srvR+v4Kq2ElGblN2jz5mz412yIFqK5VN7O2jNyuq8hfmehFucgWJxz1CSTfqSdh+U3HGeC1KaNUq1UvnKgC5zCxsUPPbbkDcmab9lRVFWuxVNciLqzkb5R8R6ufCNtTofQo4WnhVotfVm/DdhThng0/EtUULEBAXY9ATf8AyqNTLzqlM/vayI2xAvVe/QimCqejEGa7GcVqVAUQd1TPwIdWH/Ufep6aL0UTXClL8s5eHv8Ar3IVMXJvuqxvVx2G27yr6mitvtVJlNeph3BUYlPFa2ZK663uLk08qi+5JsJpBTlDrHZP+z9P0ZniKlmm7m54fjK+BrpUS6VEsRfZlPI2NnRhzBsdwdjPQPZzjVPHYdK9PTNoy80Ye8p9PuCDznmzC41kGQgPTvfu2JsD1pka028xoeYYaTonsp4sKOJ7tWJoYrwjNoyVlUsquNgxUMLjRrAjYgSjNp2l1102efiIZo34o7FERLjzxERAEREAREQBERAEREAREQBERAEREATW9oONU8FRatU2GiqN2Y7KP1oATymxJnE+13HP8RxiID+4V1p0xyIZgGf/AFfgB5zjdlcvw9HtJa7Lct9pOMVsQyiqfE1nZR7q5hdEUfyqwv8AzM9+UxqPBWq0alW5suiqASajC2g6gbev0jirXrVW5s7W8vEZs8FxwUKS0+7Jyqbm4W5JJvotyNh1sLXmGt2uROmtW1f5PqFTdOlGNNGu/wAIfD0xUchTeyKNWZ7EjyFhrz2AO8pxxAqFRsvg+SAJ/wAZfxvEGq16LVCAtMpcAWC3cM9h5CwudTllhKBAvVurE2yAXdjc3yg2GW4PiJA33sbSpOds1TcU5Weab4dW64lGGw5qm1yF+IjcA7Kv8zcvWSxeFOUW791Rpm7hSRcWsaYIOq5dD1OswMFwusWULambA3PiK5/4Ra5cj4iBtplsFFXGsaSTh++upIUlT4URNWJIAu5tc20XKAL8tdNwScm9Vw5f6ePi6tTGVlSp6RW75de+3N6rjPFFqfv6g/drdKFK/vW3J190aFm5mwB2IimJrPWcu5ux+QAGwUDQKNgBoJmcRxHfVC1rKAFReSIPdX73PUknnLAWVwhrme/t1xNdlZRWiWiRYFOMkv5Z9yy05YxiksVVmwKzErQVyRiTP4LxA4aqtUHQFc3PRWDBgOZVgGHmtuZmCRKkkJxUlZlTR6mwtcVERxs6hhbXcX35y7IJ7IOLmtgzRY3bDNkHXuyLp9NV/wBMnc7CV46nkzjlk0IiJMiIiIAiIgCIiAIiIAiIgCIiAIiIBD/ajxr9mwZRT48QQgtuEuO8PplNv9U45QrZGDjdCGHqDf8AESUe0nihxGNen8ND92B52DOfUk29FEhque9RD8TLr89ft+c4z2MNTy00ufySapU8WYaHU/7r6feW1rM7KrElcy6H1A/DSfeQ89ZYrCVZUe/lTPmIYl3NtS7nz948uZmTTpZARYAn3rfh58hfy6b0HFio7AIFawNRgTfMf4R8JO5t185etYSKT2ZXBNpJq1uvIz8bxl6gIFkBAzZb3YhFXxE62so0Fh67yNcQqXKjoNfXwn85sqg0kfZyatQHZSh+ZQf0liRCpGNOnlgrF9UgiXBpPjCTMdi1aVBZ9EqEHGWnmFWmbUmFWgqkYrQJ9aUicK2dA9j2NyYxk5Vadv8Aabj7mdtnnPsPiTTxuHYfx2PmLE2+oE9GSqm7VJR+z89Pg8/FLvJiIiXmUREQBERAEREAREQBERAEREASl3CgkmwAuT0AlUgvtS4rTWkuFaq9I1fEzKpYZFOz2YGxPS/u6ixnG7K5OnBzkoo49XxGZ3c38bMxJ31Nwx89df7Sig+aqg8/yM21fs3WNPvaRSrT/jBIt/vysPoZqeA0DUxdCnaxeoFuDoLgi+olSrU5RbT238PvyPci0pLwaJI8xsXWCKznZQT9Jncfq01rVFpLlRDlA1N8tlJN+pBPzmh48S1IUxoajKPqR/WISzRUuZ6+fuZvAzeDqVoqze9U8beraj6Cw+UzgdJjs/iyjYf/AASqo9hJImlaJbxVYbek07t42IFy1vQWAFyflL2Mq6y1TOskjNiH3beJkUaTEgXFzYXOwv5dP1eSHtFQw2EzYYUWesoW9eo5A1Aa6IptzIsenOaXh+LwgJGJqOq28K01uznmAdl5b9ZMcF2hwdapSch1qkLSBZFLU1W5DE6qWJbcA77CZMTVnCStFtLlprw15db6GCb104EHzCfbyaUOG4IU8OhOdq9R2D5MuYjMvLVKYNvDzNtBra5Q4F+wJ3oTvsTdUpliBTztuVXkFF9SbnWwF9Yy+oU1fTXhfS+tt3y4nHURBMUjKSrKysNwwKkc9QdRpMCqJKTwCrXxQpNWDuwNWs4XUC/w5tCSTYaADpYTTdo2oCrkoKQqDISSxLOpOY3bz02Hu3ttL6eIjNpR1ur9X58CDZpjPk+mfBLiDN32PF8Zh/8AOT9EYn7CekRPPns5VDxChn5Gygc3YEAeQyhyfS3Oeg5TCL7WUuFkvK7+UYMU9UhERNBkEREAREQBERAP/9k=</t>
         </is>
       </c>
     </row>
@@ -4060,25 +4060,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ABID MUSHTAQ</t>
+          <t>SHAMS MULANI</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>smat2023_104</t>
+          <t>smat2023_058</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>212.5</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -4087,88 +4087,88 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M29" t="n">
         <v>4</v>
       </c>
       <c r="N29" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P29" t="n">
-        <v>7.25</v>
+        <v>4.5</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U29" t="n">
         <v>1</v>
       </c>
       <c r="V29" t="n">
-        <v>41.7</v>
+        <v>45.8</v>
       </c>
       <c r="W29" t="n">
         <v>6</v>
       </c>
       <c r="X29" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Y29" t="n">
         <v>4</v>
       </c>
       <c r="Z29" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="AA29" t="n">
         <v>1</v>
       </c>
       <c r="AB29" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC29" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AD29" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AE29" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AF29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG29" t="n">
         <v>4</v>
       </c>
       <c r="AH29" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AI29" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="AJ29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL29" t="inlineStr">
         <is>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="AM29" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYWFRgVFRUZGBgYGhoYGBoYGBgYGBgcGhgaGRgYGBgcIS4lHB4rIRoYJjgmKy8xNTU1GiQ7QDs0Py40NTEBDAwMEA8QHxISHjQhISE0MTQ0NDQ0NDQ0NDQ0NDQ0MTQxNDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQxND80NDE0NP/AABEIAO0A1QMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAACAAEDBAUGBwj/xAA+EAACAQIEAwUHAQcCBgMAAAABAgADEQQSITEFQVEGImFxgRORobHB0fAyBxRCUpLh8SNiY3KCorLCFSQz/8QAGQEBAAMBAQAAAAAAAAAAAAAAAAECAwQF/8QAIhEAAgICAgIDAQEAAAAAAAAAAAECEQMSITFBUQQiYROB/9oADAMBAAIRAxEAPwD0Ns7d3u7hQxuT3bm+m911GsM2e2a/dNja97gageFx8YaC3pa3v0+J+MFKa3BGgtYeAuSLeV5BI7sxTLYCwHwsD58pBTwtnfmraFTryvv66eUtgaePLx5fSCg38bH4SLBD+5gMuXRVvYcwTfTyk3n/AIvt9YQjE6+G31EhgaEogqIcgCEYxyNPzprGtAEYJEICJoAMRMf8+QjSCRW1hCDDEAYCKEIMAGM0IiK356wAIudo5EZ4AROnkYAjrtCAgDAQxGtCAgDxRgY8AFfl/mN/j6RX/PhGliBL+e6OPoPlHjCQB12gQ25fnlBMAcCEBGWEIAJ2tHjH6D8+MRgCjiNeOogDERARyIgIJBYR0iP57o6CQBDnGMIRjAFGEV4ryADGaK8ZucAKmNRCH3kYeP7SSA2G0e8jzwSYBLeKRZ4oBIYhGikkD3/PWPGOnz+f2jj7fKAOftAMNtPdAAgBLCgiPAHMAGFGtAFCAlfF4pKSF3YKo3J+Q6nwnnHaPt475kwxyJfL7T+NuuT46j0voTIPTDiEvlzpmHLML8+V5zeO7d4RHCZi1jZio0Xr52nj9aq78z12t7zKppHnt666xRJ7Kv7QcHfdwL2vk0sBvve03uG8Yo11DU3zBtuR9x2PgZ87VOua3Qf3k/D+LvScMrkEG4IJBk6kWfRztIzUnLdle1iYpcrWWqBqLjK/Up9pvu8pRJOakb2sqtUje0k6kWWvaQPaSuakWaTqCzn3jhpXDw0aTqCYNHvIwYQkNAUUUUiiSwfz890Rj25eMS6wQOdvzx0+MeCuscQAmEGODGgCX7/OI/nuEf7xoAoL1AoLHYAkwhMztNiQmGqsxt3dPO4yj1NhAPOu1HEmxL5b90XAA1vfko3t8T62kOH4AcozdwAWH82u/kZp9nuHZV9o4GdtR/tB+pmwaV5hPLXCOzFhTVs5z/4WmNwT5n7SpiOFJqBceRnTVKVpVelczOOSXs3eGPo42vwZRfKSPPUe6YGKwjI12XTrynoVehvM/EYQNcHYzohlfk554V4OX4LiCtVTmtY73Iy9G9DYz3P2mgPgPeRPCsRhTQrL0uGTaxsdtZ7dha4dEcG4ZVbTxAJmz55ORqnRKxiBiMaAFHWCIYgBLJVgLJFgBrCiEK0qBrRQgIosFgwYRjEfnrIA4+8UUeAIRiNPfG+kdt/zxMAcRiI8a8Acziv2g1Cz4egNmJdvHLoPmZ2l5yHbWn/9jCt1Dr8VP1gtFcoLD0u6PIQXNpPiHyJ3RmOwHU/aYGO4bXJztXCne1tAOgvt5zj12dnpbarqy5iL8jKhdukr4NHL2FdSNiGsT6EAfKb2LoBEDG0nWiYy2/DAxIaUjeXOI13fSll8zaYuKweMQZsyOOi6++aRjZlOX4DxrC56RI/UneX6j1nU/s8xWfDMp1NNyvoUVx/5W9Jg4Z89NswysAQy9DbceE6jsLgAmERudRjUProvwCzeLpUceTuzfMEw2EYiWRmK0IRrfnrDUSQGskUQFkqwAgIYjCEFlQOBFCtFAJesaPyjGQBAcumkIQRv+ese2tuo+skDRcj5b+MV/rFIAgI9vzzEYR/z5wSMJy3bQBmoFSCy1MpAIuM4Frjle06pZw4s7Ozi5SsmXw7y6CUnLX/TfBi3t30ahcDz5TC4twt3psG7zE3Vs7IFFiP0qbMdjc322tNyslwZl1EI5n1nMpUzucU0YeC4awZSFC5dyCTc3v69Jrcedig1l/BocpbTzY6DxkHFsLmTOHDL1Gok22yVFRVHFJnV73uNdNtxpYyOnh6oucxJuMpLlhbne+v+Zo1qWlxqBv4R0onnN7o5tbZJh1JRrizFSDbY6aGdr2dpZcLhx/w0v6qD9ZyFAWml2AqkvVpk6BUIHrY/MSYsyyQ8+jrGWDllhlgFJomc4GXb82jqIeXaOFgCVZKojKslRYbIoQWSKI1oaiQBWjQyIoLcCEbr+eUeM0FRCO0Yj88/8Rf2gCO8e17QIamAMDFENvzwjiQSITiu0VBkqOU2zLVI6jQG3kR8Z2gmP2h4Y1VSUtfIy728fWVnG0bYJ6Sf6itQqBlDDUGZfFsQqGxIVQLsedugmbwLiuVMr8v7Sn2we5psD3XIX3TBQ+1M6/6fW0WcX2jphQqDMPEXBF+Y5zGq9pKjo1MUcqakZEKjXynQcIw+VR7SkttMppWvlFgbluduhk2NqYcrYisCAbiyi5vp6WvLrVPon7Ps89HGHTuFQBf9IGUeZHWbXD+MrU7l9RtIuJuCLInS5ex5d46eMyUoIHTJcEm7dNNdPCa0pI57lF9nUioFVj0Un4TqewPDMlJq7b1bBfBF0B9Tr6CcB+9F2WkguzsEAvzY239Z7Lg6eSmiWC5UVbDYWAGnrIiqKZJ3deR3SAy7/nWSM0G+p/OcsYABISiIGOokgJVkoEFBJAsADLDVYVoQWSgDaKHaKKBFb6xjCt+esEiQQLr5fK8b8+JiHPz+pi6wBXj2/PSDHMBD5ov7wYRP0+VpBIMMQSYrwDybjdD2Neog0AYsD4HvD529Ji8S4mzeyvqqa26kmdt21wYdncfqGnibAC3wnBOmdSBbYfE/5ERqRq7jwdCnaMrTAVgCR5/CZuM43VsSee3dH50mJSo2cAm3Mdf8S7iKqWuNbW/PnGiTL/1k12UsTxZjvY325e8TO/emvmvyMLFgE+Y+N/8AMjp4cuQqjU+4dTNFFIwlNtncfs04Watf94f9FL9N/wCJzsPQXPqJ6s9XWc9wHCJh6CU02AUk9WIuT6mXjXlH2RZoe1jh5nrWkqVYoF7NzkimVUeTo0gFqnDkStJAYBIIQkamHJQHiiik8ghMFo5gmCBj+e8x15/nOJ/1elo3P1MARjudR4DX1/BGJA3I25mZvFeOUMPf2jgNyRe85000Gw8TYRTBokyviuIU6dvaVES+2ZgCfIHecJxX9oTAH2NNRyu5zHzsLAfGcViuJvWcu7lmbck6+AHQeEvHE32Q5Hq3FO2GHpoSjio/JVvbzZrWAnL4ftZisQyhWSmHJsEUXVRcsczX71gbeNpxz0mCXuFDXGZja/XKN29AZp9nHGelrpdlvtclHUehYj3yXCKTotHtWd1jMOWQEnkLk6m/mfnORx3BCDmp6A3uORN78uuvhrO9VLjWQPg1Olh4+Pn1nBHJqd8sakjyvE08pOYHOLDXp+XmVVq30AO3xuBv757BX4SjCzKCL31F9th75y/FeD01JsgHgPpbzM3jmiznlhkujg66k7Ca/BaNjfnz+kufuS30EnoUgsvKZWON3bLeF7bNTc0sRTsAe66c1v3SUO+nQzrMHxGnVF6bq430Oo8xuPWea9o8PdEcbq5X0OvzImLQxbIQyki3QkEeII2mkYqSsymtWe3h4QqTzvhXbN1stYZ1/mGj+vIzs8BxGnWGam4bqNiPMSHForZqpXlqniZmAww0iiTbTECWErCYC1SJYp141BurUhq8yqdbxlpKkUC8GjysHjyQGfvGt8zCaC2/5zlQMOspcV4ilBC7kAkEIvNiNgB0va5kHaHifsKRKsoqG2QNa9ibFgvO2vhPMsXjXqPndy56k306DoPCawhfJVsy+M8Ses7PVbOR3dQAAFJ0AGlpSQu4uFOX+YjKvqx0+MbE4lkZwtgQ571rtaw2Jvl57WMz6lRmN2YserEn5zWn4ITXkvVQgFmf+hc//cSo915FRr0lsQrOf95CL4d1bk/1CRUjfSQ1aXNfWTr+k7LwjVxRNQEk97Qjla2wAGw8JHwrEkErswIYc9Ra2nmAZWw1ZhuJJXS9nT9Q3ErQs9f4JxFK1MMuhGjLzUjl/eX2M8n4NxhqTirT1FrOh2YdPMcjPSuGcTp4hM9Nr9Qd1PQieXnwuMrXTPRw5VJV5LrnpOY4xTuST7uU3Hq8pk49MwmMXTN5Lg5opaDJsQ2thJ8FSFwTa3PwHOdCZi1RkcSp3psp8/qPpOTp0wwIvZuVyAD4X5Gb3HOIixRP1Hc/y/3nNTtxRaRw5ZJyLDUHQd9GXoWUgHyJklDEMpBUkMNiDYwcNWZP0sRfcbqfBlOjDwIlkvTb9SZT1psR/wBj5h7is158mdI3uG9saqDK4FQciTZv6hv6idTwTtNTrtkIyPyUkEN/yt18J5ymGVv/AM3BP8jjIx8jcqT4ZgfCRgvTcaMjqQdRZgRqDYyrimOUezCSKZjdnuMjEJc2Dro6j4MPAzXEzaoui3SaXabTNpmXKLSAaAMUiUxQQaDCQV66ojO5sqDM3pLDH885xvbjiZU/u6GwKhn6m+qr4bA+oiEXJ0Q+DmON8R9tWd9gbBQeShQB9/UzEZu8POSVaneI62lfEaZW9DOyqRQzeJ0jmdhybXyKqfnf3TPD39Js1G/1WB2dVPrcyhjMCQbr7pAKqtYgyc76c5UzESenU2gEiN1kqdQdY9gYgtpVkoS3BuvPcSTA8RqUXz0WysNwdm8GHOQsbGLEgEByLj+K2hHj4iVlFPhkptO0ddhu2Yc9+kyNzykMvmL2PpLmI7QUch71jbnPPMjfqR7+ekFw53A/qnNL4sW+ODoj8mSVM6CrxqmL5bufDQe8zNx3GKjgqCEU8l3O+mb85TPOYcgJCxPjNI4oxM5ZZSEdYOWPniLTZGTCWSrIkkjCSiAk1k7Yl8uRrOuy5hcp/wAjbr5beEgpxs1/ISKsJtF7hnEXo1FdDYry5Ec1I6Ger8Mxq1qa1E2Ybc1PNT4gzxlTOu7D8WyVPYse5UPdvsH5e/b3Sko3ySmeirLVFpVEmpGZGhpU20igUzpFALnGOIJh6T1n1CbDmzHRVHmZ5Hj8Wzs7sbsWLH15Trv2o4kqMKCbI1Ry3TMFAW/vJnDVqmpFt5viXFmbAxI5jl8onUMvxkNSoQAenxEnoHTSbFTNKXdjzFl9wv8A+0Isw31jF+82u5Pz0jtUEgko43DXOYDfeU2pkTUNaAXv/DeQDPo4m36pcDhtjI6tEHdCPKVzhmGqG/hsfdKsIsPVtoRDw1YbSBK4fuuLGBVoEd5dRIZYkxNAocybcx0ip1ri9pPhq2YWMr1KViRykAY1IxeCacbJAGZlMEqITID0gCj0MlFQgI6yOxENYAZh2sp8oCw2OhlgQiHScjUGxBuCNwRsRAJ0gKdvGVIPYuzfFhiaIf8AjWyOP9wANx4HebCGebfs6xRGIenyenf1Qi3wZp6SswkqZrHlF2mdIoNJtI0rZJzv7VV9olNR/Czm/R+7b7e+ee4TFh110ddGHMGeocVwQrUmQ/q3B/3ePvI9Z5bxfhjK5IulQbja/n94+LmUk15RfPhcKa6DaoQf5l+PrCp4gKCRqADtv5TIGPZTlcWPX+8J8X4jx5Tss56Ej3NwbgyyAOZlLAOC4RP42AykXGp3Fpo4rBLfut4g8iNwZVSV15LOD128DplEsYWi7tlpoznoqlrDqbbDxMymR10nWYSoqJhKdRmWi/8AqVspIzBqjC7ZdT3QB4CJS1Qik+/BTfs/iDsgJ/lFSkW/pz3mTiaDoxR0ZWXcMpVhfY66+s9Y7TJiBSy4N6C4d0yKi5EdrixyMTZr6bWOs84xtdjhqeckn2lQLmvcKqpdddQLnaZqTb5L1FptGHWoq48evOVqdRkbK23Iy1VBGogNZ1tzEuZEgUHUSN2N4GFYg5TyklYc5BYjRbztezPZhBariVzd3OtNjlQIBfPUJIsDdbcrNfU904XZjAiriKaMLrmzMLgXVQWIJO17TtOK1ketRwlRmVKuZ3IZQc7FhRVioC2DAmwFiXvyEhkVboVTtPhKZyIxKq75TToIEytoqsGK58u48hvzp47h+FxaF6bIrLlBqIMjKxAVfbU7DuswPe/3aHS067Ddn8Nl7tFLWtcopN73B1G4GUTmePYfD4RkxFNMjFlpmmhsjIwvVBXn3efUg7gSFJdF3hpN30edYmiyO1NxZ0NmH1HUEWIPQiNkB2nVftE4aEajVFyXDIzMoGYoboRbwJGuug8JyFN5cyCNOA50krvpKVer0gBo9wQIBbXyipCwj011gF/hGOahWSqN1YE+K7MPUXE9sU31nhVCmXdVG7EKPf8Aee1cOq3XLzWw9LaTHJJKSXs3hBuLl6NGmdIoAaKVIsYtMvimAp1hZ11GzDQjyP02l13lOrWnl007XDPX46atHHcS7MuL5Crr0Pdb3HT4zn63AnzW9iAT1tb4Gd7i8TKuGTMcxnXD5GXp8mMvjYWtuUZ/AezaIyl7M1+Vwq6bDr5mWe0+ECOhUWzKQendIt8CJt0Kf3lTtdS7lJuQLL7wp/8AUy0ZS/um/PBSSX8XFeOTkHQHlO67GcIw+LogVrs9AZMgYr3C7OrG2pFjb/pM4wiFhsW9J86NY2sRuGB3VhzB6T0ZxtHmp0drxbH0cLWJoulR/wDTSnSRc7IKalRSDEFVQuQ5IObQ+Y8943Xu6UrhvZAh2H8VR2zVduhsv/SZrY7jClCaVPJXYEFybhFta1PmGP8AMdR56zjlfKbETKMX2yzaSpF99rTPrUmU5llkVAY4eXKFNK+tzvLIqgxnpqeVpGaHSKB03YvF+zxdJtNyovtdlKi/qZsdvKLGtTxDgEOgV7AqudO8R4XRkI579DODpuysCNxrPTOCccp4ymaNYJnNsyP3Q9lYBkYbPcqRqLd7kxhcOw+Ctg+1jslYKiIKdAulrt3w6IC5Niw7+x+M53E4l8diKS5ArMQhyk5bXuz5TooADE25CdXU7JoqVKaVmAdlBZkDEIjghQQy3UsUbMQB3QJJhsJheH03eoe8VWzVLFnBZg9NEXVbWHO9wLnLvFRvhF3kbVWY/wC0V0yUgtru9SpcE7WVbG/MEsNuU8/apNDtBxh8TVNRrgWyopNyqja55sdSTzJMzLch6STNGjgOHe1pu1zmscltri3LnfUTFUnbY8+t533DMKEQKOVh5ncn3mQ8V4ClTvr3H/iI2PQkdfGYrIu30dLxcpLs5FU03kirpYbczN+h2RqE6ulutmPwm3gOzFOnZqjZ2G1xZb+C8/Uyk/lY107Lx+Dlk+VS9md2Y4VlP7w4sB+gH/y+06vheKtU12bQ/SVMTUvpsBsPvIFaxnKpylLZnVKCjHRdHa3ilfh9bOgbnsfMRTps4NGVK9aZ1fESLE1je0zatUzhUT1iY3drCbGHoWAAkHD6AChtywuT6bfGaNMTeEaMck/CLOGpSt2lwmbDuQL5CH/p/Uf6SZew0mYXVlOxVh8JGV66teykFey/Dy9pE5kzDQSpVM9btHmCYypiaIbeGahgsYBmVMOy7ayIVGE0ydfORVaY6SrRBWSuDJUeQvREA6SoLntIwe+0rhryVDpBNl9eNYlRlXEVANrB2+8zsTVZ2LOzOx5sSx95j3gES2pBDaWOHoWqoAL99SfIG5+AMhadD2VoqQzW7wbLfnawNpjmlrFs2wQ3mkdHh6ennrL1KiDodjIaI0HlL9ATCC+qN5v7NlKlmRsjctj1HIyy5uJNxCiCmbYpt5X2mclQzlnDV2dWOblHkZ0kDixlsSDEiRFl2i9w3G5QQfD+8aZyGKa7MwcEf//Z</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUSEhMVFRUVFRYVFRUVFRUXFhUXFRUWFxUVFRUYHSggGBolGxUVITEhJSkrLi8uFx8zODMsNygtLisBCgoKDg0OGhAQGy0lHyUtLS0tLS0tLS0tLS0tLS0tLS0uLS0tLS0tLS0tLS0tLS0tLS0tLy0tLS0tLS0tLS4tLf/AABEIAKgBLAMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAFAQIDBAYAB//EADwQAAEDAgQDBgMGBAYDAAAAAAEAAhEDIQQFEjFBUXEGEyJhgZEyofAUQlKxwdEVI2JyBxaCouHxksLS/8QAGgEAAgMBAQAAAAAAAAAAAAAAAQIAAwQFBv/EAC0RAAICAQQBAgUDBQEAAAAAAAABAhEDBBIhMRNBUSIycYGRBWGhI0LR4fCx/9oADAMBAAIRAxEAPwAHRJKlLiNpS4emrYaOK4EnTNfoNoZjUHEkKycycVXqNCr1GqJ2VuLRsMozG26MuzUAXK83o1S02JVz7QTuSo5OPRbDI65D2YZ1qkBCaI1PCqalZwb/ABBVScm0PvT7DTBAQHOKvj9P3RvVZZzOKnjPQLQ1a5KmUzfdSNw4KoGtCnp4pGUZehVY6tg1Rq5eVYzDHaKbn78B1Jgfms/WzOpIJduLEzA8xHqr8EJyV2KEfsbgUjcU0O0FwnaJQpmbVIPiPWT85NlXY0gDQ/e5uD6EBaVif9wDVNqkcDHMfsp2HULfXosw3E6IOpzXWJ0mxV2lmNRpiA6RIPW+/L91VPTuuB0GmNMqaELGetHxsIvB8jMIjQxLX/CZtKzzxzjy0QkDJ4JPswT2lSU6gKqbYUyo9oCrmoiNQDgoDRCaM/cDKYJTmuhXmYNPdhRCbyICRQ+0BSMrAqKvhI2VYSE6p9EYSDQlICoMrqVuI81KZCcwpGPVc1Qm94pVkJMQAqD3gFWH1VSrtnZWY+AMs08UFcpVgUIpUSimGZCadALICaU+VHCqTGofQepTXQ51TkUw4kqlwsssmq4wgqI42UNxFa+6iZVVqxcC7g1TxEqz9ogILSrDcJa2JsleO2SwyzGBW8FiPEFjPtpndFcox8u3Rena5ApGyq14Cyma4yapg8ke78ELLZgwd670/JWqPHJJMka5disUKbdRF4sOahedLS6dhP7oNjMwIfpd4gYg7b8E0MakKies/v5DtQAE77+cIHiWgGNbjG3NXaOKe15Ak9PiH0FXxGGLjJI6WB9gVsVLoAzCsc6zX2i82idwQrVHLX7Az5t291HRbp+7B5zv5lNNd8+GxP4Zv5W3UDQzHUajb7gDcQffTKbgcweHiHcI4iRy+asYek8ulzXHmDqE81Fi8vJdIa4CeInrcIboh2y9i+7HNLnMdcEzxEOgA9Lz7qCnjzQqS12ppFxtI4yOBH6IfXpvvra6bnVx538lXqOm/HiPPmOqNJoDs2tPPmkHpwO/0IUzMcS0EWnksRhKt4O3HotdljRpAJ2t6TZZ8mKMUROy9RruPFX6FXmqoe0KKribWWVqxqDIxQCZUxcoHRxBKvsEhVvGkEkqV1Wc+VIaMpRhimVIWmV+7CY9qtxCUp9waBrnELu+PFXHUgoXYZOpIVojFUFTU6aruoeSmoNKj64IWAIUrKyjKr1pCRchL4rKdtUICazlPTq2TOAbGOKgqvMbplbEqAPVigNSIqrSVDBCIMhI5oTqQu0qU6hUhqEqUUgntpINoFFJ9NS4BpD7K73IUuCw/iRUwbQhSqmFQfUl5lGvsdkFqM8Z6pZNNDbWOqbG3BZV5BOl52jhIE3i11rKzJaR5IJTy3WQHC7j5gxe6bB0wUUauJJcPvEfC9oLXdDzVk4yqBcN8y4AH1jitSOyVh3IDbAkvcSNhMCLX4ojkPYprTrrkOO4AmPfdB6iBqjpMhk8ry6rXMNpk23iAPO25jmtrlHYqIc4+oAno38K2eBosaA0NAbGwHtbkrjlTObmu+DTDFHG+uTOU8ipMENpjqRJ9yoa+WUwPgHstDVsNuiF4p/qeSzSVGyDszeKymkZ8Ig9OULC9pezvdS9lhI+a9LqttdA8/pNqtgj4Qb+fD681bgm4y7KdTijKPR5bRw5DoNrwj+SYjwlnL69lSxLBNtybcvr91awbRTbzcdz1uujk5RxEuSfEYog7qSjWlDqz5KfSfCRwVEs0GGIU1TEgIAcaQoKuMJVPhbfI6mqD7MxEq83FArFsqmUVwtbmpPCkBSDLqyY7EqqawIVas+FWoEL78QEjcShIrQpaVUSneOgBqiZVplJU8JXbCtHEjgqJWWJEhPkoKjQVHVxJVR1ZGMWBslqMCql0KzTuuOHVidCgfSpWsXoWGy9jxMBRZn2caWEtEEAxCKyuXobHhr1MGQUgJU1RqZoT2UuIrFI0p1PDEp7sKW8ErYFFjZRPKGS5CntKMdnQdag6iaT7H4dlj8xYQ9x2uV6E1hhY3OKBLndSq99Oi7xWgK2uVJlc1HANB3EnkAbfkp8HlZqGNbGXDQXmAXGYA9kdyjKXUKvd1AA7TNjIcC6xB5J5ZKhKuwYsDc4trgN4Vu0cPdEaYIQjMHOa3wkjaS3cDiQs7WzN0O7pleoRab29zKxY47jp5cih6HomGqjiD14KV9bUdI3vHQbleQ99mEhwNRtyAJAPtK1PZR2LqPirI0jw3+Iu3JKvlHYuzPCW98qjYuqAg7GAflZCse+LRA+rLLdpK+Lo1HU6UjvJJA8Rm06f26rMOw2LJD6rcQWmbhsm3kYPFSOPerbDLN43SVm/qkkHjHJBMSYDha87+aCOqgWDqlNxH3muafUgwiOGc5zJdw3PPzS+PZzYfNv4oymIonvgHcBKsGkrhwwL3veYaCGjmYE291HiaQDvDMEAidxImD5rcp3wcyWNrn0KjqATTSUxXBsprK6KxpJvcIi3Cpj6EKbybSq2iFKBCk7pJ3KVtEo5rilcFJToKR1BI5KyUU+6XCmpXiE9lGUdxEhtJxVlrio30YErgUr5GonBStpLqLUUoYcQgQhwtJXRRCloYa0qw2gqp9l0IqhOx1ZxDpJN/0WwxDfAehWP7Gn4uv6LYYl/gPQrQKeV1KN0tKhdTPqrhVhV2x9qCODoBSYmhPBUaGNgohhMUJkquVrktSXRTGXEnZGMjwWl2ympYpqmwmMbMhVrJK6Y7xxStGnoYcQguZZS1xNlM3NgBuhVbtEClyJtqhsclHsTLMsa0vaQDcOE8wHD5SCnY8RiGQ0tY1rmA8NUg6ROwgEqlWzsamuG4N/McQrvaCr/Ko1WuJHetMk3DS0gA8zcCVPG7T9y6OaOxr2/wA2GMG5pFxZT08lp1DP6IZgK7SIHCxRfD43TEKuO1P4kXNWrixr+zdJg1uDYaNo/OUuW05dqaLJMUalQkuIDW3INtXIdEDw/bAtquaKVVoaJ1FgI9ACT8ldSk+E6Kk9seWrLvaHD31xcGVDh8kZVYHAmDuASL9AhON7Z0XPuHuB+IhpPy/ZFez+dsc5zW2BGpvnzsfRBwa7XA2+L6asX/L1Fh1ESRzuh2f6S2GiIm22wRzMMVIWQzvGNbTcSbwQEMa3SoGWoRsz2Gl3eAgRqIB6nZNxQBeSNpt0Fh+SJ5Vg9VJjjuQQPIEzPrK52WOk2W1R2ts5k57kooDGkpKFJXcRhy2xCiaQi2VEzGCFVqqwXWVR77oRiRisYnlnkkY5ShyO0FiU2qRwlKxSQErig0UqlCVNh6SdUcAlw1SShXAypMtfYdTVGcshGMM8QnPqBVpst2oE0sHCu02EKwyFco0gd0eQUitQnkiDKdlbw+HapjTASyiOmQZLloZMcTKMV6PhI8lWwtSFadWsqFmdB2GP/gYXfwQcloSE1V75BbSM9/Agpm5MEdCcj5JC7kAXZUn0Ms0o0kQ3yJvSBj8DIVQZKEeSoqUib7AByMclXzPKXmi5jS63ia2eLbiFqAuLUyySTsFpmEyDMCSACfu6p2mzb+V/kjOIzRzab305c4A6RyuZd6AH2QDOMMcLiHbaX+NscJJkEed0zH5wXM0N+80z68LXuVrlhbknQ2PUJQavkt4Z2OxHiBboBBAc+Cdtot+Su4Ts1VJJNM3mzKo1A8wXNjabKHIqtRjAxoIkwCWmSSYG4AgBT5nhMXSgsqy7fSZDuU+G0C/so5PdRbGCUFKSbB+a9nK7QHBjwD8Ie9hfO0+EoZ3uKpkfySA0eJxiY43adrbIsRinPitVDCCJOuSLc9hzlUMwqaNTW1C+Tck3Jjn/AN7qxbm6Kcjx/NG0W8LnNSpTdPxAy3zEW+vNBsU91QikLuc4MbMRLtiqjMSWggE9Dw+v0Wq7G5PqP2moJ37vqCQXIygsacjO8znSDeCy0Ma1v4QB7IgMG3kp1xKxeaXqXRcQXjssa6LIe7IhyWklKp5mPtiZZ2RhRf5fC10LoHJDzSA1EyP8AHJKMhWsLV2kclPNP3F+H2MsMiTjkq1EBdAQ8sxuPYyL8hlPoZFC1enyS6UPLMKjEBU8tgJpy5HiEjQnU3RHQCGWlTswZCMhoS6Qp5ZApFKkxwUhYVcDQlISubHSQxoUgVMVE4VVl3GvxItaAk7tVxWTu+R3MDwxJdASaVEaqb3qlsHhiS6UmlM71J3ia2TwxJQ1dpT8Phaj/gpucOYBj32RjCdl6zvjLWDrqPsLfNXQxZJ9Ipn4odsCAKPMqnd09RcGyJDjHhBcRqvawa8+gW5wvZmiz4pef6jA9h+qA/4g9nu8pEtADdAaYFm6HamPjkCTPkZ4LqaHS7clzq6dfX0Odqc0XGoff6HmBjFPc0McKQk96fic8ECQDfabn5bI7lGUspjwsA8zdx6u/ZD8npCkzSRB1O1dRAgomcyAdIGyzZskpTcWem/T9HGOFTSTb9fb9kXfsUvaBaXCT5blPzpxc+1ogetyfm6PRTYLGgh1U9AOvAfIKClWa55fPhYSZPE/iPkLlZptLo0XLdcl0v5M72swYLnClZ7WDUODo4gfii/nKxYxBiNtwReD6dCtNjMyLqrnxdziY8jsPZRjANDiQ2Cb9NV/1WvFl2xpnG1+kjvTi/qAKdI7kTx6ki5M9Fr+wtdzXnDvJLaw76meTrh7R10n2CDY5oC1mRYDTSwVX70uaOjzq/PSP9S26X+rLbLppnJ1EPEuPQ0uGy/WDEtOw1bSqNVhaS1wgjcLaYaiynTfWdswEx/aJjqbId2awZxFJz8QNUvJpk/dBu4A76ZtHCFXl0KnBzhxX8i49RtdS5MzKWVtX9lqBM+MeQdb5glUsZ2VbE03kHgHwQfUbeywPSZUaVmxsy8rtSmxeDfSdpqNLT8j0OxUBWWVp0y9QT5R2pOBTYSpNwyxjpXJFyG4OwdKWU1cSpuJtOcUyU6V0JlkEcButIKhUmhd3YU3hUTm1FxqJQxd3aG4bgqgJwCla1O0pRviIYShqm0J9OkSQAJJsANyUyVgcmuyJlOdkTwnZ2tUvp0Dm+3y3WlyDJO6Gt96hHowch5+f0TgXTxaNVc/wYsmqldRMvheyLBd73O8mw0fqUTw2TUGXbSbPN3iP+6UU4pALrZHFCPSM8ss5dsDdpcAa1EgfEzxNHON2+3zAVjIMw7+g15PiHhd/cP3EH1V0blZ7smzRWxdL7rajSByk1B+QHsta+LE17cr78MzviSfuacFNewEQdl30E5UFh572m7JOBc6iJBvo4gx93mI4biOKw78O8u7uCCPiJHwhe8ObNis52i7NMrAkeF/4hMOHJ8X9VRnw+V7rp/92dXQfqk9NDxvmP8A4eX5jmQaG06cmLDzOxP5j1Kix2ZMp0hSBBc69SD8pHnb0PNbF3+H7dOoP1OAu1rrnybI5dEPoZHhmunu9R/rv9bLnzwKHEjox/UPIvgMhkuWOqO717D3bb7HxnkPLzVvEkkknc3K3D3DTAtw5AeSFVKUmA0Eny9o80sp9JIrpzblJ8mNOBdUcGtBc5xgAXJW/wAnwkmgyQWYWmGaxtUqWL3N5tlrYP8AQD95Ff8ALQp0QJDajz/MgeLRF6bSNhtJ4ollmXSQ1ohoHt/yuxpf6UNz+Z/x/s4ermsk6j0v5KfaGvpwZb+Oq1voBr/9AtBllDu6VJnJjQesS75koL2xw3gosGxqlvq4W/VaksWmb/pRXu2zKl8bGymvZMdVIwbpwWcsK9eg17Sx4BabQUAxvZenpPd6w4/DLgQI522WmTWi5STxwn8yGjOUemedNyfETp7p89Lf+W3zVRzCCQRBBIIPAjcL0+ryG5sP3Q6vkdB5MsublwJBnnvusU9Aq+F/k1R1b/uPP1yPZj2aqM8VP+Y32cPTj6eyBlsWNo3B3C5+TDKDqSNUMikrQ2F0J0LlTRaIGpwaklKHIEHaVwakDk4PUJQulNITtaaXoWCiEFOBTmkJdQVtBOBWx7L5VoaKrx4nDwj8LTx6n8vVZ/IcGKtZrSPCPE7oOHqSAt+F0tFhXzv7GHVZH8qFSTB6pUjguiYh5TQuaU5QhEwbnmUNyfBFj8RUcINWsY/sbIafUl3yRYBNdxTKTSa9wNHRwSj5qv35cT3YEAwXumJG4aB8XI7Drdc2q4O0vid2uEw4DcQdiN4/5hQllckK6VCDKlEHhdAs4yLvJezw1OPAP68j5rQpUk4KSpjwySg7ieX/AGZ+vQQdUwWx4p5LRZdlzcPD6t6m7aYixPFxRjGOYKhewDvC3Tr5ATt533VXDZc57tRMDmdyeaox6aMXb5NOXVymqXHuIzVUdJ35I3h2aWgeV1GKlNg4NGw5nbYblCn9qaOpjZjW8NGuWky4CWt5QZkxaOa0OaXDMiTYTx+CbVDQ77lRlQdWGfmJHqrRQEdowazqbKZLWvNN9Rz2Ma0tMOs4yQL9eCL0sS186HtdG+lwP5bJ7dBljce0TNSjdNJ4rmvBNkBTjuubuU15ukqPhpI3j5qEG0ju88bN6cPdSbdSmwGgTs0AfKFwMf3HhyChBXC0KhmmU0qvxCHcHN+L/n1RAD34nkoq1UNBcSA0fE48EJRUlTCpNO0YjMslqUiTpLmC+ry/qHBDdC22OzFkPaxhrkMY4wRoioXhtxNv5buHEcJIz+MyysTqbQ0ttAaSbETMOM/kb/DaTzdRoWvih+Dfh1afE/yCtCUUk5xIMEEHkRB9iu71c1qjZuR3cru5ThXS98loNoZ3KaaBUprpn2hBk3IHNpOUgpFXGuCexkkAbkwOpV6k2zPVGl7EYaKb3ndzo9Gj93FaUKpl2CFKm2mDMceZNyfdXBPVd7HHbBI5k5bpNnfJcUsJITinSlJTSuBUILKr44kUzBgmBI+7qcGl3oDPopHVWixIBN7+g/UKvicaPh0h4c3g5t5JBFz5et1CAapmzw4tA7trSWtEQIaS0Xjc6TblHNS0M5D9LT8YqU9PmHODX/7HOVbtH4aNUxqhrrxJ8JIkuDhcWOxO0lYhmYQwP1jVbY3kLmY45cM7m7593yvo+F9jo48ePNBpcM9gCRh3VfLMT3lKnU/Exp9wpnmD1H5f9rpnOJFWxrz8I479Ercaw21D9PdT6UA1XZBhsK0CYk8yn4h0CBxOkeqmQzOcD347ouc0RqJaSLyIBI4G8qMiq+QN23rtNJtKk/8AnarNYTrLSIcJbdo+EmbWXm9cFpLHNhwPiB3lsgzzPut+7Jzhw4hg0nSAIHB4Op1Q8v6t9PsJzZgqtoMZQe/XiZfVa2YptqOY9jqg/qc93K0rFizPJlcXGuPz1/n6fU62lzRw1GPXvxf/AHHXf7mSzDNK7oBeSAAAS1si1gXkSfdaP/DfG6sW41HjUaRa2S1pJ1NgWjUYn2RztK2aBw+HbhQHSHNqGC2wDXMF/EJ3NxaFWyXLqTMTSLq9N7KDNFAAHvHONtTzEOgkgQeAHArV45KV2Xz/AFLBk00sexRdcV3x9vV/T3/Y34uontvbddReHNDmmWuAc0jiCJB9lDU1A2v5cR+6sOCSVHLqjthzIPzuoXVrEmR1Cic8lzGbTPqBf9FCFoeJ08Bt5nmpW+Xq5RRPh4KY8goQ7ew25pw+SRLKhBjaTQSQ0AncgAExtJG+590pbzunJQFCAjN8mZWE7PA8Lh+RHELH4/L30XaXjfYjY9D+i9I0oVm2cYekC2oQ48WAaj6jYeqy6jTwycvh+5fhyTT2pWYPSl0qXGZjhy492HsB4Ogj0gyPmnNgiRcLj5MTgzbz6ohDEndqxCaQqtobKzCpWzNt+HXguXK+CuQZPg9Hp6gAD4rb8evmn+E7j3CVcvQHJODW8LJ0+a5coQQlRvclXKEOfTad2g24gG3JU6uXmDpc0fh/lght5AjiL/V5RcoQA9rMG5mGqFzg7WWtHgAIJcHSSP8AVyFx5z59Qw5u1rHOceQsPVcuXP1Unvo6uhS8bf7m27OZs+lTa2oHTTENAd4XTwcDytcKPNM+c74j/a0bX8uJSrkvmnKlZYsGNNyoK5FltaqG1MR4GiNNMWJjYu5dFpcTiG026nGAPqAuXLc1si2jmbnlmkzL5h2o0ujVp/CBcuPAHz8kRwmZlrO8qiKj9mDeG8Ty3XLlTjySabNWXDBSjFIq4vNqtR5p0gyQ1riCTY62TqI4adfDcDdQNwtWwfUEB5cA1sGwIaCQQIBhxtcylXLTBtxMeaKjKkKcBTLtWgSCXN3GkuDQdMbfDPUk8VIxlNgA0AAEEW4gAA9bC/kuXJyovYXNWgaSDbaB8oCfUzenxa6ekLlyVsJWdj2OtOnqLH1SYWqJNhIHhdyB+KPYLlyBAlh3WlSteuXIkHgrpSrlCDgkrV2saXvIa0XJOwXLkJOlY0VckjIZv2kNSW0zoZz2c7/5Hz/JZjEYimN6jZ5Tf2CRcuY5PI7kdyMFiVQKlSHXBkfXNRUa7qZ8JtyOxSLlXLgspTXIbwmKFQSPUclKuXLNkioypGU//9k=</t>
         </is>
       </c>
     </row>
@@ -4187,124 +4187,124 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>AVESH KHAN</t>
+          <t>NEHAL WADHERA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>smat2023_108</t>
+          <t>smat2023_135</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>225.9</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="M30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>6.75</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V30" t="n">
-        <v>45.8</v>
+        <v>0</v>
       </c>
       <c r="W30" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="X30" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="Y30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z30" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB30" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC30" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="AD30" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AE30" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="AF30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH30" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="AI30" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AJ30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL30" t="inlineStr">
         <is>
-          <t>Bowler</t>
+          <t>All-Rounder</t>
         </is>
       </c>
       <c r="AM30" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYVFRgWFhYZGRgZHB4dGhgaHBodGhoZHBoaHBwcHhocJC4lHB4rIRoaJjgmKy8xNTU1HCQ7QDs0Py40NTEBDAwMEA8QHxISHzQsJSs6NDQ0NDQ0NDQ0ND00NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDU0NP/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCAQj/xABAEAACAQIEAwUFBgQFAwUAAAABAgADEQQSITEFQVEGImFxgRMykbHBB0JSodHwI2JygjM0Q3OyFKLhFRYkU/H/xAAZAQEAAwEBAAAAAAAAAAAAAAAAAQIDBAX/xAApEQACAgICAgAFBAMAAAAAAAAAAQIRAyESMQRBEyIyUWEFQnHRFCMz/9oADAMBAAIRAxEAPwDs0REAREQBERAEREAREQBERAEREARMLV1G7D4iYX4lSUXLqB5wDciauHx1NxdXU+R+k2oAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIia2NxS00LNewF9N4BqcW4wlBSWOoF7XE5d2l+0us10oU1VdmZjc28CLW/OaPbLtX7ZmVfcvoTluNxYgnQHx+EoWIqk373dtptqD5AXlXssqRLcS44+mV+8Tcm4JHhmEj8Rxiqw7zu1tNSSvlaaq4YgXvYkaEjS5BvqdDy+M8YhTe/JQBvfYb+sJJByZv4fjTqbqxW/LX8jylt4T9ouJoqVze0ANu9c2HUG+uvWUjJbunQjY21t1mEZk7w5H96RQs7r2Y40ca4Ac5l7zNc7ae4NrctdvznQhPzdwDjFTDFa1JsosQzKoJFzzB+7cbS0U/tAxKsG9opUWvmGjjS+mtrX5Qmg0dqiRHZ/jC4qkKi2vpmANxe19CNwZLyxUREQBERAEREAREQBERAEREAREQBERAEREAShfafxb2dH2SkAuCXJJFkHLTU3PIb2tL7OE/aq5fHsrXyoi7W0BUW/7j+clEMoeJqFz4XvsbnXnPLUjbMRp10tbkLczJbAYMuSWOZUXTLpm+6tr7Fj85O8Y4XkyIEGbLmOndLEDS/LcaeImbkXUW0U2ojDvBSLaja41H6z1RNiAx594decuj8MVaRdhcINb8wdHJ+Nx5TU4NwFK5Z2vktZT1YaX8gAJHNVZb4buiuJRzG97EX13sACVv4Hb0Mw65TdbXAtcai5AIv01k/ieHAkUgCHDMrDmVHeBBPQbTPg8GajMEADrZCt7ZrkEFb8iAOlpKkmVcWiAwpemQjaA3J9bWv4aTco0xmAChg+mUmxVr694bdelpuYlClJKhOazsDzawRRYnncMd+kjsqp30J0ZCpvyZAbHrZrjyIk+7Hqjsv2d4SpRGVQTRdb3a2ZHGtrjRlIOh1l+kF2NxXtMFQewF0A06jSTssVEREAREQBERAEREAREQBERAEREAREQBERAE4Z9qlIHHN1IS/iAo0ncpybt1w8PxJSfdyKxHkAJDdKyUrdER2e4SECu5AUWYKQdSLZbgb23mfHUS2Iao6EL90EN3idSbC4DDSyt19JNUK4VrFguml9vDbWaGIxWHcBHruQt7qO4rkm5L27x15XAPSYJ2b1xIitiWxhOHohlpbVqjW90G4VR+Ikb8paaGDSmiomiqBYb7frPOAeiFsllUdAPpMlGxca6dZRv0aJeyrdpMI2Y1E0IAA89Tc9NbC/jIqniMlWjiTfJ3Q7A2ZADo1l2AuVPgZfcSyA8jNRMPSJIATI4sUOUgPtcdAdL+njLRZWSRWeKYFRTxKE90sXpncd3vgAjcMv16SqIjGmQdCtrDpbT9+Uu+M4a1G6MGyFMtjrkKklGsdQmrA25N0lR9kUzDWzaW8Rf4ibRkYSid6+z6nlwFAH8MssheyNLLg6A/kU/EXk1LlBERAEREAREQBERAEREAREQBERAEREAREQD5Ob9pqivjzbXJSAJ8Sdh8J0LFMQrEbhSR52M5VgqAWrkNTOyoodjupLMcp8ryk3qjXHG9mlxnEqmpUlrWAAuT5DrKlj+GsxJcpTYjNld1DW8VF7es6PxTs+rqG1LAXAuR+YN5Q+IcHpllUoyFdGyC+Yc73N7nrMouuy8rfRA4KtUpuAGI163BEuqYirkzakW1PKML2fWsQ9NMgFhl5AAWJPjLVxPhn8EUkXXJcgbmwPOVk7LRTRyjiPEarsQHNidAJ7o0qlOzO7Id7EMPmJLUuDplZ3YqLEAre4JGjadDykfh8K6kn2xZzYKRfQDTZtPSXTVFGnZZ+D8WZwFeoWsNj+/Ga3EsIop0W21sfPUfSbvAezLh8/3W193KeV9Bp8JuccwoU00C3vUUhTa2Ynbpa/zkJtSJatUdU4Xl9jTykEZFAINwQFHObkp32e4iqyYhKp1p12RQLBVVVAAW3K1j6y4zdO1ZhJU6PsREkgREQBERAEREAREQBERAEREAREQBERANbGtamxPQ/KcwKKmINt3Fz5hv0InUsSmZWXqCPynKe0iGlWpPoCWZGUDkQLEn0tMci2jbG9MtyVFZB1WRtTAo5uwvr8ZGYfiVp8qY8nQc5i5G0Yk3haoVmRQAOijTy0mzTcCqLka3Tcb5f15yg9pnxqhfYMyrbMxUCxPRrys4rj+IAsbh+Z5A9RLRTasiTinRf8AG4ELUKlbBxe3K/O3SxnylwmmjB1sbciJVOz3aDEMVp4hmcHVCVPd31DW902tLHU4iAb3lZaZaLtFtw2PVFuR3rWG1gJTu1OV1IY2Bza9DlNj5A2MNxbNzkdXrmpVVAoe12ZD95NAR8Df0lk2ytJM6R9nVO2DRj7zhWY9TkQfICWqRfZ6kFoLZcubXL00At8BJSdEekc03cmz7ERLFRERAEREAREQBERAEREAREQBERAEREASE7V4EVcLWFgWCFgba3XvDX0k3MdZQVIOxBv5WgHC8Li72DGx29ZmxfEhhwGOrHbp5yAxj/xqig2KuwHoxjiz+1yD7w0JnLx2dCk6JDGcSNdAa1TIh90C92IP4frI96OH7x9sxzbAp3htzva0zUuA0rA1Kj6+IFvWfa/Zxb93EAqeuUn42l016ZKi36PtDifskC5g6j3SN16jXYX5T7SrNWBKG9t/WaOI4Ki6JUv11BvPPB6rYeqRuGFv0kNJkbi6JFquTTnOsdjuz1NcNTarTVqrd8uygsL+6M24GW2niZzTs3w04vGJT3UHM56IvvfHb1nd1AAsOUvCPsznI+gW0E9RE1MxERAEREAREQBERAEREAREQBERAEREAREw1qyopZiFUC5JNgBAMkpXa/tCUY0kPui7nw0uPhNPi/2lU1zjDpnC90O2is52CjcgAFieg8ZUf+rNWq7sb5wSfIymW4JX7O7wMEcsm5dIg+2OG9niDUX3X7x9ecikxHeBvexvLNxRfa0ijavTHdPVOXrb5ShM5GkrH5kY5ovHNxZecRSSvTH8QK1tb3PltICtwMp/r6/hF/1kUuNaw1nh8YxN7mSotGbmmWDhvDGtdqo0FwNdedpr4iqobrb9+kjP/UW5GeUDObnmdY47tkcvsdt+xzCr/wBPVr2771Cub+RVQgfEn8p0aci7B9q0w9WnhHstN0BU/hcmwv4ED5TrssnaKyTT2fYiJYgREQBERAEREAREQBERAEREAREQD5E8PUCi5MgeLcbVFZi4VF3bmfADmZaMHLoq5JEjxLi1OgrO7ABBdjfQDxPXwnDe1va+rj6hRSUw6nROb/zN+nKYu1naV8W+RbpSU91L7n8TdT8pFOgppf7xnZjwqOzNybMGMr6oi+6gPq7CxPyHpJ7h1bQA+8FIPkAbH5SrUt7nn+skcNiCGzeXylM+L4saXro7vC8hYZ2+np/2WrEoDvyAHmLbSn8a4WEOdCct9uYlmXFh0zA7/RR9bzUrMrAg66ajwnlJuDpnreRghnhyj36/JS8s+inJHH4HI38p2M11SbcjxeFdmFUEmOE4Yu4AmgqS0cBQA6CVlLRaMNle7RuRiHH4Aq/BQfrOufZj23FdFw1dv4qiyOfvryB/mH5zkHaFs2JqkdbeeVQD+YM98BuHzgkFdiORlr4qzbHj+K+J+p59nL+z/bx0yriBmTbP95T49ROi4HHU6y5qbBh+Y8xNFtWujmy43jlxl2bkREFBERAEREAREQBERAERPDuACSQANydhAPUhONdpaGGHfYFvwjUyudre2OUGnhzrsXH0nOKlUsSWNyefjNsMIyfzMTjJK0i2cT7cs9yBYchKPxXjFSse8xsNhyEy1RcTQqUp38FFaOb+TBhtDczBjKxdp9qAia/OUk/RKPZ0YeU2kHvCaje8PIzbpnUyI9lmz0lZk21B/ZE28GzFHYd/MLabrvus1GXccjrNR8ym6mx5jkf/ANmHkYVKLaWzs8XyZY5JSbr7FobDCrSW6kHKNxYgytV8OUaxm3gOOZXBe5S1ja+l+dudpZ6/BfbIHQBlYXVhsZ5e49nXlhHuLspN5PcKxOSi7ncCw8SdBNLGcIdDYqZjxGfIqAGw1PiZbTMEmiMrXDZud7nx6yzLwdqCU6h1SumdGG3ivmNPjI3D8Hep4S7cYJw+Aw+GYB1YKwY6slgS1hyUkj4kS7pxZfxpSjmWuyAw9UX8DofX/wAyV4TxZ6DXRipG4v8ASQVZyiq6rmUEFrclHUdJt4h1dQ6nz/WdngL5Xfsfq0k5pLtI6rwXtqjgCr3T+Ibeo5S2UqqsAykEHYjUT890cQRLb2X7RvRYalkPvJf8x0M2y+Mu4Hmxm12dciYcNiFqKrqbqwuDM04jUREQBERAEREAx1HCgkmwAuSeQE512k7RNiG9lSvlvYAaFz9fKWPtRVz5aPeKXBqZDYm+irm5C/ePgBK9V4StJi9FshQhSX765jcgAjUaZRYaksB1EhzUdezTGl2yNpcGRFLvZ2Av3tKanfUEj/uP9s0+13EcM5VKFGkLAF6qooYki+VSBsL6maHG0rqwFbNpop+4baHJbumQ7NIjG3ybN6vbPhM18QJnzTWrtPTwuXH5jhzceWjTqiaoXvDzm0dTPVKlvf8AdpZozRqKLuTbbQflf5zMhntFtm02AFvFjmP5TCDIRLMpbTy+UxNPaiGpkbi0kB8MKgBUANzI0J8xsZO9jOMNhaop1W/gVDZgb2QnZ16a2v4eUhcFUCProraE/hPI+Um8bwd8uZRnUjca26gjlPK8mDhK/TPb8ThnhT7XZeO0uCy2uAfHSV2nw9TraWHhFZsXgkDf4lPuN1OX3SfNbfnNH2ZW6nfnOR9mfFxbi+0a9CkF8AOfhIviuKFSqzuSRsi32QaKLctr+pmDjvEWBFNLnXvsNQB+sieGvnzvbRnNvIWA+U6MGLm6fRM8qwR5Vbel+DbvnpnJddSPG3SR+BqFCUbrax2vy9DtJHBOEZ+l72P5z3xnChkzqLFPetzXr6T1MeKMFpHl5s08suUmajVAtiN15HmuxB8VOnrNo4nIylT3T8iNJoirmTMRto3yB+Fwf/E13cgBTurW9LXE15GVHW/s042WLYdzyzJ5/eH1+M6JOBdlseaWIosPxrf+ltDO+icPkRqV/c1j0fYiJiWEREA+TFXrKis7GyqCxPgBczLKl9ofEPZ4cU1NmqnKP6RYsflJjHlJIhukUXE8crNVeqHZSzE5QdFH3VtsbC0y/wDuVmBV7A3ujqLKKlrK7rzClmfTUm3SQL6Dw/MzFUF7md0/EhJa7Ijna0y40XU01QgVcOCwztfIq0079XNyd3cBVvoANJTeLYUUahQVFew1IBWxBKkFTsbj1BEw4TiTU2uO+muamxb2bXBU3UHex0O40kfxPFmpUdyApY3sL2A2A11Nus5cWCUZtS6NZZVx0ZWrTWqVJiLzG7aTubOWjMTZvWe6tQAE9f3b5Caxe5v4zH7S5LH3U28TKuWiyNuibb77nzM2KaL0lw4X2INXCIWRkrOM4qZrjvaqj076La2oFxMHDOw2IbWqyUBZjZiWey3BIRfI211lFmjW2OLfRXkAnt0DAgy+cP7E4ckg1HqncKpWnYWBuT3r3vpJrD9nsEFNqC6EAlizNkYWuCTowPMdJR+XjXWy/wAGRxmvw9whfIxQHKXAOQE7AtsD4Sb7OcRJRqbHUWHmOvnbT0nVsRw+m9JsOoRUcMgRQAArDRhb3joCSbzir0TTfOh9y+YDpexI6iZuUc8Wl6NsE5YMifr3/Bb8DxJsO7roDVAFgdAdwRfXmRrr8J6xNYhS3M6ep5yC4ni1dUa9nTS/4l3B8xJXDOHyE7ML26aW/WeY0z2541LIn9yMxmHUUaj2YOi2Bv101HXvCeeDYdRSUcgLW85s8aw59i+p1dbnwJ5j4TDh7hbeE9PwY/K2eb+qP/Yo/gzthlBNgDuLfSTXHOCHDkG+ZCqq2mzlQSrdCbkjrN3gJC4c1aIWpVVrOQAXpplv3Q2gN794Am3lJVkZm9ozgFxZ6b0n9meRRr3DHNz6zolOpHmqOjkleh7Jyv3G92/McvhtMdWnp5DQ8yvL1BuDLlx/B06lB6tCkO438ZAwCqhByugY3Vri1hcG40lKfEXsOW469HHrofO8smmPRs4KtYqehB+Bn6M4ZVz0qbfiRT8QJ+ZEqWF/3sZ+jeyL5sFhm60aZ+KCc3kdpmkHqiaiInOSIiIAkfjgjGzorgDUFQ2/LXmdJISAx2MKd9EDZ2Iv90vmCC5v+8pjfoEPxXsPQrDOgNF7aBSWTwuhOn9tpz7jvAsZhrmpQL0x/qUruoH8wtmX1E6jU40lRWVGK1SrhDZshbKSozEZcxAzBTrYSG4XxLIwFIO1M5VdqruSzldciv8AeLEC6kr6zWPkSgrbIWLm6SOPVqtjpqDqD4TWd50LtFwTD4jEFaaPRJcKzIqshqMucj2dwwO9zax63nOHYAlb8yAetjb08p0xyclZm41o95pjqPpMOe0wvUlXMUZy+kk+z/D/AG9enTtdcwL+IGr/AB931kOhuf38Z0LsnhaeHBasrXYgGwJZFvfIFGpY6Xtr3gOso5asN1pds6G/EXKs6e7ZfZoLAsSBlAO+4IPIAEyA4txqglVjiazGqmX+FSUsid2+UsbAmzHW/OY+K8dSgTUqAIbWo4VbZ7b5nt7gPO/LQc5zbEYpqjs7td3JZj1J8JWOJT+roY5OO72dX4Fx+hXQpRpFGp5bZmVGKtcF+6eRAuL7Gbp47RRwKlTDAKLWDqzW9Mx2J9VPWcaUqep9Jsoekt/iwvRd5Ze2dTftbh1t/wDJdrACyUiBzvyFt/ylE45Up1azugZVJzKwGVg1hmbKDYAm5t4yLVo9tabwxRhtFHJs84ssQgOpUWuNjrobctJLdnsQAhzHnpf9+Mg6mIGe/K1jNepxQJcLPN8nE1N8VpnueJ5UPhrm9rRcMRikyOCwF7anzH6TTDZxZBm6nkB0Ep1biLvtNnDtVbT2pUdBedXiXCNNHB5+aObJyj0lRfuzVQ0HcEKFqLlZ2GYKb91ip0ZQSbjofCSAXFl2L4hhURluO5lGrEEC2XlfbZhOe08M41FSqx8CPrLhwio+LpCncjFUB/DzixrUbWAN9C6XtzNrGaZY++jkg6N3i+KqVMJiEqAB1emcwNkclrEZdlNqdzy0E5xiiQdRYg3+Oh+kunaRPZImFNqpHfxBD2OfKAiC2+Rb78yJQccvs3ZASV3XNuAeR8Rb8oi+MRLbPue+UfvpP0n2K/yGFt/9FP8A4CfmWm9jfoPlP0x2HFuH4T/Yp/8AATLK7RMUT8REwLCIiAYa1UKrMTYKCSegAvK3w7tRgnC0qVX2hAtZQdxvcm2t7zY7a4oJhXF7FxlAuASD7wF+drzjVXE5AFWm2UbBQAPhe5nRiw8423RSUqdHYsXwmlVVlRQjNbQ7XF7EodG0JB8Daa1fgmJuoWslNPaZiEQDKgXuoqEFdX7xJ6zmWD7b4mj3VqMF/BUW4H9LHVfQ2k/wz7SEzZa1N0B/1Kbl1/uRtbeRlZYJLrZKmYO0VbE4am+JqVclRmejRUItyjVGLVG5q5UXFvracvrFuZDDrLz9ovHExNWmKbh0RL5lPdLsdd9QQABY+MpjJ0E0hFqJVvZoVOomvebldVHPXoJpDeZSVMsjOjWsdrajrcbGTeM41WxDIxOUooF0JW5tq7G/vHnbneQYYefntPYYnfbpy+EtFlWiQV16ljzt18WO89hzyCj8zNSnNhDNkyGjOHbmZkR5gvPhaXIJvA4T2ik5rG9h0POauLw7IbMP0PkZ64ZWJVlBswsy+Y3/AH4yYw2LSqveUHkVI2M2jFSRjKTi/wAFbp4B6h7o8ydhN9OD0UH8R9fAfTeTDmy2QAfIDrI16lFWAPfJ95yb2/fhLPHFFVkk3o1HRENksR1t8wec8Ejwm3iOHAgMh7rDunl6HmOUjFqsjdCOovaZtUbKSZNJw5whe4FhfLzt9DMCVnBBWq6kaghtQeovtM+GqWRnd8/dNuguPnNB0dFUupXN7ubQkfiAOtvHaTOqRWEm27Mz1W+8Q/8AMVAcf3Lv6yt8Uq56h1vYAX8vrrJmpV03lbzZjfqbzmzPSSNkbdCkSVHM6n+kaz9Qdl6JTB4dDutJAfMKLz818JpoXDVGyIxyl7Xyjr5Xt6T9M8CpZMPRUkHLTQXGoNlGoPSY5NRRMeyRiImJcREQCg/ar/h0f6m+QnN029Iiej4//Mwn9Ro4zYyJo/eiJeRK6NGrzintETD0Sarc54EROeXZYyU5tCIkxB7WbCRE3RDPbTy0+RLFTYwPv/2n5SV4R7n9xiJthMM3TNzE/wCG39MrTe6fL6RE0yFcJ2HEf5Cj/tr/AMZx3iv+K3p8p9icsPpZt+4sPYL3z/UI7d/5+t/b/wAYiS/qRMfZX8V7h8jIRYiY5ezREk3+GJ+o+D/4FH/bT/iIiUzdImPbN2IiYFxERAP/2Q==</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAQEBIQEBAQEBAQEBUSFQ8PDw8PEBAPFRUXFxUVFRUYHSggGBolGxcVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGi8lHR0rLy0rLS0tLS0rLSstLS0tKystKystLSstLS0tLS0rLS0tLS0tLS0tLS0rLS03LS0rLf/AABEIAQMAwgMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAADAAECBAUGB//EAEIQAAEDAgMFBQYDBQYHAQAAAAEAAhEDBBIhMQUGQVFxEyJhgZEUMlKhscFC0fAjYnKC4TM0U5Ky8QckVGNzoqMV/8QAGQEAAgMBAAAAAAAAAAAAAAAAAAECAwQF/8QAJREBAAMAAgICAwACAwAAAAAAAAECEQMhEjEEQRMiUWFxFDJC/9oADAMBAAIRAxEAPwCjCUImFKFrWoQnhThKEBCEoRIShMg4ShEhNCAHCUImFUtrbRZbMDngkuMBrdSfsETOdyFmEoXHHeysHE4WYTMNg5Dhmqp3gusv2p10ws/JVTzVLXdwlC42nvRcAjEGOb/DHzBWi7eV0AiiPN5jyyT/AC1N0EJQs7Zm3KVc4YNOp8LtCfArUwqcTE+gHCaETClCYChNCLCYhIBQmIRYUSEAOE0IkJoSMOElOEkBdwpw1ThPCkSGFPhU4ShAQhKETCmhAQhNhRIShMlW8rilTdUcCQxpcQNTHBcFtfaZu6gMYWsENbMxJzJ+S6TfKuQxlMGA8knxDYgfNcewhp6rNy37wj+zDnw+aVKmIzzIUHEyRnnyVihQqOB7jusGFToxA3A0gQnbcRoTHLkhPt3aYTmrDNk14nASEtgREokg94ZEZLc2Rtp7XNbUcXMJA72rfGeS5yrQqM95rhI4g6qNOvwKdbTHcH6eoQlCzt277t6AJ95hwE840PotSFtidjTDhRhFhNCYCITQikJoSAUJiEWExCUmFCSJCSQXYT4VOE8KZIQlCnCeEAOEoRIShMpDhKFOEoQTit+ZFWlOmAx1xZ/Zcw2nLo4Fdpv7bzSpP4tqFs+Dmk/VoXK7Jpk1BGs5BY+bq0nEbOOv3b3R7QB7hDP3uK9B2fsKixsYREeaq7BxNpNxwDAyGQhbluMWhXMte0y6dOOsQz37t2pcHdk0OHEAfNGq2FOIwt9AtT2Vyr1reBmQPkoz5LIirldp7GpO/CJ5x9l5fvVskUKktGR1jgV61ebRoB2E1WSdBiC4LfmkcQdEtdlPirOG0xbJUfIrWa7Am5FsW2xcT/aPJHQDD9QV0GFYW49SbdzP8OoQOjs/zXQwuzx/9YYAsKaEWExCkAiExCLCYhBgwmhFITEJAKEkTCkka9CeFOEoUyQhKESEoQQcJQiQlCZBwlCJCUIDH3ntu0tKo4tbjHVpn7Fc3uDZtfWdUcJFMSAdMRXc1qeJrmnPE0iOciFxu4rXU61am4QQ0yPFphYfmeuva7hr+8TPp19xZ1riYq9lSGUCe95jNV6Wx3UiHMvajHAz3cLR/lLp9Vp1bc1aeAPfTbzYYcfPghN2BS7QVWtl4/D2dPB7mAkggzln1zWClum63HMzuOn2beOADaj8ZAHe0nLVY+38FcEPqOayYyfhHjmnsKWF2GZgQM5hVa9BrqjmkatIg/vCHRPMfdVxbtbNOlCju7YOEAh5iMQqCoPloszbeyQyhWoyXMDC9hOZbGYAK2KmwKMZY2uDgcQccQIEDvakQBlMIW2GE0Xt1PZOE8TkVZNu47VeGVnYc1uG39lVPOoB6N/qumhZG5li5ltjOlRxfHEDQf6ZW3C63DeLV6+nPtSa5v2HCaEWE0K1EKFGEUhNCQCITQikKMJGHCSnCdAXgEsKJCUKRIQlCnCUJkHCeFOEoTCEJQiQmhIFSMOB/WeSq7W2a1lzTuacYKjXUnkcXxiB+RHmFYqMkZa/dW6zAbd3u8H5ECHg5wOhK5vzKz579TDZwTE1z+SLs2kHNVyq1rBEyTwWZY1iwAeKr7Qv8L4e7CXEgCCSQDAAA/Waww2xLV2fUpNeQZzElxgCeXgqt9XomqcMy3Q5EOPLn5qVvsqs7vClUzEyQ3ToSqu0tk1qc1HUqrcIkuAafkCpeA8o321sDXNlq5/bmTXRmcLoHMxkEtkXrnkw4uaWnOCBIEg5+nmmuiXHzH1S71G09HZ3GsohoHZswT8WEASPmnwo1ZjcWIZ92JiFGF1fi0mtO/tg57Ra3X0FhTQiwmhaFIRamIRSExCQBhNCKQmhAChJEhJAX4ShThKFIkIShThKEyQhKESEoQA4ShEhKEjDhNhRIShAU7e4BBbObXEeYKsXQZVAxDvZZ8QRxB4LAv3Op1nubmJ7zRroDIVmyv2ugk5H6rh3rlp/26dLRka6Khc1WN/vFYCOYMKrtKrUqSTXqkH97CD5BFtWh2TnDB1VfaIa3R3dCNnE/wBVejUYxmFsDKEOg7E/LRo+Z0+6xL3aYDu7mTw5rT3cxFjy7Uv+wVvx6byRqjmv+s404TQiwmhdVhDhNhRYTQjTCIUSEaFEhACIUSEYhRIQAsKSJCSDXoShEhNCEEIShThPCekhCUKcJQlpoQlCnCUICEJNYTkBJ8FOFPbbTa2lO4dIBrtD+EU3Ahs/zR6qNrZAYF9SIrvaciQ3I8DhCyr2ywuxNJE8RktH23t6r6sQHEAA64QAB9JVh1EO5ea5F7fvMuhWP0jWKz2gDuVTEaEIFy2to55K3qAiQRl9FUuWFzsgl5H4smzsvxHM+K6Dd4jDUHEPmPAgR9CqtRgAjILW3Ht21K1w06Gi3yOIwVbwWzkiVfLGUWoShWbi3LHFp4ceBHNChdPWUKE0IsJoRoCITEIsJiEaAiFEhFIUSEAOEyJCSAvQlCnCUJoIQlCJCUI0IQlCnCJToOdoCfolpgQnZTLjABJ8FqUNmcXZ+GgWnRt2t0EKM3/iE3hjbOsf29OnVEYmPqAcD2ZYC0n+efIrY3g2cLm1rUIzew4f/I3vMP8AmAVbbLHMDLloJNqe1wiZqMILajAOJwFxA5hq1xWa5rajHBzHtDmuaZDmuEgjyKrt3CHlO68b2Yc4Ig8QciCNQfGVsNYrO+ex/Z7n2lg/YXDu9GlOvx8na9Z5qjSqQudeuS6vHeLV0fTUcVXqZnII7qkoVV0BQWYoXDIzXR/8N6BPtVXhLKY8sTj/AKguarEkHieAXou6dh7Natpkd95L3/xO4eQACu4Y71m+TbK4HtRgd2UkDtKmAOiTiwOcB4Dun0WdXs3s1EjmMwtSozHc0WmMFLtK3WpAptHo+ofILRfT59OhW2tpiGKL45KE0LobnZrXcIPMLLuNnvZnGIcwPsrIssi0SowmIRIUSFJIMhRIRCFEhBBwnUoTIDQhPCkAnAS1FGE7WEmAJJUoWvsW0/GfLolM4UzkIWmy4guzPLgFoUqYE5aK25sEdYTNp5u6z8gq1MzocBTFIanIcufgpMYO8ToMusZqDXEyTw9J5BBBVCTM8vKVjbtPwOrWRydSca1EcHWtRxMN/geXNjgMPNaz3ILrCm+oyq5vfpzheCWubIgiRwPEaZBMxqvZVWPt6jQ9rhDp0g8B4/TJeYbRsHWty+gX4mt7zHcXUj7s+Oo8l6uaTcMRkRB4aqns7YlNjTSeXVqZnD2wFRzWH8GMiSBJieaq5OKLQu4eaeOf8PN+2Qq75BjJdhvju5RpUDWt24TSI7RodINM5EwdCMj0lE3d3XomgyrXbjfUGMAkhrGnNuQ1MQs34bbjZ/ya+Pk5bdPZxfWNV+baQls+7jn3jwyHzIXYG5rO9yGN4S0OcRzJKvttG6ABrG6MaMLepHFGcwARC00p4xjFy8nnbWVaDGe1+NrdQRAiYjhmStak6RBz4eMKsQp03wVNWsPbH61HNJEJGQPuu0PwuTERPggMy82cx+cQeY+6wbm3NN2F3rwIXXtGio7WtA9mWozCcWxOtvqXMEKBCKQoEK1agkpQkgNIBPCmAnhQ0Yg1kkDmYXU2VENaByAWHs6jiqDwzXSUxEJTKrk94aszLLUZ+YzUxEyNHNBRHBMxgER+gc0lYFduccpP6+SFcDCA3jqepVwNknr9FTuBJJQSqQptTlqQCEkw5EY+CEEKSCY2x90jb1Lt9Su6sy7lvZumGtdMzJzMFdA5gwgAQGtGX0HpCNSdLR+tE1YwxOZ3uQpOyQXlTcUN2ajpuCv99rht5XtKOz6l12GGXUXOL8Ja0uJaGnKXQmO/lTRuy9oOf8IpHX0n5JtqVP8A83ajrs4xRvKRpGo3MU3FoDif4Sym6BmRi5KWzq9xYO9rque2gGkue6rjZdFw7jWGYeXGII010EqdaxMTO+itbJiM9uj3L3lG0repUFI0XUappmm52IggAzMDnp4Lo6gmP3gPXiuL/wCEdg+nbVatSJuqzqoiYLYAnzOJdxTblHwOPpqoJT0AfeUarZy6p2cDzz9T/RI69AkTl9pUMLzydn58VUhb+0qGIEcQJHUD8pWJhU626aK9wDCSLhST1LxaUJQpwlCp8jxrbFod0u5uj0b/AFWqOHj9UDZ1PDSp+v8Amk/dWQ3Ijkf6hWR6ZLzsyTSpjRQ8fUKLqwAM8B/uhEQCB5n6oD2orXS1pmQQM+YXH22/lmWVTWrMpPpVqtM0u8ag7Oo5o7upkAHLmnETJukIQ3mFhW19e3omhT9ktzpcXDcVZ4506Og6uMeBWva7ObTzLqlV/wDiVXY3eQ91v8oCJjBAoTylCUJBZszqFK6b3Ch2nveqsXLZaeiAyiUydwTDRRNx22Li5qNfTvNndravDobbudWrtwnuucB7rozEac1xdjsq3FQdvV2hWtKRxUrQ21UPGIy5rhMDPXDE+C9lCdPU9Ye7W2a9SoGusKlvbHEKVVxDThbENfSiWSNOGS6eqYxxxaI65j8lVDkS6rBpBJyg/ZJCSccz+sgFE6eJUQeeup8OQSLtTyyHVAAqe8P4v6LDuqOB7m8jl04LdqDNo5ZqltmlmHjjkfsl6XcU94ysKZEhJLyaMX4U6VPEQ3mQPVKFe2RRxVJ4NE+eg/Xgq4nZxC3Ua3MMCBwj5JceqkVHwWhiM4cR/uqt3k0kclbKr3Ayy+enmnANaOmkyMhgGSyG7r2PtBuvZqZruMl5BPe+LCcsXjErVs8qTcogEQeEE5J269EARyG4J3uUC5I4MQhuUy5DKANbuhwVl7xBEjMc1RchuQMMmhMmlRM6RUXFRYcykZwe9CjfOE0ydRMDhiyz8kmnveShdNBcyeBOXPJMDM/X5qZHDgEzSAkch4lGjA9TPj9Er2ljYRx1HUKQGngpykcTk652ElpvsGkkyRJ0jRJQ8Zafy1Rhb2yqGFgPF+Z6cAsNTZvK6llXtarabRHbW5FwzCNCWCKgy5NPVV8MxvaPNEzHTpSolZ+yt4LO6/u9xSqH4A4CoOrDDh5haRC1MuISq117pjkrbmKtdMymY8k4LALB00aZ5tRWDVVbG4a5gwnJpc3zDirbdESEUz1IqJSOEFBEcoIMnBDciO+ygdEgEUxUimSBioN949ERDJ73UJSaLsneShcO7zPP7KVc5jzUIBe2TmGn5kfkg1hqdGZRbzKK1jRoPXNBKzWk6BGFDmfIKptTbVtaibivSojgHvDXHwDdT5LEpb3m5xexUS5jTBuLkOpU5/dp++7hrh6pTMR7SrWbenT9k3xSXLe0Xv8A1YHgLanA6SSY806j+Sv9Wfgu00O4dDHHk0n5Kar7RMUap5Un/wCkrn60uEtrSlUa3GxriIgkd4HwOoW1ZVbmj/YXldgGjKrhc0/SpLh5OCybDQLVpnJW15LV9S0W4qW9w1Gb07SYO82zr+MVrc/V4Va+31vi0j2W1Yfi9oq1I/lwCfVV3FZd/wAueXmVbHPZRb41G9uRcuJdmT2jW1CDOT3ta4xyzLl3gEBcfsCi2ncuptH4gOga1sfRdiVrrO1hz7xlpDcc0ycapQmjCL1BTeolBoO+yjGSk7j0TRkogMqKkUyAioVNR5qZQ6/DqkkFeaA+K5jb+2Lq3rsNKlRfTeyJqve0h7SSfdB4Eei6a9PcnkQuY3qb+zY74ag9CCPyVPLyTXMX8PHF57V3by7Tf7rrKiPCjWrO8iXgfJUbqveVv7a+uHA/go4LZn/zAd/7JqT8k7is9ua/9bK/H44+maLClTJLWDEdXu7zz1cZJ9VubpPyqt5Oa71BH2WRXeru6dT9tUbzpg+h/qq4mZ7lZasRHTqkk0pJ+SGNCVT206Lasf8AtO+itYlnbwu/5Wr/AAgepCoi3aEQ5Wy0C0qay7TTor7HK7WqB3lBsqXaXFMcA7Gejc/rCDc3GELS3WZiNSryhg+p+yczkaqu6DYlGbuo7kwepj8l0hWPu/BNR/xEegWuSulxxMUjf45HJO2lBupUlGloeqkpEg5QKk5RKAg/QpFRqHIqSiAymITlNKRoOQ7jTzCI9QuPdKDAuRLHdFhbbp47eoOIbiHVuf2W87Np6LIcZyPHJY/lTkw2/Fj24+hUyTucc+SqVD2b3Uz+Fxb5A5IoqSFRLbVCqVY3YfFyfGm4fMFVKhyRtgmLlvi1w+R/JEeis7PEkg40lHSxo41Q2+Ztqvg2fQg/ZF7VCvCH03t+Jjh6hZK2yYSnjc3ZwWqxMBZ+zX8FoPZIW6YKJZ98ZBHNF2DtoUaL6JB7R9XLkGloBJPkVGvSWbUoYXB/Cc/opVyepVcsTmw9b3ZM0A74iT5cFrO0WXsGo00GFvuxl0Wg93dK6suQlR91TJUKI7o6KTlEBuKiU5UUGhU0PknJUX6eY+qTlEIuTJFNKRo1dFCt7p6Kb9Cov909EGrNOXksZ7sz1Wmx/d8lztxdhrS86ASsfzPUN3w47lye3nTeVAObfXCESi7KECC97qjvee4uPhPBWKbVRPrGysE4Kex/7y3wDj8iPuk7JNsUzWc7kw/MhEepE+4dR2idUu2SUE8XMRSxFOksq9zVt7/mfqtelomSW9kqFVCo1GgyDoQnSTp7K/p224VQmwokmTBHzK6Oqe4U6S6senFt7kenoOgTuSSUSgIqBSSQYVTTzCdySSiYZSCSSDM7ih/g8kkkpDLB7h6Lhrx5NBknU5+MTCSSzfI+m34nu3+lOiNEcJJLLPtu+kLnQ9FX2U49oR+4fqEklKPUo/8AqGtKSSSgvf/Z</t>
         </is>
       </c>
     </row>
@@ -4314,25 +4314,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KULDEEP SEN</t>
+          <t>GERALD COETZEE</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>smat2023_090</t>
+          <t>sat20_2023_32</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -4344,22 +4344,22 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>100</v>
+        <v>64.7</v>
       </c>
       <c r="M31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N31" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="O31" t="n">
         <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>21</v>
+        <v>10.25</v>
       </c>
       <c r="Q31" t="n">
         <v>0</v>
@@ -4371,67 +4371,67 @@
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V31" t="n">
-        <v>33.3</v>
+        <v>37.5</v>
       </c>
       <c r="W31" t="n">
         <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y31" t="n">
         <v>3</v>
       </c>
       <c r="Z31" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="AA31" t="n">
         <v>1</v>
       </c>
       <c r="AB31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AE31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AF31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG31" t="n">
         <v>3</v>
       </c>
-      <c r="AG31" t="n">
-        <v>4</v>
-      </c>
       <c r="AH31" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="AI31" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="AJ31" t="n">
         <v>0</v>
       </c>
       <c r="AK31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL31" t="inlineStr">
         <is>
-          <t>Bowler</t>
+          <t>All-Rounder</t>
         </is>
       </c>
       <c r="AM31" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUTExIWFhMVFx4WGBgXGBoYIRgYGxYWHRgfGR0aICggIBslGx0YITEiJikrLi4uGR8zODMsNyguLisBCgoKDg0OGxAQGy8lICUtLy8tLS0tLS0tLS8vLy0tLS0tMi0tLS0tLS8vLy8tLS0tLS0tLy0tLS0tLS0tLS8tLf/AABEIAOEA4QMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCAQj/xABCEAABAwIEAggDBQYFAwUAAAABAAIRAyEEEjFBBVEGEyIyYXGBkQdCoRQjscHwUmJygtHhM0OSsvE0osIVFiQ1c//EABoBAQACAwEAAAAAAAAAAAAAAAAEBQECAwb/xAA1EQACAQIEAwYFAwMFAAAAAAAAAQIDEQQSITFBUWETcYGhwfAFMpGx0RQi4RVC8SMkQ1LS/9oADAMBAAIRAxEAPwDuKIiAIiIAiIgCIiAIiIAiIgCKjdNPiThuHVaVJwNV73NNQMP+FSJEvdrLouGjWNRaYLFfHTAtzZKGIeRpZjQbjm6Rvtt4oDqyLljfjjw6L0cULTGSncyLD7zXe8C3krdwHpzw/GODKGJYahAIY6WOuJgB0SRuBMICyoiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAL88/Fv4jV6tephcNUdSoUXlpfTcWuquAh0lvyA5hGhseS73xPFto0alV5LWU2Oe4iJDWtJMTaYC/IRrtfWqOuWve57c8ZjLiQXRbNBvtKwwfMDhhlbJguJ9F6PCiXHtCLXnXNEfWy1qtB+fsNdraAStipg67QBkd4W/Wi1ujdRfIys4XaA8B4BcJ8BJ/NfcPRgNeHFrgZEGC0tOoOoIKxN4RiiZ6qpcR3TcLzUwNdlix039JufyWM0eZtklyO4fCHp4KgZw/EOca4kUnm4cxrZDSdcwaDE6garrK/HvBOIPpYyhUY7I5lVsEkN3AuXWiNZtcr9ggrdHI+oiLICIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiA0ONYNtfD1qLhLalN9Mi+jmEHS+6/LvRHhQqkE8p89F+sVwTgHDBSfVEQKdV9MejyFwxEssCRhoqVRXN/hvCP2Wqfw/DY1F/ELJw8/sxZSLabjJKr8iepbZmtERz8K8mRoq9xXgIc4lzcr/LXzCulJj5sQFp8SrNFnObm81tksrq5jNd2ZwjpZw7q3GBYEmf16r9Z4ZpDGg6hoH0XAeneADqRIAlwIHnFl+hFPoTzRKnEQy1GgiIuxwCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAh+k/FXYbDuqtaHOzMaAdO29rZ2mASYkTGo1XMsdhnnr3OOUurOqOySO8AXATJHbldE6a082GBGratN48w4EfWFSeC5qjCah7ZJL52dOnoICg4mTzZSxwtOPZ5uNykY8ENY5hrUy92Rna7zhtEWOlp3Vj6H46s4lj7ESCTeSNf14qbqcJYRckj+KPwWPh2Gb1kMGnK/uVxlK6tYkQpWd7kH0spV3PaxpJzOiQ7KNtfAStLgzAKQLaJdLyw5mvBkE3GczEX0i8EgyBeK+FY5xbUAkncbz9CtihwtjdB6kk/ibLaMtLWEofuvcrWO4W1zaLHEtYH5jJiGtY4xJ8QFe+jWLqfaK9Go81GhrKrCbwHZmkTqRLcwn9oqB4lSaCARmBBbAEzII0Ux0Iwhb1jnEFwDaci+jqjoneA4LahfOkjniIx7OT7vQtqIisCqCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiA1OJYUVaT6btHCPXb6wue8Qw1WjULXNgkAg6g6jnyA9101UP4lVjTdh6gHZOdh/i7Bb9A/6qPiKd45uKJOGquMsvBkFxLGRSh9TIDq7kPDxKhT0hqMfFPMaYbA+7Ib6uGu2yccwbsT1Ra7KB2riYMiLLRrYZuHE1cViJNxGUAHwtPuSosIplld8dETmD426qahritkOk0i2LG4draAp7BYnPSBa8PGgcPmG2m6p3C6FPEXpVsRmbo4vsD5aSp3gOBGGDmB5c3WDqImdNZ/JZmkhrpxRK0aZqV6NOYLnH6U3k/QFXvhuDFFgYDO5PMlc24JWL+IYVrST2nvPgOqfr4beq6ou+GirX4kDF1HfKtgiIpRDCIiAIiIAiIgCIiAIiIAiIgCIiAIiIAiIgCIiAKsfEDANr4J7C5ragIfSLj/mNMgDzGZpjZxWH4g9JBgsM4MdFeqC2l+7a7/5ZtzMeK4j0Lo1K2MGIr1alSoxzmjO9zyAWRdziSZzG20eIWKqcaTm9tjeks01EkXdJeqrNpvYWkAhwOx/DXdbeJ6S0XaD/AJ8lOcb4DRxLYqME7O0I8jqqZjugLm/4dUnaDsq+Lpta6Fm+1T/bqWDAdJ6LGkmBYmBHp6qLZ0vc+sQ1hcYIDW6k/wBNJWLhnw2c6DVqHKNm/wB/yV34J0ao4aAxl+ZufUm6y3TS01MJVW9XY2egBp0K5fjKjGYnEAMotJgATLmNJsXk5LeAAm66euA/EwBzsMz5utz+TWtM/XKunfD3pP8AbKJp1D/8iiAH/vt0a8eJiD48gQp2HhKVDtOtiBiUo1Wi4IiLY4hERAEREAREQBERAEREAREQBERAEREARfCqV0g+I2GoS2iDiKgt2DDAfGpof5Q70W0ISm7RVw3YupMKqce6bYfDtOQ9c+QIYeyCTF3aegn01XPcT0lxWMa7PViCSGU+y0NAGxku3u6fCFFYXC1qjQGEXY58nKLnTMXc5O+ikLDNXzPYn4fDwtGc02nyWi1S11Wut7acNd7aPSPi1TF4ipVqntGwA0awaNHgPqSTutPgGINHEsOjHnKTyd8p94HqF5pgluZ4vJ0v8xjT0XviGCrU4zUYaXZXEm7YjYbxcX2UqrTp1aXZ3Wq0+mhHVGrTm6ig1GL1umra2t6HS2HnqvFVgJ1WpwPEdbRBntCx8Y/stvE0LAwvJyjKLs1qW0XfVG7hnjSVuVKgAJJsFFYJ14hRfTjHPZQc1nef2R6/2W0U27I1eiuymcW4h9rxb6o7jPu6fkD2j6u/AKS4FjX0avWMLgQMstMGCQfa2ir/AEZwlapUNFrWZWjvEkSbaaySeQ8VZ6XD6tEB3VOcc20GWxGne8Rb2XqaahToqkt+JEwtCcqyryVo6u7V1bbb3ezOi8C6aEgCvBvGdoAMbFzeXiI8lb8Ji6dVuam8OExIMwRqDyPgVwQcRLSyGzkqECdC102Mb3GlrLFwrjdeg99WjUcHOJmTmmHGzgbOjS65SwrbstDOJp4Zwc6bs1a9tvPry4a8bH6KRc/6L/EqjWinioo1dM9+rd6nufzW8dlfWPBAIMg3BG4USdOUHaSK1O57REWhkIiIAiIgCIiAIiIAiIgCIqr8ReKnDYGplMVKv3TTyzA5j5hgdfnC2hFykoriG7HPunfS5+MquoUXEYRpy9n/ADiNS6NWcm6HUzaK7hcIXg7NbMnyE6eX58lgwlIOLWzrYW32CnaWHgsotDyS49Y4iBdpjyk2E83K5bjRhlj76+/8d8DhlWnmntp4t8OfO/Qkej/BMtMVHg5nDbduo02+s+AUviMIMwABYA06tjlGli36816qVA12UAdgtIG+VwiBzhwN/wB5bOMcP2WtEasdIvr5FVVSo6juz0lGDoxjGO1untvi9OJoYfDsyZRTbAvENPmY+b8Vs1sG17XtI7D9hvydlPaEjLGXSEoUpbl+WJJifEQDfUQYO6yPdIH0AkxpMbtgX9Fptqdajztp638fv75lONOrw+rbtU3exF7H9l45K8cMxNLEUszSCNxu08iNisFai146twDg7vTeTuQbHW8c9FUcfw6vgqhfRcTT0kXjweNx4/hZdK1GGJ12nz4S7/z7VLUpSw+sdYcuK7uha8di6OHaXOPkN3Hk0b/qVUWsq4+sSey33DByEd55/UBbfDeAPrv6zFVC2dj3j4HZo8PHZWahSa1gpgBrRoBo06Ta7nXKxRo08Lqnmnz4Lu/JtGjOu7zVo8uL7/wYMLw+nSaxrbBp3cGnMRGfsXsM0yd1krU2i2U3HjPncg+62bixEbESGC+njpBKx9XJiJEEh0a851JiQBsVjd3LSM0v2p7IrPFOGNqNebMeSDYavERYc4vFt1A47gr2MY4XFVzoAMkG7o8LSfQxKuHEqY6wM1zQIkOkcoj11/os+NwzK8Uw4BzLsOpaRIaPWSd+8fBdaVeUZavQxicLSq0kstr2ba4Wv/6e9/tbmbWxtH6+qsnRXpXXwLhcvoE9qkfHUsnuu+h35jDi8M2qSwPDatIuY8Gbw61x4yoisyDBF/A/VWqcascskeVr4eVJ3TuuD+63eq2tzP0dg8UyrTZUpnMx7Q5p5giQthUP4TY1zsM6k49x2Zn8Dybf6w4/zBXxUU4qM3FO9m0ZlGUfmVtE/Bq68mERFqahERAEREAREQBERAFyj4yYyatCjNmsNQ/zOyifLIfddXXEfilWzcQeNcjWN/7A7/yUrBq9VeJrLYgOHMcXgMcA7UEiwt7yNRZWrhQBNN0ONTM3rA7UdoTAGnMb5XFVPh2MLJLYv4/4Zm7gNz4GNPOZnA4sBwqtJjMC6pPec13yzsO19REwBMxCcmXXw2UYQ31d/B7bdVu+Gzd7RVtxrcz2kjmw67iQLWABA9164g2WnLkmAB1dtxr4+K1eMYwDDGoQS1mVxLSW2Y5peAW3zGDf/haruH4p5r5MUQ5hY2iC1p6wvL8jXG2U9jLMETfRVpMq4uNBxUk/TT3qStJrQIjT0/AxHkvYgHnaJLtOWV7eYJsVF0MLiHHq241jcSKYrOpij3WENcYqRBcGkHL6Tuo/GnF0adZwxRPU4j7OQKbRm78O35d2+uqzYj/1Olyl5fks9QdnumfKfX+6wUqcOA7LgTpMex2PisTuj+JFVtM4p5BouectNpPWNdTD6bQSB8zSDOxWrwQltbE031RW6t4YHOJAJl4PMC4jzWNzahjozlkSfvx9TdLJcZLQBoBceVtfFbZJiS2T4kWH5LFTIzHLFtmifrYQshqTlIuZuLGQNIZp2RJEoTZau1jJToF7iRDQ0AFwIF3EWLnG5iIA5jSVgr0MtnDviWEHOHNDokFpPMTyn1Wzgj98C1hdncA45RU6tuVpY4g2aXEkZuVOPLWd946chYQ1xyFuTK0PAa4stlzAARqck6Fb2KyGKqfqezvptt4+76b7XI19IuxFLMBDWvdfs2AMaX1/LmveBJAl03LniZNgcrNDbQecrbrAOqF7tQyBnjVxHLcQtLDPDqpbEinkEagxktOoBLiZOkELlYvFPNC3Jer2+qMPFcM0ucSXMJAdMToCA2OcyY8RzVM4rnzuNQS+0kERYQIEaR+rqwdJeItLu04mnRhhyuAdnEiw3AJjmT/Cq5i6xe4ufZ2lhEAaC3grfCJrU898UqqUVG+unHRrVcdOi31TOl/C+m0F5kzkaBfUEkk+4HuuiLmfww4m5xFEtblIc6YuIAET4iDHgumKlyuMpJ7pv7nP4i81VTWzjFrusl6de8IiLJACIiAIiIAiIgCIiALiPTvhVYYqtUdDg52eW6hkQJGsNAyk+EmJAXbly/pS8dbVdUqhj6R7Ia5riKWYljokOabzB8YmwWYVqlOpHIr3umvpt7tzJeEw9Os5KpPKkt/449banP3cLf1fXNhoJygkjtd75Z07JGx1jdfcNi5JaZ675WT2WiAXVGERJG4iYjeCrLxai9+HcKeV9NrzUdUaQZAFjawdlJLp7URreKZjQdwSBEOGrbC9tfRW9Kfbwb2d/p3+9Uay/wBpVt8y8pdV6XTs9d0Wbh3EBXwmLpFwc5jTBBBDgWSHCLQSD5wVKYP7U2malHFNPXNa8k0xOYN7MZgS2AYGWIHkqt0TxGfFOYY++oEANAAlhPd2DSHOcfEHfW3dFK+fDUS5wIaMlxHdluWYggRqqyostRx9+9S9VKliqUakrv3bry573e90tjC0cYaTaZxLGjKGZhTaXGmIhpfqQIuD9Vsvo4wk5saCH6luHpntCSMwAB3dflqjHw58gNAPp4AkaHYHdbbakw46nuyY7JMiHDe8EHVYTOUvh9FPReb/ADY0jg8UWuH/AKg9zXyXdgHvAh2XM6RIJs2FjwOGc2o6o+r1j6pGZzwAHRYZgNosVKucJyxJ1dNjG4jQm4NtljIs2HQNR1nd357LNzajhaUJZlHXxNRlcioYI8S0W9OYH1WwwixnfQmZ5Ax47LXaPvHdoGRfq9PpsPqFkkZoFpALcsAgyIBOjQSHO8gVomTKkb3y729D1SquDgSJaH9Y6GVAS6HNbq2AATAjWTro3Bh31GtYHOaQG9WXCQTEhpdmaIIgNnNfsiJXyn2pcXEkTPdyubDwQS4HNIc8Xnvu5r7iK7muYesc8EtBzBgnK4GJy5jBF3E+q7500U9PAYmNZSum766/XdLh70GIIyGQ0ACYM/Le3iojhuINHBurus+rNSDec5ApjyjLI2ut7j9eaTgDHWkU4AJb2jBOeO81pcVXumge2nSa1pFMkjNAicpblb+9ln3PJc4RzTS9/wCbFvXqdlQcpe/459xAVq2ciXZurlodA7fI29h68yvbnSbX/JaGFnbXYa+fmOZ32sFcOhuCw721316bqnVtDw0OIkB4FQ9lwJgFpOwEyruP7Ie+J5CtVdWbnLd+/E2fhdiSMc1o7r2PHsJ/JdqUFhcIM1BxoMaWBzRlEGkC0QIFg0wQQDGYCJ1U6qXESU55rWv6XXoZzN6N7aL7+oREXEBERAEREAREQBERAYcTUysc79lpPsJXI+MdF3YhzX06hdiHEz1pMvaCGgB2XKSHAi0CInULonTPiYw2Eq1IkkBgHMuMfhPtuuXDpg+RFPsN0BeS5vaDhkcAA3tAHu3i8rvRp1m89L3098bPgdqTo5Wqt/Dh15e7EhwzonT6kNqNirDcz2vcYD8RUpEQHZCBDDEfK7mqG1365eHp7jdXWj02A1w9srW9moQYZV6ySXNMuLiZ81T8UMznOAguJJ9/1dWOEVdOTq+Gt7b7avoYxLoNR7Fc76W4K3S+/ux54dDMTRdFnVA2OTnyyR55vcNVs6OOc01aRcAPtDmgETlBc07G47R5aa3VNqgyw7tex/8Ape0/gCrLw7F5MViJjvB7dr5RMecD/SFxxMb14q2/8lp8OzPCTae0n5x/Nn4F8rcDd9pZRNUAOpuqZmsIu17AGkZzMTmB25L7wXhJqVa7XVC3qn5Oy0dq77uDpFwAbc1NcStjsIdnNrM9mtcPwKwYMmnV4g4atIcPPqA78StFG8E7K7Sey3zZSr/W12mnN228kzV4ZwIVDWpuqVA2nUyWy9rshwcczTfK5otGixUeHjq6pzvBpVhT+WC3OGkkEG8EqyvqNY5hb/nVRPj9wY+jGqJq04GNG2djx6tY4/WVmm1J3sv7eC5pS8znPFVrazk9+L34cTB/7faMQGGpUdSfTc7Voh7HMEdloEZXWEbFa3DeEU3tqVKryKLHOaBMTBILiY9ABuDzVmfWHXhhicmdviJc1/pdihqTTUwdWmwEuZUfZutq/WW8S0iFpH90U3bhwXG+u3h0OkcTWvlzu2270tbrp4avY0MVwoNxFJoqEsqk5X2LhDZgWy6QQYuJ5Stelwhp+2ONV4ZQcWyWsM5KQe/NbTM46QpYt6t3DqDu+3Xf/DwxDr+ZHmo7Ese3A4lhBZWxVarAdYhtSqWknwFMT7c1u8kFeVrc7L/s05bco8OfULFYmVoxk+W771x5v6JciufYatStSb1jm5KYqOFoa6pOUNEWf1ckg6B43WD4i12No0MJTjsEOjk1rHNHuTr+6eYVnL2UxnJz1HXJAiXQB6WAEbABQB6JCrUdVr1nFzzJDABHIXmwEBVtKvTdftJ6JapL34u71sWdederSUW7vXkt7t9ei3sihtbFh6n9aD/geFm6EYaar6rwOrp03B7iSMvWMexgaBq9xMBvnyVidw3AYdsvFMbzUOb/AHFfOEdIsDSLjQrU2F0A5YIJbOWxkWJMRzKnT+L05JpRfl487fUrv0E0t15+/ItXAcfXeaDatMAtpuz65hI+6cRNszWvmd27Ta1qocP4y04iiYpufiA6nmbIcBTbUe0m5BbAjQQXb6K3qPVqRqNTirJ/l389jg6bptxluERFzAREQBERAEREAREQFH+Jz2GlQpPcRnqyA3Vxax1gIM6zA5LneK4DVzTSp1C0j5mkEHfWPNdb6VjK1tXIHBkiQJc3NEx4GBMcgq3SxbHxkfYj09fHwWP11Sg8sUvH2idRowqUrNK99+Pd7RTsLwRpb942rTcNZFj4iW/mo3iuB6p0B2Zp0NvUFdFqUjrY+sLC98A5hbxCzD4xUjK8o38bfkkTwtOdNRSSa48fHh9jm9bAONF1RuUiDIm4I5j23UrgeJinjTlGdteg6i6SAJcBOg2MWW9i+GnEPIoEMAkOGUFr3QC0a2OhJg2N1XOJcJrYWpRNVmWHWMhwN73b+C3njVWamt1w8b8C0wGFodjKi95WTV9+bXFfXfpY6th+k1RlMNyMqFoADszm7wMwykZudwo5vFqtM1R2C6sc1XM10tOQNIYA4AtAEDXTdRlB2btON4gfLm9Ygle6rRlkOOUbEWteJ1aToPNbqtJbJddN/r6WM/0nC5rSjv1enRWa9+KJVnFKpp0gXMy4cjI4NJzFrcoLxm0LTtuso4lVqNql5AFQBrsrf2dIBMzfnyWl2SAO0IAABg2iwBGoj1WnUrljpE5G2MEwJ3votnXne/oud+XPU5R+FYaSaUPN93Pcm+IcVqmrSqtLS4AsBDC1pDoLu84nYeoC0sPxGqxzzSdleZJGWziS4gEG5dmMCIieSjON8WAYHBzqjmEOcQIPZPaAA8tdFVq/TN2Q1KNAAzlcahccpPdMNMm0iZFy0LTtns35IxLDYShD/US221bte9+D8bL6aFnPGn5nVn1CXs0c7VuQm2VsNa2ZBtcE7lY+E8Tr1wa1d0ufGRoAAawTFv2nEkmdo8lg4fhm4ql1pHZeZdTaIaHNgQ7c3vrBU1QwwFzdQa+Jcv2LxGIWGeV0orbf0X1v1v1MlNxJBPKy38K4EEEW0hRr6kFSGCxLsvdsN/0VEjuRmamIdgaLpd1Qf5NLv6rW4jxjAvIp1cpa7QVG2PkHCFJ/bZMspVHcyGETHJxgEeqj8TxUEltTC1S3cdUarT55QR6LN7O6NbH3o9w7BtxNGrhSxpY6SGmRBaWkRMTBK6kuddCsFhftLnUaGR7R2mwWBk6ZmaBx2tK6Kp9KpOcbzd+8rcSo59Fw6egREXQjhERAEREAREQBERAV3pFxIDNRtMBxJ85ED0+qqeM4WyqJzFj9nNsR7EfVW3pRToOY6nUY0vqU3NDoALRzDu8L3EHZUKjwOm2erxVanB7uYPHrnk/VQK/zb3LLC/Jt/Jv4HC1qch9UPHy2g+Obb2C36T7XiVo02loAdUDo+Ydne1pN1kbWBsHjle39FyJXA2HMGoAB5gQtLi/D2YikaT5O4MXa4aEfrcqQoenovUCdEs07mVLK7orbKNdrQ17Jy2kXnS9p/tK+PqkkADu+MGbEB0agEWkc1Mcbxwp0yAe2eyIEwTpK9UqLQ1rWsBbbtFoMzc2MXIEzfX2mU5zmm29uSRtX+KVIWSSu+hG0alSCAAJEWH4TofJehgZILhJI1IC2cRhWsIcGwDHZO0z6bbLN1ANwY8iVwr5lLK22KeKlWjn2MBwoLSyBBC5fxXBHDV3U3S2lV56ZZvPkTHOwK6p9nds53mozivRyliHtfWaXlogSSN/Ai60pzUXrszjWpuaVrXRVOh2PdhcU7CVTAe7KDaM8AMI0nM0t05tGxXQa9EN397LTpcGotId1bS6AMxAJgaCTJsFtDDtWKk1J3t3madPIst9OBq1sQ1g1a7wGv/KjqXSEtJa1lTLsWtc76AEqcGGHNezSaFqmzd2IerxnF1D91Qgc6jgz2Ak+6yYWtjRZ5ohu8ZidfIKSJCwVHd4o2xlRauhxLxVquMlxayfBjZ/8lZlEdF6GTC051cM5/mMj6QpdWNJWgimrO820ERF0OYREQBERAEREAREQEfxTC0XNzVqbXhkxIBidYnmuRYzopHcxlVgnWes95C7U9oIIIkGxB3XI/in0c6t7a1FzqdKoMrmsMNDx4aCRsP2So2Ih/cScPUUdLGvh8GaI7WLNaN3sAg+EFZaeJbU1FtJn8tlzSq+swy3EP9x/RYqfGsQx0l4d5z+RUVwb2JDxcY8PM6xTwzBca+cfVbjMYwavNubj+ZXKD0urxGUe/wDZQ2N4lWqmSfZFTfRGrxa4I7RxXEUn0XRVYSBaHNsR6qncL6UV6MtbUpOZ8rXiMo2hwOnhFpMLngDpEvyzaZiFIcS4TWw7RUqFpEgCNzeI9pUvDxcbvci4irOpZJWOq0OJ1KrWuqlgcbwLx9Vv08eYu4R4LjWG4+4CDmH1UjQ4/OlS/sfqo1SM222TqdaMYqNjrNLiDOayjHNPJcup8Xf+17rO3jFQcvdc9Tqq0GdIdixzWN+K8VQhx2ruPqF9HHn8vqmo7WBcq2IPNeKVdxI7SqrOPDcrI3pAwaG6xZm3aw5l4w1MHUr4+l1tZlJvzED3Nz6CT6KsUekQIsb+au3w+w5q1HV3XDBlB/edrHk3/cF0jDM1E0nXjGLaZfGNAAAsAIHkvaIrIqAiIgCIiAIiIAiIgCIiAKqfE3/6+p5t/wBwRFzq/I+4ytz864zVYDsviKKiNU3Z72WHF6Iiyt0WNHZdxD1O8rX0o/6fB/8A5/k1EUrg+42/5I97+xCVNB5LRdoiLBNrkpw3urdpoijVPmZBnuZG7IURc3uDDVWs3ZfUXaJGqElw3vD9cl+hPhr/ANBT/if/AL3Ii2pfP4GsflLSiIpJkIiIAiIgCIiA/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhITEhMVFhUVFxcYFxUVFxcYFxUXFRUXFxUVFhcYHSggGBolGxUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGi0lHyUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBEQACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABQECAwQGBwj/xABEEAABAwEFBQQGBgcIAwAAAAABAAIDEQQFEiExBkFRYXEigZGhBxMyUrHBFCNCctHwFTNigrLh8SQ0Q0Rzg5KzCHSi/8QAGwEBAAMBAQEBAAAAAAAAAAAAAAECAwQFBgf/xAA8EQACAQIEAgcFBwMDBQAAAAAAAQIDEQQSITEFQRMiMlFhcZGBobHB0SMzNEJi4fAUUnIVNcIkQ4KDkv/aAAwDAQACEQMRAD8A9xQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQFC4ICoKAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIChKAirwvyOMloIc8fZBAp94nRARbNrogCXmPI5iOQOcOraBRcmxy21XpLbGcEErGU9uTDjwn3WZ0L/Ic1FyUjzG/NrpZc2SzOPvyPdiPcHYWjkGhRcmxC/p21uOdolr/qPJ6DPLuUEnUbKeky1WEOa6s7SQaSve6nHCSSR59FKZDR6FcnpssctBPFLC7eQA9vkQ7yVrlbHot1XpDaIxJA9r2neN3IjcVJBuIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIChKA8/wDSTtuLI31MecrmmpFKRjdXmVVuxZK54He19PkyJrnkBQAGvDeeZzUFjW+mOOrh95xzJ3kctyhhGM8SCeGYoPDRCS9s0Z+y4nkQQo1GhczDX2ZAOVU1J0FoY7UE0/a/FEyGjSDy08FYqerehy/nRzYSew8gOJxb8gXbsjTP+qlEM98VioQBAEAQBAEAQBAEAQBAEAQBAEAQBAEBq3pahFE950aCfAID5l2uvP1ksjzUlziaVzJO7oBQdOqz3NdjkJbO/wBo0HJTdEWZlZdzsNTrXyoozInKzGLO5vEchql0yLWMuIjMt78gR4KCTZimboSW10cKlp6+6libmK1TkZEnrWoIUpEM03Pz3U5/KikgndlZmNkJcZD2dGGlPEoyD6V2G2gFrs7an6xgAeCKE0HtU5/FWTKtHRqSAgCAIAgCAIAgCAIAgCAIAgCAIAgCA4L0u336iyYQaOecIHGmZ+HmqyehaK1PBZRQYne0c89yyua2M1w3L699T7OpP4Kk55UaU6eZnpEWz0OFrcIy3rl6V3Ozoo2MFo2MY8kg0J8ldVjN0ERFs2CJNG68a+ZWqqmTokRemwtoiGLC0jgOHgrKoivQs5993FuR04EZH8CrqVzNwsR81joTSlNc9R+KvmKNGxdxDXAjFVvx4Z/nojIsdzsPtD9HtkU0zyxoJY7C8vBa6lQ4aDOh7kTIaPoqGZr2hzCHNcAQQagg6EFaFC9AEAQBAEAQBAEAQBAEAQBAEAQBAEB4T6Y7f6y2iKnZgaK10L3gO8ACPErKb1NYLQ85ewyyNZxzPTcPJV2Vy+7sel3Jd4jaABQjzrqFxzldnfCNkdDZc+o1VLGpJQMKJENo2o4MloloZtmG1WfECCqtMmLRwG0l1BpNAKa9HbvHRXhIrUjdXPPrys5jLS3jVp4cjyqumMr6HHKNtUTtsuyF8EVoYzDiaatro7R1O9VjJ3syZxTSaIG77M5zXvi/WxGtN728uY4Z1WqZhY9v9C99vlgdG+paO03Fq017bOlcxTSpCvErI9MVioQBAEAQBAEAQBAEAQBAEAQBAEBa91ASgPnHb9jjbrQH6uLcJ3doAOd8e5qye5rHYidmYGmXHurl0GQ8gFnN6G1JanpVij3rkZ3okYxQ8D8eRCqTYkrOVKKyRtNcKK6M2YZH8/z3I2XSOcv6LE09P6Kl9TTLdHBT2T1rHtpmK9fzu/otc1nc53C90XXHATZnsP2D2geDtHDhmFdvW5klpYgrPA6N8haDXQHz3LZM52rHvXomu31dgikP+MTKOTXnsjwp4rWOxjLc7ZWICAIAgCAIAgCAIAgCAIAgCAIAgLXtqgPC/TXYxFPC7dLGGnlgxiv/ANjwWcjSJz+yjQXZaALnqPQ6qS1O/sLtFzHYiXggBUqJGaxuxwqyiQ5Gx6hWyGeYp6gKVEZ2R1usoIIO9UlE0jM5A3c1s7j74qKcQq8i3MnbsuiMtfkAXZHdnzWkNTCo7M8rvmAxzvi0Idr0d5roicktz370cT47usp91pYKClRG9zAabqhoK3jsYPc6VSQEAQBAEAQBAEAQBAEAQBAEAQBAEB47/wCQkBwWOTcHyNJ5locB5O8FWReJxWxI7LyeS5ap2UDpm22XNsTc97jl3D8VRRXM1cnyLZr6vCH/AC+Jo3g1HlmrJR7zNyn3G3dm2z35PhLTvz+RCOPcyVK+6Oojt5cAW6FZORskrGnet6ujGXOqmOpV6HIT7QXhM4sijaBX2q7u9a9VbmTc3sZorqtNayTZjhzzyVM0SyjLmdXcQeG0ccXNSrcisvE8y23Dm22YgZ1aRX9oDLxC1hsYT3PZvRRaMV3xtJ7bXPDm5dk4iaZbt/et47GE07nYqxUIAgCAIAgCAIAgCAIAgCAIAgCAIDxn0t3sy1MfCHOHqZRVhb2XUqCcR3jlxWLnd2OlUrRuc9sZZvqXGmpWFR6nRRWhOWpz4h9XGXu3DQd5We5psRM943m5mJroo86erAJfTjU/Ib1qoQMZSqckZxs/M5kbzM50riS9pa0tAJyzAGdFEsqLQU3qztNnj9W3EBUZEjQkcFhzNraGhtDAZSGg4a1zy4Za5VUrcOOhx14XJMxrHQzyCQE+sbiIHIgAjKnPULojl5o56kaiehmsthtgc3DaHvFKu9YARXgCACVSeTkXgp8zuLhLgCHjMjOnHkqRetiZxON29u8/TGOoaPYG5CujtfBbJ2Ri1eSOu9HjnxTmMu+rIo0UoS4tBxGufKimlLrI1xFK9NyPTF1HmhAEAQBAEAQBAEAQBAEAQBAEAQBAeFbexAS28O1c52Dl2Qa+NVySdpnpJXpLyKbJkeoZzCzqbk0eydZZYw4rO1zZm1JY2HUVSxXUwWuFrGENFFZy7iUtdTBYZaCgVDW1ysrcdeI+Skh2RdZ42uAxNB6jPxVlK61M3F8jOYWDQUVWkFfmZLIzOqmKIqPQi9pYS6eEtHsAk5V6Ci0lsZUldkts3CXTxHgST+7oEoq8ka4mWWk13nfLuPICAIAgCAIAgCAIAgCAIAgCAIAgCA8T9KFhk+kvc0E0dWg1LXCtQuWekmenRs6aI+4OwwNBqN3Q1oO7TuWUtSYK2h2FgfRUNbknRGEzSvUgNAOrjQfMqLE7kRZb7s7JCwvY460qCcuQVsvOxGdbXE20NlMwY57Gudo1rgD3BMt9bDOuzfUnYYgQKGvMb+aqojMWyMQlMy2M4c/irx0MqmpqNle57sIbmKVO7Xd+dEbfIU0lqyb2Ps5xuJ0aN/E6rbDrVszxs7pI61dR5wQBAEAQBAEAQBAEAQBAEAQBAEAQHH7eXMX4Z2iuAUeOW53csK0L6o68NUt1WeaYgJNdd3Ch/muY65bnR2B+ircstiegNQhBq3xYBMG9ogtzqM9dQlwtCGsuy8DCaxsqTWrW4T30U52MqL7Rs/D2fqw0Z+zkelVGZhJEzHIA1oH2RlypuVWybFS/EQVZO42RknGRVzFsx3Vd0zyQIyGkkiQ0DaUA67laNOTexHSwit9TtrusQiYGjPieJXXGKirI4ak3OV2bSsUCAIAgCAIAgCAIAgCAIAgCAIAgCAoRXIoDi9s9moGWeSaKJrZGlri4VqW1o4chnXLgsalOKi2kdFOrJySbOQsMtAuNnciein7IoqMtaxjtdvYz23huW8qSDR/Thd+pjc4e8Qc+mnxVsrNIwNe0XnaSKiKjRxA17zVTlLOCRZFfWeF8b2P6EtI4gjRQ42M2mTUR061VFuHsbT3178qc1sjBnc2OLCxjeDQPJdyVlY85u7uZlJAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEBr3hZxJFIw/aa4eIUNXJTs7ni9mkLSWnItNCOYNCPJefJWdj1Iu6uTlmmy1WTNEJ7HG6jyxrncSKkdOClNrYkxmRzPZb0zVlMnMy02iV2TmgcgT5qXMi7NuI8R+eCo3cguhlr0RES0Ny63A2mFp3ur4Bb0tZI56vZZ6Cu488IAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgPHtr24bZOR72YHOma4KvbZ6VFdRGvY7UsGbok4TwOqgkkIY2nWnOqskDLPG0aUVmkTe5pTDKo8vBUsVvY1vpDWNca8+9SijdyS2SaTOx7t5yHAUW1J9dGNZdRnoq7zzwgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgIDbfaD6FZJJmgOk0ja7Rzjx5AVPcjKyllVzyWyXnJamMtE1McoDnYRQVPALz6vbZ61H7tGKZpGiwejNBFej2a6aK6aZR3RIQbQN3nMpoWUjJ+n2e8hOY1rTfROTdEuUbuZbBC55GLjoqtkqJ2lxANli5ELWi+uilddRndL0TzAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIDTtl5RxglzhUbgc1y4jG0aEW5yXlzNqdCdR6I8R2xv2W2SuMlAyPEGMGg4k8SaarVSzJPvPNqybk0+TM1zWMNgiaPssaPJcEpXk2fR042gkXzQUTcNGpLYCcwVWwIu22V7dwPiFbJ4lHJmmwSk5ReNU6MZzpLnuh5zfQcgqtFkdVY7KGBQXMlseWRvcDQgEg893mrw7SMcQ/speRu3JtPKA5rjjw+9rhPPkscdjq2EkpWTi/VPzOLAQhiIuLdpL4HS2HaCJ+TuweenitMLxnD1tJPK/H6m1XBVIarVeBLtcCKggjiF6qaaujjasVUgIAgCAIAgCAIAgCAIAgCAxWi0NYKvcAOfyWVWtTpRzVJJLxLwhKbtFXIq0bRxjJgLj4BeTW49h4LqXk/Re864YCo+1oRFtvSWTKtBwbkB36lfP4rjGIruyeVdy+u530sJTp62u/EjDZ6nNeYpM6bnn992YxyyNO5x8DmPIr9BwtVVaEJrmj47EQcK0ovvJnZ54dEB7uX4eSwrRtI93CVVUpLvWjJWSzA7lVM3ZrOsxBUgu+ijeFZMo0XR2Vu4eSXIN+CKirYsbYChk3IC/bxBPq2nIGrjxI0Hz7lvRh+Znl47EK3Rx9pk2bGJ0rt1A3vJqfgPFePx+qlCFPnuX4PTeaU/YSxZ8BX8V8y3qfQmzYbfJEey6nwPUcV14XHVsM703p3cjKrQhVXWR0Vm2jjI+sBaeOoX0+G47h6q6/VfuPKqYCpF9XUlLLa2SCrHB3Qr1qVenVV6ck/I5J05QdpKxnWpQIAgCAIAgCAIAgLJZA0EuIAGpKrKSis0nZEpNuyOdvHaOtWwj98/IL5zHcdUerQ9foelQwHOp6EI973mrnEneSa+C+bq16laWapJs9GMIwVooyMYBkPFYtkl7QiRDKPG/hRTyCOf2wuvG0TNGgo/pud3aL6XguMt9hLnqvmjxOJ4Zv7VctzkrttphfXVpyIXvzhmVjzsPiHSlmW3M7qxStkaHNNQVyOLi7M96FSNSOaOxnlgBQtco2HJSVYMYCkgrGEBzl/bQAVZGeRcPgPxW0KfNnnYjGflp+v0Ods73yPDGCrnGgCvOcacXOTskefCDnJRW7PQrBZBDEGDM7z7zjqfzwC+FxmJeJrOo9uXkfV4WgqMFFe0z0XGzoLS2qlMm5QGmRTxQDWuacUbi08jT4LejXqQleDafgUkoyVpK6Je7dpnt7MoxD3hr/NfQYXjdSHVrq/jzOCrgYS1pv2HT2W2MkFWOB5b/BfRUcRSrK9OSZ5k6coO0lYzrYoEAQBAEBjtEwY1zjoBVZ1qqpQc3slctCLlJRXM5u07UnSNg6nNfN1ePzfYgl5/RHpQ4evzP0Iq02uWU/WOqOAyHgvFxXEK+I7ctO7kdtOhTp9lFrY1w6mtzKOSXKlQFKQLlJBVW5EGON2oPnwKQk1sTOKZyG0ezuGskQqw6tGrOP7vwX13DuKRrJQqO0vj+587jMDKm80Nvh+xEXReD4H5ZtOo3H+a9edNSWpx0MTKlK625o9BsE7Jow9hy38QeBXHKNnZnu06sakc0S2SIgqDQtbESqOcU7Nk2OU2q2kArBCTlk92leTeXNdNOPM8rFYhyvCO3M5+77qmmPZYTX7RBDR+8clFbF0aCvUkvLn6HLTw9Wq7Qidzc10x2YZuBkI7T9zRwbX8lfL4/HVcXpFPJyXf5nu4TCQw+sn1jYktwcQ2MYjy06krlp4N9qq8q950yxCWkNWDaJdPVZ8dy1eFwu/SGSr1/7B9edGtb1/JTJgYbtsZsVLZJFDYJXe1LT7v5Ct/VYaHYp+v8ZXoa8u1P0KG5BvfIerv5KP9SlHswivYT/Rxl2pN+0OuKI6g9cR+Sq+K4jw9CVgKK7/AFL4LB6o1ifI0/eJHgUjxOondpea0fqi/wDSQStFv4r3k5dV/vY4CdxcHHCCBnX8gr2OG8TlKU3Uk3FK+ttParHJi8OoKNkrt20+h1kMzXgOaagr6GlVhVipwd0zglFxdmZFoVCAx2idrGlzjQBZVq0KMHObskWhBydkcZtDeMjhiqQzE0Fo90mmfkvlYcTnjMROntFxkory19XY7p0lQjGfc1f4GuyzgL593e56uYzhiskVbK4EykZh6tTlGYrhSwuVLVNiLlAiDLHihqqvRl09LAmmY/qPxUq/Iq7cyMt9yQSVcWlhOrmaHqNPIL1sLxbEU+r2l3P+XOCvw6jUd9mc7hNkld6uY0FNRkQRvFaFfVYefT0lOSs3y7jwKjnhqzjB/ubjtpJS5o7PaIAGAguqaUGLqrTpwhFyb0R0xxmIc0nG17E1eDnaB2Gi+PeNUpym1dvby5H0DoOVtTUZd7nnESDzp81b/UEtMvvKSwi7zMLO4/by3kVp0bnn8FSWOilpDX+eAWFlfWRQ3ewnQnjUk15nisXxCtbkvYaLCU93qb9nhDdAB0C5JVJzd5O5rlUdEjLgVbE3L2hXSKsuoliAQjQuULUsTcsLVSxa5ovbitDBujaXHq7st8sXiu6L6LAzlzm1H2LV/I46n2mJiuUU37XovmTd32t0ZqNN44rLh/EauEndO8Xuv5zL16Mai8TqIJQ5ocNCv0CjWjWgqkHozxpRcXZmRalTlbwthld+yNB818DxXiMsVUsuytvqexh6Cpx8SPvKHFFI3i006jMLlwVToq8J9zRbEQz05R8C2xyYo43e80HxCvi6fRV5w7my2HnnpRl4I2AFkjRlytYFFHMAhQ00wUxBawpylsiG0i0vroF0LDxWsmZ9I+RY6Jx30S1CPK4vNlv0Ti4qFWhDsRSDg3uyw2UA6mnDcDy5KixMobJX7yzpKXMhNoIvVSxSNA455irDUV46r6TgmIlUpyjLk/czweKU1TqRnH+WLbutj7RMC8AthDnN0yc85Z76CvgFHHK/R0FTT7T9y3+Rvw77erma0j8SZdCG5ntOO87l8lc+gTuX+rqKbuHHry5KL2ILi1U3JuXNjRIhyMrWrRRKNlSFZrQgAKLC5cFaxAKiwGFTlFymFVy3FyPsOck7v2w0dGNFfMldHEOpSo0/0t//AE/ojmw3WqVJ+NvRfU3gV5Z1smbltVDhOh8ivqeA43K+hls9vP8Ac87F0r9ZE6vrTzjiWlflV7u59DYyK9ytjQuc/UtHuuc3/i4hevj+tWzr8yi/VHNhNKeXubXozexhc6ptnSW+sO4K6pLmyLlsgcj6Jcgrl3qq6lT0qXZRFg2IKvTzYyoyhUbbAUMkoqgEKSSB2qi+qB3NcD0ByPyXrcDqZMQ4cpL4anncVp56ObmmYtlbPggxnWRxcfujJo8BXvWHGa/SYlpbR0+bNuGUslFPm9SVALjiOm4fM/gvLkejtoZlUgvDVZIrcuor2Kh5p+eKSeVXIKZ8PNY9PEXK15HyU9NEXFdFZTUnZC4fuV3oSi9WKiqeAZEXI6sWL33Pd4uKvxd/9U4/2qK9EjHAr7FPvbfqzfDl5h2GzZ3row83GRjOJI/TncV9B/q9fvRxf00CFxL5dHpGQlWbK2I27G52gV0mcf8Ak1rvxXtYidqVGX6F7m0cuH7dSP6vikSgYFzObZ0FyqDFLaGhwaXAE50PDTVaKhUnFyirpGbqRi7NmUaLGOxoxRLAw2m1sjHbdTzJ7guijh6lXSCMqlWEO0zM11QDxWUo5W0XTurlVUkolgat6Q44pW8WO8aZedFvhanRVoz7mZ1odJTce9GOCzgBrPssaB4Bc05uc3N8236m9NZIJIzlUtcsXtapSKtl9FdIqVVga9vnEcbnkEhtCQNdVaFB15KnF2bM6tRU4OT5EC6/JZ3GOzsoHCge44S00q52KtBTVezhOAU4NSrSvJO9tLNe3XzPJq8QnUuqS07+42Lay12LtyOE7DlUPyY4HOuVd4z0XZiuCYetFKKUHfkr3KRxVajrLrL0sbl33vHMWhtceGrm0OWlRUjPMr5utwuthG5S7N7J3Wvs8kelh8XTrOy3tsb025Yz5HbEucVLKowW+XDHI7g1x8AVth4Z60I98l8TOtLLTlLwZo3U3DDE3gxviRU/FY8QlnxNSX6n9C2EhloQXgjbcaLiSOgzQvUXs7lJIz+sW3SmeU1X6lZGy2KNfUNPJGtWLGlYMprQOJYfFtPkvWqvNg6L7sy95yU9K815MlGGq5o2epuy8FWurlSA2ijOJknao0iumGgOdRqMjr4r3eETThOGl367ejPL4hFqUZa6Gzdt49psbt9Q056ivZz3ECo8OC58ZhLp1Ie3y7/ZzNqFezUZc/j+/I3LxtvqwAM3uyaPiTyH4LkwuGdaWukVu/kb16ypqy3exzVorNLGyoJLsWuEkaA1FTmKnIZCmi+ghbD0pStyt3/T9zyan21SMb+J1zG0AAFABQdy+VlJybb5nuRSSsVVSRRCTBbHdk9w8XAfNEruwLmNz8VVLWxZvQukbmFLWpCehdRTlIuKJYCimzBjtUAexzDo4EeIVoTlTkprdO5ScVOLi+ZyN0Y4DK2RjizFhc5oJwuANCQNxDq16L6DiGTFRpzpSSna6TdrpvVeaa2PEwqlQlKM07Xt5fsSTr5hoCDWjR2QD2iCdBvrkuCGAxmsW7Jt632vbc6pYmjutdNrbmDZWzO9ZNK8UObacycTvkunjFaDp06UHdb+xKy+ZnwylLpJ1JLw+Z0c+gXgT2PahuUa5Rclo077d/Z5vuEeOS7uH64qn5nLjPuJ+QjFAByHkAvNqO8m/F/E7KatFF0jszyyVEtCyMsRyVGVZkxKtiLGHHUNPEBXas2iUWwHIjgSPmPipnvcnmaVmfS1SjjEw+BIXqJX4fF90370jivbFtfpXxZJagN0rr0/muSKOvxNmOMDRXUbbGblfcwWuxMlaWvAI3EgHCeIqunD150JZosyrUo1Y2kiFkuWXC5gofcfizBbm0uyFDlSo+S9iHEKN1P1Vu/ex5ssJUyuHo/La4sl1Wh1Xyubjd2e1R2Fo5DWp4JUxmGh1KSeVa6aXZFLD13eVRrM9NddCYu6xNiFa1c72nVPaO+gJyXmYrETrPayWyO6hRjTW+rNxcR0hAUKgGreIqwj9pn/AGNWlG2de34FKnZNgarHmacg7cpCCAJcBTcEZfzJcGKJ4bhIJBoBQGtanTpvXdgHQ6XLVje+i834fPkzjxiqZM1N2sajZJJmYo6xTUGYpheNRiBzA4Ejet69GlhKmStHPB96aavzT2fjZ6+ZzxqTxELweWXufmaVhbacZDR6s/4rzGMjiJozca1rQcVtinglTzVOsvyrM+5Lrd1tteSMqUcQ5Wirf3O3wNi1Xg9skcUMbsnYnYqB0mfayOYBJqTRZUcJSq0pVqs1a1lbVLu9Nkk/N3NqmInCcadKPn4k84mgBpXlpXkvIlbZHqQva7MNVkaGpfp/s0vT5helwv8AFQOLH/cSMkRyHcvKmtWd62KA17yjJMznblnYqMaWBbF7DfzvKtLtMLcts32/vD4BTPl5EmjF/fH/AOiP416sP9s/9n/E4H+NX+HzJaPR/QLigdj5GxD7Lei15Ize5Vu/88EWzKy3RrWn24v9z+FdlLsT9nxOefaj7SOsHtWT/c+a78R2a3/ictPen7Sl1aQfek+AVcX/ANzyj8yaG0PNk4V4Z6RVSChVWDDavZPVv8QV6fbRWfZMrlkzQq7crsqCjJKFQgVKA075/US/dPwXThfv6f8AkviY4j7qXkyOt3+X6N/gavreJfh5HiYftxJmT2e75L4D8x9ByOWs/twf+w7/AK2r7qv/ALdL/E8CH4mP+R0jl8afSFjdCsyTRvv+7S9PmF6HCvxUPP5HHjvuJGWD2R0C82faZ3rYR7lEiTJJqqrYqWoD/9k=</t>
         </is>
       </c>
     </row>

</xml_diff>